<commit_message>
Adds testscript to search for an Author cluster
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/WAT.xlsx
+++ b/src/test/resources/xls/WAT.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="13290" windowHeight="4425"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22830" windowHeight="7965"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
   <si>
     <t>TCID</t>
   </si>
@@ -41,13 +41,19 @@
   </si>
   <si>
     <t>Verify that user is able to login WoS Author Transformation Application using valid WAT Entitled account</t>
+  </si>
+  <si>
+    <t>WAT02</t>
+  </si>
+  <si>
+    <t>Verify that user is able to search for an Author cluster and navigate to author search result page.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -121,11 +127,42 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -174,7 +211,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -206,9 +243,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -240,6 +278,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -415,14 +454,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14:C15"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="41" bestFit="1" customWidth="1" collapsed="1"/>
@@ -431,7 +470,7 @@
     <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -448,7 +487,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -462,6 +501,21 @@
         <v>5</v>
       </c>
       <c r="E2" s="4"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Code restructure for SearchAuthorClusterPage and minor change in WAT03 testscript
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/WAT.xlsx
+++ b/src/test/resources/xls/WAT.xlsx
@@ -10,12 +10,11 @@
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
-  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t>TCID</t>
   </si>
@@ -57,6 +56,9 @@
   </si>
   <si>
     <t>Verify that all static texts present in Author search page is diaplayed properly.</t>
+  </si>
+  <si>
+    <t>WAT-162||WAT-507||WAT-215||WAT-220</t>
   </si>
 </sst>
 </file>
@@ -468,7 +470,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -532,7 +534,7 @@
         <v>12</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
Adds new testscripts and minor changes to existing scripts
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/WAT.xlsx
+++ b/src/test/resources/xls/WAT.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
   <si>
     <t>TCID</t>
   </si>
@@ -59,6 +59,39 @@
   </si>
   <si>
     <t>WAT-162||WAT-507||WAT-215||WAT-220</t>
+  </si>
+  <si>
+    <t>WAT04</t>
+  </si>
+  <si>
+    <t>Verfy that Author search can be triggered only with Lastname</t>
+  </si>
+  <si>
+    <t>WAT-1156||WAT-160</t>
+  </si>
+  <si>
+    <t>WAT05</t>
+  </si>
+  <si>
+    <t>Verfy that Author search cannot be triggered only with firstname</t>
+  </si>
+  <si>
+    <t>WAT-517</t>
+  </si>
+  <si>
+    <t>WAT06</t>
+  </si>
+  <si>
+    <t>WAT-202</t>
+  </si>
+  <si>
+    <t>Verify that typeahead will be displayed for a minimum of 1 letter - Lastname field</t>
+  </si>
+  <si>
+    <t>WAT07</t>
+  </si>
+  <si>
+    <t>Verify that typeahead will be displayed for a minimum of 1 letter - Firstname field</t>
   </si>
 </sst>
 </file>
@@ -121,7 +154,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -133,6 +166,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -467,10 +504,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="E8" sqref="A1:E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -530,18 +567,79 @@
       <c r="E3" s="4"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="7" t="s">
         <v>12</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="7" t="s">
         <v>5</v>
       </c>
+      <c r="E4" s="7"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="7"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="7"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="7"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Adds 8 new WAT test scripts along with minor modification for existing testscripts
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/WAT.xlsx
+++ b/src/test/resources/xls/WAT.xlsx
@@ -4,17 +4,19 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16980" windowHeight="3135"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16980" windowHeight="3135" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
+    <sheet name="WAT09" sheetId="2" r:id="rId2"/>
+    <sheet name="WAT13" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="78">
   <si>
     <t>TCID</t>
   </si>
@@ -92,13 +94,169 @@
   </si>
   <si>
     <t>Verify that typeahead will be displayed for a minimum of 1 letter - Firstname field</t>
+  </si>
+  <si>
+    <t>WAT08</t>
+  </si>
+  <si>
+    <t>WAT09</t>
+  </si>
+  <si>
+    <t>WAT10</t>
+  </si>
+  <si>
+    <t>WAT11</t>
+  </si>
+  <si>
+    <t>Verify whether Last name field takes in blank space for searching author name</t>
+  </si>
+  <si>
+    <t>Verify whether Last name field takes in special character for searching author name</t>
+  </si>
+  <si>
+    <t>Verify whether Last name field takes in Numbers for searching author name</t>
+  </si>
+  <si>
+    <t>Verify whether Last name field takes in Alphanumeric values for searching author name</t>
+  </si>
+  <si>
+    <t>WAT-174</t>
+  </si>
+  <si>
+    <t>WAT-152</t>
+  </si>
+  <si>
+    <t>WAT-165</t>
+  </si>
+  <si>
+    <t>WAT-140</t>
+  </si>
+  <si>
+    <t>errorMessage</t>
+  </si>
+  <si>
+    <t>Symbols</t>
+  </si>
+  <si>
+    <t>No results</t>
+  </si>
+  <si>
+    <t>!</t>
+  </si>
+  <si>
+    <t>@</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>$</t>
+  </si>
+  <si>
+    <t>^</t>
+  </si>
+  <si>
+    <t>&amp;</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>(</t>
+  </si>
+  <si>
+    <t>)</t>
+  </si>
+  <si>
+    <t>_</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> =</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +</t>
+  </si>
+  <si>
+    <t>{</t>
+  </si>
+  <si>
+    <t>~</t>
+  </si>
+  <si>
+    <t>;</t>
+  </si>
+  <si>
+    <t>:</t>
+  </si>
+  <si>
+    <t>"</t>
+  </si>
+  <si>
+    <t>&lt;</t>
+  </si>
+  <si>
+    <t>&gt;</t>
+  </si>
+  <si>
+    <t>,</t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t>[</t>
+  </si>
+  <si>
+    <t>]</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>WAT12</t>
+  </si>
+  <si>
+    <t>WAT13</t>
+  </si>
+  <si>
+    <t>WAT14</t>
+  </si>
+  <si>
+    <t>WAT15</t>
+  </si>
+  <si>
+    <t>Verify whether FirstName / MiddleInitials field takes in blank space for searching author name</t>
+  </si>
+  <si>
+    <t>Verify whether FirstName / MiddleInitials field takes in special character for searching author name</t>
+  </si>
+  <si>
+    <t>Verify whether FirstName / MiddleInitials field takes in Numbers for searching author name</t>
+  </si>
+  <si>
+    <t>Verify whether FirstName / MiddleInitials field takes in Alphanumeric values for searching author name</t>
+  </si>
+  <si>
+    <t>WAT-143</t>
+  </si>
+  <si>
+    <t>WAT-204</t>
+  </si>
+  <si>
+    <t>WAT-146</t>
+  </si>
+  <si>
+    <t>WAT-208</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -112,8 +270,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -123,6 +289,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -154,7 +326,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -172,6 +344,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -504,10 +678,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E8" sqref="A1:E8"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -641,8 +815,799 @@
       </c>
       <c r="E8" s="7"/>
     </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="7"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" s="7"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" s="7"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" s="7"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" s="7"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14" s="7"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E15" s="7"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E16" s="7"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A19" sqref="A19:XFD19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="7"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="7"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="7"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="7"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="7"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="7"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="7"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="7"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="7"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="7"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="7"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="7"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" s="7"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="7"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" s="7"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" s="7"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" s="7"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" s="7"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" s="7"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" s="7"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D22" s="7"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" s="7"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D24" s="7"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D25" s="7"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D26" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19:XFD19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="7"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="7"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="7"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="7"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="7"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="7"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="7"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="7"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="7"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="7"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="7"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="7"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" s="7"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="7"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" s="7"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" s="7"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" s="7"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" s="7"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" s="7"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" s="7"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D22" s="7"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" s="7"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D24" s="7"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D25" s="7"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D26" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Adds WAT16 and WAT17 testscript
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/WAT.xlsx
+++ b/src/test/resources/xls/WAT.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16980" windowHeight="3135" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16980" windowHeight="3135"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="83">
   <si>
     <t>TCID</t>
   </si>
@@ -250,6 +250,21 @@
   </si>
   <si>
     <t>WAT-208</t>
+  </si>
+  <si>
+    <t>WAT16</t>
+  </si>
+  <si>
+    <t>WAT17</t>
+  </si>
+  <si>
+    <t>WAT-150</t>
+  </si>
+  <si>
+    <t>Verify that Typeahead works during multiple alternative name search - Lastname</t>
+  </si>
+  <si>
+    <t>Verify that Typeahead works during multiple alternative name search - Firstname</t>
   </si>
 </sst>
 </file>
@@ -299,7 +314,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -322,11 +337,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -346,6 +372,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -678,10 +705,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16:D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -934,6 +961,34 @@
         <v>5</v>
       </c>
       <c r="E16" s="7"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1281,7 +1336,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A19" sqref="A19:XFD19"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Adds WAT18,WAT19 & WAT20 testscript
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/WAT.xlsx
+++ b/src/test/resources/xls/WAT.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="92">
   <si>
     <t>TCID</t>
   </si>
@@ -265,6 +265,34 @@
   </si>
   <si>
     <t>Verify that Typeahead works during multiple alternative name search - Firstname</t>
+  </si>
+  <si>
+    <t>Verify that "Add alternative name" button should be disabled (Gryed
+ * out) until a single letter is entered in last name field</t>
+  </si>
+  <si>
+    <t>WAT18</t>
+  </si>
+  <si>
+    <t>WAT-191</t>
+  </si>
+  <si>
+    <t>WAT19</t>
+  </si>
+  <si>
+    <t>WAT20</t>
+  </si>
+  <si>
+    <t>Verify that "Add alternative name" button should be in disabled state even if First name field is having value.</t>
+  </si>
+  <si>
+    <t>Verify that "Add alternative name" button should be (Gryed out) when content of Last Name field is removed.</t>
+  </si>
+  <si>
+    <t>WAT-206</t>
+  </si>
+  <si>
+    <t>WAT-180</t>
   </si>
 </sst>
 </file>
@@ -314,7 +342,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -337,22 +365,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -372,7 +389,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -705,10 +721,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16:D18"/>
+      <selection activeCell="E21" sqref="A1:E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -962,33 +978,80 @@
       </c>
       <c r="E16" s="7"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="8" t="s">
         <v>81</v>
       </c>
       <c r="D17" s="7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17" s="7"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="B18" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="8" t="s">
         <v>82</v>
       </c>
       <c r="D18" s="7" t="s">
         <v>5</v>
       </c>
+      <c r="E18" s="7"/>
+    </row>
+    <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E19" s="7"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E20" s="7"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E21" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add WAT21 & WAT22 test script
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/WAT.xlsx
+++ b/src/test/resources/xls/WAT.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="97">
   <si>
     <t>TCID</t>
   </si>
@@ -48,9 +48,6 @@
     <t>WAT02</t>
   </si>
   <si>
-    <t>Verify that user is able to search for an Author cluster and navigate to author search result page.</t>
-  </si>
-  <si>
     <t>WAT-503</t>
   </si>
   <si>
@@ -69,9 +66,6 @@
     <t>Verfy that Author search can be triggered only with Lastname</t>
   </si>
   <si>
-    <t>WAT-1156||WAT-160</t>
-  </si>
-  <si>
     <t>WAT05</t>
   </si>
   <si>
@@ -267,10 +261,6 @@
     <t>Verify that Typeahead works during multiple alternative name search - Firstname</t>
   </si>
   <si>
-    <t>Verify that "Add alternative name" button should be disabled (Gryed
- * out) until a single letter is entered in last name field</t>
-  </si>
-  <si>
     <t>WAT18</t>
   </si>
   <si>
@@ -293,6 +283,30 @@
   </si>
   <si>
     <t>WAT-180</t>
+  </si>
+  <si>
+    <t>Verify that user is able to search for an Author cluster u7sing both Last name and First  name and navigate to author search result page.</t>
+  </si>
+  <si>
+    <t>WAT-156||WAT-160||WAT-195</t>
+  </si>
+  <si>
+    <t>WAT21</t>
+  </si>
+  <si>
+    <t>WAT-190</t>
+  </si>
+  <si>
+    <t>WAT22</t>
+  </si>
+  <si>
+    <t>Verify that when there is no result for the search name entered by User then correct error message should be displayed - Last name</t>
+  </si>
+  <si>
+    <t>Verify that when there is no result for the search name entered by User then correct error message should be displayed - First name</t>
+  </si>
+  <si>
+    <t>Verify that "Add alternative name" button should be disabled (Gryed out) until a single letter is entered in last name field</t>
   </si>
 </sst>
 </file>
@@ -721,17 +735,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E21" sqref="A1:E21"/>
+      <selection activeCell="C28" sqref="C28:C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="41" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="110.5703125" style="6" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="138.140625" style="6" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
@@ -773,10 +787,10 @@
         <v>9</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>10</v>
+        <v>89</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>5</v>
@@ -785,13 +799,13 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="8" t="s">
         <v>12</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>13</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>5</v>
@@ -800,13 +814,13 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C5" s="8" t="s">
         <v>15</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>16</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>5</v>
@@ -815,13 +829,13 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="C6" s="8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>5</v>
@@ -830,13 +844,13 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="8" t="s">
         <v>21</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>23</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>5</v>
@@ -845,13 +859,13 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>5</v>
@@ -860,13 +874,13 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>5</v>
@@ -875,13 +889,13 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>5</v>
@@ -890,13 +904,13 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D11" s="7" t="s">
         <v>5</v>
@@ -905,13 +919,13 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D12" s="7" t="s">
         <v>5</v>
@@ -920,13 +934,13 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>5</v>
@@ -935,13 +949,13 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D14" s="7" t="s">
         <v>5</v>
@@ -950,13 +964,13 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D15" s="7" t="s">
         <v>5</v>
@@ -965,13 +979,13 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D16" s="7" t="s">
         <v>5</v>
@@ -980,13 +994,13 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="B17" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="B17" s="9" t="s">
-        <v>80</v>
-      </c>
       <c r="C17" s="8" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D17" s="7" t="s">
         <v>5</v>
@@ -995,28 +1009,28 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B18" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C18" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="D18" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E18" s="7"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="B19" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="D18" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E18" s="7"/>
-    </row>
-    <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="B19" s="9" t="s">
-        <v>85</v>
-      </c>
       <c r="C19" s="8" t="s">
-        <v>83</v>
+        <v>96</v>
       </c>
       <c r="D19" s="9" t="s">
         <v>5</v>
@@ -1025,13 +1039,13 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D20" s="9" t="s">
         <v>5</v>
@@ -1040,18 +1054,48 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B21" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="B21" s="7" t="s">
-        <v>90</v>
-      </c>
       <c r="C21" s="8" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D21" s="9" t="s">
         <v>5</v>
       </c>
       <c r="E21" s="7"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E22" s="7"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E23" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1077,10 +1121,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C1" s="10" t="s">
         <v>2</v>
@@ -1091,10 +1135,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>5</v>
@@ -1103,10 +1147,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>5</v>
@@ -1115,10 +1159,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>5</v>
@@ -1127,10 +1171,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>5</v>
@@ -1139,10 +1183,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>5</v>
@@ -1151,10 +1195,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>5</v>
@@ -1163,10 +1207,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>5</v>
@@ -1175,10 +1219,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>5</v>
@@ -1187,10 +1231,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>5</v>
@@ -1199,10 +1243,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>5</v>
@@ -1211,10 +1255,10 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>5</v>
@@ -1223,10 +1267,10 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>5</v>
@@ -1235,10 +1279,10 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>5</v>
@@ -1247,10 +1291,10 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>5</v>
@@ -1259,10 +1303,10 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>5</v>
@@ -1271,10 +1315,10 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C17" s="7" t="s">
         <v>5</v>
@@ -1283,10 +1327,10 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C18" s="7" t="s">
         <v>5</v>
@@ -1295,10 +1339,10 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C19" s="7" t="s">
         <v>5</v>
@@ -1307,10 +1351,10 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C20" s="7" t="s">
         <v>5</v>
@@ -1319,10 +1363,10 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C21" s="7" t="s">
         <v>5</v>
@@ -1331,10 +1375,10 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C22" s="7" t="s">
         <v>5</v>
@@ -1343,10 +1387,10 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C23" s="7" t="s">
         <v>5</v>
@@ -1355,10 +1399,10 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C24" s="7" t="s">
         <v>5</v>
@@ -1367,10 +1411,10 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C25" s="7" t="s">
         <v>5</v>
@@ -1379,10 +1423,10 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C26" s="7" t="s">
         <v>5</v>
@@ -1413,10 +1457,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C1" s="10" t="s">
         <v>2</v>
@@ -1427,10 +1471,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>5</v>
@@ -1439,10 +1483,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>5</v>
@@ -1451,10 +1495,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>5</v>
@@ -1463,10 +1507,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>5</v>
@@ -1475,10 +1519,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>5</v>
@@ -1487,10 +1531,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>5</v>
@@ -1499,10 +1543,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>5</v>
@@ -1511,10 +1555,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>5</v>
@@ -1523,10 +1567,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>5</v>
@@ -1535,10 +1579,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>5</v>
@@ -1547,10 +1591,10 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>5</v>
@@ -1559,10 +1603,10 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>5</v>
@@ -1571,10 +1615,10 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>5</v>
@@ -1583,10 +1627,10 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>5</v>
@@ -1595,10 +1639,10 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>5</v>
@@ -1607,10 +1651,10 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C17" s="7" t="s">
         <v>5</v>
@@ -1619,10 +1663,10 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C18" s="7" t="s">
         <v>5</v>
@@ -1631,10 +1675,10 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C19" s="7" t="s">
         <v>5</v>
@@ -1643,10 +1687,10 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C20" s="7" t="s">
         <v>5</v>
@@ -1655,10 +1699,10 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C21" s="7" t="s">
         <v>5</v>
@@ -1667,10 +1711,10 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C22" s="7" t="s">
         <v>5</v>
@@ -1679,10 +1723,10 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C23" s="7" t="s">
         <v>5</v>
@@ -1691,10 +1735,10 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C24" s="7" t="s">
         <v>5</v>
@@ -1703,10 +1747,10 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C25" s="7" t="s">
         <v>5</v>
@@ -1715,10 +1759,10 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C26" s="7" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
WAT new test case
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/WAT.xlsx
+++ b/src/test/resources/xls/WAT.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="103">
   <si>
     <t>TCID</t>
   </si>
@@ -316,6 +316,15 @@
   </si>
   <si>
     <t>WAT-142</t>
+  </si>
+  <si>
+    <t>WAT-548</t>
+  </si>
+  <si>
+    <t>WAT24</t>
+  </si>
+  <si>
+    <t>Verify that total search results should match with total publication results count</t>
   </si>
 </sst>
 </file>
@@ -745,10 +754,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1122,9 +1131,27 @@
       </c>
       <c r="E24" s="7"/>
     </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E25" s="7"/>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B25" r:id="rId1" display="http://ent.jira.int.thomsonreuters.com/browse/WAT-548"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Adds new testscript WAT40
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/WAT.xlsx
+++ b/src/test/resources/xls/WAT.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16980" windowHeight="3135"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="109">
   <si>
     <t>TCID</t>
   </si>
@@ -334,13 +334,22 @@
   </si>
   <si>
     <t>Verify that all static texts present in Author search page is displayed properly.</t>
+  </si>
+  <si>
+    <t>WAT40</t>
+  </si>
+  <si>
+    <t>WAT-147</t>
+  </si>
+  <si>
+    <t>Verify that FIND button will be disabled at the beginning.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -521,7 +530,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -553,9 +562,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -587,6 +597,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -762,14 +773,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="41" bestFit="1" customWidth="1" collapsed="1"/>
@@ -778,7 +789,7 @@
     <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -795,7 +806,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -810,7 +821,7 @@
       </c>
       <c r="E2" s="4"/>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -825,7 +836,7 @@
       </c>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>11</v>
       </c>
@@ -840,7 +851,7 @@
       </c>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>13</v>
       </c>
@@ -855,7 +866,7 @@
       </c>
       <c r="E5" s="7"/>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>15</v>
       </c>
@@ -870,7 +881,7 @@
       </c>
       <c r="E6" s="7"/>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>18</v>
       </c>
@@ -885,7 +896,7 @@
       </c>
       <c r="E7" s="7"/>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>21</v>
       </c>
@@ -900,7 +911,7 @@
       </c>
       <c r="E8" s="7"/>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>23</v>
       </c>
@@ -915,7 +926,7 @@
       </c>
       <c r="E9" s="7"/>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>24</v>
       </c>
@@ -930,7 +941,7 @@
       </c>
       <c r="E10" s="7"/>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>25</v>
       </c>
@@ -945,7 +956,7 @@
       </c>
       <c r="E11" s="7"/>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>26</v>
       </c>
@@ -960,7 +971,7 @@
       </c>
       <c r="E12" s="7"/>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>63</v>
       </c>
@@ -975,7 +986,7 @@
       </c>
       <c r="E13" s="7"/>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>64</v>
       </c>
@@ -990,7 +1001,7 @@
       </c>
       <c r="E14" s="7"/>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>65</v>
       </c>
@@ -1005,7 +1016,7 @@
       </c>
       <c r="E15" s="7"/>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>66</v>
       </c>
@@ -1020,7 +1031,7 @@
       </c>
       <c r="E16" s="7"/>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>75</v>
       </c>
@@ -1035,7 +1046,7 @@
       </c>
       <c r="E17" s="7"/>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>76</v>
       </c>
@@ -1050,7 +1061,7 @@
       </c>
       <c r="E18" s="7"/>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>80</v>
       </c>
@@ -1065,7 +1076,7 @@
       </c>
       <c r="E19" s="7"/>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>82</v>
       </c>
@@ -1080,7 +1091,7 @@
       </c>
       <c r="E20" s="7"/>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>83</v>
       </c>
@@ -1095,7 +1106,7 @@
       </c>
       <c r="E21" s="7"/>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>90</v>
       </c>
@@ -1110,7 +1121,7 @@
       </c>
       <c r="E22" s="7"/>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>92</v>
       </c>
@@ -1125,7 +1136,7 @@
       </c>
       <c r="E23" s="7"/>
     </row>
-    <row r="24" spans="1:5" ht="30">
+    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>96</v>
       </c>
@@ -1140,7 +1151,7 @@
       </c>
       <c r="E24" s="7"/>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>100</v>
       </c>
@@ -1155,7 +1166,7 @@
       </c>
       <c r="E25" s="7"/>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
         <v>102</v>
       </c>
@@ -1169,6 +1180,20 @@
         <v>5</v>
       </c>
       <c r="E26" s="7"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1180,14 +1205,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A19" sqref="A19:XFD19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
@@ -1195,7 +1220,7 @@
     <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>36</v>
       </c>
@@ -1209,7 +1234,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>38</v>
       </c>
@@ -1221,7 +1246,7 @@
       </c>
       <c r="D2" s="7"/>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>39</v>
       </c>
@@ -1233,7 +1258,7 @@
       </c>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>40</v>
       </c>
@@ -1245,7 +1270,7 @@
       </c>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>41</v>
       </c>
@@ -1257,7 +1282,7 @@
       </c>
       <c r="D5" s="7"/>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>42</v>
       </c>
@@ -1269,7 +1294,7 @@
       </c>
       <c r="D6" s="7"/>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>43</v>
       </c>
@@ -1281,7 +1306,7 @@
       </c>
       <c r="D7" s="7"/>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>44</v>
       </c>
@@ -1293,7 +1318,7 @@
       </c>
       <c r="D8" s="7"/>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>45</v>
       </c>
@@ -1305,7 +1330,7 @@
       </c>
       <c r="D9" s="7"/>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>46</v>
       </c>
@@ -1317,7 +1342,7 @@
       </c>
       <c r="D10" s="7"/>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>47</v>
       </c>
@@ -1329,7 +1354,7 @@
       </c>
       <c r="D11" s="7"/>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>48</v>
       </c>
@@ -1341,7 +1366,7 @@
       </c>
       <c r="D12" s="7"/>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>49</v>
       </c>
@@ -1353,7 +1378,7 @@
       </c>
       <c r="D13" s="7"/>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>50</v>
       </c>
@@ -1365,7 +1390,7 @@
       </c>
       <c r="D14" s="7"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>51</v>
       </c>
@@ -1377,7 +1402,7 @@
       </c>
       <c r="D15" s="7"/>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>52</v>
       </c>
@@ -1389,7 +1414,7 @@
       </c>
       <c r="D16" s="7"/>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>53</v>
       </c>
@@ -1401,7 +1426,7 @@
       </c>
       <c r="D17" s="7"/>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>54</v>
       </c>
@@ -1413,7 +1438,7 @@
       </c>
       <c r="D18" s="7"/>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>55</v>
       </c>
@@ -1425,7 +1450,7 @@
       </c>
       <c r="D19" s="7"/>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>56</v>
       </c>
@@ -1437,7 +1462,7 @@
       </c>
       <c r="D20" s="7"/>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>57</v>
       </c>
@@ -1449,7 +1474,7 @@
       </c>
       <c r="D21" s="7"/>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>58</v>
       </c>
@@ -1461,7 +1486,7 @@
       </c>
       <c r="D22" s="7"/>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>59</v>
       </c>
@@ -1473,7 +1498,7 @@
       </c>
       <c r="D23" s="7"/>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>60</v>
       </c>
@@ -1485,7 +1510,7 @@
       </c>
       <c r="D24" s="7"/>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>61</v>
       </c>
@@ -1497,7 +1522,7 @@
       </c>
       <c r="D25" s="7"/>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>62</v>
       </c>
@@ -1516,14 +1541,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A19" sqref="A19:XFD19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
@@ -1531,7 +1556,7 @@
     <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>36</v>
       </c>
@@ -1545,7 +1570,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>38</v>
       </c>
@@ -1557,7 +1582,7 @@
       </c>
       <c r="D2" s="7"/>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>39</v>
       </c>
@@ -1569,7 +1594,7 @@
       </c>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>40</v>
       </c>
@@ -1581,7 +1606,7 @@
       </c>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>41</v>
       </c>
@@ -1593,7 +1618,7 @@
       </c>
       <c r="D5" s="7"/>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>42</v>
       </c>
@@ -1605,7 +1630,7 @@
       </c>
       <c r="D6" s="7"/>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>43</v>
       </c>
@@ -1617,7 +1642,7 @@
       </c>
       <c r="D7" s="7"/>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>44</v>
       </c>
@@ -1629,7 +1654,7 @@
       </c>
       <c r="D8" s="7"/>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>45</v>
       </c>
@@ -1641,7 +1666,7 @@
       </c>
       <c r="D9" s="7"/>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>46</v>
       </c>
@@ -1653,7 +1678,7 @@
       </c>
       <c r="D10" s="7"/>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>47</v>
       </c>
@@ -1665,7 +1690,7 @@
       </c>
       <c r="D11" s="7"/>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>48</v>
       </c>
@@ -1677,7 +1702,7 @@
       </c>
       <c r="D12" s="7"/>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>49</v>
       </c>
@@ -1689,7 +1714,7 @@
       </c>
       <c r="D13" s="7"/>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>50</v>
       </c>
@@ -1701,7 +1726,7 @@
       </c>
       <c r="D14" s="7"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>51</v>
       </c>
@@ -1713,7 +1738,7 @@
       </c>
       <c r="D15" s="7"/>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>52</v>
       </c>
@@ -1725,7 +1750,7 @@
       </c>
       <c r="D16" s="7"/>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>53</v>
       </c>
@@ -1737,7 +1762,7 @@
       </c>
       <c r="D17" s="7"/>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>54</v>
       </c>
@@ -1749,7 +1774,7 @@
       </c>
       <c r="D18" s="7"/>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>55</v>
       </c>
@@ -1761,7 +1786,7 @@
       </c>
       <c r="D19" s="7"/>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>56</v>
       </c>
@@ -1773,7 +1798,7 @@
       </c>
       <c r="D20" s="7"/>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>57</v>
       </c>
@@ -1785,7 +1810,7 @@
       </c>
       <c r="D21" s="7"/>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>58</v>
       </c>
@@ -1797,7 +1822,7 @@
       </c>
       <c r="D22" s="7"/>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>59</v>
       </c>
@@ -1809,7 +1834,7 @@
       </c>
       <c r="D23" s="7"/>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>60</v>
       </c>
@@ -1821,7 +1846,7 @@
       </c>
       <c r="D24" s="7"/>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>61</v>
       </c>
@@ -1833,7 +1858,7 @@
       </c>
       <c r="D25" s="7"/>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>62</v>
       </c>

</xml_diff>

<commit_message>
Adds new testscript WAT41
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/WAT.xlsx
+++ b/src/test/resources/xls/WAT.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="112">
   <si>
     <t>TCID</t>
   </si>
@@ -343,6 +343,15 @@
   </si>
   <si>
     <t>Verify that FIND button will be disabled at the beginning.</t>
+  </si>
+  <si>
+    <t>WAT41</t>
+  </si>
+  <si>
+    <t>WAT-194</t>
+  </si>
+  <si>
+    <t>Verify that "Select a country/territory where this author has published." is mentioned on top of country dropdown</t>
   </si>
 </sst>
 </file>
@@ -774,10 +783,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="E28" sqref="A1:E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1194,6 +1203,22 @@
       <c r="D27" s="7" t="s">
         <v>5</v>
       </c>
+      <c r="E27" s="7"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E28" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Adds new testscript WAT42
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/WAT.xlsx
+++ b/src/test/resources/xls/WAT.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="114">
   <si>
     <t>TCID</t>
   </si>
@@ -352,6 +352,12 @@
   </si>
   <si>
     <t>Verify that "Select a country/territory where this author has published." is mentioned on top of country dropdown</t>
+  </si>
+  <si>
+    <t>WAT42</t>
+  </si>
+  <si>
+    <t>Verify that "Select an organization where this author has published." is mentioned on top of org list dropdown</t>
   </si>
 </sst>
 </file>
@@ -783,10 +789,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E28" sqref="A1:E28"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1219,6 +1225,21 @@
         <v>5</v>
       </c>
       <c r="E28" s="7"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E29" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Adds new testscript WAT43
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/WAT.xlsx
+++ b/src/test/resources/xls/WAT.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="118">
   <si>
     <t>TCID</t>
   </si>
@@ -358,6 +358,19 @@
   </si>
   <si>
     <t>Verify that "Select an organization where this author has published." is mentioned on top of org list dropdown</t>
+  </si>
+  <si>
+    <t>WAT43</t>
+  </si>
+  <si>
+    <t>WAT-207</t>
+  </si>
+  <si>
+    <t>Verify that, If system retrieves only one country and only one organization
+System must directly display the results in search results page if the search result count is less than 50.</t>
+  </si>
+  <si>
+    <t>WAT-197</t>
   </si>
 </sst>
 </file>
@@ -789,10 +802,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1231,7 +1244,7 @@
         <v>112</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="C29" s="11" t="s">
         <v>113</v>
@@ -1240,6 +1253,21 @@
         <v>5</v>
       </c>
       <c r="E29" s="7"/>
+    </row>
+    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E30" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Adds new testscript WAT44, WAT45
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/WAT.xlsx
+++ b/src/test/resources/xls/WAT.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16980" windowHeight="3135"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="127">
   <si>
     <t>TCID</t>
   </si>
@@ -380,13 +380,31 @@
   </si>
   <si>
     <t>WAT-142||WAT-153</t>
+  </si>
+  <si>
+    <t>WAT44</t>
+  </si>
+  <si>
+    <t>WAT45</t>
+  </si>
+  <si>
+    <t>WAT-203</t>
+  </si>
+  <si>
+    <t>Verify the consistent presence of LOGO at the top left of page.</t>
+  </si>
+  <si>
+    <t>Verify that clicking on the LOGO navigates the user to http://clarivate.com/</t>
+  </si>
+  <si>
+    <t>WAT-211</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -567,7 +585,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -599,9 +617,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -633,6 +652,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -808,14 +828,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="L43" sqref="L43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="41" bestFit="1" customWidth="1" collapsed="1"/>
@@ -824,7 +844,7 @@
     <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -841,7 +861,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -856,7 +876,7 @@
       </c>
       <c r="E2" s="4"/>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -871,7 +891,7 @@
       </c>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>11</v>
       </c>
@@ -886,7 +906,7 @@
       </c>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>13</v>
       </c>
@@ -901,7 +921,7 @@
       </c>
       <c r="E5" s="7"/>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>15</v>
       </c>
@@ -916,7 +936,7 @@
       </c>
       <c r="E6" s="7"/>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>18</v>
       </c>
@@ -931,7 +951,7 @@
       </c>
       <c r="E7" s="7"/>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>21</v>
       </c>
@@ -946,7 +966,7 @@
       </c>
       <c r="E8" s="7"/>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>23</v>
       </c>
@@ -961,7 +981,7 @@
       </c>
       <c r="E9" s="7"/>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>24</v>
       </c>
@@ -976,7 +996,7 @@
       </c>
       <c r="E10" s="7"/>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>25</v>
       </c>
@@ -991,7 +1011,7 @@
       </c>
       <c r="E11" s="7"/>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>26</v>
       </c>
@@ -1006,7 +1026,7 @@
       </c>
       <c r="E12" s="7"/>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>63</v>
       </c>
@@ -1021,7 +1041,7 @@
       </c>
       <c r="E13" s="7"/>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>64</v>
       </c>
@@ -1036,7 +1056,7 @@
       </c>
       <c r="E14" s="7"/>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>65</v>
       </c>
@@ -1051,7 +1071,7 @@
       </c>
       <c r="E15" s="7"/>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>66</v>
       </c>
@@ -1066,7 +1086,7 @@
       </c>
       <c r="E16" s="7"/>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>75</v>
       </c>
@@ -1081,7 +1101,7 @@
       </c>
       <c r="E17" s="7"/>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>76</v>
       </c>
@@ -1096,7 +1116,7 @@
       </c>
       <c r="E18" s="7"/>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>80</v>
       </c>
@@ -1111,7 +1131,7 @@
       </c>
       <c r="E19" s="7"/>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>82</v>
       </c>
@@ -1126,7 +1146,7 @@
       </c>
       <c r="E20" s="7"/>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>83</v>
       </c>
@@ -1141,7 +1161,7 @@
       </c>
       <c r="E21" s="7"/>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>90</v>
       </c>
@@ -1156,7 +1176,7 @@
       </c>
       <c r="E22" s="7"/>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>92</v>
       </c>
@@ -1171,7 +1191,7 @@
       </c>
       <c r="E23" s="7"/>
     </row>
-    <row r="24" spans="1:5" ht="30">
+    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>96</v>
       </c>
@@ -1186,7 +1206,7 @@
       </c>
       <c r="E24" s="7"/>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>98</v>
       </c>
@@ -1201,7 +1221,7 @@
       </c>
       <c r="E25" s="7"/>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
         <v>100</v>
       </c>
@@ -1216,7 +1236,7 @@
       </c>
       <c r="E26" s="7"/>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
         <v>104</v>
       </c>
@@ -1231,7 +1251,7 @@
       </c>
       <c r="E27" s="7"/>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
         <v>107</v>
       </c>
@@ -1246,7 +1266,7 @@
       </c>
       <c r="E28" s="7"/>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
         <v>110</v>
       </c>
@@ -1261,7 +1281,7 @@
       </c>
       <c r="E29" s="7"/>
     </row>
-    <row r="30" spans="1:5" ht="30">
+    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
         <v>112</v>
       </c>
@@ -1276,7 +1296,7 @@
       </c>
       <c r="E30" s="7"/>
     </row>
-    <row r="31" spans="1:5" ht="30">
+    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
         <v>116</v>
       </c>
@@ -1290,6 +1310,36 @@
         <v>5</v>
       </c>
       <c r="E31" s="7"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E32" s="7"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E33" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1301,14 +1351,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A19" sqref="A19:XFD19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
@@ -1316,7 +1366,7 @@
     <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>36</v>
       </c>
@@ -1330,7 +1380,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>38</v>
       </c>
@@ -1342,7 +1392,7 @@
       </c>
       <c r="D2" s="7"/>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>39</v>
       </c>
@@ -1354,7 +1404,7 @@
       </c>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>40</v>
       </c>
@@ -1366,7 +1416,7 @@
       </c>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>41</v>
       </c>
@@ -1378,7 +1428,7 @@
       </c>
       <c r="D5" s="7"/>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>42</v>
       </c>
@@ -1390,7 +1440,7 @@
       </c>
       <c r="D6" s="7"/>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>43</v>
       </c>
@@ -1402,7 +1452,7 @@
       </c>
       <c r="D7" s="7"/>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>44</v>
       </c>
@@ -1414,7 +1464,7 @@
       </c>
       <c r="D8" s="7"/>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>45</v>
       </c>
@@ -1426,7 +1476,7 @@
       </c>
       <c r="D9" s="7"/>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>46</v>
       </c>
@@ -1438,7 +1488,7 @@
       </c>
       <c r="D10" s="7"/>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>47</v>
       </c>
@@ -1450,7 +1500,7 @@
       </c>
       <c r="D11" s="7"/>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>48</v>
       </c>
@@ -1462,7 +1512,7 @@
       </c>
       <c r="D12" s="7"/>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>49</v>
       </c>
@@ -1474,7 +1524,7 @@
       </c>
       <c r="D13" s="7"/>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>50</v>
       </c>
@@ -1486,7 +1536,7 @@
       </c>
       <c r="D14" s="7"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>51</v>
       </c>
@@ -1498,7 +1548,7 @@
       </c>
       <c r="D15" s="7"/>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>52</v>
       </c>
@@ -1510,7 +1560,7 @@
       </c>
       <c r="D16" s="7"/>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>53</v>
       </c>
@@ -1522,7 +1572,7 @@
       </c>
       <c r="D17" s="7"/>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>54</v>
       </c>
@@ -1534,7 +1584,7 @@
       </c>
       <c r="D18" s="7"/>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>55</v>
       </c>
@@ -1546,7 +1596,7 @@
       </c>
       <c r="D19" s="7"/>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>56</v>
       </c>
@@ -1558,7 +1608,7 @@
       </c>
       <c r="D20" s="7"/>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>57</v>
       </c>
@@ -1570,7 +1620,7 @@
       </c>
       <c r="D21" s="7"/>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>58</v>
       </c>
@@ -1582,7 +1632,7 @@
       </c>
       <c r="D22" s="7"/>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>59</v>
       </c>
@@ -1594,7 +1644,7 @@
       </c>
       <c r="D23" s="7"/>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>60</v>
       </c>
@@ -1606,7 +1656,7 @@
       </c>
       <c r="D24" s="7"/>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>61</v>
       </c>
@@ -1618,7 +1668,7 @@
       </c>
       <c r="D25" s="7"/>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>62</v>
       </c>
@@ -1637,14 +1687,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A19" sqref="A19:XFD19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
@@ -1652,7 +1702,7 @@
     <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>36</v>
       </c>
@@ -1666,7 +1716,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>38</v>
       </c>
@@ -1678,7 +1728,7 @@
       </c>
       <c r="D2" s="7"/>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>39</v>
       </c>
@@ -1690,7 +1740,7 @@
       </c>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>40</v>
       </c>
@@ -1702,7 +1752,7 @@
       </c>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>41</v>
       </c>
@@ -1714,7 +1764,7 @@
       </c>
       <c r="D5" s="7"/>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>42</v>
       </c>
@@ -1726,7 +1776,7 @@
       </c>
       <c r="D6" s="7"/>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>43</v>
       </c>
@@ -1738,7 +1788,7 @@
       </c>
       <c r="D7" s="7"/>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>44</v>
       </c>
@@ -1750,7 +1800,7 @@
       </c>
       <c r="D8" s="7"/>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>45</v>
       </c>
@@ -1762,7 +1812,7 @@
       </c>
       <c r="D9" s="7"/>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>46</v>
       </c>
@@ -1774,7 +1824,7 @@
       </c>
       <c r="D10" s="7"/>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>47</v>
       </c>
@@ -1786,7 +1836,7 @@
       </c>
       <c r="D11" s="7"/>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>48</v>
       </c>
@@ -1798,7 +1848,7 @@
       </c>
       <c r="D12" s="7"/>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>49</v>
       </c>
@@ -1810,7 +1860,7 @@
       </c>
       <c r="D13" s="7"/>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>50</v>
       </c>
@@ -1822,7 +1872,7 @@
       </c>
       <c r="D14" s="7"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>51</v>
       </c>
@@ -1834,7 +1884,7 @@
       </c>
       <c r="D15" s="7"/>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>52</v>
       </c>
@@ -1846,7 +1896,7 @@
       </c>
       <c r="D16" s="7"/>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>53</v>
       </c>
@@ -1858,7 +1908,7 @@
       </c>
       <c r="D17" s="7"/>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>54</v>
       </c>
@@ -1870,7 +1920,7 @@
       </c>
       <c r="D18" s="7"/>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>55</v>
       </c>
@@ -1882,7 +1932,7 @@
       </c>
       <c r="D19" s="7"/>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>56</v>
       </c>
@@ -1894,7 +1944,7 @@
       </c>
       <c r="D20" s="7"/>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>57</v>
       </c>
@@ -1906,7 +1956,7 @@
       </c>
       <c r="D21" s="7"/>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>58</v>
       </c>
@@ -1918,7 +1968,7 @@
       </c>
       <c r="D22" s="7"/>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>59</v>
       </c>
@@ -1930,7 +1980,7 @@
       </c>
       <c r="D23" s="7"/>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>60</v>
       </c>
@@ -1942,7 +1992,7 @@
       </c>
       <c r="D24" s="7"/>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>61</v>
       </c>
@@ -1954,7 +2004,7 @@
       </c>
       <c r="D25" s="7"/>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>62</v>
       </c>

</xml_diff>

<commit_message>
Adds new testscript WAT46
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/WAT.xlsx
+++ b/src/test/resources/xls/WAT.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="130">
   <si>
     <t>TCID</t>
   </si>
@@ -398,6 +398,15 @@
   </si>
   <si>
     <t>WAT-211</t>
+  </si>
+  <si>
+    <t>WAT46</t>
+  </si>
+  <si>
+    <t>Verify that user should be able to view profile details by clicking on the profile pic button top right corner.</t>
+  </si>
+  <si>
+    <t>WAT-161</t>
   </si>
 </sst>
 </file>
@@ -829,10 +838,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="L43" sqref="L43"/>
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1340,6 +1349,21 @@
         <v>5</v>
       </c>
       <c r="E33" s="7"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E34" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
new wat script implementation
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/WAT.xlsx
+++ b/src/test/resources/xls/WAT.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="139">
   <si>
     <t>TCID</t>
   </si>
@@ -425,6 +425,15 @@
   </si>
   <si>
     <t>WAT-196</t>
+  </si>
+  <si>
+    <t>WAT29</t>
+  </si>
+  <si>
+    <t>Verify that System must display "Top Journals" section listing a maximum of three journal titles.</t>
+  </si>
+  <si>
+    <t>WAT-199</t>
   </si>
 </sst>
 </file>
@@ -854,10 +863,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E36"/>
+  <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1410,6 +1419,21 @@
         <v>5</v>
       </c>
       <c r="E36" s="7"/>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="D37" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E37" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Adds new testscript WAT47
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/WAT.xlsx
+++ b/src/test/resources/xls/WAT.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16980" windowHeight="3135"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="142">
   <si>
     <t>TCID</t>
   </si>
@@ -434,13 +434,22 @@
   </si>
   <si>
     <t>WAT-199</t>
+  </si>
+  <si>
+    <t>WAT47</t>
+  </si>
+  <si>
+    <t>Verify that when error msg "No Result" is displayed,  Add alternate name should be disabled</t>
+  </si>
+  <si>
+    <t>WAT-159</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -621,7 +630,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -653,9 +662,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -687,6 +697,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -862,14 +873,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E37"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E38" sqref="A1:E38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="41" bestFit="1" customWidth="1" collapsed="1"/>
@@ -878,7 +889,7 @@
     <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -895,7 +906,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -910,7 +921,7 @@
       </c>
       <c r="E2" s="4"/>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -925,7 +936,7 @@
       </c>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>11</v>
       </c>
@@ -940,7 +951,7 @@
       </c>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>13</v>
       </c>
@@ -955,7 +966,7 @@
       </c>
       <c r="E5" s="7"/>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>15</v>
       </c>
@@ -970,7 +981,7 @@
       </c>
       <c r="E6" s="7"/>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>18</v>
       </c>
@@ -985,7 +996,7 @@
       </c>
       <c r="E7" s="7"/>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>21</v>
       </c>
@@ -1000,7 +1011,7 @@
       </c>
       <c r="E8" s="7"/>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>23</v>
       </c>
@@ -1015,7 +1026,7 @@
       </c>
       <c r="E9" s="7"/>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>24</v>
       </c>
@@ -1030,7 +1041,7 @@
       </c>
       <c r="E10" s="7"/>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>25</v>
       </c>
@@ -1045,7 +1056,7 @@
       </c>
       <c r="E11" s="7"/>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>26</v>
       </c>
@@ -1060,7 +1071,7 @@
       </c>
       <c r="E12" s="7"/>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>63</v>
       </c>
@@ -1075,7 +1086,7 @@
       </c>
       <c r="E13" s="7"/>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>64</v>
       </c>
@@ -1090,7 +1101,7 @@
       </c>
       <c r="E14" s="7"/>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>65</v>
       </c>
@@ -1105,7 +1116,7 @@
       </c>
       <c r="E15" s="7"/>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>66</v>
       </c>
@@ -1120,7 +1131,7 @@
       </c>
       <c r="E16" s="7"/>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>75</v>
       </c>
@@ -1135,7 +1146,7 @@
       </c>
       <c r="E17" s="7"/>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>76</v>
       </c>
@@ -1150,7 +1161,7 @@
       </c>
       <c r="E18" s="7"/>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>80</v>
       </c>
@@ -1165,7 +1176,7 @@
       </c>
       <c r="E19" s="7"/>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>82</v>
       </c>
@@ -1180,7 +1191,7 @@
       </c>
       <c r="E20" s="7"/>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>83</v>
       </c>
@@ -1195,7 +1206,7 @@
       </c>
       <c r="E21" s="7"/>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>90</v>
       </c>
@@ -1210,7 +1221,7 @@
       </c>
       <c r="E22" s="7"/>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>92</v>
       </c>
@@ -1225,7 +1236,7 @@
       </c>
       <c r="E23" s="7"/>
     </row>
-    <row r="24" spans="1:5" ht="30">
+    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>96</v>
       </c>
@@ -1240,7 +1251,7 @@
       </c>
       <c r="E24" s="7"/>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>98</v>
       </c>
@@ -1255,7 +1266,7 @@
       </c>
       <c r="E25" s="7"/>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
         <v>100</v>
       </c>
@@ -1270,7 +1281,7 @@
       </c>
       <c r="E26" s="7"/>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
         <v>104</v>
       </c>
@@ -1285,7 +1296,7 @@
       </c>
       <c r="E27" s="7"/>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
         <v>107</v>
       </c>
@@ -1300,7 +1311,7 @@
       </c>
       <c r="E28" s="7"/>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
         <v>110</v>
       </c>
@@ -1315,7 +1326,7 @@
       </c>
       <c r="E29" s="7"/>
     </row>
-    <row r="30" spans="1:5" ht="30">
+    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
         <v>112</v>
       </c>
@@ -1330,7 +1341,7 @@
       </c>
       <c r="E30" s="7"/>
     </row>
-    <row r="31" spans="1:5" ht="30">
+    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
         <v>116</v>
       </c>
@@ -1345,7 +1356,7 @@
       </c>
       <c r="E31" s="7"/>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
         <v>121</v>
       </c>
@@ -1360,7 +1371,7 @@
       </c>
       <c r="E32" s="7"/>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
         <v>122</v>
       </c>
@@ -1375,7 +1386,7 @@
       </c>
       <c r="E33" s="7"/>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
         <v>127</v>
       </c>
@@ -1390,7 +1401,7 @@
       </c>
       <c r="E34" s="7"/>
     </row>
-    <row r="35" spans="1:5" ht="30">
+    <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
         <v>130</v>
       </c>
@@ -1405,7 +1416,7 @@
       </c>
       <c r="E35" s="7"/>
     </row>
-    <row r="36" spans="1:5" ht="30">
+    <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
         <v>133</v>
       </c>
@@ -1420,7 +1431,7 @@
       </c>
       <c r="E36" s="7"/>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
         <v>136</v>
       </c>
@@ -1434,6 +1445,21 @@
         <v>5</v>
       </c>
       <c r="E37" s="7"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="D38" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E38" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1445,14 +1471,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A19" sqref="A19:XFD19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
@@ -1460,7 +1486,7 @@
     <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>36</v>
       </c>
@@ -1474,7 +1500,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>38</v>
       </c>
@@ -1486,7 +1512,7 @@
       </c>
       <c r="D2" s="7"/>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>39</v>
       </c>
@@ -1498,7 +1524,7 @@
       </c>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>40</v>
       </c>
@@ -1510,7 +1536,7 @@
       </c>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>41</v>
       </c>
@@ -1522,7 +1548,7 @@
       </c>
       <c r="D5" s="7"/>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>42</v>
       </c>
@@ -1534,7 +1560,7 @@
       </c>
       <c r="D6" s="7"/>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>43</v>
       </c>
@@ -1546,7 +1572,7 @@
       </c>
       <c r="D7" s="7"/>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>44</v>
       </c>
@@ -1558,7 +1584,7 @@
       </c>
       <c r="D8" s="7"/>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>45</v>
       </c>
@@ -1570,7 +1596,7 @@
       </c>
       <c r="D9" s="7"/>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>46</v>
       </c>
@@ -1582,7 +1608,7 @@
       </c>
       <c r="D10" s="7"/>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>47</v>
       </c>
@@ -1594,7 +1620,7 @@
       </c>
       <c r="D11" s="7"/>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>48</v>
       </c>
@@ -1606,7 +1632,7 @@
       </c>
       <c r="D12" s="7"/>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>49</v>
       </c>
@@ -1618,7 +1644,7 @@
       </c>
       <c r="D13" s="7"/>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>50</v>
       </c>
@@ -1630,7 +1656,7 @@
       </c>
       <c r="D14" s="7"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>51</v>
       </c>
@@ -1642,7 +1668,7 @@
       </c>
       <c r="D15" s="7"/>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>52</v>
       </c>
@@ -1654,7 +1680,7 @@
       </c>
       <c r="D16" s="7"/>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>53</v>
       </c>
@@ -1666,7 +1692,7 @@
       </c>
       <c r="D17" s="7"/>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>54</v>
       </c>
@@ -1678,7 +1704,7 @@
       </c>
       <c r="D18" s="7"/>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>55</v>
       </c>
@@ -1690,7 +1716,7 @@
       </c>
       <c r="D19" s="7"/>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>56</v>
       </c>
@@ -1702,7 +1728,7 @@
       </c>
       <c r="D20" s="7"/>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>57</v>
       </c>
@@ -1714,7 +1740,7 @@
       </c>
       <c r="D21" s="7"/>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>58</v>
       </c>
@@ -1726,7 +1752,7 @@
       </c>
       <c r="D22" s="7"/>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>59</v>
       </c>
@@ -1738,7 +1764,7 @@
       </c>
       <c r="D23" s="7"/>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>60</v>
       </c>
@@ -1750,7 +1776,7 @@
       </c>
       <c r="D24" s="7"/>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>61</v>
       </c>
@@ -1762,7 +1788,7 @@
       </c>
       <c r="D25" s="7"/>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>62</v>
       </c>
@@ -1781,14 +1807,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A19" sqref="A19:XFD19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
@@ -1796,7 +1822,7 @@
     <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>36</v>
       </c>
@@ -1810,7 +1836,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>38</v>
       </c>
@@ -1822,7 +1848,7 @@
       </c>
       <c r="D2" s="7"/>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>39</v>
       </c>
@@ -1834,7 +1860,7 @@
       </c>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>40</v>
       </c>
@@ -1846,7 +1872,7 @@
       </c>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>41</v>
       </c>
@@ -1858,7 +1884,7 @@
       </c>
       <c r="D5" s="7"/>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>42</v>
       </c>
@@ -1870,7 +1896,7 @@
       </c>
       <c r="D6" s="7"/>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>43</v>
       </c>
@@ -1882,7 +1908,7 @@
       </c>
       <c r="D7" s="7"/>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>44</v>
       </c>
@@ -1894,7 +1920,7 @@
       </c>
       <c r="D8" s="7"/>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>45</v>
       </c>
@@ -1906,7 +1932,7 @@
       </c>
       <c r="D9" s="7"/>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>46</v>
       </c>
@@ -1918,7 +1944,7 @@
       </c>
       <c r="D10" s="7"/>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>47</v>
       </c>
@@ -1930,7 +1956,7 @@
       </c>
       <c r="D11" s="7"/>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>48</v>
       </c>
@@ -1942,7 +1968,7 @@
       </c>
       <c r="D12" s="7"/>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>49</v>
       </c>
@@ -1954,7 +1980,7 @@
       </c>
       <c r="D13" s="7"/>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>50</v>
       </c>
@@ -1966,7 +1992,7 @@
       </c>
       <c r="D14" s="7"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>51</v>
       </c>
@@ -1978,7 +2004,7 @@
       </c>
       <c r="D15" s="7"/>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>52</v>
       </c>
@@ -1990,7 +2016,7 @@
       </c>
       <c r="D16" s="7"/>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>53</v>
       </c>
@@ -2002,7 +2028,7 @@
       </c>
       <c r="D17" s="7"/>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>54</v>
       </c>
@@ -2014,7 +2040,7 @@
       </c>
       <c r="D18" s="7"/>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>55</v>
       </c>
@@ -2026,7 +2052,7 @@
       </c>
       <c r="D19" s="7"/>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>56</v>
       </c>
@@ -2038,7 +2064,7 @@
       </c>
       <c r="D20" s="7"/>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>57</v>
       </c>
@@ -2050,7 +2076,7 @@
       </c>
       <c r="D21" s="7"/>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>58</v>
       </c>
@@ -2062,7 +2088,7 @@
       </c>
       <c r="D22" s="7"/>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>59</v>
       </c>
@@ -2074,7 +2100,7 @@
       </c>
       <c r="D23" s="7"/>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>60</v>
       </c>
@@ -2086,7 +2112,7 @@
       </c>
       <c r="D24" s="7"/>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>61</v>
       </c>
@@ -2098,7 +2124,7 @@
       </c>
       <c r="D25" s="7"/>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>62</v>
       </c>

</xml_diff>

<commit_message>
Adds new test scripts WAT48 and WAT 49
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/WAT.xlsx
+++ b/src/test/resources/xls/WAT.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="148">
   <si>
     <t>TCID</t>
   </si>
@@ -443,6 +443,24 @@
   </si>
   <si>
     <t>WAT-159</t>
+  </si>
+  <si>
+    <t>WAT48</t>
+  </si>
+  <si>
+    <t>Verify that upon clicking ORCiD tab, Orcid search field should be displayed with an example of orcid number</t>
+  </si>
+  <si>
+    <t>WAT-323</t>
+  </si>
+  <si>
+    <t>WAT-558</t>
+  </si>
+  <si>
+    <t>WAT49</t>
+  </si>
+  <si>
+    <t>Verify that FIND button in ORCid Search page is disabled at the beginning.</t>
   </si>
 </sst>
 </file>
@@ -874,10 +892,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E38"/>
+  <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E38" sqref="A1:E38"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G58" sqref="G58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1460,6 +1478,36 @@
         <v>5</v>
       </c>
       <c r="E38" s="7"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="C39" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="D39" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E39" s="7"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="B40" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="C40" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="D40" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E40" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Adds new test script WAT50
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/WAT.xlsx
+++ b/src/test/resources/xls/WAT.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="151">
   <si>
     <t>TCID</t>
   </si>
@@ -461,6 +461,15 @@
   </si>
   <si>
     <t>Verify that FIND button in ORCid Search page is disabled at the beginning.</t>
+  </si>
+  <si>
+    <t>WAT50</t>
+  </si>
+  <si>
+    <t>WAT-333</t>
+  </si>
+  <si>
+    <t>Verify that error "Please enter a valid ORCiD number or try the Name Search" is displayed when there is no search result available for a correctly formatted ORCiD.</t>
   </si>
 </sst>
 </file>
@@ -510,7 +519,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -533,11 +542,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -560,6 +580,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -892,10 +913,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E40"/>
+  <dimension ref="A1:E41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A26" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G58" sqref="G58"/>
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1508,6 +1529,20 @@
         <v>5</v>
       </c>
       <c r="E40" s="7"/>
+    </row>
+    <row r="41" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A41" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="B41" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="C41" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="D41" s="12" t="s">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Adds new test script WAT51
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/WAT.xlsx
+++ b/src/test/resources/xls/WAT.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16980" windowHeight="3135"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="160">
   <si>
     <t>TCID</t>
   </si>
@@ -488,13 +488,22 @@
   </si>
   <si>
     <t>Verify that system must display Author search results in default sort order (sorted by relevance) when user click on 'Find' button</t>
+  </si>
+  <si>
+    <t>WAT51</t>
+  </si>
+  <si>
+    <t>WAT-561</t>
+  </si>
+  <si>
+    <t>Verify that user is able to search for an Author cluster using ORCid search</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -675,7 +684,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -707,9 +716,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -741,6 +751,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -916,14 +927,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E43"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A26" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="41" bestFit="1" customWidth="1" collapsed="1"/>
@@ -932,7 +943,7 @@
     <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -949,7 +960,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -964,7 +975,7 @@
       </c>
       <c r="E2" s="4"/>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -979,7 +990,7 @@
       </c>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>11</v>
       </c>
@@ -994,7 +1005,7 @@
       </c>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>13</v>
       </c>
@@ -1009,7 +1020,7 @@
       </c>
       <c r="E5" s="7"/>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>15</v>
       </c>
@@ -1024,7 +1035,7 @@
       </c>
       <c r="E6" s="7"/>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>18</v>
       </c>
@@ -1039,7 +1050,7 @@
       </c>
       <c r="E7" s="7"/>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>21</v>
       </c>
@@ -1054,7 +1065,7 @@
       </c>
       <c r="E8" s="7"/>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>23</v>
       </c>
@@ -1069,7 +1080,7 @@
       </c>
       <c r="E9" s="7"/>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>24</v>
       </c>
@@ -1084,7 +1095,7 @@
       </c>
       <c r="E10" s="7"/>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>25</v>
       </c>
@@ -1099,7 +1110,7 @@
       </c>
       <c r="E11" s="7"/>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>26</v>
       </c>
@@ -1114,7 +1125,7 @@
       </c>
       <c r="E12" s="7"/>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>63</v>
       </c>
@@ -1129,7 +1140,7 @@
       </c>
       <c r="E13" s="7"/>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>64</v>
       </c>
@@ -1144,7 +1155,7 @@
       </c>
       <c r="E14" s="7"/>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>65</v>
       </c>
@@ -1159,7 +1170,7 @@
       </c>
       <c r="E15" s="7"/>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>66</v>
       </c>
@@ -1174,7 +1185,7 @@
       </c>
       <c r="E16" s="7"/>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>75</v>
       </c>
@@ -1189,7 +1200,7 @@
       </c>
       <c r="E17" s="7"/>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>76</v>
       </c>
@@ -1204,7 +1215,7 @@
       </c>
       <c r="E18" s="7"/>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>80</v>
       </c>
@@ -1219,7 +1230,7 @@
       </c>
       <c r="E19" s="7"/>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>82</v>
       </c>
@@ -1234,7 +1245,7 @@
       </c>
       <c r="E20" s="7"/>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>83</v>
       </c>
@@ -1249,7 +1260,7 @@
       </c>
       <c r="E21" s="7"/>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>90</v>
       </c>
@@ -1264,7 +1275,7 @@
       </c>
       <c r="E22" s="7"/>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>92</v>
       </c>
@@ -1279,7 +1290,7 @@
       </c>
       <c r="E23" s="7"/>
     </row>
-    <row r="24" spans="1:5" ht="30">
+    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>96</v>
       </c>
@@ -1294,7 +1305,7 @@
       </c>
       <c r="E24" s="7"/>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>98</v>
       </c>
@@ -1309,7 +1320,7 @@
       </c>
       <c r="E25" s="7"/>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
         <v>100</v>
       </c>
@@ -1324,7 +1335,7 @@
       </c>
       <c r="E26" s="7"/>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
         <v>104</v>
       </c>
@@ -1339,7 +1350,7 @@
       </c>
       <c r="E27" s="7"/>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
         <v>107</v>
       </c>
@@ -1354,7 +1365,7 @@
       </c>
       <c r="E28" s="7"/>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
         <v>110</v>
       </c>
@@ -1369,7 +1380,7 @@
       </c>
       <c r="E29" s="7"/>
     </row>
-    <row r="30" spans="1:5" ht="30">
+    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
         <v>112</v>
       </c>
@@ -1384,7 +1395,7 @@
       </c>
       <c r="E30" s="7"/>
     </row>
-    <row r="31" spans="1:5" ht="30">
+    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
         <v>116</v>
       </c>
@@ -1399,7 +1410,7 @@
       </c>
       <c r="E31" s="7"/>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
         <v>121</v>
       </c>
@@ -1414,7 +1425,7 @@
       </c>
       <c r="E32" s="7"/>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
         <v>122</v>
       </c>
@@ -1429,7 +1440,7 @@
       </c>
       <c r="E33" s="7"/>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
         <v>127</v>
       </c>
@@ -1444,7 +1455,7 @@
       </c>
       <c r="E34" s="7"/>
     </row>
-    <row r="35" spans="1:5" ht="30">
+    <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
         <v>130</v>
       </c>
@@ -1459,7 +1470,7 @@
       </c>
       <c r="E35" s="7"/>
     </row>
-    <row r="36" spans="1:5" ht="30">
+    <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
         <v>133</v>
       </c>
@@ -1474,7 +1485,7 @@
       </c>
       <c r="E36" s="7"/>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
         <v>136</v>
       </c>
@@ -1489,7 +1500,7 @@
       </c>
       <c r="E37" s="7"/>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="9" t="s">
         <v>139</v>
       </c>
@@ -1504,7 +1515,7 @@
       </c>
       <c r="E38" s="7"/>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="s">
         <v>142</v>
       </c>
@@ -1519,7 +1530,7 @@
       </c>
       <c r="E39" s="7"/>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="9" t="s">
         <v>146</v>
       </c>
@@ -1534,7 +1545,7 @@
       </c>
       <c r="E40" s="7"/>
     </row>
-    <row r="41" spans="1:5" ht="30">
+    <row r="41" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
         <v>148</v>
       </c>
@@ -1549,7 +1560,7 @@
       </c>
       <c r="E41" s="7"/>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="9" t="s">
         <v>151</v>
       </c>
@@ -1564,7 +1575,7 @@
       </c>
       <c r="E42" s="7"/>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="9" t="s">
         <v>154</v>
       </c>
@@ -1578,6 +1589,21 @@
         <v>5</v>
       </c>
       <c r="E43" s="7"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="C44" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="D44" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E44" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1589,14 +1615,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A19" sqref="A19:XFD19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
@@ -1604,7 +1630,7 @@
     <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>36</v>
       </c>
@@ -1618,7 +1644,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>38</v>
       </c>
@@ -1630,7 +1656,7 @@
       </c>
       <c r="D2" s="7"/>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>39</v>
       </c>
@@ -1642,7 +1668,7 @@
       </c>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>40</v>
       </c>
@@ -1654,7 +1680,7 @@
       </c>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>41</v>
       </c>
@@ -1666,7 +1692,7 @@
       </c>
       <c r="D5" s="7"/>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>42</v>
       </c>
@@ -1678,7 +1704,7 @@
       </c>
       <c r="D6" s="7"/>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>43</v>
       </c>
@@ -1690,7 +1716,7 @@
       </c>
       <c r="D7" s="7"/>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>44</v>
       </c>
@@ -1702,7 +1728,7 @@
       </c>
       <c r="D8" s="7"/>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>45</v>
       </c>
@@ -1714,7 +1740,7 @@
       </c>
       <c r="D9" s="7"/>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>46</v>
       </c>
@@ -1726,7 +1752,7 @@
       </c>
       <c r="D10" s="7"/>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>47</v>
       </c>
@@ -1738,7 +1764,7 @@
       </c>
       <c r="D11" s="7"/>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>48</v>
       </c>
@@ -1750,7 +1776,7 @@
       </c>
       <c r="D12" s="7"/>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>49</v>
       </c>
@@ -1762,7 +1788,7 @@
       </c>
       <c r="D13" s="7"/>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>50</v>
       </c>
@@ -1774,7 +1800,7 @@
       </c>
       <c r="D14" s="7"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>51</v>
       </c>
@@ -1786,7 +1812,7 @@
       </c>
       <c r="D15" s="7"/>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>52</v>
       </c>
@@ -1798,7 +1824,7 @@
       </c>
       <c r="D16" s="7"/>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>53</v>
       </c>
@@ -1810,7 +1836,7 @@
       </c>
       <c r="D17" s="7"/>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>54</v>
       </c>
@@ -1822,7 +1848,7 @@
       </c>
       <c r="D18" s="7"/>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>55</v>
       </c>
@@ -1834,7 +1860,7 @@
       </c>
       <c r="D19" s="7"/>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>56</v>
       </c>
@@ -1846,7 +1872,7 @@
       </c>
       <c r="D20" s="7"/>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>57</v>
       </c>
@@ -1858,7 +1884,7 @@
       </c>
       <c r="D21" s="7"/>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>58</v>
       </c>
@@ -1870,7 +1896,7 @@
       </c>
       <c r="D22" s="7"/>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>59</v>
       </c>
@@ -1882,7 +1908,7 @@
       </c>
       <c r="D23" s="7"/>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>60</v>
       </c>
@@ -1894,7 +1920,7 @@
       </c>
       <c r="D24" s="7"/>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>61</v>
       </c>
@@ -1906,7 +1932,7 @@
       </c>
       <c r="D25" s="7"/>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>62</v>
       </c>
@@ -1925,14 +1951,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A19" sqref="A19:XFD19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
@@ -1940,7 +1966,7 @@
     <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>36</v>
       </c>
@@ -1954,7 +1980,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>38</v>
       </c>
@@ -1966,7 +1992,7 @@
       </c>
       <c r="D2" s="7"/>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>39</v>
       </c>
@@ -1978,7 +2004,7 @@
       </c>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>40</v>
       </c>
@@ -1990,7 +2016,7 @@
       </c>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>41</v>
       </c>
@@ -2002,7 +2028,7 @@
       </c>
       <c r="D5" s="7"/>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>42</v>
       </c>
@@ -2014,7 +2040,7 @@
       </c>
       <c r="D6" s="7"/>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>43</v>
       </c>
@@ -2026,7 +2052,7 @@
       </c>
       <c r="D7" s="7"/>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>44</v>
       </c>
@@ -2038,7 +2064,7 @@
       </c>
       <c r="D8" s="7"/>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>45</v>
       </c>
@@ -2050,7 +2076,7 @@
       </c>
       <c r="D9" s="7"/>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>46</v>
       </c>
@@ -2062,7 +2088,7 @@
       </c>
       <c r="D10" s="7"/>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>47</v>
       </c>
@@ -2074,7 +2100,7 @@
       </c>
       <c r="D11" s="7"/>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>48</v>
       </c>
@@ -2086,7 +2112,7 @@
       </c>
       <c r="D12" s="7"/>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>49</v>
       </c>
@@ -2098,7 +2124,7 @@
       </c>
       <c r="D13" s="7"/>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>50</v>
       </c>
@@ -2110,7 +2136,7 @@
       </c>
       <c r="D14" s="7"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>51</v>
       </c>
@@ -2122,7 +2148,7 @@
       </c>
       <c r="D15" s="7"/>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>52</v>
       </c>
@@ -2134,7 +2160,7 @@
       </c>
       <c r="D16" s="7"/>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>53</v>
       </c>
@@ -2146,7 +2172,7 @@
       </c>
       <c r="D17" s="7"/>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>54</v>
       </c>
@@ -2158,7 +2184,7 @@
       </c>
       <c r="D18" s="7"/>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>55</v>
       </c>
@@ -2170,7 +2196,7 @@
       </c>
       <c r="D19" s="7"/>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>56</v>
       </c>
@@ -2182,7 +2208,7 @@
       </c>
       <c r="D20" s="7"/>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>57</v>
       </c>
@@ -2194,7 +2220,7 @@
       </c>
       <c r="D21" s="7"/>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>58</v>
       </c>
@@ -2206,7 +2232,7 @@
       </c>
       <c r="D22" s="7"/>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>59</v>
       </c>
@@ -2218,7 +2244,7 @@
       </c>
       <c r="D23" s="7"/>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>60</v>
       </c>
@@ -2230,7 +2256,7 @@
       </c>
       <c r="D24" s="7"/>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>61</v>
       </c>
@@ -2242,7 +2268,7 @@
       </c>
       <c r="D25" s="7"/>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>62</v>
       </c>

</xml_diff>

<commit_message>
Minor change to WAT50 and Adds new testscript WAT52
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/WAT.xlsx
+++ b/src/test/resources/xls/WAT.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="163">
   <si>
     <t>TCID</t>
   </si>
@@ -497,6 +497,15 @@
   </si>
   <si>
     <t>Verify that user is able to search for an Author cluster using ORCid search</t>
+  </si>
+  <si>
+    <t>WAT52</t>
+  </si>
+  <si>
+    <t>WAT-562</t>
+  </si>
+  <si>
+    <t>Verify that clicking on the text "Name Search" in the error in ORCid Search page takes the user to Name search tab</t>
   </si>
 </sst>
 </file>
@@ -928,10 +937,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E44"/>
+  <dimension ref="A1:E45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E45" sqref="A1:E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1604,6 +1613,21 @@
         <v>5</v>
       </c>
       <c r="E44" s="7"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="C45" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="D45" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E45" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
WAT new test cases implementation
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/WAT.xlsx
+++ b/src/test/resources/xls/WAT.xlsx
@@ -11,12 +11,12 @@
     <sheet name="WAT09" sheetId="2" r:id="rId2"/>
     <sheet name="WAT13" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725" concurrentCalc="0"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="178">
   <si>
     <t>TCID</t>
   </si>
@@ -511,10 +511,46 @@
     <t>WAT32</t>
   </si>
   <si>
-    <t>WAT-567||WAT-568</t>
-  </si>
-  <si>
-    <t>Verify that System must display the department name (sub-organization) in addition to the institution/org name.||Verify that System must display the sub-organization below the Organization name.</t>
+    <t>WAT33</t>
+  </si>
+  <si>
+    <t>WAT34</t>
+  </si>
+  <si>
+    <t>WAT35</t>
+  </si>
+  <si>
+    <t>Verify that System must display the department name (sub-organization) in addition to the institution/org name.</t>
+  </si>
+  <si>
+    <t>WAT-567</t>
+  </si>
+  <si>
+    <t>WAT36</t>
+  </si>
+  <si>
+    <t>WAT-611</t>
+  </si>
+  <si>
+    <t>Verify that System must provide "Search Results" tab on Author record page</t>
+  </si>
+  <si>
+    <t>Verify that User must be navigated back to the ORCID search results page and the ORCID original search results must be displayed when the "Search results" tab is clicked.</t>
+  </si>
+  <si>
+    <t>WAT-613</t>
+  </si>
+  <si>
+    <t>Verify that User must be navigated back to the search results page and the original search results must be displayed when the "Search results" tab is clicked.</t>
+  </si>
+  <si>
+    <t>WAT-612</t>
+  </si>
+  <si>
+    <t>WAT-614</t>
+  </si>
+  <si>
+    <t>Verify that "Search Results" tab should be highlighted when user navigate back from Author record page to Search Results page</t>
   </si>
 </sst>
 </file>
@@ -950,10 +986,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E46"/>
+  <dimension ref="A1:E50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C53" sqref="C53"/>
+      <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1642,20 +1678,80 @@
       </c>
       <c r="E45" s="7"/>
     </row>
-    <row r="46" spans="1:5" ht="30">
+    <row r="46" spans="1:5">
       <c r="A46" s="12" t="s">
         <v>163</v>
       </c>
       <c r="B46" s="13" t="s">
+        <v>168</v>
+      </c>
+      <c r="C46" s="12" t="s">
+        <v>167</v>
+      </c>
+      <c r="D46" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E46" s="7"/>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" s="12" t="s">
         <v>164</v>
       </c>
-      <c r="C46" s="12" t="s">
+      <c r="B47" s="13" t="s">
+        <v>170</v>
+      </c>
+      <c r="C47" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="D47" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E47" s="7"/>
+    </row>
+    <row r="48" spans="1:5" ht="30">
+      <c r="A48" s="12" t="s">
         <v>165</v>
       </c>
-      <c r="D46" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="E46" s="7"/>
+      <c r="B48" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="C48" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="D48" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E48" s="7"/>
+    </row>
+    <row r="49" spans="1:5" ht="30">
+      <c r="A49" s="12" t="s">
+        <v>166</v>
+      </c>
+      <c r="B49" s="13" t="s">
+        <v>175</v>
+      </c>
+      <c r="C49" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="D49" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E49" s="7"/>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" s="12" t="s">
+        <v>169</v>
+      </c>
+      <c r="B50" s="13" t="s">
+        <v>176</v>
+      </c>
+      <c r="C50" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="D50" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E50" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
WAT new testcase implementation
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/WAT.xlsx
+++ b/src/test/resources/xls/WAT.xlsx
@@ -544,13 +544,13 @@
     <t>Verify that User must be navigated back to the search results page and the original search results must be displayed when the "Search results" tab is clicked.</t>
   </si>
   <si>
-    <t>WAT-612</t>
-  </si>
-  <si>
     <t>WAT-614</t>
   </si>
   <si>
     <t>Verify that "Search Results" tab should be highlighted when user navigate back from Author record page to Search Results page</t>
+  </si>
+  <si>
+    <t>WAT-612||WAT-677</t>
   </si>
 </sst>
 </file>
@@ -1728,7 +1728,7 @@
         <v>166</v>
       </c>
       <c r="B49" s="13" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="C49" s="11" t="s">
         <v>174</v>
@@ -1743,10 +1743,10 @@
         <v>169</v>
       </c>
       <c r="B50" s="13" t="s">
+        <v>175</v>
+      </c>
+      <c r="C50" s="11" t="s">
         <v>176</v>
-      </c>
-      <c r="C50" s="11" t="s">
-        <v>177</v>
       </c>
       <c r="D50" s="12" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
Adds WAT 38 test script
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/WAT.xlsx
+++ b/src/test/resources/xls/WAT.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13935" windowHeight="1995"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="210">
   <si>
     <t>TCID</t>
   </si>
@@ -641,13 +641,19 @@
   </si>
   <si>
     <t>Verify that system must display the author's last known organization(when available)||Verify that last known organization contains following details, Latest publication (publication date) where the author name is linked to an address||Verify that system must display corresponding organization fully/abbrivated based on conditions</t>
+  </si>
+  <si>
+    <t>WAT38</t>
+  </si>
+  <si>
+    <t>Verify that user should be able to select all the records by clicking SELECT ALL link</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -837,7 +843,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -869,9 +875,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -903,6 +910,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1078,14 +1086,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E60"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E61"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A54" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C72" sqref="C72"/>
+      <selection activeCell="C61" sqref="C61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="41" bestFit="1" customWidth="1" collapsed="1"/>
@@ -1094,7 +1102,7 @@
     <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1111,7 +1119,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -1126,7 +1134,7 @@
       </c>
       <c r="E2" s="4"/>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -1141,7 +1149,7 @@
       </c>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>11</v>
       </c>
@@ -1156,7 +1164,7 @@
       </c>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>13</v>
       </c>
@@ -1171,7 +1179,7 @@
       </c>
       <c r="E5" s="7"/>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>15</v>
       </c>
@@ -1186,7 +1194,7 @@
       </c>
       <c r="E6" s="7"/>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>18</v>
       </c>
@@ -1201,7 +1209,7 @@
       </c>
       <c r="E7" s="7"/>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>21</v>
       </c>
@@ -1216,7 +1224,7 @@
       </c>
       <c r="E8" s="7"/>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>23</v>
       </c>
@@ -1231,7 +1239,7 @@
       </c>
       <c r="E9" s="7"/>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>24</v>
       </c>
@@ -1246,7 +1254,7 @@
       </c>
       <c r="E10" s="7"/>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>25</v>
       </c>
@@ -1261,7 +1269,7 @@
       </c>
       <c r="E11" s="7"/>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>26</v>
       </c>
@@ -1276,7 +1284,7 @@
       </c>
       <c r="E12" s="7"/>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>63</v>
       </c>
@@ -1291,7 +1299,7 @@
       </c>
       <c r="E13" s="7"/>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>64</v>
       </c>
@@ -1306,7 +1314,7 @@
       </c>
       <c r="E14" s="7"/>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>65</v>
       </c>
@@ -1321,7 +1329,7 @@
       </c>
       <c r="E15" s="7"/>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>66</v>
       </c>
@@ -1336,7 +1344,7 @@
       </c>
       <c r="E16" s="7"/>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>75</v>
       </c>
@@ -1351,7 +1359,7 @@
       </c>
       <c r="E17" s="7"/>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>76</v>
       </c>
@@ -1366,7 +1374,7 @@
       </c>
       <c r="E18" s="7"/>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>80</v>
       </c>
@@ -1381,7 +1389,7 @@
       </c>
       <c r="E19" s="7"/>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>82</v>
       </c>
@@ -1396,7 +1404,7 @@
       </c>
       <c r="E20" s="7"/>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>83</v>
       </c>
@@ -1411,7 +1419,7 @@
       </c>
       <c r="E21" s="7"/>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>90</v>
       </c>
@@ -1426,7 +1434,7 @@
       </c>
       <c r="E22" s="7"/>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>92</v>
       </c>
@@ -1441,7 +1449,7 @@
       </c>
       <c r="E23" s="7"/>
     </row>
-    <row r="24" spans="1:5" ht="30">
+    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>96</v>
       </c>
@@ -1456,7 +1464,7 @@
       </c>
       <c r="E24" s="7"/>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>98</v>
       </c>
@@ -1471,7 +1479,7 @@
       </c>
       <c r="E25" s="7"/>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
         <v>100</v>
       </c>
@@ -1486,7 +1494,7 @@
       </c>
       <c r="E26" s="7"/>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
         <v>104</v>
       </c>
@@ -1501,7 +1509,7 @@
       </c>
       <c r="E27" s="7"/>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
         <v>107</v>
       </c>
@@ -1516,7 +1524,7 @@
       </c>
       <c r="E28" s="7"/>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
         <v>110</v>
       </c>
@@ -1531,7 +1539,7 @@
       </c>
       <c r="E29" s="7"/>
     </row>
-    <row r="30" spans="1:5" ht="30">
+    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
         <v>112</v>
       </c>
@@ -1546,7 +1554,7 @@
       </c>
       <c r="E30" s="7"/>
     </row>
-    <row r="31" spans="1:5" ht="30">
+    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
         <v>116</v>
       </c>
@@ -1561,7 +1569,7 @@
       </c>
       <c r="E31" s="7"/>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
         <v>121</v>
       </c>
@@ -1576,7 +1584,7 @@
       </c>
       <c r="E32" s="7"/>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
         <v>122</v>
       </c>
@@ -1591,7 +1599,7 @@
       </c>
       <c r="E33" s="7"/>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
         <v>127</v>
       </c>
@@ -1606,7 +1614,7 @@
       </c>
       <c r="E34" s="7"/>
     </row>
-    <row r="35" spans="1:5" ht="30">
+    <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
         <v>130</v>
       </c>
@@ -1621,7 +1629,7 @@
       </c>
       <c r="E35" s="7"/>
     </row>
-    <row r="36" spans="1:5" ht="30">
+    <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
         <v>133</v>
       </c>
@@ -1636,7 +1644,7 @@
       </c>
       <c r="E36" s="7"/>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
         <v>136</v>
       </c>
@@ -1651,7 +1659,7 @@
       </c>
       <c r="E37" s="7"/>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="9" t="s">
         <v>139</v>
       </c>
@@ -1666,7 +1674,7 @@
       </c>
       <c r="E38" s="7"/>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="s">
         <v>142</v>
       </c>
@@ -1681,7 +1689,7 @@
       </c>
       <c r="E39" s="7"/>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="9" t="s">
         <v>146</v>
       </c>
@@ -1696,7 +1704,7 @@
       </c>
       <c r="E40" s="7"/>
     </row>
-    <row r="41" spans="1:5" ht="30">
+    <row r="41" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
         <v>148</v>
       </c>
@@ -1711,7 +1719,7 @@
       </c>
       <c r="E41" s="7"/>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="9" t="s">
         <v>151</v>
       </c>
@@ -1726,7 +1734,7 @@
       </c>
       <c r="E42" s="7"/>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="9" t="s">
         <v>154</v>
       </c>
@@ -1741,7 +1749,7 @@
       </c>
       <c r="E43" s="7"/>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="9" t="s">
         <v>157</v>
       </c>
@@ -1756,7 +1764,7 @@
       </c>
       <c r="E44" s="7"/>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="9" t="s">
         <v>160</v>
       </c>
@@ -1771,7 +1779,7 @@
       </c>
       <c r="E45" s="7"/>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="12" t="s">
         <v>163</v>
       </c>
@@ -1786,7 +1794,7 @@
       </c>
       <c r="E46" s="7"/>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="12" t="s">
         <v>164</v>
       </c>
@@ -1801,7 +1809,7 @@
       </c>
       <c r="E47" s="7"/>
     </row>
-    <row r="48" spans="1:5" ht="30">
+    <row r="48" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="12" t="s">
         <v>165</v>
       </c>
@@ -1816,7 +1824,7 @@
       </c>
       <c r="E48" s="7"/>
     </row>
-    <row r="49" spans="1:5" ht="30">
+    <row r="49" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="12" t="s">
         <v>166</v>
       </c>
@@ -1831,7 +1839,7 @@
       </c>
       <c r="E49" s="7"/>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="12" t="s">
         <v>169</v>
       </c>
@@ -1846,7 +1854,7 @@
       </c>
       <c r="E50" s="7"/>
     </row>
-    <row r="51" spans="1:5" ht="30">
+    <row r="51" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="9" t="s">
         <v>178</v>
       </c>
@@ -1861,7 +1869,7 @@
       </c>
       <c r="E51" s="7"/>
     </row>
-    <row r="52" spans="1:5">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="9" t="s">
         <v>179</v>
       </c>
@@ -1876,7 +1884,7 @@
       </c>
       <c r="E52" s="7"/>
     </row>
-    <row r="53" spans="1:5">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="9" t="s">
         <v>184</v>
       </c>
@@ -1891,7 +1899,7 @@
       </c>
       <c r="E53" s="7"/>
     </row>
-    <row r="54" spans="1:5">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="9" t="s">
         <v>185</v>
       </c>
@@ -1906,7 +1914,7 @@
       </c>
       <c r="E54" s="7"/>
     </row>
-    <row r="55" spans="1:5">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="9" t="s">
         <v>190</v>
       </c>
@@ -1921,7 +1929,7 @@
       </c>
       <c r="E55" s="7"/>
     </row>
-    <row r="56" spans="1:5">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="s">
         <v>193</v>
       </c>
@@ -1936,7 +1944,7 @@
       </c>
       <c r="E56" s="7"/>
     </row>
-    <row r="57" spans="1:5" ht="30">
+    <row r="57" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="9" t="s">
         <v>196</v>
       </c>
@@ -1951,7 +1959,7 @@
       </c>
       <c r="E57" s="7"/>
     </row>
-    <row r="58" spans="1:5">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="9" t="s">
         <v>199</v>
       </c>
@@ -1966,7 +1974,7 @@
       </c>
       <c r="E58" s="7"/>
     </row>
-    <row r="59" spans="1:5">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
         <v>202</v>
       </c>
@@ -1981,7 +1989,7 @@
       </c>
       <c r="E59" s="7"/>
     </row>
-    <row r="60" spans="1:5" ht="45">
+    <row r="60" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
         <v>205</v>
       </c>
@@ -1995,6 +2003,21 @@
         <v>5</v>
       </c>
       <c r="E60" s="7"/>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" s="9" t="s">
+        <v>208</v>
+      </c>
+      <c r="B61" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="C61" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="D61" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E61" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2007,14 +2030,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A19" sqref="A19:XFD19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
@@ -2022,7 +2045,7 @@
     <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>36</v>
       </c>
@@ -2036,7 +2059,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>38</v>
       </c>
@@ -2048,7 +2071,7 @@
       </c>
       <c r="D2" s="7"/>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>39</v>
       </c>
@@ -2060,7 +2083,7 @@
       </c>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>40</v>
       </c>
@@ -2072,7 +2095,7 @@
       </c>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>41</v>
       </c>
@@ -2084,7 +2107,7 @@
       </c>
       <c r="D5" s="7"/>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>42</v>
       </c>
@@ -2096,7 +2119,7 @@
       </c>
       <c r="D6" s="7"/>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>43</v>
       </c>
@@ -2108,7 +2131,7 @@
       </c>
       <c r="D7" s="7"/>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>44</v>
       </c>
@@ -2120,7 +2143,7 @@
       </c>
       <c r="D8" s="7"/>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>45</v>
       </c>
@@ -2132,7 +2155,7 @@
       </c>
       <c r="D9" s="7"/>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>46</v>
       </c>
@@ -2144,7 +2167,7 @@
       </c>
       <c r="D10" s="7"/>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>47</v>
       </c>
@@ -2156,7 +2179,7 @@
       </c>
       <c r="D11" s="7"/>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>48</v>
       </c>
@@ -2168,7 +2191,7 @@
       </c>
       <c r="D12" s="7"/>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>49</v>
       </c>
@@ -2180,7 +2203,7 @@
       </c>
       <c r="D13" s="7"/>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>50</v>
       </c>
@@ -2192,7 +2215,7 @@
       </c>
       <c r="D14" s="7"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>51</v>
       </c>
@@ -2204,7 +2227,7 @@
       </c>
       <c r="D15" s="7"/>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>52</v>
       </c>
@@ -2216,7 +2239,7 @@
       </c>
       <c r="D16" s="7"/>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>53</v>
       </c>
@@ -2228,7 +2251,7 @@
       </c>
       <c r="D17" s="7"/>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>54</v>
       </c>
@@ -2240,7 +2263,7 @@
       </c>
       <c r="D18" s="7"/>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>55</v>
       </c>
@@ -2252,7 +2275,7 @@
       </c>
       <c r="D19" s="7"/>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>56</v>
       </c>
@@ -2264,7 +2287,7 @@
       </c>
       <c r="D20" s="7"/>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>57</v>
       </c>
@@ -2276,7 +2299,7 @@
       </c>
       <c r="D21" s="7"/>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>58</v>
       </c>
@@ -2288,7 +2311,7 @@
       </c>
       <c r="D22" s="7"/>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>59</v>
       </c>
@@ -2300,7 +2323,7 @@
       </c>
       <c r="D23" s="7"/>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>60</v>
       </c>
@@ -2312,7 +2335,7 @@
       </c>
       <c r="D24" s="7"/>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>61</v>
       </c>
@@ -2324,7 +2347,7 @@
       </c>
       <c r="D25" s="7"/>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>62</v>
       </c>
@@ -2343,14 +2366,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A19" sqref="A19:XFD19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
@@ -2358,7 +2381,7 @@
     <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>36</v>
       </c>
@@ -2372,7 +2395,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>38</v>
       </c>
@@ -2384,7 +2407,7 @@
       </c>
       <c r="D2" s="7"/>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>39</v>
       </c>
@@ -2396,7 +2419,7 @@
       </c>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>40</v>
       </c>
@@ -2408,7 +2431,7 @@
       </c>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>41</v>
       </c>
@@ -2420,7 +2443,7 @@
       </c>
       <c r="D5" s="7"/>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>42</v>
       </c>
@@ -2432,7 +2455,7 @@
       </c>
       <c r="D6" s="7"/>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>43</v>
       </c>
@@ -2444,7 +2467,7 @@
       </c>
       <c r="D7" s="7"/>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>44</v>
       </c>
@@ -2456,7 +2479,7 @@
       </c>
       <c r="D8" s="7"/>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>45</v>
       </c>
@@ -2468,7 +2491,7 @@
       </c>
       <c r="D9" s="7"/>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>46</v>
       </c>
@@ -2480,7 +2503,7 @@
       </c>
       <c r="D10" s="7"/>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>47</v>
       </c>
@@ -2492,7 +2515,7 @@
       </c>
       <c r="D11" s="7"/>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>48</v>
       </c>
@@ -2504,7 +2527,7 @@
       </c>
       <c r="D12" s="7"/>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>49</v>
       </c>
@@ -2516,7 +2539,7 @@
       </c>
       <c r="D13" s="7"/>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>50</v>
       </c>
@@ -2528,7 +2551,7 @@
       </c>
       <c r="D14" s="7"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>51</v>
       </c>
@@ -2540,7 +2563,7 @@
       </c>
       <c r="D15" s="7"/>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>52</v>
       </c>
@@ -2552,7 +2575,7 @@
       </c>
       <c r="D16" s="7"/>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>53</v>
       </c>
@@ -2564,7 +2587,7 @@
       </c>
       <c r="D17" s="7"/>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>54</v>
       </c>
@@ -2576,7 +2599,7 @@
       </c>
       <c r="D18" s="7"/>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>55</v>
       </c>
@@ -2588,7 +2611,7 @@
       </c>
       <c r="D19" s="7"/>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>56</v>
       </c>
@@ -2600,7 +2623,7 @@
       </c>
       <c r="D20" s="7"/>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>57</v>
       </c>
@@ -2612,7 +2635,7 @@
       </c>
       <c r="D21" s="7"/>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>58</v>
       </c>
@@ -2624,7 +2647,7 @@
       </c>
       <c r="D22" s="7"/>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>59</v>
       </c>
@@ -2636,7 +2659,7 @@
       </c>
       <c r="D23" s="7"/>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>60</v>
       </c>
@@ -2648,7 +2671,7 @@
       </c>
       <c r="D24" s="7"/>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>61</v>
       </c>
@@ -2660,7 +2683,7 @@
       </c>
       <c r="D25" s="7"/>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>62</v>
       </c>

</xml_diff>

<commit_message>
Created new scripts in WAT application
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/WAT.xlsx
+++ b/src/test/resources/xls/WAT.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13935" windowHeight="1890"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13932" windowHeight="1896"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
     <sheet name="WAT09" sheetId="2" r:id="rId2"/>
     <sheet name="WAT13" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="238">
   <si>
     <t>TCID</t>
   </si>
@@ -705,13 +704,40 @@
   </si>
   <si>
     <t>WAT74</t>
+  </si>
+  <si>
+    <t>WAT81</t>
+  </si>
+  <si>
+    <t>WAT82</t>
+  </si>
+  <si>
+    <t>WAT83</t>
+  </si>
+  <si>
+    <t>WAT-352</t>
+  </si>
+  <si>
+    <t>Verify that system must display 'Alternative names' tab for author record</t>
+  </si>
+  <si>
+    <t>WAT-353</t>
+  </si>
+  <si>
+    <t>Verify that while click on 'Alternative names' tab, tab should be highlighted by highlight bar</t>
+  </si>
+  <si>
+    <t>Verify that System must display a maximum of 5 alternative names</t>
+  </si>
+  <si>
+    <t>WAT-355</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -901,7 +927,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -933,10 +959,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -968,7 +993,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1144,23 +1168,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E67"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A67" sqref="A67"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B70" sqref="B70"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="9.88671875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="41" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="138.140625" style="6" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="138.109375" style="6" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8.5546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1177,7 +1201,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -1192,7 +1216,7 @@
       </c>
       <c r="E2" s="4"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -1207,7 +1231,7 @@
       </c>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" s="7" t="s">
         <v>11</v>
       </c>
@@ -1222,7 +1246,7 @@
       </c>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" s="7" t="s">
         <v>13</v>
       </c>
@@ -1237,7 +1261,7 @@
       </c>
       <c r="E5" s="7"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" s="7" t="s">
         <v>15</v>
       </c>
@@ -1252,7 +1276,7 @@
       </c>
       <c r="E6" s="7"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" s="7" t="s">
         <v>18</v>
       </c>
@@ -1267,7 +1291,7 @@
       </c>
       <c r="E7" s="7"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" s="7" t="s">
         <v>21</v>
       </c>
@@ -1282,7 +1306,7 @@
       </c>
       <c r="E8" s="7"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" s="7" t="s">
         <v>23</v>
       </c>
@@ -1297,7 +1321,7 @@
       </c>
       <c r="E9" s="7"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10" s="7" t="s">
         <v>24</v>
       </c>
@@ -1312,7 +1336,7 @@
       </c>
       <c r="E10" s="7"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11" s="7" t="s">
         <v>25</v>
       </c>
@@ -1327,7 +1351,7 @@
       </c>
       <c r="E11" s="7"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12" s="7" t="s">
         <v>26</v>
       </c>
@@ -1342,7 +1366,7 @@
       </c>
       <c r="E12" s="7"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13" s="7" t="s">
         <v>63</v>
       </c>
@@ -1357,7 +1381,7 @@
       </c>
       <c r="E13" s="7"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="A14" s="7" t="s">
         <v>64</v>
       </c>
@@ -1372,7 +1396,7 @@
       </c>
       <c r="E14" s="7"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="A15" s="7" t="s">
         <v>65</v>
       </c>
@@ -1387,7 +1411,7 @@
       </c>
       <c r="E15" s="7"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="A16" s="7" t="s">
         <v>66</v>
       </c>
@@ -1402,7 +1426,7 @@
       </c>
       <c r="E16" s="7"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5">
       <c r="A17" s="7" t="s">
         <v>75</v>
       </c>
@@ -1417,7 +1441,7 @@
       </c>
       <c r="E17" s="7"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5">
       <c r="A18" s="7" t="s">
         <v>76</v>
       </c>
@@ -1432,7 +1456,7 @@
       </c>
       <c r="E18" s="7"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5">
       <c r="A19" s="7" t="s">
         <v>80</v>
       </c>
@@ -1447,7 +1471,7 @@
       </c>
       <c r="E19" s="7"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5">
       <c r="A20" s="7" t="s">
         <v>82</v>
       </c>
@@ -1462,7 +1486,7 @@
       </c>
       <c r="E20" s="7"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5">
       <c r="A21" s="7" t="s">
         <v>83</v>
       </c>
@@ -1477,7 +1501,7 @@
       </c>
       <c r="E21" s="7"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5">
       <c r="A22" s="7" t="s">
         <v>90</v>
       </c>
@@ -1492,7 +1516,7 @@
       </c>
       <c r="E22" s="7"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5">
       <c r="A23" s="7" t="s">
         <v>92</v>
       </c>
@@ -1507,7 +1531,7 @@
       </c>
       <c r="E23" s="7"/>
     </row>
-    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5">
       <c r="A24" s="9" t="s">
         <v>96</v>
       </c>
@@ -1522,7 +1546,7 @@
       </c>
       <c r="E24" s="7"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5">
       <c r="A25" s="9" t="s">
         <v>98</v>
       </c>
@@ -1537,7 +1561,7 @@
       </c>
       <c r="E25" s="7"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5">
       <c r="A26" s="9" t="s">
         <v>100</v>
       </c>
@@ -1552,7 +1576,7 @@
       </c>
       <c r="E26" s="7"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5">
       <c r="A27" s="9" t="s">
         <v>104</v>
       </c>
@@ -1567,7 +1591,7 @@
       </c>
       <c r="E27" s="7"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5">
       <c r="A28" s="9" t="s">
         <v>107</v>
       </c>
@@ -1582,7 +1606,7 @@
       </c>
       <c r="E28" s="7"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5">
       <c r="A29" s="9" t="s">
         <v>110</v>
       </c>
@@ -1597,7 +1621,7 @@
       </c>
       <c r="E29" s="7"/>
     </row>
-    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" ht="28.8">
       <c r="A30" s="9" t="s">
         <v>112</v>
       </c>
@@ -1612,7 +1636,7 @@
       </c>
       <c r="E30" s="7"/>
     </row>
-    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" ht="28.8">
       <c r="A31" s="9" t="s">
         <v>116</v>
       </c>
@@ -1627,7 +1651,7 @@
       </c>
       <c r="E31" s="7"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5">
       <c r="A32" s="9" t="s">
         <v>121</v>
       </c>
@@ -1642,7 +1666,7 @@
       </c>
       <c r="E32" s="7"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5">
       <c r="A33" s="9" t="s">
         <v>122</v>
       </c>
@@ -1657,7 +1681,7 @@
       </c>
       <c r="E33" s="7"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5">
       <c r="A34" s="9" t="s">
         <v>127</v>
       </c>
@@ -1672,7 +1696,7 @@
       </c>
       <c r="E34" s="7"/>
     </row>
-    <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" ht="28.8">
       <c r="A35" s="9" t="s">
         <v>130</v>
       </c>
@@ -1687,7 +1711,7 @@
       </c>
       <c r="E35" s="7"/>
     </row>
-    <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" ht="28.8">
       <c r="A36" s="9" t="s">
         <v>133</v>
       </c>
@@ -1702,7 +1726,7 @@
       </c>
       <c r="E36" s="7"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5">
       <c r="A37" s="9" t="s">
         <v>136</v>
       </c>
@@ -1717,7 +1741,7 @@
       </c>
       <c r="E37" s="7"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5">
       <c r="A38" s="9" t="s">
         <v>139</v>
       </c>
@@ -1732,7 +1756,7 @@
       </c>
       <c r="E38" s="7"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5">
       <c r="A39" s="9" t="s">
         <v>142</v>
       </c>
@@ -1747,7 +1771,7 @@
       </c>
       <c r="E39" s="7"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5">
       <c r="A40" s="9" t="s">
         <v>146</v>
       </c>
@@ -1762,7 +1786,7 @@
       </c>
       <c r="E40" s="7"/>
     </row>
-    <row r="41" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5">
       <c r="A41" s="9" t="s">
         <v>148</v>
       </c>
@@ -1777,7 +1801,7 @@
       </c>
       <c r="E41" s="7"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5">
       <c r="A42" s="9" t="s">
         <v>151</v>
       </c>
@@ -1792,7 +1816,7 @@
       </c>
       <c r="E42" s="7"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5">
       <c r="A43" s="9" t="s">
         <v>154</v>
       </c>
@@ -1807,7 +1831,7 @@
       </c>
       <c r="E43" s="7"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5">
       <c r="A44" s="9" t="s">
         <v>157</v>
       </c>
@@ -1822,7 +1846,7 @@
       </c>
       <c r="E44" s="7"/>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5">
       <c r="A45" s="9" t="s">
         <v>160</v>
       </c>
@@ -1837,7 +1861,7 @@
       </c>
       <c r="E45" s="7"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5">
       <c r="A46" s="12" t="s">
         <v>163</v>
       </c>
@@ -1852,7 +1876,7 @@
       </c>
       <c r="E46" s="7"/>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5">
       <c r="A47" s="12" t="s">
         <v>164</v>
       </c>
@@ -1867,7 +1891,7 @@
       </c>
       <c r="E47" s="7"/>
     </row>
-    <row r="48" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" ht="28.8">
       <c r="A48" s="12" t="s">
         <v>165</v>
       </c>
@@ -1882,7 +1906,7 @@
       </c>
       <c r="E48" s="7"/>
     </row>
-    <row r="49" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5">
       <c r="A49" s="12" t="s">
         <v>166</v>
       </c>
@@ -1897,7 +1921,7 @@
       </c>
       <c r="E49" s="7"/>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5">
       <c r="A50" s="12" t="s">
         <v>169</v>
       </c>
@@ -1912,7 +1936,7 @@
       </c>
       <c r="E50" s="7"/>
     </row>
-    <row r="51" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" ht="28.8">
       <c r="A51" s="9" t="s">
         <v>178</v>
       </c>
@@ -1927,7 +1951,7 @@
       </c>
       <c r="E51" s="7"/>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5">
       <c r="A52" s="9" t="s">
         <v>179</v>
       </c>
@@ -1942,7 +1966,7 @@
       </c>
       <c r="E52" s="7"/>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5">
       <c r="A53" s="9" t="s">
         <v>184</v>
       </c>
@@ -1957,7 +1981,7 @@
       </c>
       <c r="E53" s="7"/>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5">
       <c r="A54" s="9" t="s">
         <v>185</v>
       </c>
@@ -1972,7 +1996,7 @@
       </c>
       <c r="E54" s="7"/>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5">
       <c r="A55" s="9" t="s">
         <v>190</v>
       </c>
@@ -1987,7 +2011,7 @@
       </c>
       <c r="E55" s="7"/>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5">
       <c r="A56" s="9" t="s">
         <v>193</v>
       </c>
@@ -2002,7 +2026,7 @@
       </c>
       <c r="E56" s="7"/>
     </row>
-    <row r="57" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5">
       <c r="A57" s="9" t="s">
         <v>196</v>
       </c>
@@ -2017,7 +2041,7 @@
       </c>
       <c r="E57" s="7"/>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5">
       <c r="A58" s="9" t="s">
         <v>199</v>
       </c>
@@ -2032,7 +2056,7 @@
       </c>
       <c r="E58" s="7"/>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5">
       <c r="A59" s="7" t="s">
         <v>201</v>
       </c>
@@ -2047,7 +2071,7 @@
       </c>
       <c r="E59" s="7"/>
     </row>
-    <row r="60" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" ht="43.2">
       <c r="A60" s="7" t="s">
         <v>204</v>
       </c>
@@ -2062,7 +2086,7 @@
       </c>
       <c r="E60" s="7"/>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5">
       <c r="A61" s="9" t="s">
         <v>207</v>
       </c>
@@ -2077,7 +2101,7 @@
       </c>
       <c r="E61" s="7"/>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5">
       <c r="A62" s="9" t="s">
         <v>209</v>
       </c>
@@ -2092,7 +2116,7 @@
       </c>
       <c r="E62" s="7"/>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5">
       <c r="A63" s="9" t="s">
         <v>211</v>
       </c>
@@ -2107,7 +2131,7 @@
       </c>
       <c r="E63" s="7"/>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5">
       <c r="A64" s="9" t="s">
         <v>213</v>
       </c>
@@ -2122,7 +2146,7 @@
       </c>
       <c r="E64" s="7"/>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5">
       <c r="A65" s="9" t="s">
         <v>222</v>
       </c>
@@ -2137,7 +2161,7 @@
       </c>
       <c r="E65" s="7"/>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5">
       <c r="A66" s="9" t="s">
         <v>223</v>
       </c>
@@ -2152,7 +2176,7 @@
       </c>
       <c r="E66" s="7"/>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5">
       <c r="A67" s="9" t="s">
         <v>228</v>
       </c>
@@ -2163,6 +2187,48 @@
         <v>226</v>
       </c>
       <c r="D67" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5">
+      <c r="A68" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="B68" s="9" t="s">
+        <v>232</v>
+      </c>
+      <c r="C68" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="D68" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5">
+      <c r="A69" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="B69" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="C69" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="D69" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5">
+      <c r="A70" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="B70" s="9" t="s">
+        <v>237</v>
+      </c>
+      <c r="C70" s="9" t="s">
+        <v>236</v>
+      </c>
+      <c r="D70" s="9" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2177,22 +2243,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A19" sqref="A19:XFD19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="10" t="s">
         <v>36</v>
       </c>
@@ -2206,7 +2272,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="7" t="s">
         <v>38</v>
       </c>
@@ -2218,7 +2284,7 @@
       </c>
       <c r="D2" s="7"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="7" t="s">
         <v>39</v>
       </c>
@@ -2230,7 +2296,7 @@
       </c>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="7" t="s">
         <v>40</v>
       </c>
@@ -2242,7 +2308,7 @@
       </c>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" s="7" t="s">
         <v>41</v>
       </c>
@@ -2254,7 +2320,7 @@
       </c>
       <c r="D5" s="7"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" s="7" t="s">
         <v>42</v>
       </c>
@@ -2266,7 +2332,7 @@
       </c>
       <c r="D6" s="7"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="7" t="s">
         <v>43</v>
       </c>
@@ -2278,7 +2344,7 @@
       </c>
       <c r="D7" s="7"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="7" t="s">
         <v>44</v>
       </c>
@@ -2290,7 +2356,7 @@
       </c>
       <c r="D8" s="7"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="7" t="s">
         <v>45</v>
       </c>
@@ -2302,7 +2368,7 @@
       </c>
       <c r="D9" s="7"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="7" t="s">
         <v>46</v>
       </c>
@@ -2314,7 +2380,7 @@
       </c>
       <c r="D10" s="7"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11" s="7" t="s">
         <v>47</v>
       </c>
@@ -2326,7 +2392,7 @@
       </c>
       <c r="D11" s="7"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="A12" s="7" t="s">
         <v>48</v>
       </c>
@@ -2338,7 +2404,7 @@
       </c>
       <c r="D12" s="7"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="A13" s="7" t="s">
         <v>49</v>
       </c>
@@ -2350,7 +2416,7 @@
       </c>
       <c r="D13" s="7"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="A14" s="7" t="s">
         <v>50</v>
       </c>
@@ -2362,7 +2428,7 @@
       </c>
       <c r="D14" s="7"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="A15" s="7" t="s">
         <v>51</v>
       </c>
@@ -2374,7 +2440,7 @@
       </c>
       <c r="D15" s="7"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="A16" s="7" t="s">
         <v>52</v>
       </c>
@@ -2386,7 +2452,7 @@
       </c>
       <c r="D16" s="7"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4">
       <c r="A17" s="7" t="s">
         <v>53</v>
       </c>
@@ -2398,7 +2464,7 @@
       </c>
       <c r="D17" s="7"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4">
       <c r="A18" s="7" t="s">
         <v>54</v>
       </c>
@@ -2410,7 +2476,7 @@
       </c>
       <c r="D18" s="7"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4">
       <c r="A19" s="7" t="s">
         <v>55</v>
       </c>
@@ -2422,7 +2488,7 @@
       </c>
       <c r="D19" s="7"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4">
       <c r="A20" s="7" t="s">
         <v>56</v>
       </c>
@@ -2434,7 +2500,7 @@
       </c>
       <c r="D20" s="7"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4">
       <c r="A21" s="7" t="s">
         <v>57</v>
       </c>
@@ -2446,7 +2512,7 @@
       </c>
       <c r="D21" s="7"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4">
       <c r="A22" s="7" t="s">
         <v>58</v>
       </c>
@@ -2458,7 +2524,7 @@
       </c>
       <c r="D22" s="7"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4">
       <c r="A23" s="7" t="s">
         <v>59</v>
       </c>
@@ -2470,7 +2536,7 @@
       </c>
       <c r="D23" s="7"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4">
       <c r="A24" s="7" t="s">
         <v>60</v>
       </c>
@@ -2482,7 +2548,7 @@
       </c>
       <c r="D24" s="7"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4">
       <c r="A25" s="7" t="s">
         <v>61</v>
       </c>
@@ -2494,7 +2560,7 @@
       </c>
       <c r="D25" s="7"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4">
       <c r="A26" s="7" t="s">
         <v>62</v>
       </c>
@@ -2513,22 +2579,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A19" sqref="A19:XFD19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="10" t="s">
         <v>36</v>
       </c>
@@ -2542,7 +2608,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="7" t="s">
         <v>38</v>
       </c>
@@ -2554,7 +2620,7 @@
       </c>
       <c r="D2" s="7"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="7" t="s">
         <v>39</v>
       </c>
@@ -2566,7 +2632,7 @@
       </c>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="7" t="s">
         <v>40</v>
       </c>
@@ -2578,7 +2644,7 @@
       </c>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" s="7" t="s">
         <v>41</v>
       </c>
@@ -2590,7 +2656,7 @@
       </c>
       <c r="D5" s="7"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" s="7" t="s">
         <v>42</v>
       </c>
@@ -2602,7 +2668,7 @@
       </c>
       <c r="D6" s="7"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="7" t="s">
         <v>43</v>
       </c>
@@ -2614,7 +2680,7 @@
       </c>
       <c r="D7" s="7"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="7" t="s">
         <v>44</v>
       </c>
@@ -2626,7 +2692,7 @@
       </c>
       <c r="D8" s="7"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="7" t="s">
         <v>45</v>
       </c>
@@ -2638,7 +2704,7 @@
       </c>
       <c r="D9" s="7"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="7" t="s">
         <v>46</v>
       </c>
@@ -2650,7 +2716,7 @@
       </c>
       <c r="D10" s="7"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11" s="7" t="s">
         <v>47</v>
       </c>
@@ -2662,7 +2728,7 @@
       </c>
       <c r="D11" s="7"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="A12" s="7" t="s">
         <v>48</v>
       </c>
@@ -2674,7 +2740,7 @@
       </c>
       <c r="D12" s="7"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="A13" s="7" t="s">
         <v>49</v>
       </c>
@@ -2686,7 +2752,7 @@
       </c>
       <c r="D13" s="7"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="A14" s="7" t="s">
         <v>50</v>
       </c>
@@ -2698,7 +2764,7 @@
       </c>
       <c r="D14" s="7"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="A15" s="7" t="s">
         <v>51</v>
       </c>
@@ -2710,7 +2776,7 @@
       </c>
       <c r="D15" s="7"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="A16" s="7" t="s">
         <v>52</v>
       </c>
@@ -2722,7 +2788,7 @@
       </c>
       <c r="D16" s="7"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4">
       <c r="A17" s="7" t="s">
         <v>53</v>
       </c>
@@ -2734,7 +2800,7 @@
       </c>
       <c r="D17" s="7"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4">
       <c r="A18" s="7" t="s">
         <v>54</v>
       </c>
@@ -2746,7 +2812,7 @@
       </c>
       <c r="D18" s="7"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4">
       <c r="A19" s="7" t="s">
         <v>55</v>
       </c>
@@ -2758,7 +2824,7 @@
       </c>
       <c r="D19" s="7"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4">
       <c r="A20" s="7" t="s">
         <v>56</v>
       </c>
@@ -2770,7 +2836,7 @@
       </c>
       <c r="D20" s="7"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4">
       <c r="A21" s="7" t="s">
         <v>57</v>
       </c>
@@ -2782,7 +2848,7 @@
       </c>
       <c r="D21" s="7"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4">
       <c r="A22" s="7" t="s">
         <v>58</v>
       </c>
@@ -2794,7 +2860,7 @@
       </c>
       <c r="D22" s="7"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4">
       <c r="A23" s="7" t="s">
         <v>59</v>
       </c>
@@ -2806,7 +2872,7 @@
       </c>
       <c r="D23" s="7"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4">
       <c r="A24" s="7" t="s">
         <v>60</v>
       </c>
@@ -2818,7 +2884,7 @@
       </c>
       <c r="D24" s="7"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4">
       <c r="A25" s="7" t="s">
         <v>61</v>
       </c>
@@ -2830,7 +2896,7 @@
       </c>
       <c r="D25" s="7"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4">
       <c r="A26" s="7" t="s">
         <v>62</v>
       </c>

</xml_diff>

<commit_message>
Created new scripts in wat module.
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/WAT.xlsx
+++ b/src/test/resources/xls/WAT.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13305" windowHeight="2415"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13308" windowHeight="2412"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
     <sheet name="WAT09" sheetId="2" r:id="rId2"/>
     <sheet name="WAT13" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="253">
   <si>
     <t>TCID</t>
   </si>
@@ -768,13 +767,22 @@
   </si>
   <si>
     <t>WAT-602</t>
+  </si>
+  <si>
+    <t>WAT84</t>
+  </si>
+  <si>
+    <t>Verify that System must display name variations associated with the author record in the alternative names tab. Authors in format Last,FirstName OR Last, FirstInitials</t>
+  </si>
+  <si>
+    <t>WAT-354</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -983,7 +991,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1015,10 +1023,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1050,7 +1057,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1226,23 +1232,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E74"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B73" sqref="B73:B74"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B75" sqref="B75"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="9.88671875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="41" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="138.140625" style="6" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="138.109375" style="6" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8.5546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1259,7 +1265,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -1274,7 +1280,7 @@
       </c>
       <c r="E2" s="4"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -1289,7 +1295,7 @@
       </c>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" s="7" t="s">
         <v>11</v>
       </c>
@@ -1304,7 +1310,7 @@
       </c>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" s="7" t="s">
         <v>13</v>
       </c>
@@ -1319,7 +1325,7 @@
       </c>
       <c r="E5" s="7"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" s="7" t="s">
         <v>15</v>
       </c>
@@ -1334,7 +1340,7 @@
       </c>
       <c r="E6" s="7"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" s="7" t="s">
         <v>18</v>
       </c>
@@ -1349,7 +1355,7 @@
       </c>
       <c r="E7" s="7"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" s="7" t="s">
         <v>21</v>
       </c>
@@ -1364,7 +1370,7 @@
       </c>
       <c r="E8" s="7"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" s="7" t="s">
         <v>23</v>
       </c>
@@ -1379,7 +1385,7 @@
       </c>
       <c r="E9" s="7"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10" s="7" t="s">
         <v>24</v>
       </c>
@@ -1394,7 +1400,7 @@
       </c>
       <c r="E10" s="7"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11" s="7" t="s">
         <v>25</v>
       </c>
@@ -1409,7 +1415,7 @@
       </c>
       <c r="E11" s="7"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12" s="7" t="s">
         <v>26</v>
       </c>
@@ -1424,7 +1430,7 @@
       </c>
       <c r="E12" s="7"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13" s="7" t="s">
         <v>63</v>
       </c>
@@ -1439,7 +1445,7 @@
       </c>
       <c r="E13" s="7"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="A14" s="7" t="s">
         <v>64</v>
       </c>
@@ -1454,7 +1460,7 @@
       </c>
       <c r="E14" s="7"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="A15" s="7" t="s">
         <v>65</v>
       </c>
@@ -1469,7 +1475,7 @@
       </c>
       <c r="E15" s="7"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="A16" s="7" t="s">
         <v>66</v>
       </c>
@@ -1484,7 +1490,7 @@
       </c>
       <c r="E16" s="7"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5">
       <c r="A17" s="7" t="s">
         <v>75</v>
       </c>
@@ -1499,7 +1505,7 @@
       </c>
       <c r="E17" s="7"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5">
       <c r="A18" s="7" t="s">
         <v>76</v>
       </c>
@@ -1514,7 +1520,7 @@
       </c>
       <c r="E18" s="7"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5">
       <c r="A19" s="7" t="s">
         <v>80</v>
       </c>
@@ -1529,7 +1535,7 @@
       </c>
       <c r="E19" s="7"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5">
       <c r="A20" s="7" t="s">
         <v>82</v>
       </c>
@@ -1544,7 +1550,7 @@
       </c>
       <c r="E20" s="7"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5">
       <c r="A21" s="7" t="s">
         <v>83</v>
       </c>
@@ -1559,7 +1565,7 @@
       </c>
       <c r="E21" s="7"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5">
       <c r="A22" s="7" t="s">
         <v>90</v>
       </c>
@@ -1574,7 +1580,7 @@
       </c>
       <c r="E22" s="7"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5">
       <c r="A23" s="7" t="s">
         <v>92</v>
       </c>
@@ -1589,7 +1595,7 @@
       </c>
       <c r="E23" s="7"/>
     </row>
-    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5">
       <c r="A24" s="9" t="s">
         <v>96</v>
       </c>
@@ -1604,7 +1610,7 @@
       </c>
       <c r="E24" s="7"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5">
       <c r="A25" s="9" t="s">
         <v>98</v>
       </c>
@@ -1619,7 +1625,7 @@
       </c>
       <c r="E25" s="7"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5">
       <c r="A26" s="9" t="s">
         <v>100</v>
       </c>
@@ -1634,7 +1640,7 @@
       </c>
       <c r="E26" s="7"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5">
       <c r="A27" s="9" t="s">
         <v>104</v>
       </c>
@@ -1649,7 +1655,7 @@
       </c>
       <c r="E27" s="7"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5">
       <c r="A28" s="9" t="s">
         <v>107</v>
       </c>
@@ -1664,7 +1670,7 @@
       </c>
       <c r="E28" s="7"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5">
       <c r="A29" s="9" t="s">
         <v>110</v>
       </c>
@@ -1679,7 +1685,7 @@
       </c>
       <c r="E29" s="7"/>
     </row>
-    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" ht="28.8">
       <c r="A30" s="9" t="s">
         <v>112</v>
       </c>
@@ -1694,7 +1700,7 @@
       </c>
       <c r="E30" s="7"/>
     </row>
-    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" ht="28.8">
       <c r="A31" s="9" t="s">
         <v>116</v>
       </c>
@@ -1709,7 +1715,7 @@
       </c>
       <c r="E31" s="7"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5">
       <c r="A32" s="9" t="s">
         <v>121</v>
       </c>
@@ -1724,7 +1730,7 @@
       </c>
       <c r="E32" s="7"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5">
       <c r="A33" s="9" t="s">
         <v>122</v>
       </c>
@@ -1739,7 +1745,7 @@
       </c>
       <c r="E33" s="7"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5">
       <c r="A34" s="9" t="s">
         <v>127</v>
       </c>
@@ -1754,7 +1760,7 @@
       </c>
       <c r="E34" s="7"/>
     </row>
-    <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" ht="28.8">
       <c r="A35" s="9" t="s">
         <v>130</v>
       </c>
@@ -1769,7 +1775,7 @@
       </c>
       <c r="E35" s="7"/>
     </row>
-    <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" ht="28.8">
       <c r="A36" s="9" t="s">
         <v>133</v>
       </c>
@@ -1784,7 +1790,7 @@
       </c>
       <c r="E36" s="7"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5">
       <c r="A37" s="9" t="s">
         <v>136</v>
       </c>
@@ -1799,7 +1805,7 @@
       </c>
       <c r="E37" s="7"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5">
       <c r="A38" s="9" t="s">
         <v>139</v>
       </c>
@@ -1814,7 +1820,7 @@
       </c>
       <c r="E38" s="7"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5">
       <c r="A39" s="9" t="s">
         <v>142</v>
       </c>
@@ -1829,7 +1835,7 @@
       </c>
       <c r="E39" s="7"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5">
       <c r="A40" s="9" t="s">
         <v>146</v>
       </c>
@@ -1844,7 +1850,7 @@
       </c>
       <c r="E40" s="7"/>
     </row>
-    <row r="41" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5">
       <c r="A41" s="9" t="s">
         <v>148</v>
       </c>
@@ -1859,7 +1865,7 @@
       </c>
       <c r="E41" s="7"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5">
       <c r="A42" s="9" t="s">
         <v>151</v>
       </c>
@@ -1874,7 +1880,7 @@
       </c>
       <c r="E42" s="7"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5">
       <c r="A43" s="9" t="s">
         <v>154</v>
       </c>
@@ -1889,7 +1895,7 @@
       </c>
       <c r="E43" s="7"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5">
       <c r="A44" s="9" t="s">
         <v>157</v>
       </c>
@@ -1904,7 +1910,7 @@
       </c>
       <c r="E44" s="7"/>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5">
       <c r="A45" s="9" t="s">
         <v>160</v>
       </c>
@@ -1919,7 +1925,7 @@
       </c>
       <c r="E45" s="7"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5">
       <c r="A46" s="12" t="s">
         <v>163</v>
       </c>
@@ -1934,7 +1940,7 @@
       </c>
       <c r="E46" s="7"/>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5">
       <c r="A47" s="12" t="s">
         <v>164</v>
       </c>
@@ -1949,7 +1955,7 @@
       </c>
       <c r="E47" s="7"/>
     </row>
-    <row r="48" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" ht="28.8">
       <c r="A48" s="12" t="s">
         <v>165</v>
       </c>
@@ -1964,7 +1970,7 @@
       </c>
       <c r="E48" s="7"/>
     </row>
-    <row r="49" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5">
       <c r="A49" s="12" t="s">
         <v>166</v>
       </c>
@@ -1979,7 +1985,7 @@
       </c>
       <c r="E49" s="7"/>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5">
       <c r="A50" s="12" t="s">
         <v>169</v>
       </c>
@@ -1994,7 +2000,7 @@
       </c>
       <c r="E50" s="7"/>
     </row>
-    <row r="51" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" ht="28.8">
       <c r="A51" s="9" t="s">
         <v>178</v>
       </c>
@@ -2009,7 +2015,7 @@
       </c>
       <c r="E51" s="7"/>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5">
       <c r="A52" s="9" t="s">
         <v>179</v>
       </c>
@@ -2024,7 +2030,7 @@
       </c>
       <c r="E52" s="7"/>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5">
       <c r="A53" s="9" t="s">
         <v>184</v>
       </c>
@@ -2039,7 +2045,7 @@
       </c>
       <c r="E53" s="7"/>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5">
       <c r="A54" s="9" t="s">
         <v>185</v>
       </c>
@@ -2054,7 +2060,7 @@
       </c>
       <c r="E54" s="7"/>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5">
       <c r="A55" s="9" t="s">
         <v>190</v>
       </c>
@@ -2069,7 +2075,7 @@
       </c>
       <c r="E55" s="7"/>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5">
       <c r="A56" s="9" t="s">
         <v>193</v>
       </c>
@@ -2084,7 +2090,7 @@
       </c>
       <c r="E56" s="7"/>
     </row>
-    <row r="57" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5">
       <c r="A57" s="9" t="s">
         <v>196</v>
       </c>
@@ -2099,7 +2105,7 @@
       </c>
       <c r="E57" s="7"/>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5">
       <c r="A58" s="9" t="s">
         <v>199</v>
       </c>
@@ -2114,7 +2120,7 @@
       </c>
       <c r="E58" s="7"/>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5">
       <c r="A59" s="7" t="s">
         <v>201</v>
       </c>
@@ -2129,7 +2135,7 @@
       </c>
       <c r="E59" s="7"/>
     </row>
-    <row r="60" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" ht="43.2">
       <c r="A60" s="7" t="s">
         <v>204</v>
       </c>
@@ -2144,7 +2150,7 @@
       </c>
       <c r="E60" s="7"/>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5">
       <c r="A61" s="9" t="s">
         <v>207</v>
       </c>
@@ -2159,7 +2165,7 @@
       </c>
       <c r="E61" s="7"/>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5">
       <c r="A62" s="9" t="s">
         <v>209</v>
       </c>
@@ -2174,7 +2180,7 @@
       </c>
       <c r="E62" s="7"/>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5">
       <c r="A63" s="9" t="s">
         <v>211</v>
       </c>
@@ -2189,7 +2195,7 @@
       </c>
       <c r="E63" s="7"/>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5">
       <c r="A64" s="9" t="s">
         <v>213</v>
       </c>
@@ -2204,7 +2210,7 @@
       </c>
       <c r="E64" s="7"/>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5">
       <c r="A65" s="9" t="s">
         <v>222</v>
       </c>
@@ -2219,7 +2225,7 @@
       </c>
       <c r="E65" s="7"/>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5">
       <c r="A66" s="9" t="s">
         <v>223</v>
       </c>
@@ -2234,7 +2240,7 @@
       </c>
       <c r="E66" s="7"/>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5">
       <c r="A67" s="9" t="s">
         <v>228</v>
       </c>
@@ -2247,8 +2253,9 @@
       <c r="D67" s="9" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E67" s="7"/>
+    </row>
+    <row r="68" spans="1:5">
       <c r="A68" s="9" t="s">
         <v>229</v>
       </c>
@@ -2261,8 +2268,9 @@
       <c r="D68" s="9" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E68" s="7"/>
+    </row>
+    <row r="69" spans="1:5">
       <c r="A69" s="9" t="s">
         <v>230</v>
       </c>
@@ -2275,8 +2283,9 @@
       <c r="D69" s="9" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E69" s="7"/>
+    </row>
+    <row r="70" spans="1:5">
       <c r="A70" s="9" t="s">
         <v>231</v>
       </c>
@@ -2289,8 +2298,9 @@
       <c r="D70" s="9" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E70" s="7"/>
+    </row>
+    <row r="71" spans="1:5">
       <c r="A71" s="9" t="s">
         <v>238</v>
       </c>
@@ -2303,8 +2313,9 @@
       <c r="D71" s="9" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E71" s="7"/>
+    </row>
+    <row r="72" spans="1:5">
       <c r="A72" s="15" t="s">
         <v>242</v>
       </c>
@@ -2317,8 +2328,9 @@
       <c r="D72" s="15" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E72" s="7"/>
+    </row>
+    <row r="73" spans="1:5">
       <c r="A73" s="15" t="s">
         <v>244</v>
       </c>
@@ -2331,8 +2343,9 @@
       <c r="D73" s="15" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E73" s="7"/>
+    </row>
+    <row r="74" spans="1:5">
       <c r="A74" s="15" t="s">
         <v>248</v>
       </c>
@@ -2345,6 +2358,22 @@
       <c r="D74" s="15" t="s">
         <v>5</v>
       </c>
+      <c r="E74" s="7"/>
+    </row>
+    <row r="75" spans="1:5" ht="28.8">
+      <c r="A75" s="15" t="s">
+        <v>250</v>
+      </c>
+      <c r="B75" s="9" t="s">
+        <v>252</v>
+      </c>
+      <c r="C75" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="D75" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="E75" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2357,22 +2386,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A19" sqref="A19:XFD19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="10" t="s">
         <v>36</v>
       </c>
@@ -2386,7 +2415,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="7" t="s">
         <v>38</v>
       </c>
@@ -2398,7 +2427,7 @@
       </c>
       <c r="D2" s="7"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="7" t="s">
         <v>39</v>
       </c>
@@ -2410,7 +2439,7 @@
       </c>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="7" t="s">
         <v>40</v>
       </c>
@@ -2422,7 +2451,7 @@
       </c>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" s="7" t="s">
         <v>41</v>
       </c>
@@ -2434,7 +2463,7 @@
       </c>
       <c r="D5" s="7"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" s="7" t="s">
         <v>42</v>
       </c>
@@ -2446,7 +2475,7 @@
       </c>
       <c r="D6" s="7"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="7" t="s">
         <v>43</v>
       </c>
@@ -2458,7 +2487,7 @@
       </c>
       <c r="D7" s="7"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="7" t="s">
         <v>44</v>
       </c>
@@ -2470,7 +2499,7 @@
       </c>
       <c r="D8" s="7"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="7" t="s">
         <v>45</v>
       </c>
@@ -2482,7 +2511,7 @@
       </c>
       <c r="D9" s="7"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="7" t="s">
         <v>46</v>
       </c>
@@ -2494,7 +2523,7 @@
       </c>
       <c r="D10" s="7"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11" s="7" t="s">
         <v>47</v>
       </c>
@@ -2506,7 +2535,7 @@
       </c>
       <c r="D11" s="7"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="A12" s="7" t="s">
         <v>48</v>
       </c>
@@ -2518,7 +2547,7 @@
       </c>
       <c r="D12" s="7"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="A13" s="7" t="s">
         <v>49</v>
       </c>
@@ -2530,7 +2559,7 @@
       </c>
       <c r="D13" s="7"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="A14" s="7" t="s">
         <v>50</v>
       </c>
@@ -2542,7 +2571,7 @@
       </c>
       <c r="D14" s="7"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="A15" s="7" t="s">
         <v>51</v>
       </c>
@@ -2554,7 +2583,7 @@
       </c>
       <c r="D15" s="7"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="A16" s="7" t="s">
         <v>52</v>
       </c>
@@ -2566,7 +2595,7 @@
       </c>
       <c r="D16" s="7"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4">
       <c r="A17" s="7" t="s">
         <v>53</v>
       </c>
@@ -2578,7 +2607,7 @@
       </c>
       <c r="D17" s="7"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4">
       <c r="A18" s="7" t="s">
         <v>54</v>
       </c>
@@ -2590,7 +2619,7 @@
       </c>
       <c r="D18" s="7"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4">
       <c r="A19" s="7" t="s">
         <v>55</v>
       </c>
@@ -2602,7 +2631,7 @@
       </c>
       <c r="D19" s="7"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4">
       <c r="A20" s="7" t="s">
         <v>56</v>
       </c>
@@ -2614,7 +2643,7 @@
       </c>
       <c r="D20" s="7"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4">
       <c r="A21" s="7" t="s">
         <v>57</v>
       </c>
@@ -2626,7 +2655,7 @@
       </c>
       <c r="D21" s="7"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4">
       <c r="A22" s="7" t="s">
         <v>58</v>
       </c>
@@ -2638,7 +2667,7 @@
       </c>
       <c r="D22" s="7"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4">
       <c r="A23" s="7" t="s">
         <v>59</v>
       </c>
@@ -2650,7 +2679,7 @@
       </c>
       <c r="D23" s="7"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4">
       <c r="A24" s="7" t="s">
         <v>60</v>
       </c>
@@ -2662,7 +2691,7 @@
       </c>
       <c r="D24" s="7"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4">
       <c r="A25" s="7" t="s">
         <v>61</v>
       </c>
@@ -2674,7 +2703,7 @@
       </c>
       <c r="D25" s="7"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4">
       <c r="A26" s="7" t="s">
         <v>62</v>
       </c>
@@ -2693,22 +2722,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A19" sqref="A19:XFD19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="10" t="s">
         <v>36</v>
       </c>
@@ -2722,7 +2751,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="7" t="s">
         <v>38</v>
       </c>
@@ -2734,7 +2763,7 @@
       </c>
       <c r="D2" s="7"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="7" t="s">
         <v>39</v>
       </c>
@@ -2746,7 +2775,7 @@
       </c>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="7" t="s">
         <v>40</v>
       </c>
@@ -2758,7 +2787,7 @@
       </c>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" s="7" t="s">
         <v>41</v>
       </c>
@@ -2770,7 +2799,7 @@
       </c>
       <c r="D5" s="7"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" s="7" t="s">
         <v>42</v>
       </c>
@@ -2782,7 +2811,7 @@
       </c>
       <c r="D6" s="7"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="7" t="s">
         <v>43</v>
       </c>
@@ -2794,7 +2823,7 @@
       </c>
       <c r="D7" s="7"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="7" t="s">
         <v>44</v>
       </c>
@@ -2806,7 +2835,7 @@
       </c>
       <c r="D8" s="7"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="7" t="s">
         <v>45</v>
       </c>
@@ -2818,7 +2847,7 @@
       </c>
       <c r="D9" s="7"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="7" t="s">
         <v>46</v>
       </c>
@@ -2830,7 +2859,7 @@
       </c>
       <c r="D10" s="7"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11" s="7" t="s">
         <v>47</v>
       </c>
@@ -2842,7 +2871,7 @@
       </c>
       <c r="D11" s="7"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="A12" s="7" t="s">
         <v>48</v>
       </c>
@@ -2854,7 +2883,7 @@
       </c>
       <c r="D12" s="7"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="A13" s="7" t="s">
         <v>49</v>
       </c>
@@ -2866,7 +2895,7 @@
       </c>
       <c r="D13" s="7"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="A14" s="7" t="s">
         <v>50</v>
       </c>
@@ -2878,7 +2907,7 @@
       </c>
       <c r="D14" s="7"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="A15" s="7" t="s">
         <v>51</v>
       </c>
@@ -2890,7 +2919,7 @@
       </c>
       <c r="D15" s="7"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="A16" s="7" t="s">
         <v>52</v>
       </c>
@@ -2902,7 +2931,7 @@
       </c>
       <c r="D16" s="7"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4">
       <c r="A17" s="7" t="s">
         <v>53</v>
       </c>
@@ -2914,7 +2943,7 @@
       </c>
       <c r="D17" s="7"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4">
       <c r="A18" s="7" t="s">
         <v>54</v>
       </c>
@@ -2926,7 +2955,7 @@
       </c>
       <c r="D18" s="7"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4">
       <c r="A19" s="7" t="s">
         <v>55</v>
       </c>
@@ -2938,7 +2967,7 @@
       </c>
       <c r="D19" s="7"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4">
       <c r="A20" s="7" t="s">
         <v>56</v>
       </c>
@@ -2950,7 +2979,7 @@
       </c>
       <c r="D20" s="7"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4">
       <c r="A21" s="7" t="s">
         <v>57</v>
       </c>
@@ -2962,7 +2991,7 @@
       </c>
       <c r="D21" s="7"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4">
       <c r="A22" s="7" t="s">
         <v>58</v>
       </c>
@@ -2974,7 +3003,7 @@
       </c>
       <c r="D22" s="7"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4">
       <c r="A23" s="7" t="s">
         <v>59</v>
       </c>
@@ -2986,7 +3015,7 @@
       </c>
       <c r="D23" s="7"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4">
       <c r="A24" s="7" t="s">
         <v>60</v>
       </c>
@@ -2998,7 +3027,7 @@
       </c>
       <c r="D24" s="7"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4">
       <c r="A25" s="7" t="s">
         <v>61</v>
       </c>
@@ -3010,7 +3039,7 @@
       </c>
       <c r="D25" s="7"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4">
       <c r="A26" s="7" t="s">
         <v>62</v>
       </c>

</xml_diff>

<commit_message>
Minor xls change in WAT module
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/WAT.xlsx
+++ b/src/test/resources/xls/WAT.xlsx
@@ -11,7 +11,7 @@
     <sheet name="WAT09" sheetId="2" r:id="rId2"/>
     <sheet name="WAT13" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -285,9 +285,6 @@
     <t>Verify that user is able to search for an Author cluster u7sing both Last name and First  name and navigate to author search result page.</t>
   </si>
   <si>
-    <t>WAT-156||WAT-160||WAT-195</t>
-  </si>
-  <si>
     <t>WAT21</t>
   </si>
   <si>
@@ -451,9 +448,6 @@
     <t>Verify that upon clicking ORCiD tab, Orcid search field should be displayed with an example of orcid number</t>
   </si>
   <si>
-    <t>WAT-323</t>
-  </si>
-  <si>
     <t>WAT-558</t>
   </si>
   <si>
@@ -466,9 +460,6 @@
     <t>WAT50</t>
   </si>
   <si>
-    <t>WAT-333</t>
-  </si>
-  <si>
     <t>Verify that error "Please enter a valid ORCiD number or try the Name Search" is displayed when there is no search result available for a correctly formatted ORCiD.</t>
   </si>
   <si>
@@ -493,9 +484,6 @@
     <t>WAT51</t>
   </si>
   <si>
-    <t>WAT-561</t>
-  </si>
-  <si>
     <t>Verify that user is able to search for an Author cluster using ORCid search</t>
   </si>
   <si>
@@ -785,6 +773,18 @@
   </si>
   <si>
     <t>Verify that system must display a "Suggest updates" button, which when clicked will enter into curation mode</t>
+  </si>
+  <si>
+    <t>WAT-333||WAT-302||WAT-301||WAT-300</t>
+  </si>
+  <si>
+    <t>WAT-156||WAT-160||WAT-195||WAT-298</t>
+  </si>
+  <si>
+    <t>WAT-561||WAT-303||WAT-298</t>
+  </si>
+  <si>
+    <t>WAT-323||WAT-297</t>
   </si>
 </sst>
 </file>
@@ -1246,8 +1246,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C76" sqref="C76"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1314,7 +1314,7 @@
         <v>12</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>5</v>
@@ -1326,7 +1326,7 @@
         <v>13</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>89</v>
+        <v>253</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>14</v>
@@ -1539,7 +1539,7 @@
         <v>81</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D19" s="9" t="s">
         <v>5</v>
@@ -1578,13 +1578,13 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="B22" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="B22" s="7" t="s">
-        <v>91</v>
-      </c>
       <c r="C22" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D22" s="9" t="s">
         <v>5</v>
@@ -1593,13 +1593,13 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D23" s="9" t="s">
         <v>5</v>
@@ -1608,13 +1608,13 @@
     </row>
     <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="C24" s="11" t="s">
         <v>96</v>
-      </c>
-      <c r="B24" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="C24" s="11" t="s">
-        <v>97</v>
       </c>
       <c r="D24" s="7" t="s">
         <v>5</v>
@@ -1623,13 +1623,13 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="C25" s="8" t="s">
         <v>98</v>
-      </c>
-      <c r="B25" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="C25" s="8" t="s">
-        <v>99</v>
       </c>
       <c r="D25" s="7" t="s">
         <v>5</v>
@@ -1638,13 +1638,13 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="C26" s="8" t="s">
         <v>100</v>
-      </c>
-      <c r="B26" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="C26" s="8" t="s">
-        <v>101</v>
       </c>
       <c r="D26" s="7" t="s">
         <v>5</v>
@@ -1653,13 +1653,13 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="B27" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="B27" s="7" t="s">
+      <c r="C27" s="8" t="s">
         <v>105</v>
-      </c>
-      <c r="C27" s="8" t="s">
-        <v>106</v>
       </c>
       <c r="D27" s="7" t="s">
         <v>5</v>
@@ -1668,13 +1668,13 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="B28" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="B28" s="7" t="s">
+      <c r="C28" s="9" t="s">
         <v>108</v>
-      </c>
-      <c r="C28" s="9" t="s">
-        <v>109</v>
       </c>
       <c r="D28" s="7" t="s">
         <v>5</v>
@@ -1683,13 +1683,13 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="C29" s="11" t="s">
         <v>110</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="C29" s="11" t="s">
-        <v>111</v>
       </c>
       <c r="D29" s="7" t="s">
         <v>5</v>
@@ -1698,13 +1698,13 @@
     </row>
     <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D30" s="7" t="s">
         <v>5</v>
@@ -1713,13 +1713,13 @@
     </row>
     <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="B31" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="B31" s="9" t="s">
+      <c r="C31" s="11" t="s">
         <v>117</v>
-      </c>
-      <c r="C31" s="11" t="s">
-        <v>118</v>
       </c>
       <c r="D31" s="7" t="s">
         <v>5</v>
@@ -1728,13 +1728,13 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B32" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="C32" s="8" t="s">
         <v>123</v>
-      </c>
-      <c r="C32" s="8" t="s">
-        <v>124</v>
       </c>
       <c r="D32" s="9" t="s">
         <v>5</v>
@@ -1743,13 +1743,13 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D33" s="9" t="s">
         <v>5</v>
@@ -1758,13 +1758,13 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="C34" s="8" t="s">
         <v>127</v>
-      </c>
-      <c r="B34" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="C34" s="8" t="s">
-        <v>128</v>
       </c>
       <c r="D34" s="9" t="s">
         <v>5</v>
@@ -1773,13 +1773,13 @@
     </row>
     <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="B35" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="B35" s="7" t="s">
+      <c r="C35" s="8" t="s">
         <v>131</v>
-      </c>
-      <c r="C35" s="8" t="s">
-        <v>132</v>
       </c>
       <c r="D35" s="7" t="s">
         <v>5</v>
@@ -1788,13 +1788,13 @@
     </row>
     <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="C36" s="8" t="s">
         <v>133</v>
-      </c>
-      <c r="B36" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="C36" s="8" t="s">
-        <v>134</v>
       </c>
       <c r="D36" s="7" t="s">
         <v>5</v>
@@ -1803,13 +1803,13 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="C37" s="8" t="s">
         <v>136</v>
-      </c>
-      <c r="B37" s="7" t="s">
-        <v>138</v>
-      </c>
-      <c r="C37" s="8" t="s">
-        <v>137</v>
       </c>
       <c r="D37" s="7" t="s">
         <v>5</v>
@@ -1818,13 +1818,13 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="C38" s="9" t="s">
         <v>139</v>
-      </c>
-      <c r="B38" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="C38" s="9" t="s">
-        <v>140</v>
       </c>
       <c r="D38" s="9" t="s">
         <v>5</v>
@@ -1833,13 +1833,13 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="C39" s="11" t="s">
         <v>142</v>
-      </c>
-      <c r="B39" s="7" t="s">
-        <v>144</v>
-      </c>
-      <c r="C39" s="11" t="s">
-        <v>143</v>
       </c>
       <c r="D39" s="9" t="s">
         <v>5</v>
@@ -1848,13 +1848,13 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="9" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B40" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="C40" s="11" t="s">
         <v>145</v>
-      </c>
-      <c r="C40" s="11" t="s">
-        <v>147</v>
       </c>
       <c r="D40" s="9" t="s">
         <v>5</v>
@@ -1863,13 +1863,13 @@
     </row>
     <row r="41" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>149</v>
+        <v>252</v>
       </c>
       <c r="C41" s="11" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D41" s="9" t="s">
         <v>5</v>
@@ -1878,13 +1878,13 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="9" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D42" s="7" t="s">
         <v>5</v>
@@ -1893,13 +1893,13 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="9" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D43" s="9" t="s">
         <v>5</v>
@@ -1908,13 +1908,13 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="9" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>158</v>
+        <v>254</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="D44" s="9" t="s">
         <v>5</v>
@@ -1923,13 +1923,13 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="9" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C45" s="11" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="D45" s="9" t="s">
         <v>5</v>
@@ -1938,13 +1938,13 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="B46" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="C46" s="12" t="s">
         <v>163</v>
-      </c>
-      <c r="B46" s="13" t="s">
-        <v>168</v>
-      </c>
-      <c r="C46" s="12" t="s">
-        <v>167</v>
       </c>
       <c r="D46" s="12" t="s">
         <v>5</v>
@@ -1953,13 +1953,13 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="12" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="B47" s="13" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="C47" s="11" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D47" s="12" t="s">
         <v>5</v>
@@ -1968,13 +1968,13 @@
     </row>
     <row r="48" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="12" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B48" s="13" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C48" s="11" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="D48" s="12" t="s">
         <v>5</v>
@@ -1983,13 +1983,13 @@
     </row>
     <row r="49" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="12" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="B49" s="13" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="C49" s="11" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D49" s="12" t="s">
         <v>5</v>
@@ -1998,13 +1998,13 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="12" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="B50" s="13" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C50" s="11" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="D50" s="12" t="s">
         <v>5</v>
@@ -2013,13 +2013,13 @@
     </row>
     <row r="51" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="9" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C51" s="11" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="D51" s="9" t="s">
         <v>5</v>
@@ -2028,13 +2028,13 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="9" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="C52" s="11" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="D52" s="7" t="s">
         <v>5</v>
@@ -2043,13 +2043,13 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="9" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="C53" s="11" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="D53" s="12" t="s">
         <v>5</v>
@@ -2058,13 +2058,13 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="B54" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="C54" s="11" t="s">
         <v>185</v>
-      </c>
-      <c r="B54" s="7" t="s">
-        <v>188</v>
-      </c>
-      <c r="C54" s="11" t="s">
-        <v>189</v>
       </c>
       <c r="D54" s="7" t="s">
         <v>5</v>
@@ -2073,13 +2073,13 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="9" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="C55" s="11" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D55" s="7" t="s">
         <v>5</v>
@@ -2088,13 +2088,13 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C56" s="11" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="D56" s="7" t="s">
         <v>5</v>
@@ -2103,13 +2103,13 @@
     </row>
     <row r="57" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="9" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="C57" s="11" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="D57" s="9" t="s">
         <v>5</v>
@@ -2118,13 +2118,13 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="9" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="B58" s="9" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="D58" s="9" t="s">
         <v>5</v>
@@ -2133,13 +2133,13 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="C59" s="8" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="D59" s="7" t="s">
         <v>5</v>
@@ -2148,13 +2148,13 @@
     </row>
     <row r="60" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="C60" s="14" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="D60" s="7" t="s">
         <v>5</v>
@@ -2163,13 +2163,13 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="9" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="B61" s="9" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="C61" s="7" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D61" s="9" t="s">
         <v>5</v>
@@ -2178,13 +2178,13 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="9" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="B62" s="9" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="C62" s="8" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="D62" s="9" t="s">
         <v>5</v>
@@ -2193,13 +2193,13 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="9" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="B63" s="9" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="C63" s="8" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="D63" s="9" t="s">
         <v>5</v>
@@ -2208,13 +2208,13 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="9" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="B64" s="9" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="C64" s="8" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="D64" s="9" t="s">
         <v>5</v>
@@ -2223,13 +2223,13 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="9" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="B65" s="9" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="C65" s="8" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="D65" s="9" t="s">
         <v>5</v>
@@ -2238,13 +2238,13 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="9" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="B66" s="9" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="C66" s="9" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="D66" s="9" t="s">
         <v>5</v>
@@ -2253,13 +2253,13 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="9" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="B67" s="9" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="C67" s="9" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="D67" s="9" t="s">
         <v>5</v>
@@ -2268,13 +2268,13 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="9" t="s">
+        <v>225</v>
+      </c>
+      <c r="B68" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="C68" s="9" t="s">
         <v>229</v>
-      </c>
-      <c r="B68" s="9" t="s">
-        <v>232</v>
-      </c>
-      <c r="C68" s="9" t="s">
-        <v>233</v>
       </c>
       <c r="D68" s="9" t="s">
         <v>5</v>
@@ -2283,13 +2283,13 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="9" t="s">
+        <v>226</v>
+      </c>
+      <c r="B69" s="9" t="s">
         <v>230</v>
       </c>
-      <c r="B69" s="9" t="s">
-        <v>234</v>
-      </c>
       <c r="C69" s="9" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="D69" s="9" t="s">
         <v>5</v>
@@ -2298,13 +2298,13 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="9" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="B70" s="9" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="C70" s="9" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="D70" s="9" t="s">
         <v>5</v>
@@ -2313,13 +2313,13 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="9" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="B71" s="9" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="C71" s="7" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="D71" s="9" t="s">
         <v>5</v>
@@ -2328,13 +2328,13 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="15" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="B72" s="9" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="C72" s="6" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="D72" s="15" t="s">
         <v>5</v>
@@ -2343,13 +2343,13 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="15" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="B73" s="9" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="C73" s="16" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="D73" s="15" t="s">
         <v>5</v>
@@ -2358,13 +2358,13 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="15" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="B74" s="9" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="C74" s="6" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="D74" s="15" t="s">
         <v>5</v>
@@ -2373,13 +2373,13 @@
     </row>
     <row r="75" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" s="15" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="B75" s="9" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="C75" s="6" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="D75" s="15" t="s">
         <v>5</v>
@@ -2388,13 +2388,13 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="15" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="B76" s="9" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="C76" s="6" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="D76" s="15" t="s">
         <v>5</v>
@@ -2414,8 +2414,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:XFD19"/>
+    <sheetView topLeftCell="A10" zoomScale="80" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2562,7 +2562,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B12" s="7" t="s">
         <v>37</v>
@@ -2574,7 +2574,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>37</v>
@@ -2586,7 +2586,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>37</v>
@@ -2598,7 +2598,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B15" s="7" t="s">
         <v>37</v>
@@ -2610,7 +2610,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B16" s="7" t="s">
         <v>37</v>
@@ -2622,7 +2622,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B17" s="7" t="s">
         <v>37</v>
@@ -2634,7 +2634,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B18" s="7" t="s">
         <v>37</v>
@@ -2646,7 +2646,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B19" s="7" t="s">
         <v>37</v>
@@ -2658,7 +2658,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B20" s="7" t="s">
         <v>37</v>
@@ -2670,7 +2670,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B21" s="7" t="s">
         <v>37</v>
@@ -2682,7 +2682,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B22" s="7" t="s">
         <v>37</v>
@@ -2694,7 +2694,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B23" s="7" t="s">
         <v>37</v>
@@ -2706,7 +2706,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B24" s="7" t="s">
         <v>37</v>
@@ -2718,7 +2718,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B25" s="7" t="s">
         <v>37</v>
@@ -2730,7 +2730,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="B26" s="7" t="s">
         <v>37</v>

</xml_diff>

<commit_message>
Adds WAT85 and WAT86 testscripts
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/WAT.xlsx
+++ b/src/test/resources/xls/WAT.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13305" windowHeight="2415"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22830" windowHeight="7965"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="261">
   <si>
     <t>TCID</t>
   </si>
@@ -52,9 +52,6 @@
   </si>
   <si>
     <t>WAT03</t>
-  </si>
-  <si>
-    <t>WAT-162||WAT-507||WAT-215||WAT-220</t>
   </si>
   <si>
     <t>WAT04</t>
@@ -785,6 +782,24 @@
   </si>
   <si>
     <t>WAT-323||WAT-297</t>
+  </si>
+  <si>
+    <t>WAT-162||WAT-507||WAT-215||WAT-220||WAT-315</t>
+  </si>
+  <si>
+    <t>WAT85</t>
+  </si>
+  <si>
+    <t>WAT-584</t>
+  </si>
+  <si>
+    <t>WAT86</t>
+  </si>
+  <si>
+    <t>Verify that Symbol (-) works for only LN</t>
+  </si>
+  <si>
+    <t>Verify that Symbol (-) works for both LN&amp;FN</t>
   </si>
 </sst>
 </file>
@@ -1244,10 +1259,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E76"/>
+  <dimension ref="A1:E78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C78" sqref="C78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1299,7 +1314,7 @@
         <v>10</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>5</v>
@@ -1311,10 +1326,10 @@
         <v>11</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>12</v>
+        <v>255</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>5</v>
@@ -1323,13 +1338,13 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="C5" s="8" t="s">
         <v>13</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>14</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>5</v>
@@ -1338,13 +1353,13 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="8" t="s">
         <v>15</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>16</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>5</v>
@@ -1353,13 +1368,13 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="C7" s="8" t="s">
         <v>19</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>20</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>5</v>
@@ -1368,13 +1383,13 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="8" t="s">
         <v>21</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>22</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>5</v>
@@ -1383,13 +1398,13 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>5</v>
@@ -1398,13 +1413,13 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>5</v>
@@ -1413,13 +1428,13 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D11" s="7" t="s">
         <v>5</v>
@@ -1428,13 +1443,13 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D12" s="7" t="s">
         <v>5</v>
@@ -1443,13 +1458,13 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>5</v>
@@ -1458,13 +1473,13 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D14" s="7" t="s">
         <v>5</v>
@@ -1473,13 +1488,13 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D15" s="7" t="s">
         <v>5</v>
@@ -1488,13 +1503,13 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D16" s="7" t="s">
         <v>5</v>
@@ -1503,13 +1518,13 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B17" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C17" s="8" t="s">
         <v>77</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>78</v>
       </c>
       <c r="D17" s="7" t="s">
         <v>5</v>
@@ -1518,13 +1533,13 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="B18" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="B18" s="9" t="s">
-        <v>77</v>
-      </c>
       <c r="C18" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D18" s="7" t="s">
         <v>5</v>
@@ -1533,13 +1548,13 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="B19" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="B19" s="9" t="s">
-        <v>81</v>
-      </c>
       <c r="C19" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D19" s="9" t="s">
         <v>5</v>
@@ -1548,13 +1563,13 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D20" s="9" t="s">
         <v>5</v>
@@ -1563,13 +1578,13 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D21" s="9" t="s">
         <v>5</v>
@@ -1578,13 +1593,13 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="B22" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="B22" s="7" t="s">
-        <v>90</v>
-      </c>
       <c r="C22" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D22" s="9" t="s">
         <v>5</v>
@@ -1593,13 +1608,13 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D23" s="9" t="s">
         <v>5</v>
@@ -1608,13 +1623,13 @@
     </row>
     <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="C24" s="11" t="s">
         <v>95</v>
-      </c>
-      <c r="B24" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="C24" s="11" t="s">
-        <v>96</v>
       </c>
       <c r="D24" s="7" t="s">
         <v>5</v>
@@ -1623,13 +1638,13 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="C25" s="8" t="s">
         <v>97</v>
-      </c>
-      <c r="B25" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="C25" s="8" t="s">
-        <v>98</v>
       </c>
       <c r="D25" s="7" t="s">
         <v>5</v>
@@ -1638,13 +1653,13 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="C26" s="8" t="s">
         <v>99</v>
-      </c>
-      <c r="B26" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="C26" s="8" t="s">
-        <v>100</v>
       </c>
       <c r="D26" s="7" t="s">
         <v>5</v>
@@ -1653,13 +1668,13 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="B27" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="B27" s="7" t="s">
+      <c r="C27" s="8" t="s">
         <v>104</v>
-      </c>
-      <c r="C27" s="8" t="s">
-        <v>105</v>
       </c>
       <c r="D27" s="7" t="s">
         <v>5</v>
@@ -1668,13 +1683,13 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="B28" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="B28" s="7" t="s">
+      <c r="C28" s="9" t="s">
         <v>107</v>
-      </c>
-      <c r="C28" s="9" t="s">
-        <v>108</v>
       </c>
       <c r="D28" s="7" t="s">
         <v>5</v>
@@ -1683,13 +1698,13 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="C29" s="11" t="s">
         <v>109</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="C29" s="11" t="s">
-        <v>110</v>
       </c>
       <c r="D29" s="7" t="s">
         <v>5</v>
@@ -1698,13 +1713,13 @@
     </row>
     <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D30" s="7" t="s">
         <v>5</v>
@@ -1713,13 +1728,13 @@
     </row>
     <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="B31" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="B31" s="9" t="s">
+      <c r="C31" s="11" t="s">
         <v>116</v>
-      </c>
-      <c r="C31" s="11" t="s">
-        <v>117</v>
       </c>
       <c r="D31" s="7" t="s">
         <v>5</v>
@@ -1728,13 +1743,13 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B32" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="C32" s="8" t="s">
         <v>122</v>
-      </c>
-      <c r="C32" s="8" t="s">
-        <v>123</v>
       </c>
       <c r="D32" s="9" t="s">
         <v>5</v>
@@ -1743,13 +1758,13 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D33" s="9" t="s">
         <v>5</v>
@@ -1758,13 +1773,13 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="C34" s="8" t="s">
         <v>126</v>
-      </c>
-      <c r="B34" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="C34" s="8" t="s">
-        <v>127</v>
       </c>
       <c r="D34" s="9" t="s">
         <v>5</v>
@@ -1773,13 +1788,13 @@
     </row>
     <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="B35" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="B35" s="7" t="s">
+      <c r="C35" s="8" t="s">
         <v>130</v>
-      </c>
-      <c r="C35" s="8" t="s">
-        <v>131</v>
       </c>
       <c r="D35" s="7" t="s">
         <v>5</v>
@@ -1788,13 +1803,13 @@
     </row>
     <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="C36" s="8" t="s">
         <v>132</v>
-      </c>
-      <c r="B36" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="C36" s="8" t="s">
-        <v>133</v>
       </c>
       <c r="D36" s="7" t="s">
         <v>5</v>
@@ -1803,13 +1818,13 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="C37" s="8" t="s">
         <v>135</v>
-      </c>
-      <c r="B37" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="C37" s="8" t="s">
-        <v>136</v>
       </c>
       <c r="D37" s="7" t="s">
         <v>5</v>
@@ -1818,13 +1833,13 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="C38" s="9" t="s">
         <v>138</v>
-      </c>
-      <c r="B38" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="C38" s="9" t="s">
-        <v>139</v>
       </c>
       <c r="D38" s="9" t="s">
         <v>5</v>
@@ -1833,13 +1848,13 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="C39" s="11" t="s">
         <v>141</v>
-      </c>
-      <c r="B39" s="7" t="s">
-        <v>255</v>
-      </c>
-      <c r="C39" s="11" t="s">
-        <v>142</v>
       </c>
       <c r="D39" s="9" t="s">
         <v>5</v>
@@ -1848,13 +1863,13 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="B40" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="C40" s="11" t="s">
         <v>144</v>
-      </c>
-      <c r="B40" s="9" t="s">
-        <v>143</v>
-      </c>
-      <c r="C40" s="11" t="s">
-        <v>145</v>
       </c>
       <c r="D40" s="9" t="s">
         <v>5</v>
@@ -1863,13 +1878,13 @@
     </row>
     <row r="41" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>251</v>
+      </c>
+      <c r="C41" s="11" t="s">
         <v>146</v>
-      </c>
-      <c r="B41" s="9" t="s">
-        <v>252</v>
-      </c>
-      <c r="C41" s="11" t="s">
-        <v>147</v>
       </c>
       <c r="D41" s="9" t="s">
         <v>5</v>
@@ -1878,13 +1893,13 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="B42" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="B42" s="7" t="s">
+      <c r="C42" s="9" t="s">
         <v>149</v>
-      </c>
-      <c r="C42" s="9" t="s">
-        <v>150</v>
       </c>
       <c r="D42" s="7" t="s">
         <v>5</v>
@@ -1893,13 +1908,13 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="B43" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="B43" s="7" t="s">
+      <c r="C43" s="9" t="s">
         <v>152</v>
-      </c>
-      <c r="C43" s="9" t="s">
-        <v>153</v>
       </c>
       <c r="D43" s="9" t="s">
         <v>5</v>
@@ -1908,13 +1923,13 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="C44" s="9" t="s">
         <v>154</v>
-      </c>
-      <c r="B44" s="7" t="s">
-        <v>254</v>
-      </c>
-      <c r="C44" s="9" t="s">
-        <v>155</v>
       </c>
       <c r="D44" s="9" t="s">
         <v>5</v>
@@ -1923,13 +1938,13 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="B45" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="B45" s="7" t="s">
+      <c r="C45" s="11" t="s">
         <v>157</v>
-      </c>
-      <c r="C45" s="11" t="s">
-        <v>158</v>
       </c>
       <c r="D45" s="9" t="s">
         <v>5</v>
@@ -1938,13 +1953,13 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="12" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B46" s="13" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C46" s="12" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D46" s="12" t="s">
         <v>5</v>
@@ -1953,13 +1968,13 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="12" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B47" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="C47" s="11" t="s">
         <v>166</v>
-      </c>
-      <c r="C47" s="11" t="s">
-        <v>167</v>
       </c>
       <c r="D47" s="12" t="s">
         <v>5</v>
@@ -1968,13 +1983,13 @@
     </row>
     <row r="48" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="12" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B48" s="13" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C48" s="11" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D48" s="12" t="s">
         <v>5</v>
@@ -1983,13 +1998,13 @@
     </row>
     <row r="49" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="12" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B49" s="13" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C49" s="11" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D49" s="12" t="s">
         <v>5</v>
@@ -1998,13 +2013,13 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="12" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B50" s="13" t="s">
+        <v>170</v>
+      </c>
+      <c r="C50" s="11" t="s">
         <v>171</v>
-      </c>
-      <c r="C50" s="11" t="s">
-        <v>172</v>
       </c>
       <c r="D50" s="12" t="s">
         <v>5</v>
@@ -2013,13 +2028,13 @@
     </row>
     <row r="51" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C51" s="11" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D51" s="9" t="s">
         <v>5</v>
@@ -2028,13 +2043,13 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="9" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B52" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="C52" s="11" t="s">
         <v>177</v>
-      </c>
-      <c r="C52" s="11" t="s">
-        <v>178</v>
       </c>
       <c r="D52" s="7" t="s">
         <v>5</v>
@@ -2043,13 +2058,13 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="9" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B53" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="C53" s="11" t="s">
         <v>182</v>
-      </c>
-      <c r="C53" s="11" t="s">
-        <v>183</v>
       </c>
       <c r="D53" s="12" t="s">
         <v>5</v>
@@ -2058,13 +2073,13 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="9" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B54" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="C54" s="11" t="s">
         <v>184</v>
-      </c>
-      <c r="C54" s="11" t="s">
-        <v>185</v>
       </c>
       <c r="D54" s="7" t="s">
         <v>5</v>
@@ -2073,13 +2088,13 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="B55" s="7" t="s">
         <v>186</v>
       </c>
-      <c r="B55" s="7" t="s">
+      <c r="C55" s="11" t="s">
         <v>187</v>
-      </c>
-      <c r="C55" s="11" t="s">
-        <v>188</v>
       </c>
       <c r="D55" s="7" t="s">
         <v>5</v>
@@ -2088,13 +2103,13 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="B56" s="7" t="s">
         <v>189</v>
       </c>
-      <c r="B56" s="7" t="s">
+      <c r="C56" s="11" t="s">
         <v>190</v>
-      </c>
-      <c r="C56" s="11" t="s">
-        <v>191</v>
       </c>
       <c r="D56" s="7" t="s">
         <v>5</v>
@@ -2103,13 +2118,13 @@
     </row>
     <row r="57" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="B57" s="7" t="s">
         <v>192</v>
       </c>
-      <c r="B57" s="7" t="s">
+      <c r="C57" s="11" t="s">
         <v>193</v>
-      </c>
-      <c r="C57" s="11" t="s">
-        <v>194</v>
       </c>
       <c r="D57" s="9" t="s">
         <v>5</v>
@@ -2118,13 +2133,13 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="B58" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="C58" s="7" t="s">
         <v>195</v>
-      </c>
-      <c r="B58" s="9" t="s">
-        <v>211</v>
-      </c>
-      <c r="C58" s="7" t="s">
-        <v>196</v>
       </c>
       <c r="D58" s="9" t="s">
         <v>5</v>
@@ -2133,13 +2148,13 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="B59" s="7" t="s">
         <v>197</v>
       </c>
-      <c r="B59" s="7" t="s">
+      <c r="C59" s="8" t="s">
         <v>198</v>
-      </c>
-      <c r="C59" s="8" t="s">
-        <v>199</v>
       </c>
       <c r="D59" s="7" t="s">
         <v>5</v>
@@ -2148,13 +2163,13 @@
     </row>
     <row r="60" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="B60" s="7" t="s">
         <v>200</v>
       </c>
-      <c r="B60" s="7" t="s">
+      <c r="C60" s="14" t="s">
         <v>201</v>
-      </c>
-      <c r="C60" s="14" t="s">
-        <v>202</v>
       </c>
       <c r="D60" s="7" t="s">
         <v>5</v>
@@ -2163,13 +2178,13 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="B61" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="C61" s="7" t="s">
         <v>203</v>
-      </c>
-      <c r="B61" s="9" t="s">
-        <v>212</v>
-      </c>
-      <c r="C61" s="7" t="s">
-        <v>204</v>
       </c>
       <c r="D61" s="9" t="s">
         <v>5</v>
@@ -2178,13 +2193,13 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="B62" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="C62" s="8" t="s">
         <v>205</v>
-      </c>
-      <c r="B62" s="9" t="s">
-        <v>213</v>
-      </c>
-      <c r="C62" s="8" t="s">
-        <v>206</v>
       </c>
       <c r="D62" s="9" t="s">
         <v>5</v>
@@ -2193,13 +2208,13 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="B63" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="C63" s="8" t="s">
         <v>207</v>
-      </c>
-      <c r="B63" s="9" t="s">
-        <v>214</v>
-      </c>
-      <c r="C63" s="8" t="s">
-        <v>208</v>
       </c>
       <c r="D63" s="9" t="s">
         <v>5</v>
@@ -2208,13 +2223,13 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="9" t="s">
+        <v>208</v>
+      </c>
+      <c r="B64" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="C64" s="8" t="s">
         <v>209</v>
-      </c>
-      <c r="B64" s="9" t="s">
-        <v>215</v>
-      </c>
-      <c r="C64" s="8" t="s">
-        <v>210</v>
       </c>
       <c r="D64" s="9" t="s">
         <v>5</v>
@@ -2223,13 +2238,13 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="9" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B65" s="9" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C65" s="8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D65" s="9" t="s">
         <v>5</v>
@@ -2238,13 +2253,13 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="9" t="s">
+        <v>218</v>
+      </c>
+      <c r="B66" s="9" t="s">
+        <v>220</v>
+      </c>
+      <c r="C66" s="9" t="s">
         <v>219</v>
-      </c>
-      <c r="B66" s="9" t="s">
-        <v>221</v>
-      </c>
-      <c r="C66" s="9" t="s">
-        <v>220</v>
       </c>
       <c r="D66" s="9" t="s">
         <v>5</v>
@@ -2253,13 +2268,13 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="9" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B67" s="9" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C67" s="9" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D67" s="9" t="s">
         <v>5</v>
@@ -2268,13 +2283,13 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="9" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B68" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="C68" s="9" t="s">
         <v>228</v>
-      </c>
-      <c r="C68" s="9" t="s">
-        <v>229</v>
       </c>
       <c r="D68" s="9" t="s">
         <v>5</v>
@@ -2283,13 +2298,13 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="9" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B69" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="C69" s="9" t="s">
         <v>230</v>
-      </c>
-      <c r="C69" s="9" t="s">
-        <v>231</v>
       </c>
       <c r="D69" s="9" t="s">
         <v>5</v>
@@ -2298,13 +2313,13 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="9" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B70" s="9" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C70" s="9" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D70" s="9" t="s">
         <v>5</v>
@@ -2313,13 +2328,13 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="B71" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="C71" s="7" t="s">
         <v>234</v>
-      </c>
-      <c r="B71" s="9" t="s">
-        <v>236</v>
-      </c>
-      <c r="C71" s="7" t="s">
-        <v>235</v>
       </c>
       <c r="D71" s="9" t="s">
         <v>5</v>
@@ -2328,13 +2343,13 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="15" t="s">
+        <v>237</v>
+      </c>
+      <c r="B72" s="9" t="s">
         <v>238</v>
       </c>
-      <c r="B72" s="9" t="s">
-        <v>239</v>
-      </c>
       <c r="C72" s="6" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D72" s="15" t="s">
         <v>5</v>
@@ -2343,13 +2358,13 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="15" t="s">
+        <v>239</v>
+      </c>
+      <c r="B73" s="9" t="s">
         <v>240</v>
       </c>
-      <c r="B73" s="9" t="s">
+      <c r="C73" s="16" t="s">
         <v>241</v>
-      </c>
-      <c r="C73" s="16" t="s">
-        <v>242</v>
       </c>
       <c r="D73" s="15" t="s">
         <v>5</v>
@@ -2358,13 +2373,13 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="15" t="s">
+        <v>243</v>
+      </c>
+      <c r="B74" s="9" t="s">
         <v>244</v>
       </c>
-      <c r="B74" s="9" t="s">
-        <v>245</v>
-      </c>
       <c r="C74" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D74" s="15" t="s">
         <v>5</v>
@@ -2373,13 +2388,13 @@
     </row>
     <row r="75" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" s="15" t="s">
+        <v>245</v>
+      </c>
+      <c r="B75" s="9" t="s">
+        <v>247</v>
+      </c>
+      <c r="C75" s="6" t="s">
         <v>246</v>
-      </c>
-      <c r="B75" s="9" t="s">
-        <v>248</v>
-      </c>
-      <c r="C75" s="6" t="s">
-        <v>247</v>
       </c>
       <c r="D75" s="15" t="s">
         <v>5</v>
@@ -2388,15 +2403,43 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="15" t="s">
+        <v>248</v>
+      </c>
+      <c r="B76" s="9" t="s">
         <v>249</v>
       </c>
-      <c r="B76" s="9" t="s">
+      <c r="C76" s="6" t="s">
         <v>250</v>
       </c>
-      <c r="C76" s="6" t="s">
-        <v>251</v>
-      </c>
       <c r="D76" s="15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" s="15" t="s">
+        <v>256</v>
+      </c>
+      <c r="B77" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="C77" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="D77" s="15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" s="15" t="s">
+        <v>258</v>
+      </c>
+      <c r="B78" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="C78" s="6" t="s">
+        <v>260</v>
+      </c>
+      <c r="D78" s="15" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2428,10 +2471,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C1" s="10" t="s">
         <v>2</v>
@@ -2442,10 +2485,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>5</v>
@@ -2454,10 +2497,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>5</v>
@@ -2466,10 +2509,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>5</v>
@@ -2478,10 +2521,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>5</v>
@@ -2490,10 +2533,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>5</v>
@@ -2502,10 +2545,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>5</v>
@@ -2514,10 +2557,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>5</v>
@@ -2526,10 +2569,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>5</v>
@@ -2538,10 +2581,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>5</v>
@@ -2550,10 +2593,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>5</v>
@@ -2562,10 +2605,10 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>5</v>
@@ -2574,10 +2617,10 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>5</v>
@@ -2586,10 +2629,10 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>5</v>
@@ -2598,10 +2641,10 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>5</v>
@@ -2610,10 +2653,10 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>5</v>
@@ -2622,10 +2665,10 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C17" s="7" t="s">
         <v>5</v>
@@ -2634,10 +2677,10 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C18" s="7" t="s">
         <v>5</v>
@@ -2646,10 +2689,10 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C19" s="7" t="s">
         <v>5</v>
@@ -2658,10 +2701,10 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C20" s="7" t="s">
         <v>5</v>
@@ -2670,10 +2713,10 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C21" s="7" t="s">
         <v>5</v>
@@ -2682,10 +2725,10 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C22" s="7" t="s">
         <v>5</v>
@@ -2694,10 +2737,10 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C23" s="7" t="s">
         <v>5</v>
@@ -2706,10 +2749,10 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C24" s="7" t="s">
         <v>5</v>
@@ -2718,10 +2761,10 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C25" s="7" t="s">
         <v>5</v>
@@ -2730,10 +2773,10 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C26" s="7" t="s">
         <v>5</v>
@@ -2764,10 +2807,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C1" s="10" t="s">
         <v>2</v>
@@ -2778,10 +2821,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>5</v>
@@ -2790,10 +2833,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>5</v>
@@ -2802,10 +2845,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>5</v>
@@ -2814,10 +2857,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>5</v>
@@ -2826,10 +2869,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>5</v>
@@ -2838,10 +2881,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>5</v>
@@ -2850,10 +2893,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>5</v>
@@ -2862,10 +2905,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>5</v>
@@ -2874,10 +2917,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>5</v>
@@ -2886,10 +2929,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>5</v>
@@ -2898,10 +2941,10 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>5</v>
@@ -2910,10 +2953,10 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>5</v>
@@ -2922,10 +2965,10 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>5</v>
@@ -2934,10 +2977,10 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>5</v>
@@ -2946,10 +2989,10 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>5</v>
@@ -2958,10 +3001,10 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C17" s="7" t="s">
         <v>5</v>
@@ -2970,10 +3013,10 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C18" s="7" t="s">
         <v>5</v>
@@ -2982,10 +3025,10 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C19" s="7" t="s">
         <v>5</v>
@@ -2994,10 +3037,10 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C20" s="7" t="s">
         <v>5</v>
@@ -3006,10 +3049,10 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C21" s="7" t="s">
         <v>5</v>
@@ -3018,10 +3061,10 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C22" s="7" t="s">
         <v>5</v>
@@ -3030,10 +3073,10 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C23" s="7" t="s">
         <v>5</v>
@@ -3042,10 +3085,10 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C24" s="7" t="s">
         <v>5</v>
@@ -3054,10 +3097,10 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C25" s="7" t="s">
         <v>5</v>
@@ -3066,10 +3109,10 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C26" s="7" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
Adds WAT87 test script
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/WAT.xlsx
+++ b/src/test/resources/xls/WAT.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="264">
   <si>
     <t>TCID</t>
   </si>
@@ -790,9 +790,6 @@
     <t>WAT85</t>
   </si>
   <si>
-    <t>WAT-584</t>
-  </si>
-  <si>
     <t>WAT86</t>
   </si>
   <si>
@@ -800,6 +797,18 @@
   </si>
   <si>
     <t>Verify that Symbol (-) works for both LN&amp;FN</t>
+  </si>
+  <si>
+    <t>WAT-584||WAT-583</t>
+  </si>
+  <si>
+    <t>WAT87</t>
+  </si>
+  <si>
+    <t>WAT-582</t>
+  </si>
+  <si>
+    <t>Verify that when user gets into Author search page there will be no (-) symbol present</t>
   </si>
 </sst>
 </file>
@@ -1259,10 +1268,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E78"/>
+  <dimension ref="A1:E79"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A70" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C78" sqref="C78"/>
+      <selection activeCell="C87" sqref="C87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2420,10 +2429,10 @@
         <v>256</v>
       </c>
       <c r="B77" s="9" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="C77" s="6" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D77" s="15" t="s">
         <v>5</v>
@@ -2431,15 +2440,29 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="15" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B78" s="9" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="C78" s="6" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D78" s="15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="B79" s="9" t="s">
+        <v>262</v>
+      </c>
+      <c r="C79" s="6" t="s">
+        <v>263</v>
+      </c>
+      <c r="D79" s="15" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adds WAT 89,90,91 testscript
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/WAT.xlsx
+++ b/src/test/resources/xls/WAT.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="276">
   <si>
     <t>TCID</t>
   </si>
@@ -818,6 +818,33 @@
   </si>
   <si>
     <t>Verify that upon clicking the symbol (-) corresponding LN &amp; FN should be deleted</t>
+  </si>
+  <si>
+    <t>WAT89</t>
+  </si>
+  <si>
+    <t>Verify that user should able to access feedback survey page using 'Tell us what you think' link within the informational text on the author Search page</t>
+  </si>
+  <si>
+    <t>WAT90</t>
+  </si>
+  <si>
+    <t>WAT-637</t>
+  </si>
+  <si>
+    <t>WAT-638</t>
+  </si>
+  <si>
+    <t>Verify that user should able to access feedback survey page using 'Tell us what you think' link within the informational text on the author Search result page</t>
+  </si>
+  <si>
+    <t>WAT-639</t>
+  </si>
+  <si>
+    <t>WAT91</t>
+  </si>
+  <si>
+    <t>Verify that user should able to access feedback survey page using 'Tell us what you think' link within the informational text on the author Record page</t>
   </si>
 </sst>
 </file>
@@ -1277,10 +1304,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E80"/>
+  <dimension ref="A1:E83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C86" sqref="C86"/>
+    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C88" sqref="C88:C89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2486,6 +2513,48 @@
         <v>266</v>
       </c>
       <c r="D80" s="15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" s="15" t="s">
+        <v>267</v>
+      </c>
+      <c r="B81" s="9" t="s">
+        <v>270</v>
+      </c>
+      <c r="C81" s="6" t="s">
+        <v>268</v>
+      </c>
+      <c r="D81" s="15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A82" s="15" t="s">
+        <v>269</v>
+      </c>
+      <c r="B82" s="9" t="s">
+        <v>271</v>
+      </c>
+      <c r="C82" s="6" t="s">
+        <v>272</v>
+      </c>
+      <c r="D82" s="15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" s="15" t="s">
+        <v>274</v>
+      </c>
+      <c r="B83" s="9" t="s">
+        <v>273</v>
+      </c>
+      <c r="C83" s="6" t="s">
+        <v>275</v>
+      </c>
+      <c r="D83" s="15" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adds WAT92 test script and related changes
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/WAT.xlsx
+++ b/src/test/resources/xls/WAT.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22830" windowHeight="7965"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13305" windowHeight="2415"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -12,11 +12,12 @@
     <sheet name="WAT13" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="279">
   <si>
     <t>TCID</t>
   </si>
@@ -845,6 +846,15 @@
   </si>
   <si>
     <t>Verify that user should able to access feedback survey page using 'Tell us what you think' link within the informational text on the author Record page</t>
+  </si>
+  <si>
+    <t>WAT-190||WAT-212</t>
+  </si>
+  <si>
+    <t>WAT92</t>
+  </si>
+  <si>
+    <t>WAT-198</t>
   </si>
 </sst>
 </file>
@@ -1304,10 +1314,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E83"/>
+  <dimension ref="A1:E84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C88" sqref="C88:C89"/>
+    <sheetView tabSelected="1" topLeftCell="A81" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B81" sqref="B81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1641,7 +1651,7 @@
         <v>88</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>89</v>
+        <v>276</v>
       </c>
       <c r="C22" s="9" t="s">
         <v>91</v>
@@ -2555,6 +2565,20 @@
         <v>275</v>
       </c>
       <c r="D83" s="15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" s="15" t="s">
+        <v>277</v>
+      </c>
+      <c r="B84" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="C84" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="D84" s="15" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adds WAT93 testscript and related changes
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/WAT.xlsx
+++ b/src/test/resources/xls/WAT.xlsx
@@ -12,12 +12,11 @@
     <sheet name="WAT13" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="282">
   <si>
     <t>TCID</t>
   </si>
@@ -855,6 +854,15 @@
   </si>
   <si>
     <t>WAT-198</t>
+  </si>
+  <si>
+    <t>WAT93</t>
+  </si>
+  <si>
+    <t>WAT-166</t>
+  </si>
+  <si>
+    <t>Default LastName field value should be "Last Name"</t>
   </si>
 </sst>
 </file>
@@ -1314,10 +1322,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E84"/>
+  <dimension ref="A1:E85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A81" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B81" sqref="B81"/>
+    <sheetView tabSelected="1" topLeftCell="A75" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C90" sqref="C90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2579,6 +2587,20 @@
         <v>169</v>
       </c>
       <c r="D84" s="15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" s="15" t="s">
+        <v>279</v>
+      </c>
+      <c r="B85" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="C85" s="6" t="s">
+        <v>281</v>
+      </c>
+      <c r="D85" s="15" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adds WAT94 and related changes
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/WAT.xlsx
+++ b/src/test/resources/xls/WAT.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="285">
   <si>
     <t>TCID</t>
   </si>
@@ -863,6 +863,15 @@
   </si>
   <si>
     <t>Default LastName field value should be "Last Name"</t>
+  </si>
+  <si>
+    <t>WAT94</t>
+  </si>
+  <si>
+    <t>WAT-144</t>
+  </si>
+  <si>
+    <t>Verify that System must provide a "Search" tab on the Results page.</t>
   </si>
 </sst>
 </file>
@@ -1322,10 +1331,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E85"/>
+  <dimension ref="A1:E86"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A75" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C90" sqref="C90"/>
+      <selection activeCell="C91" sqref="C91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2601,6 +2610,20 @@
         <v>281</v>
       </c>
       <c r="D85" s="15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" s="15" t="s">
+        <v>282</v>
+      </c>
+      <c r="B86" s="9" t="s">
+        <v>283</v>
+      </c>
+      <c r="C86" s="6" t="s">
+        <v>284</v>
+      </c>
+      <c r="D86" s="15" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adds WAT95 and related changes
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/WAT.xlsx
+++ b/src/test/resources/xls/WAT.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="288">
   <si>
     <t>TCID</t>
   </si>
@@ -872,6 +872,15 @@
   </si>
   <si>
     <t>Verify that System must provide a "Search" tab on the Results page.</t>
+  </si>
+  <si>
+    <t>WAT95</t>
+  </si>
+  <si>
+    <t>WAT-139</t>
+  </si>
+  <si>
+    <t>Verify that System must navigate to the Search page when the "Search" tab is clicked.</t>
   </si>
 </sst>
 </file>
@@ -1331,10 +1340,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E86"/>
+  <dimension ref="A1:E87"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A75" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C91" sqref="C91"/>
+      <selection activeCell="C87" sqref="C87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2624,6 +2633,20 @@
         <v>284</v>
       </c>
       <c r="D86" s="15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" s="15" t="s">
+        <v>285</v>
+      </c>
+      <c r="B87" s="9" t="s">
+        <v>286</v>
+      </c>
+      <c r="C87" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="D87" s="15" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adds WAT80 testscript and related changes
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/WAT.xlsx
+++ b/src/test/resources/xls/WAT.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="291">
   <si>
     <t>TCID</t>
   </si>
@@ -881,6 +881,15 @@
   </si>
   <si>
     <t>Verify that System must navigate to the Search page when the "Search" tab is clicked.</t>
+  </si>
+  <si>
+    <t>WAT80</t>
+  </si>
+  <si>
+    <t>WAT-586</t>
+  </si>
+  <si>
+    <t>Verify the static text in Author search result page</t>
   </si>
 </sst>
 </file>
@@ -936,7 +945,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -959,22 +968,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1006,8 +1004,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1340,10 +1337,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E87"/>
+  <dimension ref="A1:E88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A75" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C87" sqref="C87"/>
+    <sheetView tabSelected="1" topLeftCell="A72" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E88" sqref="A1:E88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2423,232 +2420,259 @@
       <c r="E71" s="7"/>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72" s="15" t="s">
+      <c r="A72" s="9" t="s">
         <v>237</v>
       </c>
       <c r="B72" s="9" t="s">
         <v>238</v>
       </c>
-      <c r="C72" s="6" t="s">
+      <c r="C72" s="8" t="s">
         <v>236</v>
       </c>
-      <c r="D72" s="15" t="s">
+      <c r="D72" s="9" t="s">
         <v>5</v>
       </c>
       <c r="E72" s="7"/>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A73" s="15" t="s">
+      <c r="A73" s="9" t="s">
         <v>239</v>
       </c>
       <c r="B73" s="9" t="s">
         <v>240</v>
       </c>
-      <c r="C73" s="16" t="s">
+      <c r="C73" s="15" t="s">
         <v>241</v>
       </c>
-      <c r="D73" s="15" t="s">
+      <c r="D73" s="9" t="s">
         <v>5</v>
       </c>
       <c r="E73" s="7"/>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A74" s="15" t="s">
+      <c r="A74" s="9" t="s">
         <v>243</v>
       </c>
       <c r="B74" s="9" t="s">
         <v>244</v>
       </c>
-      <c r="C74" s="6" t="s">
+      <c r="C74" s="8" t="s">
         <v>242</v>
       </c>
-      <c r="D74" s="15" t="s">
+      <c r="D74" s="9" t="s">
         <v>5</v>
       </c>
       <c r="E74" s="7"/>
     </row>
     <row r="75" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A75" s="15" t="s">
+      <c r="A75" s="9" t="s">
         <v>245</v>
       </c>
       <c r="B75" s="9" t="s">
         <v>247</v>
       </c>
-      <c r="C75" s="6" t="s">
+      <c r="C75" s="8" t="s">
         <v>246</v>
       </c>
-      <c r="D75" s="15" t="s">
+      <c r="D75" s="9" t="s">
         <v>5</v>
       </c>
       <c r="E75" s="7"/>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A76" s="15" t="s">
+      <c r="A76" s="9" t="s">
         <v>248</v>
       </c>
       <c r="B76" s="9" t="s">
         <v>249</v>
       </c>
-      <c r="C76" s="6" t="s">
+      <c r="C76" s="8" t="s">
         <v>250</v>
       </c>
-      <c r="D76" s="15" t="s">
-        <v>5</v>
-      </c>
+      <c r="D76" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E76" s="7"/>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A77" s="15" t="s">
+      <c r="A77" s="9" t="s">
         <v>256</v>
       </c>
       <c r="B77" s="9" t="s">
         <v>260</v>
       </c>
-      <c r="C77" s="6" t="s">
+      <c r="C77" s="8" t="s">
         <v>258</v>
       </c>
-      <c r="D77" s="15" t="s">
-        <v>5</v>
-      </c>
+      <c r="D77" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E77" s="7"/>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A78" s="15" t="s">
+      <c r="A78" s="9" t="s">
         <v>257</v>
       </c>
       <c r="B78" s="9" t="s">
         <v>260</v>
       </c>
-      <c r="C78" s="6" t="s">
+      <c r="C78" s="8" t="s">
         <v>259</v>
       </c>
-      <c r="D78" s="15" t="s">
-        <v>5</v>
-      </c>
+      <c r="D78" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E78" s="7"/>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A79" s="15" t="s">
+      <c r="A79" s="9" t="s">
         <v>261</v>
       </c>
       <c r="B79" s="9" t="s">
         <v>262</v>
       </c>
-      <c r="C79" s="6" t="s">
+      <c r="C79" s="8" t="s">
         <v>263</v>
       </c>
-      <c r="D79" s="15" t="s">
-        <v>5</v>
-      </c>
+      <c r="D79" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E79" s="7"/>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A80" s="15" t="s">
+      <c r="A80" s="9" t="s">
         <v>264</v>
       </c>
       <c r="B80" s="9" t="s">
         <v>265</v>
       </c>
-      <c r="C80" s="6" t="s">
+      <c r="C80" s="8" t="s">
         <v>266</v>
       </c>
-      <c r="D80" s="15" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="15" t="s">
+      <c r="D80" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E80" s="7"/>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" s="9" t="s">
         <v>267</v>
       </c>
       <c r="B81" s="9" t="s">
         <v>270</v>
       </c>
-      <c r="C81" s="6" t="s">
+      <c r="C81" s="8" t="s">
         <v>268</v>
       </c>
-      <c r="D81" s="15" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A82" s="15" t="s">
+      <c r="D81" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E81" s="7"/>
+    </row>
+    <row r="82" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A82" s="9" t="s">
         <v>269</v>
       </c>
       <c r="B82" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="C82" s="6" t="s">
+      <c r="C82" s="8" t="s">
         <v>272</v>
       </c>
-      <c r="D82" s="15" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="15" t="s">
+      <c r="D82" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E82" s="7"/>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" s="9" t="s">
         <v>274</v>
       </c>
       <c r="B83" s="9" t="s">
         <v>273</v>
       </c>
-      <c r="C83" s="6" t="s">
+      <c r="C83" s="8" t="s">
         <v>275</v>
       </c>
-      <c r="D83" s="15" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="15" t="s">
+      <c r="D83" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E83" s="7"/>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" s="9" t="s">
         <v>277</v>
       </c>
       <c r="B84" s="9" t="s">
         <v>278</v>
       </c>
-      <c r="C84" s="6" t="s">
+      <c r="C84" s="8" t="s">
         <v>169</v>
       </c>
-      <c r="D84" s="15" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="15" t="s">
+      <c r="D84" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E84" s="7"/>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" s="9" t="s">
         <v>279</v>
       </c>
       <c r="B85" s="9" t="s">
         <v>280</v>
       </c>
-      <c r="C85" s="6" t="s">
+      <c r="C85" s="8" t="s">
         <v>281</v>
       </c>
-      <c r="D85" s="15" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="15" t="s">
+      <c r="D85" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E85" s="7"/>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" s="9" t="s">
         <v>282</v>
       </c>
       <c r="B86" s="9" t="s">
         <v>283</v>
       </c>
-      <c r="C86" s="6" t="s">
+      <c r="C86" s="8" t="s">
         <v>284</v>
       </c>
-      <c r="D86" s="15" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" s="15" t="s">
+      <c r="D86" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E86" s="7"/>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87" s="9" t="s">
         <v>285</v>
       </c>
       <c r="B87" s="9" t="s">
         <v>286</v>
       </c>
-      <c r="C87" s="6" t="s">
+      <c r="C87" s="8" t="s">
         <v>287</v>
       </c>
-      <c r="D87" s="15" t="s">
-        <v>5</v>
-      </c>
+      <c r="D87" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E87" s="7"/>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88" s="9" t="s">
+        <v>288</v>
+      </c>
+      <c r="B88" s="9" t="s">
+        <v>289</v>
+      </c>
+      <c r="C88" s="8" t="s">
+        <v>290</v>
+      </c>
+      <c r="D88" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E88" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Adds WAT96 and WAT97 testscript and related changes
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/WAT.xlsx
+++ b/src/test/resources/xls/WAT.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="297">
   <si>
     <t>TCID</t>
   </si>
@@ -890,6 +890,24 @@
   </si>
   <si>
     <t>Verify the static text in Author search result page</t>
+  </si>
+  <si>
+    <t>WAT96</t>
+  </si>
+  <si>
+    <t>WAT-305</t>
+  </si>
+  <si>
+    <t>Verify that system provides the filter option "Filter by organization" in the Author search result page</t>
+  </si>
+  <si>
+    <t>WAT97</t>
+  </si>
+  <si>
+    <t>WAT-304</t>
+  </si>
+  <si>
+    <t>Verify that system provides the filter option "Filter by author name" in the Author search result page</t>
   </si>
 </sst>
 </file>
@@ -1337,10 +1355,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E88"/>
+  <dimension ref="A1:E90"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A72" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E88" sqref="A1:E88"/>
+      <selection activeCell="C89" sqref="C89:C90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2673,6 +2691,36 @@
         <v>5</v>
       </c>
       <c r="E88" s="7"/>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89" s="9" t="s">
+        <v>291</v>
+      </c>
+      <c r="B89" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="C89" s="8" t="s">
+        <v>293</v>
+      </c>
+      <c r="D89" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E89" s="7"/>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" s="9" t="s">
+        <v>294</v>
+      </c>
+      <c r="B90" s="9" t="s">
+        <v>295</v>
+      </c>
+      <c r="C90" s="8" t="s">
+        <v>296</v>
+      </c>
+      <c r="D90" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E90" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Adds WAT98 testscript and related changes
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/WAT.xlsx
+++ b/src/test/resources/xls/WAT.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="300">
   <si>
     <t>TCID</t>
   </si>
@@ -908,6 +908,15 @@
   </si>
   <si>
     <t>Verify that system provides the filter option "Filter by author name" in the Author search result page</t>
+  </si>
+  <si>
+    <t>WAT98</t>
+  </si>
+  <si>
+    <t>WAT-309</t>
+  </si>
+  <si>
+    <t>Verify that in the author search result page, user should be provided with REFINE capability.</t>
   </si>
 </sst>
 </file>
@@ -1355,10 +1364,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E90"/>
+  <dimension ref="A1:E91"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A72" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C89" sqref="C89:C90"/>
+      <selection activeCell="C91" sqref="C91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2721,6 +2730,21 @@
         <v>5</v>
       </c>
       <c r="E90" s="7"/>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91" s="9" t="s">
+        <v>297</v>
+      </c>
+      <c r="B91" s="9" t="s">
+        <v>298</v>
+      </c>
+      <c r="C91" s="8" t="s">
+        <v>299</v>
+      </c>
+      <c r="D91" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E91" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Adds WAT99 test script and related changes
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/WAT.xlsx
+++ b/src/test/resources/xls/WAT.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="303">
   <si>
     <t>TCID</t>
   </si>
@@ -917,6 +917,15 @@
   </si>
   <si>
     <t>Verify that in the author search result page, user should be provided with REFINE capability.</t>
+  </si>
+  <si>
+    <t>WAT99</t>
+  </si>
+  <si>
+    <t>WAT-312</t>
+  </si>
+  <si>
+    <t>Verify that the user should be able to further refine the search result based on Subject Category</t>
   </si>
 </sst>
 </file>
@@ -1364,10 +1373,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E91"/>
+  <dimension ref="A1:E92"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A72" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C91" sqref="C91"/>
+      <selection activeCell="C92" sqref="C92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2745,6 +2754,21 @@
         <v>5</v>
       </c>
       <c r="E91" s="7"/>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A92" s="9" t="s">
+        <v>300</v>
+      </c>
+      <c r="B92" s="9" t="s">
+        <v>301</v>
+      </c>
+      <c r="C92" s="8" t="s">
+        <v>302</v>
+      </c>
+      <c r="D92" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E92" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Adds WAT100 & WAT101 testscript and related changes
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/WAT.xlsx
+++ b/src/test/resources/xls/WAT.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="309">
   <si>
     <t>TCID</t>
   </si>
@@ -926,6 +926,24 @@
   </si>
   <si>
     <t>Verify that the user should be able to further refine the search result based on Subject Category</t>
+  </si>
+  <si>
+    <t>WAT100</t>
+  </si>
+  <si>
+    <t>WAT-311</t>
+  </si>
+  <si>
+    <t>Verify that the user should be able to further refine the search result based on Organization</t>
+  </si>
+  <si>
+    <t>WAT101</t>
+  </si>
+  <si>
+    <t>WAT-310</t>
+  </si>
+  <si>
+    <t>Verify that the user should be able to further refine the search result based on Author Name</t>
   </si>
 </sst>
 </file>
@@ -1373,10 +1391,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E92"/>
+  <dimension ref="A1:E94"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A72" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C92" sqref="C92"/>
+      <selection activeCell="C94" sqref="C94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2769,6 +2787,36 @@
         <v>5</v>
       </c>
       <c r="E92" s="7"/>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A93" s="9" t="s">
+        <v>303</v>
+      </c>
+      <c r="B93" s="9" t="s">
+        <v>304</v>
+      </c>
+      <c r="C93" s="8" t="s">
+        <v>305</v>
+      </c>
+      <c r="D93" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E93" s="7"/>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A94" s="9" t="s">
+        <v>306</v>
+      </c>
+      <c r="B94" s="9" t="s">
+        <v>307</v>
+      </c>
+      <c r="C94" s="8" t="s">
+        <v>308</v>
+      </c>
+      <c r="D94" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E94" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Adds WAT102 testscript and related changes
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/WAT.xlsx
+++ b/src/test/resources/xls/WAT.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="312">
   <si>
     <t>TCID</t>
   </si>
@@ -944,6 +944,15 @@
   </si>
   <si>
     <t>Verify that the user should be able to further refine the search result based on Author Name</t>
+  </si>
+  <si>
+    <t>WAT102</t>
+  </si>
+  <si>
+    <t>Verify that The user shall be taken to the ResearcherID record in a new browser window/tab when they click on the ResearcherID</t>
+  </si>
+  <si>
+    <t>WAT-348</t>
   </si>
 </sst>
 </file>
@@ -1391,10 +1400,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E94"/>
+  <dimension ref="A1:E95"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A72" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C94" sqref="C94"/>
+      <selection activeCell="B95" sqref="B95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2817,6 +2826,21 @@
         <v>5</v>
       </c>
       <c r="E94" s="7"/>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A95" s="9" t="s">
+        <v>309</v>
+      </c>
+      <c r="B95" s="9" t="s">
+        <v>311</v>
+      </c>
+      <c r="C95" s="8" t="s">
+        <v>310</v>
+      </c>
+      <c r="D95" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E95" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Adds WAT103 testscript and related changes
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/WAT.xlsx
+++ b/src/test/resources/xls/WAT.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="315">
   <si>
     <t>TCID</t>
   </si>
@@ -953,6 +953,15 @@
   </si>
   <si>
     <t>WAT-348</t>
+  </si>
+  <si>
+    <t>WAT-347</t>
+  </si>
+  <si>
+    <t>Verify that The user shall be taken to the ORCiD record in a new browser window/tab when they click on the ORCID</t>
+  </si>
+  <si>
+    <t>WAT103</t>
   </si>
 </sst>
 </file>
@@ -1400,10 +1409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E95"/>
+  <dimension ref="A1:E96"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A72" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B95" sqref="B95"/>
+      <selection activeCell="A96" sqref="A96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2832,15 +2841,29 @@
         <v>309</v>
       </c>
       <c r="B95" s="9" t="s">
+        <v>312</v>
+      </c>
+      <c r="C95" s="8" t="s">
+        <v>313</v>
+      </c>
+      <c r="D95" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E95" s="7"/>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A96" s="9" t="s">
+        <v>314</v>
+      </c>
+      <c r="B96" s="9" t="s">
         <v>311</v>
       </c>
-      <c r="C95" s="8" t="s">
+      <c r="C96" s="8" t="s">
         <v>310</v>
       </c>
-      <c r="D95" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="E95" s="7"/>
+      <c r="D96" s="9" t="s">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Adds WAT104 & WAT105 testscript and related changes
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/WAT.xlsx
+++ b/src/test/resources/xls/WAT.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="321">
   <si>
     <t>TCID</t>
   </si>
@@ -962,6 +962,24 @@
   </si>
   <si>
     <t>WAT103</t>
+  </si>
+  <si>
+    <t>WAT104</t>
+  </si>
+  <si>
+    <t>WAT-346</t>
+  </si>
+  <si>
+    <t>Verify that ResearcherID format (text) label followed by the ResearcherID number i.e. ResearcherID A-1009-2008</t>
+  </si>
+  <si>
+    <t>Verify the ORCID format followed by orcid.org/&lt;orcid-identifier&gt; i.e.orcid.org/0000-0002-1825-0097</t>
+  </si>
+  <si>
+    <t>WAT105</t>
+  </si>
+  <si>
+    <t>WAT-344</t>
   </si>
 </sst>
 </file>
@@ -1409,10 +1427,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E96"/>
+  <dimension ref="A1:E98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A72" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A96" sqref="A96"/>
+    <sheetView tabSelected="1" topLeftCell="A69" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D97" sqref="D97:E98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2864,6 +2882,37 @@
       <c r="D96" s="9" t="s">
         <v>5</v>
       </c>
+      <c r="E96" s="7"/>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A97" s="9" t="s">
+        <v>315</v>
+      </c>
+      <c r="B97" s="9" t="s">
+        <v>316</v>
+      </c>
+      <c r="C97" s="8" t="s">
+        <v>317</v>
+      </c>
+      <c r="D97" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E97" s="7"/>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A98" s="9" t="s">
+        <v>319</v>
+      </c>
+      <c r="B98" s="9" t="s">
+        <v>320</v>
+      </c>
+      <c r="C98" s="8" t="s">
+        <v>318</v>
+      </c>
+      <c r="D98" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E98" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Adds WAT107 and related changes
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/WAT.xlsx
+++ b/src/test/resources/xls/WAT.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13305" windowHeight="2415"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="579" uniqueCount="342">
   <si>
     <t>TCID</t>
   </si>
@@ -1025,13 +1025,31 @@
   </si>
   <si>
     <t>Verify that System must grey out / inactivate the Alternative names tab when there are no alternative names to display.</t>
+  </si>
+  <si>
+    <t>WAT106</t>
+  </si>
+  <si>
+    <t>WAT107</t>
+  </si>
+  <si>
+    <t>WAT-330</t>
+  </si>
+  <si>
+    <t>WAT-327</t>
+  </si>
+  <si>
+    <t>Verify that the Organization list provided should be arranged alphabetically.</t>
+  </si>
+  <si>
+    <t>Verify that the Country list provided should be arranged alphabetically.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1228,7 +1246,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1260,9 +1278,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1294,6 +1313,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1469,14 +1489,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E103"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E105"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A76" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A103" sqref="A103:E103"/>
+      <selection activeCell="C107" sqref="C107"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="41" bestFit="1" customWidth="1" collapsed="1"/>
@@ -1485,7 +1505,7 @@
     <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1502,7 +1522,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -1517,7 +1537,7 @@
       </c>
       <c r="E2" s="4"/>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -1532,7 +1552,7 @@
       </c>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>11</v>
       </c>
@@ -1547,7 +1567,7 @@
       </c>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>12</v>
       </c>
@@ -1562,7 +1582,7 @@
       </c>
       <c r="E5" s="7"/>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>14</v>
       </c>
@@ -1577,7 +1597,7 @@
       </c>
       <c r="E6" s="7"/>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>17</v>
       </c>
@@ -1592,7 +1612,7 @@
       </c>
       <c r="E7" s="7"/>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>20</v>
       </c>
@@ -1607,7 +1627,7 @@
       </c>
       <c r="E8" s="7"/>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>22</v>
       </c>
@@ -1622,7 +1642,7 @@
       </c>
       <c r="E9" s="7"/>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>23</v>
       </c>
@@ -1637,7 +1657,7 @@
       </c>
       <c r="E10" s="7"/>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>24</v>
       </c>
@@ -1652,7 +1672,7 @@
       </c>
       <c r="E11" s="7"/>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>25</v>
       </c>
@@ -1667,7 +1687,7 @@
       </c>
       <c r="E12" s="7"/>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>62</v>
       </c>
@@ -1682,7 +1702,7 @@
       </c>
       <c r="E13" s="7"/>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>63</v>
       </c>
@@ -1697,7 +1717,7 @@
       </c>
       <c r="E14" s="7"/>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>64</v>
       </c>
@@ -1712,7 +1732,7 @@
       </c>
       <c r="E15" s="7"/>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>65</v>
       </c>
@@ -1727,7 +1747,7 @@
       </c>
       <c r="E16" s="7"/>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>74</v>
       </c>
@@ -1742,7 +1762,7 @@
       </c>
       <c r="E17" s="7"/>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>75</v>
       </c>
@@ -1757,7 +1777,7 @@
       </c>
       <c r="E18" s="7"/>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>79</v>
       </c>
@@ -1772,7 +1792,7 @@
       </c>
       <c r="E19" s="7"/>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>81</v>
       </c>
@@ -1787,7 +1807,7 @@
       </c>
       <c r="E20" s="7"/>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>82</v>
       </c>
@@ -1802,7 +1822,7 @@
       </c>
       <c r="E21" s="7"/>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>88</v>
       </c>
@@ -1817,7 +1837,7 @@
       </c>
       <c r="E22" s="7"/>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>90</v>
       </c>
@@ -1832,7 +1852,7 @@
       </c>
       <c r="E23" s="7"/>
     </row>
-    <row r="24" spans="1:5" ht="30">
+    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>94</v>
       </c>
@@ -1847,7 +1867,7 @@
       </c>
       <c r="E24" s="7"/>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>96</v>
       </c>
@@ -1862,7 +1882,7 @@
       </c>
       <c r="E25" s="7"/>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
         <v>98</v>
       </c>
@@ -1877,7 +1897,7 @@
       </c>
       <c r="E26" s="7"/>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
         <v>102</v>
       </c>
@@ -1892,7 +1912,7 @@
       </c>
       <c r="E27" s="7"/>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
         <v>105</v>
       </c>
@@ -1907,7 +1927,7 @@
       </c>
       <c r="E28" s="7"/>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
         <v>108</v>
       </c>
@@ -1922,7 +1942,7 @@
       </c>
       <c r="E29" s="7"/>
     </row>
-    <row r="30" spans="1:5" ht="30">
+    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
         <v>110</v>
       </c>
@@ -1937,7 +1957,7 @@
       </c>
       <c r="E30" s="7"/>
     </row>
-    <row r="31" spans="1:5" ht="30">
+    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
         <v>114</v>
       </c>
@@ -1952,7 +1972,7 @@
       </c>
       <c r="E31" s="7"/>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
         <v>119</v>
       </c>
@@ -1967,7 +1987,7 @@
       </c>
       <c r="E32" s="7"/>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
         <v>120</v>
       </c>
@@ -1982,7 +2002,7 @@
       </c>
       <c r="E33" s="7"/>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
         <v>125</v>
       </c>
@@ -1997,7 +2017,7 @@
       </c>
       <c r="E34" s="7"/>
     </row>
-    <row r="35" spans="1:5" ht="30">
+    <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
         <v>128</v>
       </c>
@@ -2012,7 +2032,7 @@
       </c>
       <c r="E35" s="7"/>
     </row>
-    <row r="36" spans="1:5" ht="30">
+    <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
         <v>131</v>
       </c>
@@ -2027,7 +2047,7 @@
       </c>
       <c r="E36" s="7"/>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
         <v>134</v>
       </c>
@@ -2042,7 +2062,7 @@
       </c>
       <c r="E37" s="7"/>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="9" t="s">
         <v>137</v>
       </c>
@@ -2057,7 +2077,7 @@
       </c>
       <c r="E38" s="7"/>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="s">
         <v>140</v>
       </c>
@@ -2072,7 +2092,7 @@
       </c>
       <c r="E39" s="7"/>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="9" t="s">
         <v>143</v>
       </c>
@@ -2087,7 +2107,7 @@
       </c>
       <c r="E40" s="7"/>
     </row>
-    <row r="41" spans="1:5" ht="30">
+    <row r="41" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
         <v>145</v>
       </c>
@@ -2102,7 +2122,7 @@
       </c>
       <c r="E41" s="7"/>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="9" t="s">
         <v>147</v>
       </c>
@@ -2117,7 +2137,7 @@
       </c>
       <c r="E42" s="7"/>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="9" t="s">
         <v>150</v>
       </c>
@@ -2132,7 +2152,7 @@
       </c>
       <c r="E43" s="7"/>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="9" t="s">
         <v>153</v>
       </c>
@@ -2147,7 +2167,7 @@
       </c>
       <c r="E44" s="7"/>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="9" t="s">
         <v>155</v>
       </c>
@@ -2162,7 +2182,7 @@
       </c>
       <c r="E45" s="7"/>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="12" t="s">
         <v>158</v>
       </c>
@@ -2177,7 +2197,7 @@
       </c>
       <c r="E46" s="7"/>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="12" t="s">
         <v>159</v>
       </c>
@@ -2192,7 +2212,7 @@
       </c>
       <c r="E47" s="7"/>
     </row>
-    <row r="48" spans="1:5" ht="30">
+    <row r="48" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="12" t="s">
         <v>160</v>
       </c>
@@ -2207,7 +2227,7 @@
       </c>
       <c r="E48" s="7"/>
     </row>
-    <row r="49" spans="1:5" ht="30">
+    <row r="49" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="12" t="s">
         <v>161</v>
       </c>
@@ -2222,7 +2242,7 @@
       </c>
       <c r="E49" s="7"/>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="12" t="s">
         <v>164</v>
       </c>
@@ -2237,7 +2257,7 @@
       </c>
       <c r="E50" s="7"/>
     </row>
-    <row r="51" spans="1:5" ht="30">
+    <row r="51" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="9" t="s">
         <v>173</v>
       </c>
@@ -2252,7 +2272,7 @@
       </c>
       <c r="E51" s="7"/>
     </row>
-    <row r="52" spans="1:5">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="9" t="s">
         <v>174</v>
       </c>
@@ -2267,7 +2287,7 @@
       </c>
       <c r="E52" s="7"/>
     </row>
-    <row r="53" spans="1:5">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="9" t="s">
         <v>179</v>
       </c>
@@ -2282,7 +2302,7 @@
       </c>
       <c r="E53" s="7"/>
     </row>
-    <row r="54" spans="1:5">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="9" t="s">
         <v>180</v>
       </c>
@@ -2297,7 +2317,7 @@
       </c>
       <c r="E54" s="7"/>
     </row>
-    <row r="55" spans="1:5">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="9" t="s">
         <v>185</v>
       </c>
@@ -2312,7 +2332,7 @@
       </c>
       <c r="E55" s="7"/>
     </row>
-    <row r="56" spans="1:5">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="s">
         <v>188</v>
       </c>
@@ -2327,7 +2347,7 @@
       </c>
       <c r="E56" s="7"/>
     </row>
-    <row r="57" spans="1:5" ht="30">
+    <row r="57" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="9" t="s">
         <v>191</v>
       </c>
@@ -2342,7 +2362,7 @@
       </c>
       <c r="E57" s="7"/>
     </row>
-    <row r="58" spans="1:5">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="9" t="s">
         <v>194</v>
       </c>
@@ -2357,7 +2377,7 @@
       </c>
       <c r="E58" s="7"/>
     </row>
-    <row r="59" spans="1:5">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
         <v>196</v>
       </c>
@@ -2372,7 +2392,7 @@
       </c>
       <c r="E59" s="7"/>
     </row>
-    <row r="60" spans="1:5" ht="45">
+    <row r="60" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
         <v>199</v>
       </c>
@@ -2387,7 +2407,7 @@
       </c>
       <c r="E60" s="7"/>
     </row>
-    <row r="61" spans="1:5">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="9" t="s">
         <v>202</v>
       </c>
@@ -2402,7 +2422,7 @@
       </c>
       <c r="E61" s="7"/>
     </row>
-    <row r="62" spans="1:5">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="9" t="s">
         <v>204</v>
       </c>
@@ -2417,7 +2437,7 @@
       </c>
       <c r="E62" s="7"/>
     </row>
-    <row r="63" spans="1:5">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="9" t="s">
         <v>206</v>
       </c>
@@ -2432,7 +2452,7 @@
       </c>
       <c r="E63" s="7"/>
     </row>
-    <row r="64" spans="1:5">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="9" t="s">
         <v>208</v>
       </c>
@@ -2447,7 +2467,7 @@
       </c>
       <c r="E64" s="7"/>
     </row>
-    <row r="65" spans="1:5">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="9" t="s">
         <v>217</v>
       </c>
@@ -2462,7 +2482,7 @@
       </c>
       <c r="E65" s="7"/>
     </row>
-    <row r="66" spans="1:5">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="9" t="s">
         <v>218</v>
       </c>
@@ -2477,7 +2497,7 @@
       </c>
       <c r="E66" s="7"/>
     </row>
-    <row r="67" spans="1:5">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="9" t="s">
         <v>223</v>
       </c>
@@ -2492,7 +2512,7 @@
       </c>
       <c r="E67" s="7"/>
     </row>
-    <row r="68" spans="1:5">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="9" t="s">
         <v>224</v>
       </c>
@@ -2507,7 +2527,7 @@
       </c>
       <c r="E68" s="7"/>
     </row>
-    <row r="69" spans="1:5">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="9" t="s">
         <v>225</v>
       </c>
@@ -2522,7 +2542,7 @@
       </c>
       <c r="E69" s="7"/>
     </row>
-    <row r="70" spans="1:5">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="9" t="s">
         <v>226</v>
       </c>
@@ -2537,7 +2557,7 @@
       </c>
       <c r="E70" s="7"/>
     </row>
-    <row r="71" spans="1:5">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="9" t="s">
         <v>233</v>
       </c>
@@ -2552,7 +2572,7 @@
       </c>
       <c r="E71" s="7"/>
     </row>
-    <row r="72" spans="1:5">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="9" t="s">
         <v>237</v>
       </c>
@@ -2567,7 +2587,7 @@
       </c>
       <c r="E72" s="7"/>
     </row>
-    <row r="73" spans="1:5">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="9" t="s">
         <v>239</v>
       </c>
@@ -2582,7 +2602,7 @@
       </c>
       <c r="E73" s="7"/>
     </row>
-    <row r="74" spans="1:5">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="9" t="s">
         <v>243</v>
       </c>
@@ -2597,7 +2617,7 @@
       </c>
       <c r="E74" s="7"/>
     </row>
-    <row r="75" spans="1:5" ht="30">
+    <row r="75" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" s="9" t="s">
         <v>245</v>
       </c>
@@ -2612,7 +2632,7 @@
       </c>
       <c r="E75" s="7"/>
     </row>
-    <row r="76" spans="1:5">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="9" t="s">
         <v>248</v>
       </c>
@@ -2627,7 +2647,7 @@
       </c>
       <c r="E76" s="7"/>
     </row>
-    <row r="77" spans="1:5">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="9" t="s">
         <v>256</v>
       </c>
@@ -2642,7 +2662,7 @@
       </c>
       <c r="E77" s="7"/>
     </row>
-    <row r="78" spans="1:5">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="9" t="s">
         <v>257</v>
       </c>
@@ -2657,7 +2677,7 @@
       </c>
       <c r="E78" s="7"/>
     </row>
-    <row r="79" spans="1:5">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="9" t="s">
         <v>261</v>
       </c>
@@ -2672,7 +2692,7 @@
       </c>
       <c r="E79" s="7"/>
     </row>
-    <row r="80" spans="1:5">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="9" t="s">
         <v>264</v>
       </c>
@@ -2687,7 +2707,7 @@
       </c>
       <c r="E80" s="7"/>
     </row>
-    <row r="81" spans="1:5">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="9" t="s">
         <v>267</v>
       </c>
@@ -2702,7 +2722,7 @@
       </c>
       <c r="E81" s="7"/>
     </row>
-    <row r="82" spans="1:5" ht="30">
+    <row r="82" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A82" s="9" t="s">
         <v>269</v>
       </c>
@@ -2717,7 +2737,7 @@
       </c>
       <c r="E82" s="7"/>
     </row>
-    <row r="83" spans="1:5">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="9" t="s">
         <v>274</v>
       </c>
@@ -2732,7 +2752,7 @@
       </c>
       <c r="E83" s="7"/>
     </row>
-    <row r="84" spans="1:5" ht="30">
+    <row r="84" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A84" s="9" t="s">
         <v>277</v>
       </c>
@@ -2747,7 +2767,7 @@
       </c>
       <c r="E84" s="7"/>
     </row>
-    <row r="85" spans="1:5">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="9" t="s">
         <v>279</v>
       </c>
@@ -2762,7 +2782,7 @@
       </c>
       <c r="E85" s="7"/>
     </row>
-    <row r="86" spans="1:5">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="9" t="s">
         <v>282</v>
       </c>
@@ -2777,7 +2797,7 @@
       </c>
       <c r="E86" s="7"/>
     </row>
-    <row r="87" spans="1:5">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="9" t="s">
         <v>285</v>
       </c>
@@ -2792,7 +2812,7 @@
       </c>
       <c r="E87" s="7"/>
     </row>
-    <row r="88" spans="1:5">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="9" t="s">
         <v>288</v>
       </c>
@@ -2807,7 +2827,7 @@
       </c>
       <c r="E88" s="7"/>
     </row>
-    <row r="89" spans="1:5">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="9" t="s">
         <v>291</v>
       </c>
@@ -2822,7 +2842,7 @@
       </c>
       <c r="E89" s="7"/>
     </row>
-    <row r="90" spans="1:5">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="9" t="s">
         <v>294</v>
       </c>
@@ -2837,7 +2857,7 @@
       </c>
       <c r="E90" s="7"/>
     </row>
-    <row r="91" spans="1:5">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="9" t="s">
         <v>297</v>
       </c>
@@ -2852,7 +2872,7 @@
       </c>
       <c r="E91" s="7"/>
     </row>
-    <row r="92" spans="1:5">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="9" t="s">
         <v>300</v>
       </c>
@@ -2867,7 +2887,7 @@
       </c>
       <c r="E92" s="7"/>
     </row>
-    <row r="93" spans="1:5">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="9" t="s">
         <v>303</v>
       </c>
@@ -2882,7 +2902,7 @@
       </c>
       <c r="E93" s="7"/>
     </row>
-    <row r="94" spans="1:5">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="9" t="s">
         <v>306</v>
       </c>
@@ -2897,7 +2917,7 @@
       </c>
       <c r="E94" s="7"/>
     </row>
-    <row r="95" spans="1:5">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="9" t="s">
         <v>309</v>
       </c>
@@ -2912,7 +2932,7 @@
       </c>
       <c r="E95" s="7"/>
     </row>
-    <row r="96" spans="1:5">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="9" t="s">
         <v>314</v>
       </c>
@@ -2927,7 +2947,7 @@
       </c>
       <c r="E96" s="7"/>
     </row>
-    <row r="97" spans="1:5">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="9" t="s">
         <v>315</v>
       </c>
@@ -2942,7 +2962,7 @@
       </c>
       <c r="E97" s="7"/>
     </row>
-    <row r="98" spans="1:5">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="9" t="s">
         <v>319</v>
       </c>
@@ -2957,7 +2977,7 @@
       </c>
       <c r="E98" s="7"/>
     </row>
-    <row r="99" spans="1:5">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="9" t="s">
         <v>321</v>
       </c>
@@ -2972,7 +2992,7 @@
       </c>
       <c r="E99" s="7"/>
     </row>
-    <row r="100" spans="1:5">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="9" t="s">
         <v>322</v>
       </c>
@@ -2987,7 +3007,7 @@
       </c>
       <c r="E100" s="7"/>
     </row>
-    <row r="101" spans="1:5" ht="30">
+    <row r="101" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A101" s="9" t="s">
         <v>323</v>
       </c>
@@ -3002,7 +3022,7 @@
       </c>
       <c r="E101" s="7"/>
     </row>
-    <row r="102" spans="1:5">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="9" t="s">
         <v>328</v>
       </c>
@@ -3017,7 +3037,7 @@
       </c>
       <c r="E102" s="7"/>
     </row>
-    <row r="103" spans="1:5">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="9" t="s">
         <v>333</v>
       </c>
@@ -3031,6 +3051,36 @@
         <v>5</v>
       </c>
       <c r="E103" s="7"/>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A104" s="9" t="s">
+        <v>336</v>
+      </c>
+      <c r="B104" s="9" t="s">
+        <v>338</v>
+      </c>
+      <c r="C104" s="8" t="s">
+        <v>340</v>
+      </c>
+      <c r="D104" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E104" s="7"/>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A105" s="9" t="s">
+        <v>337</v>
+      </c>
+      <c r="B105" s="9" t="s">
+        <v>339</v>
+      </c>
+      <c r="C105" s="8" t="s">
+        <v>341</v>
+      </c>
+      <c r="D105" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E105" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -3043,14 +3093,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView topLeftCell="A10" zoomScale="80" workbookViewId="0">
       <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
@@ -3058,7 +3108,7 @@
     <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>35</v>
       </c>
@@ -3072,7 +3122,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>37</v>
       </c>
@@ -3084,7 +3134,7 @@
       </c>
       <c r="D2" s="7"/>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>38</v>
       </c>
@@ -3096,7 +3146,7 @@
       </c>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>39</v>
       </c>
@@ -3108,7 +3158,7 @@
       </c>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>40</v>
       </c>
@@ -3120,7 +3170,7 @@
       </c>
       <c r="D5" s="7"/>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>41</v>
       </c>
@@ -3132,7 +3182,7 @@
       </c>
       <c r="D6" s="7"/>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>42</v>
       </c>
@@ -3144,7 +3194,7 @@
       </c>
       <c r="D7" s="7"/>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>43</v>
       </c>
@@ -3156,7 +3206,7 @@
       </c>
       <c r="D8" s="7"/>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>44</v>
       </c>
@@ -3168,7 +3218,7 @@
       </c>
       <c r="D9" s="7"/>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>45</v>
       </c>
@@ -3180,7 +3230,7 @@
       </c>
       <c r="D10" s="7"/>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>46</v>
       </c>
@@ -3192,7 +3242,7 @@
       </c>
       <c r="D11" s="7"/>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>48</v>
       </c>
@@ -3204,7 +3254,7 @@
       </c>
       <c r="D12" s="7"/>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>49</v>
       </c>
@@ -3216,7 +3266,7 @@
       </c>
       <c r="D13" s="7"/>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>50</v>
       </c>
@@ -3228,7 +3278,7 @@
       </c>
       <c r="D14" s="7"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>51</v>
       </c>
@@ -3240,7 +3290,7 @@
       </c>
       <c r="D15" s="7"/>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>52</v>
       </c>
@@ -3252,7 +3302,7 @@
       </c>
       <c r="D16" s="7"/>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>53</v>
       </c>
@@ -3264,7 +3314,7 @@
       </c>
       <c r="D17" s="7"/>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>54</v>
       </c>
@@ -3276,7 +3326,7 @@
       </c>
       <c r="D18" s="7"/>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>55</v>
       </c>
@@ -3288,7 +3338,7 @@
       </c>
       <c r="D19" s="7"/>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>56</v>
       </c>
@@ -3300,7 +3350,7 @@
       </c>
       <c r="D20" s="7"/>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>57</v>
       </c>
@@ -3312,7 +3362,7 @@
       </c>
       <c r="D21" s="7"/>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>58</v>
       </c>
@@ -3324,7 +3374,7 @@
       </c>
       <c r="D22" s="7"/>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>59</v>
       </c>
@@ -3336,7 +3386,7 @@
       </c>
       <c r="D23" s="7"/>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>60</v>
       </c>
@@ -3348,7 +3398,7 @@
       </c>
       <c r="D24" s="7"/>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>61</v>
       </c>
@@ -3360,7 +3410,7 @@
       </c>
       <c r="D25" s="7"/>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>47</v>
       </c>
@@ -3379,14 +3429,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A19" sqref="A19:XFD19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
@@ -3394,7 +3444,7 @@
     <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>35</v>
       </c>
@@ -3408,7 +3458,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>37</v>
       </c>
@@ -3420,7 +3470,7 @@
       </c>
       <c r="D2" s="7"/>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>38</v>
       </c>
@@ -3432,7 +3482,7 @@
       </c>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>39</v>
       </c>
@@ -3444,7 +3494,7 @@
       </c>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>40</v>
       </c>
@@ -3456,7 +3506,7 @@
       </c>
       <c r="D5" s="7"/>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>41</v>
       </c>
@@ -3468,7 +3518,7 @@
       </c>
       <c r="D6" s="7"/>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>42</v>
       </c>
@@ -3480,7 +3530,7 @@
       </c>
       <c r="D7" s="7"/>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>43</v>
       </c>
@@ -3492,7 +3542,7 @@
       </c>
       <c r="D8" s="7"/>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>44</v>
       </c>
@@ -3504,7 +3554,7 @@
       </c>
       <c r="D9" s="7"/>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>45</v>
       </c>
@@ -3516,7 +3566,7 @@
       </c>
       <c r="D10" s="7"/>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>46</v>
       </c>
@@ -3528,7 +3578,7 @@
       </c>
       <c r="D11" s="7"/>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>47</v>
       </c>
@@ -3540,7 +3590,7 @@
       </c>
       <c r="D12" s="7"/>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>48</v>
       </c>
@@ -3552,7 +3602,7 @@
       </c>
       <c r="D13" s="7"/>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>49</v>
       </c>
@@ -3564,7 +3614,7 @@
       </c>
       <c r="D14" s="7"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>50</v>
       </c>
@@ -3576,7 +3626,7 @@
       </c>
       <c r="D15" s="7"/>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>51</v>
       </c>
@@ -3588,7 +3638,7 @@
       </c>
       <c r="D16" s="7"/>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>52</v>
       </c>
@@ -3600,7 +3650,7 @@
       </c>
       <c r="D17" s="7"/>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>53</v>
       </c>
@@ -3612,7 +3662,7 @@
       </c>
       <c r="D18" s="7"/>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>54</v>
       </c>
@@ -3624,7 +3674,7 @@
       </c>
       <c r="D19" s="7"/>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>55</v>
       </c>
@@ -3636,7 +3686,7 @@
       </c>
       <c r="D20" s="7"/>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>56</v>
       </c>
@@ -3648,7 +3698,7 @@
       </c>
       <c r="D21" s="7"/>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>57</v>
       </c>
@@ -3660,7 +3710,7 @@
       </c>
       <c r="D22" s="7"/>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>58</v>
       </c>
@@ -3672,7 +3722,7 @@
       </c>
       <c r="D23" s="7"/>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>59</v>
       </c>
@@ -3684,7 +3734,7 @@
       </c>
       <c r="D24" s="7"/>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>60</v>
       </c>
@@ -3696,7 +3746,7 @@
       </c>
       <c r="D25" s="7"/>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>61</v>
       </c>

</xml_diff>

<commit_message>
Adds WAT108 test script and related changes
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/WAT.xlsx
+++ b/src/test/resources/xls/WAT.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13305" windowHeight="2415"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="345">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="348">
   <si>
     <t>TCID</t>
   </si>
@@ -1052,13 +1052,22 @@
   </si>
   <si>
     <t>Verify that system must display a metric's tab on author record||Verify that while click on 'Metrics' tab, tab should be highlighted by highlight bar</t>
+  </si>
+  <si>
+    <t>WAT108</t>
+  </si>
+  <si>
+    <t>WAT-326</t>
+  </si>
+  <si>
+    <t>"Verify that specific text is displayed when the author search results fetched are more than 50 clusters."</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1255,7 +1264,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1287,9 +1296,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1321,6 +1331,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1496,14 +1507,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E106"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E107"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A92" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C110" sqref="C110"/>
+      <selection activeCell="C107" sqref="C107"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="41" bestFit="1" customWidth="1" collapsed="1"/>
@@ -1512,7 +1523,7 @@
     <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1529,7 +1540,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -1544,7 +1555,7 @@
       </c>
       <c r="E2" s="4"/>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -1559,7 +1570,7 @@
       </c>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>11</v>
       </c>
@@ -1574,7 +1585,7 @@
       </c>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>12</v>
       </c>
@@ -1589,7 +1600,7 @@
       </c>
       <c r="E5" s="7"/>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>14</v>
       </c>
@@ -1604,7 +1615,7 @@
       </c>
       <c r="E6" s="7"/>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>17</v>
       </c>
@@ -1619,7 +1630,7 @@
       </c>
       <c r="E7" s="7"/>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>20</v>
       </c>
@@ -1634,7 +1645,7 @@
       </c>
       <c r="E8" s="7"/>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>22</v>
       </c>
@@ -1649,7 +1660,7 @@
       </c>
       <c r="E9" s="7"/>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>23</v>
       </c>
@@ -1664,7 +1675,7 @@
       </c>
       <c r="E10" s="7"/>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>24</v>
       </c>
@@ -1679,7 +1690,7 @@
       </c>
       <c r="E11" s="7"/>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>25</v>
       </c>
@@ -1694,7 +1705,7 @@
       </c>
       <c r="E12" s="7"/>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>62</v>
       </c>
@@ -1709,7 +1720,7 @@
       </c>
       <c r="E13" s="7"/>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>63</v>
       </c>
@@ -1724,7 +1735,7 @@
       </c>
       <c r="E14" s="7"/>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>64</v>
       </c>
@@ -1739,7 +1750,7 @@
       </c>
       <c r="E15" s="7"/>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>65</v>
       </c>
@@ -1754,7 +1765,7 @@
       </c>
       <c r="E16" s="7"/>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>74</v>
       </c>
@@ -1769,7 +1780,7 @@
       </c>
       <c r="E17" s="7"/>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>75</v>
       </c>
@@ -1784,7 +1795,7 @@
       </c>
       <c r="E18" s="7"/>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>79</v>
       </c>
@@ -1799,7 +1810,7 @@
       </c>
       <c r="E19" s="7"/>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>81</v>
       </c>
@@ -1814,7 +1825,7 @@
       </c>
       <c r="E20" s="7"/>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>82</v>
       </c>
@@ -1829,7 +1840,7 @@
       </c>
       <c r="E21" s="7"/>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>88</v>
       </c>
@@ -1844,7 +1855,7 @@
       </c>
       <c r="E22" s="7"/>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>90</v>
       </c>
@@ -1859,7 +1870,7 @@
       </c>
       <c r="E23" s="7"/>
     </row>
-    <row r="24" spans="1:5" ht="30">
+    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>94</v>
       </c>
@@ -1874,7 +1885,7 @@
       </c>
       <c r="E24" s="7"/>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>96</v>
       </c>
@@ -1889,7 +1900,7 @@
       </c>
       <c r="E25" s="7"/>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
         <v>98</v>
       </c>
@@ -1904,7 +1915,7 @@
       </c>
       <c r="E26" s="7"/>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
         <v>102</v>
       </c>
@@ -1919,7 +1930,7 @@
       </c>
       <c r="E27" s="7"/>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
         <v>105</v>
       </c>
@@ -1934,7 +1945,7 @@
       </c>
       <c r="E28" s="7"/>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
         <v>108</v>
       </c>
@@ -1949,7 +1960,7 @@
       </c>
       <c r="E29" s="7"/>
     </row>
-    <row r="30" spans="1:5" ht="30">
+    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
         <v>110</v>
       </c>
@@ -1964,7 +1975,7 @@
       </c>
       <c r="E30" s="7"/>
     </row>
-    <row r="31" spans="1:5" ht="30">
+    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
         <v>114</v>
       </c>
@@ -1979,7 +1990,7 @@
       </c>
       <c r="E31" s="7"/>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
         <v>119</v>
       </c>
@@ -1994,7 +2005,7 @@
       </c>
       <c r="E32" s="7"/>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
         <v>120</v>
       </c>
@@ -2009,7 +2020,7 @@
       </c>
       <c r="E33" s="7"/>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
         <v>125</v>
       </c>
@@ -2024,7 +2035,7 @@
       </c>
       <c r="E34" s="7"/>
     </row>
-    <row r="35" spans="1:5" ht="30">
+    <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
         <v>128</v>
       </c>
@@ -2039,7 +2050,7 @@
       </c>
       <c r="E35" s="7"/>
     </row>
-    <row r="36" spans="1:5" ht="30">
+    <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
         <v>131</v>
       </c>
@@ -2054,7 +2065,7 @@
       </c>
       <c r="E36" s="7"/>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
         <v>134</v>
       </c>
@@ -2069,7 +2080,7 @@
       </c>
       <c r="E37" s="7"/>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="9" t="s">
         <v>137</v>
       </c>
@@ -2084,7 +2095,7 @@
       </c>
       <c r="E38" s="7"/>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="s">
         <v>140</v>
       </c>
@@ -2099,7 +2110,7 @@
       </c>
       <c r="E39" s="7"/>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="9" t="s">
         <v>143</v>
       </c>
@@ -2114,7 +2125,7 @@
       </c>
       <c r="E40" s="7"/>
     </row>
-    <row r="41" spans="1:5" ht="30">
+    <row r="41" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
         <v>145</v>
       </c>
@@ -2129,7 +2140,7 @@
       </c>
       <c r="E41" s="7"/>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="9" t="s">
         <v>147</v>
       </c>
@@ -2144,7 +2155,7 @@
       </c>
       <c r="E42" s="7"/>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="9" t="s">
         <v>150</v>
       </c>
@@ -2159,7 +2170,7 @@
       </c>
       <c r="E43" s="7"/>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="9" t="s">
         <v>153</v>
       </c>
@@ -2174,7 +2185,7 @@
       </c>
       <c r="E44" s="7"/>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="9" t="s">
         <v>155</v>
       </c>
@@ -2189,7 +2200,7 @@
       </c>
       <c r="E45" s="7"/>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="12" t="s">
         <v>158</v>
       </c>
@@ -2204,7 +2215,7 @@
       </c>
       <c r="E46" s="7"/>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="12" t="s">
         <v>159</v>
       </c>
@@ -2219,7 +2230,7 @@
       </c>
       <c r="E47" s="7"/>
     </row>
-    <row r="48" spans="1:5" ht="30">
+    <row r="48" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="12" t="s">
         <v>160</v>
       </c>
@@ -2234,7 +2245,7 @@
       </c>
       <c r="E48" s="7"/>
     </row>
-    <row r="49" spans="1:5" ht="30">
+    <row r="49" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="12" t="s">
         <v>161</v>
       </c>
@@ -2249,7 +2260,7 @@
       </c>
       <c r="E49" s="7"/>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="12" t="s">
         <v>164</v>
       </c>
@@ -2264,7 +2275,7 @@
       </c>
       <c r="E50" s="7"/>
     </row>
-    <row r="51" spans="1:5" ht="30">
+    <row r="51" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="9" t="s">
         <v>173</v>
       </c>
@@ -2279,7 +2290,7 @@
       </c>
       <c r="E51" s="7"/>
     </row>
-    <row r="52" spans="1:5">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="9" t="s">
         <v>174</v>
       </c>
@@ -2294,7 +2305,7 @@
       </c>
       <c r="E52" s="7"/>
     </row>
-    <row r="53" spans="1:5">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="9" t="s">
         <v>179</v>
       </c>
@@ -2309,7 +2320,7 @@
       </c>
       <c r="E53" s="7"/>
     </row>
-    <row r="54" spans="1:5">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="9" t="s">
         <v>180</v>
       </c>
@@ -2324,7 +2335,7 @@
       </c>
       <c r="E54" s="7"/>
     </row>
-    <row r="55" spans="1:5">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="9" t="s">
         <v>185</v>
       </c>
@@ -2339,7 +2350,7 @@
       </c>
       <c r="E55" s="7"/>
     </row>
-    <row r="56" spans="1:5">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="s">
         <v>188</v>
       </c>
@@ -2354,7 +2365,7 @@
       </c>
       <c r="E56" s="7"/>
     </row>
-    <row r="57" spans="1:5" ht="30">
+    <row r="57" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="9" t="s">
         <v>191</v>
       </c>
@@ -2369,7 +2380,7 @@
       </c>
       <c r="E57" s="7"/>
     </row>
-    <row r="58" spans="1:5">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="9" t="s">
         <v>194</v>
       </c>
@@ -2384,7 +2395,7 @@
       </c>
       <c r="E58" s="7"/>
     </row>
-    <row r="59" spans="1:5">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
         <v>196</v>
       </c>
@@ -2399,7 +2410,7 @@
       </c>
       <c r="E59" s="7"/>
     </row>
-    <row r="60" spans="1:5" ht="45">
+    <row r="60" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
         <v>199</v>
       </c>
@@ -2414,7 +2425,7 @@
       </c>
       <c r="E60" s="7"/>
     </row>
-    <row r="61" spans="1:5">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="9" t="s">
         <v>202</v>
       </c>
@@ -2429,7 +2440,7 @@
       </c>
       <c r="E61" s="7"/>
     </row>
-    <row r="62" spans="1:5">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="9" t="s">
         <v>204</v>
       </c>
@@ -2444,7 +2455,7 @@
       </c>
       <c r="E62" s="7"/>
     </row>
-    <row r="63" spans="1:5">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="9" t="s">
         <v>206</v>
       </c>
@@ -2459,7 +2470,7 @@
       </c>
       <c r="E63" s="7"/>
     </row>
-    <row r="64" spans="1:5">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="9" t="s">
         <v>208</v>
       </c>
@@ -2474,7 +2485,7 @@
       </c>
       <c r="E64" s="7"/>
     </row>
-    <row r="65" spans="1:5">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="9" t="s">
         <v>217</v>
       </c>
@@ -2489,7 +2500,7 @@
       </c>
       <c r="E65" s="7"/>
     </row>
-    <row r="66" spans="1:5">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="9" t="s">
         <v>218</v>
       </c>
@@ -2504,7 +2515,7 @@
       </c>
       <c r="E66" s="7"/>
     </row>
-    <row r="67" spans="1:5">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="9" t="s">
         <v>223</v>
       </c>
@@ -2519,7 +2530,7 @@
       </c>
       <c r="E67" s="7"/>
     </row>
-    <row r="68" spans="1:5">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="9" t="s">
         <v>224</v>
       </c>
@@ -2534,7 +2545,7 @@
       </c>
       <c r="E68" s="7"/>
     </row>
-    <row r="69" spans="1:5">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="9" t="s">
         <v>225</v>
       </c>
@@ -2549,7 +2560,7 @@
       </c>
       <c r="E69" s="7"/>
     </row>
-    <row r="70" spans="1:5">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="9" t="s">
         <v>226</v>
       </c>
@@ -2564,7 +2575,7 @@
       </c>
       <c r="E70" s="7"/>
     </row>
-    <row r="71" spans="1:5">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="9" t="s">
         <v>233</v>
       </c>
@@ -2579,7 +2590,7 @@
       </c>
       <c r="E71" s="7"/>
     </row>
-    <row r="72" spans="1:5">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="9" t="s">
         <v>237</v>
       </c>
@@ -2594,7 +2605,7 @@
       </c>
       <c r="E72" s="7"/>
     </row>
-    <row r="73" spans="1:5">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="9" t="s">
         <v>239</v>
       </c>
@@ -2609,7 +2620,7 @@
       </c>
       <c r="E73" s="7"/>
     </row>
-    <row r="74" spans="1:5">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="9" t="s">
         <v>243</v>
       </c>
@@ -2624,7 +2635,7 @@
       </c>
       <c r="E74" s="7"/>
     </row>
-    <row r="75" spans="1:5" ht="30">
+    <row r="75" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" s="9" t="s">
         <v>245</v>
       </c>
@@ -2639,7 +2650,7 @@
       </c>
       <c r="E75" s="7"/>
     </row>
-    <row r="76" spans="1:5">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="9" t="s">
         <v>248</v>
       </c>
@@ -2654,7 +2665,7 @@
       </c>
       <c r="E76" s="7"/>
     </row>
-    <row r="77" spans="1:5">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="9" t="s">
         <v>256</v>
       </c>
@@ -2669,7 +2680,7 @@
       </c>
       <c r="E77" s="7"/>
     </row>
-    <row r="78" spans="1:5">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="9" t="s">
         <v>257</v>
       </c>
@@ -2684,7 +2695,7 @@
       </c>
       <c r="E78" s="7"/>
     </row>
-    <row r="79" spans="1:5">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="9" t="s">
         <v>261</v>
       </c>
@@ -2699,7 +2710,7 @@
       </c>
       <c r="E79" s="7"/>
     </row>
-    <row r="80" spans="1:5">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="9" t="s">
         <v>264</v>
       </c>
@@ -2714,7 +2725,7 @@
       </c>
       <c r="E80" s="7"/>
     </row>
-    <row r="81" spans="1:5">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="9" t="s">
         <v>267</v>
       </c>
@@ -2729,7 +2740,7 @@
       </c>
       <c r="E81" s="7"/>
     </row>
-    <row r="82" spans="1:5" ht="30">
+    <row r="82" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A82" s="9" t="s">
         <v>269</v>
       </c>
@@ -2744,7 +2755,7 @@
       </c>
       <c r="E82" s="7"/>
     </row>
-    <row r="83" spans="1:5">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="9" t="s">
         <v>274</v>
       </c>
@@ -2759,7 +2770,7 @@
       </c>
       <c r="E83" s="7"/>
     </row>
-    <row r="84" spans="1:5" ht="30">
+    <row r="84" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A84" s="9" t="s">
         <v>277</v>
       </c>
@@ -2774,7 +2785,7 @@
       </c>
       <c r="E84" s="7"/>
     </row>
-    <row r="85" spans="1:5">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="9" t="s">
         <v>279</v>
       </c>
@@ -2789,7 +2800,7 @@
       </c>
       <c r="E85" s="7"/>
     </row>
-    <row r="86" spans="1:5">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="9" t="s">
         <v>282</v>
       </c>
@@ -2804,7 +2815,7 @@
       </c>
       <c r="E86" s="7"/>
     </row>
-    <row r="87" spans="1:5">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="9" t="s">
         <v>285</v>
       </c>
@@ -2819,7 +2830,7 @@
       </c>
       <c r="E87" s="7"/>
     </row>
-    <row r="88" spans="1:5">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="9" t="s">
         <v>288</v>
       </c>
@@ -2834,7 +2845,7 @@
       </c>
       <c r="E88" s="7"/>
     </row>
-    <row r="89" spans="1:5">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="9" t="s">
         <v>291</v>
       </c>
@@ -2849,7 +2860,7 @@
       </c>
       <c r="E89" s="7"/>
     </row>
-    <row r="90" spans="1:5">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="9" t="s">
         <v>294</v>
       </c>
@@ -2864,7 +2875,7 @@
       </c>
       <c r="E90" s="7"/>
     </row>
-    <row r="91" spans="1:5">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="9" t="s">
         <v>297</v>
       </c>
@@ -2879,7 +2890,7 @@
       </c>
       <c r="E91" s="7"/>
     </row>
-    <row r="92" spans="1:5">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="9" t="s">
         <v>300</v>
       </c>
@@ -2894,7 +2905,7 @@
       </c>
       <c r="E92" s="7"/>
     </row>
-    <row r="93" spans="1:5">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="9" t="s">
         <v>303</v>
       </c>
@@ -2909,7 +2920,7 @@
       </c>
       <c r="E93" s="7"/>
     </row>
-    <row r="94" spans="1:5">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="9" t="s">
         <v>306</v>
       </c>
@@ -2924,7 +2935,7 @@
       </c>
       <c r="E94" s="7"/>
     </row>
-    <row r="95" spans="1:5">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="9" t="s">
         <v>309</v>
       </c>
@@ -2939,7 +2950,7 @@
       </c>
       <c r="E95" s="7"/>
     </row>
-    <row r="96" spans="1:5">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="9" t="s">
         <v>314</v>
       </c>
@@ -2954,7 +2965,7 @@
       </c>
       <c r="E96" s="7"/>
     </row>
-    <row r="97" spans="1:5">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="9" t="s">
         <v>315</v>
       </c>
@@ -2969,7 +2980,7 @@
       </c>
       <c r="E97" s="7"/>
     </row>
-    <row r="98" spans="1:5">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="9" t="s">
         <v>319</v>
       </c>
@@ -2984,7 +2995,7 @@
       </c>
       <c r="E98" s="7"/>
     </row>
-    <row r="99" spans="1:5">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="9" t="s">
         <v>321</v>
       </c>
@@ -2999,7 +3010,7 @@
       </c>
       <c r="E99" s="7"/>
     </row>
-    <row r="100" spans="1:5">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="9" t="s">
         <v>322</v>
       </c>
@@ -3014,7 +3025,7 @@
       </c>
       <c r="E100" s="7"/>
     </row>
-    <row r="101" spans="1:5" ht="30">
+    <row r="101" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A101" s="9" t="s">
         <v>323</v>
       </c>
@@ -3029,7 +3040,7 @@
       </c>
       <c r="E101" s="7"/>
     </row>
-    <row r="102" spans="1:5">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="9" t="s">
         <v>328</v>
       </c>
@@ -3044,7 +3055,7 @@
       </c>
       <c r="E102" s="7"/>
     </row>
-    <row r="103" spans="1:5">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="9" t="s">
         <v>333</v>
       </c>
@@ -3059,7 +3070,7 @@
       </c>
       <c r="E103" s="7"/>
     </row>
-    <row r="104" spans="1:5">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="9" t="s">
         <v>336</v>
       </c>
@@ -3074,7 +3085,7 @@
       </c>
       <c r="E104" s="7"/>
     </row>
-    <row r="105" spans="1:5">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="9" t="s">
         <v>337</v>
       </c>
@@ -3089,7 +3100,7 @@
       </c>
       <c r="E105" s="7"/>
     </row>
-    <row r="106" spans="1:5">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="9" t="s">
         <v>342</v>
       </c>
@@ -3103,6 +3114,21 @@
         <v>5</v>
       </c>
       <c r="E106" s="7"/>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A107" s="9" t="s">
+        <v>345</v>
+      </c>
+      <c r="B107" s="9" t="s">
+        <v>346</v>
+      </c>
+      <c r="C107" s="8" t="s">
+        <v>347</v>
+      </c>
+      <c r="D107" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E107" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -3115,14 +3141,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView topLeftCell="A10" zoomScale="80" workbookViewId="0">
       <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
@@ -3130,7 +3156,7 @@
     <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>35</v>
       </c>
@@ -3144,7 +3170,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>37</v>
       </c>
@@ -3156,7 +3182,7 @@
       </c>
       <c r="D2" s="7"/>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>38</v>
       </c>
@@ -3168,7 +3194,7 @@
       </c>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>39</v>
       </c>
@@ -3180,7 +3206,7 @@
       </c>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>40</v>
       </c>
@@ -3192,7 +3218,7 @@
       </c>
       <c r="D5" s="7"/>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>41</v>
       </c>
@@ -3204,7 +3230,7 @@
       </c>
       <c r="D6" s="7"/>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>42</v>
       </c>
@@ -3216,7 +3242,7 @@
       </c>
       <c r="D7" s="7"/>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>43</v>
       </c>
@@ -3228,7 +3254,7 @@
       </c>
       <c r="D8" s="7"/>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>44</v>
       </c>
@@ -3240,7 +3266,7 @@
       </c>
       <c r="D9" s="7"/>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>45</v>
       </c>
@@ -3252,7 +3278,7 @@
       </c>
       <c r="D10" s="7"/>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>46</v>
       </c>
@@ -3264,7 +3290,7 @@
       </c>
       <c r="D11" s="7"/>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>48</v>
       </c>
@@ -3276,7 +3302,7 @@
       </c>
       <c r="D12" s="7"/>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>49</v>
       </c>
@@ -3288,7 +3314,7 @@
       </c>
       <c r="D13" s="7"/>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>50</v>
       </c>
@@ -3300,7 +3326,7 @@
       </c>
       <c r="D14" s="7"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>51</v>
       </c>
@@ -3312,7 +3338,7 @@
       </c>
       <c r="D15" s="7"/>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>52</v>
       </c>
@@ -3324,7 +3350,7 @@
       </c>
       <c r="D16" s="7"/>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>53</v>
       </c>
@@ -3336,7 +3362,7 @@
       </c>
       <c r="D17" s="7"/>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>54</v>
       </c>
@@ -3348,7 +3374,7 @@
       </c>
       <c r="D18" s="7"/>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>55</v>
       </c>
@@ -3360,7 +3386,7 @@
       </c>
       <c r="D19" s="7"/>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>56</v>
       </c>
@@ -3372,7 +3398,7 @@
       </c>
       <c r="D20" s="7"/>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>57</v>
       </c>
@@ -3384,7 +3410,7 @@
       </c>
       <c r="D21" s="7"/>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>58</v>
       </c>
@@ -3396,7 +3422,7 @@
       </c>
       <c r="D22" s="7"/>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>59</v>
       </c>
@@ -3408,7 +3434,7 @@
       </c>
       <c r="D23" s="7"/>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>60</v>
       </c>
@@ -3420,7 +3446,7 @@
       </c>
       <c r="D24" s="7"/>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>61</v>
       </c>
@@ -3432,7 +3458,7 @@
       </c>
       <c r="D25" s="7"/>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>47</v>
       </c>
@@ -3451,14 +3477,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A19" sqref="A19:XFD19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
@@ -3466,7 +3492,7 @@
     <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>35</v>
       </c>
@@ -3480,7 +3506,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>37</v>
       </c>
@@ -3492,7 +3518,7 @@
       </c>
       <c r="D2" s="7"/>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>38</v>
       </c>
@@ -3504,7 +3530,7 @@
       </c>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>39</v>
       </c>
@@ -3516,7 +3542,7 @@
       </c>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>40</v>
       </c>
@@ -3528,7 +3554,7 @@
       </c>
       <c r="D5" s="7"/>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>41</v>
       </c>
@@ -3540,7 +3566,7 @@
       </c>
       <c r="D6" s="7"/>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>42</v>
       </c>
@@ -3552,7 +3578,7 @@
       </c>
       <c r="D7" s="7"/>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>43</v>
       </c>
@@ -3564,7 +3590,7 @@
       </c>
       <c r="D8" s="7"/>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>44</v>
       </c>
@@ -3576,7 +3602,7 @@
       </c>
       <c r="D9" s="7"/>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>45</v>
       </c>
@@ -3588,7 +3614,7 @@
       </c>
       <c r="D10" s="7"/>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>46</v>
       </c>
@@ -3600,7 +3626,7 @@
       </c>
       <c r="D11" s="7"/>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>47</v>
       </c>
@@ -3612,7 +3638,7 @@
       </c>
       <c r="D12" s="7"/>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>48</v>
       </c>
@@ -3624,7 +3650,7 @@
       </c>
       <c r="D13" s="7"/>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>49</v>
       </c>
@@ -3636,7 +3662,7 @@
       </c>
       <c r="D14" s="7"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>50</v>
       </c>
@@ -3648,7 +3674,7 @@
       </c>
       <c r="D15" s="7"/>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>51</v>
       </c>
@@ -3660,7 +3686,7 @@
       </c>
       <c r="D16" s="7"/>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>52</v>
       </c>
@@ -3672,7 +3698,7 @@
       </c>
       <c r="D17" s="7"/>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>53</v>
       </c>
@@ -3684,7 +3710,7 @@
       </c>
       <c r="D18" s="7"/>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>54</v>
       </c>
@@ -3696,7 +3722,7 @@
       </c>
       <c r="D19" s="7"/>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>55</v>
       </c>
@@ -3708,7 +3734,7 @@
       </c>
       <c r="D20" s="7"/>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>56</v>
       </c>
@@ -3720,7 +3746,7 @@
       </c>
       <c r="D21" s="7"/>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>57</v>
       </c>
@@ -3732,7 +3758,7 @@
       </c>
       <c r="D22" s="7"/>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>58</v>
       </c>
@@ -3744,7 +3770,7 @@
       </c>
       <c r="D23" s="7"/>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>59</v>
       </c>
@@ -3756,7 +3782,7 @@
       </c>
       <c r="D24" s="7"/>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>60</v>
       </c>
@@ -3768,7 +3794,7 @@
       </c>
       <c r="D25" s="7"/>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>61</v>
       </c>

</xml_diff>

<commit_message>
Adds WAT109 testscript and related changes
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/WAT.xlsx
+++ b/src/test/resources/xls/WAT.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="351">
   <si>
     <t>TCID</t>
   </si>
@@ -1060,7 +1060,16 @@
     <t>WAT-326</t>
   </si>
   <si>
-    <t>"Verify that specific text is displayed when the author search results fetched are more than 50 clusters."</t>
+    <t>WAT-325</t>
+  </si>
+  <si>
+    <t>Verify that there is an option to remove alternate name in search page.</t>
+  </si>
+  <si>
+    <t>Verify that specific text is displayed when the author search results fetched are more than 50 clusters.</t>
+  </si>
+  <si>
+    <t>WAT109</t>
   </si>
 </sst>
 </file>
@@ -1508,10 +1517,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E107"/>
+  <dimension ref="A1:E108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A92" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C107" sqref="C107"/>
+    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A108" sqref="A108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3123,12 +3132,27 @@
         <v>346</v>
       </c>
       <c r="C107" s="8" t="s">
+        <v>349</v>
+      </c>
+      <c r="D107" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E107" s="7"/>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A108" s="9" t="s">
+        <v>350</v>
+      </c>
+      <c r="B108" s="9" t="s">
         <v>347</v>
       </c>
-      <c r="D107" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="E107" s="7"/>
+      <c r="C108" s="8" t="s">
+        <v>348</v>
+      </c>
+      <c r="D108" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E108" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Adds WAT110 testscript and related changes
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/WAT.xlsx
+++ b/src/test/resources/xls/WAT.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13305" windowHeight="2415"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="595" uniqueCount="354">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="357">
   <si>
     <t>TCID</t>
   </si>
@@ -1079,13 +1079,22 @@
   </si>
   <si>
     <t>WAT-375||WAT-377</t>
+  </si>
+  <si>
+    <t>WAT110</t>
+  </si>
+  <si>
+    <t>WAT-324</t>
+  </si>
+  <si>
+    <t>Verify that tab name for ORCiD search will be "ORCiD search"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1282,7 +1291,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1314,9 +1323,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1348,6 +1358,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1523,14 +1534,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E109"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E110"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A83" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D107" sqref="D107"/>
+      <selection activeCell="C110" sqref="C110"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="41" bestFit="1" customWidth="1" collapsed="1"/>
@@ -1539,7 +1550,7 @@
     <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1556,7 +1567,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -1571,7 +1582,7 @@
       </c>
       <c r="E2" s="4"/>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -1586,7 +1597,7 @@
       </c>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>11</v>
       </c>
@@ -1601,7 +1612,7 @@
       </c>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>12</v>
       </c>
@@ -1616,7 +1627,7 @@
       </c>
       <c r="E5" s="7"/>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>14</v>
       </c>
@@ -1631,7 +1642,7 @@
       </c>
       <c r="E6" s="7"/>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>17</v>
       </c>
@@ -1646,7 +1657,7 @@
       </c>
       <c r="E7" s="7"/>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>20</v>
       </c>
@@ -1661,7 +1672,7 @@
       </c>
       <c r="E8" s="7"/>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>22</v>
       </c>
@@ -1676,7 +1687,7 @@
       </c>
       <c r="E9" s="7"/>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>23</v>
       </c>
@@ -1691,7 +1702,7 @@
       </c>
       <c r="E10" s="7"/>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>24</v>
       </c>
@@ -1706,7 +1717,7 @@
       </c>
       <c r="E11" s="7"/>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>25</v>
       </c>
@@ -1721,7 +1732,7 @@
       </c>
       <c r="E12" s="7"/>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>62</v>
       </c>
@@ -1736,7 +1747,7 @@
       </c>
       <c r="E13" s="7"/>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>63</v>
       </c>
@@ -1751,7 +1762,7 @@
       </c>
       <c r="E14" s="7"/>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>64</v>
       </c>
@@ -1766,7 +1777,7 @@
       </c>
       <c r="E15" s="7"/>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>65</v>
       </c>
@@ -1781,7 +1792,7 @@
       </c>
       <c r="E16" s="7"/>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>74</v>
       </c>
@@ -1796,7 +1807,7 @@
       </c>
       <c r="E17" s="7"/>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>75</v>
       </c>
@@ -1811,7 +1822,7 @@
       </c>
       <c r="E18" s="7"/>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>79</v>
       </c>
@@ -1826,7 +1837,7 @@
       </c>
       <c r="E19" s="7"/>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>81</v>
       </c>
@@ -1841,7 +1852,7 @@
       </c>
       <c r="E20" s="7"/>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>82</v>
       </c>
@@ -1856,7 +1867,7 @@
       </c>
       <c r="E21" s="7"/>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>88</v>
       </c>
@@ -1871,7 +1882,7 @@
       </c>
       <c r="E22" s="7"/>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>90</v>
       </c>
@@ -1886,7 +1897,7 @@
       </c>
       <c r="E23" s="7"/>
     </row>
-    <row r="24" spans="1:5" ht="30">
+    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>94</v>
       </c>
@@ -1901,7 +1912,7 @@
       </c>
       <c r="E24" s="7"/>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>96</v>
       </c>
@@ -1916,7 +1927,7 @@
       </c>
       <c r="E25" s="7"/>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
         <v>98</v>
       </c>
@@ -1931,7 +1942,7 @@
       </c>
       <c r="E26" s="7"/>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
         <v>102</v>
       </c>
@@ -1946,7 +1957,7 @@
       </c>
       <c r="E27" s="7"/>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
         <v>105</v>
       </c>
@@ -1961,7 +1972,7 @@
       </c>
       <c r="E28" s="7"/>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
         <v>108</v>
       </c>
@@ -1976,7 +1987,7 @@
       </c>
       <c r="E29" s="7"/>
     </row>
-    <row r="30" spans="1:5" ht="30">
+    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
         <v>110</v>
       </c>
@@ -1991,7 +2002,7 @@
       </c>
       <c r="E30" s="7"/>
     </row>
-    <row r="31" spans="1:5" ht="30">
+    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
         <v>114</v>
       </c>
@@ -2006,7 +2017,7 @@
       </c>
       <c r="E31" s="7"/>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
         <v>119</v>
       </c>
@@ -2021,7 +2032,7 @@
       </c>
       <c r="E32" s="7"/>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
         <v>120</v>
       </c>
@@ -2036,7 +2047,7 @@
       </c>
       <c r="E33" s="7"/>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
         <v>125</v>
       </c>
@@ -2051,7 +2062,7 @@
       </c>
       <c r="E34" s="7"/>
     </row>
-    <row r="35" spans="1:5" ht="30">
+    <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
         <v>128</v>
       </c>
@@ -2066,7 +2077,7 @@
       </c>
       <c r="E35" s="7"/>
     </row>
-    <row r="36" spans="1:5" ht="30">
+    <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
         <v>131</v>
       </c>
@@ -2081,7 +2092,7 @@
       </c>
       <c r="E36" s="7"/>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
         <v>134</v>
       </c>
@@ -2096,7 +2107,7 @@
       </c>
       <c r="E37" s="7"/>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="9" t="s">
         <v>137</v>
       </c>
@@ -2111,7 +2122,7 @@
       </c>
       <c r="E38" s="7"/>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="s">
         <v>140</v>
       </c>
@@ -2126,7 +2137,7 @@
       </c>
       <c r="E39" s="7"/>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="9" t="s">
         <v>143</v>
       </c>
@@ -2141,7 +2152,7 @@
       </c>
       <c r="E40" s="7"/>
     </row>
-    <row r="41" spans="1:5" ht="30">
+    <row r="41" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
         <v>145</v>
       </c>
@@ -2156,7 +2167,7 @@
       </c>
       <c r="E41" s="7"/>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="9" t="s">
         <v>147</v>
       </c>
@@ -2171,7 +2182,7 @@
       </c>
       <c r="E42" s="7"/>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="9" t="s">
         <v>150</v>
       </c>
@@ -2186,7 +2197,7 @@
       </c>
       <c r="E43" s="7"/>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="9" t="s">
         <v>153</v>
       </c>
@@ -2201,7 +2212,7 @@
       </c>
       <c r="E44" s="7"/>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="9" t="s">
         <v>155</v>
       </c>
@@ -2216,7 +2227,7 @@
       </c>
       <c r="E45" s="7"/>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="12" t="s">
         <v>158</v>
       </c>
@@ -2231,7 +2242,7 @@
       </c>
       <c r="E46" s="7"/>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="12" t="s">
         <v>159</v>
       </c>
@@ -2246,7 +2257,7 @@
       </c>
       <c r="E47" s="7"/>
     </row>
-    <row r="48" spans="1:5" ht="30">
+    <row r="48" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="12" t="s">
         <v>160</v>
       </c>
@@ -2261,7 +2272,7 @@
       </c>
       <c r="E48" s="7"/>
     </row>
-    <row r="49" spans="1:5" ht="30">
+    <row r="49" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="12" t="s">
         <v>161</v>
       </c>
@@ -2276,7 +2287,7 @@
       </c>
       <c r="E49" s="7"/>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="12" t="s">
         <v>164</v>
       </c>
@@ -2291,7 +2302,7 @@
       </c>
       <c r="E50" s="7"/>
     </row>
-    <row r="51" spans="1:5" ht="30">
+    <row r="51" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="9" t="s">
         <v>173</v>
       </c>
@@ -2306,7 +2317,7 @@
       </c>
       <c r="E51" s="7"/>
     </row>
-    <row r="52" spans="1:5">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="9" t="s">
         <v>174</v>
       </c>
@@ -2321,7 +2332,7 @@
       </c>
       <c r="E52" s="7"/>
     </row>
-    <row r="53" spans="1:5">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="9" t="s">
         <v>179</v>
       </c>
@@ -2336,7 +2347,7 @@
       </c>
       <c r="E53" s="7"/>
     </row>
-    <row r="54" spans="1:5">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="9" t="s">
         <v>180</v>
       </c>
@@ -2351,7 +2362,7 @@
       </c>
       <c r="E54" s="7"/>
     </row>
-    <row r="55" spans="1:5">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="9" t="s">
         <v>185</v>
       </c>
@@ -2366,7 +2377,7 @@
       </c>
       <c r="E55" s="7"/>
     </row>
-    <row r="56" spans="1:5">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="s">
         <v>188</v>
       </c>
@@ -2381,7 +2392,7 @@
       </c>
       <c r="E56" s="7"/>
     </row>
-    <row r="57" spans="1:5" ht="30">
+    <row r="57" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="9" t="s">
         <v>191</v>
       </c>
@@ -2396,7 +2407,7 @@
       </c>
       <c r="E57" s="7"/>
     </row>
-    <row r="58" spans="1:5">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="9" t="s">
         <v>194</v>
       </c>
@@ -2411,7 +2422,7 @@
       </c>
       <c r="E58" s="7"/>
     </row>
-    <row r="59" spans="1:5">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
         <v>196</v>
       </c>
@@ -2426,7 +2437,7 @@
       </c>
       <c r="E59" s="7"/>
     </row>
-    <row r="60" spans="1:5" ht="45">
+    <row r="60" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
         <v>199</v>
       </c>
@@ -2441,7 +2452,7 @@
       </c>
       <c r="E60" s="7"/>
     </row>
-    <row r="61" spans="1:5">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="9" t="s">
         <v>202</v>
       </c>
@@ -2456,7 +2467,7 @@
       </c>
       <c r="E61" s="7"/>
     </row>
-    <row r="62" spans="1:5">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="9" t="s">
         <v>204</v>
       </c>
@@ -2471,7 +2482,7 @@
       </c>
       <c r="E62" s="7"/>
     </row>
-    <row r="63" spans="1:5">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="9" t="s">
         <v>206</v>
       </c>
@@ -2486,7 +2497,7 @@
       </c>
       <c r="E63" s="7"/>
     </row>
-    <row r="64" spans="1:5">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="9" t="s">
         <v>208</v>
       </c>
@@ -2501,7 +2512,7 @@
       </c>
       <c r="E64" s="7"/>
     </row>
-    <row r="65" spans="1:5">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="9" t="s">
         <v>217</v>
       </c>
@@ -2516,7 +2527,7 @@
       </c>
       <c r="E65" s="7"/>
     </row>
-    <row r="66" spans="1:5">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="9" t="s">
         <v>218</v>
       </c>
@@ -2531,7 +2542,7 @@
       </c>
       <c r="E66" s="7"/>
     </row>
-    <row r="67" spans="1:5">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="9" t="s">
         <v>223</v>
       </c>
@@ -2546,7 +2557,7 @@
       </c>
       <c r="E67" s="7"/>
     </row>
-    <row r="68" spans="1:5">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="9" t="s">
         <v>224</v>
       </c>
@@ -2561,7 +2572,7 @@
       </c>
       <c r="E68" s="7"/>
     </row>
-    <row r="69" spans="1:5">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="9" t="s">
         <v>225</v>
       </c>
@@ -2576,7 +2587,7 @@
       </c>
       <c r="E69" s="7"/>
     </row>
-    <row r="70" spans="1:5">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="9" t="s">
         <v>226</v>
       </c>
@@ -2591,7 +2602,7 @@
       </c>
       <c r="E70" s="7"/>
     </row>
-    <row r="71" spans="1:5">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="9" t="s">
         <v>233</v>
       </c>
@@ -2606,7 +2617,7 @@
       </c>
       <c r="E71" s="7"/>
     </row>
-    <row r="72" spans="1:5">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="9" t="s">
         <v>237</v>
       </c>
@@ -2621,7 +2632,7 @@
       </c>
       <c r="E72" s="7"/>
     </row>
-    <row r="73" spans="1:5">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="9" t="s">
         <v>239</v>
       </c>
@@ -2636,7 +2647,7 @@
       </c>
       <c r="E73" s="7"/>
     </row>
-    <row r="74" spans="1:5">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="9" t="s">
         <v>243</v>
       </c>
@@ -2651,7 +2662,7 @@
       </c>
       <c r="E74" s="7"/>
     </row>
-    <row r="75" spans="1:5" ht="30">
+    <row r="75" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" s="9" t="s">
         <v>245</v>
       </c>
@@ -2666,7 +2677,7 @@
       </c>
       <c r="E75" s="7"/>
     </row>
-    <row r="76" spans="1:5">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="9" t="s">
         <v>248</v>
       </c>
@@ -2681,7 +2692,7 @@
       </c>
       <c r="E76" s="7"/>
     </row>
-    <row r="77" spans="1:5">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="9" t="s">
         <v>256</v>
       </c>
@@ -2696,7 +2707,7 @@
       </c>
       <c r="E77" s="7"/>
     </row>
-    <row r="78" spans="1:5">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="9" t="s">
         <v>257</v>
       </c>
@@ -2711,7 +2722,7 @@
       </c>
       <c r="E78" s="7"/>
     </row>
-    <row r="79" spans="1:5">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="9" t="s">
         <v>261</v>
       </c>
@@ -2726,7 +2737,7 @@
       </c>
       <c r="E79" s="7"/>
     </row>
-    <row r="80" spans="1:5">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="9" t="s">
         <v>264</v>
       </c>
@@ -2741,7 +2752,7 @@
       </c>
       <c r="E80" s="7"/>
     </row>
-    <row r="81" spans="1:5">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="9" t="s">
         <v>267</v>
       </c>
@@ -2756,7 +2767,7 @@
       </c>
       <c r="E81" s="7"/>
     </row>
-    <row r="82" spans="1:5" ht="30">
+    <row r="82" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A82" s="9" t="s">
         <v>269</v>
       </c>
@@ -2771,7 +2782,7 @@
       </c>
       <c r="E82" s="7"/>
     </row>
-    <row r="83" spans="1:5">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="9" t="s">
         <v>274</v>
       </c>
@@ -2786,7 +2797,7 @@
       </c>
       <c r="E83" s="7"/>
     </row>
-    <row r="84" spans="1:5" ht="30">
+    <row r="84" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A84" s="9" t="s">
         <v>277</v>
       </c>
@@ -2801,7 +2812,7 @@
       </c>
       <c r="E84" s="7"/>
     </row>
-    <row r="85" spans="1:5">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="9" t="s">
         <v>279</v>
       </c>
@@ -2816,7 +2827,7 @@
       </c>
       <c r="E85" s="7"/>
     </row>
-    <row r="86" spans="1:5">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="9" t="s">
         <v>282</v>
       </c>
@@ -2831,7 +2842,7 @@
       </c>
       <c r="E86" s="7"/>
     </row>
-    <row r="87" spans="1:5">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="9" t="s">
         <v>285</v>
       </c>
@@ -2846,7 +2857,7 @@
       </c>
       <c r="E87" s="7"/>
     </row>
-    <row r="88" spans="1:5">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="9" t="s">
         <v>288</v>
       </c>
@@ -2861,7 +2872,7 @@
       </c>
       <c r="E88" s="7"/>
     </row>
-    <row r="89" spans="1:5">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="9" t="s">
         <v>291</v>
       </c>
@@ -2876,7 +2887,7 @@
       </c>
       <c r="E89" s="7"/>
     </row>
-    <row r="90" spans="1:5">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="9" t="s">
         <v>294</v>
       </c>
@@ -2891,7 +2902,7 @@
       </c>
       <c r="E90" s="7"/>
     </row>
-    <row r="91" spans="1:5">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="9" t="s">
         <v>297</v>
       </c>
@@ -2906,7 +2917,7 @@
       </c>
       <c r="E91" s="7"/>
     </row>
-    <row r="92" spans="1:5">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="9" t="s">
         <v>300</v>
       </c>
@@ -2921,7 +2932,7 @@
       </c>
       <c r="E92" s="7"/>
     </row>
-    <row r="93" spans="1:5">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="9" t="s">
         <v>303</v>
       </c>
@@ -2936,7 +2947,7 @@
       </c>
       <c r="E93" s="7"/>
     </row>
-    <row r="94" spans="1:5">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="9" t="s">
         <v>306</v>
       </c>
@@ -2951,7 +2962,7 @@
       </c>
       <c r="E94" s="7"/>
     </row>
-    <row r="95" spans="1:5">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="9" t="s">
         <v>309</v>
       </c>
@@ -2966,7 +2977,7 @@
       </c>
       <c r="E95" s="7"/>
     </row>
-    <row r="96" spans="1:5">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="9" t="s">
         <v>314</v>
       </c>
@@ -2981,7 +2992,7 @@
       </c>
       <c r="E96" s="7"/>
     </row>
-    <row r="97" spans="1:5">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="9" t="s">
         <v>315</v>
       </c>
@@ -2996,7 +3007,7 @@
       </c>
       <c r="E97" s="7"/>
     </row>
-    <row r="98" spans="1:5">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="9" t="s">
         <v>319</v>
       </c>
@@ -3011,7 +3022,7 @@
       </c>
       <c r="E98" s="7"/>
     </row>
-    <row r="99" spans="1:5">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="9" t="s">
         <v>321</v>
       </c>
@@ -3026,7 +3037,7 @@
       </c>
       <c r="E99" s="7"/>
     </row>
-    <row r="100" spans="1:5">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="9" t="s">
         <v>322</v>
       </c>
@@ -3041,7 +3052,7 @@
       </c>
       <c r="E100" s="7"/>
     </row>
-    <row r="101" spans="1:5" ht="30">
+    <row r="101" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A101" s="9" t="s">
         <v>323</v>
       </c>
@@ -3056,7 +3067,7 @@
       </c>
       <c r="E101" s="7"/>
     </row>
-    <row r="102" spans="1:5">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="9" t="s">
         <v>328</v>
       </c>
@@ -3071,7 +3082,7 @@
       </c>
       <c r="E102" s="7"/>
     </row>
-    <row r="103" spans="1:5">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="9" t="s">
         <v>333</v>
       </c>
@@ -3086,7 +3097,7 @@
       </c>
       <c r="E103" s="7"/>
     </row>
-    <row r="104" spans="1:5">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="9" t="s">
         <v>336</v>
       </c>
@@ -3101,7 +3112,7 @@
       </c>
       <c r="E104" s="7"/>
     </row>
-    <row r="105" spans="1:5">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="9" t="s">
         <v>337</v>
       </c>
@@ -3116,7 +3127,7 @@
       </c>
       <c r="E105" s="7"/>
     </row>
-    <row r="106" spans="1:5">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="9" t="s">
         <v>342</v>
       </c>
@@ -3131,7 +3142,7 @@
       </c>
       <c r="E106" s="7"/>
     </row>
-    <row r="107" spans="1:5">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="9" t="s">
         <v>345</v>
       </c>
@@ -3146,7 +3157,7 @@
       </c>
       <c r="E107" s="7"/>
     </row>
-    <row r="108" spans="1:5">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="9" t="s">
         <v>350</v>
       </c>
@@ -3161,7 +3172,7 @@
       </c>
       <c r="E108" s="7"/>
     </row>
-    <row r="109" spans="1:5" ht="30">
+    <row r="109" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A109" s="9" t="s">
         <v>351</v>
       </c>
@@ -3175,6 +3186,21 @@
         <v>5</v>
       </c>
       <c r="E109" s="7"/>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A110" s="9" t="s">
+        <v>354</v>
+      </c>
+      <c r="B110" s="9" t="s">
+        <v>355</v>
+      </c>
+      <c r="C110" s="8" t="s">
+        <v>356</v>
+      </c>
+      <c r="D110" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E110" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -3187,14 +3213,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView topLeftCell="A10" zoomScale="80" workbookViewId="0">
       <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
@@ -3202,7 +3228,7 @@
     <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>35</v>
       </c>
@@ -3216,7 +3242,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>37</v>
       </c>
@@ -3228,7 +3254,7 @@
       </c>
       <c r="D2" s="7"/>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>38</v>
       </c>
@@ -3240,7 +3266,7 @@
       </c>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>39</v>
       </c>
@@ -3252,7 +3278,7 @@
       </c>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>40</v>
       </c>
@@ -3264,7 +3290,7 @@
       </c>
       <c r="D5" s="7"/>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>41</v>
       </c>
@@ -3276,7 +3302,7 @@
       </c>
       <c r="D6" s="7"/>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>42</v>
       </c>
@@ -3288,7 +3314,7 @@
       </c>
       <c r="D7" s="7"/>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>43</v>
       </c>
@@ -3300,7 +3326,7 @@
       </c>
       <c r="D8" s="7"/>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>44</v>
       </c>
@@ -3312,7 +3338,7 @@
       </c>
       <c r="D9" s="7"/>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>45</v>
       </c>
@@ -3324,7 +3350,7 @@
       </c>
       <c r="D10" s="7"/>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>46</v>
       </c>
@@ -3336,7 +3362,7 @@
       </c>
       <c r="D11" s="7"/>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>48</v>
       </c>
@@ -3348,7 +3374,7 @@
       </c>
       <c r="D12" s="7"/>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>49</v>
       </c>
@@ -3360,7 +3386,7 @@
       </c>
       <c r="D13" s="7"/>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>50</v>
       </c>
@@ -3372,7 +3398,7 @@
       </c>
       <c r="D14" s="7"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>51</v>
       </c>
@@ -3384,7 +3410,7 @@
       </c>
       <c r="D15" s="7"/>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>52</v>
       </c>
@@ -3396,7 +3422,7 @@
       </c>
       <c r="D16" s="7"/>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>53</v>
       </c>
@@ -3408,7 +3434,7 @@
       </c>
       <c r="D17" s="7"/>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>54</v>
       </c>
@@ -3420,7 +3446,7 @@
       </c>
       <c r="D18" s="7"/>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>55</v>
       </c>
@@ -3432,7 +3458,7 @@
       </c>
       <c r="D19" s="7"/>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>56</v>
       </c>
@@ -3444,7 +3470,7 @@
       </c>
       <c r="D20" s="7"/>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>57</v>
       </c>
@@ -3456,7 +3482,7 @@
       </c>
       <c r="D21" s="7"/>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>58</v>
       </c>
@@ -3468,7 +3494,7 @@
       </c>
       <c r="D22" s="7"/>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>59</v>
       </c>
@@ -3480,7 +3506,7 @@
       </c>
       <c r="D23" s="7"/>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>60</v>
       </c>
@@ -3492,7 +3518,7 @@
       </c>
       <c r="D24" s="7"/>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>61</v>
       </c>
@@ -3504,7 +3530,7 @@
       </c>
       <c r="D25" s="7"/>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>47</v>
       </c>
@@ -3523,14 +3549,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A19" sqref="A19:XFD19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
@@ -3538,7 +3564,7 @@
     <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>35</v>
       </c>
@@ -3552,7 +3578,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>37</v>
       </c>
@@ -3564,7 +3590,7 @@
       </c>
       <c r="D2" s="7"/>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>38</v>
       </c>
@@ -3576,7 +3602,7 @@
       </c>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>39</v>
       </c>
@@ -3588,7 +3614,7 @@
       </c>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>40</v>
       </c>
@@ -3600,7 +3626,7 @@
       </c>
       <c r="D5" s="7"/>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>41</v>
       </c>
@@ -3612,7 +3638,7 @@
       </c>
       <c r="D6" s="7"/>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>42</v>
       </c>
@@ -3624,7 +3650,7 @@
       </c>
       <c r="D7" s="7"/>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>43</v>
       </c>
@@ -3636,7 +3662,7 @@
       </c>
       <c r="D8" s="7"/>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>44</v>
       </c>
@@ -3648,7 +3674,7 @@
       </c>
       <c r="D9" s="7"/>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>45</v>
       </c>
@@ -3660,7 +3686,7 @@
       </c>
       <c r="D10" s="7"/>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>46</v>
       </c>
@@ -3672,7 +3698,7 @@
       </c>
       <c r="D11" s="7"/>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>47</v>
       </c>
@@ -3684,7 +3710,7 @@
       </c>
       <c r="D12" s="7"/>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>48</v>
       </c>
@@ -3696,7 +3722,7 @@
       </c>
       <c r="D13" s="7"/>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>49</v>
       </c>
@@ -3708,7 +3734,7 @@
       </c>
       <c r="D14" s="7"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>50</v>
       </c>
@@ -3720,7 +3746,7 @@
       </c>
       <c r="D15" s="7"/>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>51</v>
       </c>
@@ -3732,7 +3758,7 @@
       </c>
       <c r="D16" s="7"/>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>52</v>
       </c>
@@ -3744,7 +3770,7 @@
       </c>
       <c r="D17" s="7"/>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>53</v>
       </c>
@@ -3756,7 +3782,7 @@
       </c>
       <c r="D18" s="7"/>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>54</v>
       </c>
@@ -3768,7 +3794,7 @@
       </c>
       <c r="D19" s="7"/>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>55</v>
       </c>
@@ -3780,7 +3806,7 @@
       </c>
       <c r="D20" s="7"/>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>56</v>
       </c>
@@ -3792,7 +3818,7 @@
       </c>
       <c r="D21" s="7"/>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>57</v>
       </c>
@@ -3804,7 +3830,7 @@
       </c>
       <c r="D22" s="7"/>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>58</v>
       </c>
@@ -3816,7 +3842,7 @@
       </c>
       <c r="D23" s="7"/>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>59</v>
       </c>
@@ -3828,7 +3854,7 @@
       </c>
       <c r="D24" s="7"/>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>60</v>
       </c>
@@ -3840,7 +3866,7 @@
       </c>
       <c r="D25" s="7"/>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>61</v>
       </c>

</xml_diff>

<commit_message>
Adds WAT111 and related changes
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/WAT.xlsx
+++ b/src/test/resources/xls/WAT.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="357">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="360">
   <si>
     <t>TCID</t>
   </si>
@@ -1088,6 +1088,15 @@
   </si>
   <si>
     <t>Verify that tab name for ORCiD search will be "ORCiD search"</t>
+  </si>
+  <si>
+    <t>WAT111</t>
+  </si>
+  <si>
+    <t>WAT-322</t>
+  </si>
+  <si>
+    <t>Verify that Add alternative name icon is gray until the name has been entered in each name module</t>
   </si>
 </sst>
 </file>
@@ -1535,10 +1544,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E110"/>
+  <dimension ref="A1:E111"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A83" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C110" sqref="C110"/>
+      <selection activeCell="C111" sqref="C111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3201,6 +3210,21 @@
         <v>5</v>
       </c>
       <c r="E110" s="7"/>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A111" s="9" t="s">
+        <v>357</v>
+      </c>
+      <c r="B111" s="9" t="s">
+        <v>358</v>
+      </c>
+      <c r="C111" s="8" t="s">
+        <v>359</v>
+      </c>
+      <c r="D111" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E111" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Adds WAT112 testscript and related changes
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/WAT.xlsx
+++ b/src/test/resources/xls/WAT.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="360">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="363">
   <si>
     <t>TCID</t>
   </si>
@@ -1097,13 +1097,22 @@
   </si>
   <si>
     <t>Verify that Add alternative name icon is gray until the name has been entered in each name module</t>
+  </si>
+  <si>
+    <t>WAT-321</t>
+  </si>
+  <si>
+    <t>WAT112</t>
+  </si>
+  <si>
+    <t>Verify that the Name Search is enabled by default</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1131,6 +1140,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1152,7 +1167,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -1175,11 +1190,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1212,6 +1242,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1544,10 +1577,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E111"/>
+  <dimension ref="A1:E112"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A83" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C111" sqref="C111"/>
+      <selection activeCell="C112" sqref="C112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3225,6 +3258,21 @@
         <v>5</v>
       </c>
       <c r="E111" s="7"/>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A112" s="9" t="s">
+        <v>361</v>
+      </c>
+      <c r="B112" s="9" t="s">
+        <v>360</v>
+      </c>
+      <c r="C112" s="16" t="s">
+        <v>362</v>
+      </c>
+      <c r="D112" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E112" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Adds WAT113 testscript and related changes
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/WAT.xlsx
+++ b/src/test/resources/xls/WAT.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="363">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="366">
   <si>
     <t>TCID</t>
   </si>
@@ -1106,6 +1106,15 @@
   </si>
   <si>
     <t>Verify that the Name Search is enabled by default</t>
+  </si>
+  <si>
+    <t>WAT113</t>
+  </si>
+  <si>
+    <t>WAT-317</t>
+  </si>
+  <si>
+    <t>Verify that sub text below the search title is "Enter the author's name or ORCiD to begin your search against Web of Science article groups"</t>
   </si>
 </sst>
 </file>
@@ -1577,10 +1586,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E112"/>
+  <dimension ref="A1:E113"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A83" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C112" sqref="C112"/>
+      <selection activeCell="C113" sqref="C113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3273,6 +3282,21 @@
         <v>5</v>
       </c>
       <c r="E112" s="7"/>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A113" s="9" t="s">
+        <v>363</v>
+      </c>
+      <c r="B113" s="9" t="s">
+        <v>364</v>
+      </c>
+      <c r="C113" s="16" t="s">
+        <v>365</v>
+      </c>
+      <c r="D113" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E113" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Adds WAT-114 test script
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/WAT.xlsx
+++ b/src/test/resources/xls/WAT.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13305" windowHeight="2415"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="378">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="381">
   <si>
     <t>TCID</t>
   </si>
@@ -1151,13 +1151,22 @@
   </si>
   <si>
     <t xml:space="preserve">Verify that ballon popover should disappear when user clicked on outside of the popover on the Search page </t>
+  </si>
+  <si>
+    <t>WAT114</t>
+  </si>
+  <si>
+    <t>WAT-1318</t>
+  </si>
+  <si>
+    <t>Verify that during an author search, if the system determines that there are &gt;50 search results then country dropdown should be displayed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1409,7 +1418,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1441,9 +1450,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1475,6 +1485,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1650,14 +1661,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E117"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A101" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C123" sqref="C123"/>
+    <sheetView tabSelected="1" topLeftCell="A98" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C124" sqref="C124"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="41" bestFit="1" customWidth="1" collapsed="1"/>
@@ -1666,7 +1677,7 @@
     <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1683,7 +1694,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -1698,7 +1709,7 @@
       </c>
       <c r="E2" s="4"/>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -1713,7 +1724,7 @@
       </c>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>11</v>
       </c>
@@ -1728,7 +1739,7 @@
       </c>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>12</v>
       </c>
@@ -1743,7 +1754,7 @@
       </c>
       <c r="E5" s="7"/>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>14</v>
       </c>
@@ -1758,7 +1769,7 @@
       </c>
       <c r="E6" s="7"/>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>17</v>
       </c>
@@ -1773,7 +1784,7 @@
       </c>
       <c r="E7" s="7"/>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>20</v>
       </c>
@@ -1788,7 +1799,7 @@
       </c>
       <c r="E8" s="7"/>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>22</v>
       </c>
@@ -1803,7 +1814,7 @@
       </c>
       <c r="E9" s="7"/>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>23</v>
       </c>
@@ -1818,7 +1829,7 @@
       </c>
       <c r="E10" s="7"/>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>24</v>
       </c>
@@ -1833,7 +1844,7 @@
       </c>
       <c r="E11" s="7"/>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>25</v>
       </c>
@@ -1848,7 +1859,7 @@
       </c>
       <c r="E12" s="7"/>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>62</v>
       </c>
@@ -1863,7 +1874,7 @@
       </c>
       <c r="E13" s="7"/>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>63</v>
       </c>
@@ -1878,7 +1889,7 @@
       </c>
       <c r="E14" s="7"/>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>64</v>
       </c>
@@ -1893,7 +1904,7 @@
       </c>
       <c r="E15" s="7"/>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>65</v>
       </c>
@@ -1908,7 +1919,7 @@
       </c>
       <c r="E16" s="7"/>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>74</v>
       </c>
@@ -1923,7 +1934,7 @@
       </c>
       <c r="E17" s="7"/>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>75</v>
       </c>
@@ -1938,7 +1949,7 @@
       </c>
       <c r="E18" s="7"/>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>79</v>
       </c>
@@ -1953,7 +1964,7 @@
       </c>
       <c r="E19" s="7"/>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>81</v>
       </c>
@@ -1968,7 +1979,7 @@
       </c>
       <c r="E20" s="7"/>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>82</v>
       </c>
@@ -1983,7 +1994,7 @@
       </c>
       <c r="E21" s="7"/>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>88</v>
       </c>
@@ -1998,7 +2009,7 @@
       </c>
       <c r="E22" s="7"/>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>90</v>
       </c>
@@ -2013,7 +2024,7 @@
       </c>
       <c r="E23" s="7"/>
     </row>
-    <row r="24" spans="1:5" ht="30">
+    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>94</v>
       </c>
@@ -2028,7 +2039,7 @@
       </c>
       <c r="E24" s="7"/>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>96</v>
       </c>
@@ -2043,7 +2054,7 @@
       </c>
       <c r="E25" s="7"/>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
         <v>98</v>
       </c>
@@ -2058,7 +2069,7 @@
       </c>
       <c r="E26" s="7"/>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
         <v>102</v>
       </c>
@@ -2073,7 +2084,7 @@
       </c>
       <c r="E27" s="7"/>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
         <v>105</v>
       </c>
@@ -2088,7 +2099,7 @@
       </c>
       <c r="E28" s="7"/>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
         <v>108</v>
       </c>
@@ -2103,7 +2114,7 @@
       </c>
       <c r="E29" s="7"/>
     </row>
-    <row r="30" spans="1:5" ht="30">
+    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
         <v>110</v>
       </c>
@@ -2118,7 +2129,7 @@
       </c>
       <c r="E30" s="7"/>
     </row>
-    <row r="31" spans="1:5" ht="30">
+    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
         <v>114</v>
       </c>
@@ -2133,7 +2144,7 @@
       </c>
       <c r="E31" s="7"/>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
         <v>119</v>
       </c>
@@ -2148,7 +2159,7 @@
       </c>
       <c r="E32" s="7"/>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
         <v>120</v>
       </c>
@@ -2163,7 +2174,7 @@
       </c>
       <c r="E33" s="7"/>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
         <v>125</v>
       </c>
@@ -2178,7 +2189,7 @@
       </c>
       <c r="E34" s="7"/>
     </row>
-    <row r="35" spans="1:5" ht="30">
+    <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
         <v>128</v>
       </c>
@@ -2193,7 +2204,7 @@
       </c>
       <c r="E35" s="7"/>
     </row>
-    <row r="36" spans="1:5" ht="30">
+    <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
         <v>131</v>
       </c>
@@ -2208,7 +2219,7 @@
       </c>
       <c r="E36" s="7"/>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
         <v>134</v>
       </c>
@@ -2223,7 +2234,7 @@
       </c>
       <c r="E37" s="7"/>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="9" t="s">
         <v>137</v>
       </c>
@@ -2238,7 +2249,7 @@
       </c>
       <c r="E38" s="7"/>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="s">
         <v>140</v>
       </c>
@@ -2253,7 +2264,7 @@
       </c>
       <c r="E39" s="7"/>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="9" t="s">
         <v>143</v>
       </c>
@@ -2268,7 +2279,7 @@
       </c>
       <c r="E40" s="7"/>
     </row>
-    <row r="41" spans="1:5" ht="30">
+    <row r="41" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
         <v>145</v>
       </c>
@@ -2283,7 +2294,7 @@
       </c>
       <c r="E41" s="7"/>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="9" t="s">
         <v>147</v>
       </c>
@@ -2298,7 +2309,7 @@
       </c>
       <c r="E42" s="7"/>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="9" t="s">
         <v>150</v>
       </c>
@@ -2313,7 +2324,7 @@
       </c>
       <c r="E43" s="7"/>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="9" t="s">
         <v>153</v>
       </c>
@@ -2328,7 +2339,7 @@
       </c>
       <c r="E44" s="7"/>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="9" t="s">
         <v>155</v>
       </c>
@@ -2343,7 +2354,7 @@
       </c>
       <c r="E45" s="7"/>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="12" t="s">
         <v>158</v>
       </c>
@@ -2358,7 +2369,7 @@
       </c>
       <c r="E46" s="7"/>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="12" t="s">
         <v>159</v>
       </c>
@@ -2373,7 +2384,7 @@
       </c>
       <c r="E47" s="7"/>
     </row>
-    <row r="48" spans="1:5" ht="30">
+    <row r="48" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="12" t="s">
         <v>160</v>
       </c>
@@ -2388,7 +2399,7 @@
       </c>
       <c r="E48" s="7"/>
     </row>
-    <row r="49" spans="1:5" ht="30">
+    <row r="49" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="12" t="s">
         <v>161</v>
       </c>
@@ -2403,7 +2414,7 @@
       </c>
       <c r="E49" s="7"/>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="12" t="s">
         <v>164</v>
       </c>
@@ -2418,7 +2429,7 @@
       </c>
       <c r="E50" s="7"/>
     </row>
-    <row r="51" spans="1:5" ht="30">
+    <row r="51" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="9" t="s">
         <v>173</v>
       </c>
@@ -2433,7 +2444,7 @@
       </c>
       <c r="E51" s="7"/>
     </row>
-    <row r="52" spans="1:5">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="9" t="s">
         <v>174</v>
       </c>
@@ -2448,7 +2459,7 @@
       </c>
       <c r="E52" s="7"/>
     </row>
-    <row r="53" spans="1:5">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="9" t="s">
         <v>179</v>
       </c>
@@ -2463,7 +2474,7 @@
       </c>
       <c r="E53" s="7"/>
     </row>
-    <row r="54" spans="1:5">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="9" t="s">
         <v>180</v>
       </c>
@@ -2478,7 +2489,7 @@
       </c>
       <c r="E54" s="7"/>
     </row>
-    <row r="55" spans="1:5">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="9" t="s">
         <v>185</v>
       </c>
@@ -2493,7 +2504,7 @@
       </c>
       <c r="E55" s="7"/>
     </row>
-    <row r="56" spans="1:5">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="s">
         <v>188</v>
       </c>
@@ -2508,7 +2519,7 @@
       </c>
       <c r="E56" s="7"/>
     </row>
-    <row r="57" spans="1:5" ht="30">
+    <row r="57" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="9" t="s">
         <v>191</v>
       </c>
@@ -2523,7 +2534,7 @@
       </c>
       <c r="E57" s="7"/>
     </row>
-    <row r="58" spans="1:5">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="9" t="s">
         <v>194</v>
       </c>
@@ -2538,7 +2549,7 @@
       </c>
       <c r="E58" s="7"/>
     </row>
-    <row r="59" spans="1:5">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
         <v>196</v>
       </c>
@@ -2553,7 +2564,7 @@
       </c>
       <c r="E59" s="7"/>
     </row>
-    <row r="60" spans="1:5" ht="45">
+    <row r="60" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
         <v>199</v>
       </c>
@@ -2568,7 +2579,7 @@
       </c>
       <c r="E60" s="7"/>
     </row>
-    <row r="61" spans="1:5">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="9" t="s">
         <v>202</v>
       </c>
@@ -2583,7 +2594,7 @@
       </c>
       <c r="E61" s="7"/>
     </row>
-    <row r="62" spans="1:5">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="9" t="s">
         <v>204</v>
       </c>
@@ -2598,7 +2609,7 @@
       </c>
       <c r="E62" s="7"/>
     </row>
-    <row r="63" spans="1:5">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="9" t="s">
         <v>206</v>
       </c>
@@ -2613,7 +2624,7 @@
       </c>
       <c r="E63" s="7"/>
     </row>
-    <row r="64" spans="1:5">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="9" t="s">
         <v>208</v>
       </c>
@@ -2628,7 +2639,7 @@
       </c>
       <c r="E64" s="7"/>
     </row>
-    <row r="65" spans="1:5">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="9" t="s">
         <v>217</v>
       </c>
@@ -2643,7 +2654,7 @@
       </c>
       <c r="E65" s="7"/>
     </row>
-    <row r="66" spans="1:5">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="9" t="s">
         <v>218</v>
       </c>
@@ -2658,7 +2669,7 @@
       </c>
       <c r="E66" s="7"/>
     </row>
-    <row r="67" spans="1:5">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="9" t="s">
         <v>223</v>
       </c>
@@ -2673,7 +2684,7 @@
       </c>
       <c r="E67" s="7"/>
     </row>
-    <row r="68" spans="1:5">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="9" t="s">
         <v>224</v>
       </c>
@@ -2688,7 +2699,7 @@
       </c>
       <c r="E68" s="7"/>
     </row>
-    <row r="69" spans="1:5">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="9" t="s">
         <v>225</v>
       </c>
@@ -2703,7 +2714,7 @@
       </c>
       <c r="E69" s="7"/>
     </row>
-    <row r="70" spans="1:5">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="9" t="s">
         <v>226</v>
       </c>
@@ -2718,7 +2729,7 @@
       </c>
       <c r="E70" s="7"/>
     </row>
-    <row r="71" spans="1:5">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="9" t="s">
         <v>233</v>
       </c>
@@ -2733,7 +2744,7 @@
       </c>
       <c r="E71" s="7"/>
     </row>
-    <row r="72" spans="1:5">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="9" t="s">
         <v>237</v>
       </c>
@@ -2748,7 +2759,7 @@
       </c>
       <c r="E72" s="7"/>
     </row>
-    <row r="73" spans="1:5">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="9" t="s">
         <v>239</v>
       </c>
@@ -2763,7 +2774,7 @@
       </c>
       <c r="E73" s="7"/>
     </row>
-    <row r="74" spans="1:5">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="9" t="s">
         <v>243</v>
       </c>
@@ -2778,7 +2789,7 @@
       </c>
       <c r="E74" s="7"/>
     </row>
-    <row r="75" spans="1:5" ht="30">
+    <row r="75" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" s="9" t="s">
         <v>245</v>
       </c>
@@ -2793,7 +2804,7 @@
       </c>
       <c r="E75" s="7"/>
     </row>
-    <row r="76" spans="1:5">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="9" t="s">
         <v>248</v>
       </c>
@@ -2808,7 +2819,7 @@
       </c>
       <c r="E76" s="7"/>
     </row>
-    <row r="77" spans="1:5">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="9" t="s">
         <v>256</v>
       </c>
@@ -2823,7 +2834,7 @@
       </c>
       <c r="E77" s="7"/>
     </row>
-    <row r="78" spans="1:5">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="9" t="s">
         <v>257</v>
       </c>
@@ -2838,7 +2849,7 @@
       </c>
       <c r="E78" s="7"/>
     </row>
-    <row r="79" spans="1:5">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="9" t="s">
         <v>261</v>
       </c>
@@ -2853,7 +2864,7 @@
       </c>
       <c r="E79" s="7"/>
     </row>
-    <row r="80" spans="1:5">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="9" t="s">
         <v>264</v>
       </c>
@@ -2868,7 +2879,7 @@
       </c>
       <c r="E80" s="7"/>
     </row>
-    <row r="81" spans="1:5">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="9" t="s">
         <v>267</v>
       </c>
@@ -2883,7 +2894,7 @@
       </c>
       <c r="E81" s="7"/>
     </row>
-    <row r="82" spans="1:5" ht="30">
+    <row r="82" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A82" s="9" t="s">
         <v>269</v>
       </c>
@@ -2898,7 +2909,7 @@
       </c>
       <c r="E82" s="7"/>
     </row>
-    <row r="83" spans="1:5">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="9" t="s">
         <v>274</v>
       </c>
@@ -2913,7 +2924,7 @@
       </c>
       <c r="E83" s="7"/>
     </row>
-    <row r="84" spans="1:5" ht="30">
+    <row r="84" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A84" s="9" t="s">
         <v>277</v>
       </c>
@@ -2928,7 +2939,7 @@
       </c>
       <c r="E84" s="7"/>
     </row>
-    <row r="85" spans="1:5">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="9" t="s">
         <v>279</v>
       </c>
@@ -2943,7 +2954,7 @@
       </c>
       <c r="E85" s="7"/>
     </row>
-    <row r="86" spans="1:5">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="9" t="s">
         <v>282</v>
       </c>
@@ -2958,7 +2969,7 @@
       </c>
       <c r="E86" s="7"/>
     </row>
-    <row r="87" spans="1:5">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="9" t="s">
         <v>285</v>
       </c>
@@ -2973,7 +2984,7 @@
       </c>
       <c r="E87" s="7"/>
     </row>
-    <row r="88" spans="1:5">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="9" t="s">
         <v>288</v>
       </c>
@@ -2988,7 +2999,7 @@
       </c>
       <c r="E88" s="7"/>
     </row>
-    <row r="89" spans="1:5">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="9" t="s">
         <v>291</v>
       </c>
@@ -3003,7 +3014,7 @@
       </c>
       <c r="E89" s="7"/>
     </row>
-    <row r="90" spans="1:5">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="9" t="s">
         <v>294</v>
       </c>
@@ -3018,7 +3029,7 @@
       </c>
       <c r="E90" s="7"/>
     </row>
-    <row r="91" spans="1:5">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="9" t="s">
         <v>297</v>
       </c>
@@ -3033,7 +3044,7 @@
       </c>
       <c r="E91" s="7"/>
     </row>
-    <row r="92" spans="1:5">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="9" t="s">
         <v>300</v>
       </c>
@@ -3048,7 +3059,7 @@
       </c>
       <c r="E92" s="7"/>
     </row>
-    <row r="93" spans="1:5">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="9" t="s">
         <v>303</v>
       </c>
@@ -3063,7 +3074,7 @@
       </c>
       <c r="E93" s="7"/>
     </row>
-    <row r="94" spans="1:5">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="9" t="s">
         <v>306</v>
       </c>
@@ -3078,7 +3089,7 @@
       </c>
       <c r="E94" s="7"/>
     </row>
-    <row r="95" spans="1:5">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="9" t="s">
         <v>309</v>
       </c>
@@ -3093,7 +3104,7 @@
       </c>
       <c r="E95" s="7"/>
     </row>
-    <row r="96" spans="1:5">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="9" t="s">
         <v>314</v>
       </c>
@@ -3108,7 +3119,7 @@
       </c>
       <c r="E96" s="7"/>
     </row>
-    <row r="97" spans="1:5">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="9" t="s">
         <v>315</v>
       </c>
@@ -3123,7 +3134,7 @@
       </c>
       <c r="E97" s="7"/>
     </row>
-    <row r="98" spans="1:5">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="9" t="s">
         <v>319</v>
       </c>
@@ -3138,7 +3149,7 @@
       </c>
       <c r="E98" s="7"/>
     </row>
-    <row r="99" spans="1:5">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="9" t="s">
         <v>321</v>
       </c>
@@ -3153,7 +3164,7 @@
       </c>
       <c r="E99" s="7"/>
     </row>
-    <row r="100" spans="1:5">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="9" t="s">
         <v>322</v>
       </c>
@@ -3168,7 +3179,7 @@
       </c>
       <c r="E100" s="7"/>
     </row>
-    <row r="101" spans="1:5" ht="30">
+    <row r="101" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A101" s="9" t="s">
         <v>323</v>
       </c>
@@ -3183,7 +3194,7 @@
       </c>
       <c r="E101" s="7"/>
     </row>
-    <row r="102" spans="1:5">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="9" t="s">
         <v>328</v>
       </c>
@@ -3198,7 +3209,7 @@
       </c>
       <c r="E102" s="7"/>
     </row>
-    <row r="103" spans="1:5">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="9" t="s">
         <v>333</v>
       </c>
@@ -3213,7 +3224,7 @@
       </c>
       <c r="E103" s="7"/>
     </row>
-    <row r="104" spans="1:5">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="9" t="s">
         <v>336</v>
       </c>
@@ -3228,7 +3239,7 @@
       </c>
       <c r="E104" s="7"/>
     </row>
-    <row r="105" spans="1:5">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="9" t="s">
         <v>337</v>
       </c>
@@ -3243,7 +3254,7 @@
       </c>
       <c r="E105" s="7"/>
     </row>
-    <row r="106" spans="1:5">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="9" t="s">
         <v>342</v>
       </c>
@@ -3258,7 +3269,7 @@
       </c>
       <c r="E106" s="7"/>
     </row>
-    <row r="107" spans="1:5">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="9" t="s">
         <v>345</v>
       </c>
@@ -3273,7 +3284,7 @@
       </c>
       <c r="E107" s="7"/>
     </row>
-    <row r="108" spans="1:5">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="9" t="s">
         <v>350</v>
       </c>
@@ -3288,7 +3299,7 @@
       </c>
       <c r="E108" s="7"/>
     </row>
-    <row r="109" spans="1:5" ht="30">
+    <row r="109" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A109" s="9" t="s">
         <v>351</v>
       </c>
@@ -3303,7 +3314,7 @@
       </c>
       <c r="E109" s="7"/>
     </row>
-    <row r="110" spans="1:5">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="9" t="s">
         <v>354</v>
       </c>
@@ -3318,7 +3329,7 @@
       </c>
       <c r="E110" s="7"/>
     </row>
-    <row r="111" spans="1:5">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="9" t="s">
         <v>357</v>
       </c>
@@ -3333,7 +3344,7 @@
       </c>
       <c r="E111" s="7"/>
     </row>
-    <row r="112" spans="1:5">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="9" t="s">
         <v>361</v>
       </c>
@@ -3348,7 +3359,7 @@
       </c>
       <c r="E112" s="7"/>
     </row>
-    <row r="113" spans="1:5">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="17" t="s">
         <v>363</v>
       </c>
@@ -3363,7 +3374,7 @@
       </c>
       <c r="E113" s="19"/>
     </row>
-    <row r="114" spans="1:5" ht="30">
+    <row r="114" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A114" s="9" t="s">
         <v>366</v>
       </c>
@@ -3378,7 +3389,7 @@
       </c>
       <c r="E114" s="7"/>
     </row>
-    <row r="115" spans="1:5">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="9" t="s">
         <v>369</v>
       </c>
@@ -3393,7 +3404,7 @@
       </c>
       <c r="E115" s="7"/>
     </row>
-    <row r="116" spans="1:5">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="9" t="s">
         <v>370</v>
       </c>
@@ -3408,7 +3419,7 @@
       </c>
       <c r="E116" s="7"/>
     </row>
-    <row r="117" spans="1:5">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" s="9" t="s">
         <v>371</v>
       </c>
@@ -3422,6 +3433,21 @@
         <v>5</v>
       </c>
       <c r="E117" s="7"/>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A118" s="9" t="s">
+        <v>378</v>
+      </c>
+      <c r="B118" s="7" t="s">
+        <v>379</v>
+      </c>
+      <c r="C118" s="7" t="s">
+        <v>380</v>
+      </c>
+      <c r="D118" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E118" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -3434,14 +3460,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView topLeftCell="A10" zoomScale="80" workbookViewId="0">
       <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
@@ -3449,7 +3475,7 @@
     <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>35</v>
       </c>
@@ -3463,7 +3489,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>37</v>
       </c>
@@ -3475,7 +3501,7 @@
       </c>
       <c r="D2" s="7"/>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>38</v>
       </c>
@@ -3487,7 +3513,7 @@
       </c>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>39</v>
       </c>
@@ -3499,7 +3525,7 @@
       </c>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>40</v>
       </c>
@@ -3511,7 +3537,7 @@
       </c>
       <c r="D5" s="7"/>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>41</v>
       </c>
@@ -3523,7 +3549,7 @@
       </c>
       <c r="D6" s="7"/>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>42</v>
       </c>
@@ -3535,7 +3561,7 @@
       </c>
       <c r="D7" s="7"/>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>43</v>
       </c>
@@ -3547,7 +3573,7 @@
       </c>
       <c r="D8" s="7"/>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>44</v>
       </c>
@@ -3559,7 +3585,7 @@
       </c>
       <c r="D9" s="7"/>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>45</v>
       </c>
@@ -3571,7 +3597,7 @@
       </c>
       <c r="D10" s="7"/>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>46</v>
       </c>
@@ -3583,7 +3609,7 @@
       </c>
       <c r="D11" s="7"/>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>48</v>
       </c>
@@ -3595,7 +3621,7 @@
       </c>
       <c r="D12" s="7"/>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>49</v>
       </c>
@@ -3607,7 +3633,7 @@
       </c>
       <c r="D13" s="7"/>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>50</v>
       </c>
@@ -3619,7 +3645,7 @@
       </c>
       <c r="D14" s="7"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>51</v>
       </c>
@@ -3631,7 +3657,7 @@
       </c>
       <c r="D15" s="7"/>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>52</v>
       </c>
@@ -3643,7 +3669,7 @@
       </c>
       <c r="D16" s="7"/>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>53</v>
       </c>
@@ -3655,7 +3681,7 @@
       </c>
       <c r="D17" s="7"/>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>54</v>
       </c>
@@ -3667,7 +3693,7 @@
       </c>
       <c r="D18" s="7"/>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>55</v>
       </c>
@@ -3679,7 +3705,7 @@
       </c>
       <c r="D19" s="7"/>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>56</v>
       </c>
@@ -3691,7 +3717,7 @@
       </c>
       <c r="D20" s="7"/>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>57</v>
       </c>
@@ -3703,7 +3729,7 @@
       </c>
       <c r="D21" s="7"/>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>58</v>
       </c>
@@ -3715,7 +3741,7 @@
       </c>
       <c r="D22" s="7"/>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>59</v>
       </c>
@@ -3727,7 +3753,7 @@
       </c>
       <c r="D23" s="7"/>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>60</v>
       </c>
@@ -3739,7 +3765,7 @@
       </c>
       <c r="D24" s="7"/>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>61</v>
       </c>
@@ -3751,7 +3777,7 @@
       </c>
       <c r="D25" s="7"/>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>47</v>
       </c>
@@ -3770,14 +3796,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A19" sqref="A19:XFD19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
@@ -3785,7 +3811,7 @@
     <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>35</v>
       </c>
@@ -3799,7 +3825,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>37</v>
       </c>
@@ -3811,7 +3837,7 @@
       </c>
       <c r="D2" s="7"/>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>38</v>
       </c>
@@ -3823,7 +3849,7 @@
       </c>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>39</v>
       </c>
@@ -3835,7 +3861,7 @@
       </c>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>40</v>
       </c>
@@ -3847,7 +3873,7 @@
       </c>
       <c r="D5" s="7"/>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>41</v>
       </c>
@@ -3859,7 +3885,7 @@
       </c>
       <c r="D6" s="7"/>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>42</v>
       </c>
@@ -3871,7 +3897,7 @@
       </c>
       <c r="D7" s="7"/>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>43</v>
       </c>
@@ -3883,7 +3909,7 @@
       </c>
       <c r="D8" s="7"/>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>44</v>
       </c>
@@ -3895,7 +3921,7 @@
       </c>
       <c r="D9" s="7"/>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>45</v>
       </c>
@@ -3907,7 +3933,7 @@
       </c>
       <c r="D10" s="7"/>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>46</v>
       </c>
@@ -3919,7 +3945,7 @@
       </c>
       <c r="D11" s="7"/>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>47</v>
       </c>
@@ -3931,7 +3957,7 @@
       </c>
       <c r="D12" s="7"/>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>48</v>
       </c>
@@ -3943,7 +3969,7 @@
       </c>
       <c r="D13" s="7"/>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>49</v>
       </c>
@@ -3955,7 +3981,7 @@
       </c>
       <c r="D14" s="7"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>50</v>
       </c>
@@ -3967,7 +3993,7 @@
       </c>
       <c r="D15" s="7"/>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>51</v>
       </c>
@@ -3979,7 +4005,7 @@
       </c>
       <c r="D16" s="7"/>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>52</v>
       </c>
@@ -3991,7 +4017,7 @@
       </c>
       <c r="D17" s="7"/>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>53</v>
       </c>
@@ -4003,7 +4029,7 @@
       </c>
       <c r="D18" s="7"/>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>54</v>
       </c>
@@ -4015,7 +4041,7 @@
       </c>
       <c r="D19" s="7"/>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>55</v>
       </c>
@@ -4027,7 +4053,7 @@
       </c>
       <c r="D20" s="7"/>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>56</v>
       </c>
@@ -4039,7 +4065,7 @@
       </c>
       <c r="D21" s="7"/>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>57</v>
       </c>
@@ -4051,7 +4077,7 @@
       </c>
       <c r="D22" s="7"/>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>58</v>
       </c>
@@ -4063,7 +4089,7 @@
       </c>
       <c r="D23" s="7"/>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>59</v>
       </c>
@@ -4075,7 +4101,7 @@
       </c>
       <c r="D24" s="7"/>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>60</v>
       </c>
@@ -4087,7 +4113,7 @@
       </c>
       <c r="D25" s="7"/>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>61</v>
       </c>

</xml_diff>

<commit_message>
WAT RID Search Scripts
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/WAT.xlsx
+++ b/src/test/resources/xls/WAT.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13305" windowHeight="2415"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="387">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="647" uniqueCount="393">
   <si>
     <t>TCID</t>
   </si>
@@ -1178,13 +1178,31 @@
   </si>
   <si>
     <t>Verify that Find button is still enabled after user clicks on a country name from country dropdown</t>
+  </si>
+  <si>
+    <t>WAT154</t>
+  </si>
+  <si>
+    <t>WAT-1157||WAT-1158</t>
+  </si>
+  <si>
+    <t>Verify that user should be able to perform author search using RID||Verify that the System should provide as results any and all author clusters where the specified RID(s) appear on 1 or more authorships</t>
+  </si>
+  <si>
+    <t>WAT155</t>
+  </si>
+  <si>
+    <t>WAT-1159</t>
+  </si>
+  <si>
+    <t>Verify that Error messages should display for invalid pattern RID search/ RID but DNE/ RID older than 2007</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1436,7 +1454,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1468,10 +1486,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1503,7 +1520,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1679,14 +1695,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E120"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E122"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A98" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C128" sqref="C128"/>
+      <selection activeCell="G119" sqref="G119"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="41" bestFit="1" customWidth="1" collapsed="1"/>
@@ -1695,7 +1711,7 @@
     <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1712,7 +1728,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -1727,7 +1743,7 @@
       </c>
       <c r="E2" s="4"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -1742,7 +1758,7 @@
       </c>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" s="7" t="s">
         <v>11</v>
       </c>
@@ -1757,7 +1773,7 @@
       </c>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" s="7" t="s">
         <v>12</v>
       </c>
@@ -1772,7 +1788,7 @@
       </c>
       <c r="E5" s="7"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" s="7" t="s">
         <v>14</v>
       </c>
@@ -1787,7 +1803,7 @@
       </c>
       <c r="E6" s="7"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" s="7" t="s">
         <v>17</v>
       </c>
@@ -1802,7 +1818,7 @@
       </c>
       <c r="E7" s="7"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" s="7" t="s">
         <v>20</v>
       </c>
@@ -1817,7 +1833,7 @@
       </c>
       <c r="E8" s="7"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" s="7" t="s">
         <v>22</v>
       </c>
@@ -1832,7 +1848,7 @@
       </c>
       <c r="E9" s="7"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10" s="7" t="s">
         <v>23</v>
       </c>
@@ -1847,7 +1863,7 @@
       </c>
       <c r="E10" s="7"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11" s="7" t="s">
         <v>24</v>
       </c>
@@ -1862,7 +1878,7 @@
       </c>
       <c r="E11" s="7"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12" s="7" t="s">
         <v>25</v>
       </c>
@@ -1877,7 +1893,7 @@
       </c>
       <c r="E12" s="7"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13" s="7" t="s">
         <v>62</v>
       </c>
@@ -1892,7 +1908,7 @@
       </c>
       <c r="E13" s="7"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="A14" s="7" t="s">
         <v>63</v>
       </c>
@@ -1907,7 +1923,7 @@
       </c>
       <c r="E14" s="7"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="A15" s="7" t="s">
         <v>64</v>
       </c>
@@ -1922,7 +1938,7 @@
       </c>
       <c r="E15" s="7"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="A16" s="7" t="s">
         <v>65</v>
       </c>
@@ -1937,7 +1953,7 @@
       </c>
       <c r="E16" s="7"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5">
       <c r="A17" s="7" t="s">
         <v>74</v>
       </c>
@@ -1952,7 +1968,7 @@
       </c>
       <c r="E17" s="7"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5">
       <c r="A18" s="7" t="s">
         <v>75</v>
       </c>
@@ -1967,7 +1983,7 @@
       </c>
       <c r="E18" s="7"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5">
       <c r="A19" s="7" t="s">
         <v>79</v>
       </c>
@@ -1982,7 +1998,7 @@
       </c>
       <c r="E19" s="7"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5">
       <c r="A20" s="7" t="s">
         <v>81</v>
       </c>
@@ -1997,7 +2013,7 @@
       </c>
       <c r="E20" s="7"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5">
       <c r="A21" s="7" t="s">
         <v>82</v>
       </c>
@@ -2012,7 +2028,7 @@
       </c>
       <c r="E21" s="7"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5">
       <c r="A22" s="7" t="s">
         <v>88</v>
       </c>
@@ -2027,7 +2043,7 @@
       </c>
       <c r="E22" s="7"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5">
       <c r="A23" s="7" t="s">
         <v>90</v>
       </c>
@@ -2042,7 +2058,7 @@
       </c>
       <c r="E23" s="7"/>
     </row>
-    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="30">
       <c r="A24" s="9" t="s">
         <v>94</v>
       </c>
@@ -2057,7 +2073,7 @@
       </c>
       <c r="E24" s="7"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5">
       <c r="A25" s="9" t="s">
         <v>96</v>
       </c>
@@ -2072,7 +2088,7 @@
       </c>
       <c r="E25" s="7"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5">
       <c r="A26" s="9" t="s">
         <v>98</v>
       </c>
@@ -2087,7 +2103,7 @@
       </c>
       <c r="E26" s="7"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5">
       <c r="A27" s="9" t="s">
         <v>102</v>
       </c>
@@ -2102,7 +2118,7 @@
       </c>
       <c r="E27" s="7"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5">
       <c r="A28" s="9" t="s">
         <v>105</v>
       </c>
@@ -2117,7 +2133,7 @@
       </c>
       <c r="E28" s="7"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5">
       <c r="A29" s="9" t="s">
         <v>108</v>
       </c>
@@ -2132,7 +2148,7 @@
       </c>
       <c r="E29" s="7"/>
     </row>
-    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" ht="30">
       <c r="A30" s="9" t="s">
         <v>110</v>
       </c>
@@ -2147,7 +2163,7 @@
       </c>
       <c r="E30" s="7"/>
     </row>
-    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" ht="30">
       <c r="A31" s="9" t="s">
         <v>114</v>
       </c>
@@ -2162,7 +2178,7 @@
       </c>
       <c r="E31" s="7"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5">
       <c r="A32" s="9" t="s">
         <v>119</v>
       </c>
@@ -2177,7 +2193,7 @@
       </c>
       <c r="E32" s="7"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5">
       <c r="A33" s="9" t="s">
         <v>120</v>
       </c>
@@ -2192,7 +2208,7 @@
       </c>
       <c r="E33" s="7"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5">
       <c r="A34" s="9" t="s">
         <v>125</v>
       </c>
@@ -2207,7 +2223,7 @@
       </c>
       <c r="E34" s="7"/>
     </row>
-    <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" ht="30">
       <c r="A35" s="9" t="s">
         <v>128</v>
       </c>
@@ -2222,7 +2238,7 @@
       </c>
       <c r="E35" s="7"/>
     </row>
-    <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" ht="30">
       <c r="A36" s="9" t="s">
         <v>131</v>
       </c>
@@ -2237,7 +2253,7 @@
       </c>
       <c r="E36" s="7"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5">
       <c r="A37" s="9" t="s">
         <v>134</v>
       </c>
@@ -2252,7 +2268,7 @@
       </c>
       <c r="E37" s="7"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5">
       <c r="A38" s="9" t="s">
         <v>137</v>
       </c>
@@ -2267,7 +2283,7 @@
       </c>
       <c r="E38" s="7"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5">
       <c r="A39" s="9" t="s">
         <v>140</v>
       </c>
@@ -2282,7 +2298,7 @@
       </c>
       <c r="E39" s="7"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5">
       <c r="A40" s="9" t="s">
         <v>143</v>
       </c>
@@ -2297,7 +2313,7 @@
       </c>
       <c r="E40" s="7"/>
     </row>
-    <row r="41" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" ht="30">
       <c r="A41" s="9" t="s">
         <v>145</v>
       </c>
@@ -2312,7 +2328,7 @@
       </c>
       <c r="E41" s="7"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5">
       <c r="A42" s="9" t="s">
         <v>147</v>
       </c>
@@ -2327,7 +2343,7 @@
       </c>
       <c r="E42" s="7"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5">
       <c r="A43" s="9" t="s">
         <v>150</v>
       </c>
@@ -2342,7 +2358,7 @@
       </c>
       <c r="E43" s="7"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5">
       <c r="A44" s="9" t="s">
         <v>153</v>
       </c>
@@ -2357,7 +2373,7 @@
       </c>
       <c r="E44" s="7"/>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5">
       <c r="A45" s="9" t="s">
         <v>155</v>
       </c>
@@ -2372,7 +2388,7 @@
       </c>
       <c r="E45" s="7"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5">
       <c r="A46" s="12" t="s">
         <v>158</v>
       </c>
@@ -2387,7 +2403,7 @@
       </c>
       <c r="E46" s="7"/>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5">
       <c r="A47" s="12" t="s">
         <v>159</v>
       </c>
@@ -2402,7 +2418,7 @@
       </c>
       <c r="E47" s="7"/>
     </row>
-    <row r="48" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" ht="30">
       <c r="A48" s="12" t="s">
         <v>160</v>
       </c>
@@ -2417,7 +2433,7 @@
       </c>
       <c r="E48" s="7"/>
     </row>
-    <row r="49" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" ht="30">
       <c r="A49" s="12" t="s">
         <v>161</v>
       </c>
@@ -2432,7 +2448,7 @@
       </c>
       <c r="E49" s="7"/>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5">
       <c r="A50" s="12" t="s">
         <v>164</v>
       </c>
@@ -2447,7 +2463,7 @@
       </c>
       <c r="E50" s="7"/>
     </row>
-    <row r="51" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" ht="30">
       <c r="A51" s="9" t="s">
         <v>173</v>
       </c>
@@ -2462,7 +2478,7 @@
       </c>
       <c r="E51" s="7"/>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5">
       <c r="A52" s="9" t="s">
         <v>174</v>
       </c>
@@ -2477,7 +2493,7 @@
       </c>
       <c r="E52" s="7"/>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5">
       <c r="A53" s="9" t="s">
         <v>179</v>
       </c>
@@ -2492,7 +2508,7 @@
       </c>
       <c r="E53" s="7"/>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5">
       <c r="A54" s="9" t="s">
         <v>180</v>
       </c>
@@ -2507,7 +2523,7 @@
       </c>
       <c r="E54" s="7"/>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5">
       <c r="A55" s="9" t="s">
         <v>185</v>
       </c>
@@ -2522,7 +2538,7 @@
       </c>
       <c r="E55" s="7"/>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5">
       <c r="A56" s="9" t="s">
         <v>188</v>
       </c>
@@ -2537,7 +2553,7 @@
       </c>
       <c r="E56" s="7"/>
     </row>
-    <row r="57" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" ht="30">
       <c r="A57" s="9" t="s">
         <v>191</v>
       </c>
@@ -2552,7 +2568,7 @@
       </c>
       <c r="E57" s="7"/>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5">
       <c r="A58" s="9" t="s">
         <v>194</v>
       </c>
@@ -2567,7 +2583,7 @@
       </c>
       <c r="E58" s="7"/>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5">
       <c r="A59" s="7" t="s">
         <v>196</v>
       </c>
@@ -2582,7 +2598,7 @@
       </c>
       <c r="E59" s="7"/>
     </row>
-    <row r="60" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" ht="45">
       <c r="A60" s="7" t="s">
         <v>199</v>
       </c>
@@ -2597,7 +2613,7 @@
       </c>
       <c r="E60" s="7"/>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5">
       <c r="A61" s="9" t="s">
         <v>202</v>
       </c>
@@ -2612,7 +2628,7 @@
       </c>
       <c r="E61" s="7"/>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5">
       <c r="A62" s="9" t="s">
         <v>204</v>
       </c>
@@ -2627,7 +2643,7 @@
       </c>
       <c r="E62" s="7"/>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5">
       <c r="A63" s="9" t="s">
         <v>206</v>
       </c>
@@ -2642,7 +2658,7 @@
       </c>
       <c r="E63" s="7"/>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5">
       <c r="A64" s="9" t="s">
         <v>208</v>
       </c>
@@ -2657,7 +2673,7 @@
       </c>
       <c r="E64" s="7"/>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5">
       <c r="A65" s="9" t="s">
         <v>217</v>
       </c>
@@ -2672,7 +2688,7 @@
       </c>
       <c r="E65" s="7"/>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5">
       <c r="A66" s="9" t="s">
         <v>218</v>
       </c>
@@ -2687,7 +2703,7 @@
       </c>
       <c r="E66" s="7"/>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5">
       <c r="A67" s="9" t="s">
         <v>223</v>
       </c>
@@ -2702,7 +2718,7 @@
       </c>
       <c r="E67" s="7"/>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5">
       <c r="A68" s="9" t="s">
         <v>224</v>
       </c>
@@ -2717,7 +2733,7 @@
       </c>
       <c r="E68" s="7"/>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5">
       <c r="A69" s="9" t="s">
         <v>225</v>
       </c>
@@ -2732,7 +2748,7 @@
       </c>
       <c r="E69" s="7"/>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5">
       <c r="A70" s="9" t="s">
         <v>226</v>
       </c>
@@ -2747,7 +2763,7 @@
       </c>
       <c r="E70" s="7"/>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5">
       <c r="A71" s="9" t="s">
         <v>233</v>
       </c>
@@ -2762,7 +2778,7 @@
       </c>
       <c r="E71" s="7"/>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5">
       <c r="A72" s="9" t="s">
         <v>237</v>
       </c>
@@ -2777,7 +2793,7 @@
       </c>
       <c r="E72" s="7"/>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5">
       <c r="A73" s="9" t="s">
         <v>239</v>
       </c>
@@ -2792,7 +2808,7 @@
       </c>
       <c r="E73" s="7"/>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5">
       <c r="A74" s="9" t="s">
         <v>243</v>
       </c>
@@ -2807,7 +2823,7 @@
       </c>
       <c r="E74" s="7"/>
     </row>
-    <row r="75" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" ht="30">
       <c r="A75" s="9" t="s">
         <v>245</v>
       </c>
@@ -2822,7 +2838,7 @@
       </c>
       <c r="E75" s="7"/>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5">
       <c r="A76" s="9" t="s">
         <v>248</v>
       </c>
@@ -2837,7 +2853,7 @@
       </c>
       <c r="E76" s="7"/>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5">
       <c r="A77" s="9" t="s">
         <v>256</v>
       </c>
@@ -2852,7 +2868,7 @@
       </c>
       <c r="E77" s="7"/>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5">
       <c r="A78" s="9" t="s">
         <v>257</v>
       </c>
@@ -2867,7 +2883,7 @@
       </c>
       <c r="E78" s="7"/>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5">
       <c r="A79" s="9" t="s">
         <v>261</v>
       </c>
@@ -2882,7 +2898,7 @@
       </c>
       <c r="E79" s="7"/>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5">
       <c r="A80" s="9" t="s">
         <v>264</v>
       </c>
@@ -2897,7 +2913,7 @@
       </c>
       <c r="E80" s="7"/>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5">
       <c r="A81" s="9" t="s">
         <v>267</v>
       </c>
@@ -2912,7 +2928,7 @@
       </c>
       <c r="E81" s="7"/>
     </row>
-    <row r="82" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" ht="30">
       <c r="A82" s="9" t="s">
         <v>269</v>
       </c>
@@ -2927,7 +2943,7 @@
       </c>
       <c r="E82" s="7"/>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5">
       <c r="A83" s="9" t="s">
         <v>274</v>
       </c>
@@ -2942,7 +2958,7 @@
       </c>
       <c r="E83" s="7"/>
     </row>
-    <row r="84" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" ht="30">
       <c r="A84" s="9" t="s">
         <v>277</v>
       </c>
@@ -2957,7 +2973,7 @@
       </c>
       <c r="E84" s="7"/>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5">
       <c r="A85" s="9" t="s">
         <v>279</v>
       </c>
@@ -2972,7 +2988,7 @@
       </c>
       <c r="E85" s="7"/>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5">
       <c r="A86" s="9" t="s">
         <v>282</v>
       </c>
@@ -2987,7 +3003,7 @@
       </c>
       <c r="E86" s="7"/>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5">
       <c r="A87" s="9" t="s">
         <v>285</v>
       </c>
@@ -3002,7 +3018,7 @@
       </c>
       <c r="E87" s="7"/>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5">
       <c r="A88" s="9" t="s">
         <v>288</v>
       </c>
@@ -3017,7 +3033,7 @@
       </c>
       <c r="E88" s="7"/>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5">
       <c r="A89" s="9" t="s">
         <v>291</v>
       </c>
@@ -3032,7 +3048,7 @@
       </c>
       <c r="E89" s="7"/>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5">
       <c r="A90" s="9" t="s">
         <v>294</v>
       </c>
@@ -3047,7 +3063,7 @@
       </c>
       <c r="E90" s="7"/>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5">
       <c r="A91" s="9" t="s">
         <v>297</v>
       </c>
@@ -3062,7 +3078,7 @@
       </c>
       <c r="E91" s="7"/>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5">
       <c r="A92" s="9" t="s">
         <v>300</v>
       </c>
@@ -3077,7 +3093,7 @@
       </c>
       <c r="E92" s="7"/>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5">
       <c r="A93" s="9" t="s">
         <v>303</v>
       </c>
@@ -3092,7 +3108,7 @@
       </c>
       <c r="E93" s="7"/>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5">
       <c r="A94" s="9" t="s">
         <v>306</v>
       </c>
@@ -3107,7 +3123,7 @@
       </c>
       <c r="E94" s="7"/>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5">
       <c r="A95" s="9" t="s">
         <v>309</v>
       </c>
@@ -3122,7 +3138,7 @@
       </c>
       <c r="E95" s="7"/>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5">
       <c r="A96" s="9" t="s">
         <v>314</v>
       </c>
@@ -3137,7 +3153,7 @@
       </c>
       <c r="E96" s="7"/>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5">
       <c r="A97" s="9" t="s">
         <v>315</v>
       </c>
@@ -3152,7 +3168,7 @@
       </c>
       <c r="E97" s="7"/>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5">
       <c r="A98" s="9" t="s">
         <v>319</v>
       </c>
@@ -3167,7 +3183,7 @@
       </c>
       <c r="E98" s="7"/>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5">
       <c r="A99" s="9" t="s">
         <v>321</v>
       </c>
@@ -3182,7 +3198,7 @@
       </c>
       <c r="E99" s="7"/>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5">
       <c r="A100" s="9" t="s">
         <v>322</v>
       </c>
@@ -3197,7 +3213,7 @@
       </c>
       <c r="E100" s="7"/>
     </row>
-    <row r="101" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" ht="30">
       <c r="A101" s="9" t="s">
         <v>323</v>
       </c>
@@ -3212,7 +3228,7 @@
       </c>
       <c r="E101" s="7"/>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5">
       <c r="A102" s="9" t="s">
         <v>328</v>
       </c>
@@ -3227,7 +3243,7 @@
       </c>
       <c r="E102" s="7"/>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5">
       <c r="A103" s="9" t="s">
         <v>333</v>
       </c>
@@ -3242,7 +3258,7 @@
       </c>
       <c r="E103" s="7"/>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5">
       <c r="A104" s="9" t="s">
         <v>336</v>
       </c>
@@ -3257,7 +3273,7 @@
       </c>
       <c r="E104" s="7"/>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5">
       <c r="A105" s="9" t="s">
         <v>337</v>
       </c>
@@ -3272,7 +3288,7 @@
       </c>
       <c r="E105" s="7"/>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5">
       <c r="A106" s="9" t="s">
         <v>342</v>
       </c>
@@ -3287,7 +3303,7 @@
       </c>
       <c r="E106" s="7"/>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5">
       <c r="A107" s="9" t="s">
         <v>345</v>
       </c>
@@ -3302,7 +3318,7 @@
       </c>
       <c r="E107" s="7"/>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5">
       <c r="A108" s="9" t="s">
         <v>350</v>
       </c>
@@ -3317,7 +3333,7 @@
       </c>
       <c r="E108" s="7"/>
     </row>
-    <row r="109" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" ht="30">
       <c r="A109" s="9" t="s">
         <v>351</v>
       </c>
@@ -3332,7 +3348,7 @@
       </c>
       <c r="E109" s="7"/>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5">
       <c r="A110" s="9" t="s">
         <v>354</v>
       </c>
@@ -3347,7 +3363,7 @@
       </c>
       <c r="E110" s="7"/>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5">
       <c r="A111" s="9" t="s">
         <v>357</v>
       </c>
@@ -3362,7 +3378,7 @@
       </c>
       <c r="E111" s="7"/>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5">
       <c r="A112" s="9" t="s">
         <v>361</v>
       </c>
@@ -3377,7 +3393,7 @@
       </c>
       <c r="E112" s="7"/>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5">
       <c r="A113" s="17" t="s">
         <v>363</v>
       </c>
@@ -3392,7 +3408,7 @@
       </c>
       <c r="E113" s="19"/>
     </row>
-    <row r="114" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" ht="30">
       <c r="A114" s="9" t="s">
         <v>366</v>
       </c>
@@ -3407,7 +3423,7 @@
       </c>
       <c r="E114" s="7"/>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5">
       <c r="A115" s="9" t="s">
         <v>369</v>
       </c>
@@ -3422,7 +3438,7 @@
       </c>
       <c r="E115" s="7"/>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5">
       <c r="A116" s="9" t="s">
         <v>370</v>
       </c>
@@ -3437,7 +3453,7 @@
       </c>
       <c r="E116" s="7"/>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5">
       <c r="A117" s="9" t="s">
         <v>371</v>
       </c>
@@ -3452,7 +3468,7 @@
       </c>
       <c r="E117" s="7"/>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5">
       <c r="A118" s="9" t="s">
         <v>378</v>
       </c>
@@ -3467,7 +3483,7 @@
       </c>
       <c r="E118" s="7"/>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5">
       <c r="A119" s="9" t="s">
         <v>381</v>
       </c>
@@ -3482,7 +3498,7 @@
       </c>
       <c r="E119" s="7"/>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5">
       <c r="A120" s="9" t="s">
         <v>384</v>
       </c>
@@ -3496,6 +3512,36 @@
         <v>5</v>
       </c>
       <c r="E120" s="7"/>
+    </row>
+    <row r="121" spans="1:5" ht="30">
+      <c r="A121" s="9" t="s">
+        <v>387</v>
+      </c>
+      <c r="B121" s="7" t="s">
+        <v>388</v>
+      </c>
+      <c r="C121" s="8" t="s">
+        <v>389</v>
+      </c>
+      <c r="D121" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E121" s="7"/>
+    </row>
+    <row r="122" spans="1:5">
+      <c r="A122" s="9" t="s">
+        <v>390</v>
+      </c>
+      <c r="B122" s="7" t="s">
+        <v>391</v>
+      </c>
+      <c r="C122" s="8" t="s">
+        <v>392</v>
+      </c>
+      <c r="D122" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E122" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -3508,14 +3554,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView topLeftCell="A10" zoomScale="80" workbookViewId="0">
       <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
@@ -3523,7 +3569,7 @@
     <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="10" t="s">
         <v>35</v>
       </c>
@@ -3537,7 +3583,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="7" t="s">
         <v>37</v>
       </c>
@@ -3549,7 +3595,7 @@
       </c>
       <c r="D2" s="7"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="7" t="s">
         <v>38</v>
       </c>
@@ -3561,7 +3607,7 @@
       </c>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="7" t="s">
         <v>39</v>
       </c>
@@ -3573,7 +3619,7 @@
       </c>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" s="7" t="s">
         <v>40</v>
       </c>
@@ -3585,7 +3631,7 @@
       </c>
       <c r="D5" s="7"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" s="7" t="s">
         <v>41</v>
       </c>
@@ -3597,7 +3643,7 @@
       </c>
       <c r="D6" s="7"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="7" t="s">
         <v>42</v>
       </c>
@@ -3609,7 +3655,7 @@
       </c>
       <c r="D7" s="7"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="7" t="s">
         <v>43</v>
       </c>
@@ -3621,7 +3667,7 @@
       </c>
       <c r="D8" s="7"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="7" t="s">
         <v>44</v>
       </c>
@@ -3633,7 +3679,7 @@
       </c>
       <c r="D9" s="7"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="7" t="s">
         <v>45</v>
       </c>
@@ -3645,7 +3691,7 @@
       </c>
       <c r="D10" s="7"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11" s="7" t="s">
         <v>46</v>
       </c>
@@ -3657,7 +3703,7 @@
       </c>
       <c r="D11" s="7"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="A12" s="7" t="s">
         <v>48</v>
       </c>
@@ -3669,7 +3715,7 @@
       </c>
       <c r="D12" s="7"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="A13" s="7" t="s">
         <v>49</v>
       </c>
@@ -3681,7 +3727,7 @@
       </c>
       <c r="D13" s="7"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="A14" s="7" t="s">
         <v>50</v>
       </c>
@@ -3693,7 +3739,7 @@
       </c>
       <c r="D14" s="7"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="A15" s="7" t="s">
         <v>51</v>
       </c>
@@ -3705,7 +3751,7 @@
       </c>
       <c r="D15" s="7"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="A16" s="7" t="s">
         <v>52</v>
       </c>
@@ -3717,7 +3763,7 @@
       </c>
       <c r="D16" s="7"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4">
       <c r="A17" s="7" t="s">
         <v>53</v>
       </c>
@@ -3729,7 +3775,7 @@
       </c>
       <c r="D17" s="7"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4">
       <c r="A18" s="7" t="s">
         <v>54</v>
       </c>
@@ -3741,7 +3787,7 @@
       </c>
       <c r="D18" s="7"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4">
       <c r="A19" s="7" t="s">
         <v>55</v>
       </c>
@@ -3753,7 +3799,7 @@
       </c>
       <c r="D19" s="7"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4">
       <c r="A20" s="7" t="s">
         <v>56</v>
       </c>
@@ -3765,7 +3811,7 @@
       </c>
       <c r="D20" s="7"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4">
       <c r="A21" s="7" t="s">
         <v>57</v>
       </c>
@@ -3777,7 +3823,7 @@
       </c>
       <c r="D21" s="7"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4">
       <c r="A22" s="7" t="s">
         <v>58</v>
       </c>
@@ -3789,7 +3835,7 @@
       </c>
       <c r="D22" s="7"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4">
       <c r="A23" s="7" t="s">
         <v>59</v>
       </c>
@@ -3801,7 +3847,7 @@
       </c>
       <c r="D23" s="7"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4">
       <c r="A24" s="7" t="s">
         <v>60</v>
       </c>
@@ -3813,7 +3859,7 @@
       </c>
       <c r="D24" s="7"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4">
       <c r="A25" s="7" t="s">
         <v>61</v>
       </c>
@@ -3825,7 +3871,7 @@
       </c>
       <c r="D25" s="7"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4">
       <c r="A26" s="7" t="s">
         <v>47</v>
       </c>
@@ -3844,14 +3890,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A19" sqref="A19:XFD19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
@@ -3859,7 +3905,7 @@
     <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="10" t="s">
         <v>35</v>
       </c>
@@ -3873,7 +3919,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="7" t="s">
         <v>37</v>
       </c>
@@ -3885,7 +3931,7 @@
       </c>
       <c r="D2" s="7"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="7" t="s">
         <v>38</v>
       </c>
@@ -3897,7 +3943,7 @@
       </c>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="7" t="s">
         <v>39</v>
       </c>
@@ -3909,7 +3955,7 @@
       </c>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" s="7" t="s">
         <v>40</v>
       </c>
@@ -3921,7 +3967,7 @@
       </c>
       <c r="D5" s="7"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" s="7" t="s">
         <v>41</v>
       </c>
@@ -3933,7 +3979,7 @@
       </c>
       <c r="D6" s="7"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="7" t="s">
         <v>42</v>
       </c>
@@ -3945,7 +3991,7 @@
       </c>
       <c r="D7" s="7"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="7" t="s">
         <v>43</v>
       </c>
@@ -3957,7 +4003,7 @@
       </c>
       <c r="D8" s="7"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="7" t="s">
         <v>44</v>
       </c>
@@ -3969,7 +4015,7 @@
       </c>
       <c r="D9" s="7"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="7" t="s">
         <v>45</v>
       </c>
@@ -3981,7 +4027,7 @@
       </c>
       <c r="D10" s="7"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11" s="7" t="s">
         <v>46</v>
       </c>
@@ -3993,7 +4039,7 @@
       </c>
       <c r="D11" s="7"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="A12" s="7" t="s">
         <v>47</v>
       </c>
@@ -4005,7 +4051,7 @@
       </c>
       <c r="D12" s="7"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="A13" s="7" t="s">
         <v>48</v>
       </c>
@@ -4017,7 +4063,7 @@
       </c>
       <c r="D13" s="7"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="A14" s="7" t="s">
         <v>49</v>
       </c>
@@ -4029,7 +4075,7 @@
       </c>
       <c r="D14" s="7"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="A15" s="7" t="s">
         <v>50</v>
       </c>
@@ -4041,7 +4087,7 @@
       </c>
       <c r="D15" s="7"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="A16" s="7" t="s">
         <v>51</v>
       </c>
@@ -4053,7 +4099,7 @@
       </c>
       <c r="D16" s="7"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4">
       <c r="A17" s="7" t="s">
         <v>52</v>
       </c>
@@ -4065,7 +4111,7 @@
       </c>
       <c r="D17" s="7"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4">
       <c r="A18" s="7" t="s">
         <v>53</v>
       </c>
@@ -4077,7 +4123,7 @@
       </c>
       <c r="D18" s="7"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4">
       <c r="A19" s="7" t="s">
         <v>54</v>
       </c>
@@ -4089,7 +4135,7 @@
       </c>
       <c r="D19" s="7"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4">
       <c r="A20" s="7" t="s">
         <v>55</v>
       </c>
@@ -4101,7 +4147,7 @@
       </c>
       <c r="D20" s="7"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4">
       <c r="A21" s="7" t="s">
         <v>56</v>
       </c>
@@ -4113,7 +4159,7 @@
       </c>
       <c r="D21" s="7"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4">
       <c r="A22" s="7" t="s">
         <v>57</v>
       </c>
@@ -4125,7 +4171,7 @@
       </c>
       <c r="D22" s="7"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4">
       <c r="A23" s="7" t="s">
         <v>58</v>
       </c>
@@ -4137,7 +4183,7 @@
       </c>
       <c r="D23" s="7"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4">
       <c r="A24" s="7" t="s">
         <v>59</v>
       </c>
@@ -4149,7 +4195,7 @@
       </c>
       <c r="D24" s="7"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4">
       <c r="A25" s="7" t="s">
         <v>60</v>
       </c>
@@ -4161,7 +4207,7 @@
       </c>
       <c r="D25" s="7"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4">
       <c r="A26" s="7" t="s">
         <v>61</v>
       </c>

</xml_diff>

<commit_message>
Adds WAT-117 test script
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/WAT.xlsx
+++ b/src/test/resources/xls/WAT.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="387">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="390">
   <si>
     <t>TCID</t>
   </si>
@@ -1178,6 +1178,15 @@
   </si>
   <si>
     <t>Verify that Find button is still enabled after user clicks on a country name from country dropdown</t>
+  </si>
+  <si>
+    <t>WAT117</t>
+  </si>
+  <si>
+    <t>WAT-1321</t>
+  </si>
+  <si>
+    <t>Verify that User should be able to ignore Country dropdown and proceed with author search</t>
   </si>
 </sst>
 </file>
@@ -1680,10 +1689,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E120"/>
+  <dimension ref="A1:E121"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A98" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C128" sqref="C128"/>
+      <selection activeCell="C121" sqref="C121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3496,6 +3505,21 @@
         <v>5</v>
       </c>
       <c r="E120" s="7"/>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A121" s="9" t="s">
+        <v>387</v>
+      </c>
+      <c r="B121" s="7" t="s">
+        <v>388</v>
+      </c>
+      <c r="C121" s="7" t="s">
+        <v>389</v>
+      </c>
+      <c r="D121" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E121" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
script entry in WAT Xlsx
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/WAT.xlsx
+++ b/src/test/resources/xls/WAT.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13305" windowHeight="2415"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="390">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="396">
   <si>
     <t>TCID</t>
   </si>
@@ -1187,13 +1187,31 @@
   </si>
   <si>
     <t>Verify that User should be able to ignore Country dropdown and proceed with author search</t>
+  </si>
+  <si>
+    <t>WAT154</t>
+  </si>
+  <si>
+    <t>WAT-1157||WAT-1158</t>
+  </si>
+  <si>
+    <t>Verify that user should be able to perform author search using RID||Verify that the System should provide as results any and all author clusters where the specified RID(s) appear on 1 or more authorships</t>
+  </si>
+  <si>
+    <t>WAT155</t>
+  </si>
+  <si>
+    <t>WAT-1159</t>
+  </si>
+  <si>
+    <t>Verify that Error messages should display for invalid pattern RID search/ RID but DNE/ RID older than 2007</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1445,7 +1463,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1477,10 +1495,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1512,7 +1529,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1688,14 +1704,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E121"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E123"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A98" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A124" sqref="A124"/>
+      <selection activeCell="C109" sqref="C109"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="41" bestFit="1" customWidth="1" collapsed="1"/>
@@ -1704,7 +1720,7 @@
     <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1721,7 +1737,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -1736,7 +1752,7 @@
       </c>
       <c r="E2" s="4"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -1751,7 +1767,7 @@
       </c>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" s="7" t="s">
         <v>11</v>
       </c>
@@ -1766,7 +1782,7 @@
       </c>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" s="7" t="s">
         <v>12</v>
       </c>
@@ -1781,7 +1797,7 @@
       </c>
       <c r="E5" s="7"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" s="7" t="s">
         <v>14</v>
       </c>
@@ -1796,7 +1812,7 @@
       </c>
       <c r="E6" s="7"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" s="7" t="s">
         <v>17</v>
       </c>
@@ -1811,7 +1827,7 @@
       </c>
       <c r="E7" s="7"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" s="7" t="s">
         <v>20</v>
       </c>
@@ -1826,7 +1842,7 @@
       </c>
       <c r="E8" s="7"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" s="7" t="s">
         <v>22</v>
       </c>
@@ -1841,7 +1857,7 @@
       </c>
       <c r="E9" s="7"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10" s="7" t="s">
         <v>23</v>
       </c>
@@ -1856,7 +1872,7 @@
       </c>
       <c r="E10" s="7"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11" s="7" t="s">
         <v>24</v>
       </c>
@@ -1871,7 +1887,7 @@
       </c>
       <c r="E11" s="7"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12" s="7" t="s">
         <v>25</v>
       </c>
@@ -1886,7 +1902,7 @@
       </c>
       <c r="E12" s="7"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13" s="7" t="s">
         <v>62</v>
       </c>
@@ -1901,7 +1917,7 @@
       </c>
       <c r="E13" s="7"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="A14" s="7" t="s">
         <v>63</v>
       </c>
@@ -1916,7 +1932,7 @@
       </c>
       <c r="E14" s="7"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="A15" s="7" t="s">
         <v>64</v>
       </c>
@@ -1931,7 +1947,7 @@
       </c>
       <c r="E15" s="7"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="A16" s="7" t="s">
         <v>65</v>
       </c>
@@ -1946,7 +1962,7 @@
       </c>
       <c r="E16" s="7"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5">
       <c r="A17" s="7" t="s">
         <v>74</v>
       </c>
@@ -1961,7 +1977,7 @@
       </c>
       <c r="E17" s="7"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5">
       <c r="A18" s="7" t="s">
         <v>75</v>
       </c>
@@ -1976,7 +1992,7 @@
       </c>
       <c r="E18" s="7"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5">
       <c r="A19" s="7" t="s">
         <v>79</v>
       </c>
@@ -1991,7 +2007,7 @@
       </c>
       <c r="E19" s="7"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5">
       <c r="A20" s="7" t="s">
         <v>81</v>
       </c>
@@ -2006,7 +2022,7 @@
       </c>
       <c r="E20" s="7"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5">
       <c r="A21" s="7" t="s">
         <v>82</v>
       </c>
@@ -2021,7 +2037,7 @@
       </c>
       <c r="E21" s="7"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5">
       <c r="A22" s="7" t="s">
         <v>88</v>
       </c>
@@ -2036,7 +2052,7 @@
       </c>
       <c r="E22" s="7"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5">
       <c r="A23" s="7" t="s">
         <v>90</v>
       </c>
@@ -2051,7 +2067,7 @@
       </c>
       <c r="E23" s="7"/>
     </row>
-    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="30">
       <c r="A24" s="9" t="s">
         <v>94</v>
       </c>
@@ -2066,7 +2082,7 @@
       </c>
       <c r="E24" s="7"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5">
       <c r="A25" s="9" t="s">
         <v>96</v>
       </c>
@@ -2081,7 +2097,7 @@
       </c>
       <c r="E25" s="7"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5">
       <c r="A26" s="9" t="s">
         <v>98</v>
       </c>
@@ -2096,7 +2112,7 @@
       </c>
       <c r="E26" s="7"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5">
       <c r="A27" s="9" t="s">
         <v>102</v>
       </c>
@@ -2111,7 +2127,7 @@
       </c>
       <c r="E27" s="7"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5">
       <c r="A28" s="9" t="s">
         <v>105</v>
       </c>
@@ -2126,7 +2142,7 @@
       </c>
       <c r="E28" s="7"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5">
       <c r="A29" s="9" t="s">
         <v>108</v>
       </c>
@@ -2141,7 +2157,7 @@
       </c>
       <c r="E29" s="7"/>
     </row>
-    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" ht="30">
       <c r="A30" s="9" t="s">
         <v>110</v>
       </c>
@@ -2156,7 +2172,7 @@
       </c>
       <c r="E30" s="7"/>
     </row>
-    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" ht="30">
       <c r="A31" s="9" t="s">
         <v>114</v>
       </c>
@@ -2171,7 +2187,7 @@
       </c>
       <c r="E31" s="7"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5">
       <c r="A32" s="9" t="s">
         <v>119</v>
       </c>
@@ -2186,7 +2202,7 @@
       </c>
       <c r="E32" s="7"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5">
       <c r="A33" s="9" t="s">
         <v>120</v>
       </c>
@@ -2201,7 +2217,7 @@
       </c>
       <c r="E33" s="7"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5">
       <c r="A34" s="9" t="s">
         <v>125</v>
       </c>
@@ -2216,7 +2232,7 @@
       </c>
       <c r="E34" s="7"/>
     </row>
-    <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" ht="30">
       <c r="A35" s="9" t="s">
         <v>128</v>
       </c>
@@ -2231,7 +2247,7 @@
       </c>
       <c r="E35" s="7"/>
     </row>
-    <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" ht="30">
       <c r="A36" s="9" t="s">
         <v>131</v>
       </c>
@@ -2246,7 +2262,7 @@
       </c>
       <c r="E36" s="7"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5">
       <c r="A37" s="9" t="s">
         <v>134</v>
       </c>
@@ -2261,7 +2277,7 @@
       </c>
       <c r="E37" s="7"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5">
       <c r="A38" s="9" t="s">
         <v>137</v>
       </c>
@@ -2276,7 +2292,7 @@
       </c>
       <c r="E38" s="7"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5">
       <c r="A39" s="9" t="s">
         <v>140</v>
       </c>
@@ -2291,7 +2307,7 @@
       </c>
       <c r="E39" s="7"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5">
       <c r="A40" s="9" t="s">
         <v>143</v>
       </c>
@@ -2306,7 +2322,7 @@
       </c>
       <c r="E40" s="7"/>
     </row>
-    <row r="41" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" ht="30">
       <c r="A41" s="9" t="s">
         <v>145</v>
       </c>
@@ -2321,7 +2337,7 @@
       </c>
       <c r="E41" s="7"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5">
       <c r="A42" s="9" t="s">
         <v>147</v>
       </c>
@@ -2336,7 +2352,7 @@
       </c>
       <c r="E42" s="7"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5">
       <c r="A43" s="9" t="s">
         <v>150</v>
       </c>
@@ -2351,7 +2367,7 @@
       </c>
       <c r="E43" s="7"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5">
       <c r="A44" s="9" t="s">
         <v>153</v>
       </c>
@@ -2366,7 +2382,7 @@
       </c>
       <c r="E44" s="7"/>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5">
       <c r="A45" s="9" t="s">
         <v>155</v>
       </c>
@@ -2381,7 +2397,7 @@
       </c>
       <c r="E45" s="7"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5">
       <c r="A46" s="12" t="s">
         <v>158</v>
       </c>
@@ -2396,7 +2412,7 @@
       </c>
       <c r="E46" s="7"/>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5">
       <c r="A47" s="12" t="s">
         <v>159</v>
       </c>
@@ -2411,7 +2427,7 @@
       </c>
       <c r="E47" s="7"/>
     </row>
-    <row r="48" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" ht="30">
       <c r="A48" s="12" t="s">
         <v>160</v>
       </c>
@@ -2426,7 +2442,7 @@
       </c>
       <c r="E48" s="7"/>
     </row>
-    <row r="49" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" ht="30">
       <c r="A49" s="12" t="s">
         <v>161</v>
       </c>
@@ -2441,7 +2457,7 @@
       </c>
       <c r="E49" s="7"/>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5">
       <c r="A50" s="12" t="s">
         <v>164</v>
       </c>
@@ -2456,7 +2472,7 @@
       </c>
       <c r="E50" s="7"/>
     </row>
-    <row r="51" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" ht="30">
       <c r="A51" s="9" t="s">
         <v>173</v>
       </c>
@@ -2471,7 +2487,7 @@
       </c>
       <c r="E51" s="7"/>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5">
       <c r="A52" s="9" t="s">
         <v>174</v>
       </c>
@@ -2486,7 +2502,7 @@
       </c>
       <c r="E52" s="7"/>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5">
       <c r="A53" s="9" t="s">
         <v>179</v>
       </c>
@@ -2501,7 +2517,7 @@
       </c>
       <c r="E53" s="7"/>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5">
       <c r="A54" s="9" t="s">
         <v>180</v>
       </c>
@@ -2516,7 +2532,7 @@
       </c>
       <c r="E54" s="7"/>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5">
       <c r="A55" s="9" t="s">
         <v>185</v>
       </c>
@@ -2531,7 +2547,7 @@
       </c>
       <c r="E55" s="7"/>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5">
       <c r="A56" s="9" t="s">
         <v>188</v>
       </c>
@@ -2546,7 +2562,7 @@
       </c>
       <c r="E56" s="7"/>
     </row>
-    <row r="57" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" ht="30">
       <c r="A57" s="9" t="s">
         <v>191</v>
       </c>
@@ -2561,7 +2577,7 @@
       </c>
       <c r="E57" s="7"/>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5">
       <c r="A58" s="9" t="s">
         <v>194</v>
       </c>
@@ -2576,7 +2592,7 @@
       </c>
       <c r="E58" s="7"/>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5">
       <c r="A59" s="7" t="s">
         <v>196</v>
       </c>
@@ -2591,7 +2607,7 @@
       </c>
       <c r="E59" s="7"/>
     </row>
-    <row r="60" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" ht="45">
       <c r="A60" s="7" t="s">
         <v>199</v>
       </c>
@@ -2606,7 +2622,7 @@
       </c>
       <c r="E60" s="7"/>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5">
       <c r="A61" s="9" t="s">
         <v>202</v>
       </c>
@@ -2621,7 +2637,7 @@
       </c>
       <c r="E61" s="7"/>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5">
       <c r="A62" s="9" t="s">
         <v>204</v>
       </c>
@@ -2636,7 +2652,7 @@
       </c>
       <c r="E62" s="7"/>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5">
       <c r="A63" s="9" t="s">
         <v>206</v>
       </c>
@@ -2651,7 +2667,7 @@
       </c>
       <c r="E63" s="7"/>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5">
       <c r="A64" s="9" t="s">
         <v>208</v>
       </c>
@@ -2666,7 +2682,7 @@
       </c>
       <c r="E64" s="7"/>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5">
       <c r="A65" s="9" t="s">
         <v>217</v>
       </c>
@@ -2681,7 +2697,7 @@
       </c>
       <c r="E65" s="7"/>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5">
       <c r="A66" s="9" t="s">
         <v>218</v>
       </c>
@@ -2696,7 +2712,7 @@
       </c>
       <c r="E66" s="7"/>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5">
       <c r="A67" s="9" t="s">
         <v>223</v>
       </c>
@@ -2711,7 +2727,7 @@
       </c>
       <c r="E67" s="7"/>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5">
       <c r="A68" s="9" t="s">
         <v>224</v>
       </c>
@@ -2726,7 +2742,7 @@
       </c>
       <c r="E68" s="7"/>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5">
       <c r="A69" s="9" t="s">
         <v>225</v>
       </c>
@@ -2741,7 +2757,7 @@
       </c>
       <c r="E69" s="7"/>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5">
       <c r="A70" s="9" t="s">
         <v>226</v>
       </c>
@@ -2756,7 +2772,7 @@
       </c>
       <c r="E70" s="7"/>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5">
       <c r="A71" s="9" t="s">
         <v>233</v>
       </c>
@@ -2771,7 +2787,7 @@
       </c>
       <c r="E71" s="7"/>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5">
       <c r="A72" s="9" t="s">
         <v>237</v>
       </c>
@@ -2786,7 +2802,7 @@
       </c>
       <c r="E72" s="7"/>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5">
       <c r="A73" s="9" t="s">
         <v>239</v>
       </c>
@@ -2801,7 +2817,7 @@
       </c>
       <c r="E73" s="7"/>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5">
       <c r="A74" s="9" t="s">
         <v>243</v>
       </c>
@@ -2816,7 +2832,7 @@
       </c>
       <c r="E74" s="7"/>
     </row>
-    <row r="75" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" ht="30">
       <c r="A75" s="9" t="s">
         <v>245</v>
       </c>
@@ -2831,7 +2847,7 @@
       </c>
       <c r="E75" s="7"/>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5">
       <c r="A76" s="9" t="s">
         <v>248</v>
       </c>
@@ -2846,7 +2862,7 @@
       </c>
       <c r="E76" s="7"/>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5">
       <c r="A77" s="9" t="s">
         <v>256</v>
       </c>
@@ -2861,7 +2877,7 @@
       </c>
       <c r="E77" s="7"/>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5">
       <c r="A78" s="9" t="s">
         <v>257</v>
       </c>
@@ -2876,7 +2892,7 @@
       </c>
       <c r="E78" s="7"/>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5">
       <c r="A79" s="9" t="s">
         <v>261</v>
       </c>
@@ -2891,7 +2907,7 @@
       </c>
       <c r="E79" s="7"/>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5">
       <c r="A80" s="9" t="s">
         <v>264</v>
       </c>
@@ -2906,7 +2922,7 @@
       </c>
       <c r="E80" s="7"/>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5">
       <c r="A81" s="9" t="s">
         <v>267</v>
       </c>
@@ -2921,7 +2937,7 @@
       </c>
       <c r="E81" s="7"/>
     </row>
-    <row r="82" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" ht="30">
       <c r="A82" s="9" t="s">
         <v>269</v>
       </c>
@@ -2936,7 +2952,7 @@
       </c>
       <c r="E82" s="7"/>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5">
       <c r="A83" s="9" t="s">
         <v>274</v>
       </c>
@@ -2951,7 +2967,7 @@
       </c>
       <c r="E83" s="7"/>
     </row>
-    <row r="84" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" ht="30">
       <c r="A84" s="9" t="s">
         <v>277</v>
       </c>
@@ -2966,7 +2982,7 @@
       </c>
       <c r="E84" s="7"/>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5">
       <c r="A85" s="9" t="s">
         <v>279</v>
       </c>
@@ -2981,7 +2997,7 @@
       </c>
       <c r="E85" s="7"/>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5">
       <c r="A86" s="9" t="s">
         <v>282</v>
       </c>
@@ -2996,7 +3012,7 @@
       </c>
       <c r="E86" s="7"/>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5">
       <c r="A87" s="9" t="s">
         <v>285</v>
       </c>
@@ -3011,7 +3027,7 @@
       </c>
       <c r="E87" s="7"/>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5">
       <c r="A88" s="9" t="s">
         <v>288</v>
       </c>
@@ -3026,7 +3042,7 @@
       </c>
       <c r="E88" s="7"/>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5">
       <c r="A89" s="9" t="s">
         <v>291</v>
       </c>
@@ -3041,7 +3057,7 @@
       </c>
       <c r="E89" s="7"/>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5">
       <c r="A90" s="9" t="s">
         <v>294</v>
       </c>
@@ -3056,7 +3072,7 @@
       </c>
       <c r="E90" s="7"/>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5">
       <c r="A91" s="9" t="s">
         <v>297</v>
       </c>
@@ -3071,7 +3087,7 @@
       </c>
       <c r="E91" s="7"/>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5">
       <c r="A92" s="9" t="s">
         <v>300</v>
       </c>
@@ -3086,7 +3102,7 @@
       </c>
       <c r="E92" s="7"/>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5">
       <c r="A93" s="9" t="s">
         <v>303</v>
       </c>
@@ -3101,7 +3117,7 @@
       </c>
       <c r="E93" s="7"/>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5">
       <c r="A94" s="9" t="s">
         <v>306</v>
       </c>
@@ -3116,7 +3132,7 @@
       </c>
       <c r="E94" s="7"/>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5">
       <c r="A95" s="9" t="s">
         <v>309</v>
       </c>
@@ -3131,7 +3147,7 @@
       </c>
       <c r="E95" s="7"/>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5">
       <c r="A96" s="9" t="s">
         <v>314</v>
       </c>
@@ -3146,7 +3162,7 @@
       </c>
       <c r="E96" s="7"/>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5">
       <c r="A97" s="9" t="s">
         <v>315</v>
       </c>
@@ -3161,7 +3177,7 @@
       </c>
       <c r="E97" s="7"/>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5">
       <c r="A98" s="9" t="s">
         <v>319</v>
       </c>
@@ -3176,7 +3192,7 @@
       </c>
       <c r="E98" s="7"/>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5">
       <c r="A99" s="9" t="s">
         <v>321</v>
       </c>
@@ -3191,7 +3207,7 @@
       </c>
       <c r="E99" s="7"/>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5">
       <c r="A100" s="9" t="s">
         <v>322</v>
       </c>
@@ -3206,7 +3222,7 @@
       </c>
       <c r="E100" s="7"/>
     </row>
-    <row r="101" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" ht="30">
       <c r="A101" s="9" t="s">
         <v>323</v>
       </c>
@@ -3221,7 +3237,7 @@
       </c>
       <c r="E101" s="7"/>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5">
       <c r="A102" s="9" t="s">
         <v>328</v>
       </c>
@@ -3236,7 +3252,7 @@
       </c>
       <c r="E102" s="7"/>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5">
       <c r="A103" s="9" t="s">
         <v>333</v>
       </c>
@@ -3251,7 +3267,7 @@
       </c>
       <c r="E103" s="7"/>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5">
       <c r="A104" s="9" t="s">
         <v>336</v>
       </c>
@@ -3266,7 +3282,7 @@
       </c>
       <c r="E104" s="7"/>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5">
       <c r="A105" s="9" t="s">
         <v>337</v>
       </c>
@@ -3281,7 +3297,7 @@
       </c>
       <c r="E105" s="7"/>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5">
       <c r="A106" s="9" t="s">
         <v>342</v>
       </c>
@@ -3296,7 +3312,7 @@
       </c>
       <c r="E106" s="7"/>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5">
       <c r="A107" s="9" t="s">
         <v>345</v>
       </c>
@@ -3311,7 +3327,7 @@
       </c>
       <c r="E107" s="7"/>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5">
       <c r="A108" s="9" t="s">
         <v>350</v>
       </c>
@@ -3326,7 +3342,7 @@
       </c>
       <c r="E108" s="7"/>
     </row>
-    <row r="109" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" ht="30">
       <c r="A109" s="9" t="s">
         <v>351</v>
       </c>
@@ -3341,7 +3357,7 @@
       </c>
       <c r="E109" s="7"/>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5">
       <c r="A110" s="9" t="s">
         <v>354</v>
       </c>
@@ -3356,7 +3372,7 @@
       </c>
       <c r="E110" s="7"/>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5">
       <c r="A111" s="9" t="s">
         <v>357</v>
       </c>
@@ -3371,7 +3387,7 @@
       </c>
       <c r="E111" s="7"/>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5">
       <c r="A112" s="9" t="s">
         <v>361</v>
       </c>
@@ -3386,7 +3402,7 @@
       </c>
       <c r="E112" s="7"/>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5">
       <c r="A113" s="17" t="s">
         <v>363</v>
       </c>
@@ -3401,7 +3417,7 @@
       </c>
       <c r="E113" s="19"/>
     </row>
-    <row r="114" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" ht="30">
       <c r="A114" s="9" t="s">
         <v>366</v>
       </c>
@@ -3416,7 +3432,7 @@
       </c>
       <c r="E114" s="7"/>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5">
       <c r="A115" s="9" t="s">
         <v>369</v>
       </c>
@@ -3431,7 +3447,7 @@
       </c>
       <c r="E115" s="7"/>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5">
       <c r="A116" s="9" t="s">
         <v>370</v>
       </c>
@@ -3446,7 +3462,7 @@
       </c>
       <c r="E116" s="7"/>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5">
       <c r="A117" s="9" t="s">
         <v>371</v>
       </c>
@@ -3461,7 +3477,7 @@
       </c>
       <c r="E117" s="7"/>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5">
       <c r="A118" s="9" t="s">
         <v>378</v>
       </c>
@@ -3476,7 +3492,7 @@
       </c>
       <c r="E118" s="7"/>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5">
       <c r="A119" s="9" t="s">
         <v>381</v>
       </c>
@@ -3491,7 +3507,7 @@
       </c>
       <c r="E119" s="7"/>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5">
       <c r="A120" s="9" t="s">
         <v>384</v>
       </c>
@@ -3506,7 +3522,7 @@
       </c>
       <c r="E120" s="7"/>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5">
       <c r="A121" s="9" t="s">
         <v>387</v>
       </c>
@@ -3520,6 +3536,36 @@
         <v>5</v>
       </c>
       <c r="E121" s="7"/>
+    </row>
+    <row r="122" spans="1:5">
+      <c r="A122" s="7" t="s">
+        <v>390</v>
+      </c>
+      <c r="B122" s="7" t="s">
+        <v>391</v>
+      </c>
+      <c r="C122" s="7" t="s">
+        <v>392</v>
+      </c>
+      <c r="D122" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E122" s="7"/>
+    </row>
+    <row r="123" spans="1:5">
+      <c r="A123" s="7" t="s">
+        <v>393</v>
+      </c>
+      <c r="B123" s="7" t="s">
+        <v>394</v>
+      </c>
+      <c r="C123" s="7" t="s">
+        <v>395</v>
+      </c>
+      <c r="D123" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E123" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -3532,14 +3578,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView topLeftCell="A10" zoomScale="80" workbookViewId="0">
       <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
@@ -3547,7 +3593,7 @@
     <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="10" t="s">
         <v>35</v>
       </c>
@@ -3561,7 +3607,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="7" t="s">
         <v>37</v>
       </c>
@@ -3573,7 +3619,7 @@
       </c>
       <c r="D2" s="7"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="7" t="s">
         <v>38</v>
       </c>
@@ -3585,7 +3631,7 @@
       </c>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="7" t="s">
         <v>39</v>
       </c>
@@ -3597,7 +3643,7 @@
       </c>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" s="7" t="s">
         <v>40</v>
       </c>
@@ -3609,7 +3655,7 @@
       </c>
       <c r="D5" s="7"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" s="7" t="s">
         <v>41</v>
       </c>
@@ -3621,7 +3667,7 @@
       </c>
       <c r="D6" s="7"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="7" t="s">
         <v>42</v>
       </c>
@@ -3633,7 +3679,7 @@
       </c>
       <c r="D7" s="7"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="7" t="s">
         <v>43</v>
       </c>
@@ -3645,7 +3691,7 @@
       </c>
       <c r="D8" s="7"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="7" t="s">
         <v>44</v>
       </c>
@@ -3657,7 +3703,7 @@
       </c>
       <c r="D9" s="7"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="7" t="s">
         <v>45</v>
       </c>
@@ -3669,7 +3715,7 @@
       </c>
       <c r="D10" s="7"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11" s="7" t="s">
         <v>46</v>
       </c>
@@ -3681,7 +3727,7 @@
       </c>
       <c r="D11" s="7"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="A12" s="7" t="s">
         <v>48</v>
       </c>
@@ -3693,7 +3739,7 @@
       </c>
       <c r="D12" s="7"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="A13" s="7" t="s">
         <v>49</v>
       </c>
@@ -3705,7 +3751,7 @@
       </c>
       <c r="D13" s="7"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="A14" s="7" t="s">
         <v>50</v>
       </c>
@@ -3717,7 +3763,7 @@
       </c>
       <c r="D14" s="7"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="A15" s="7" t="s">
         <v>51</v>
       </c>
@@ -3729,7 +3775,7 @@
       </c>
       <c r="D15" s="7"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="A16" s="7" t="s">
         <v>52</v>
       </c>
@@ -3741,7 +3787,7 @@
       </c>
       <c r="D16" s="7"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4">
       <c r="A17" s="7" t="s">
         <v>53</v>
       </c>
@@ -3753,7 +3799,7 @@
       </c>
       <c r="D17" s="7"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4">
       <c r="A18" s="7" t="s">
         <v>54</v>
       </c>
@@ -3765,7 +3811,7 @@
       </c>
       <c r="D18" s="7"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4">
       <c r="A19" s="7" t="s">
         <v>55</v>
       </c>
@@ -3777,7 +3823,7 @@
       </c>
       <c r="D19" s="7"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4">
       <c r="A20" s="7" t="s">
         <v>56</v>
       </c>
@@ -3789,7 +3835,7 @@
       </c>
       <c r="D20" s="7"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4">
       <c r="A21" s="7" t="s">
         <v>57</v>
       </c>
@@ -3801,7 +3847,7 @@
       </c>
       <c r="D21" s="7"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4">
       <c r="A22" s="7" t="s">
         <v>58</v>
       </c>
@@ -3813,7 +3859,7 @@
       </c>
       <c r="D22" s="7"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4">
       <c r="A23" s="7" t="s">
         <v>59</v>
       </c>
@@ -3825,7 +3871,7 @@
       </c>
       <c r="D23" s="7"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4">
       <c r="A24" s="7" t="s">
         <v>60</v>
       </c>
@@ -3837,7 +3883,7 @@
       </c>
       <c r="D24" s="7"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4">
       <c r="A25" s="7" t="s">
         <v>61</v>
       </c>
@@ -3849,7 +3895,7 @@
       </c>
       <c r="D25" s="7"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4">
       <c r="A26" s="7" t="s">
         <v>47</v>
       </c>
@@ -3868,14 +3914,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A19" sqref="A19:XFD19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
@@ -3883,7 +3929,7 @@
     <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="10" t="s">
         <v>35</v>
       </c>
@@ -3897,7 +3943,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="7" t="s">
         <v>37</v>
       </c>
@@ -3909,7 +3955,7 @@
       </c>
       <c r="D2" s="7"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="7" t="s">
         <v>38</v>
       </c>
@@ -3921,7 +3967,7 @@
       </c>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="7" t="s">
         <v>39</v>
       </c>
@@ -3933,7 +3979,7 @@
       </c>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" s="7" t="s">
         <v>40</v>
       </c>
@@ -3945,7 +3991,7 @@
       </c>
       <c r="D5" s="7"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" s="7" t="s">
         <v>41</v>
       </c>
@@ -3957,7 +4003,7 @@
       </c>
       <c r="D6" s="7"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="7" t="s">
         <v>42</v>
       </c>
@@ -3969,7 +4015,7 @@
       </c>
       <c r="D7" s="7"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="7" t="s">
         <v>43</v>
       </c>
@@ -3981,7 +4027,7 @@
       </c>
       <c r="D8" s="7"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="7" t="s">
         <v>44</v>
       </c>
@@ -3993,7 +4039,7 @@
       </c>
       <c r="D9" s="7"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="7" t="s">
         <v>45</v>
       </c>
@@ -4005,7 +4051,7 @@
       </c>
       <c r="D10" s="7"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11" s="7" t="s">
         <v>46</v>
       </c>
@@ -4017,7 +4063,7 @@
       </c>
       <c r="D11" s="7"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="A12" s="7" t="s">
         <v>47</v>
       </c>
@@ -4029,7 +4075,7 @@
       </c>
       <c r="D12" s="7"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="A13" s="7" t="s">
         <v>48</v>
       </c>
@@ -4041,7 +4087,7 @@
       </c>
       <c r="D13" s="7"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="A14" s="7" t="s">
         <v>49</v>
       </c>
@@ -4053,7 +4099,7 @@
       </c>
       <c r="D14" s="7"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="A15" s="7" t="s">
         <v>50</v>
       </c>
@@ -4065,7 +4111,7 @@
       </c>
       <c r="D15" s="7"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="A16" s="7" t="s">
         <v>51</v>
       </c>
@@ -4077,7 +4123,7 @@
       </c>
       <c r="D16" s="7"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4">
       <c r="A17" s="7" t="s">
         <v>52</v>
       </c>
@@ -4089,7 +4135,7 @@
       </c>
       <c r="D17" s="7"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4">
       <c r="A18" s="7" t="s">
         <v>53</v>
       </c>
@@ -4101,7 +4147,7 @@
       </c>
       <c r="D18" s="7"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4">
       <c r="A19" s="7" t="s">
         <v>54</v>
       </c>
@@ -4113,7 +4159,7 @@
       </c>
       <c r="D19" s="7"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4">
       <c r="A20" s="7" t="s">
         <v>55</v>
       </c>
@@ -4125,7 +4171,7 @@
       </c>
       <c r="D20" s="7"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4">
       <c r="A21" s="7" t="s">
         <v>56</v>
       </c>
@@ -4137,7 +4183,7 @@
       </c>
       <c r="D21" s="7"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4">
       <c r="A22" s="7" t="s">
         <v>57</v>
       </c>
@@ -4149,7 +4195,7 @@
       </c>
       <c r="D22" s="7"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4">
       <c r="A23" s="7" t="s">
         <v>58</v>
       </c>
@@ -4161,7 +4207,7 @@
       </c>
       <c r="D23" s="7"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4">
       <c r="A24" s="7" t="s">
         <v>59</v>
       </c>
@@ -4173,7 +4219,7 @@
       </c>
       <c r="D24" s="7"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4">
       <c r="A25" s="7" t="s">
         <v>60</v>
       </c>
@@ -4185,7 +4231,7 @@
       </c>
       <c r="D25" s="7"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4">
       <c r="A26" s="7" t="s">
         <v>61</v>
       </c>

</xml_diff>

<commit_message>
WAT new script for RID Search
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/WAT.xlsx
+++ b/src/test/resources/xls/WAT.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="396">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="655" uniqueCount="399">
   <si>
     <t>TCID</t>
   </si>
@@ -1205,6 +1205,15 @@
   </si>
   <si>
     <t>Verify that Error messages should display for invalid pattern RID search/ RID but DNE/ RID older than 2007</t>
+  </si>
+  <si>
+    <t>WAT156</t>
+  </si>
+  <si>
+    <t>WAT-1160</t>
+  </si>
+  <si>
+    <t>Verify that following Error messages should display for invalid/unavailable/invalid pattern ORCiD search</t>
   </si>
 </sst>
 </file>
@@ -1705,10 +1714,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E123"/>
+  <dimension ref="A1:E124"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A98" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C109" sqref="C109"/>
+      <selection activeCell="A124" sqref="A124:E124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3566,6 +3575,21 @@
         <v>5</v>
       </c>
       <c r="E123" s="7"/>
+    </row>
+    <row r="124" spans="1:5">
+      <c r="A124" s="7" t="s">
+        <v>396</v>
+      </c>
+      <c r="B124" s="7" t="s">
+        <v>397</v>
+      </c>
+      <c r="C124" s="7" t="s">
+        <v>398</v>
+      </c>
+      <c r="D124" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E124" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Adds wat-118 test script
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/WAT.xlsx
+++ b/src/test/resources/xls/WAT.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13305" windowHeight="2415"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="655" uniqueCount="399">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="402">
   <si>
     <t>TCID</t>
   </si>
@@ -1214,13 +1214,22 @@
   </si>
   <si>
     <t>Verify that following Error messages should display for invalid/unavailable/invalid pattern ORCiD search</t>
+  </si>
+  <si>
+    <t>WAT118</t>
+  </si>
+  <si>
+    <t>WAT-1322</t>
+  </si>
+  <si>
+    <t>Verify that User should be able to ignore Org dropdown and proceed with author search</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1472,7 +1481,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1504,9 +1513,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1538,6 +1548,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1713,14 +1724,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E124"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E125"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A98" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A124" sqref="A124:E124"/>
+      <selection activeCell="C128" sqref="C128"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="41" bestFit="1" customWidth="1" collapsed="1"/>
@@ -1729,7 +1740,7 @@
     <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1746,7 +1757,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -1761,7 +1772,7 @@
       </c>
       <c r="E2" s="4"/>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -1776,7 +1787,7 @@
       </c>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>11</v>
       </c>
@@ -1791,7 +1802,7 @@
       </c>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>12</v>
       </c>
@@ -1806,7 +1817,7 @@
       </c>
       <c r="E5" s="7"/>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>14</v>
       </c>
@@ -1821,7 +1832,7 @@
       </c>
       <c r="E6" s="7"/>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>17</v>
       </c>
@@ -1836,7 +1847,7 @@
       </c>
       <c r="E7" s="7"/>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>20</v>
       </c>
@@ -1851,7 +1862,7 @@
       </c>
       <c r="E8" s="7"/>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>22</v>
       </c>
@@ -1866,7 +1877,7 @@
       </c>
       <c r="E9" s="7"/>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>23</v>
       </c>
@@ -1881,7 +1892,7 @@
       </c>
       <c r="E10" s="7"/>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>24</v>
       </c>
@@ -1896,7 +1907,7 @@
       </c>
       <c r="E11" s="7"/>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>25</v>
       </c>
@@ -1911,7 +1922,7 @@
       </c>
       <c r="E12" s="7"/>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>62</v>
       </c>
@@ -1926,7 +1937,7 @@
       </c>
       <c r="E13" s="7"/>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>63</v>
       </c>
@@ -1941,7 +1952,7 @@
       </c>
       <c r="E14" s="7"/>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>64</v>
       </c>
@@ -1956,7 +1967,7 @@
       </c>
       <c r="E15" s="7"/>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>65</v>
       </c>
@@ -1971,7 +1982,7 @@
       </c>
       <c r="E16" s="7"/>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>74</v>
       </c>
@@ -1986,7 +1997,7 @@
       </c>
       <c r="E17" s="7"/>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>75</v>
       </c>
@@ -2001,7 +2012,7 @@
       </c>
       <c r="E18" s="7"/>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>79</v>
       </c>
@@ -2016,7 +2027,7 @@
       </c>
       <c r="E19" s="7"/>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>81</v>
       </c>
@@ -2031,7 +2042,7 @@
       </c>
       <c r="E20" s="7"/>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>82</v>
       </c>
@@ -2046,7 +2057,7 @@
       </c>
       <c r="E21" s="7"/>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>88</v>
       </c>
@@ -2061,7 +2072,7 @@
       </c>
       <c r="E22" s="7"/>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>90</v>
       </c>
@@ -2076,7 +2087,7 @@
       </c>
       <c r="E23" s="7"/>
     </row>
-    <row r="24" spans="1:5" ht="30">
+    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>94</v>
       </c>
@@ -2091,7 +2102,7 @@
       </c>
       <c r="E24" s="7"/>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>96</v>
       </c>
@@ -2106,7 +2117,7 @@
       </c>
       <c r="E25" s="7"/>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
         <v>98</v>
       </c>
@@ -2121,7 +2132,7 @@
       </c>
       <c r="E26" s="7"/>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
         <v>102</v>
       </c>
@@ -2136,7 +2147,7 @@
       </c>
       <c r="E27" s="7"/>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
         <v>105</v>
       </c>
@@ -2151,7 +2162,7 @@
       </c>
       <c r="E28" s="7"/>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
         <v>108</v>
       </c>
@@ -2166,7 +2177,7 @@
       </c>
       <c r="E29" s="7"/>
     </row>
-    <row r="30" spans="1:5" ht="30">
+    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
         <v>110</v>
       </c>
@@ -2181,7 +2192,7 @@
       </c>
       <c r="E30" s="7"/>
     </row>
-    <row r="31" spans="1:5" ht="30">
+    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
         <v>114</v>
       </c>
@@ -2196,7 +2207,7 @@
       </c>
       <c r="E31" s="7"/>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
         <v>119</v>
       </c>
@@ -2211,7 +2222,7 @@
       </c>
       <c r="E32" s="7"/>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
         <v>120</v>
       </c>
@@ -2226,7 +2237,7 @@
       </c>
       <c r="E33" s="7"/>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
         <v>125</v>
       </c>
@@ -2241,7 +2252,7 @@
       </c>
       <c r="E34" s="7"/>
     </row>
-    <row r="35" spans="1:5" ht="30">
+    <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
         <v>128</v>
       </c>
@@ -2256,7 +2267,7 @@
       </c>
       <c r="E35" s="7"/>
     </row>
-    <row r="36" spans="1:5" ht="30">
+    <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
         <v>131</v>
       </c>
@@ -2271,7 +2282,7 @@
       </c>
       <c r="E36" s="7"/>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
         <v>134</v>
       </c>
@@ -2286,7 +2297,7 @@
       </c>
       <c r="E37" s="7"/>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="9" t="s">
         <v>137</v>
       </c>
@@ -2301,7 +2312,7 @@
       </c>
       <c r="E38" s="7"/>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="s">
         <v>140</v>
       </c>
@@ -2316,7 +2327,7 @@
       </c>
       <c r="E39" s="7"/>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="9" t="s">
         <v>143</v>
       </c>
@@ -2331,7 +2342,7 @@
       </c>
       <c r="E40" s="7"/>
     </row>
-    <row r="41" spans="1:5" ht="30">
+    <row r="41" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
         <v>145</v>
       </c>
@@ -2346,7 +2357,7 @@
       </c>
       <c r="E41" s="7"/>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="9" t="s">
         <v>147</v>
       </c>
@@ -2361,7 +2372,7 @@
       </c>
       <c r="E42" s="7"/>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="9" t="s">
         <v>150</v>
       </c>
@@ -2376,7 +2387,7 @@
       </c>
       <c r="E43" s="7"/>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="9" t="s">
         <v>153</v>
       </c>
@@ -2391,7 +2402,7 @@
       </c>
       <c r="E44" s="7"/>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="9" t="s">
         <v>155</v>
       </c>
@@ -2406,7 +2417,7 @@
       </c>
       <c r="E45" s="7"/>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="12" t="s">
         <v>158</v>
       </c>
@@ -2421,7 +2432,7 @@
       </c>
       <c r="E46" s="7"/>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="12" t="s">
         <v>159</v>
       </c>
@@ -2436,7 +2447,7 @@
       </c>
       <c r="E47" s="7"/>
     </row>
-    <row r="48" spans="1:5" ht="30">
+    <row r="48" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="12" t="s">
         <v>160</v>
       </c>
@@ -2451,7 +2462,7 @@
       </c>
       <c r="E48" s="7"/>
     </row>
-    <row r="49" spans="1:5" ht="30">
+    <row r="49" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="12" t="s">
         <v>161</v>
       </c>
@@ -2466,7 +2477,7 @@
       </c>
       <c r="E49" s="7"/>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="12" t="s">
         <v>164</v>
       </c>
@@ -2481,7 +2492,7 @@
       </c>
       <c r="E50" s="7"/>
     </row>
-    <row r="51" spans="1:5" ht="30">
+    <row r="51" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="9" t="s">
         <v>173</v>
       </c>
@@ -2496,7 +2507,7 @@
       </c>
       <c r="E51" s="7"/>
     </row>
-    <row r="52" spans="1:5">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="9" t="s">
         <v>174</v>
       </c>
@@ -2511,7 +2522,7 @@
       </c>
       <c r="E52" s="7"/>
     </row>
-    <row r="53" spans="1:5">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="9" t="s">
         <v>179</v>
       </c>
@@ -2526,7 +2537,7 @@
       </c>
       <c r="E53" s="7"/>
     </row>
-    <row r="54" spans="1:5">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="9" t="s">
         <v>180</v>
       </c>
@@ -2541,7 +2552,7 @@
       </c>
       <c r="E54" s="7"/>
     </row>
-    <row r="55" spans="1:5">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="9" t="s">
         <v>185</v>
       </c>
@@ -2556,7 +2567,7 @@
       </c>
       <c r="E55" s="7"/>
     </row>
-    <row r="56" spans="1:5">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="s">
         <v>188</v>
       </c>
@@ -2571,7 +2582,7 @@
       </c>
       <c r="E56" s="7"/>
     </row>
-    <row r="57" spans="1:5" ht="30">
+    <row r="57" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="9" t="s">
         <v>191</v>
       </c>
@@ -2586,7 +2597,7 @@
       </c>
       <c r="E57" s="7"/>
     </row>
-    <row r="58" spans="1:5">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="9" t="s">
         <v>194</v>
       </c>
@@ -2601,7 +2612,7 @@
       </c>
       <c r="E58" s="7"/>
     </row>
-    <row r="59" spans="1:5">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
         <v>196</v>
       </c>
@@ -2616,7 +2627,7 @@
       </c>
       <c r="E59" s="7"/>
     </row>
-    <row r="60" spans="1:5" ht="45">
+    <row r="60" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
         <v>199</v>
       </c>
@@ -2631,7 +2642,7 @@
       </c>
       <c r="E60" s="7"/>
     </row>
-    <row r="61" spans="1:5">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="9" t="s">
         <v>202</v>
       </c>
@@ -2646,7 +2657,7 @@
       </c>
       <c r="E61" s="7"/>
     </row>
-    <row r="62" spans="1:5">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="9" t="s">
         <v>204</v>
       </c>
@@ -2661,7 +2672,7 @@
       </c>
       <c r="E62" s="7"/>
     </row>
-    <row r="63" spans="1:5">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="9" t="s">
         <v>206</v>
       </c>
@@ -2676,7 +2687,7 @@
       </c>
       <c r="E63" s="7"/>
     </row>
-    <row r="64" spans="1:5">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="9" t="s">
         <v>208</v>
       </c>
@@ -2691,7 +2702,7 @@
       </c>
       <c r="E64" s="7"/>
     </row>
-    <row r="65" spans="1:5">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="9" t="s">
         <v>217</v>
       </c>
@@ -2706,7 +2717,7 @@
       </c>
       <c r="E65" s="7"/>
     </row>
-    <row r="66" spans="1:5">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="9" t="s">
         <v>218</v>
       </c>
@@ -2721,7 +2732,7 @@
       </c>
       <c r="E66" s="7"/>
     </row>
-    <row r="67" spans="1:5">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="9" t="s">
         <v>223</v>
       </c>
@@ -2736,7 +2747,7 @@
       </c>
       <c r="E67" s="7"/>
     </row>
-    <row r="68" spans="1:5">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="9" t="s">
         <v>224</v>
       </c>
@@ -2751,7 +2762,7 @@
       </c>
       <c r="E68" s="7"/>
     </row>
-    <row r="69" spans="1:5">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="9" t="s">
         <v>225</v>
       </c>
@@ -2766,7 +2777,7 @@
       </c>
       <c r="E69" s="7"/>
     </row>
-    <row r="70" spans="1:5">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="9" t="s">
         <v>226</v>
       </c>
@@ -2781,7 +2792,7 @@
       </c>
       <c r="E70" s="7"/>
     </row>
-    <row r="71" spans="1:5">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="9" t="s">
         <v>233</v>
       </c>
@@ -2796,7 +2807,7 @@
       </c>
       <c r="E71" s="7"/>
     </row>
-    <row r="72" spans="1:5">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="9" t="s">
         <v>237</v>
       </c>
@@ -2811,7 +2822,7 @@
       </c>
       <c r="E72" s="7"/>
     </row>
-    <row r="73" spans="1:5">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="9" t="s">
         <v>239</v>
       </c>
@@ -2826,7 +2837,7 @@
       </c>
       <c r="E73" s="7"/>
     </row>
-    <row r="74" spans="1:5">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="9" t="s">
         <v>243</v>
       </c>
@@ -2841,7 +2852,7 @@
       </c>
       <c r="E74" s="7"/>
     </row>
-    <row r="75" spans="1:5" ht="30">
+    <row r="75" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" s="9" t="s">
         <v>245</v>
       </c>
@@ -2856,7 +2867,7 @@
       </c>
       <c r="E75" s="7"/>
     </row>
-    <row r="76" spans="1:5">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="9" t="s">
         <v>248</v>
       </c>
@@ -2871,7 +2882,7 @@
       </c>
       <c r="E76" s="7"/>
     </row>
-    <row r="77" spans="1:5">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="9" t="s">
         <v>256</v>
       </c>
@@ -2886,7 +2897,7 @@
       </c>
       <c r="E77" s="7"/>
     </row>
-    <row r="78" spans="1:5">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="9" t="s">
         <v>257</v>
       </c>
@@ -2901,7 +2912,7 @@
       </c>
       <c r="E78" s="7"/>
     </row>
-    <row r="79" spans="1:5">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="9" t="s">
         <v>261</v>
       </c>
@@ -2916,7 +2927,7 @@
       </c>
       <c r="E79" s="7"/>
     </row>
-    <row r="80" spans="1:5">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="9" t="s">
         <v>264</v>
       </c>
@@ -2931,7 +2942,7 @@
       </c>
       <c r="E80" s="7"/>
     </row>
-    <row r="81" spans="1:5">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="9" t="s">
         <v>267</v>
       </c>
@@ -2946,7 +2957,7 @@
       </c>
       <c r="E81" s="7"/>
     </row>
-    <row r="82" spans="1:5" ht="30">
+    <row r="82" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A82" s="9" t="s">
         <v>269</v>
       </c>
@@ -2961,7 +2972,7 @@
       </c>
       <c r="E82" s="7"/>
     </row>
-    <row r="83" spans="1:5">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="9" t="s">
         <v>274</v>
       </c>
@@ -2976,7 +2987,7 @@
       </c>
       <c r="E83" s="7"/>
     </row>
-    <row r="84" spans="1:5" ht="30">
+    <row r="84" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A84" s="9" t="s">
         <v>277</v>
       </c>
@@ -2991,7 +3002,7 @@
       </c>
       <c r="E84" s="7"/>
     </row>
-    <row r="85" spans="1:5">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="9" t="s">
         <v>279</v>
       </c>
@@ -3006,7 +3017,7 @@
       </c>
       <c r="E85" s="7"/>
     </row>
-    <row r="86" spans="1:5">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="9" t="s">
         <v>282</v>
       </c>
@@ -3021,7 +3032,7 @@
       </c>
       <c r="E86" s="7"/>
     </row>
-    <row r="87" spans="1:5">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="9" t="s">
         <v>285</v>
       </c>
@@ -3036,7 +3047,7 @@
       </c>
       <c r="E87" s="7"/>
     </row>
-    <row r="88" spans="1:5">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="9" t="s">
         <v>288</v>
       </c>
@@ -3051,7 +3062,7 @@
       </c>
       <c r="E88" s="7"/>
     </row>
-    <row r="89" spans="1:5">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="9" t="s">
         <v>291</v>
       </c>
@@ -3066,7 +3077,7 @@
       </c>
       <c r="E89" s="7"/>
     </row>
-    <row r="90" spans="1:5">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="9" t="s">
         <v>294</v>
       </c>
@@ -3081,7 +3092,7 @@
       </c>
       <c r="E90" s="7"/>
     </row>
-    <row r="91" spans="1:5">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="9" t="s">
         <v>297</v>
       </c>
@@ -3096,7 +3107,7 @@
       </c>
       <c r="E91" s="7"/>
     </row>
-    <row r="92" spans="1:5">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="9" t="s">
         <v>300</v>
       </c>
@@ -3111,7 +3122,7 @@
       </c>
       <c r="E92" s="7"/>
     </row>
-    <row r="93" spans="1:5">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="9" t="s">
         <v>303</v>
       </c>
@@ -3126,7 +3137,7 @@
       </c>
       <c r="E93" s="7"/>
     </row>
-    <row r="94" spans="1:5">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="9" t="s">
         <v>306</v>
       </c>
@@ -3141,7 +3152,7 @@
       </c>
       <c r="E94" s="7"/>
     </row>
-    <row r="95" spans="1:5">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="9" t="s">
         <v>309</v>
       </c>
@@ -3156,7 +3167,7 @@
       </c>
       <c r="E95" s="7"/>
     </row>
-    <row r="96" spans="1:5">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="9" t="s">
         <v>314</v>
       </c>
@@ -3171,7 +3182,7 @@
       </c>
       <c r="E96" s="7"/>
     </row>
-    <row r="97" spans="1:5">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="9" t="s">
         <v>315</v>
       </c>
@@ -3186,7 +3197,7 @@
       </c>
       <c r="E97" s="7"/>
     </row>
-    <row r="98" spans="1:5">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="9" t="s">
         <v>319</v>
       </c>
@@ -3201,7 +3212,7 @@
       </c>
       <c r="E98" s="7"/>
     </row>
-    <row r="99" spans="1:5">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="9" t="s">
         <v>321</v>
       </c>
@@ -3216,7 +3227,7 @@
       </c>
       <c r="E99" s="7"/>
     </row>
-    <row r="100" spans="1:5">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="9" t="s">
         <v>322</v>
       </c>
@@ -3231,7 +3242,7 @@
       </c>
       <c r="E100" s="7"/>
     </row>
-    <row r="101" spans="1:5" ht="30">
+    <row r="101" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A101" s="9" t="s">
         <v>323</v>
       </c>
@@ -3246,7 +3257,7 @@
       </c>
       <c r="E101" s="7"/>
     </row>
-    <row r="102" spans="1:5">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="9" t="s">
         <v>328</v>
       </c>
@@ -3261,7 +3272,7 @@
       </c>
       <c r="E102" s="7"/>
     </row>
-    <row r="103" spans="1:5">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="9" t="s">
         <v>333</v>
       </c>
@@ -3276,7 +3287,7 @@
       </c>
       <c r="E103" s="7"/>
     </row>
-    <row r="104" spans="1:5">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="9" t="s">
         <v>336</v>
       </c>
@@ -3291,7 +3302,7 @@
       </c>
       <c r="E104" s="7"/>
     </row>
-    <row r="105" spans="1:5">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="9" t="s">
         <v>337</v>
       </c>
@@ -3306,7 +3317,7 @@
       </c>
       <c r="E105" s="7"/>
     </row>
-    <row r="106" spans="1:5">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="9" t="s">
         <v>342</v>
       </c>
@@ -3321,7 +3332,7 @@
       </c>
       <c r="E106" s="7"/>
     </row>
-    <row r="107" spans="1:5">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="9" t="s">
         <v>345</v>
       </c>
@@ -3336,7 +3347,7 @@
       </c>
       <c r="E107" s="7"/>
     </row>
-    <row r="108" spans="1:5">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="9" t="s">
         <v>350</v>
       </c>
@@ -3351,7 +3362,7 @@
       </c>
       <c r="E108" s="7"/>
     </row>
-    <row r="109" spans="1:5" ht="30">
+    <row r="109" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A109" s="9" t="s">
         <v>351</v>
       </c>
@@ -3366,7 +3377,7 @@
       </c>
       <c r="E109" s="7"/>
     </row>
-    <row r="110" spans="1:5">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="9" t="s">
         <v>354</v>
       </c>
@@ -3381,7 +3392,7 @@
       </c>
       <c r="E110" s="7"/>
     </row>
-    <row r="111" spans="1:5">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="9" t="s">
         <v>357</v>
       </c>
@@ -3396,7 +3407,7 @@
       </c>
       <c r="E111" s="7"/>
     </row>
-    <row r="112" spans="1:5">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="9" t="s">
         <v>361</v>
       </c>
@@ -3411,7 +3422,7 @@
       </c>
       <c r="E112" s="7"/>
     </row>
-    <row r="113" spans="1:5">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="17" t="s">
         <v>363</v>
       </c>
@@ -3426,7 +3437,7 @@
       </c>
       <c r="E113" s="19"/>
     </row>
-    <row r="114" spans="1:5" ht="30">
+    <row r="114" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A114" s="9" t="s">
         <v>366</v>
       </c>
@@ -3441,7 +3452,7 @@
       </c>
       <c r="E114" s="7"/>
     </row>
-    <row r="115" spans="1:5">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="9" t="s">
         <v>369</v>
       </c>
@@ -3456,7 +3467,7 @@
       </c>
       <c r="E115" s="7"/>
     </row>
-    <row r="116" spans="1:5">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="9" t="s">
         <v>370</v>
       </c>
@@ -3471,7 +3482,7 @@
       </c>
       <c r="E116" s="7"/>
     </row>
-    <row r="117" spans="1:5">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" s="9" t="s">
         <v>371</v>
       </c>
@@ -3486,7 +3497,7 @@
       </c>
       <c r="E117" s="7"/>
     </row>
-    <row r="118" spans="1:5">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" s="9" t="s">
         <v>378</v>
       </c>
@@ -3501,7 +3512,7 @@
       </c>
       <c r="E118" s="7"/>
     </row>
-    <row r="119" spans="1:5">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" s="9" t="s">
         <v>381</v>
       </c>
@@ -3516,7 +3527,7 @@
       </c>
       <c r="E119" s="7"/>
     </row>
-    <row r="120" spans="1:5">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" s="9" t="s">
         <v>384</v>
       </c>
@@ -3531,7 +3542,7 @@
       </c>
       <c r="E120" s="7"/>
     </row>
-    <row r="121" spans="1:5">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="9" t="s">
         <v>387</v>
       </c>
@@ -3546,7 +3557,7 @@
       </c>
       <c r="E121" s="7"/>
     </row>
-    <row r="122" spans="1:5">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" s="7" t="s">
         <v>390</v>
       </c>
@@ -3561,7 +3572,7 @@
       </c>
       <c r="E122" s="7"/>
     </row>
-    <row r="123" spans="1:5">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" s="7" t="s">
         <v>393</v>
       </c>
@@ -3576,7 +3587,7 @@
       </c>
       <c r="E123" s="7"/>
     </row>
-    <row r="124" spans="1:5">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" s="7" t="s">
         <v>396</v>
       </c>
@@ -3590,6 +3601,21 @@
         <v>5</v>
       </c>
       <c r="E124" s="7"/>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A125" s="9" t="s">
+        <v>399</v>
+      </c>
+      <c r="B125" s="7" t="s">
+        <v>400</v>
+      </c>
+      <c r="C125" s="7" t="s">
+        <v>401</v>
+      </c>
+      <c r="D125" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E125" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -3602,14 +3628,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView topLeftCell="A10" zoomScale="80" workbookViewId="0">
       <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
@@ -3617,7 +3643,7 @@
     <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>35</v>
       </c>
@@ -3631,7 +3657,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>37</v>
       </c>
@@ -3643,7 +3669,7 @@
       </c>
       <c r="D2" s="7"/>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>38</v>
       </c>
@@ -3655,7 +3681,7 @@
       </c>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>39</v>
       </c>
@@ -3667,7 +3693,7 @@
       </c>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>40</v>
       </c>
@@ -3679,7 +3705,7 @@
       </c>
       <c r="D5" s="7"/>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>41</v>
       </c>
@@ -3691,7 +3717,7 @@
       </c>
       <c r="D6" s="7"/>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>42</v>
       </c>
@@ -3703,7 +3729,7 @@
       </c>
       <c r="D7" s="7"/>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>43</v>
       </c>
@@ -3715,7 +3741,7 @@
       </c>
       <c r="D8" s="7"/>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>44</v>
       </c>
@@ -3727,7 +3753,7 @@
       </c>
       <c r="D9" s="7"/>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>45</v>
       </c>
@@ -3739,7 +3765,7 @@
       </c>
       <c r="D10" s="7"/>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>46</v>
       </c>
@@ -3751,7 +3777,7 @@
       </c>
       <c r="D11" s="7"/>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>48</v>
       </c>
@@ -3763,7 +3789,7 @@
       </c>
       <c r="D12" s="7"/>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>49</v>
       </c>
@@ -3775,7 +3801,7 @@
       </c>
       <c r="D13" s="7"/>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>50</v>
       </c>
@@ -3787,7 +3813,7 @@
       </c>
       <c r="D14" s="7"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>51</v>
       </c>
@@ -3799,7 +3825,7 @@
       </c>
       <c r="D15" s="7"/>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>52</v>
       </c>
@@ -3811,7 +3837,7 @@
       </c>
       <c r="D16" s="7"/>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>53</v>
       </c>
@@ -3823,7 +3849,7 @@
       </c>
       <c r="D17" s="7"/>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>54</v>
       </c>
@@ -3835,7 +3861,7 @@
       </c>
       <c r="D18" s="7"/>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>55</v>
       </c>
@@ -3847,7 +3873,7 @@
       </c>
       <c r="D19" s="7"/>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>56</v>
       </c>
@@ -3859,7 +3885,7 @@
       </c>
       <c r="D20" s="7"/>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>57</v>
       </c>
@@ -3871,7 +3897,7 @@
       </c>
       <c r="D21" s="7"/>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>58</v>
       </c>
@@ -3883,7 +3909,7 @@
       </c>
       <c r="D22" s="7"/>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>59</v>
       </c>
@@ -3895,7 +3921,7 @@
       </c>
       <c r="D23" s="7"/>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>60</v>
       </c>
@@ -3907,7 +3933,7 @@
       </c>
       <c r="D24" s="7"/>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>61</v>
       </c>
@@ -3919,7 +3945,7 @@
       </c>
       <c r="D25" s="7"/>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>47</v>
       </c>
@@ -3938,14 +3964,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A19" sqref="A19:XFD19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
@@ -3953,7 +3979,7 @@
     <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>35</v>
       </c>
@@ -3967,7 +3993,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>37</v>
       </c>
@@ -3979,7 +4005,7 @@
       </c>
       <c r="D2" s="7"/>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>38</v>
       </c>
@@ -3991,7 +4017,7 @@
       </c>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>39</v>
       </c>
@@ -4003,7 +4029,7 @@
       </c>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>40</v>
       </c>
@@ -4015,7 +4041,7 @@
       </c>
       <c r="D5" s="7"/>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>41</v>
       </c>
@@ -4027,7 +4053,7 @@
       </c>
       <c r="D6" s="7"/>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>42</v>
       </c>
@@ -4039,7 +4065,7 @@
       </c>
       <c r="D7" s="7"/>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>43</v>
       </c>
@@ -4051,7 +4077,7 @@
       </c>
       <c r="D8" s="7"/>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>44</v>
       </c>
@@ -4063,7 +4089,7 @@
       </c>
       <c r="D9" s="7"/>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>45</v>
       </c>
@@ -4075,7 +4101,7 @@
       </c>
       <c r="D10" s="7"/>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>46</v>
       </c>
@@ -4087,7 +4113,7 @@
       </c>
       <c r="D11" s="7"/>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>47</v>
       </c>
@@ -4099,7 +4125,7 @@
       </c>
       <c r="D12" s="7"/>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>48</v>
       </c>
@@ -4111,7 +4137,7 @@
       </c>
       <c r="D13" s="7"/>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>49</v>
       </c>
@@ -4123,7 +4149,7 @@
       </c>
       <c r="D14" s="7"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>50</v>
       </c>
@@ -4135,7 +4161,7 @@
       </c>
       <c r="D15" s="7"/>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>51</v>
       </c>
@@ -4147,7 +4173,7 @@
       </c>
       <c r="D16" s="7"/>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>52</v>
       </c>
@@ -4159,7 +4185,7 @@
       </c>
       <c r="D17" s="7"/>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>53</v>
       </c>
@@ -4171,7 +4197,7 @@
       </c>
       <c r="D18" s="7"/>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>54</v>
       </c>
@@ -4183,7 +4209,7 @@
       </c>
       <c r="D19" s="7"/>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>55</v>
       </c>
@@ -4195,7 +4221,7 @@
       </c>
       <c r="D20" s="7"/>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>56</v>
       </c>
@@ -4207,7 +4233,7 @@
       </c>
       <c r="D21" s="7"/>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>57</v>
       </c>
@@ -4219,7 +4245,7 @@
       </c>
       <c r="D22" s="7"/>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>58</v>
       </c>
@@ -4231,7 +4257,7 @@
       </c>
       <c r="D23" s="7"/>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>59</v>
       </c>
@@ -4243,7 +4269,7 @@
       </c>
       <c r="D24" s="7"/>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>60</v>
       </c>
@@ -4255,7 +4281,7 @@
       </c>
       <c r="D25" s="7"/>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>61</v>
       </c>

</xml_diff>

<commit_message>
WAT New Test script added WAT157,158,159
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/WAT.xlsx
+++ b/src/test/resources/xls/WAT.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13305" windowHeight="2415"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="402">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="671" uniqueCount="411">
   <si>
     <t>TCID</t>
   </si>
@@ -1223,13 +1223,40 @@
   </si>
   <si>
     <t>Verify that User should be able to ignore Org dropdown and proceed with author search</t>
+  </si>
+  <si>
+    <t>WAT157</t>
+  </si>
+  <si>
+    <t>WAT-1210</t>
+  </si>
+  <si>
+    <t>Verify that ‘Select All’ option should not display when quantity of search results of an author morethan 50.</t>
+  </si>
+  <si>
+    <t>WAT158</t>
+  </si>
+  <si>
+    <t>WAT-1211</t>
+  </si>
+  <si>
+    <t>Verify that ‘Select All’ option should display when quantity of search results of an author lessthan 50.</t>
+  </si>
+  <si>
+    <t>WAT159</t>
+  </si>
+  <si>
+    <t>WAT-1333</t>
+  </si>
+  <si>
+    <t>Verify that ‘Select All’ option should not display when quantity of search results of an author Only 1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1481,7 +1508,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1513,10 +1540,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1548,7 +1574,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1724,14 +1749,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E125"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A98" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C128" sqref="C128"/>
+    <sheetView tabSelected="1" topLeftCell="A101" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A126" sqref="A126:E128"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="41" bestFit="1" customWidth="1" collapsed="1"/>
@@ -1740,7 +1765,7 @@
     <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1757,7 +1782,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -1772,7 +1797,7 @@
       </c>
       <c r="E2" s="4"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -1787,7 +1812,7 @@
       </c>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" s="7" t="s">
         <v>11</v>
       </c>
@@ -1802,7 +1827,7 @@
       </c>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" s="7" t="s">
         <v>12</v>
       </c>
@@ -1817,7 +1842,7 @@
       </c>
       <c r="E5" s="7"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" s="7" t="s">
         <v>14</v>
       </c>
@@ -1832,7 +1857,7 @@
       </c>
       <c r="E6" s="7"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" s="7" t="s">
         <v>17</v>
       </c>
@@ -1847,7 +1872,7 @@
       </c>
       <c r="E7" s="7"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" s="7" t="s">
         <v>20</v>
       </c>
@@ -1862,7 +1887,7 @@
       </c>
       <c r="E8" s="7"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" s="7" t="s">
         <v>22</v>
       </c>
@@ -1877,7 +1902,7 @@
       </c>
       <c r="E9" s="7"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10" s="7" t="s">
         <v>23</v>
       </c>
@@ -1892,7 +1917,7 @@
       </c>
       <c r="E10" s="7"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11" s="7" t="s">
         <v>24</v>
       </c>
@@ -1907,7 +1932,7 @@
       </c>
       <c r="E11" s="7"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12" s="7" t="s">
         <v>25</v>
       </c>
@@ -1922,7 +1947,7 @@
       </c>
       <c r="E12" s="7"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13" s="7" t="s">
         <v>62</v>
       </c>
@@ -1937,7 +1962,7 @@
       </c>
       <c r="E13" s="7"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="A14" s="7" t="s">
         <v>63</v>
       </c>
@@ -1952,7 +1977,7 @@
       </c>
       <c r="E14" s="7"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="A15" s="7" t="s">
         <v>64</v>
       </c>
@@ -1967,7 +1992,7 @@
       </c>
       <c r="E15" s="7"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="A16" s="7" t="s">
         <v>65</v>
       </c>
@@ -1982,7 +2007,7 @@
       </c>
       <c r="E16" s="7"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5">
       <c r="A17" s="7" t="s">
         <v>74</v>
       </c>
@@ -1997,7 +2022,7 @@
       </c>
       <c r="E17" s="7"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5">
       <c r="A18" s="7" t="s">
         <v>75</v>
       </c>
@@ -2012,7 +2037,7 @@
       </c>
       <c r="E18" s="7"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5">
       <c r="A19" s="7" t="s">
         <v>79</v>
       </c>
@@ -2027,7 +2052,7 @@
       </c>
       <c r="E19" s="7"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5">
       <c r="A20" s="7" t="s">
         <v>81</v>
       </c>
@@ -2042,7 +2067,7 @@
       </c>
       <c r="E20" s="7"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5">
       <c r="A21" s="7" t="s">
         <v>82</v>
       </c>
@@ -2057,7 +2082,7 @@
       </c>
       <c r="E21" s="7"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5">
       <c r="A22" s="7" t="s">
         <v>88</v>
       </c>
@@ -2072,7 +2097,7 @@
       </c>
       <c r="E22" s="7"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5">
       <c r="A23" s="7" t="s">
         <v>90</v>
       </c>
@@ -2087,7 +2112,7 @@
       </c>
       <c r="E23" s="7"/>
     </row>
-    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="30">
       <c r="A24" s="9" t="s">
         <v>94</v>
       </c>
@@ -2102,7 +2127,7 @@
       </c>
       <c r="E24" s="7"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5">
       <c r="A25" s="9" t="s">
         <v>96</v>
       </c>
@@ -2117,7 +2142,7 @@
       </c>
       <c r="E25" s="7"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5">
       <c r="A26" s="9" t="s">
         <v>98</v>
       </c>
@@ -2132,7 +2157,7 @@
       </c>
       <c r="E26" s="7"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5">
       <c r="A27" s="9" t="s">
         <v>102</v>
       </c>
@@ -2147,7 +2172,7 @@
       </c>
       <c r="E27" s="7"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5">
       <c r="A28" s="9" t="s">
         <v>105</v>
       </c>
@@ -2162,7 +2187,7 @@
       </c>
       <c r="E28" s="7"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5">
       <c r="A29" s="9" t="s">
         <v>108</v>
       </c>
@@ -2177,7 +2202,7 @@
       </c>
       <c r="E29" s="7"/>
     </row>
-    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" ht="30">
       <c r="A30" s="9" t="s">
         <v>110</v>
       </c>
@@ -2192,7 +2217,7 @@
       </c>
       <c r="E30" s="7"/>
     </row>
-    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" ht="30">
       <c r="A31" s="9" t="s">
         <v>114</v>
       </c>
@@ -2207,7 +2232,7 @@
       </c>
       <c r="E31" s="7"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5">
       <c r="A32" s="9" t="s">
         <v>119</v>
       </c>
@@ -2222,7 +2247,7 @@
       </c>
       <c r="E32" s="7"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5">
       <c r="A33" s="9" t="s">
         <v>120</v>
       </c>
@@ -2237,7 +2262,7 @@
       </c>
       <c r="E33" s="7"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5">
       <c r="A34" s="9" t="s">
         <v>125</v>
       </c>
@@ -2252,7 +2277,7 @@
       </c>
       <c r="E34" s="7"/>
     </row>
-    <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" ht="30">
       <c r="A35" s="9" t="s">
         <v>128</v>
       </c>
@@ -2267,7 +2292,7 @@
       </c>
       <c r="E35" s="7"/>
     </row>
-    <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" ht="30">
       <c r="A36" s="9" t="s">
         <v>131</v>
       </c>
@@ -2282,7 +2307,7 @@
       </c>
       <c r="E36" s="7"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5">
       <c r="A37" s="9" t="s">
         <v>134</v>
       </c>
@@ -2297,7 +2322,7 @@
       </c>
       <c r="E37" s="7"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5">
       <c r="A38" s="9" t="s">
         <v>137</v>
       </c>
@@ -2312,7 +2337,7 @@
       </c>
       <c r="E38" s="7"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5">
       <c r="A39" s="9" t="s">
         <v>140</v>
       </c>
@@ -2327,7 +2352,7 @@
       </c>
       <c r="E39" s="7"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5">
       <c r="A40" s="9" t="s">
         <v>143</v>
       </c>
@@ -2342,7 +2367,7 @@
       </c>
       <c r="E40" s="7"/>
     </row>
-    <row r="41" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" ht="30">
       <c r="A41" s="9" t="s">
         <v>145</v>
       </c>
@@ -2357,7 +2382,7 @@
       </c>
       <c r="E41" s="7"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5">
       <c r="A42" s="9" t="s">
         <v>147</v>
       </c>
@@ -2372,7 +2397,7 @@
       </c>
       <c r="E42" s="7"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5">
       <c r="A43" s="9" t="s">
         <v>150</v>
       </c>
@@ -2387,7 +2412,7 @@
       </c>
       <c r="E43" s="7"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5">
       <c r="A44" s="9" t="s">
         <v>153</v>
       </c>
@@ -2402,7 +2427,7 @@
       </c>
       <c r="E44" s="7"/>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5">
       <c r="A45" s="9" t="s">
         <v>155</v>
       </c>
@@ -2417,7 +2442,7 @@
       </c>
       <c r="E45" s="7"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5">
       <c r="A46" s="12" t="s">
         <v>158</v>
       </c>
@@ -2432,7 +2457,7 @@
       </c>
       <c r="E46" s="7"/>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5">
       <c r="A47" s="12" t="s">
         <v>159</v>
       </c>
@@ -2447,7 +2472,7 @@
       </c>
       <c r="E47" s="7"/>
     </row>
-    <row r="48" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" ht="30">
       <c r="A48" s="12" t="s">
         <v>160</v>
       </c>
@@ -2462,7 +2487,7 @@
       </c>
       <c r="E48" s="7"/>
     </row>
-    <row r="49" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" ht="30">
       <c r="A49" s="12" t="s">
         <v>161</v>
       </c>
@@ -2477,7 +2502,7 @@
       </c>
       <c r="E49" s="7"/>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5">
       <c r="A50" s="12" t="s">
         <v>164</v>
       </c>
@@ -2492,7 +2517,7 @@
       </c>
       <c r="E50" s="7"/>
     </row>
-    <row r="51" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" ht="30">
       <c r="A51" s="9" t="s">
         <v>173</v>
       </c>
@@ -2507,7 +2532,7 @@
       </c>
       <c r="E51" s="7"/>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5">
       <c r="A52" s="9" t="s">
         <v>174</v>
       </c>
@@ -2522,7 +2547,7 @@
       </c>
       <c r="E52" s="7"/>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5">
       <c r="A53" s="9" t="s">
         <v>179</v>
       </c>
@@ -2537,7 +2562,7 @@
       </c>
       <c r="E53" s="7"/>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5">
       <c r="A54" s="9" t="s">
         <v>180</v>
       </c>
@@ -2552,7 +2577,7 @@
       </c>
       <c r="E54" s="7"/>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5">
       <c r="A55" s="9" t="s">
         <v>185</v>
       </c>
@@ -2567,7 +2592,7 @@
       </c>
       <c r="E55" s="7"/>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5">
       <c r="A56" s="9" t="s">
         <v>188</v>
       </c>
@@ -2582,7 +2607,7 @@
       </c>
       <c r="E56" s="7"/>
     </row>
-    <row r="57" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" ht="30">
       <c r="A57" s="9" t="s">
         <v>191</v>
       </c>
@@ -2597,7 +2622,7 @@
       </c>
       <c r="E57" s="7"/>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5">
       <c r="A58" s="9" t="s">
         <v>194</v>
       </c>
@@ -2612,7 +2637,7 @@
       </c>
       <c r="E58" s="7"/>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5">
       <c r="A59" s="7" t="s">
         <v>196</v>
       </c>
@@ -2627,7 +2652,7 @@
       </c>
       <c r="E59" s="7"/>
     </row>
-    <row r="60" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" ht="45">
       <c r="A60" s="7" t="s">
         <v>199</v>
       </c>
@@ -2642,7 +2667,7 @@
       </c>
       <c r="E60" s="7"/>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5">
       <c r="A61" s="9" t="s">
         <v>202</v>
       </c>
@@ -2657,7 +2682,7 @@
       </c>
       <c r="E61" s="7"/>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5">
       <c r="A62" s="9" t="s">
         <v>204</v>
       </c>
@@ -2672,7 +2697,7 @@
       </c>
       <c r="E62" s="7"/>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5">
       <c r="A63" s="9" t="s">
         <v>206</v>
       </c>
@@ -2687,7 +2712,7 @@
       </c>
       <c r="E63" s="7"/>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5">
       <c r="A64" s="9" t="s">
         <v>208</v>
       </c>
@@ -2702,7 +2727,7 @@
       </c>
       <c r="E64" s="7"/>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5">
       <c r="A65" s="9" t="s">
         <v>217</v>
       </c>
@@ -2717,7 +2742,7 @@
       </c>
       <c r="E65" s="7"/>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5">
       <c r="A66" s="9" t="s">
         <v>218</v>
       </c>
@@ -2732,7 +2757,7 @@
       </c>
       <c r="E66" s="7"/>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5">
       <c r="A67" s="9" t="s">
         <v>223</v>
       </c>
@@ -2747,7 +2772,7 @@
       </c>
       <c r="E67" s="7"/>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5">
       <c r="A68" s="9" t="s">
         <v>224</v>
       </c>
@@ -2762,7 +2787,7 @@
       </c>
       <c r="E68" s="7"/>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5">
       <c r="A69" s="9" t="s">
         <v>225</v>
       </c>
@@ -2777,7 +2802,7 @@
       </c>
       <c r="E69" s="7"/>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5">
       <c r="A70" s="9" t="s">
         <v>226</v>
       </c>
@@ -2792,7 +2817,7 @@
       </c>
       <c r="E70" s="7"/>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5">
       <c r="A71" s="9" t="s">
         <v>233</v>
       </c>
@@ -2807,7 +2832,7 @@
       </c>
       <c r="E71" s="7"/>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5">
       <c r="A72" s="9" t="s">
         <v>237</v>
       </c>
@@ -2822,7 +2847,7 @@
       </c>
       <c r="E72" s="7"/>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5">
       <c r="A73" s="9" t="s">
         <v>239</v>
       </c>
@@ -2837,7 +2862,7 @@
       </c>
       <c r="E73" s="7"/>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5">
       <c r="A74" s="9" t="s">
         <v>243</v>
       </c>
@@ -2852,7 +2877,7 @@
       </c>
       <c r="E74" s="7"/>
     </row>
-    <row r="75" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" ht="30">
       <c r="A75" s="9" t="s">
         <v>245</v>
       </c>
@@ -2867,7 +2892,7 @@
       </c>
       <c r="E75" s="7"/>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5">
       <c r="A76" s="9" t="s">
         <v>248</v>
       </c>
@@ -2882,7 +2907,7 @@
       </c>
       <c r="E76" s="7"/>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5">
       <c r="A77" s="9" t="s">
         <v>256</v>
       </c>
@@ -2897,7 +2922,7 @@
       </c>
       <c r="E77" s="7"/>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5">
       <c r="A78" s="9" t="s">
         <v>257</v>
       </c>
@@ -2912,7 +2937,7 @@
       </c>
       <c r="E78" s="7"/>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5">
       <c r="A79" s="9" t="s">
         <v>261</v>
       </c>
@@ -2927,7 +2952,7 @@
       </c>
       <c r="E79" s="7"/>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5">
       <c r="A80" s="9" t="s">
         <v>264</v>
       </c>
@@ -2942,7 +2967,7 @@
       </c>
       <c r="E80" s="7"/>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5">
       <c r="A81" s="9" t="s">
         <v>267</v>
       </c>
@@ -2957,7 +2982,7 @@
       </c>
       <c r="E81" s="7"/>
     </row>
-    <row r="82" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" ht="30">
       <c r="A82" s="9" t="s">
         <v>269</v>
       </c>
@@ -2972,7 +2997,7 @@
       </c>
       <c r="E82" s="7"/>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5">
       <c r="A83" s="9" t="s">
         <v>274</v>
       </c>
@@ -2987,7 +3012,7 @@
       </c>
       <c r="E83" s="7"/>
     </row>
-    <row r="84" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" ht="30">
       <c r="A84" s="9" t="s">
         <v>277</v>
       </c>
@@ -3002,7 +3027,7 @@
       </c>
       <c r="E84" s="7"/>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5">
       <c r="A85" s="9" t="s">
         <v>279</v>
       </c>
@@ -3017,7 +3042,7 @@
       </c>
       <c r="E85" s="7"/>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5">
       <c r="A86" s="9" t="s">
         <v>282</v>
       </c>
@@ -3032,7 +3057,7 @@
       </c>
       <c r="E86" s="7"/>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5">
       <c r="A87" s="9" t="s">
         <v>285</v>
       </c>
@@ -3047,7 +3072,7 @@
       </c>
       <c r="E87" s="7"/>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5">
       <c r="A88" s="9" t="s">
         <v>288</v>
       </c>
@@ -3062,7 +3087,7 @@
       </c>
       <c r="E88" s="7"/>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5">
       <c r="A89" s="9" t="s">
         <v>291</v>
       </c>
@@ -3077,7 +3102,7 @@
       </c>
       <c r="E89" s="7"/>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5">
       <c r="A90" s="9" t="s">
         <v>294</v>
       </c>
@@ -3092,7 +3117,7 @@
       </c>
       <c r="E90" s="7"/>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5">
       <c r="A91" s="9" t="s">
         <v>297</v>
       </c>
@@ -3107,7 +3132,7 @@
       </c>
       <c r="E91" s="7"/>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5">
       <c r="A92" s="9" t="s">
         <v>300</v>
       </c>
@@ -3122,7 +3147,7 @@
       </c>
       <c r="E92" s="7"/>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5">
       <c r="A93" s="9" t="s">
         <v>303</v>
       </c>
@@ -3137,7 +3162,7 @@
       </c>
       <c r="E93" s="7"/>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5">
       <c r="A94" s="9" t="s">
         <v>306</v>
       </c>
@@ -3152,7 +3177,7 @@
       </c>
       <c r="E94" s="7"/>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5">
       <c r="A95" s="9" t="s">
         <v>309</v>
       </c>
@@ -3167,7 +3192,7 @@
       </c>
       <c r="E95" s="7"/>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5">
       <c r="A96" s="9" t="s">
         <v>314</v>
       </c>
@@ -3182,7 +3207,7 @@
       </c>
       <c r="E96" s="7"/>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5">
       <c r="A97" s="9" t="s">
         <v>315</v>
       </c>
@@ -3197,7 +3222,7 @@
       </c>
       <c r="E97" s="7"/>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5">
       <c r="A98" s="9" t="s">
         <v>319</v>
       </c>
@@ -3212,7 +3237,7 @@
       </c>
       <c r="E98" s="7"/>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5">
       <c r="A99" s="9" t="s">
         <v>321</v>
       </c>
@@ -3227,7 +3252,7 @@
       </c>
       <c r="E99" s="7"/>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5">
       <c r="A100" s="9" t="s">
         <v>322</v>
       </c>
@@ -3242,7 +3267,7 @@
       </c>
       <c r="E100" s="7"/>
     </row>
-    <row r="101" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" ht="30">
       <c r="A101" s="9" t="s">
         <v>323</v>
       </c>
@@ -3257,7 +3282,7 @@
       </c>
       <c r="E101" s="7"/>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5">
       <c r="A102" s="9" t="s">
         <v>328</v>
       </c>
@@ -3272,7 +3297,7 @@
       </c>
       <c r="E102" s="7"/>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5">
       <c r="A103" s="9" t="s">
         <v>333</v>
       </c>
@@ -3287,7 +3312,7 @@
       </c>
       <c r="E103" s="7"/>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5">
       <c r="A104" s="9" t="s">
         <v>336</v>
       </c>
@@ -3302,7 +3327,7 @@
       </c>
       <c r="E104" s="7"/>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5">
       <c r="A105" s="9" t="s">
         <v>337</v>
       </c>
@@ -3317,7 +3342,7 @@
       </c>
       <c r="E105" s="7"/>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5">
       <c r="A106" s="9" t="s">
         <v>342</v>
       </c>
@@ -3332,7 +3357,7 @@
       </c>
       <c r="E106" s="7"/>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5">
       <c r="A107" s="9" t="s">
         <v>345</v>
       </c>
@@ -3347,7 +3372,7 @@
       </c>
       <c r="E107" s="7"/>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5">
       <c r="A108" s="9" t="s">
         <v>350</v>
       </c>
@@ -3362,7 +3387,7 @@
       </c>
       <c r="E108" s="7"/>
     </row>
-    <row r="109" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" ht="30">
       <c r="A109" s="9" t="s">
         <v>351</v>
       </c>
@@ -3377,7 +3402,7 @@
       </c>
       <c r="E109" s="7"/>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5">
       <c r="A110" s="9" t="s">
         <v>354</v>
       </c>
@@ -3392,7 +3417,7 @@
       </c>
       <c r="E110" s="7"/>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5">
       <c r="A111" s="9" t="s">
         <v>357</v>
       </c>
@@ -3407,7 +3432,7 @@
       </c>
       <c r="E111" s="7"/>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5">
       <c r="A112" s="9" t="s">
         <v>361</v>
       </c>
@@ -3422,7 +3447,7 @@
       </c>
       <c r="E112" s="7"/>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5">
       <c r="A113" s="17" t="s">
         <v>363</v>
       </c>
@@ -3437,7 +3462,7 @@
       </c>
       <c r="E113" s="19"/>
     </row>
-    <row r="114" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" ht="30">
       <c r="A114" s="9" t="s">
         <v>366</v>
       </c>
@@ -3452,7 +3477,7 @@
       </c>
       <c r="E114" s="7"/>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5">
       <c r="A115" s="9" t="s">
         <v>369</v>
       </c>
@@ -3467,7 +3492,7 @@
       </c>
       <c r="E115" s="7"/>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5">
       <c r="A116" s="9" t="s">
         <v>370</v>
       </c>
@@ -3482,7 +3507,7 @@
       </c>
       <c r="E116" s="7"/>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5">
       <c r="A117" s="9" t="s">
         <v>371</v>
       </c>
@@ -3497,7 +3522,7 @@
       </c>
       <c r="E117" s="7"/>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5">
       <c r="A118" s="9" t="s">
         <v>378</v>
       </c>
@@ -3512,7 +3537,7 @@
       </c>
       <c r="E118" s="7"/>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5">
       <c r="A119" s="9" t="s">
         <v>381</v>
       </c>
@@ -3527,7 +3552,7 @@
       </c>
       <c r="E119" s="7"/>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5">
       <c r="A120" s="9" t="s">
         <v>384</v>
       </c>
@@ -3542,7 +3567,7 @@
       </c>
       <c r="E120" s="7"/>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5">
       <c r="A121" s="9" t="s">
         <v>387</v>
       </c>
@@ -3557,7 +3582,7 @@
       </c>
       <c r="E121" s="7"/>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5">
       <c r="A122" s="7" t="s">
         <v>390</v>
       </c>
@@ -3572,7 +3597,7 @@
       </c>
       <c r="E122" s="7"/>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5">
       <c r="A123" s="7" t="s">
         <v>393</v>
       </c>
@@ -3587,7 +3612,7 @@
       </c>
       <c r="E123" s="7"/>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5">
       <c r="A124" s="7" t="s">
         <v>396</v>
       </c>
@@ -3602,7 +3627,7 @@
       </c>
       <c r="E124" s="7"/>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5">
       <c r="A125" s="9" t="s">
         <v>399</v>
       </c>
@@ -3616,6 +3641,51 @@
         <v>5</v>
       </c>
       <c r="E125" s="7"/>
+    </row>
+    <row r="126" spans="1:5">
+      <c r="A126" s="7" t="s">
+        <v>402</v>
+      </c>
+      <c r="B126" s="7" t="s">
+        <v>403</v>
+      </c>
+      <c r="C126" s="7" t="s">
+        <v>404</v>
+      </c>
+      <c r="D126" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E126" s="7"/>
+    </row>
+    <row r="127" spans="1:5">
+      <c r="A127" s="7" t="s">
+        <v>405</v>
+      </c>
+      <c r="B127" s="7" t="s">
+        <v>406</v>
+      </c>
+      <c r="C127" s="7" t="s">
+        <v>407</v>
+      </c>
+      <c r="D127" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E127" s="7"/>
+    </row>
+    <row r="128" spans="1:5">
+      <c r="A128" s="7" t="s">
+        <v>408</v>
+      </c>
+      <c r="B128" s="7" t="s">
+        <v>409</v>
+      </c>
+      <c r="C128" s="7" t="s">
+        <v>410</v>
+      </c>
+      <c r="D128" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E128" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -3628,14 +3698,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView topLeftCell="A10" zoomScale="80" workbookViewId="0">
       <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
@@ -3643,7 +3713,7 @@
     <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="10" t="s">
         <v>35</v>
       </c>
@@ -3657,7 +3727,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="7" t="s">
         <v>37</v>
       </c>
@@ -3669,7 +3739,7 @@
       </c>
       <c r="D2" s="7"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="7" t="s">
         <v>38</v>
       </c>
@@ -3681,7 +3751,7 @@
       </c>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="7" t="s">
         <v>39</v>
       </c>
@@ -3693,7 +3763,7 @@
       </c>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" s="7" t="s">
         <v>40</v>
       </c>
@@ -3705,7 +3775,7 @@
       </c>
       <c r="D5" s="7"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" s="7" t="s">
         <v>41</v>
       </c>
@@ -3717,7 +3787,7 @@
       </c>
       <c r="D6" s="7"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="7" t="s">
         <v>42</v>
       </c>
@@ -3729,7 +3799,7 @@
       </c>
       <c r="D7" s="7"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="7" t="s">
         <v>43</v>
       </c>
@@ -3741,7 +3811,7 @@
       </c>
       <c r="D8" s="7"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="7" t="s">
         <v>44</v>
       </c>
@@ -3753,7 +3823,7 @@
       </c>
       <c r="D9" s="7"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="7" t="s">
         <v>45</v>
       </c>
@@ -3765,7 +3835,7 @@
       </c>
       <c r="D10" s="7"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11" s="7" t="s">
         <v>46</v>
       </c>
@@ -3777,7 +3847,7 @@
       </c>
       <c r="D11" s="7"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="A12" s="7" t="s">
         <v>48</v>
       </c>
@@ -3789,7 +3859,7 @@
       </c>
       <c r="D12" s="7"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="A13" s="7" t="s">
         <v>49</v>
       </c>
@@ -3801,7 +3871,7 @@
       </c>
       <c r="D13" s="7"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="A14" s="7" t="s">
         <v>50</v>
       </c>
@@ -3813,7 +3883,7 @@
       </c>
       <c r="D14" s="7"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="A15" s="7" t="s">
         <v>51</v>
       </c>
@@ -3825,7 +3895,7 @@
       </c>
       <c r="D15" s="7"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="A16" s="7" t="s">
         <v>52</v>
       </c>
@@ -3837,7 +3907,7 @@
       </c>
       <c r="D16" s="7"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4">
       <c r="A17" s="7" t="s">
         <v>53</v>
       </c>
@@ -3849,7 +3919,7 @@
       </c>
       <c r="D17" s="7"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4">
       <c r="A18" s="7" t="s">
         <v>54</v>
       </c>
@@ -3861,7 +3931,7 @@
       </c>
       <c r="D18" s="7"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4">
       <c r="A19" s="7" t="s">
         <v>55</v>
       </c>
@@ -3873,7 +3943,7 @@
       </c>
       <c r="D19" s="7"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4">
       <c r="A20" s="7" t="s">
         <v>56</v>
       </c>
@@ -3885,7 +3955,7 @@
       </c>
       <c r="D20" s="7"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4">
       <c r="A21" s="7" t="s">
         <v>57</v>
       </c>
@@ -3897,7 +3967,7 @@
       </c>
       <c r="D21" s="7"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4">
       <c r="A22" s="7" t="s">
         <v>58</v>
       </c>
@@ -3909,7 +3979,7 @@
       </c>
       <c r="D22" s="7"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4">
       <c r="A23" s="7" t="s">
         <v>59</v>
       </c>
@@ -3921,7 +3991,7 @@
       </c>
       <c r="D23" s="7"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4">
       <c r="A24" s="7" t="s">
         <v>60</v>
       </c>
@@ -3933,7 +4003,7 @@
       </c>
       <c r="D24" s="7"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4">
       <c r="A25" s="7" t="s">
         <v>61</v>
       </c>
@@ -3945,7 +4015,7 @@
       </c>
       <c r="D25" s="7"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4">
       <c r="A26" s="7" t="s">
         <v>47</v>
       </c>
@@ -3964,14 +4034,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A19" sqref="A19:XFD19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
@@ -3979,7 +4049,7 @@
     <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="10" t="s">
         <v>35</v>
       </c>
@@ -3993,7 +4063,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="7" t="s">
         <v>37</v>
       </c>
@@ -4005,7 +4075,7 @@
       </c>
       <c r="D2" s="7"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="7" t="s">
         <v>38</v>
       </c>
@@ -4017,7 +4087,7 @@
       </c>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="7" t="s">
         <v>39</v>
       </c>
@@ -4029,7 +4099,7 @@
       </c>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" s="7" t="s">
         <v>40</v>
       </c>
@@ -4041,7 +4111,7 @@
       </c>
       <c r="D5" s="7"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" s="7" t="s">
         <v>41</v>
       </c>
@@ -4053,7 +4123,7 @@
       </c>
       <c r="D6" s="7"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="7" t="s">
         <v>42</v>
       </c>
@@ -4065,7 +4135,7 @@
       </c>
       <c r="D7" s="7"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="7" t="s">
         <v>43</v>
       </c>
@@ -4077,7 +4147,7 @@
       </c>
       <c r="D8" s="7"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="7" t="s">
         <v>44</v>
       </c>
@@ -4089,7 +4159,7 @@
       </c>
       <c r="D9" s="7"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="7" t="s">
         <v>45</v>
       </c>
@@ -4101,7 +4171,7 @@
       </c>
       <c r="D10" s="7"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11" s="7" t="s">
         <v>46</v>
       </c>
@@ -4113,7 +4183,7 @@
       </c>
       <c r="D11" s="7"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="A12" s="7" t="s">
         <v>47</v>
       </c>
@@ -4125,7 +4195,7 @@
       </c>
       <c r="D12" s="7"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="A13" s="7" t="s">
         <v>48</v>
       </c>
@@ -4137,7 +4207,7 @@
       </c>
       <c r="D13" s="7"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="A14" s="7" t="s">
         <v>49</v>
       </c>
@@ -4149,7 +4219,7 @@
       </c>
       <c r="D14" s="7"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="A15" s="7" t="s">
         <v>50</v>
       </c>
@@ -4161,7 +4231,7 @@
       </c>
       <c r="D15" s="7"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="A16" s="7" t="s">
         <v>51</v>
       </c>
@@ -4173,7 +4243,7 @@
       </c>
       <c r="D16" s="7"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4">
       <c r="A17" s="7" t="s">
         <v>52</v>
       </c>
@@ -4185,7 +4255,7 @@
       </c>
       <c r="D17" s="7"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4">
       <c r="A18" s="7" t="s">
         <v>53</v>
       </c>
@@ -4197,7 +4267,7 @@
       </c>
       <c r="D18" s="7"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4">
       <c r="A19" s="7" t="s">
         <v>54</v>
       </c>
@@ -4209,7 +4279,7 @@
       </c>
       <c r="D19" s="7"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4">
       <c r="A20" s="7" t="s">
         <v>55</v>
       </c>
@@ -4221,7 +4291,7 @@
       </c>
       <c r="D20" s="7"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4">
       <c r="A21" s="7" t="s">
         <v>56</v>
       </c>
@@ -4233,7 +4303,7 @@
       </c>
       <c r="D21" s="7"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4">
       <c r="A22" s="7" t="s">
         <v>57</v>
       </c>
@@ -4245,7 +4315,7 @@
       </c>
       <c r="D22" s="7"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4">
       <c r="A23" s="7" t="s">
         <v>58</v>
       </c>
@@ -4257,7 +4327,7 @@
       </c>
       <c r="D23" s="7"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4">
       <c r="A24" s="7" t="s">
         <v>59</v>
       </c>
@@ -4269,7 +4339,7 @@
       </c>
       <c r="D24" s="7"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4">
       <c r="A25" s="7" t="s">
         <v>60</v>
       </c>
@@ -4281,7 +4351,7 @@
       </c>
       <c r="D25" s="7"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4">
       <c r="A26" s="7" t="s">
         <v>61</v>
       </c>

</xml_diff>

<commit_message>
Adds WAT-119 test script and related changes
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/WAT.xlsx
+++ b/src/test/resources/xls/WAT.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13305" windowHeight="2415"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="671" uniqueCount="411">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="675" uniqueCount="414">
   <si>
     <t>TCID</t>
   </si>
@@ -1250,13 +1250,22 @@
   </si>
   <si>
     <t>Verify that ‘Select All’ option should not display when quantity of search results of an author Only 1</t>
+  </si>
+  <si>
+    <t>WAT119</t>
+  </si>
+  <si>
+    <t>Change text to "Include Alternative name".</t>
+  </si>
+  <si>
+    <t>WAT-1340</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1508,7 +1517,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1540,9 +1549,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1574,6 +1584,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1749,14 +1760,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E128"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E129"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A101" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A126" sqref="A126:E128"/>
+      <selection activeCell="C131" sqref="C131"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="41" bestFit="1" customWidth="1" collapsed="1"/>
@@ -1765,7 +1776,7 @@
     <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1782,7 +1793,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -1797,7 +1808,7 @@
       </c>
       <c r="E2" s="4"/>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -1812,7 +1823,7 @@
       </c>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>11</v>
       </c>
@@ -1827,7 +1838,7 @@
       </c>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>12</v>
       </c>
@@ -1842,7 +1853,7 @@
       </c>
       <c r="E5" s="7"/>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>14</v>
       </c>
@@ -1857,7 +1868,7 @@
       </c>
       <c r="E6" s="7"/>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>17</v>
       </c>
@@ -1872,7 +1883,7 @@
       </c>
       <c r="E7" s="7"/>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>20</v>
       </c>
@@ -1887,7 +1898,7 @@
       </c>
       <c r="E8" s="7"/>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>22</v>
       </c>
@@ -1902,7 +1913,7 @@
       </c>
       <c r="E9" s="7"/>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>23</v>
       </c>
@@ -1917,7 +1928,7 @@
       </c>
       <c r="E10" s="7"/>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>24</v>
       </c>
@@ -1932,7 +1943,7 @@
       </c>
       <c r="E11" s="7"/>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>25</v>
       </c>
@@ -1947,7 +1958,7 @@
       </c>
       <c r="E12" s="7"/>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>62</v>
       </c>
@@ -1962,7 +1973,7 @@
       </c>
       <c r="E13" s="7"/>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>63</v>
       </c>
@@ -1977,7 +1988,7 @@
       </c>
       <c r="E14" s="7"/>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>64</v>
       </c>
@@ -1992,7 +2003,7 @@
       </c>
       <c r="E15" s="7"/>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>65</v>
       </c>
@@ -2007,7 +2018,7 @@
       </c>
       <c r="E16" s="7"/>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>74</v>
       </c>
@@ -2022,7 +2033,7 @@
       </c>
       <c r="E17" s="7"/>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>75</v>
       </c>
@@ -2037,7 +2048,7 @@
       </c>
       <c r="E18" s="7"/>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>79</v>
       </c>
@@ -2052,7 +2063,7 @@
       </c>
       <c r="E19" s="7"/>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>81</v>
       </c>
@@ -2067,7 +2078,7 @@
       </c>
       <c r="E20" s="7"/>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>82</v>
       </c>
@@ -2082,7 +2093,7 @@
       </c>
       <c r="E21" s="7"/>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>88</v>
       </c>
@@ -2097,7 +2108,7 @@
       </c>
       <c r="E22" s="7"/>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>90</v>
       </c>
@@ -2112,7 +2123,7 @@
       </c>
       <c r="E23" s="7"/>
     </row>
-    <row r="24" spans="1:5" ht="30">
+    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>94</v>
       </c>
@@ -2127,7 +2138,7 @@
       </c>
       <c r="E24" s="7"/>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>96</v>
       </c>
@@ -2142,7 +2153,7 @@
       </c>
       <c r="E25" s="7"/>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
         <v>98</v>
       </c>
@@ -2157,7 +2168,7 @@
       </c>
       <c r="E26" s="7"/>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
         <v>102</v>
       </c>
@@ -2172,7 +2183,7 @@
       </c>
       <c r="E27" s="7"/>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
         <v>105</v>
       </c>
@@ -2187,7 +2198,7 @@
       </c>
       <c r="E28" s="7"/>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
         <v>108</v>
       </c>
@@ -2202,7 +2213,7 @@
       </c>
       <c r="E29" s="7"/>
     </row>
-    <row r="30" spans="1:5" ht="30">
+    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
         <v>110</v>
       </c>
@@ -2217,7 +2228,7 @@
       </c>
       <c r="E30" s="7"/>
     </row>
-    <row r="31" spans="1:5" ht="30">
+    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
         <v>114</v>
       </c>
@@ -2232,7 +2243,7 @@
       </c>
       <c r="E31" s="7"/>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
         <v>119</v>
       </c>
@@ -2247,7 +2258,7 @@
       </c>
       <c r="E32" s="7"/>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
         <v>120</v>
       </c>
@@ -2262,7 +2273,7 @@
       </c>
       <c r="E33" s="7"/>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
         <v>125</v>
       </c>
@@ -2277,7 +2288,7 @@
       </c>
       <c r="E34" s="7"/>
     </row>
-    <row r="35" spans="1:5" ht="30">
+    <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
         <v>128</v>
       </c>
@@ -2292,7 +2303,7 @@
       </c>
       <c r="E35" s="7"/>
     </row>
-    <row r="36" spans="1:5" ht="30">
+    <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
         <v>131</v>
       </c>
@@ -2307,7 +2318,7 @@
       </c>
       <c r="E36" s="7"/>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
         <v>134</v>
       </c>
@@ -2322,7 +2333,7 @@
       </c>
       <c r="E37" s="7"/>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="9" t="s">
         <v>137</v>
       </c>
@@ -2337,7 +2348,7 @@
       </c>
       <c r="E38" s="7"/>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="s">
         <v>140</v>
       </c>
@@ -2352,7 +2363,7 @@
       </c>
       <c r="E39" s="7"/>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="9" t="s">
         <v>143</v>
       </c>
@@ -2367,7 +2378,7 @@
       </c>
       <c r="E40" s="7"/>
     </row>
-    <row r="41" spans="1:5" ht="30">
+    <row r="41" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
         <v>145</v>
       </c>
@@ -2382,7 +2393,7 @@
       </c>
       <c r="E41" s="7"/>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="9" t="s">
         <v>147</v>
       </c>
@@ -2397,7 +2408,7 @@
       </c>
       <c r="E42" s="7"/>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="9" t="s">
         <v>150</v>
       </c>
@@ -2412,7 +2423,7 @@
       </c>
       <c r="E43" s="7"/>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="9" t="s">
         <v>153</v>
       </c>
@@ -2427,7 +2438,7 @@
       </c>
       <c r="E44" s="7"/>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="9" t="s">
         <v>155</v>
       </c>
@@ -2442,7 +2453,7 @@
       </c>
       <c r="E45" s="7"/>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="12" t="s">
         <v>158</v>
       </c>
@@ -2457,7 +2468,7 @@
       </c>
       <c r="E46" s="7"/>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="12" t="s">
         <v>159</v>
       </c>
@@ -2472,7 +2483,7 @@
       </c>
       <c r="E47" s="7"/>
     </row>
-    <row r="48" spans="1:5" ht="30">
+    <row r="48" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="12" t="s">
         <v>160</v>
       </c>
@@ -2487,7 +2498,7 @@
       </c>
       <c r="E48" s="7"/>
     </row>
-    <row r="49" spans="1:5" ht="30">
+    <row r="49" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="12" t="s">
         <v>161</v>
       </c>
@@ -2502,7 +2513,7 @@
       </c>
       <c r="E49" s="7"/>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="12" t="s">
         <v>164</v>
       </c>
@@ -2517,7 +2528,7 @@
       </c>
       <c r="E50" s="7"/>
     </row>
-    <row r="51" spans="1:5" ht="30">
+    <row r="51" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="9" t="s">
         <v>173</v>
       </c>
@@ -2532,7 +2543,7 @@
       </c>
       <c r="E51" s="7"/>
     </row>
-    <row r="52" spans="1:5">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="9" t="s">
         <v>174</v>
       </c>
@@ -2547,7 +2558,7 @@
       </c>
       <c r="E52" s="7"/>
     </row>
-    <row r="53" spans="1:5">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="9" t="s">
         <v>179</v>
       </c>
@@ -2562,7 +2573,7 @@
       </c>
       <c r="E53" s="7"/>
     </row>
-    <row r="54" spans="1:5">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="9" t="s">
         <v>180</v>
       </c>
@@ -2577,7 +2588,7 @@
       </c>
       <c r="E54" s="7"/>
     </row>
-    <row r="55" spans="1:5">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="9" t="s">
         <v>185</v>
       </c>
@@ -2592,7 +2603,7 @@
       </c>
       <c r="E55" s="7"/>
     </row>
-    <row r="56" spans="1:5">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="s">
         <v>188</v>
       </c>
@@ -2607,7 +2618,7 @@
       </c>
       <c r="E56" s="7"/>
     </row>
-    <row r="57" spans="1:5" ht="30">
+    <row r="57" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="9" t="s">
         <v>191</v>
       </c>
@@ -2622,7 +2633,7 @@
       </c>
       <c r="E57" s="7"/>
     </row>
-    <row r="58" spans="1:5">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="9" t="s">
         <v>194</v>
       </c>
@@ -2637,7 +2648,7 @@
       </c>
       <c r="E58" s="7"/>
     </row>
-    <row r="59" spans="1:5">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
         <v>196</v>
       </c>
@@ -2652,7 +2663,7 @@
       </c>
       <c r="E59" s="7"/>
     </row>
-    <row r="60" spans="1:5" ht="45">
+    <row r="60" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
         <v>199</v>
       </c>
@@ -2667,7 +2678,7 @@
       </c>
       <c r="E60" s="7"/>
     </row>
-    <row r="61" spans="1:5">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="9" t="s">
         <v>202</v>
       </c>
@@ -2682,7 +2693,7 @@
       </c>
       <c r="E61" s="7"/>
     </row>
-    <row r="62" spans="1:5">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="9" t="s">
         <v>204</v>
       </c>
@@ -2697,7 +2708,7 @@
       </c>
       <c r="E62" s="7"/>
     </row>
-    <row r="63" spans="1:5">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="9" t="s">
         <v>206</v>
       </c>
@@ -2712,7 +2723,7 @@
       </c>
       <c r="E63" s="7"/>
     </row>
-    <row r="64" spans="1:5">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="9" t="s">
         <v>208</v>
       </c>
@@ -2727,7 +2738,7 @@
       </c>
       <c r="E64" s="7"/>
     </row>
-    <row r="65" spans="1:5">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="9" t="s">
         <v>217</v>
       </c>
@@ -2742,7 +2753,7 @@
       </c>
       <c r="E65" s="7"/>
     </row>
-    <row r="66" spans="1:5">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="9" t="s">
         <v>218</v>
       </c>
@@ -2757,7 +2768,7 @@
       </c>
       <c r="E66" s="7"/>
     </row>
-    <row r="67" spans="1:5">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="9" t="s">
         <v>223</v>
       </c>
@@ -2772,7 +2783,7 @@
       </c>
       <c r="E67" s="7"/>
     </row>
-    <row r="68" spans="1:5">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="9" t="s">
         <v>224</v>
       </c>
@@ -2787,7 +2798,7 @@
       </c>
       <c r="E68" s="7"/>
     </row>
-    <row r="69" spans="1:5">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="9" t="s">
         <v>225</v>
       </c>
@@ -2802,7 +2813,7 @@
       </c>
       <c r="E69" s="7"/>
     </row>
-    <row r="70" spans="1:5">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="9" t="s">
         <v>226</v>
       </c>
@@ -2817,7 +2828,7 @@
       </c>
       <c r="E70" s="7"/>
     </row>
-    <row r="71" spans="1:5">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="9" t="s">
         <v>233</v>
       </c>
@@ -2832,7 +2843,7 @@
       </c>
       <c r="E71" s="7"/>
     </row>
-    <row r="72" spans="1:5">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="9" t="s">
         <v>237</v>
       </c>
@@ -2847,7 +2858,7 @@
       </c>
       <c r="E72" s="7"/>
     </row>
-    <row r="73" spans="1:5">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="9" t="s">
         <v>239</v>
       </c>
@@ -2862,7 +2873,7 @@
       </c>
       <c r="E73" s="7"/>
     </row>
-    <row r="74" spans="1:5">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="9" t="s">
         <v>243</v>
       </c>
@@ -2877,7 +2888,7 @@
       </c>
       <c r="E74" s="7"/>
     </row>
-    <row r="75" spans="1:5" ht="30">
+    <row r="75" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" s="9" t="s">
         <v>245</v>
       </c>
@@ -2892,7 +2903,7 @@
       </c>
       <c r="E75" s="7"/>
     </row>
-    <row r="76" spans="1:5">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="9" t="s">
         <v>248</v>
       </c>
@@ -2907,7 +2918,7 @@
       </c>
       <c r="E76" s="7"/>
     </row>
-    <row r="77" spans="1:5">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="9" t="s">
         <v>256</v>
       </c>
@@ -2922,7 +2933,7 @@
       </c>
       <c r="E77" s="7"/>
     </row>
-    <row r="78" spans="1:5">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="9" t="s">
         <v>257</v>
       </c>
@@ -2937,7 +2948,7 @@
       </c>
       <c r="E78" s="7"/>
     </row>
-    <row r="79" spans="1:5">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="9" t="s">
         <v>261</v>
       </c>
@@ -2952,7 +2963,7 @@
       </c>
       <c r="E79" s="7"/>
     </row>
-    <row r="80" spans="1:5">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="9" t="s">
         <v>264</v>
       </c>
@@ -2967,7 +2978,7 @@
       </c>
       <c r="E80" s="7"/>
     </row>
-    <row r="81" spans="1:5">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="9" t="s">
         <v>267</v>
       </c>
@@ -2982,7 +2993,7 @@
       </c>
       <c r="E81" s="7"/>
     </row>
-    <row r="82" spans="1:5" ht="30">
+    <row r="82" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A82" s="9" t="s">
         <v>269</v>
       </c>
@@ -2997,7 +3008,7 @@
       </c>
       <c r="E82" s="7"/>
     </row>
-    <row r="83" spans="1:5">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="9" t="s">
         <v>274</v>
       </c>
@@ -3012,7 +3023,7 @@
       </c>
       <c r="E83" s="7"/>
     </row>
-    <row r="84" spans="1:5" ht="30">
+    <row r="84" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A84" s="9" t="s">
         <v>277</v>
       </c>
@@ -3027,7 +3038,7 @@
       </c>
       <c r="E84" s="7"/>
     </row>
-    <row r="85" spans="1:5">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="9" t="s">
         <v>279</v>
       </c>
@@ -3042,7 +3053,7 @@
       </c>
       <c r="E85" s="7"/>
     </row>
-    <row r="86" spans="1:5">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="9" t="s">
         <v>282</v>
       </c>
@@ -3057,7 +3068,7 @@
       </c>
       <c r="E86" s="7"/>
     </row>
-    <row r="87" spans="1:5">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="9" t="s">
         <v>285</v>
       </c>
@@ -3072,7 +3083,7 @@
       </c>
       <c r="E87" s="7"/>
     </row>
-    <row r="88" spans="1:5">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="9" t="s">
         <v>288</v>
       </c>
@@ -3087,7 +3098,7 @@
       </c>
       <c r="E88" s="7"/>
     </row>
-    <row r="89" spans="1:5">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="9" t="s">
         <v>291</v>
       </c>
@@ -3102,7 +3113,7 @@
       </c>
       <c r="E89" s="7"/>
     </row>
-    <row r="90" spans="1:5">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="9" t="s">
         <v>294</v>
       </c>
@@ -3117,7 +3128,7 @@
       </c>
       <c r="E90" s="7"/>
     </row>
-    <row r="91" spans="1:5">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="9" t="s">
         <v>297</v>
       </c>
@@ -3132,7 +3143,7 @@
       </c>
       <c r="E91" s="7"/>
     </row>
-    <row r="92" spans="1:5">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="9" t="s">
         <v>300</v>
       </c>
@@ -3147,7 +3158,7 @@
       </c>
       <c r="E92" s="7"/>
     </row>
-    <row r="93" spans="1:5">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="9" t="s">
         <v>303</v>
       </c>
@@ -3162,7 +3173,7 @@
       </c>
       <c r="E93" s="7"/>
     </row>
-    <row r="94" spans="1:5">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="9" t="s">
         <v>306</v>
       </c>
@@ -3177,7 +3188,7 @@
       </c>
       <c r="E94" s="7"/>
     </row>
-    <row r="95" spans="1:5">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="9" t="s">
         <v>309</v>
       </c>
@@ -3192,7 +3203,7 @@
       </c>
       <c r="E95" s="7"/>
     </row>
-    <row r="96" spans="1:5">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="9" t="s">
         <v>314</v>
       </c>
@@ -3207,7 +3218,7 @@
       </c>
       <c r="E96" s="7"/>
     </row>
-    <row r="97" spans="1:5">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="9" t="s">
         <v>315</v>
       </c>
@@ -3222,7 +3233,7 @@
       </c>
       <c r="E97" s="7"/>
     </row>
-    <row r="98" spans="1:5">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="9" t="s">
         <v>319</v>
       </c>
@@ -3237,7 +3248,7 @@
       </c>
       <c r="E98" s="7"/>
     </row>
-    <row r="99" spans="1:5">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="9" t="s">
         <v>321</v>
       </c>
@@ -3252,7 +3263,7 @@
       </c>
       <c r="E99" s="7"/>
     </row>
-    <row r="100" spans="1:5">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="9" t="s">
         <v>322</v>
       </c>
@@ -3267,7 +3278,7 @@
       </c>
       <c r="E100" s="7"/>
     </row>
-    <row r="101" spans="1:5" ht="30">
+    <row r="101" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A101" s="9" t="s">
         <v>323</v>
       </c>
@@ -3282,7 +3293,7 @@
       </c>
       <c r="E101" s="7"/>
     </row>
-    <row r="102" spans="1:5">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="9" t="s">
         <v>328</v>
       </c>
@@ -3297,7 +3308,7 @@
       </c>
       <c r="E102" s="7"/>
     </row>
-    <row r="103" spans="1:5">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="9" t="s">
         <v>333</v>
       </c>
@@ -3312,7 +3323,7 @@
       </c>
       <c r="E103" s="7"/>
     </row>
-    <row r="104" spans="1:5">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="9" t="s">
         <v>336</v>
       </c>
@@ -3327,7 +3338,7 @@
       </c>
       <c r="E104" s="7"/>
     </row>
-    <row r="105" spans="1:5">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="9" t="s">
         <v>337</v>
       </c>
@@ -3342,7 +3353,7 @@
       </c>
       <c r="E105" s="7"/>
     </row>
-    <row r="106" spans="1:5">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="9" t="s">
         <v>342</v>
       </c>
@@ -3357,7 +3368,7 @@
       </c>
       <c r="E106" s="7"/>
     </row>
-    <row r="107" spans="1:5">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="9" t="s">
         <v>345</v>
       </c>
@@ -3372,7 +3383,7 @@
       </c>
       <c r="E107" s="7"/>
     </row>
-    <row r="108" spans="1:5">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="9" t="s">
         <v>350</v>
       </c>
@@ -3387,7 +3398,7 @@
       </c>
       <c r="E108" s="7"/>
     </row>
-    <row r="109" spans="1:5" ht="30">
+    <row r="109" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A109" s="9" t="s">
         <v>351</v>
       </c>
@@ -3402,7 +3413,7 @@
       </c>
       <c r="E109" s="7"/>
     </row>
-    <row r="110" spans="1:5">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="9" t="s">
         <v>354</v>
       </c>
@@ -3417,7 +3428,7 @@
       </c>
       <c r="E110" s="7"/>
     </row>
-    <row r="111" spans="1:5">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="9" t="s">
         <v>357</v>
       </c>
@@ -3432,7 +3443,7 @@
       </c>
       <c r="E111" s="7"/>
     </row>
-    <row r="112" spans="1:5">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="9" t="s">
         <v>361</v>
       </c>
@@ -3447,7 +3458,7 @@
       </c>
       <c r="E112" s="7"/>
     </row>
-    <row r="113" spans="1:5">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="17" t="s">
         <v>363</v>
       </c>
@@ -3462,7 +3473,7 @@
       </c>
       <c r="E113" s="19"/>
     </row>
-    <row r="114" spans="1:5" ht="30">
+    <row r="114" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A114" s="9" t="s">
         <v>366</v>
       </c>
@@ -3477,7 +3488,7 @@
       </c>
       <c r="E114" s="7"/>
     </row>
-    <row r="115" spans="1:5">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="9" t="s">
         <v>369</v>
       </c>
@@ -3492,7 +3503,7 @@
       </c>
       <c r="E115" s="7"/>
     </row>
-    <row r="116" spans="1:5">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="9" t="s">
         <v>370</v>
       </c>
@@ -3507,7 +3518,7 @@
       </c>
       <c r="E116" s="7"/>
     </row>
-    <row r="117" spans="1:5">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" s="9" t="s">
         <v>371</v>
       </c>
@@ -3522,7 +3533,7 @@
       </c>
       <c r="E117" s="7"/>
     </row>
-    <row r="118" spans="1:5">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" s="9" t="s">
         <v>378</v>
       </c>
@@ -3537,7 +3548,7 @@
       </c>
       <c r="E118" s="7"/>
     </row>
-    <row r="119" spans="1:5">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" s="9" t="s">
         <v>381</v>
       </c>
@@ -3552,7 +3563,7 @@
       </c>
       <c r="E119" s="7"/>
     </row>
-    <row r="120" spans="1:5">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" s="9" t="s">
         <v>384</v>
       </c>
@@ -3567,7 +3578,7 @@
       </c>
       <c r="E120" s="7"/>
     </row>
-    <row r="121" spans="1:5">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="9" t="s">
         <v>387</v>
       </c>
@@ -3582,7 +3593,7 @@
       </c>
       <c r="E121" s="7"/>
     </row>
-    <row r="122" spans="1:5">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" s="7" t="s">
         <v>390</v>
       </c>
@@ -3597,7 +3608,7 @@
       </c>
       <c r="E122" s="7"/>
     </row>
-    <row r="123" spans="1:5">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" s="7" t="s">
         <v>393</v>
       </c>
@@ -3612,7 +3623,7 @@
       </c>
       <c r="E123" s="7"/>
     </row>
-    <row r="124" spans="1:5">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" s="7" t="s">
         <v>396</v>
       </c>
@@ -3627,7 +3638,7 @@
       </c>
       <c r="E124" s="7"/>
     </row>
-    <row r="125" spans="1:5">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" s="9" t="s">
         <v>399</v>
       </c>
@@ -3642,7 +3653,7 @@
       </c>
       <c r="E125" s="7"/>
     </row>
-    <row r="126" spans="1:5">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" s="7" t="s">
         <v>402</v>
       </c>
@@ -3657,7 +3668,7 @@
       </c>
       <c r="E126" s="7"/>
     </row>
-    <row r="127" spans="1:5">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" s="7" t="s">
         <v>405</v>
       </c>
@@ -3672,7 +3683,7 @@
       </c>
       <c r="E127" s="7"/>
     </row>
-    <row r="128" spans="1:5">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" s="7" t="s">
         <v>408</v>
       </c>
@@ -3686,6 +3697,21 @@
         <v>5</v>
       </c>
       <c r="E128" s="7"/>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A129" s="9" t="s">
+        <v>411</v>
+      </c>
+      <c r="B129" s="7" t="s">
+        <v>413</v>
+      </c>
+      <c r="C129" s="7" t="s">
+        <v>412</v>
+      </c>
+      <c r="D129" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E129" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -3698,14 +3724,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView topLeftCell="A10" zoomScale="80" workbookViewId="0">
       <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
@@ -3713,7 +3739,7 @@
     <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>35</v>
       </c>
@@ -3727,7 +3753,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>37</v>
       </c>
@@ -3739,7 +3765,7 @@
       </c>
       <c r="D2" s="7"/>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>38</v>
       </c>
@@ -3751,7 +3777,7 @@
       </c>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>39</v>
       </c>
@@ -3763,7 +3789,7 @@
       </c>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>40</v>
       </c>
@@ -3775,7 +3801,7 @@
       </c>
       <c r="D5" s="7"/>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>41</v>
       </c>
@@ -3787,7 +3813,7 @@
       </c>
       <c r="D6" s="7"/>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>42</v>
       </c>
@@ -3799,7 +3825,7 @@
       </c>
       <c r="D7" s="7"/>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>43</v>
       </c>
@@ -3811,7 +3837,7 @@
       </c>
       <c r="D8" s="7"/>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>44</v>
       </c>
@@ -3823,7 +3849,7 @@
       </c>
       <c r="D9" s="7"/>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>45</v>
       </c>
@@ -3835,7 +3861,7 @@
       </c>
       <c r="D10" s="7"/>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>46</v>
       </c>
@@ -3847,7 +3873,7 @@
       </c>
       <c r="D11" s="7"/>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>48</v>
       </c>
@@ -3859,7 +3885,7 @@
       </c>
       <c r="D12" s="7"/>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>49</v>
       </c>
@@ -3871,7 +3897,7 @@
       </c>
       <c r="D13" s="7"/>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>50</v>
       </c>
@@ -3883,7 +3909,7 @@
       </c>
       <c r="D14" s="7"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>51</v>
       </c>
@@ -3895,7 +3921,7 @@
       </c>
       <c r="D15" s="7"/>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>52</v>
       </c>
@@ -3907,7 +3933,7 @@
       </c>
       <c r="D16" s="7"/>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>53</v>
       </c>
@@ -3919,7 +3945,7 @@
       </c>
       <c r="D17" s="7"/>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>54</v>
       </c>
@@ -3931,7 +3957,7 @@
       </c>
       <c r="D18" s="7"/>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>55</v>
       </c>
@@ -3943,7 +3969,7 @@
       </c>
       <c r="D19" s="7"/>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>56</v>
       </c>
@@ -3955,7 +3981,7 @@
       </c>
       <c r="D20" s="7"/>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>57</v>
       </c>
@@ -3967,7 +3993,7 @@
       </c>
       <c r="D21" s="7"/>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>58</v>
       </c>
@@ -3979,7 +4005,7 @@
       </c>
       <c r="D22" s="7"/>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>59</v>
       </c>
@@ -3991,7 +4017,7 @@
       </c>
       <c r="D23" s="7"/>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>60</v>
       </c>
@@ -4003,7 +4029,7 @@
       </c>
       <c r="D24" s="7"/>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>61</v>
       </c>
@@ -4015,7 +4041,7 @@
       </c>
       <c r="D25" s="7"/>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>47</v>
       </c>
@@ -4034,14 +4060,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A19" sqref="A19:XFD19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
@@ -4049,7 +4075,7 @@
     <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>35</v>
       </c>
@@ -4063,7 +4089,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>37</v>
       </c>
@@ -4075,7 +4101,7 @@
       </c>
       <c r="D2" s="7"/>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>38</v>
       </c>
@@ -4087,7 +4113,7 @@
       </c>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>39</v>
       </c>
@@ -4099,7 +4125,7 @@
       </c>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>40</v>
       </c>
@@ -4111,7 +4137,7 @@
       </c>
       <c r="D5" s="7"/>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>41</v>
       </c>
@@ -4123,7 +4149,7 @@
       </c>
       <c r="D6" s="7"/>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>42</v>
       </c>
@@ -4135,7 +4161,7 @@
       </c>
       <c r="D7" s="7"/>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>43</v>
       </c>
@@ -4147,7 +4173,7 @@
       </c>
       <c r="D8" s="7"/>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>44</v>
       </c>
@@ -4159,7 +4185,7 @@
       </c>
       <c r="D9" s="7"/>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>45</v>
       </c>
@@ -4171,7 +4197,7 @@
       </c>
       <c r="D10" s="7"/>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>46</v>
       </c>
@@ -4183,7 +4209,7 @@
       </c>
       <c r="D11" s="7"/>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>47</v>
       </c>
@@ -4195,7 +4221,7 @@
       </c>
       <c r="D12" s="7"/>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>48</v>
       </c>
@@ -4207,7 +4233,7 @@
       </c>
       <c r="D13" s="7"/>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>49</v>
       </c>
@@ -4219,7 +4245,7 @@
       </c>
       <c r="D14" s="7"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>50</v>
       </c>
@@ -4231,7 +4257,7 @@
       </c>
       <c r="D15" s="7"/>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>51</v>
       </c>
@@ -4243,7 +4269,7 @@
       </c>
       <c r="D16" s="7"/>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>52</v>
       </c>
@@ -4255,7 +4281,7 @@
       </c>
       <c r="D17" s="7"/>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>53</v>
       </c>
@@ -4267,7 +4293,7 @@
       </c>
       <c r="D18" s="7"/>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>54</v>
       </c>
@@ -4279,7 +4305,7 @@
       </c>
       <c r="D19" s="7"/>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>55</v>
       </c>
@@ -4291,7 +4317,7 @@
       </c>
       <c r="D20" s="7"/>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>56</v>
       </c>
@@ -4303,7 +4329,7 @@
       </c>
       <c r="D21" s="7"/>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>57</v>
       </c>
@@ -4315,7 +4341,7 @@
       </c>
       <c r="D22" s="7"/>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>58</v>
       </c>
@@ -4327,7 +4353,7 @@
       </c>
       <c r="D23" s="7"/>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>59</v>
       </c>
@@ -4339,7 +4365,7 @@
       </c>
       <c r="D24" s="7"/>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>60</v>
       </c>
@@ -4351,7 +4377,7 @@
       </c>
       <c r="D25" s="7"/>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>61</v>
       </c>

</xml_diff>

<commit_message>
WAT New script added
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/WAT.xlsx
+++ b/src/test/resources/xls/WAT.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13305" windowHeight="2415"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="683" uniqueCount="419">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="422">
   <si>
     <t>TCID</t>
   </si>
@@ -1274,13 +1274,22 @@
   </si>
   <si>
     <t>WAT-725</t>
+  </si>
+  <si>
+    <t>WAT160</t>
+  </si>
+  <si>
+    <t>WAT-568</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Verify that System must display the sub-organization below the Organization name.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1532,7 +1541,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1564,10 +1573,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1599,7 +1607,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1775,14 +1782,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E131"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A124" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B131" sqref="B131"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C99" sqref="C99"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="41" bestFit="1" customWidth="1" collapsed="1"/>
@@ -1791,7 +1798,7 @@
     <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1808,7 +1815,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -1823,7 +1830,7 @@
       </c>
       <c r="E2" s="4"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -1838,7 +1845,7 @@
       </c>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" s="7" t="s">
         <v>11</v>
       </c>
@@ -1853,7 +1860,7 @@
       </c>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" s="7" t="s">
         <v>12</v>
       </c>
@@ -1868,7 +1875,7 @@
       </c>
       <c r="E5" s="7"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" s="7" t="s">
         <v>14</v>
       </c>
@@ -1883,7 +1890,7 @@
       </c>
       <c r="E6" s="7"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" s="7" t="s">
         <v>17</v>
       </c>
@@ -1898,7 +1905,7 @@
       </c>
       <c r="E7" s="7"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" s="7" t="s">
         <v>20</v>
       </c>
@@ -1913,7 +1920,7 @@
       </c>
       <c r="E8" s="7"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" s="7" t="s">
         <v>22</v>
       </c>
@@ -1928,7 +1935,7 @@
       </c>
       <c r="E9" s="7"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10" s="7" t="s">
         <v>23</v>
       </c>
@@ -1943,7 +1950,7 @@
       </c>
       <c r="E10" s="7"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11" s="7" t="s">
         <v>24</v>
       </c>
@@ -1958,7 +1965,7 @@
       </c>
       <c r="E11" s="7"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12" s="7" t="s">
         <v>25</v>
       </c>
@@ -1973,7 +1980,7 @@
       </c>
       <c r="E12" s="7"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13" s="7" t="s">
         <v>62</v>
       </c>
@@ -1988,7 +1995,7 @@
       </c>
       <c r="E13" s="7"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="A14" s="7" t="s">
         <v>63</v>
       </c>
@@ -2003,7 +2010,7 @@
       </c>
       <c r="E14" s="7"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="A15" s="7" t="s">
         <v>64</v>
       </c>
@@ -2018,7 +2025,7 @@
       </c>
       <c r="E15" s="7"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="A16" s="7" t="s">
         <v>65</v>
       </c>
@@ -2033,7 +2040,7 @@
       </c>
       <c r="E16" s="7"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5">
       <c r="A17" s="7" t="s">
         <v>74</v>
       </c>
@@ -2048,7 +2055,7 @@
       </c>
       <c r="E17" s="7"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5">
       <c r="A18" s="7" t="s">
         <v>75</v>
       </c>
@@ -2063,7 +2070,7 @@
       </c>
       <c r="E18" s="7"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5">
       <c r="A19" s="7" t="s">
         <v>79</v>
       </c>
@@ -2078,7 +2085,7 @@
       </c>
       <c r="E19" s="7"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5">
       <c r="A20" s="7" t="s">
         <v>81</v>
       </c>
@@ -2093,7 +2100,7 @@
       </c>
       <c r="E20" s="7"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5">
       <c r="A21" s="7" t="s">
         <v>82</v>
       </c>
@@ -2108,7 +2115,7 @@
       </c>
       <c r="E21" s="7"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5">
       <c r="A22" s="7" t="s">
         <v>88</v>
       </c>
@@ -2123,7 +2130,7 @@
       </c>
       <c r="E22" s="7"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5">
       <c r="A23" s="7" t="s">
         <v>90</v>
       </c>
@@ -2138,7 +2145,7 @@
       </c>
       <c r="E23" s="7"/>
     </row>
-    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="30">
       <c r="A24" s="9" t="s">
         <v>94</v>
       </c>
@@ -2153,7 +2160,7 @@
       </c>
       <c r="E24" s="7"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5">
       <c r="A25" s="9" t="s">
         <v>96</v>
       </c>
@@ -2168,7 +2175,7 @@
       </c>
       <c r="E25" s="7"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5">
       <c r="A26" s="9" t="s">
         <v>98</v>
       </c>
@@ -2183,7 +2190,7 @@
       </c>
       <c r="E26" s="7"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5">
       <c r="A27" s="9" t="s">
         <v>102</v>
       </c>
@@ -2198,7 +2205,7 @@
       </c>
       <c r="E27" s="7"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5">
       <c r="A28" s="9" t="s">
         <v>105</v>
       </c>
@@ -2213,7 +2220,7 @@
       </c>
       <c r="E28" s="7"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5">
       <c r="A29" s="9" t="s">
         <v>108</v>
       </c>
@@ -2228,7 +2235,7 @@
       </c>
       <c r="E29" s="7"/>
     </row>
-    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" ht="30">
       <c r="A30" s="9" t="s">
         <v>110</v>
       </c>
@@ -2243,7 +2250,7 @@
       </c>
       <c r="E30" s="7"/>
     </row>
-    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" ht="30">
       <c r="A31" s="9" t="s">
         <v>114</v>
       </c>
@@ -2258,7 +2265,7 @@
       </c>
       <c r="E31" s="7"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5">
       <c r="A32" s="9" t="s">
         <v>119</v>
       </c>
@@ -2273,7 +2280,7 @@
       </c>
       <c r="E32" s="7"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5">
       <c r="A33" s="9" t="s">
         <v>120</v>
       </c>
@@ -2288,7 +2295,7 @@
       </c>
       <c r="E33" s="7"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5">
       <c r="A34" s="9" t="s">
         <v>125</v>
       </c>
@@ -2303,7 +2310,7 @@
       </c>
       <c r="E34" s="7"/>
     </row>
-    <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" ht="30">
       <c r="A35" s="9" t="s">
         <v>128</v>
       </c>
@@ -2318,7 +2325,7 @@
       </c>
       <c r="E35" s="7"/>
     </row>
-    <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" ht="30">
       <c r="A36" s="9" t="s">
         <v>131</v>
       </c>
@@ -2333,7 +2340,7 @@
       </c>
       <c r="E36" s="7"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5">
       <c r="A37" s="9" t="s">
         <v>134</v>
       </c>
@@ -2348,7 +2355,7 @@
       </c>
       <c r="E37" s="7"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5">
       <c r="A38" s="9" t="s">
         <v>137</v>
       </c>
@@ -2363,7 +2370,7 @@
       </c>
       <c r="E38" s="7"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5">
       <c r="A39" s="9" t="s">
         <v>140</v>
       </c>
@@ -2378,7 +2385,7 @@
       </c>
       <c r="E39" s="7"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5">
       <c r="A40" s="9" t="s">
         <v>143</v>
       </c>
@@ -2393,7 +2400,7 @@
       </c>
       <c r="E40" s="7"/>
     </row>
-    <row r="41" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" ht="30">
       <c r="A41" s="9" t="s">
         <v>145</v>
       </c>
@@ -2408,7 +2415,7 @@
       </c>
       <c r="E41" s="7"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5">
       <c r="A42" s="9" t="s">
         <v>147</v>
       </c>
@@ -2423,7 +2430,7 @@
       </c>
       <c r="E42" s="7"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5">
       <c r="A43" s="9" t="s">
         <v>150</v>
       </c>
@@ -2438,7 +2445,7 @@
       </c>
       <c r="E43" s="7"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5">
       <c r="A44" s="9" t="s">
         <v>153</v>
       </c>
@@ -2453,7 +2460,7 @@
       </c>
       <c r="E44" s="7"/>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5">
       <c r="A45" s="9" t="s">
         <v>155</v>
       </c>
@@ -2468,7 +2475,7 @@
       </c>
       <c r="E45" s="7"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5">
       <c r="A46" s="12" t="s">
         <v>158</v>
       </c>
@@ -2483,7 +2490,7 @@
       </c>
       <c r="E46" s="7"/>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5">
       <c r="A47" s="12" t="s">
         <v>159</v>
       </c>
@@ -2498,7 +2505,7 @@
       </c>
       <c r="E47" s="7"/>
     </row>
-    <row r="48" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" ht="30">
       <c r="A48" s="12" t="s">
         <v>160</v>
       </c>
@@ -2513,7 +2520,7 @@
       </c>
       <c r="E48" s="7"/>
     </row>
-    <row r="49" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" ht="30">
       <c r="A49" s="12" t="s">
         <v>161</v>
       </c>
@@ -2528,7 +2535,7 @@
       </c>
       <c r="E49" s="7"/>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5">
       <c r="A50" s="12" t="s">
         <v>164</v>
       </c>
@@ -2543,7 +2550,7 @@
       </c>
       <c r="E50" s="7"/>
     </row>
-    <row r="51" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" ht="30">
       <c r="A51" s="9" t="s">
         <v>173</v>
       </c>
@@ -2558,7 +2565,7 @@
       </c>
       <c r="E51" s="7"/>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5">
       <c r="A52" s="9" t="s">
         <v>174</v>
       </c>
@@ -2573,7 +2580,7 @@
       </c>
       <c r="E52" s="7"/>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5">
       <c r="A53" s="9" t="s">
         <v>179</v>
       </c>
@@ -2588,7 +2595,7 @@
       </c>
       <c r="E53" s="7"/>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5">
       <c r="A54" s="9" t="s">
         <v>180</v>
       </c>
@@ -2603,7 +2610,7 @@
       </c>
       <c r="E54" s="7"/>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5">
       <c r="A55" s="9" t="s">
         <v>185</v>
       </c>
@@ -2618,7 +2625,7 @@
       </c>
       <c r="E55" s="7"/>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5">
       <c r="A56" s="9" t="s">
         <v>188</v>
       </c>
@@ -2633,7 +2640,7 @@
       </c>
       <c r="E56" s="7"/>
     </row>
-    <row r="57" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" ht="30">
       <c r="A57" s="9" t="s">
         <v>191</v>
       </c>
@@ -2648,7 +2655,7 @@
       </c>
       <c r="E57" s="7"/>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5">
       <c r="A58" s="9" t="s">
         <v>194</v>
       </c>
@@ -2663,7 +2670,7 @@
       </c>
       <c r="E58" s="7"/>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5">
       <c r="A59" s="7" t="s">
         <v>196</v>
       </c>
@@ -2678,7 +2685,7 @@
       </c>
       <c r="E59" s="7"/>
     </row>
-    <row r="60" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" ht="45">
       <c r="A60" s="7" t="s">
         <v>199</v>
       </c>
@@ -2693,7 +2700,7 @@
       </c>
       <c r="E60" s="7"/>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5">
       <c r="A61" s="9" t="s">
         <v>202</v>
       </c>
@@ -2708,7 +2715,7 @@
       </c>
       <c r="E61" s="7"/>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5">
       <c r="A62" s="9" t="s">
         <v>204</v>
       </c>
@@ -2723,7 +2730,7 @@
       </c>
       <c r="E62" s="7"/>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5">
       <c r="A63" s="9" t="s">
         <v>206</v>
       </c>
@@ -2738,7 +2745,7 @@
       </c>
       <c r="E63" s="7"/>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5">
       <c r="A64" s="9" t="s">
         <v>208</v>
       </c>
@@ -2753,7 +2760,7 @@
       </c>
       <c r="E64" s="7"/>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5">
       <c r="A65" s="9" t="s">
         <v>217</v>
       </c>
@@ -2768,7 +2775,7 @@
       </c>
       <c r="E65" s="7"/>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5">
       <c r="A66" s="9" t="s">
         <v>218</v>
       </c>
@@ -2783,7 +2790,7 @@
       </c>
       <c r="E66" s="7"/>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5">
       <c r="A67" s="9" t="s">
         <v>223</v>
       </c>
@@ -2798,7 +2805,7 @@
       </c>
       <c r="E67" s="7"/>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5">
       <c r="A68" s="9" t="s">
         <v>224</v>
       </c>
@@ -2813,7 +2820,7 @@
       </c>
       <c r="E68" s="7"/>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5">
       <c r="A69" s="9" t="s">
         <v>225</v>
       </c>
@@ -2828,7 +2835,7 @@
       </c>
       <c r="E69" s="7"/>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5">
       <c r="A70" s="9" t="s">
         <v>226</v>
       </c>
@@ -2843,7 +2850,7 @@
       </c>
       <c r="E70" s="7"/>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5">
       <c r="A71" s="9" t="s">
         <v>233</v>
       </c>
@@ -2858,7 +2865,7 @@
       </c>
       <c r="E71" s="7"/>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5">
       <c r="A72" s="9" t="s">
         <v>237</v>
       </c>
@@ -2873,7 +2880,7 @@
       </c>
       <c r="E72" s="7"/>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5">
       <c r="A73" s="9" t="s">
         <v>239</v>
       </c>
@@ -2888,7 +2895,7 @@
       </c>
       <c r="E73" s="7"/>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5">
       <c r="A74" s="9" t="s">
         <v>243</v>
       </c>
@@ -2903,7 +2910,7 @@
       </c>
       <c r="E74" s="7"/>
     </row>
-    <row r="75" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" ht="30">
       <c r="A75" s="9" t="s">
         <v>245</v>
       </c>
@@ -2918,7 +2925,7 @@
       </c>
       <c r="E75" s="7"/>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5">
       <c r="A76" s="9" t="s">
         <v>248</v>
       </c>
@@ -2933,7 +2940,7 @@
       </c>
       <c r="E76" s="7"/>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5">
       <c r="A77" s="9" t="s">
         <v>256</v>
       </c>
@@ -2948,7 +2955,7 @@
       </c>
       <c r="E77" s="7"/>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5">
       <c r="A78" s="9" t="s">
         <v>257</v>
       </c>
@@ -2963,7 +2970,7 @@
       </c>
       <c r="E78" s="7"/>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5">
       <c r="A79" s="9" t="s">
         <v>261</v>
       </c>
@@ -2978,7 +2985,7 @@
       </c>
       <c r="E79" s="7"/>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5">
       <c r="A80" s="9" t="s">
         <v>264</v>
       </c>
@@ -2993,7 +3000,7 @@
       </c>
       <c r="E80" s="7"/>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5">
       <c r="A81" s="9" t="s">
         <v>267</v>
       </c>
@@ -3008,7 +3015,7 @@
       </c>
       <c r="E81" s="7"/>
     </row>
-    <row r="82" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" ht="30">
       <c r="A82" s="9" t="s">
         <v>269</v>
       </c>
@@ -3023,7 +3030,7 @@
       </c>
       <c r="E82" s="7"/>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5">
       <c r="A83" s="9" t="s">
         <v>274</v>
       </c>
@@ -3038,7 +3045,7 @@
       </c>
       <c r="E83" s="7"/>
     </row>
-    <row r="84" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" ht="30">
       <c r="A84" s="9" t="s">
         <v>277</v>
       </c>
@@ -3053,7 +3060,7 @@
       </c>
       <c r="E84" s="7"/>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5">
       <c r="A85" s="9" t="s">
         <v>279</v>
       </c>
@@ -3068,7 +3075,7 @@
       </c>
       <c r="E85" s="7"/>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5">
       <c r="A86" s="9" t="s">
         <v>282</v>
       </c>
@@ -3083,7 +3090,7 @@
       </c>
       <c r="E86" s="7"/>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5">
       <c r="A87" s="9" t="s">
         <v>285</v>
       </c>
@@ -3098,7 +3105,7 @@
       </c>
       <c r="E87" s="7"/>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5">
       <c r="A88" s="9" t="s">
         <v>288</v>
       </c>
@@ -3113,7 +3120,7 @@
       </c>
       <c r="E88" s="7"/>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5">
       <c r="A89" s="9" t="s">
         <v>291</v>
       </c>
@@ -3128,7 +3135,7 @@
       </c>
       <c r="E89" s="7"/>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5">
       <c r="A90" s="9" t="s">
         <v>294</v>
       </c>
@@ -3143,7 +3150,7 @@
       </c>
       <c r="E90" s="7"/>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5">
       <c r="A91" s="9" t="s">
         <v>297</v>
       </c>
@@ -3158,7 +3165,7 @@
       </c>
       <c r="E91" s="7"/>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5">
       <c r="A92" s="9" t="s">
         <v>300</v>
       </c>
@@ -3173,7 +3180,7 @@
       </c>
       <c r="E92" s="7"/>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5">
       <c r="A93" s="9" t="s">
         <v>303</v>
       </c>
@@ -3188,7 +3195,7 @@
       </c>
       <c r="E93" s="7"/>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5">
       <c r="A94" s="9" t="s">
         <v>306</v>
       </c>
@@ -3203,7 +3210,7 @@
       </c>
       <c r="E94" s="7"/>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5">
       <c r="A95" s="9" t="s">
         <v>309</v>
       </c>
@@ -3218,7 +3225,7 @@
       </c>
       <c r="E95" s="7"/>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5">
       <c r="A96" s="9" t="s">
         <v>314</v>
       </c>
@@ -3233,7 +3240,7 @@
       </c>
       <c r="E96" s="7"/>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5">
       <c r="A97" s="9" t="s">
         <v>315</v>
       </c>
@@ -3248,7 +3255,7 @@
       </c>
       <c r="E97" s="7"/>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5">
       <c r="A98" s="9" t="s">
         <v>319</v>
       </c>
@@ -3263,7 +3270,7 @@
       </c>
       <c r="E98" s="7"/>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5">
       <c r="A99" s="9" t="s">
         <v>321</v>
       </c>
@@ -3278,7 +3285,7 @@
       </c>
       <c r="E99" s="7"/>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5">
       <c r="A100" s="9" t="s">
         <v>322</v>
       </c>
@@ -3293,7 +3300,7 @@
       </c>
       <c r="E100" s="7"/>
     </row>
-    <row r="101" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" ht="30">
       <c r="A101" s="9" t="s">
         <v>323</v>
       </c>
@@ -3308,7 +3315,7 @@
       </c>
       <c r="E101" s="7"/>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5">
       <c r="A102" s="9" t="s">
         <v>328</v>
       </c>
@@ -3323,7 +3330,7 @@
       </c>
       <c r="E102" s="7"/>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5">
       <c r="A103" s="9" t="s">
         <v>333</v>
       </c>
@@ -3338,7 +3345,7 @@
       </c>
       <c r="E103" s="7"/>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5">
       <c r="A104" s="9" t="s">
         <v>336</v>
       </c>
@@ -3353,7 +3360,7 @@
       </c>
       <c r="E104" s="7"/>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5">
       <c r="A105" s="9" t="s">
         <v>337</v>
       </c>
@@ -3368,7 +3375,7 @@
       </c>
       <c r="E105" s="7"/>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5">
       <c r="A106" s="9" t="s">
         <v>342</v>
       </c>
@@ -3383,7 +3390,7 @@
       </c>
       <c r="E106" s="7"/>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5">
       <c r="A107" s="9" t="s">
         <v>345</v>
       </c>
@@ -3398,7 +3405,7 @@
       </c>
       <c r="E107" s="7"/>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5">
       <c r="A108" s="9" t="s">
         <v>350</v>
       </c>
@@ -3413,7 +3420,7 @@
       </c>
       <c r="E108" s="7"/>
     </row>
-    <row r="109" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" ht="30">
       <c r="A109" s="9" t="s">
         <v>351</v>
       </c>
@@ -3428,7 +3435,7 @@
       </c>
       <c r="E109" s="7"/>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5">
       <c r="A110" s="9" t="s">
         <v>354</v>
       </c>
@@ -3443,7 +3450,7 @@
       </c>
       <c r="E110" s="7"/>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5">
       <c r="A111" s="9" t="s">
         <v>357</v>
       </c>
@@ -3458,7 +3465,7 @@
       </c>
       <c r="E111" s="7"/>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5">
       <c r="A112" s="9" t="s">
         <v>361</v>
       </c>
@@ -3473,7 +3480,7 @@
       </c>
       <c r="E112" s="7"/>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5">
       <c r="A113" s="17" t="s">
         <v>363</v>
       </c>
@@ -3488,7 +3495,7 @@
       </c>
       <c r="E113" s="19"/>
     </row>
-    <row r="114" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" ht="30">
       <c r="A114" s="9" t="s">
         <v>366</v>
       </c>
@@ -3503,7 +3510,7 @@
       </c>
       <c r="E114" s="7"/>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5">
       <c r="A115" s="9" t="s">
         <v>369</v>
       </c>
@@ -3518,7 +3525,7 @@
       </c>
       <c r="E115" s="7"/>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5">
       <c r="A116" s="9" t="s">
         <v>370</v>
       </c>
@@ -3533,7 +3540,7 @@
       </c>
       <c r="E116" s="7"/>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5">
       <c r="A117" s="9" t="s">
         <v>371</v>
       </c>
@@ -3548,7 +3555,7 @@
       </c>
       <c r="E117" s="7"/>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5">
       <c r="A118" s="9" t="s">
         <v>378</v>
       </c>
@@ -3563,7 +3570,7 @@
       </c>
       <c r="E118" s="7"/>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5">
       <c r="A119" s="9" t="s">
         <v>381</v>
       </c>
@@ -3578,7 +3585,7 @@
       </c>
       <c r="E119" s="7"/>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5">
       <c r="A120" s="9" t="s">
         <v>384</v>
       </c>
@@ -3593,7 +3600,7 @@
       </c>
       <c r="E120" s="7"/>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5">
       <c r="A121" s="9" t="s">
         <v>387</v>
       </c>
@@ -3608,7 +3615,7 @@
       </c>
       <c r="E121" s="7"/>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5">
       <c r="A122" s="7" t="s">
         <v>390</v>
       </c>
@@ -3623,7 +3630,7 @@
       </c>
       <c r="E122" s="7"/>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5">
       <c r="A123" s="7" t="s">
         <v>393</v>
       </c>
@@ -3638,7 +3645,7 @@
       </c>
       <c r="E123" s="7"/>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5">
       <c r="A124" s="7" t="s">
         <v>396</v>
       </c>
@@ -3653,7 +3660,7 @@
       </c>
       <c r="E124" s="7"/>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5">
       <c r="A125" s="9" t="s">
         <v>399</v>
       </c>
@@ -3668,7 +3675,7 @@
       </c>
       <c r="E125" s="7"/>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5">
       <c r="A126" s="7" t="s">
         <v>402</v>
       </c>
@@ -3683,7 +3690,7 @@
       </c>
       <c r="E126" s="7"/>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5">
       <c r="A127" s="7" t="s">
         <v>405</v>
       </c>
@@ -3698,7 +3705,7 @@
       </c>
       <c r="E127" s="7"/>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5">
       <c r="A128" s="7" t="s">
         <v>408</v>
       </c>
@@ -3713,7 +3720,7 @@
       </c>
       <c r="E128" s="7"/>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5">
       <c r="A129" s="9" t="s">
         <v>411</v>
       </c>
@@ -3728,7 +3735,7 @@
       </c>
       <c r="E129" s="7"/>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5">
       <c r="A130" s="9" t="s">
         <v>414</v>
       </c>
@@ -3743,7 +3750,7 @@
       </c>
       <c r="E130" s="7"/>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5">
       <c r="A131" s="9" t="s">
         <v>416</v>
       </c>
@@ -3757,6 +3764,21 @@
         <v>5</v>
       </c>
       <c r="E131" s="7"/>
+    </row>
+    <row r="132" spans="1:5">
+      <c r="A132" s="7" t="s">
+        <v>419</v>
+      </c>
+      <c r="B132" s="7" t="s">
+        <v>420</v>
+      </c>
+      <c r="C132" s="8" t="s">
+        <v>421</v>
+      </c>
+      <c r="D132" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E132" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -3769,14 +3791,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView topLeftCell="A10" zoomScale="80" workbookViewId="0">
       <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
@@ -3784,7 +3806,7 @@
     <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="10" t="s">
         <v>35</v>
       </c>
@@ -3798,7 +3820,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="7" t="s">
         <v>37</v>
       </c>
@@ -3810,7 +3832,7 @@
       </c>
       <c r="D2" s="7"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="7" t="s">
         <v>38</v>
       </c>
@@ -3822,7 +3844,7 @@
       </c>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="7" t="s">
         <v>39</v>
       </c>
@@ -3834,7 +3856,7 @@
       </c>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" s="7" t="s">
         <v>40</v>
       </c>
@@ -3846,7 +3868,7 @@
       </c>
       <c r="D5" s="7"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" s="7" t="s">
         <v>41</v>
       </c>
@@ -3858,7 +3880,7 @@
       </c>
       <c r="D6" s="7"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="7" t="s">
         <v>42</v>
       </c>
@@ -3870,7 +3892,7 @@
       </c>
       <c r="D7" s="7"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="7" t="s">
         <v>43</v>
       </c>
@@ -3882,7 +3904,7 @@
       </c>
       <c r="D8" s="7"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="7" t="s">
         <v>44</v>
       </c>
@@ -3894,7 +3916,7 @@
       </c>
       <c r="D9" s="7"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="7" t="s">
         <v>45</v>
       </c>
@@ -3906,7 +3928,7 @@
       </c>
       <c r="D10" s="7"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11" s="7" t="s">
         <v>46</v>
       </c>
@@ -3918,7 +3940,7 @@
       </c>
       <c r="D11" s="7"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="A12" s="7" t="s">
         <v>48</v>
       </c>
@@ -3930,7 +3952,7 @@
       </c>
       <c r="D12" s="7"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="A13" s="7" t="s">
         <v>49</v>
       </c>
@@ -3942,7 +3964,7 @@
       </c>
       <c r="D13" s="7"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="A14" s="7" t="s">
         <v>50</v>
       </c>
@@ -3954,7 +3976,7 @@
       </c>
       <c r="D14" s="7"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="A15" s="7" t="s">
         <v>51</v>
       </c>
@@ -3966,7 +3988,7 @@
       </c>
       <c r="D15" s="7"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="A16" s="7" t="s">
         <v>52</v>
       </c>
@@ -3978,7 +4000,7 @@
       </c>
       <c r="D16" s="7"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4">
       <c r="A17" s="7" t="s">
         <v>53</v>
       </c>
@@ -3990,7 +4012,7 @@
       </c>
       <c r="D17" s="7"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4">
       <c r="A18" s="7" t="s">
         <v>54</v>
       </c>
@@ -4002,7 +4024,7 @@
       </c>
       <c r="D18" s="7"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4">
       <c r="A19" s="7" t="s">
         <v>55</v>
       </c>
@@ -4014,7 +4036,7 @@
       </c>
       <c r="D19" s="7"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4">
       <c r="A20" s="7" t="s">
         <v>56</v>
       </c>
@@ -4026,7 +4048,7 @@
       </c>
       <c r="D20" s="7"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4">
       <c r="A21" s="7" t="s">
         <v>57</v>
       </c>
@@ -4038,7 +4060,7 @@
       </c>
       <c r="D21" s="7"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4">
       <c r="A22" s="7" t="s">
         <v>58</v>
       </c>
@@ -4050,7 +4072,7 @@
       </c>
       <c r="D22" s="7"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4">
       <c r="A23" s="7" t="s">
         <v>59</v>
       </c>
@@ -4062,7 +4084,7 @@
       </c>
       <c r="D23" s="7"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4">
       <c r="A24" s="7" t="s">
         <v>60</v>
       </c>
@@ -4074,7 +4096,7 @@
       </c>
       <c r="D24" s="7"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4">
       <c r="A25" s="7" t="s">
         <v>61</v>
       </c>
@@ -4086,7 +4108,7 @@
       </c>
       <c r="D25" s="7"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4">
       <c r="A26" s="7" t="s">
         <v>47</v>
       </c>
@@ -4105,14 +4127,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A19" sqref="A19:XFD19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
@@ -4120,7 +4142,7 @@
     <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="10" t="s">
         <v>35</v>
       </c>
@@ -4134,7 +4156,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="7" t="s">
         <v>37</v>
       </c>
@@ -4146,7 +4168,7 @@
       </c>
       <c r="D2" s="7"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="7" t="s">
         <v>38</v>
       </c>
@@ -4158,7 +4180,7 @@
       </c>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="7" t="s">
         <v>39</v>
       </c>
@@ -4170,7 +4192,7 @@
       </c>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" s="7" t="s">
         <v>40</v>
       </c>
@@ -4182,7 +4204,7 @@
       </c>
       <c r="D5" s="7"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" s="7" t="s">
         <v>41</v>
       </c>
@@ -4194,7 +4216,7 @@
       </c>
       <c r="D6" s="7"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="7" t="s">
         <v>42</v>
       </c>
@@ -4206,7 +4228,7 @@
       </c>
       <c r="D7" s="7"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="7" t="s">
         <v>43</v>
       </c>
@@ -4218,7 +4240,7 @@
       </c>
       <c r="D8" s="7"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="7" t="s">
         <v>44</v>
       </c>
@@ -4230,7 +4252,7 @@
       </c>
       <c r="D9" s="7"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="7" t="s">
         <v>45</v>
       </c>
@@ -4242,7 +4264,7 @@
       </c>
       <c r="D10" s="7"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11" s="7" t="s">
         <v>46</v>
       </c>
@@ -4254,7 +4276,7 @@
       </c>
       <c r="D11" s="7"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="A12" s="7" t="s">
         <v>47</v>
       </c>
@@ -4266,7 +4288,7 @@
       </c>
       <c r="D12" s="7"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="A13" s="7" t="s">
         <v>48</v>
       </c>
@@ -4278,7 +4300,7 @@
       </c>
       <c r="D13" s="7"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="A14" s="7" t="s">
         <v>49</v>
       </c>
@@ -4290,7 +4312,7 @@
       </c>
       <c r="D14" s="7"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="A15" s="7" t="s">
         <v>50</v>
       </c>
@@ -4302,7 +4324,7 @@
       </c>
       <c r="D15" s="7"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="A16" s="7" t="s">
         <v>51</v>
       </c>
@@ -4314,7 +4336,7 @@
       </c>
       <c r="D16" s="7"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4">
       <c r="A17" s="7" t="s">
         <v>52</v>
       </c>
@@ -4326,7 +4348,7 @@
       </c>
       <c r="D17" s="7"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4">
       <c r="A18" s="7" t="s">
         <v>53</v>
       </c>
@@ -4338,7 +4360,7 @@
       </c>
       <c r="D18" s="7"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4">
       <c r="A19" s="7" t="s">
         <v>54</v>
       </c>
@@ -4350,7 +4372,7 @@
       </c>
       <c r="D19" s="7"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4">
       <c r="A20" s="7" t="s">
         <v>55</v>
       </c>
@@ -4362,7 +4384,7 @@
       </c>
       <c r="D20" s="7"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4">
       <c r="A21" s="7" t="s">
         <v>56</v>
       </c>
@@ -4374,7 +4396,7 @@
       </c>
       <c r="D21" s="7"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4">
       <c r="A22" s="7" t="s">
         <v>57</v>
       </c>
@@ -4386,7 +4408,7 @@
       </c>
       <c r="D22" s="7"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4">
       <c r="A23" s="7" t="s">
         <v>58</v>
       </c>
@@ -4398,7 +4420,7 @@
       </c>
       <c r="D23" s="7"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4">
       <c r="A24" s="7" t="s">
         <v>59</v>
       </c>
@@ -4410,7 +4432,7 @@
       </c>
       <c r="D24" s="7"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4">
       <c r="A25" s="7" t="s">
         <v>60</v>
       </c>
@@ -4422,7 +4444,7 @@
       </c>
       <c r="D25" s="7"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4">
       <c r="A26" s="7" t="s">
         <v>61</v>
       </c>

</xml_diff>

<commit_message>
Adds WAT-123 testscript and related chnages
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/WAT.xlsx
+++ b/src/test/resources/xls/WAT.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13305" windowHeight="2415"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="699" uniqueCount="431">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="703" uniqueCount="434">
   <si>
     <t>TCID</t>
   </si>
@@ -1310,13 +1310,22 @@
   </si>
   <si>
     <t>Verify that System displays the author's last known organization (when available). || Verify that System displays the author's last know sub-organization (when available).</t>
+  </si>
+  <si>
+    <t>WAT123</t>
+  </si>
+  <si>
+    <t>WAT-587</t>
+  </si>
+  <si>
+    <t>Verify the static text in Author record Page</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1568,7 +1577,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1600,9 +1609,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1634,6 +1644,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1809,14 +1820,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E135"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E136"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A118" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C141" sqref="C140:C141"/>
+      <selection activeCell="C147" sqref="C147"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="41" bestFit="1" customWidth="1" collapsed="1"/>
@@ -1825,7 +1836,7 @@
     <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1842,7 +1853,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -1857,7 +1868,7 @@
       </c>
       <c r="E2" s="4"/>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -1872,7 +1883,7 @@
       </c>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>11</v>
       </c>
@@ -1887,7 +1898,7 @@
       </c>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>12</v>
       </c>
@@ -1902,7 +1913,7 @@
       </c>
       <c r="E5" s="7"/>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>14</v>
       </c>
@@ -1917,7 +1928,7 @@
       </c>
       <c r="E6" s="7"/>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>17</v>
       </c>
@@ -1932,7 +1943,7 @@
       </c>
       <c r="E7" s="7"/>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>20</v>
       </c>
@@ -1947,7 +1958,7 @@
       </c>
       <c r="E8" s="7"/>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>22</v>
       </c>
@@ -1962,7 +1973,7 @@
       </c>
       <c r="E9" s="7"/>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>23</v>
       </c>
@@ -1977,7 +1988,7 @@
       </c>
       <c r="E10" s="7"/>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>24</v>
       </c>
@@ -1992,7 +2003,7 @@
       </c>
       <c r="E11" s="7"/>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>25</v>
       </c>
@@ -2007,7 +2018,7 @@
       </c>
       <c r="E12" s="7"/>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>62</v>
       </c>
@@ -2022,7 +2033,7 @@
       </c>
       <c r="E13" s="7"/>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>63</v>
       </c>
@@ -2037,7 +2048,7 @@
       </c>
       <c r="E14" s="7"/>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>64</v>
       </c>
@@ -2052,7 +2063,7 @@
       </c>
       <c r="E15" s="7"/>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>65</v>
       </c>
@@ -2067,7 +2078,7 @@
       </c>
       <c r="E16" s="7"/>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>74</v>
       </c>
@@ -2082,7 +2093,7 @@
       </c>
       <c r="E17" s="7"/>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>75</v>
       </c>
@@ -2097,7 +2108,7 @@
       </c>
       <c r="E18" s="7"/>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>79</v>
       </c>
@@ -2112,7 +2123,7 @@
       </c>
       <c r="E19" s="7"/>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>81</v>
       </c>
@@ -2127,7 +2138,7 @@
       </c>
       <c r="E20" s="7"/>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>82</v>
       </c>
@@ -2142,7 +2153,7 @@
       </c>
       <c r="E21" s="7"/>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>88</v>
       </c>
@@ -2157,7 +2168,7 @@
       </c>
       <c r="E22" s="7"/>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>90</v>
       </c>
@@ -2172,7 +2183,7 @@
       </c>
       <c r="E23" s="7"/>
     </row>
-    <row r="24" spans="1:5" ht="30">
+    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>94</v>
       </c>
@@ -2187,7 +2198,7 @@
       </c>
       <c r="E24" s="7"/>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>96</v>
       </c>
@@ -2202,7 +2213,7 @@
       </c>
       <c r="E25" s="7"/>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
         <v>98</v>
       </c>
@@ -2217,7 +2228,7 @@
       </c>
       <c r="E26" s="7"/>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
         <v>102</v>
       </c>
@@ -2232,7 +2243,7 @@
       </c>
       <c r="E27" s="7"/>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
         <v>105</v>
       </c>
@@ -2247,7 +2258,7 @@
       </c>
       <c r="E28" s="7"/>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
         <v>108</v>
       </c>
@@ -2262,7 +2273,7 @@
       </c>
       <c r="E29" s="7"/>
     </row>
-    <row r="30" spans="1:5" ht="30">
+    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
         <v>110</v>
       </c>
@@ -2277,7 +2288,7 @@
       </c>
       <c r="E30" s="7"/>
     </row>
-    <row r="31" spans="1:5" ht="30">
+    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
         <v>114</v>
       </c>
@@ -2292,7 +2303,7 @@
       </c>
       <c r="E31" s="7"/>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
         <v>119</v>
       </c>
@@ -2307,7 +2318,7 @@
       </c>
       <c r="E32" s="7"/>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
         <v>120</v>
       </c>
@@ -2322,7 +2333,7 @@
       </c>
       <c r="E33" s="7"/>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
         <v>125</v>
       </c>
@@ -2337,7 +2348,7 @@
       </c>
       <c r="E34" s="7"/>
     </row>
-    <row r="35" spans="1:5" ht="30">
+    <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
         <v>128</v>
       </c>
@@ -2352,7 +2363,7 @@
       </c>
       <c r="E35" s="7"/>
     </row>
-    <row r="36" spans="1:5" ht="30">
+    <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
         <v>131</v>
       </c>
@@ -2367,7 +2378,7 @@
       </c>
       <c r="E36" s="7"/>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
         <v>134</v>
       </c>
@@ -2382,7 +2393,7 @@
       </c>
       <c r="E37" s="7"/>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="9" t="s">
         <v>137</v>
       </c>
@@ -2397,7 +2408,7 @@
       </c>
       <c r="E38" s="7"/>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="s">
         <v>140</v>
       </c>
@@ -2412,7 +2423,7 @@
       </c>
       <c r="E39" s="7"/>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="9" t="s">
         <v>143</v>
       </c>
@@ -2427,7 +2438,7 @@
       </c>
       <c r="E40" s="7"/>
     </row>
-    <row r="41" spans="1:5" ht="30">
+    <row r="41" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
         <v>145</v>
       </c>
@@ -2442,7 +2453,7 @@
       </c>
       <c r="E41" s="7"/>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="9" t="s">
         <v>147</v>
       </c>
@@ -2457,7 +2468,7 @@
       </c>
       <c r="E42" s="7"/>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="9" t="s">
         <v>150</v>
       </c>
@@ -2472,7 +2483,7 @@
       </c>
       <c r="E43" s="7"/>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="9" t="s">
         <v>153</v>
       </c>
@@ -2487,7 +2498,7 @@
       </c>
       <c r="E44" s="7"/>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="9" t="s">
         <v>155</v>
       </c>
@@ -2502,7 +2513,7 @@
       </c>
       <c r="E45" s="7"/>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="12" t="s">
         <v>158</v>
       </c>
@@ -2517,7 +2528,7 @@
       </c>
       <c r="E46" s="7"/>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="12" t="s">
         <v>159</v>
       </c>
@@ -2532,7 +2543,7 @@
       </c>
       <c r="E47" s="7"/>
     </row>
-    <row r="48" spans="1:5" ht="30">
+    <row r="48" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="12" t="s">
         <v>160</v>
       </c>
@@ -2547,7 +2558,7 @@
       </c>
       <c r="E48" s="7"/>
     </row>
-    <row r="49" spans="1:5" ht="30">
+    <row r="49" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="12" t="s">
         <v>161</v>
       </c>
@@ -2562,7 +2573,7 @@
       </c>
       <c r="E49" s="7"/>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="12" t="s">
         <v>164</v>
       </c>
@@ -2577,7 +2588,7 @@
       </c>
       <c r="E50" s="7"/>
     </row>
-    <row r="51" spans="1:5" ht="30">
+    <row r="51" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="9" t="s">
         <v>173</v>
       </c>
@@ -2592,7 +2603,7 @@
       </c>
       <c r="E51" s="7"/>
     </row>
-    <row r="52" spans="1:5">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="9" t="s">
         <v>174</v>
       </c>
@@ -2607,7 +2618,7 @@
       </c>
       <c r="E52" s="7"/>
     </row>
-    <row r="53" spans="1:5">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="9" t="s">
         <v>179</v>
       </c>
@@ -2622,7 +2633,7 @@
       </c>
       <c r="E53" s="7"/>
     </row>
-    <row r="54" spans="1:5">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="9" t="s">
         <v>180</v>
       </c>
@@ -2637,7 +2648,7 @@
       </c>
       <c r="E54" s="7"/>
     </row>
-    <row r="55" spans="1:5">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="9" t="s">
         <v>185</v>
       </c>
@@ -2652,7 +2663,7 @@
       </c>
       <c r="E55" s="7"/>
     </row>
-    <row r="56" spans="1:5">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="s">
         <v>188</v>
       </c>
@@ -2667,7 +2678,7 @@
       </c>
       <c r="E56" s="7"/>
     </row>
-    <row r="57" spans="1:5" ht="30">
+    <row r="57" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="9" t="s">
         <v>191</v>
       </c>
@@ -2682,7 +2693,7 @@
       </c>
       <c r="E57" s="7"/>
     </row>
-    <row r="58" spans="1:5">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="9" t="s">
         <v>194</v>
       </c>
@@ -2697,7 +2708,7 @@
       </c>
       <c r="E58" s="7"/>
     </row>
-    <row r="59" spans="1:5">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
         <v>196</v>
       </c>
@@ -2712,7 +2723,7 @@
       </c>
       <c r="E59" s="7"/>
     </row>
-    <row r="60" spans="1:5" ht="45">
+    <row r="60" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
         <v>199</v>
       </c>
@@ -2727,7 +2738,7 @@
       </c>
       <c r="E60" s="7"/>
     </row>
-    <row r="61" spans="1:5">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="9" t="s">
         <v>202</v>
       </c>
@@ -2742,7 +2753,7 @@
       </c>
       <c r="E61" s="7"/>
     </row>
-    <row r="62" spans="1:5">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="9" t="s">
         <v>204</v>
       </c>
@@ -2757,7 +2768,7 @@
       </c>
       <c r="E62" s="7"/>
     </row>
-    <row r="63" spans="1:5">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="9" t="s">
         <v>206</v>
       </c>
@@ -2772,7 +2783,7 @@
       </c>
       <c r="E63" s="7"/>
     </row>
-    <row r="64" spans="1:5">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="9" t="s">
         <v>208</v>
       </c>
@@ -2787,7 +2798,7 @@
       </c>
       <c r="E64" s="7"/>
     </row>
-    <row r="65" spans="1:5">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="9" t="s">
         <v>217</v>
       </c>
@@ -2802,7 +2813,7 @@
       </c>
       <c r="E65" s="7"/>
     </row>
-    <row r="66" spans="1:5">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="9" t="s">
         <v>218</v>
       </c>
@@ -2817,7 +2828,7 @@
       </c>
       <c r="E66" s="7"/>
     </row>
-    <row r="67" spans="1:5">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="9" t="s">
         <v>223</v>
       </c>
@@ -2832,7 +2843,7 @@
       </c>
       <c r="E67" s="7"/>
     </row>
-    <row r="68" spans="1:5">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="9" t="s">
         <v>224</v>
       </c>
@@ -2847,7 +2858,7 @@
       </c>
       <c r="E68" s="7"/>
     </row>
-    <row r="69" spans="1:5">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="9" t="s">
         <v>225</v>
       </c>
@@ -2862,7 +2873,7 @@
       </c>
       <c r="E69" s="7"/>
     </row>
-    <row r="70" spans="1:5">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="9" t="s">
         <v>226</v>
       </c>
@@ -2877,7 +2888,7 @@
       </c>
       <c r="E70" s="7"/>
     </row>
-    <row r="71" spans="1:5">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="9" t="s">
         <v>233</v>
       </c>
@@ -2892,7 +2903,7 @@
       </c>
       <c r="E71" s="7"/>
     </row>
-    <row r="72" spans="1:5">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="9" t="s">
         <v>237</v>
       </c>
@@ -2907,7 +2918,7 @@
       </c>
       <c r="E72" s="7"/>
     </row>
-    <row r="73" spans="1:5">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="9" t="s">
         <v>239</v>
       </c>
@@ -2922,7 +2933,7 @@
       </c>
       <c r="E73" s="7"/>
     </row>
-    <row r="74" spans="1:5">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="9" t="s">
         <v>243</v>
       </c>
@@ -2937,7 +2948,7 @@
       </c>
       <c r="E74" s="7"/>
     </row>
-    <row r="75" spans="1:5" ht="30">
+    <row r="75" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" s="9" t="s">
         <v>245</v>
       </c>
@@ -2952,7 +2963,7 @@
       </c>
       <c r="E75" s="7"/>
     </row>
-    <row r="76" spans="1:5">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="9" t="s">
         <v>248</v>
       </c>
@@ -2967,7 +2978,7 @@
       </c>
       <c r="E76" s="7"/>
     </row>
-    <row r="77" spans="1:5">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="9" t="s">
         <v>256</v>
       </c>
@@ -2982,7 +2993,7 @@
       </c>
       <c r="E77" s="7"/>
     </row>
-    <row r="78" spans="1:5">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="9" t="s">
         <v>257</v>
       </c>
@@ -2997,7 +3008,7 @@
       </c>
       <c r="E78" s="7"/>
     </row>
-    <row r="79" spans="1:5">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="9" t="s">
         <v>261</v>
       </c>
@@ -3012,7 +3023,7 @@
       </c>
       <c r="E79" s="7"/>
     </row>
-    <row r="80" spans="1:5">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="9" t="s">
         <v>264</v>
       </c>
@@ -3027,7 +3038,7 @@
       </c>
       <c r="E80" s="7"/>
     </row>
-    <row r="81" spans="1:5">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="9" t="s">
         <v>267</v>
       </c>
@@ -3042,7 +3053,7 @@
       </c>
       <c r="E81" s="7"/>
     </row>
-    <row r="82" spans="1:5" ht="30">
+    <row r="82" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A82" s="9" t="s">
         <v>269</v>
       </c>
@@ -3057,7 +3068,7 @@
       </c>
       <c r="E82" s="7"/>
     </row>
-    <row r="83" spans="1:5">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="9" t="s">
         <v>274</v>
       </c>
@@ -3072,7 +3083,7 @@
       </c>
       <c r="E83" s="7"/>
     </row>
-    <row r="84" spans="1:5" ht="30">
+    <row r="84" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A84" s="9" t="s">
         <v>277</v>
       </c>
@@ -3087,7 +3098,7 @@
       </c>
       <c r="E84" s="7"/>
     </row>
-    <row r="85" spans="1:5">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="9" t="s">
         <v>279</v>
       </c>
@@ -3102,7 +3113,7 @@
       </c>
       <c r="E85" s="7"/>
     </row>
-    <row r="86" spans="1:5">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="9" t="s">
         <v>282</v>
       </c>
@@ -3117,7 +3128,7 @@
       </c>
       <c r="E86" s="7"/>
     </row>
-    <row r="87" spans="1:5">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="9" t="s">
         <v>285</v>
       </c>
@@ -3132,7 +3143,7 @@
       </c>
       <c r="E87" s="7"/>
     </row>
-    <row r="88" spans="1:5">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="9" t="s">
         <v>288</v>
       </c>
@@ -3147,7 +3158,7 @@
       </c>
       <c r="E88" s="7"/>
     </row>
-    <row r="89" spans="1:5">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="9" t="s">
         <v>291</v>
       </c>
@@ -3162,7 +3173,7 @@
       </c>
       <c r="E89" s="7"/>
     </row>
-    <row r="90" spans="1:5">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="9" t="s">
         <v>294</v>
       </c>
@@ -3177,7 +3188,7 @@
       </c>
       <c r="E90" s="7"/>
     </row>
-    <row r="91" spans="1:5">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="9" t="s">
         <v>297</v>
       </c>
@@ -3192,7 +3203,7 @@
       </c>
       <c r="E91" s="7"/>
     </row>
-    <row r="92" spans="1:5">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="9" t="s">
         <v>300</v>
       </c>
@@ -3207,7 +3218,7 @@
       </c>
       <c r="E92" s="7"/>
     </row>
-    <row r="93" spans="1:5">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="9" t="s">
         <v>303</v>
       </c>
@@ -3222,7 +3233,7 @@
       </c>
       <c r="E93" s="7"/>
     </row>
-    <row r="94" spans="1:5">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="9" t="s">
         <v>306</v>
       </c>
@@ -3237,7 +3248,7 @@
       </c>
       <c r="E94" s="7"/>
     </row>
-    <row r="95" spans="1:5">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="9" t="s">
         <v>309</v>
       </c>
@@ -3252,7 +3263,7 @@
       </c>
       <c r="E95" s="7"/>
     </row>
-    <row r="96" spans="1:5">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="9" t="s">
         <v>314</v>
       </c>
@@ -3267,7 +3278,7 @@
       </c>
       <c r="E96" s="7"/>
     </row>
-    <row r="97" spans="1:5">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="9" t="s">
         <v>315</v>
       </c>
@@ -3282,7 +3293,7 @@
       </c>
       <c r="E97" s="7"/>
     </row>
-    <row r="98" spans="1:5">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="9" t="s">
         <v>319</v>
       </c>
@@ -3297,7 +3308,7 @@
       </c>
       <c r="E98" s="7"/>
     </row>
-    <row r="99" spans="1:5">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="9" t="s">
         <v>321</v>
       </c>
@@ -3312,7 +3323,7 @@
       </c>
       <c r="E99" s="7"/>
     </row>
-    <row r="100" spans="1:5">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="9" t="s">
         <v>322</v>
       </c>
@@ -3327,7 +3338,7 @@
       </c>
       <c r="E100" s="7"/>
     </row>
-    <row r="101" spans="1:5" ht="30">
+    <row r="101" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A101" s="9" t="s">
         <v>323</v>
       </c>
@@ -3342,7 +3353,7 @@
       </c>
       <c r="E101" s="7"/>
     </row>
-    <row r="102" spans="1:5">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="9" t="s">
         <v>328</v>
       </c>
@@ -3357,7 +3368,7 @@
       </c>
       <c r="E102" s="7"/>
     </row>
-    <row r="103" spans="1:5">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="9" t="s">
         <v>333</v>
       </c>
@@ -3372,7 +3383,7 @@
       </c>
       <c r="E103" s="7"/>
     </row>
-    <row r="104" spans="1:5">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="9" t="s">
         <v>336</v>
       </c>
@@ -3387,7 +3398,7 @@
       </c>
       <c r="E104" s="7"/>
     </row>
-    <row r="105" spans="1:5">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="9" t="s">
         <v>337</v>
       </c>
@@ -3402,7 +3413,7 @@
       </c>
       <c r="E105" s="7"/>
     </row>
-    <row r="106" spans="1:5">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="9" t="s">
         <v>342</v>
       </c>
@@ -3417,7 +3428,7 @@
       </c>
       <c r="E106" s="7"/>
     </row>
-    <row r="107" spans="1:5">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="9" t="s">
         <v>345</v>
       </c>
@@ -3432,7 +3443,7 @@
       </c>
       <c r="E107" s="7"/>
     </row>
-    <row r="108" spans="1:5">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="9" t="s">
         <v>350</v>
       </c>
@@ -3447,7 +3458,7 @@
       </c>
       <c r="E108" s="7"/>
     </row>
-    <row r="109" spans="1:5" ht="30">
+    <row r="109" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A109" s="9" t="s">
         <v>351</v>
       </c>
@@ -3462,7 +3473,7 @@
       </c>
       <c r="E109" s="7"/>
     </row>
-    <row r="110" spans="1:5">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="9" t="s">
         <v>354</v>
       </c>
@@ -3477,7 +3488,7 @@
       </c>
       <c r="E110" s="7"/>
     </row>
-    <row r="111" spans="1:5">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="9" t="s">
         <v>357</v>
       </c>
@@ -3492,7 +3503,7 @@
       </c>
       <c r="E111" s="7"/>
     </row>
-    <row r="112" spans="1:5">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="9" t="s">
         <v>361</v>
       </c>
@@ -3507,7 +3518,7 @@
       </c>
       <c r="E112" s="7"/>
     </row>
-    <row r="113" spans="1:5">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="17" t="s">
         <v>363</v>
       </c>
@@ -3522,7 +3533,7 @@
       </c>
       <c r="E113" s="19"/>
     </row>
-    <row r="114" spans="1:5" ht="30">
+    <row r="114" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A114" s="9" t="s">
         <v>366</v>
       </c>
@@ -3537,7 +3548,7 @@
       </c>
       <c r="E114" s="7"/>
     </row>
-    <row r="115" spans="1:5">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="9" t="s">
         <v>369</v>
       </c>
@@ -3552,7 +3563,7 @@
       </c>
       <c r="E115" s="7"/>
     </row>
-    <row r="116" spans="1:5">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="9" t="s">
         <v>370</v>
       </c>
@@ -3567,7 +3578,7 @@
       </c>
       <c r="E116" s="7"/>
     </row>
-    <row r="117" spans="1:5">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" s="9" t="s">
         <v>371</v>
       </c>
@@ -3582,7 +3593,7 @@
       </c>
       <c r="E117" s="7"/>
     </row>
-    <row r="118" spans="1:5">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" s="9" t="s">
         <v>378</v>
       </c>
@@ -3597,7 +3608,7 @@
       </c>
       <c r="E118" s="7"/>
     </row>
-    <row r="119" spans="1:5">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" s="9" t="s">
         <v>381</v>
       </c>
@@ -3612,7 +3623,7 @@
       </c>
       <c r="E119" s="7"/>
     </row>
-    <row r="120" spans="1:5">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" s="9" t="s">
         <v>384</v>
       </c>
@@ -3627,7 +3638,7 @@
       </c>
       <c r="E120" s="7"/>
     </row>
-    <row r="121" spans="1:5">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="9" t="s">
         <v>387</v>
       </c>
@@ -3642,7 +3653,7 @@
       </c>
       <c r="E121" s="7"/>
     </row>
-    <row r="122" spans="1:5">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" s="7" t="s">
         <v>390</v>
       </c>
@@ -3657,7 +3668,7 @@
       </c>
       <c r="E122" s="7"/>
     </row>
-    <row r="123" spans="1:5">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" s="7" t="s">
         <v>393</v>
       </c>
@@ -3672,7 +3683,7 @@
       </c>
       <c r="E123" s="7"/>
     </row>
-    <row r="124" spans="1:5">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" s="7" t="s">
         <v>396</v>
       </c>
@@ -3687,7 +3698,7 @@
       </c>
       <c r="E124" s="7"/>
     </row>
-    <row r="125" spans="1:5">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" s="9" t="s">
         <v>399</v>
       </c>
@@ -3702,7 +3713,7 @@
       </c>
       <c r="E125" s="7"/>
     </row>
-    <row r="126" spans="1:5">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" s="7" t="s">
         <v>402</v>
       </c>
@@ -3717,7 +3728,7 @@
       </c>
       <c r="E126" s="7"/>
     </row>
-    <row r="127" spans="1:5">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" s="7" t="s">
         <v>405</v>
       </c>
@@ -3732,7 +3743,7 @@
       </c>
       <c r="E127" s="7"/>
     </row>
-    <row r="128" spans="1:5">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" s="7" t="s">
         <v>408</v>
       </c>
@@ -3747,7 +3758,7 @@
       </c>
       <c r="E128" s="7"/>
     </row>
-    <row r="129" spans="1:5">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" s="9" t="s">
         <v>411</v>
       </c>
@@ -3762,7 +3773,7 @@
       </c>
       <c r="E129" s="7"/>
     </row>
-    <row r="130" spans="1:5">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" s="9" t="s">
         <v>414</v>
       </c>
@@ -3777,7 +3788,7 @@
       </c>
       <c r="E130" s="7"/>
     </row>
-    <row r="131" spans="1:5">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" s="9" t="s">
         <v>416</v>
       </c>
@@ -3792,7 +3803,7 @@
       </c>
       <c r="E131" s="7"/>
     </row>
-    <row r="132" spans="1:5">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" s="7" t="s">
         <v>419</v>
       </c>
@@ -3807,7 +3818,7 @@
       </c>
       <c r="E132" s="7"/>
     </row>
-    <row r="133" spans="1:5">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" s="9" t="s">
         <v>422</v>
       </c>
@@ -3822,7 +3833,7 @@
       </c>
       <c r="E133" s="7"/>
     </row>
-    <row r="134" spans="1:5" ht="30">
+    <row r="134" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A134" s="7" t="s">
         <v>425</v>
       </c>
@@ -3837,7 +3848,7 @@
       </c>
       <c r="E134" s="7"/>
     </row>
-    <row r="135" spans="1:5" ht="30">
+    <row r="135" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A135" s="7" t="s">
         <v>426</v>
       </c>
@@ -3851,6 +3862,21 @@
         <v>5</v>
       </c>
       <c r="E135" s="7"/>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A136" s="9" t="s">
+        <v>431</v>
+      </c>
+      <c r="B136" s="7" t="s">
+        <v>432</v>
+      </c>
+      <c r="C136" s="7" t="s">
+        <v>433</v>
+      </c>
+      <c r="D136" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E136" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -3863,14 +3889,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView topLeftCell="A10" zoomScale="80" workbookViewId="0">
       <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
@@ -3878,7 +3904,7 @@
     <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>35</v>
       </c>
@@ -3892,7 +3918,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>37</v>
       </c>
@@ -3904,7 +3930,7 @@
       </c>
       <c r="D2" s="7"/>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>38</v>
       </c>
@@ -3916,7 +3942,7 @@
       </c>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>39</v>
       </c>
@@ -3928,7 +3954,7 @@
       </c>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>40</v>
       </c>
@@ -3940,7 +3966,7 @@
       </c>
       <c r="D5" s="7"/>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>41</v>
       </c>
@@ -3952,7 +3978,7 @@
       </c>
       <c r="D6" s="7"/>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>42</v>
       </c>
@@ -3964,7 +3990,7 @@
       </c>
       <c r="D7" s="7"/>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>43</v>
       </c>
@@ -3976,7 +4002,7 @@
       </c>
       <c r="D8" s="7"/>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>44</v>
       </c>
@@ -3988,7 +4014,7 @@
       </c>
       <c r="D9" s="7"/>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>45</v>
       </c>
@@ -4000,7 +4026,7 @@
       </c>
       <c r="D10" s="7"/>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>46</v>
       </c>
@@ -4012,7 +4038,7 @@
       </c>
       <c r="D11" s="7"/>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>48</v>
       </c>
@@ -4024,7 +4050,7 @@
       </c>
       <c r="D12" s="7"/>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>49</v>
       </c>
@@ -4036,7 +4062,7 @@
       </c>
       <c r="D13" s="7"/>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>50</v>
       </c>
@@ -4048,7 +4074,7 @@
       </c>
       <c r="D14" s="7"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>51</v>
       </c>
@@ -4060,7 +4086,7 @@
       </c>
       <c r="D15" s="7"/>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>52</v>
       </c>
@@ -4072,7 +4098,7 @@
       </c>
       <c r="D16" s="7"/>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>53</v>
       </c>
@@ -4084,7 +4110,7 @@
       </c>
       <c r="D17" s="7"/>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>54</v>
       </c>
@@ -4096,7 +4122,7 @@
       </c>
       <c r="D18" s="7"/>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>55</v>
       </c>
@@ -4108,7 +4134,7 @@
       </c>
       <c r="D19" s="7"/>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>56</v>
       </c>
@@ -4120,7 +4146,7 @@
       </c>
       <c r="D20" s="7"/>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>57</v>
       </c>
@@ -4132,7 +4158,7 @@
       </c>
       <c r="D21" s="7"/>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>58</v>
       </c>
@@ -4144,7 +4170,7 @@
       </c>
       <c r="D22" s="7"/>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>59</v>
       </c>
@@ -4156,7 +4182,7 @@
       </c>
       <c r="D23" s="7"/>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>60</v>
       </c>
@@ -4168,7 +4194,7 @@
       </c>
       <c r="D24" s="7"/>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>61</v>
       </c>
@@ -4180,7 +4206,7 @@
       </c>
       <c r="D25" s="7"/>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>47</v>
       </c>
@@ -4199,14 +4225,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A19" sqref="A19:XFD19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
@@ -4214,7 +4240,7 @@
     <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>35</v>
       </c>
@@ -4228,7 +4254,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>37</v>
       </c>
@@ -4240,7 +4266,7 @@
       </c>
       <c r="D2" s="7"/>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>38</v>
       </c>
@@ -4252,7 +4278,7 @@
       </c>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>39</v>
       </c>
@@ -4264,7 +4290,7 @@
       </c>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>40</v>
       </c>
@@ -4276,7 +4302,7 @@
       </c>
       <c r="D5" s="7"/>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>41</v>
       </c>
@@ -4288,7 +4314,7 @@
       </c>
       <c r="D6" s="7"/>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>42</v>
       </c>
@@ -4300,7 +4326,7 @@
       </c>
       <c r="D7" s="7"/>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>43</v>
       </c>
@@ -4312,7 +4338,7 @@
       </c>
       <c r="D8" s="7"/>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>44</v>
       </c>
@@ -4324,7 +4350,7 @@
       </c>
       <c r="D9" s="7"/>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>45</v>
       </c>
@@ -4336,7 +4362,7 @@
       </c>
       <c r="D10" s="7"/>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>46</v>
       </c>
@@ -4348,7 +4374,7 @@
       </c>
       <c r="D11" s="7"/>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>47</v>
       </c>
@@ -4360,7 +4386,7 @@
       </c>
       <c r="D12" s="7"/>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>48</v>
       </c>
@@ -4372,7 +4398,7 @@
       </c>
       <c r="D13" s="7"/>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>49</v>
       </c>
@@ -4384,7 +4410,7 @@
       </c>
       <c r="D14" s="7"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>50</v>
       </c>
@@ -4396,7 +4422,7 @@
       </c>
       <c r="D15" s="7"/>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>51</v>
       </c>
@@ -4408,7 +4434,7 @@
       </c>
       <c r="D16" s="7"/>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>52</v>
       </c>
@@ -4420,7 +4446,7 @@
       </c>
       <c r="D17" s="7"/>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>53</v>
       </c>
@@ -4432,7 +4458,7 @@
       </c>
       <c r="D18" s="7"/>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>54</v>
       </c>
@@ -4444,7 +4470,7 @@
       </c>
       <c r="D19" s="7"/>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>55</v>
       </c>
@@ -4456,7 +4482,7 @@
       </c>
       <c r="D20" s="7"/>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>56</v>
       </c>
@@ -4468,7 +4494,7 @@
       </c>
       <c r="D21" s="7"/>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>57</v>
       </c>
@@ -4480,7 +4506,7 @@
       </c>
       <c r="D22" s="7"/>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>58</v>
       </c>
@@ -4492,7 +4518,7 @@
       </c>
       <c r="D23" s="7"/>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>59</v>
       </c>
@@ -4504,7 +4530,7 @@
       </c>
       <c r="D24" s="7"/>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>60</v>
       </c>
@@ -4516,7 +4542,7 @@
       </c>
       <c r="D25" s="7"/>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>61</v>
       </c>

</xml_diff>

<commit_message>
WAT new scripts 163,164,165
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/WAT.xlsx
+++ b/src/test/resources/xls/WAT.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13305" windowHeight="2415"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="703" uniqueCount="434">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="443">
   <si>
     <t>TCID</t>
   </si>
@@ -1319,13 +1319,41 @@
   </si>
   <si>
     <t>Verify the static text in Author record Page</t>
+  </si>
+  <si>
+    <t>WAT163</t>
+  </si>
+  <si>
+    <t>WAT164</t>
+  </si>
+  <si>
+    <t>WAT165</t>
+  </si>
+  <si>
+    <t>Verify that System displays city/state/country (when available) which corresponds to the last known organization.</t>
+  </si>
+  <si>
+    <t>WAT-620</t>
+  </si>
+  <si>
+    <t>WAT-621||WAT-623</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that System displays the author's ORCiD (when available) as a URI||Verify that upon clicking the orcid link user shall be taken to the ORCiD record in a new browser window/tab 
+</t>
+  </si>
+  <si>
+    <t>Verify that System displays the author's ResearcherID (when available) || Verify that upon clicking the Researcher ID link user shall be taken to the ResearcherID record in a new browser window/tab</t>
+  </si>
+  <si>
+    <t>WAT-622||WAT-624</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1577,7 +1605,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1609,10 +1637,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1644,7 +1671,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1820,14 +1846,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E136"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E139"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A118" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C147" sqref="C147"/>
+      <selection activeCell="C142" sqref="C142"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="41" bestFit="1" customWidth="1" collapsed="1"/>
@@ -1836,7 +1862,7 @@
     <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1853,7 +1879,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -1868,7 +1894,7 @@
       </c>
       <c r="E2" s="4"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -1883,7 +1909,7 @@
       </c>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" s="7" t="s">
         <v>11</v>
       </c>
@@ -1898,7 +1924,7 @@
       </c>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" s="7" t="s">
         <v>12</v>
       </c>
@@ -1913,7 +1939,7 @@
       </c>
       <c r="E5" s="7"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" s="7" t="s">
         <v>14</v>
       </c>
@@ -1928,7 +1954,7 @@
       </c>
       <c r="E6" s="7"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" s="7" t="s">
         <v>17</v>
       </c>
@@ -1943,7 +1969,7 @@
       </c>
       <c r="E7" s="7"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" s="7" t="s">
         <v>20</v>
       </c>
@@ -1958,7 +1984,7 @@
       </c>
       <c r="E8" s="7"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" s="7" t="s">
         <v>22</v>
       </c>
@@ -1973,7 +1999,7 @@
       </c>
       <c r="E9" s="7"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10" s="7" t="s">
         <v>23</v>
       </c>
@@ -1988,7 +2014,7 @@
       </c>
       <c r="E10" s="7"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11" s="7" t="s">
         <v>24</v>
       </c>
@@ -2003,7 +2029,7 @@
       </c>
       <c r="E11" s="7"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12" s="7" t="s">
         <v>25</v>
       </c>
@@ -2018,7 +2044,7 @@
       </c>
       <c r="E12" s="7"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13" s="7" t="s">
         <v>62</v>
       </c>
@@ -2033,7 +2059,7 @@
       </c>
       <c r="E13" s="7"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="A14" s="7" t="s">
         <v>63</v>
       </c>
@@ -2048,7 +2074,7 @@
       </c>
       <c r="E14" s="7"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="A15" s="7" t="s">
         <v>64</v>
       </c>
@@ -2063,7 +2089,7 @@
       </c>
       <c r="E15" s="7"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="A16" s="7" t="s">
         <v>65</v>
       </c>
@@ -2078,7 +2104,7 @@
       </c>
       <c r="E16" s="7"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5">
       <c r="A17" s="7" t="s">
         <v>74</v>
       </c>
@@ -2093,7 +2119,7 @@
       </c>
       <c r="E17" s="7"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5">
       <c r="A18" s="7" t="s">
         <v>75</v>
       </c>
@@ -2108,7 +2134,7 @@
       </c>
       <c r="E18" s="7"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5">
       <c r="A19" s="7" t="s">
         <v>79</v>
       </c>
@@ -2123,7 +2149,7 @@
       </c>
       <c r="E19" s="7"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5">
       <c r="A20" s="7" t="s">
         <v>81</v>
       </c>
@@ -2138,7 +2164,7 @@
       </c>
       <c r="E20" s="7"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5">
       <c r="A21" s="7" t="s">
         <v>82</v>
       </c>
@@ -2153,7 +2179,7 @@
       </c>
       <c r="E21" s="7"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5">
       <c r="A22" s="7" t="s">
         <v>88</v>
       </c>
@@ -2168,7 +2194,7 @@
       </c>
       <c r="E22" s="7"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5">
       <c r="A23" s="7" t="s">
         <v>90</v>
       </c>
@@ -2183,7 +2209,7 @@
       </c>
       <c r="E23" s="7"/>
     </row>
-    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="30">
       <c r="A24" s="9" t="s">
         <v>94</v>
       </c>
@@ -2198,7 +2224,7 @@
       </c>
       <c r="E24" s="7"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5">
       <c r="A25" s="9" t="s">
         <v>96</v>
       </c>
@@ -2213,7 +2239,7 @@
       </c>
       <c r="E25" s="7"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5">
       <c r="A26" s="9" t="s">
         <v>98</v>
       </c>
@@ -2228,7 +2254,7 @@
       </c>
       <c r="E26" s="7"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5">
       <c r="A27" s="9" t="s">
         <v>102</v>
       </c>
@@ -2243,7 +2269,7 @@
       </c>
       <c r="E27" s="7"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5">
       <c r="A28" s="9" t="s">
         <v>105</v>
       </c>
@@ -2258,7 +2284,7 @@
       </c>
       <c r="E28" s="7"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5">
       <c r="A29" s="9" t="s">
         <v>108</v>
       </c>
@@ -2273,7 +2299,7 @@
       </c>
       <c r="E29" s="7"/>
     </row>
-    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" ht="30">
       <c r="A30" s="9" t="s">
         <v>110</v>
       </c>
@@ -2288,7 +2314,7 @@
       </c>
       <c r="E30" s="7"/>
     </row>
-    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" ht="30">
       <c r="A31" s="9" t="s">
         <v>114</v>
       </c>
@@ -2303,7 +2329,7 @@
       </c>
       <c r="E31" s="7"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5">
       <c r="A32" s="9" t="s">
         <v>119</v>
       </c>
@@ -2318,7 +2344,7 @@
       </c>
       <c r="E32" s="7"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5">
       <c r="A33" s="9" t="s">
         <v>120</v>
       </c>
@@ -2333,7 +2359,7 @@
       </c>
       <c r="E33" s="7"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5">
       <c r="A34" s="9" t="s">
         <v>125</v>
       </c>
@@ -2348,7 +2374,7 @@
       </c>
       <c r="E34" s="7"/>
     </row>
-    <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" ht="30">
       <c r="A35" s="9" t="s">
         <v>128</v>
       </c>
@@ -2363,7 +2389,7 @@
       </c>
       <c r="E35" s="7"/>
     </row>
-    <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" ht="30">
       <c r="A36" s="9" t="s">
         <v>131</v>
       </c>
@@ -2378,7 +2404,7 @@
       </c>
       <c r="E36" s="7"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5">
       <c r="A37" s="9" t="s">
         <v>134</v>
       </c>
@@ -2393,7 +2419,7 @@
       </c>
       <c r="E37" s="7"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5">
       <c r="A38" s="9" t="s">
         <v>137</v>
       </c>
@@ -2408,7 +2434,7 @@
       </c>
       <c r="E38" s="7"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5">
       <c r="A39" s="9" t="s">
         <v>140</v>
       </c>
@@ -2423,7 +2449,7 @@
       </c>
       <c r="E39" s="7"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5">
       <c r="A40" s="9" t="s">
         <v>143</v>
       </c>
@@ -2438,7 +2464,7 @@
       </c>
       <c r="E40" s="7"/>
     </row>
-    <row r="41" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" ht="30">
       <c r="A41" s="9" t="s">
         <v>145</v>
       </c>
@@ -2453,7 +2479,7 @@
       </c>
       <c r="E41" s="7"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5">
       <c r="A42" s="9" t="s">
         <v>147</v>
       </c>
@@ -2468,7 +2494,7 @@
       </c>
       <c r="E42" s="7"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5">
       <c r="A43" s="9" t="s">
         <v>150</v>
       </c>
@@ -2483,7 +2509,7 @@
       </c>
       <c r="E43" s="7"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5">
       <c r="A44" s="9" t="s">
         <v>153</v>
       </c>
@@ -2498,7 +2524,7 @@
       </c>
       <c r="E44" s="7"/>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5">
       <c r="A45" s="9" t="s">
         <v>155</v>
       </c>
@@ -2513,7 +2539,7 @@
       </c>
       <c r="E45" s="7"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5">
       <c r="A46" s="12" t="s">
         <v>158</v>
       </c>
@@ -2528,7 +2554,7 @@
       </c>
       <c r="E46" s="7"/>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5">
       <c r="A47" s="12" t="s">
         <v>159</v>
       </c>
@@ -2543,7 +2569,7 @@
       </c>
       <c r="E47" s="7"/>
     </row>
-    <row r="48" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" ht="30">
       <c r="A48" s="12" t="s">
         <v>160</v>
       </c>
@@ -2558,7 +2584,7 @@
       </c>
       <c r="E48" s="7"/>
     </row>
-    <row r="49" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" ht="30">
       <c r="A49" s="12" t="s">
         <v>161</v>
       </c>
@@ -2573,7 +2599,7 @@
       </c>
       <c r="E49" s="7"/>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5">
       <c r="A50" s="12" t="s">
         <v>164</v>
       </c>
@@ -2588,7 +2614,7 @@
       </c>
       <c r="E50" s="7"/>
     </row>
-    <row r="51" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" ht="30">
       <c r="A51" s="9" t="s">
         <v>173</v>
       </c>
@@ -2603,7 +2629,7 @@
       </c>
       <c r="E51" s="7"/>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5">
       <c r="A52" s="9" t="s">
         <v>174</v>
       </c>
@@ -2618,7 +2644,7 @@
       </c>
       <c r="E52" s="7"/>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5">
       <c r="A53" s="9" t="s">
         <v>179</v>
       </c>
@@ -2633,7 +2659,7 @@
       </c>
       <c r="E53" s="7"/>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5">
       <c r="A54" s="9" t="s">
         <v>180</v>
       </c>
@@ -2648,7 +2674,7 @@
       </c>
       <c r="E54" s="7"/>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5">
       <c r="A55" s="9" t="s">
         <v>185</v>
       </c>
@@ -2663,7 +2689,7 @@
       </c>
       <c r="E55" s="7"/>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5">
       <c r="A56" s="9" t="s">
         <v>188</v>
       </c>
@@ -2678,7 +2704,7 @@
       </c>
       <c r="E56" s="7"/>
     </row>
-    <row r="57" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" ht="30">
       <c r="A57" s="9" t="s">
         <v>191</v>
       </c>
@@ -2693,7 +2719,7 @@
       </c>
       <c r="E57" s="7"/>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5">
       <c r="A58" s="9" t="s">
         <v>194</v>
       </c>
@@ -2708,7 +2734,7 @@
       </c>
       <c r="E58" s="7"/>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5">
       <c r="A59" s="7" t="s">
         <v>196</v>
       </c>
@@ -2723,7 +2749,7 @@
       </c>
       <c r="E59" s="7"/>
     </row>
-    <row r="60" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" ht="45">
       <c r="A60" s="7" t="s">
         <v>199</v>
       </c>
@@ -2738,7 +2764,7 @@
       </c>
       <c r="E60" s="7"/>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5">
       <c r="A61" s="9" t="s">
         <v>202</v>
       </c>
@@ -2753,7 +2779,7 @@
       </c>
       <c r="E61" s="7"/>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5">
       <c r="A62" s="9" t="s">
         <v>204</v>
       </c>
@@ -2768,7 +2794,7 @@
       </c>
       <c r="E62" s="7"/>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5">
       <c r="A63" s="9" t="s">
         <v>206</v>
       </c>
@@ -2783,7 +2809,7 @@
       </c>
       <c r="E63" s="7"/>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5">
       <c r="A64" s="9" t="s">
         <v>208</v>
       </c>
@@ -2798,7 +2824,7 @@
       </c>
       <c r="E64" s="7"/>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5">
       <c r="A65" s="9" t="s">
         <v>217</v>
       </c>
@@ -2813,7 +2839,7 @@
       </c>
       <c r="E65" s="7"/>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5">
       <c r="A66" s="9" t="s">
         <v>218</v>
       </c>
@@ -2828,7 +2854,7 @@
       </c>
       <c r="E66" s="7"/>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5">
       <c r="A67" s="9" t="s">
         <v>223</v>
       </c>
@@ -2843,7 +2869,7 @@
       </c>
       <c r="E67" s="7"/>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5">
       <c r="A68" s="9" t="s">
         <v>224</v>
       </c>
@@ -2858,7 +2884,7 @@
       </c>
       <c r="E68" s="7"/>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5">
       <c r="A69" s="9" t="s">
         <v>225</v>
       </c>
@@ -2873,7 +2899,7 @@
       </c>
       <c r="E69" s="7"/>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5">
       <c r="A70" s="9" t="s">
         <v>226</v>
       </c>
@@ -2888,7 +2914,7 @@
       </c>
       <c r="E70" s="7"/>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5">
       <c r="A71" s="9" t="s">
         <v>233</v>
       </c>
@@ -2903,7 +2929,7 @@
       </c>
       <c r="E71" s="7"/>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5">
       <c r="A72" s="9" t="s">
         <v>237</v>
       </c>
@@ -2918,7 +2944,7 @@
       </c>
       <c r="E72" s="7"/>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5">
       <c r="A73" s="9" t="s">
         <v>239</v>
       </c>
@@ -2933,7 +2959,7 @@
       </c>
       <c r="E73" s="7"/>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5">
       <c r="A74" s="9" t="s">
         <v>243</v>
       </c>
@@ -2948,7 +2974,7 @@
       </c>
       <c r="E74" s="7"/>
     </row>
-    <row r="75" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" ht="30">
       <c r="A75" s="9" t="s">
         <v>245</v>
       </c>
@@ -2963,7 +2989,7 @@
       </c>
       <c r="E75" s="7"/>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5">
       <c r="A76" s="9" t="s">
         <v>248</v>
       </c>
@@ -2978,7 +3004,7 @@
       </c>
       <c r="E76" s="7"/>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5">
       <c r="A77" s="9" t="s">
         <v>256</v>
       </c>
@@ -2993,7 +3019,7 @@
       </c>
       <c r="E77" s="7"/>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5">
       <c r="A78" s="9" t="s">
         <v>257</v>
       </c>
@@ -3008,7 +3034,7 @@
       </c>
       <c r="E78" s="7"/>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5">
       <c r="A79" s="9" t="s">
         <v>261</v>
       </c>
@@ -3023,7 +3049,7 @@
       </c>
       <c r="E79" s="7"/>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5">
       <c r="A80" s="9" t="s">
         <v>264</v>
       </c>
@@ -3038,7 +3064,7 @@
       </c>
       <c r="E80" s="7"/>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5">
       <c r="A81" s="9" t="s">
         <v>267</v>
       </c>
@@ -3053,7 +3079,7 @@
       </c>
       <c r="E81" s="7"/>
     </row>
-    <row r="82" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" ht="30">
       <c r="A82" s="9" t="s">
         <v>269</v>
       </c>
@@ -3068,7 +3094,7 @@
       </c>
       <c r="E82" s="7"/>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5">
       <c r="A83" s="9" t="s">
         <v>274</v>
       </c>
@@ -3083,7 +3109,7 @@
       </c>
       <c r="E83" s="7"/>
     </row>
-    <row r="84" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" ht="30">
       <c r="A84" s="9" t="s">
         <v>277</v>
       </c>
@@ -3098,7 +3124,7 @@
       </c>
       <c r="E84" s="7"/>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5">
       <c r="A85" s="9" t="s">
         <v>279</v>
       </c>
@@ -3113,7 +3139,7 @@
       </c>
       <c r="E85" s="7"/>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5">
       <c r="A86" s="9" t="s">
         <v>282</v>
       </c>
@@ -3128,7 +3154,7 @@
       </c>
       <c r="E86" s="7"/>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5">
       <c r="A87" s="9" t="s">
         <v>285</v>
       </c>
@@ -3143,7 +3169,7 @@
       </c>
       <c r="E87" s="7"/>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5">
       <c r="A88" s="9" t="s">
         <v>288</v>
       </c>
@@ -3158,7 +3184,7 @@
       </c>
       <c r="E88" s="7"/>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5">
       <c r="A89" s="9" t="s">
         <v>291</v>
       </c>
@@ -3173,7 +3199,7 @@
       </c>
       <c r="E89" s="7"/>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5">
       <c r="A90" s="9" t="s">
         <v>294</v>
       </c>
@@ -3188,7 +3214,7 @@
       </c>
       <c r="E90" s="7"/>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5">
       <c r="A91" s="9" t="s">
         <v>297</v>
       </c>
@@ -3203,7 +3229,7 @@
       </c>
       <c r="E91" s="7"/>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5">
       <c r="A92" s="9" t="s">
         <v>300</v>
       </c>
@@ -3218,7 +3244,7 @@
       </c>
       <c r="E92" s="7"/>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5">
       <c r="A93" s="9" t="s">
         <v>303</v>
       </c>
@@ -3233,7 +3259,7 @@
       </c>
       <c r="E93" s="7"/>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5">
       <c r="A94" s="9" t="s">
         <v>306</v>
       </c>
@@ -3248,7 +3274,7 @@
       </c>
       <c r="E94" s="7"/>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5">
       <c r="A95" s="9" t="s">
         <v>309</v>
       </c>
@@ -3263,7 +3289,7 @@
       </c>
       <c r="E95" s="7"/>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5">
       <c r="A96" s="9" t="s">
         <v>314</v>
       </c>
@@ -3278,7 +3304,7 @@
       </c>
       <c r="E96" s="7"/>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5">
       <c r="A97" s="9" t="s">
         <v>315</v>
       </c>
@@ -3293,7 +3319,7 @@
       </c>
       <c r="E97" s="7"/>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5">
       <c r="A98" s="9" t="s">
         <v>319</v>
       </c>
@@ -3308,7 +3334,7 @@
       </c>
       <c r="E98" s="7"/>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5">
       <c r="A99" s="9" t="s">
         <v>321</v>
       </c>
@@ -3323,7 +3349,7 @@
       </c>
       <c r="E99" s="7"/>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5">
       <c r="A100" s="9" t="s">
         <v>322</v>
       </c>
@@ -3338,7 +3364,7 @@
       </c>
       <c r="E100" s="7"/>
     </row>
-    <row r="101" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" ht="30">
       <c r="A101" s="9" t="s">
         <v>323</v>
       </c>
@@ -3353,7 +3379,7 @@
       </c>
       <c r="E101" s="7"/>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5">
       <c r="A102" s="9" t="s">
         <v>328</v>
       </c>
@@ -3368,7 +3394,7 @@
       </c>
       <c r="E102" s="7"/>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5">
       <c r="A103" s="9" t="s">
         <v>333</v>
       </c>
@@ -3383,7 +3409,7 @@
       </c>
       <c r="E103" s="7"/>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5">
       <c r="A104" s="9" t="s">
         <v>336</v>
       </c>
@@ -3398,7 +3424,7 @@
       </c>
       <c r="E104" s="7"/>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5">
       <c r="A105" s="9" t="s">
         <v>337</v>
       </c>
@@ -3413,7 +3439,7 @@
       </c>
       <c r="E105" s="7"/>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5">
       <c r="A106" s="9" t="s">
         <v>342</v>
       </c>
@@ -3428,7 +3454,7 @@
       </c>
       <c r="E106" s="7"/>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5">
       <c r="A107" s="9" t="s">
         <v>345</v>
       </c>
@@ -3443,7 +3469,7 @@
       </c>
       <c r="E107" s="7"/>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5">
       <c r="A108" s="9" t="s">
         <v>350</v>
       </c>
@@ -3458,7 +3484,7 @@
       </c>
       <c r="E108" s="7"/>
     </row>
-    <row r="109" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" ht="30">
       <c r="A109" s="9" t="s">
         <v>351</v>
       </c>
@@ -3473,7 +3499,7 @@
       </c>
       <c r="E109" s="7"/>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5">
       <c r="A110" s="9" t="s">
         <v>354</v>
       </c>
@@ -3488,7 +3514,7 @@
       </c>
       <c r="E110" s="7"/>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5">
       <c r="A111" s="9" t="s">
         <v>357</v>
       </c>
@@ -3503,7 +3529,7 @@
       </c>
       <c r="E111" s="7"/>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5">
       <c r="A112" s="9" t="s">
         <v>361</v>
       </c>
@@ -3518,7 +3544,7 @@
       </c>
       <c r="E112" s="7"/>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5">
       <c r="A113" s="17" t="s">
         <v>363</v>
       </c>
@@ -3533,7 +3559,7 @@
       </c>
       <c r="E113" s="19"/>
     </row>
-    <row r="114" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" ht="30">
       <c r="A114" s="9" t="s">
         <v>366</v>
       </c>
@@ -3548,7 +3574,7 @@
       </c>
       <c r="E114" s="7"/>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5">
       <c r="A115" s="9" t="s">
         <v>369</v>
       </c>
@@ -3563,7 +3589,7 @@
       </c>
       <c r="E115" s="7"/>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5">
       <c r="A116" s="9" t="s">
         <v>370</v>
       </c>
@@ -3578,7 +3604,7 @@
       </c>
       <c r="E116" s="7"/>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5">
       <c r="A117" s="9" t="s">
         <v>371</v>
       </c>
@@ -3593,7 +3619,7 @@
       </c>
       <c r="E117" s="7"/>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5">
       <c r="A118" s="9" t="s">
         <v>378</v>
       </c>
@@ -3608,7 +3634,7 @@
       </c>
       <c r="E118" s="7"/>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5">
       <c r="A119" s="9" t="s">
         <v>381</v>
       </c>
@@ -3623,7 +3649,7 @@
       </c>
       <c r="E119" s="7"/>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5">
       <c r="A120" s="9" t="s">
         <v>384</v>
       </c>
@@ -3638,7 +3664,7 @@
       </c>
       <c r="E120" s="7"/>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5">
       <c r="A121" s="9" t="s">
         <v>387</v>
       </c>
@@ -3653,7 +3679,7 @@
       </c>
       <c r="E121" s="7"/>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5">
       <c r="A122" s="7" t="s">
         <v>390</v>
       </c>
@@ -3668,7 +3694,7 @@
       </c>
       <c r="E122" s="7"/>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5">
       <c r="A123" s="7" t="s">
         <v>393</v>
       </c>
@@ -3683,7 +3709,7 @@
       </c>
       <c r="E123" s="7"/>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5">
       <c r="A124" s="7" t="s">
         <v>396</v>
       </c>
@@ -3698,7 +3724,7 @@
       </c>
       <c r="E124" s="7"/>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5">
       <c r="A125" s="9" t="s">
         <v>399</v>
       </c>
@@ -3713,7 +3739,7 @@
       </c>
       <c r="E125" s="7"/>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5">
       <c r="A126" s="7" t="s">
         <v>402</v>
       </c>
@@ -3728,7 +3754,7 @@
       </c>
       <c r="E126" s="7"/>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5">
       <c r="A127" s="7" t="s">
         <v>405</v>
       </c>
@@ -3743,7 +3769,7 @@
       </c>
       <c r="E127" s="7"/>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5">
       <c r="A128" s="7" t="s">
         <v>408</v>
       </c>
@@ -3758,7 +3784,7 @@
       </c>
       <c r="E128" s="7"/>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5">
       <c r="A129" s="9" t="s">
         <v>411</v>
       </c>
@@ -3773,7 +3799,7 @@
       </c>
       <c r="E129" s="7"/>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5">
       <c r="A130" s="9" t="s">
         <v>414</v>
       </c>
@@ -3788,7 +3814,7 @@
       </c>
       <c r="E130" s="7"/>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5">
       <c r="A131" s="9" t="s">
         <v>416</v>
       </c>
@@ -3803,7 +3829,7 @@
       </c>
       <c r="E131" s="7"/>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5">
       <c r="A132" s="7" t="s">
         <v>419</v>
       </c>
@@ -3818,7 +3844,7 @@
       </c>
       <c r="E132" s="7"/>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5">
       <c r="A133" s="9" t="s">
         <v>422</v>
       </c>
@@ -3833,7 +3859,7 @@
       </c>
       <c r="E133" s="7"/>
     </row>
-    <row r="134" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5" ht="30">
       <c r="A134" s="7" t="s">
         <v>425</v>
       </c>
@@ -3848,7 +3874,7 @@
       </c>
       <c r="E134" s="7"/>
     </row>
-    <row r="135" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5" ht="30">
       <c r="A135" s="7" t="s">
         <v>426</v>
       </c>
@@ -3863,7 +3889,7 @@
       </c>
       <c r="E135" s="7"/>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5">
       <c r="A136" s="9" t="s">
         <v>431</v>
       </c>
@@ -3877,6 +3903,51 @@
         <v>5</v>
       </c>
       <c r="E136" s="7"/>
+    </row>
+    <row r="137" spans="1:5">
+      <c r="A137" s="7" t="s">
+        <v>434</v>
+      </c>
+      <c r="B137" s="7" t="s">
+        <v>438</v>
+      </c>
+      <c r="C137" s="7" t="s">
+        <v>437</v>
+      </c>
+      <c r="D137" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E137" s="7"/>
+    </row>
+    <row r="138" spans="1:5" ht="45">
+      <c r="A138" s="7" t="s">
+        <v>435</v>
+      </c>
+      <c r="B138" s="7" t="s">
+        <v>439</v>
+      </c>
+      <c r="C138" s="8" t="s">
+        <v>440</v>
+      </c>
+      <c r="D138" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E138" s="7"/>
+    </row>
+    <row r="139" spans="1:5" ht="30">
+      <c r="A139" s="7" t="s">
+        <v>436</v>
+      </c>
+      <c r="B139" s="7" t="s">
+        <v>442</v>
+      </c>
+      <c r="C139" s="8" t="s">
+        <v>441</v>
+      </c>
+      <c r="D139" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E139" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -3889,14 +3960,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView topLeftCell="A10" zoomScale="80" workbookViewId="0">
       <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
@@ -3904,7 +3975,7 @@
     <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="10" t="s">
         <v>35</v>
       </c>
@@ -3918,7 +3989,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="7" t="s">
         <v>37</v>
       </c>
@@ -3930,7 +4001,7 @@
       </c>
       <c r="D2" s="7"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="7" t="s">
         <v>38</v>
       </c>
@@ -3942,7 +4013,7 @@
       </c>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="7" t="s">
         <v>39</v>
       </c>
@@ -3954,7 +4025,7 @@
       </c>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" s="7" t="s">
         <v>40</v>
       </c>
@@ -3966,7 +4037,7 @@
       </c>
       <c r="D5" s="7"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" s="7" t="s">
         <v>41</v>
       </c>
@@ -3978,7 +4049,7 @@
       </c>
       <c r="D6" s="7"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="7" t="s">
         <v>42</v>
       </c>
@@ -3990,7 +4061,7 @@
       </c>
       <c r="D7" s="7"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="7" t="s">
         <v>43</v>
       </c>
@@ -4002,7 +4073,7 @@
       </c>
       <c r="D8" s="7"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="7" t="s">
         <v>44</v>
       </c>
@@ -4014,7 +4085,7 @@
       </c>
       <c r="D9" s="7"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="7" t="s">
         <v>45</v>
       </c>
@@ -4026,7 +4097,7 @@
       </c>
       <c r="D10" s="7"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11" s="7" t="s">
         <v>46</v>
       </c>
@@ -4038,7 +4109,7 @@
       </c>
       <c r="D11" s="7"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="A12" s="7" t="s">
         <v>48</v>
       </c>
@@ -4050,7 +4121,7 @@
       </c>
       <c r="D12" s="7"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="A13" s="7" t="s">
         <v>49</v>
       </c>
@@ -4062,7 +4133,7 @@
       </c>
       <c r="D13" s="7"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="A14" s="7" t="s">
         <v>50</v>
       </c>
@@ -4074,7 +4145,7 @@
       </c>
       <c r="D14" s="7"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="A15" s="7" t="s">
         <v>51</v>
       </c>
@@ -4086,7 +4157,7 @@
       </c>
       <c r="D15" s="7"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="A16" s="7" t="s">
         <v>52</v>
       </c>
@@ -4098,7 +4169,7 @@
       </c>
       <c r="D16" s="7"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4">
       <c r="A17" s="7" t="s">
         <v>53</v>
       </c>
@@ -4110,7 +4181,7 @@
       </c>
       <c r="D17" s="7"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4">
       <c r="A18" s="7" t="s">
         <v>54</v>
       </c>
@@ -4122,7 +4193,7 @@
       </c>
       <c r="D18" s="7"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4">
       <c r="A19" s="7" t="s">
         <v>55</v>
       </c>
@@ -4134,7 +4205,7 @@
       </c>
       <c r="D19" s="7"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4">
       <c r="A20" s="7" t="s">
         <v>56</v>
       </c>
@@ -4146,7 +4217,7 @@
       </c>
       <c r="D20" s="7"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4">
       <c r="A21" s="7" t="s">
         <v>57</v>
       </c>
@@ -4158,7 +4229,7 @@
       </c>
       <c r="D21" s="7"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4">
       <c r="A22" s="7" t="s">
         <v>58</v>
       </c>
@@ -4170,7 +4241,7 @@
       </c>
       <c r="D22" s="7"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4">
       <c r="A23" s="7" t="s">
         <v>59</v>
       </c>
@@ -4182,7 +4253,7 @@
       </c>
       <c r="D23" s="7"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4">
       <c r="A24" s="7" t="s">
         <v>60</v>
       </c>
@@ -4194,7 +4265,7 @@
       </c>
       <c r="D24" s="7"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4">
       <c r="A25" s="7" t="s">
         <v>61</v>
       </c>
@@ -4206,7 +4277,7 @@
       </c>
       <c r="D25" s="7"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4">
       <c r="A26" s="7" t="s">
         <v>47</v>
       </c>
@@ -4225,14 +4296,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A19" sqref="A19:XFD19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
@@ -4240,7 +4311,7 @@
     <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="10" t="s">
         <v>35</v>
       </c>
@@ -4254,7 +4325,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="7" t="s">
         <v>37</v>
       </c>
@@ -4266,7 +4337,7 @@
       </c>
       <c r="D2" s="7"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="7" t="s">
         <v>38</v>
       </c>
@@ -4278,7 +4349,7 @@
       </c>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="7" t="s">
         <v>39</v>
       </c>
@@ -4290,7 +4361,7 @@
       </c>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" s="7" t="s">
         <v>40</v>
       </c>
@@ -4302,7 +4373,7 @@
       </c>
       <c r="D5" s="7"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" s="7" t="s">
         <v>41</v>
       </c>
@@ -4314,7 +4385,7 @@
       </c>
       <c r="D6" s="7"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="7" t="s">
         <v>42</v>
       </c>
@@ -4326,7 +4397,7 @@
       </c>
       <c r="D7" s="7"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="7" t="s">
         <v>43</v>
       </c>
@@ -4338,7 +4409,7 @@
       </c>
       <c r="D8" s="7"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="7" t="s">
         <v>44</v>
       </c>
@@ -4350,7 +4421,7 @@
       </c>
       <c r="D9" s="7"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="7" t="s">
         <v>45</v>
       </c>
@@ -4362,7 +4433,7 @@
       </c>
       <c r="D10" s="7"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11" s="7" t="s">
         <v>46</v>
       </c>
@@ -4374,7 +4445,7 @@
       </c>
       <c r="D11" s="7"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="A12" s="7" t="s">
         <v>47</v>
       </c>
@@ -4386,7 +4457,7 @@
       </c>
       <c r="D12" s="7"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="A13" s="7" t="s">
         <v>48</v>
       </c>
@@ -4398,7 +4469,7 @@
       </c>
       <c r="D13" s="7"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="A14" s="7" t="s">
         <v>49</v>
       </c>
@@ -4410,7 +4481,7 @@
       </c>
       <c r="D14" s="7"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="A15" s="7" t="s">
         <v>50</v>
       </c>
@@ -4422,7 +4493,7 @@
       </c>
       <c r="D15" s="7"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="A16" s="7" t="s">
         <v>51</v>
       </c>
@@ -4434,7 +4505,7 @@
       </c>
       <c r="D16" s="7"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4">
       <c r="A17" s="7" t="s">
         <v>52</v>
       </c>
@@ -4446,7 +4517,7 @@
       </c>
       <c r="D17" s="7"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4">
       <c r="A18" s="7" t="s">
         <v>53</v>
       </c>
@@ -4458,7 +4529,7 @@
       </c>
       <c r="D18" s="7"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4">
       <c r="A19" s="7" t="s">
         <v>54</v>
       </c>
@@ -4470,7 +4541,7 @@
       </c>
       <c r="D19" s="7"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4">
       <c r="A20" s="7" t="s">
         <v>55</v>
       </c>
@@ -4482,7 +4553,7 @@
       </c>
       <c r="D20" s="7"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4">
       <c r="A21" s="7" t="s">
         <v>56</v>
       </c>
@@ -4494,7 +4565,7 @@
       </c>
       <c r="D21" s="7"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4">
       <c r="A22" s="7" t="s">
         <v>57</v>
       </c>
@@ -4506,7 +4577,7 @@
       </c>
       <c r="D22" s="7"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4">
       <c r="A23" s="7" t="s">
         <v>58</v>
       </c>
@@ -4518,7 +4589,7 @@
       </c>
       <c r="D23" s="7"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4">
       <c r="A24" s="7" t="s">
         <v>59</v>
       </c>
@@ -4530,7 +4601,7 @@
       </c>
       <c r="D24" s="7"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4">
       <c r="A25" s="7" t="s">
         <v>60</v>
       </c>
@@ -4542,7 +4613,7 @@
       </c>
       <c r="D25" s="7"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4">
       <c r="A26" s="7" t="s">
         <v>61</v>
       </c>

</xml_diff>

<commit_message>
Adds WAT-124 test script and related changes
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/WAT.xlsx
+++ b/src/test/resources/xls/WAT.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13305" windowHeight="2415"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="443">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="719" uniqueCount="446">
   <si>
     <t>TCID</t>
   </si>
@@ -1347,13 +1347,22 @@
   </si>
   <si>
     <t>WAT-622||WAT-624</t>
+  </si>
+  <si>
+    <t>WAT124</t>
+  </si>
+  <si>
+    <t>WAT-625 || WAT-626</t>
+  </si>
+  <si>
+    <t>Verify that the system displays (static) publication metadata for each publication || Verify the labels in combined author metadata</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1408,7 +1417,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -1431,52 +1440,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1509,14 +1477,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1605,7 +1571,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1637,9 +1603,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1671,6 +1638,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1846,14 +1814,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E139"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E140"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A118" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C142" sqref="C142"/>
+    <sheetView tabSelected="1" topLeftCell="A127" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E140" sqref="A1:E140"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="41" bestFit="1" customWidth="1" collapsed="1"/>
@@ -1862,7 +1830,7 @@
     <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1879,7 +1847,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -1894,7 +1862,7 @@
       </c>
       <c r="E2" s="4"/>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -1909,7 +1877,7 @@
       </c>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>11</v>
       </c>
@@ -1924,7 +1892,7 @@
       </c>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>12</v>
       </c>
@@ -1939,7 +1907,7 @@
       </c>
       <c r="E5" s="7"/>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>14</v>
       </c>
@@ -1954,7 +1922,7 @@
       </c>
       <c r="E6" s="7"/>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>17</v>
       </c>
@@ -1969,7 +1937,7 @@
       </c>
       <c r="E7" s="7"/>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>20</v>
       </c>
@@ -1984,7 +1952,7 @@
       </c>
       <c r="E8" s="7"/>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>22</v>
       </c>
@@ -1999,7 +1967,7 @@
       </c>
       <c r="E9" s="7"/>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>23</v>
       </c>
@@ -2014,7 +1982,7 @@
       </c>
       <c r="E10" s="7"/>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>24</v>
       </c>
@@ -2029,7 +1997,7 @@
       </c>
       <c r="E11" s="7"/>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>25</v>
       </c>
@@ -2044,7 +2012,7 @@
       </c>
       <c r="E12" s="7"/>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>62</v>
       </c>
@@ -2059,7 +2027,7 @@
       </c>
       <c r="E13" s="7"/>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>63</v>
       </c>
@@ -2074,7 +2042,7 @@
       </c>
       <c r="E14" s="7"/>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>64</v>
       </c>
@@ -2089,7 +2057,7 @@
       </c>
       <c r="E15" s="7"/>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>65</v>
       </c>
@@ -2104,7 +2072,7 @@
       </c>
       <c r="E16" s="7"/>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>74</v>
       </c>
@@ -2119,7 +2087,7 @@
       </c>
       <c r="E17" s="7"/>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>75</v>
       </c>
@@ -2134,7 +2102,7 @@
       </c>
       <c r="E18" s="7"/>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>79</v>
       </c>
@@ -2149,7 +2117,7 @@
       </c>
       <c r="E19" s="7"/>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>81</v>
       </c>
@@ -2164,7 +2132,7 @@
       </c>
       <c r="E20" s="7"/>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>82</v>
       </c>
@@ -2179,7 +2147,7 @@
       </c>
       <c r="E21" s="7"/>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>88</v>
       </c>
@@ -2194,7 +2162,7 @@
       </c>
       <c r="E22" s="7"/>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>90</v>
       </c>
@@ -2209,7 +2177,7 @@
       </c>
       <c r="E23" s="7"/>
     </row>
-    <row r="24" spans="1:5" ht="30">
+    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>94</v>
       </c>
@@ -2224,7 +2192,7 @@
       </c>
       <c r="E24" s="7"/>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>96</v>
       </c>
@@ -2239,7 +2207,7 @@
       </c>
       <c r="E25" s="7"/>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
         <v>98</v>
       </c>
@@ -2254,7 +2222,7 @@
       </c>
       <c r="E26" s="7"/>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
         <v>102</v>
       </c>
@@ -2269,7 +2237,7 @@
       </c>
       <c r="E27" s="7"/>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
         <v>105</v>
       </c>
@@ -2284,7 +2252,7 @@
       </c>
       <c r="E28" s="7"/>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
         <v>108</v>
       </c>
@@ -2299,7 +2267,7 @@
       </c>
       <c r="E29" s="7"/>
     </row>
-    <row r="30" spans="1:5" ht="30">
+    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
         <v>110</v>
       </c>
@@ -2314,7 +2282,7 @@
       </c>
       <c r="E30" s="7"/>
     </row>
-    <row r="31" spans="1:5" ht="30">
+    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
         <v>114</v>
       </c>
@@ -2329,7 +2297,7 @@
       </c>
       <c r="E31" s="7"/>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
         <v>119</v>
       </c>
@@ -2344,7 +2312,7 @@
       </c>
       <c r="E32" s="7"/>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
         <v>120</v>
       </c>
@@ -2359,7 +2327,7 @@
       </c>
       <c r="E33" s="7"/>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
         <v>125</v>
       </c>
@@ -2374,7 +2342,7 @@
       </c>
       <c r="E34" s="7"/>
     </row>
-    <row r="35" spans="1:5" ht="30">
+    <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
         <v>128</v>
       </c>
@@ -2389,7 +2357,7 @@
       </c>
       <c r="E35" s="7"/>
     </row>
-    <row r="36" spans="1:5" ht="30">
+    <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
         <v>131</v>
       </c>
@@ -2404,7 +2372,7 @@
       </c>
       <c r="E36" s="7"/>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
         <v>134</v>
       </c>
@@ -2419,7 +2387,7 @@
       </c>
       <c r="E37" s="7"/>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="9" t="s">
         <v>137</v>
       </c>
@@ -2434,7 +2402,7 @@
       </c>
       <c r="E38" s="7"/>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="s">
         <v>140</v>
       </c>
@@ -2449,7 +2417,7 @@
       </c>
       <c r="E39" s="7"/>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="9" t="s">
         <v>143</v>
       </c>
@@ -2464,7 +2432,7 @@
       </c>
       <c r="E40" s="7"/>
     </row>
-    <row r="41" spans="1:5" ht="30">
+    <row r="41" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
         <v>145</v>
       </c>
@@ -2479,7 +2447,7 @@
       </c>
       <c r="E41" s="7"/>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="9" t="s">
         <v>147</v>
       </c>
@@ -2494,7 +2462,7 @@
       </c>
       <c r="E42" s="7"/>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="9" t="s">
         <v>150</v>
       </c>
@@ -2509,7 +2477,7 @@
       </c>
       <c r="E43" s="7"/>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="9" t="s">
         <v>153</v>
       </c>
@@ -2524,7 +2492,7 @@
       </c>
       <c r="E44" s="7"/>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="9" t="s">
         <v>155</v>
       </c>
@@ -2539,7 +2507,7 @@
       </c>
       <c r="E45" s="7"/>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="12" t="s">
         <v>158</v>
       </c>
@@ -2554,7 +2522,7 @@
       </c>
       <c r="E46" s="7"/>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="12" t="s">
         <v>159</v>
       </c>
@@ -2569,7 +2537,7 @@
       </c>
       <c r="E47" s="7"/>
     </row>
-    <row r="48" spans="1:5" ht="30">
+    <row r="48" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="12" t="s">
         <v>160</v>
       </c>
@@ -2584,7 +2552,7 @@
       </c>
       <c r="E48" s="7"/>
     </row>
-    <row r="49" spans="1:5" ht="30">
+    <row r="49" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="12" t="s">
         <v>161</v>
       </c>
@@ -2599,7 +2567,7 @@
       </c>
       <c r="E49" s="7"/>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="12" t="s">
         <v>164</v>
       </c>
@@ -2614,7 +2582,7 @@
       </c>
       <c r="E50" s="7"/>
     </row>
-    <row r="51" spans="1:5" ht="30">
+    <row r="51" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="9" t="s">
         <v>173</v>
       </c>
@@ -2629,7 +2597,7 @@
       </c>
       <c r="E51" s="7"/>
     </row>
-    <row r="52" spans="1:5">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="9" t="s">
         <v>174</v>
       </c>
@@ -2644,7 +2612,7 @@
       </c>
       <c r="E52" s="7"/>
     </row>
-    <row r="53" spans="1:5">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="9" t="s">
         <v>179</v>
       </c>
@@ -2659,7 +2627,7 @@
       </c>
       <c r="E53" s="7"/>
     </row>
-    <row r="54" spans="1:5">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="9" t="s">
         <v>180</v>
       </c>
@@ -2674,7 +2642,7 @@
       </c>
       <c r="E54" s="7"/>
     </row>
-    <row r="55" spans="1:5">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="9" t="s">
         <v>185</v>
       </c>
@@ -2689,7 +2657,7 @@
       </c>
       <c r="E55" s="7"/>
     </row>
-    <row r="56" spans="1:5">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="s">
         <v>188</v>
       </c>
@@ -2704,7 +2672,7 @@
       </c>
       <c r="E56" s="7"/>
     </row>
-    <row r="57" spans="1:5" ht="30">
+    <row r="57" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="9" t="s">
         <v>191</v>
       </c>
@@ -2719,7 +2687,7 @@
       </c>
       <c r="E57" s="7"/>
     </row>
-    <row r="58" spans="1:5">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="9" t="s">
         <v>194</v>
       </c>
@@ -2734,7 +2702,7 @@
       </c>
       <c r="E58" s="7"/>
     </row>
-    <row r="59" spans="1:5">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
         <v>196</v>
       </c>
@@ -2749,7 +2717,7 @@
       </c>
       <c r="E59" s="7"/>
     </row>
-    <row r="60" spans="1:5" ht="45">
+    <row r="60" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
         <v>199</v>
       </c>
@@ -2764,7 +2732,7 @@
       </c>
       <c r="E60" s="7"/>
     </row>
-    <row r="61" spans="1:5">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="9" t="s">
         <v>202</v>
       </c>
@@ -2779,7 +2747,7 @@
       </c>
       <c r="E61" s="7"/>
     </row>
-    <row r="62" spans="1:5">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="9" t="s">
         <v>204</v>
       </c>
@@ -2794,7 +2762,7 @@
       </c>
       <c r="E62" s="7"/>
     </row>
-    <row r="63" spans="1:5">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="9" t="s">
         <v>206</v>
       </c>
@@ -2809,7 +2777,7 @@
       </c>
       <c r="E63" s="7"/>
     </row>
-    <row r="64" spans="1:5">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="9" t="s">
         <v>208</v>
       </c>
@@ -2824,7 +2792,7 @@
       </c>
       <c r="E64" s="7"/>
     </row>
-    <row r="65" spans="1:5">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="9" t="s">
         <v>217</v>
       </c>
@@ -2839,7 +2807,7 @@
       </c>
       <c r="E65" s="7"/>
     </row>
-    <row r="66" spans="1:5">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="9" t="s">
         <v>218</v>
       </c>
@@ -2854,7 +2822,7 @@
       </c>
       <c r="E66" s="7"/>
     </row>
-    <row r="67" spans="1:5">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="9" t="s">
         <v>223</v>
       </c>
@@ -2869,7 +2837,7 @@
       </c>
       <c r="E67" s="7"/>
     </row>
-    <row r="68" spans="1:5">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="9" t="s">
         <v>224</v>
       </c>
@@ -2884,7 +2852,7 @@
       </c>
       <c r="E68" s="7"/>
     </row>
-    <row r="69" spans="1:5">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="9" t="s">
         <v>225</v>
       </c>
@@ -2899,7 +2867,7 @@
       </c>
       <c r="E69" s="7"/>
     </row>
-    <row r="70" spans="1:5">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="9" t="s">
         <v>226</v>
       </c>
@@ -2914,7 +2882,7 @@
       </c>
       <c r="E70" s="7"/>
     </row>
-    <row r="71" spans="1:5">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="9" t="s">
         <v>233</v>
       </c>
@@ -2929,7 +2897,7 @@
       </c>
       <c r="E71" s="7"/>
     </row>
-    <row r="72" spans="1:5">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="9" t="s">
         <v>237</v>
       </c>
@@ -2944,7 +2912,7 @@
       </c>
       <c r="E72" s="7"/>
     </row>
-    <row r="73" spans="1:5">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="9" t="s">
         <v>239</v>
       </c>
@@ -2959,7 +2927,7 @@
       </c>
       <c r="E73" s="7"/>
     </row>
-    <row r="74" spans="1:5">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="9" t="s">
         <v>243</v>
       </c>
@@ -2974,7 +2942,7 @@
       </c>
       <c r="E74" s="7"/>
     </row>
-    <row r="75" spans="1:5" ht="30">
+    <row r="75" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" s="9" t="s">
         <v>245</v>
       </c>
@@ -2989,7 +2957,7 @@
       </c>
       <c r="E75" s="7"/>
     </row>
-    <row r="76" spans="1:5">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="9" t="s">
         <v>248</v>
       </c>
@@ -3004,7 +2972,7 @@
       </c>
       <c r="E76" s="7"/>
     </row>
-    <row r="77" spans="1:5">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="9" t="s">
         <v>256</v>
       </c>
@@ -3019,7 +2987,7 @@
       </c>
       <c r="E77" s="7"/>
     </row>
-    <row r="78" spans="1:5">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="9" t="s">
         <v>257</v>
       </c>
@@ -3034,7 +3002,7 @@
       </c>
       <c r="E78" s="7"/>
     </row>
-    <row r="79" spans="1:5">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="9" t="s">
         <v>261</v>
       </c>
@@ -3049,7 +3017,7 @@
       </c>
       <c r="E79" s="7"/>
     </row>
-    <row r="80" spans="1:5">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="9" t="s">
         <v>264</v>
       </c>
@@ -3064,7 +3032,7 @@
       </c>
       <c r="E80" s="7"/>
     </row>
-    <row r="81" spans="1:5">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="9" t="s">
         <v>267</v>
       </c>
@@ -3079,7 +3047,7 @@
       </c>
       <c r="E81" s="7"/>
     </row>
-    <row r="82" spans="1:5" ht="30">
+    <row r="82" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A82" s="9" t="s">
         <v>269</v>
       </c>
@@ -3094,7 +3062,7 @@
       </c>
       <c r="E82" s="7"/>
     </row>
-    <row r="83" spans="1:5">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="9" t="s">
         <v>274</v>
       </c>
@@ -3109,7 +3077,7 @@
       </c>
       <c r="E83" s="7"/>
     </row>
-    <row r="84" spans="1:5" ht="30">
+    <row r="84" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A84" s="9" t="s">
         <v>277</v>
       </c>
@@ -3124,7 +3092,7 @@
       </c>
       <c r="E84" s="7"/>
     </row>
-    <row r="85" spans="1:5">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="9" t="s">
         <v>279</v>
       </c>
@@ -3139,7 +3107,7 @@
       </c>
       <c r="E85" s="7"/>
     </row>
-    <row r="86" spans="1:5">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="9" t="s">
         <v>282</v>
       </c>
@@ -3154,7 +3122,7 @@
       </c>
       <c r="E86" s="7"/>
     </row>
-    <row r="87" spans="1:5">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="9" t="s">
         <v>285</v>
       </c>
@@ -3169,7 +3137,7 @@
       </c>
       <c r="E87" s="7"/>
     </row>
-    <row r="88" spans="1:5">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="9" t="s">
         <v>288</v>
       </c>
@@ -3184,7 +3152,7 @@
       </c>
       <c r="E88" s="7"/>
     </row>
-    <row r="89" spans="1:5">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="9" t="s">
         <v>291</v>
       </c>
@@ -3199,7 +3167,7 @@
       </c>
       <c r="E89" s="7"/>
     </row>
-    <row r="90" spans="1:5">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="9" t="s">
         <v>294</v>
       </c>
@@ -3214,7 +3182,7 @@
       </c>
       <c r="E90" s="7"/>
     </row>
-    <row r="91" spans="1:5">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="9" t="s">
         <v>297</v>
       </c>
@@ -3229,7 +3197,7 @@
       </c>
       <c r="E91" s="7"/>
     </row>
-    <row r="92" spans="1:5">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="9" t="s">
         <v>300</v>
       </c>
@@ -3244,7 +3212,7 @@
       </c>
       <c r="E92" s="7"/>
     </row>
-    <row r="93" spans="1:5">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="9" t="s">
         <v>303</v>
       </c>
@@ -3259,7 +3227,7 @@
       </c>
       <c r="E93" s="7"/>
     </row>
-    <row r="94" spans="1:5">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="9" t="s">
         <v>306</v>
       </c>
@@ -3274,7 +3242,7 @@
       </c>
       <c r="E94" s="7"/>
     </row>
-    <row r="95" spans="1:5">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="9" t="s">
         <v>309</v>
       </c>
@@ -3289,7 +3257,7 @@
       </c>
       <c r="E95" s="7"/>
     </row>
-    <row r="96" spans="1:5">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="9" t="s">
         <v>314</v>
       </c>
@@ -3304,7 +3272,7 @@
       </c>
       <c r="E96" s="7"/>
     </row>
-    <row r="97" spans="1:5">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="9" t="s">
         <v>315</v>
       </c>
@@ -3319,7 +3287,7 @@
       </c>
       <c r="E97" s="7"/>
     </row>
-    <row r="98" spans="1:5">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="9" t="s">
         <v>319</v>
       </c>
@@ -3334,7 +3302,7 @@
       </c>
       <c r="E98" s="7"/>
     </row>
-    <row r="99" spans="1:5">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="9" t="s">
         <v>321</v>
       </c>
@@ -3349,7 +3317,7 @@
       </c>
       <c r="E99" s="7"/>
     </row>
-    <row r="100" spans="1:5">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="9" t="s">
         <v>322</v>
       </c>
@@ -3364,7 +3332,7 @@
       </c>
       <c r="E100" s="7"/>
     </row>
-    <row r="101" spans="1:5" ht="30">
+    <row r="101" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A101" s="9" t="s">
         <v>323</v>
       </c>
@@ -3379,7 +3347,7 @@
       </c>
       <c r="E101" s="7"/>
     </row>
-    <row r="102" spans="1:5">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="9" t="s">
         <v>328</v>
       </c>
@@ -3394,7 +3362,7 @@
       </c>
       <c r="E102" s="7"/>
     </row>
-    <row r="103" spans="1:5">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="9" t="s">
         <v>333</v>
       </c>
@@ -3409,7 +3377,7 @@
       </c>
       <c r="E103" s="7"/>
     </row>
-    <row r="104" spans="1:5">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="9" t="s">
         <v>336</v>
       </c>
@@ -3424,7 +3392,7 @@
       </c>
       <c r="E104" s="7"/>
     </row>
-    <row r="105" spans="1:5">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="9" t="s">
         <v>337</v>
       </c>
@@ -3439,7 +3407,7 @@
       </c>
       <c r="E105" s="7"/>
     </row>
-    <row r="106" spans="1:5">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="9" t="s">
         <v>342</v>
       </c>
@@ -3454,7 +3422,7 @@
       </c>
       <c r="E106" s="7"/>
     </row>
-    <row r="107" spans="1:5">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="9" t="s">
         <v>345</v>
       </c>
@@ -3469,7 +3437,7 @@
       </c>
       <c r="E107" s="7"/>
     </row>
-    <row r="108" spans="1:5">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="9" t="s">
         <v>350</v>
       </c>
@@ -3484,7 +3452,7 @@
       </c>
       <c r="E108" s="7"/>
     </row>
-    <row r="109" spans="1:5" ht="30">
+    <row r="109" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A109" s="9" t="s">
         <v>351</v>
       </c>
@@ -3499,7 +3467,7 @@
       </c>
       <c r="E109" s="7"/>
     </row>
-    <row r="110" spans="1:5">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="9" t="s">
         <v>354</v>
       </c>
@@ -3514,7 +3482,7 @@
       </c>
       <c r="E110" s="7"/>
     </row>
-    <row r="111" spans="1:5">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="9" t="s">
         <v>357</v>
       </c>
@@ -3529,7 +3497,7 @@
       </c>
       <c r="E111" s="7"/>
     </row>
-    <row r="112" spans="1:5">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="9" t="s">
         <v>361</v>
       </c>
@@ -3544,22 +3512,22 @@
       </c>
       <c r="E112" s="7"/>
     </row>
-    <row r="113" spans="1:5">
-      <c r="A113" s="17" t="s">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A113" s="9" t="s">
         <v>363</v>
       </c>
-      <c r="B113" s="17" t="s">
+      <c r="B113" s="9" t="s">
         <v>364</v>
       </c>
-      <c r="C113" s="18" t="s">
+      <c r="C113" s="16" t="s">
         <v>365</v>
       </c>
-      <c r="D113" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="E113" s="19"/>
-    </row>
-    <row r="114" spans="1:5" ht="30">
+      <c r="D113" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E113" s="7"/>
+    </row>
+    <row r="114" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A114" s="9" t="s">
         <v>366</v>
       </c>
@@ -3574,7 +3542,7 @@
       </c>
       <c r="E114" s="7"/>
     </row>
-    <row r="115" spans="1:5">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="9" t="s">
         <v>369</v>
       </c>
@@ -3589,7 +3557,7 @@
       </c>
       <c r="E115" s="7"/>
     </row>
-    <row r="116" spans="1:5">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="9" t="s">
         <v>370</v>
       </c>
@@ -3604,7 +3572,7 @@
       </c>
       <c r="E116" s="7"/>
     </row>
-    <row r="117" spans="1:5">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" s="9" t="s">
         <v>371</v>
       </c>
@@ -3619,7 +3587,7 @@
       </c>
       <c r="E117" s="7"/>
     </row>
-    <row r="118" spans="1:5">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" s="9" t="s">
         <v>378</v>
       </c>
@@ -3634,7 +3602,7 @@
       </c>
       <c r="E118" s="7"/>
     </row>
-    <row r="119" spans="1:5">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" s="9" t="s">
         <v>381</v>
       </c>
@@ -3649,7 +3617,7 @@
       </c>
       <c r="E119" s="7"/>
     </row>
-    <row r="120" spans="1:5">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" s="9" t="s">
         <v>384</v>
       </c>
@@ -3664,7 +3632,7 @@
       </c>
       <c r="E120" s="7"/>
     </row>
-    <row r="121" spans="1:5">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="9" t="s">
         <v>387</v>
       </c>
@@ -3679,7 +3647,7 @@
       </c>
       <c r="E121" s="7"/>
     </row>
-    <row r="122" spans="1:5">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" s="7" t="s">
         <v>390</v>
       </c>
@@ -3694,7 +3662,7 @@
       </c>
       <c r="E122" s="7"/>
     </row>
-    <row r="123" spans="1:5">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" s="7" t="s">
         <v>393</v>
       </c>
@@ -3709,7 +3677,7 @@
       </c>
       <c r="E123" s="7"/>
     </row>
-    <row r="124" spans="1:5">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" s="7" t="s">
         <v>396</v>
       </c>
@@ -3724,7 +3692,7 @@
       </c>
       <c r="E124" s="7"/>
     </row>
-    <row r="125" spans="1:5">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" s="9" t="s">
         <v>399</v>
       </c>
@@ -3739,7 +3707,7 @@
       </c>
       <c r="E125" s="7"/>
     </row>
-    <row r="126" spans="1:5">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" s="7" t="s">
         <v>402</v>
       </c>
@@ -3754,7 +3722,7 @@
       </c>
       <c r="E126" s="7"/>
     </row>
-    <row r="127" spans="1:5">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" s="7" t="s">
         <v>405</v>
       </c>
@@ -3769,7 +3737,7 @@
       </c>
       <c r="E127" s="7"/>
     </row>
-    <row r="128" spans="1:5">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" s="7" t="s">
         <v>408</v>
       </c>
@@ -3784,7 +3752,7 @@
       </c>
       <c r="E128" s="7"/>
     </row>
-    <row r="129" spans="1:5">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" s="9" t="s">
         <v>411</v>
       </c>
@@ -3799,7 +3767,7 @@
       </c>
       <c r="E129" s="7"/>
     </row>
-    <row r="130" spans="1:5">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" s="9" t="s">
         <v>414</v>
       </c>
@@ -3814,7 +3782,7 @@
       </c>
       <c r="E130" s="7"/>
     </row>
-    <row r="131" spans="1:5">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" s="9" t="s">
         <v>416</v>
       </c>
@@ -3829,7 +3797,7 @@
       </c>
       <c r="E131" s="7"/>
     </row>
-    <row r="132" spans="1:5">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" s="7" t="s">
         <v>419</v>
       </c>
@@ -3844,7 +3812,7 @@
       </c>
       <c r="E132" s="7"/>
     </row>
-    <row r="133" spans="1:5">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" s="9" t="s">
         <v>422</v>
       </c>
@@ -3859,7 +3827,7 @@
       </c>
       <c r="E133" s="7"/>
     </row>
-    <row r="134" spans="1:5" ht="30">
+    <row r="134" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A134" s="7" t="s">
         <v>425</v>
       </c>
@@ -3874,7 +3842,7 @@
       </c>
       <c r="E134" s="7"/>
     </row>
-    <row r="135" spans="1:5" ht="30">
+    <row r="135" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A135" s="7" t="s">
         <v>426</v>
       </c>
@@ -3889,7 +3857,7 @@
       </c>
       <c r="E135" s="7"/>
     </row>
-    <row r="136" spans="1:5">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" s="9" t="s">
         <v>431</v>
       </c>
@@ -3904,7 +3872,7 @@
       </c>
       <c r="E136" s="7"/>
     </row>
-    <row r="137" spans="1:5">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" s="7" t="s">
         <v>434</v>
       </c>
@@ -3919,7 +3887,7 @@
       </c>
       <c r="E137" s="7"/>
     </row>
-    <row r="138" spans="1:5" ht="45">
+    <row r="138" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A138" s="7" t="s">
         <v>435</v>
       </c>
@@ -3934,7 +3902,7 @@
       </c>
       <c r="E138" s="7"/>
     </row>
-    <row r="139" spans="1:5" ht="30">
+    <row r="139" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A139" s="7" t="s">
         <v>436</v>
       </c>
@@ -3948,6 +3916,21 @@
         <v>5</v>
       </c>
       <c r="E139" s="7"/>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A140" s="17" t="s">
+        <v>443</v>
+      </c>
+      <c r="B140" s="7" t="s">
+        <v>444</v>
+      </c>
+      <c r="C140" s="8" t="s">
+        <v>445</v>
+      </c>
+      <c r="D140" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E140" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -3960,14 +3943,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView topLeftCell="A10" zoomScale="80" workbookViewId="0">
       <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
@@ -3975,7 +3958,7 @@
     <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>35</v>
       </c>
@@ -3989,7 +3972,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>37</v>
       </c>
@@ -4001,7 +3984,7 @@
       </c>
       <c r="D2" s="7"/>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>38</v>
       </c>
@@ -4013,7 +3996,7 @@
       </c>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>39</v>
       </c>
@@ -4025,7 +4008,7 @@
       </c>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>40</v>
       </c>
@@ -4037,7 +4020,7 @@
       </c>
       <c r="D5" s="7"/>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>41</v>
       </c>
@@ -4049,7 +4032,7 @@
       </c>
       <c r="D6" s="7"/>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>42</v>
       </c>
@@ -4061,7 +4044,7 @@
       </c>
       <c r="D7" s="7"/>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>43</v>
       </c>
@@ -4073,7 +4056,7 @@
       </c>
       <c r="D8" s="7"/>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>44</v>
       </c>
@@ -4085,7 +4068,7 @@
       </c>
       <c r="D9" s="7"/>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>45</v>
       </c>
@@ -4097,7 +4080,7 @@
       </c>
       <c r="D10" s="7"/>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>46</v>
       </c>
@@ -4109,7 +4092,7 @@
       </c>
       <c r="D11" s="7"/>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>48</v>
       </c>
@@ -4121,7 +4104,7 @@
       </c>
       <c r="D12" s="7"/>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>49</v>
       </c>
@@ -4133,7 +4116,7 @@
       </c>
       <c r="D13" s="7"/>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>50</v>
       </c>
@@ -4145,7 +4128,7 @@
       </c>
       <c r="D14" s="7"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>51</v>
       </c>
@@ -4157,7 +4140,7 @@
       </c>
       <c r="D15" s="7"/>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>52</v>
       </c>
@@ -4169,7 +4152,7 @@
       </c>
       <c r="D16" s="7"/>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>53</v>
       </c>
@@ -4181,7 +4164,7 @@
       </c>
       <c r="D17" s="7"/>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>54</v>
       </c>
@@ -4193,7 +4176,7 @@
       </c>
       <c r="D18" s="7"/>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>55</v>
       </c>
@@ -4205,7 +4188,7 @@
       </c>
       <c r="D19" s="7"/>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>56</v>
       </c>
@@ -4217,7 +4200,7 @@
       </c>
       <c r="D20" s="7"/>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>57</v>
       </c>
@@ -4229,7 +4212,7 @@
       </c>
       <c r="D21" s="7"/>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>58</v>
       </c>
@@ -4241,7 +4224,7 @@
       </c>
       <c r="D22" s="7"/>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>59</v>
       </c>
@@ -4253,7 +4236,7 @@
       </c>
       <c r="D23" s="7"/>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>60</v>
       </c>
@@ -4265,7 +4248,7 @@
       </c>
       <c r="D24" s="7"/>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>61</v>
       </c>
@@ -4277,7 +4260,7 @@
       </c>
       <c r="D25" s="7"/>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>47</v>
       </c>
@@ -4296,14 +4279,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A19" sqref="A19:XFD19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
@@ -4311,7 +4294,7 @@
     <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>35</v>
       </c>
@@ -4325,7 +4308,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>37</v>
       </c>
@@ -4337,7 +4320,7 @@
       </c>
       <c r="D2" s="7"/>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>38</v>
       </c>
@@ -4349,7 +4332,7 @@
       </c>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>39</v>
       </c>
@@ -4361,7 +4344,7 @@
       </c>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>40</v>
       </c>
@@ -4373,7 +4356,7 @@
       </c>
       <c r="D5" s="7"/>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>41</v>
       </c>
@@ -4385,7 +4368,7 @@
       </c>
       <c r="D6" s="7"/>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>42</v>
       </c>
@@ -4397,7 +4380,7 @@
       </c>
       <c r="D7" s="7"/>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>43</v>
       </c>
@@ -4409,7 +4392,7 @@
       </c>
       <c r="D8" s="7"/>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>44</v>
       </c>
@@ -4421,7 +4404,7 @@
       </c>
       <c r="D9" s="7"/>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>45</v>
       </c>
@@ -4433,7 +4416,7 @@
       </c>
       <c r="D10" s="7"/>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>46</v>
       </c>
@@ -4445,7 +4428,7 @@
       </c>
       <c r="D11" s="7"/>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>47</v>
       </c>
@@ -4457,7 +4440,7 @@
       </c>
       <c r="D12" s="7"/>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>48</v>
       </c>
@@ -4469,7 +4452,7 @@
       </c>
       <c r="D13" s="7"/>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>49</v>
       </c>
@@ -4481,7 +4464,7 @@
       </c>
       <c r="D14" s="7"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>50</v>
       </c>
@@ -4493,7 +4476,7 @@
       </c>
       <c r="D15" s="7"/>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>51</v>
       </c>
@@ -4505,7 +4488,7 @@
       </c>
       <c r="D16" s="7"/>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>52</v>
       </c>
@@ -4517,7 +4500,7 @@
       </c>
       <c r="D17" s="7"/>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>53</v>
       </c>
@@ -4529,7 +4512,7 @@
       </c>
       <c r="D18" s="7"/>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>54</v>
       </c>
@@ -4541,7 +4524,7 @@
       </c>
       <c r="D19" s="7"/>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>55</v>
       </c>
@@ -4553,7 +4536,7 @@
       </c>
       <c r="D20" s="7"/>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>56</v>
       </c>
@@ -4565,7 +4548,7 @@
       </c>
       <c r="D21" s="7"/>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>57</v>
       </c>
@@ -4577,7 +4560,7 @@
       </c>
       <c r="D22" s="7"/>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>58</v>
       </c>
@@ -4589,7 +4572,7 @@
       </c>
       <c r="D23" s="7"/>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>59</v>
       </c>
@@ -4601,7 +4584,7 @@
       </c>
       <c r="D24" s="7"/>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>60</v>
       </c>
@@ -4613,7 +4596,7 @@
       </c>
       <c r="D25" s="7"/>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>61</v>
       </c>

</xml_diff>

<commit_message>
Adds WAT-125 test script and related changes
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/WAT.xlsx
+++ b/src/test/resources/xls/WAT.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="719" uniqueCount="446">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="723" uniqueCount="449">
   <si>
     <t>TCID</t>
   </si>
@@ -1356,6 +1356,15 @@
   </si>
   <si>
     <t>Verify that the system displays (static) publication metadata for each publication || Verify the labels in combined author metadata</t>
+  </si>
+  <si>
+    <t>WAT125</t>
+  </si>
+  <si>
+    <t>WAT-628</t>
+  </si>
+  <si>
+    <t>Verify that the publication list shall be sorted by Most recent (by publication year) - default.</t>
   </si>
 </sst>
 </file>
@@ -1815,10 +1824,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E140"/>
+  <dimension ref="A1:E141"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A127" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E140" sqref="A1:E140"/>
+      <selection activeCell="C141" sqref="C141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3931,6 +3940,21 @@
         <v>5</v>
       </c>
       <c r="E140" s="7"/>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A141" s="17" t="s">
+        <v>446</v>
+      </c>
+      <c r="B141" s="7" t="s">
+        <v>447</v>
+      </c>
+      <c r="C141" s="8" t="s">
+        <v>448</v>
+      </c>
+      <c r="D141" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E141" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Adds WAT-126 test script and related changes
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/WAT.xlsx
+++ b/src/test/resources/xls/WAT.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="723" uniqueCount="449">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="727" uniqueCount="452">
   <si>
     <t>TCID</t>
   </si>
@@ -1365,6 +1365,15 @@
   </si>
   <si>
     <t>Verify that the publication list shall be sorted by Most recent (by publication year) - default.</t>
+  </si>
+  <si>
+    <t>WAT126</t>
+  </si>
+  <si>
+    <t>WAT-1213</t>
+  </si>
+  <si>
+    <t>Verify that user is able to see the selections they made in the Author filter in Author search results page</t>
   </si>
 </sst>
 </file>
@@ -1824,10 +1833,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E141"/>
+  <dimension ref="A1:E142"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A127" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C141" sqref="C141"/>
+      <selection activeCell="C142" sqref="C142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3955,6 +3964,21 @@
         <v>5</v>
       </c>
       <c r="E141" s="7"/>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A142" s="17" t="s">
+        <v>449</v>
+      </c>
+      <c r="B142" s="7" t="s">
+        <v>450</v>
+      </c>
+      <c r="C142" s="8" t="s">
+        <v>451</v>
+      </c>
+      <c r="D142" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E142" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Adds WAT-127 testscript and related changes
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/WAT.xlsx
+++ b/src/test/resources/xls/WAT.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="727" uniqueCount="452">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="735" uniqueCount="458">
   <si>
     <t>TCID</t>
   </si>
@@ -1374,6 +1374,24 @@
   </si>
   <si>
     <t>Verify that user is able to see the selections they made in the Author filter in Author search results page</t>
+  </si>
+  <si>
+    <t>WAT127</t>
+  </si>
+  <si>
+    <t>WAT128</t>
+  </si>
+  <si>
+    <t>WAT-1214</t>
+  </si>
+  <si>
+    <t>WAT-1215</t>
+  </si>
+  <si>
+    <t>Verify that user is able to see the selections they made in the Journal filter in Author search results page</t>
+  </si>
+  <si>
+    <t>Verify that user is able to see the selections they made in the Subject Category filter in Author search results page</t>
   </si>
 </sst>
 </file>
@@ -1833,10 +1851,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E142"/>
+  <dimension ref="A1:E144"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A127" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C142" sqref="C142"/>
+      <selection activeCell="C144" sqref="C144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3979,6 +3997,36 @@
         <v>5</v>
       </c>
       <c r="E142" s="7"/>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A143" s="17" t="s">
+        <v>452</v>
+      </c>
+      <c r="B143" s="7" t="s">
+        <v>454</v>
+      </c>
+      <c r="C143" s="8" t="s">
+        <v>456</v>
+      </c>
+      <c r="D143" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E143" s="7"/>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A144" s="17" t="s">
+        <v>453</v>
+      </c>
+      <c r="B144" s="7" t="s">
+        <v>455</v>
+      </c>
+      <c r="C144" s="8" t="s">
+        <v>457</v>
+      </c>
+      <c r="D144" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E144" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Adds WAT-129 test script and related changes
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/WAT.xlsx
+++ b/src/test/resources/xls/WAT.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="735" uniqueCount="458">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="739" uniqueCount="461">
   <si>
     <t>TCID</t>
   </si>
@@ -1392,6 +1392,15 @@
   </si>
   <si>
     <t>Verify that user is able to see the selections they made in the Subject Category filter in Author search results page</t>
+  </si>
+  <si>
+    <t>WAT129</t>
+  </si>
+  <si>
+    <t>WAT-1216</t>
+  </si>
+  <si>
+    <t>Verify that selected options should stay visible at the top of each filter</t>
   </si>
 </sst>
 </file>
@@ -1851,10 +1860,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E144"/>
+  <dimension ref="A1:E145"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A127" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C144" sqref="C144"/>
+      <selection activeCell="C151" sqref="C151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4027,6 +4036,21 @@
         <v>5</v>
       </c>
       <c r="E144" s="7"/>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A145" s="17" t="s">
+        <v>458</v>
+      </c>
+      <c r="B145" s="7" t="s">
+        <v>459</v>
+      </c>
+      <c r="C145" s="8" t="s">
+        <v>460</v>
+      </c>
+      <c r="D145" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E145" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Adds WAT-130 and related changes
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/WAT.xlsx
+++ b/src/test/resources/xls/WAT.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="739" uniqueCount="461">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="743" uniqueCount="464">
   <si>
     <t>TCID</t>
   </si>
@@ -1401,6 +1401,15 @@
   </si>
   <si>
     <t>Verify that selected options should stay visible at the top of each filter</t>
+  </si>
+  <si>
+    <t>WAT130</t>
+  </si>
+  <si>
+    <t>Verify that the unselected options section must begin below the selected section</t>
+  </si>
+  <si>
+    <t>WAT-1219</t>
   </si>
 </sst>
 </file>
@@ -1860,10 +1869,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E145"/>
+  <dimension ref="A1:E146"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A127" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C151" sqref="C151"/>
+    <sheetView tabSelected="1" topLeftCell="A133" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B146" sqref="B146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4051,6 +4060,21 @@
         <v>5</v>
       </c>
       <c r="E145" s="7"/>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A146" s="17" t="s">
+        <v>461</v>
+      </c>
+      <c r="B146" s="7" t="s">
+        <v>463</v>
+      </c>
+      <c r="C146" s="8" t="s">
+        <v>462</v>
+      </c>
+      <c r="D146" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E146" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Adds WAT-131 test script and related changes
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/WAT.xlsx
+++ b/src/test/resources/xls/WAT.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="743" uniqueCount="464">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="747" uniqueCount="467">
   <si>
     <t>TCID</t>
   </si>
@@ -1410,6 +1410,15 @@
   </si>
   <si>
     <t>WAT-1219</t>
+  </si>
+  <si>
+    <t>WAT131</t>
+  </si>
+  <si>
+    <t>Verify that when a user deselects a filter option then it must return to it’s place in the list of unselected filter section.</t>
+  </si>
+  <si>
+    <t>WAT-1221</t>
   </si>
 </sst>
 </file>
@@ -1869,10 +1878,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E146"/>
+  <dimension ref="A1:E147"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A133" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B146" sqref="B146"/>
+      <selection activeCell="B147" sqref="B147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4075,6 +4084,21 @@
         <v>5</v>
       </c>
       <c r="E146" s="7"/>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A147" s="17" t="s">
+        <v>464</v>
+      </c>
+      <c r="B147" s="7" t="s">
+        <v>466</v>
+      </c>
+      <c r="C147" s="8" t="s">
+        <v>465</v>
+      </c>
+      <c r="D147" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E147" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Adds WAT-132 testscript and related changes
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/WAT.xlsx
+++ b/src/test/resources/xls/WAT.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="747" uniqueCount="467">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751" uniqueCount="470">
   <si>
     <t>TCID</t>
   </si>
@@ -1419,6 +1419,15 @@
   </si>
   <si>
     <t>WAT-1221</t>
+  </si>
+  <si>
+    <t>WAT132</t>
+  </si>
+  <si>
+    <t>WAT-1222</t>
+  </si>
+  <si>
+    <t>Verify that divider or spacing is present to visually separate selected options</t>
   </si>
 </sst>
 </file>
@@ -1878,10 +1887,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E147"/>
+  <dimension ref="A1:E148"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A133" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B147" sqref="B147"/>
+      <selection activeCell="C148" sqref="C148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4099,6 +4108,21 @@
         <v>5</v>
       </c>
       <c r="E147" s="7"/>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A148" s="17" t="s">
+        <v>467</v>
+      </c>
+      <c r="B148" s="7" t="s">
+        <v>468</v>
+      </c>
+      <c r="C148" s="8" t="s">
+        <v>469</v>
+      </c>
+      <c r="D148" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E148" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
WAT 166,167 and 168 scripts implementation
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/WAT.xlsx
+++ b/src/test/resources/xls/WAT.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13305" windowHeight="2415"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751" uniqueCount="470">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="763" uniqueCount="479">
   <si>
     <t>TCID</t>
   </si>
@@ -1428,13 +1428,40 @@
   </si>
   <si>
     <t>Verify that divider or spacing is present to visually separate selected options</t>
+  </si>
+  <si>
+    <t>WAT166</t>
+  </si>
+  <si>
+    <t>WAT167</t>
+  </si>
+  <si>
+    <t>WAT168</t>
+  </si>
+  <si>
+    <t>WAT-654</t>
+  </si>
+  <si>
+    <t>WAT-655</t>
+  </si>
+  <si>
+    <t>WAT-656</t>
+  </si>
+  <si>
+    <t>Verify that user is able to sort author records/results using Sort by 'Relevance'</t>
+  </si>
+  <si>
+    <t>Verify that user is able to sort author records/results using Sort by 'Publication years (newest first)'</t>
+  </si>
+  <si>
+    <t>Verify that user is able to sort author records/results using Sort by 'Publication years (oldest first)'</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1643,7 +1670,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1675,10 +1702,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1710,7 +1736,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1886,23 +1911,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E148"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E151"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A133" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C148" sqref="C148"/>
+      <selection activeCell="C155" sqref="C155"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="41" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="30.5703125" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="138.140625" style="6" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1919,7 +1944,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -1934,7 +1959,7 @@
       </c>
       <c r="E2" s="4"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -1949,7 +1974,7 @@
       </c>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" s="7" t="s">
         <v>11</v>
       </c>
@@ -1964,7 +1989,7 @@
       </c>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" s="7" t="s">
         <v>12</v>
       </c>
@@ -1979,7 +2004,7 @@
       </c>
       <c r="E5" s="7"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" s="7" t="s">
         <v>14</v>
       </c>
@@ -1994,7 +2019,7 @@
       </c>
       <c r="E6" s="7"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" s="7" t="s">
         <v>17</v>
       </c>
@@ -2009,7 +2034,7 @@
       </c>
       <c r="E7" s="7"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" s="7" t="s">
         <v>20</v>
       </c>
@@ -2024,7 +2049,7 @@
       </c>
       <c r="E8" s="7"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" s="7" t="s">
         <v>22</v>
       </c>
@@ -2039,7 +2064,7 @@
       </c>
       <c r="E9" s="7"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10" s="7" t="s">
         <v>23</v>
       </c>
@@ -2054,7 +2079,7 @@
       </c>
       <c r="E10" s="7"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11" s="7" t="s">
         <v>24</v>
       </c>
@@ -2069,7 +2094,7 @@
       </c>
       <c r="E11" s="7"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12" s="7" t="s">
         <v>25</v>
       </c>
@@ -2084,7 +2109,7 @@
       </c>
       <c r="E12" s="7"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13" s="7" t="s">
         <v>62</v>
       </c>
@@ -2099,7 +2124,7 @@
       </c>
       <c r="E13" s="7"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="A14" s="7" t="s">
         <v>63</v>
       </c>
@@ -2114,7 +2139,7 @@
       </c>
       <c r="E14" s="7"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="A15" s="7" t="s">
         <v>64</v>
       </c>
@@ -2129,7 +2154,7 @@
       </c>
       <c r="E15" s="7"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="A16" s="7" t="s">
         <v>65</v>
       </c>
@@ -2144,7 +2169,7 @@
       </c>
       <c r="E16" s="7"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5">
       <c r="A17" s="7" t="s">
         <v>74</v>
       </c>
@@ -2159,7 +2184,7 @@
       </c>
       <c r="E17" s="7"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5">
       <c r="A18" s="7" t="s">
         <v>75</v>
       </c>
@@ -2174,7 +2199,7 @@
       </c>
       <c r="E18" s="7"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5">
       <c r="A19" s="7" t="s">
         <v>79</v>
       </c>
@@ -2189,7 +2214,7 @@
       </c>
       <c r="E19" s="7"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5">
       <c r="A20" s="7" t="s">
         <v>81</v>
       </c>
@@ -2204,7 +2229,7 @@
       </c>
       <c r="E20" s="7"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5">
       <c r="A21" s="7" t="s">
         <v>82</v>
       </c>
@@ -2219,7 +2244,7 @@
       </c>
       <c r="E21" s="7"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5">
       <c r="A22" s="7" t="s">
         <v>88</v>
       </c>
@@ -2234,7 +2259,7 @@
       </c>
       <c r="E22" s="7"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5">
       <c r="A23" s="7" t="s">
         <v>90</v>
       </c>
@@ -2249,7 +2274,7 @@
       </c>
       <c r="E23" s="7"/>
     </row>
-    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="30">
       <c r="A24" s="9" t="s">
         <v>94</v>
       </c>
@@ -2264,7 +2289,7 @@
       </c>
       <c r="E24" s="7"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5">
       <c r="A25" s="9" t="s">
         <v>96</v>
       </c>
@@ -2279,7 +2304,7 @@
       </c>
       <c r="E25" s="7"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5">
       <c r="A26" s="9" t="s">
         <v>98</v>
       </c>
@@ -2294,7 +2319,7 @@
       </c>
       <c r="E26" s="7"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5">
       <c r="A27" s="9" t="s">
         <v>102</v>
       </c>
@@ -2309,7 +2334,7 @@
       </c>
       <c r="E27" s="7"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5">
       <c r="A28" s="9" t="s">
         <v>105</v>
       </c>
@@ -2324,7 +2349,7 @@
       </c>
       <c r="E28" s="7"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5">
       <c r="A29" s="9" t="s">
         <v>108</v>
       </c>
@@ -2339,7 +2364,7 @@
       </c>
       <c r="E29" s="7"/>
     </row>
-    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" ht="30">
       <c r="A30" s="9" t="s">
         <v>110</v>
       </c>
@@ -2354,7 +2379,7 @@
       </c>
       <c r="E30" s="7"/>
     </row>
-    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" ht="30">
       <c r="A31" s="9" t="s">
         <v>114</v>
       </c>
@@ -2369,7 +2394,7 @@
       </c>
       <c r="E31" s="7"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5">
       <c r="A32" s="9" t="s">
         <v>119</v>
       </c>
@@ -2384,7 +2409,7 @@
       </c>
       <c r="E32" s="7"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5">
       <c r="A33" s="9" t="s">
         <v>120</v>
       </c>
@@ -2399,7 +2424,7 @@
       </c>
       <c r="E33" s="7"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5">
       <c r="A34" s="9" t="s">
         <v>125</v>
       </c>
@@ -2414,7 +2439,7 @@
       </c>
       <c r="E34" s="7"/>
     </row>
-    <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" ht="30">
       <c r="A35" s="9" t="s">
         <v>128</v>
       </c>
@@ -2429,7 +2454,7 @@
       </c>
       <c r="E35" s="7"/>
     </row>
-    <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" ht="30">
       <c r="A36" s="9" t="s">
         <v>131</v>
       </c>
@@ -2444,7 +2469,7 @@
       </c>
       <c r="E36" s="7"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5">
       <c r="A37" s="9" t="s">
         <v>134</v>
       </c>
@@ -2459,7 +2484,7 @@
       </c>
       <c r="E37" s="7"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5">
       <c r="A38" s="9" t="s">
         <v>137</v>
       </c>
@@ -2474,7 +2499,7 @@
       </c>
       <c r="E38" s="7"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5">
       <c r="A39" s="9" t="s">
         <v>140</v>
       </c>
@@ -2489,7 +2514,7 @@
       </c>
       <c r="E39" s="7"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5">
       <c r="A40" s="9" t="s">
         <v>143</v>
       </c>
@@ -2504,7 +2529,7 @@
       </c>
       <c r="E40" s="7"/>
     </row>
-    <row r="41" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" ht="30">
       <c r="A41" s="9" t="s">
         <v>145</v>
       </c>
@@ -2519,7 +2544,7 @@
       </c>
       <c r="E41" s="7"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5">
       <c r="A42" s="9" t="s">
         <v>147</v>
       </c>
@@ -2534,7 +2559,7 @@
       </c>
       <c r="E42" s="7"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5">
       <c r="A43" s="9" t="s">
         <v>150</v>
       </c>
@@ -2549,7 +2574,7 @@
       </c>
       <c r="E43" s="7"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5">
       <c r="A44" s="9" t="s">
         <v>153</v>
       </c>
@@ -2564,7 +2589,7 @@
       </c>
       <c r="E44" s="7"/>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5">
       <c r="A45" s="9" t="s">
         <v>155</v>
       </c>
@@ -2579,7 +2604,7 @@
       </c>
       <c r="E45" s="7"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5">
       <c r="A46" s="12" t="s">
         <v>158</v>
       </c>
@@ -2594,7 +2619,7 @@
       </c>
       <c r="E46" s="7"/>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5">
       <c r="A47" s="12" t="s">
         <v>159</v>
       </c>
@@ -2609,7 +2634,7 @@
       </c>
       <c r="E47" s="7"/>
     </row>
-    <row r="48" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" ht="30">
       <c r="A48" s="12" t="s">
         <v>160</v>
       </c>
@@ -2624,7 +2649,7 @@
       </c>
       <c r="E48" s="7"/>
     </row>
-    <row r="49" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" ht="30">
       <c r="A49" s="12" t="s">
         <v>161</v>
       </c>
@@ -2639,7 +2664,7 @@
       </c>
       <c r="E49" s="7"/>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5">
       <c r="A50" s="12" t="s">
         <v>164</v>
       </c>
@@ -2654,7 +2679,7 @@
       </c>
       <c r="E50" s="7"/>
     </row>
-    <row r="51" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" ht="30">
       <c r="A51" s="9" t="s">
         <v>173</v>
       </c>
@@ -2669,7 +2694,7 @@
       </c>
       <c r="E51" s="7"/>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5">
       <c r="A52" s="9" t="s">
         <v>174</v>
       </c>
@@ -2684,7 +2709,7 @@
       </c>
       <c r="E52" s="7"/>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5">
       <c r="A53" s="9" t="s">
         <v>179</v>
       </c>
@@ -2699,7 +2724,7 @@
       </c>
       <c r="E53" s="7"/>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5">
       <c r="A54" s="9" t="s">
         <v>180</v>
       </c>
@@ -2714,7 +2739,7 @@
       </c>
       <c r="E54" s="7"/>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5">
       <c r="A55" s="9" t="s">
         <v>185</v>
       </c>
@@ -2729,7 +2754,7 @@
       </c>
       <c r="E55" s="7"/>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5">
       <c r="A56" s="9" t="s">
         <v>188</v>
       </c>
@@ -2744,7 +2769,7 @@
       </c>
       <c r="E56" s="7"/>
     </row>
-    <row r="57" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" ht="30">
       <c r="A57" s="9" t="s">
         <v>191</v>
       </c>
@@ -2759,7 +2784,7 @@
       </c>
       <c r="E57" s="7"/>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5">
       <c r="A58" s="9" t="s">
         <v>194</v>
       </c>
@@ -2774,7 +2799,7 @@
       </c>
       <c r="E58" s="7"/>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5">
       <c r="A59" s="7" t="s">
         <v>196</v>
       </c>
@@ -2789,7 +2814,7 @@
       </c>
       <c r="E59" s="7"/>
     </row>
-    <row r="60" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" ht="45">
       <c r="A60" s="7" t="s">
         <v>199</v>
       </c>
@@ -2804,7 +2829,7 @@
       </c>
       <c r="E60" s="7"/>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5">
       <c r="A61" s="9" t="s">
         <v>202</v>
       </c>
@@ -2819,7 +2844,7 @@
       </c>
       <c r="E61" s="7"/>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5">
       <c r="A62" s="9" t="s">
         <v>204</v>
       </c>
@@ -2834,7 +2859,7 @@
       </c>
       <c r="E62" s="7"/>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5">
       <c r="A63" s="9" t="s">
         <v>206</v>
       </c>
@@ -2849,7 +2874,7 @@
       </c>
       <c r="E63" s="7"/>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5">
       <c r="A64" s="9" t="s">
         <v>208</v>
       </c>
@@ -2864,7 +2889,7 @@
       </c>
       <c r="E64" s="7"/>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5">
       <c r="A65" s="9" t="s">
         <v>217</v>
       </c>
@@ -2879,7 +2904,7 @@
       </c>
       <c r="E65" s="7"/>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5">
       <c r="A66" s="9" t="s">
         <v>218</v>
       </c>
@@ -2894,7 +2919,7 @@
       </c>
       <c r="E66" s="7"/>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5">
       <c r="A67" s="9" t="s">
         <v>223</v>
       </c>
@@ -2909,7 +2934,7 @@
       </c>
       <c r="E67" s="7"/>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5">
       <c r="A68" s="9" t="s">
         <v>224</v>
       </c>
@@ -2924,7 +2949,7 @@
       </c>
       <c r="E68" s="7"/>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5">
       <c r="A69" s="9" t="s">
         <v>225</v>
       </c>
@@ -2939,7 +2964,7 @@
       </c>
       <c r="E69" s="7"/>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5">
       <c r="A70" s="9" t="s">
         <v>226</v>
       </c>
@@ -2954,7 +2979,7 @@
       </c>
       <c r="E70" s="7"/>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5">
       <c r="A71" s="9" t="s">
         <v>233</v>
       </c>
@@ -2969,7 +2994,7 @@
       </c>
       <c r="E71" s="7"/>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5">
       <c r="A72" s="9" t="s">
         <v>237</v>
       </c>
@@ -2984,7 +3009,7 @@
       </c>
       <c r="E72" s="7"/>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5">
       <c r="A73" s="9" t="s">
         <v>239</v>
       </c>
@@ -2999,7 +3024,7 @@
       </c>
       <c r="E73" s="7"/>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5">
       <c r="A74" s="9" t="s">
         <v>243</v>
       </c>
@@ -3014,7 +3039,7 @@
       </c>
       <c r="E74" s="7"/>
     </row>
-    <row r="75" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" ht="30">
       <c r="A75" s="9" t="s">
         <v>245</v>
       </c>
@@ -3029,7 +3054,7 @@
       </c>
       <c r="E75" s="7"/>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5">
       <c r="A76" s="9" t="s">
         <v>248</v>
       </c>
@@ -3044,7 +3069,7 @@
       </c>
       <c r="E76" s="7"/>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5">
       <c r="A77" s="9" t="s">
         <v>256</v>
       </c>
@@ -3059,7 +3084,7 @@
       </c>
       <c r="E77" s="7"/>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5">
       <c r="A78" s="9" t="s">
         <v>257</v>
       </c>
@@ -3074,7 +3099,7 @@
       </c>
       <c r="E78" s="7"/>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5">
       <c r="A79" s="9" t="s">
         <v>261</v>
       </c>
@@ -3089,7 +3114,7 @@
       </c>
       <c r="E79" s="7"/>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5">
       <c r="A80" s="9" t="s">
         <v>264</v>
       </c>
@@ -3104,7 +3129,7 @@
       </c>
       <c r="E80" s="7"/>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5">
       <c r="A81" s="9" t="s">
         <v>267</v>
       </c>
@@ -3119,7 +3144,7 @@
       </c>
       <c r="E81" s="7"/>
     </row>
-    <row r="82" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" ht="30">
       <c r="A82" s="9" t="s">
         <v>269</v>
       </c>
@@ -3134,7 +3159,7 @@
       </c>
       <c r="E82" s="7"/>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5">
       <c r="A83" s="9" t="s">
         <v>274</v>
       </c>
@@ -3149,7 +3174,7 @@
       </c>
       <c r="E83" s="7"/>
     </row>
-    <row r="84" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" ht="30">
       <c r="A84" s="9" t="s">
         <v>277</v>
       </c>
@@ -3164,7 +3189,7 @@
       </c>
       <c r="E84" s="7"/>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5">
       <c r="A85" s="9" t="s">
         <v>279</v>
       </c>
@@ -3179,7 +3204,7 @@
       </c>
       <c r="E85" s="7"/>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5">
       <c r="A86" s="9" t="s">
         <v>282</v>
       </c>
@@ -3194,7 +3219,7 @@
       </c>
       <c r="E86" s="7"/>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5">
       <c r="A87" s="9" t="s">
         <v>285</v>
       </c>
@@ -3209,7 +3234,7 @@
       </c>
       <c r="E87" s="7"/>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5">
       <c r="A88" s="9" t="s">
         <v>288</v>
       </c>
@@ -3224,7 +3249,7 @@
       </c>
       <c r="E88" s="7"/>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5">
       <c r="A89" s="9" t="s">
         <v>291</v>
       </c>
@@ -3239,7 +3264,7 @@
       </c>
       <c r="E89" s="7"/>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5">
       <c r="A90" s="9" t="s">
         <v>294</v>
       </c>
@@ -3254,7 +3279,7 @@
       </c>
       <c r="E90" s="7"/>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5">
       <c r="A91" s="9" t="s">
         <v>297</v>
       </c>
@@ -3269,7 +3294,7 @@
       </c>
       <c r="E91" s="7"/>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5">
       <c r="A92" s="9" t="s">
         <v>300</v>
       </c>
@@ -3284,7 +3309,7 @@
       </c>
       <c r="E92" s="7"/>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5">
       <c r="A93" s="9" t="s">
         <v>303</v>
       </c>
@@ -3299,7 +3324,7 @@
       </c>
       <c r="E93" s="7"/>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5">
       <c r="A94" s="9" t="s">
         <v>306</v>
       </c>
@@ -3314,7 +3339,7 @@
       </c>
       <c r="E94" s="7"/>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5">
       <c r="A95" s="9" t="s">
         <v>309</v>
       </c>
@@ -3329,7 +3354,7 @@
       </c>
       <c r="E95" s="7"/>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5">
       <c r="A96" s="9" t="s">
         <v>314</v>
       </c>
@@ -3344,7 +3369,7 @@
       </c>
       <c r="E96" s="7"/>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5">
       <c r="A97" s="9" t="s">
         <v>315</v>
       </c>
@@ -3359,7 +3384,7 @@
       </c>
       <c r="E97" s="7"/>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5">
       <c r="A98" s="9" t="s">
         <v>319</v>
       </c>
@@ -3374,7 +3399,7 @@
       </c>
       <c r="E98" s="7"/>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5">
       <c r="A99" s="9" t="s">
         <v>321</v>
       </c>
@@ -3389,7 +3414,7 @@
       </c>
       <c r="E99" s="7"/>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5">
       <c r="A100" s="9" t="s">
         <v>322</v>
       </c>
@@ -3404,7 +3429,7 @@
       </c>
       <c r="E100" s="7"/>
     </row>
-    <row r="101" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" ht="30">
       <c r="A101" s="9" t="s">
         <v>323</v>
       </c>
@@ -3419,7 +3444,7 @@
       </c>
       <c r="E101" s="7"/>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5">
       <c r="A102" s="9" t="s">
         <v>328</v>
       </c>
@@ -3434,7 +3459,7 @@
       </c>
       <c r="E102" s="7"/>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5">
       <c r="A103" s="9" t="s">
         <v>333</v>
       </c>
@@ -3449,7 +3474,7 @@
       </c>
       <c r="E103" s="7"/>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5">
       <c r="A104" s="9" t="s">
         <v>336</v>
       </c>
@@ -3464,7 +3489,7 @@
       </c>
       <c r="E104" s="7"/>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5">
       <c r="A105" s="9" t="s">
         <v>337</v>
       </c>
@@ -3479,7 +3504,7 @@
       </c>
       <c r="E105" s="7"/>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5">
       <c r="A106" s="9" t="s">
         <v>342</v>
       </c>
@@ -3494,7 +3519,7 @@
       </c>
       <c r="E106" s="7"/>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5">
       <c r="A107" s="9" t="s">
         <v>345</v>
       </c>
@@ -3509,7 +3534,7 @@
       </c>
       <c r="E107" s="7"/>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5">
       <c r="A108" s="9" t="s">
         <v>350</v>
       </c>
@@ -3524,7 +3549,7 @@
       </c>
       <c r="E108" s="7"/>
     </row>
-    <row r="109" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" ht="30">
       <c r="A109" s="9" t="s">
         <v>351</v>
       </c>
@@ -3539,7 +3564,7 @@
       </c>
       <c r="E109" s="7"/>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5">
       <c r="A110" s="9" t="s">
         <v>354</v>
       </c>
@@ -3554,7 +3579,7 @@
       </c>
       <c r="E110" s="7"/>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5">
       <c r="A111" s="9" t="s">
         <v>357</v>
       </c>
@@ -3569,7 +3594,7 @@
       </c>
       <c r="E111" s="7"/>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5">
       <c r="A112" s="9" t="s">
         <v>361</v>
       </c>
@@ -3584,7 +3609,7 @@
       </c>
       <c r="E112" s="7"/>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5">
       <c r="A113" s="9" t="s">
         <v>363</v>
       </c>
@@ -3599,7 +3624,7 @@
       </c>
       <c r="E113" s="7"/>
     </row>
-    <row r="114" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" ht="30">
       <c r="A114" s="9" t="s">
         <v>366</v>
       </c>
@@ -3614,7 +3639,7 @@
       </c>
       <c r="E114" s="7"/>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5">
       <c r="A115" s="9" t="s">
         <v>369</v>
       </c>
@@ -3629,7 +3654,7 @@
       </c>
       <c r="E115" s="7"/>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5">
       <c r="A116" s="9" t="s">
         <v>370</v>
       </c>
@@ -3644,7 +3669,7 @@
       </c>
       <c r="E116" s="7"/>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5">
       <c r="A117" s="9" t="s">
         <v>371</v>
       </c>
@@ -3659,7 +3684,7 @@
       </c>
       <c r="E117" s="7"/>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5">
       <c r="A118" s="9" t="s">
         <v>378</v>
       </c>
@@ -3674,7 +3699,7 @@
       </c>
       <c r="E118" s="7"/>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5">
       <c r="A119" s="9" t="s">
         <v>381</v>
       </c>
@@ -3689,7 +3714,7 @@
       </c>
       <c r="E119" s="7"/>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5">
       <c r="A120" s="9" t="s">
         <v>384</v>
       </c>
@@ -3704,7 +3729,7 @@
       </c>
       <c r="E120" s="7"/>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5">
       <c r="A121" s="9" t="s">
         <v>387</v>
       </c>
@@ -3719,7 +3744,7 @@
       </c>
       <c r="E121" s="7"/>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5">
       <c r="A122" s="7" t="s">
         <v>390</v>
       </c>
@@ -3734,7 +3759,7 @@
       </c>
       <c r="E122" s="7"/>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5">
       <c r="A123" s="7" t="s">
         <v>393</v>
       </c>
@@ -3749,7 +3774,7 @@
       </c>
       <c r="E123" s="7"/>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5">
       <c r="A124" s="7" t="s">
         <v>396</v>
       </c>
@@ -3764,7 +3789,7 @@
       </c>
       <c r="E124" s="7"/>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5">
       <c r="A125" s="9" t="s">
         <v>399</v>
       </c>
@@ -3779,7 +3804,7 @@
       </c>
       <c r="E125" s="7"/>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5">
       <c r="A126" s="7" t="s">
         <v>402</v>
       </c>
@@ -3794,7 +3819,7 @@
       </c>
       <c r="E126" s="7"/>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5">
       <c r="A127" s="7" t="s">
         <v>405</v>
       </c>
@@ -3809,7 +3834,7 @@
       </c>
       <c r="E127" s="7"/>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5">
       <c r="A128" s="7" t="s">
         <v>408</v>
       </c>
@@ -3824,7 +3849,7 @@
       </c>
       <c r="E128" s="7"/>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5">
       <c r="A129" s="9" t="s">
         <v>411</v>
       </c>
@@ -3839,7 +3864,7 @@
       </c>
       <c r="E129" s="7"/>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5">
       <c r="A130" s="9" t="s">
         <v>414</v>
       </c>
@@ -3854,7 +3879,7 @@
       </c>
       <c r="E130" s="7"/>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5">
       <c r="A131" s="9" t="s">
         <v>416</v>
       </c>
@@ -3869,7 +3894,7 @@
       </c>
       <c r="E131" s="7"/>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5">
       <c r="A132" s="7" t="s">
         <v>419</v>
       </c>
@@ -3884,7 +3909,7 @@
       </c>
       <c r="E132" s="7"/>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5">
       <c r="A133" s="9" t="s">
         <v>422</v>
       </c>
@@ -3899,7 +3924,7 @@
       </c>
       <c r="E133" s="7"/>
     </row>
-    <row r="134" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5" ht="30">
       <c r="A134" s="7" t="s">
         <v>425</v>
       </c>
@@ -3914,7 +3939,7 @@
       </c>
       <c r="E134" s="7"/>
     </row>
-    <row r="135" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5" ht="30">
       <c r="A135" s="7" t="s">
         <v>426</v>
       </c>
@@ -3929,7 +3954,7 @@
       </c>
       <c r="E135" s="7"/>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5">
       <c r="A136" s="9" t="s">
         <v>431</v>
       </c>
@@ -3944,7 +3969,7 @@
       </c>
       <c r="E136" s="7"/>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5">
       <c r="A137" s="7" t="s">
         <v>434</v>
       </c>
@@ -3959,7 +3984,7 @@
       </c>
       <c r="E137" s="7"/>
     </row>
-    <row r="138" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" ht="45">
       <c r="A138" s="7" t="s">
         <v>435</v>
       </c>
@@ -3974,7 +3999,7 @@
       </c>
       <c r="E138" s="7"/>
     </row>
-    <row r="139" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5" ht="30">
       <c r="A139" s="7" t="s">
         <v>436</v>
       </c>
@@ -3989,7 +4014,7 @@
       </c>
       <c r="E139" s="7"/>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5">
       <c r="A140" s="17" t="s">
         <v>443</v>
       </c>
@@ -4004,7 +4029,7 @@
       </c>
       <c r="E140" s="7"/>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5">
       <c r="A141" s="17" t="s">
         <v>446</v>
       </c>
@@ -4019,7 +4044,7 @@
       </c>
       <c r="E141" s="7"/>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:5">
       <c r="A142" s="17" t="s">
         <v>449</v>
       </c>
@@ -4034,7 +4059,7 @@
       </c>
       <c r="E142" s="7"/>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:5">
       <c r="A143" s="17" t="s">
         <v>452</v>
       </c>
@@ -4049,7 +4074,7 @@
       </c>
       <c r="E143" s="7"/>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:5">
       <c r="A144" s="17" t="s">
         <v>453</v>
       </c>
@@ -4064,7 +4089,7 @@
       </c>
       <c r="E144" s="7"/>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:5">
       <c r="A145" s="17" t="s">
         <v>458</v>
       </c>
@@ -4079,7 +4104,7 @@
       </c>
       <c r="E145" s="7"/>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:5">
       <c r="A146" s="17" t="s">
         <v>461</v>
       </c>
@@ -4094,7 +4119,7 @@
       </c>
       <c r="E146" s="7"/>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:5">
       <c r="A147" s="17" t="s">
         <v>464</v>
       </c>
@@ -4109,7 +4134,7 @@
       </c>
       <c r="E147" s="7"/>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:5">
       <c r="A148" s="17" t="s">
         <v>467</v>
       </c>
@@ -4123,6 +4148,51 @@
         <v>5</v>
       </c>
       <c r="E148" s="7"/>
+    </row>
+    <row r="149" spans="1:5">
+      <c r="A149" s="7" t="s">
+        <v>470</v>
+      </c>
+      <c r="B149" s="7" t="s">
+        <v>473</v>
+      </c>
+      <c r="C149" s="8" t="s">
+        <v>476</v>
+      </c>
+      <c r="D149" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E149" s="7"/>
+    </row>
+    <row r="150" spans="1:5">
+      <c r="A150" s="7" t="s">
+        <v>471</v>
+      </c>
+      <c r="B150" s="7" t="s">
+        <v>474</v>
+      </c>
+      <c r="C150" s="8" t="s">
+        <v>477</v>
+      </c>
+      <c r="D150" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E150" s="7"/>
+    </row>
+    <row r="151" spans="1:5">
+      <c r="A151" s="7" t="s">
+        <v>472</v>
+      </c>
+      <c r="B151" s="7" t="s">
+        <v>475</v>
+      </c>
+      <c r="C151" s="8" t="s">
+        <v>478</v>
+      </c>
+      <c r="D151" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E151" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -4135,14 +4205,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView topLeftCell="A10" zoomScale="80" workbookViewId="0">
       <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
@@ -4150,7 +4220,7 @@
     <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="10" t="s">
         <v>35</v>
       </c>
@@ -4164,7 +4234,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="7" t="s">
         <v>37</v>
       </c>
@@ -4176,7 +4246,7 @@
       </c>
       <c r="D2" s="7"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="7" t="s">
         <v>38</v>
       </c>
@@ -4188,7 +4258,7 @@
       </c>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="7" t="s">
         <v>39</v>
       </c>
@@ -4200,7 +4270,7 @@
       </c>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" s="7" t="s">
         <v>40</v>
       </c>
@@ -4212,7 +4282,7 @@
       </c>
       <c r="D5" s="7"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" s="7" t="s">
         <v>41</v>
       </c>
@@ -4224,7 +4294,7 @@
       </c>
       <c r="D6" s="7"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="7" t="s">
         <v>42</v>
       </c>
@@ -4236,7 +4306,7 @@
       </c>
       <c r="D7" s="7"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="7" t="s">
         <v>43</v>
       </c>
@@ -4248,7 +4318,7 @@
       </c>
       <c r="D8" s="7"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="7" t="s">
         <v>44</v>
       </c>
@@ -4260,7 +4330,7 @@
       </c>
       <c r="D9" s="7"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="7" t="s">
         <v>45</v>
       </c>
@@ -4272,7 +4342,7 @@
       </c>
       <c r="D10" s="7"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11" s="7" t="s">
         <v>46</v>
       </c>
@@ -4284,7 +4354,7 @@
       </c>
       <c r="D11" s="7"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="A12" s="7" t="s">
         <v>48</v>
       </c>
@@ -4296,7 +4366,7 @@
       </c>
       <c r="D12" s="7"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="A13" s="7" t="s">
         <v>49</v>
       </c>
@@ -4308,7 +4378,7 @@
       </c>
       <c r="D13" s="7"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="A14" s="7" t="s">
         <v>50</v>
       </c>
@@ -4320,7 +4390,7 @@
       </c>
       <c r="D14" s="7"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="A15" s="7" t="s">
         <v>51</v>
       </c>
@@ -4332,7 +4402,7 @@
       </c>
       <c r="D15" s="7"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="A16" s="7" t="s">
         <v>52</v>
       </c>
@@ -4344,7 +4414,7 @@
       </c>
       <c r="D16" s="7"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4">
       <c r="A17" s="7" t="s">
         <v>53</v>
       </c>
@@ -4356,7 +4426,7 @@
       </c>
       <c r="D17" s="7"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4">
       <c r="A18" s="7" t="s">
         <v>54</v>
       </c>
@@ -4368,7 +4438,7 @@
       </c>
       <c r="D18" s="7"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4">
       <c r="A19" s="7" t="s">
         <v>55</v>
       </c>
@@ -4380,7 +4450,7 @@
       </c>
       <c r="D19" s="7"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4">
       <c r="A20" s="7" t="s">
         <v>56</v>
       </c>
@@ -4392,7 +4462,7 @@
       </c>
       <c r="D20" s="7"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4">
       <c r="A21" s="7" t="s">
         <v>57</v>
       </c>
@@ -4404,7 +4474,7 @@
       </c>
       <c r="D21" s="7"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4">
       <c r="A22" s="7" t="s">
         <v>58</v>
       </c>
@@ -4416,7 +4486,7 @@
       </c>
       <c r="D22" s="7"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4">
       <c r="A23" s="7" t="s">
         <v>59</v>
       </c>
@@ -4428,7 +4498,7 @@
       </c>
       <c r="D23" s="7"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4">
       <c r="A24" s="7" t="s">
         <v>60</v>
       </c>
@@ -4440,7 +4510,7 @@
       </c>
       <c r="D24" s="7"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4">
       <c r="A25" s="7" t="s">
         <v>61</v>
       </c>
@@ -4452,7 +4522,7 @@
       </c>
       <c r="D25" s="7"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4">
       <c r="A26" s="7" t="s">
         <v>47</v>
       </c>
@@ -4471,14 +4541,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A19" sqref="A19:XFD19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
@@ -4486,7 +4556,7 @@
     <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="10" t="s">
         <v>35</v>
       </c>
@@ -4500,7 +4570,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="7" t="s">
         <v>37</v>
       </c>
@@ -4512,7 +4582,7 @@
       </c>
       <c r="D2" s="7"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="7" t="s">
         <v>38</v>
       </c>
@@ -4524,7 +4594,7 @@
       </c>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="7" t="s">
         <v>39</v>
       </c>
@@ -4536,7 +4606,7 @@
       </c>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" s="7" t="s">
         <v>40</v>
       </c>
@@ -4548,7 +4618,7 @@
       </c>
       <c r="D5" s="7"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" s="7" t="s">
         <v>41</v>
       </c>
@@ -4560,7 +4630,7 @@
       </c>
       <c r="D6" s="7"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="7" t="s">
         <v>42</v>
       </c>
@@ -4572,7 +4642,7 @@
       </c>
       <c r="D7" s="7"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="7" t="s">
         <v>43</v>
       </c>
@@ -4584,7 +4654,7 @@
       </c>
       <c r="D8" s="7"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="7" t="s">
         <v>44</v>
       </c>
@@ -4596,7 +4666,7 @@
       </c>
       <c r="D9" s="7"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="7" t="s">
         <v>45</v>
       </c>
@@ -4608,7 +4678,7 @@
       </c>
       <c r="D10" s="7"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11" s="7" t="s">
         <v>46</v>
       </c>
@@ -4620,7 +4690,7 @@
       </c>
       <c r="D11" s="7"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="A12" s="7" t="s">
         <v>47</v>
       </c>
@@ -4632,7 +4702,7 @@
       </c>
       <c r="D12" s="7"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="A13" s="7" t="s">
         <v>48</v>
       </c>
@@ -4644,7 +4714,7 @@
       </c>
       <c r="D13" s="7"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="A14" s="7" t="s">
         <v>49</v>
       </c>
@@ -4656,7 +4726,7 @@
       </c>
       <c r="D14" s="7"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="A15" s="7" t="s">
         <v>50</v>
       </c>
@@ -4668,7 +4738,7 @@
       </c>
       <c r="D15" s="7"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="A16" s="7" t="s">
         <v>51</v>
       </c>
@@ -4680,7 +4750,7 @@
       </c>
       <c r="D16" s="7"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4">
       <c r="A17" s="7" t="s">
         <v>52</v>
       </c>
@@ -4692,7 +4762,7 @@
       </c>
       <c r="D17" s="7"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4">
       <c r="A18" s="7" t="s">
         <v>53</v>
       </c>
@@ -4704,7 +4774,7 @@
       </c>
       <c r="D18" s="7"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4">
       <c r="A19" s="7" t="s">
         <v>54</v>
       </c>
@@ -4716,7 +4786,7 @@
       </c>
       <c r="D19" s="7"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4">
       <c r="A20" s="7" t="s">
         <v>55</v>
       </c>
@@ -4728,7 +4798,7 @@
       </c>
       <c r="D20" s="7"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4">
       <c r="A21" s="7" t="s">
         <v>56</v>
       </c>
@@ -4740,7 +4810,7 @@
       </c>
       <c r="D21" s="7"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4">
       <c r="A22" s="7" t="s">
         <v>57</v>
       </c>
@@ -4752,7 +4822,7 @@
       </c>
       <c r="D22" s="7"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4">
       <c r="A23" s="7" t="s">
         <v>58</v>
       </c>
@@ -4764,7 +4834,7 @@
       </c>
       <c r="D23" s="7"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4">
       <c r="A24" s="7" t="s">
         <v>59</v>
       </c>
@@ -4776,7 +4846,7 @@
       </c>
       <c r="D24" s="7"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4">
       <c r="A25" s="7" t="s">
         <v>60</v>
       </c>
@@ -4788,7 +4858,7 @@
       </c>
       <c r="D25" s="7"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4">
       <c r="A26" s="7" t="s">
         <v>61</v>
       </c>

</xml_diff>

<commit_message>
WAT 169 script implementation
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/WAT.xlsx
+++ b/src/test/resources/xls/WAT.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="763" uniqueCount="479">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="767" uniqueCount="482">
   <si>
     <t>TCID</t>
   </si>
@@ -1455,6 +1455,15 @@
   </si>
   <si>
     <t>Verify that user is able to sort author records/results using Sort by 'Publication years (oldest first)'</t>
+  </si>
+  <si>
+    <t>WAT169</t>
+  </si>
+  <si>
+    <t>WAT-1398</t>
+  </si>
+  <si>
+    <t>Verify that author records list in the author results page should support following sorted options: 1.Relevance (Top hits, aggregated by count {Number of publications}), 2.Publication years (newest first) 3. Publication years (oldest first).</t>
   </si>
 </sst>
 </file>
@@ -1912,10 +1921,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E151"/>
+  <dimension ref="A1:E152"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A133" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C155" sqref="C155"/>
+      <selection activeCell="A152" sqref="A152:E152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4193,6 +4202,21 @@
         <v>5</v>
       </c>
       <c r="E151" s="7"/>
+    </row>
+    <row r="152" spans="1:5" ht="30">
+      <c r="A152" s="7" t="s">
+        <v>479</v>
+      </c>
+      <c r="B152" s="7" t="s">
+        <v>480</v>
+      </c>
+      <c r="C152" s="8" t="s">
+        <v>481</v>
+      </c>
+      <c r="D152" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E152" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Adds WAT-133 test script and related changes
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/WAT.xlsx
+++ b/src/test/resources/xls/WAT.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13305" windowHeight="2415"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="767" uniqueCount="482">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="771" uniqueCount="484">
   <si>
     <t>TCID</t>
   </si>
@@ -1464,13 +1464,19 @@
   </si>
   <si>
     <t>Verify that author records list in the author results page should support following sorted options: 1.Relevance (Top hits, aggregated by count {Number of publications}), 2.Publication years (newest first) 3. Publication years (oldest first).</t>
+  </si>
+  <si>
+    <t>WAT133</t>
+  </si>
+  <si>
+    <t>Verify that system must display a "Suggest updates" button, which when clicked will enter into curation mode.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1679,7 +1685,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1711,9 +1717,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1745,6 +1752,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1920,14 +1928,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E152"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E153"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A133" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A152" sqref="A152:E152"/>
+      <selection activeCell="C153" sqref="C153"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="30.5703125" customWidth="1" collapsed="1"/>
@@ -1936,7 +1944,7 @@
     <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1953,7 +1961,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -1968,7 +1976,7 @@
       </c>
       <c r="E2" s="4"/>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -1983,7 +1991,7 @@
       </c>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>11</v>
       </c>
@@ -1998,7 +2006,7 @@
       </c>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>12</v>
       </c>
@@ -2013,7 +2021,7 @@
       </c>
       <c r="E5" s="7"/>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>14</v>
       </c>
@@ -2028,7 +2036,7 @@
       </c>
       <c r="E6" s="7"/>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>17</v>
       </c>
@@ -2043,7 +2051,7 @@
       </c>
       <c r="E7" s="7"/>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>20</v>
       </c>
@@ -2058,7 +2066,7 @@
       </c>
       <c r="E8" s="7"/>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>22</v>
       </c>
@@ -2073,7 +2081,7 @@
       </c>
       <c r="E9" s="7"/>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>23</v>
       </c>
@@ -2088,7 +2096,7 @@
       </c>
       <c r="E10" s="7"/>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>24</v>
       </c>
@@ -2103,7 +2111,7 @@
       </c>
       <c r="E11" s="7"/>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>25</v>
       </c>
@@ -2118,7 +2126,7 @@
       </c>
       <c r="E12" s="7"/>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>62</v>
       </c>
@@ -2133,7 +2141,7 @@
       </c>
       <c r="E13" s="7"/>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>63</v>
       </c>
@@ -2148,7 +2156,7 @@
       </c>
       <c r="E14" s="7"/>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>64</v>
       </c>
@@ -2163,7 +2171,7 @@
       </c>
       <c r="E15" s="7"/>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>65</v>
       </c>
@@ -2178,7 +2186,7 @@
       </c>
       <c r="E16" s="7"/>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>74</v>
       </c>
@@ -2193,7 +2201,7 @@
       </c>
       <c r="E17" s="7"/>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>75</v>
       </c>
@@ -2208,7 +2216,7 @@
       </c>
       <c r="E18" s="7"/>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>79</v>
       </c>
@@ -2223,7 +2231,7 @@
       </c>
       <c r="E19" s="7"/>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>81</v>
       </c>
@@ -2238,7 +2246,7 @@
       </c>
       <c r="E20" s="7"/>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>82</v>
       </c>
@@ -2253,7 +2261,7 @@
       </c>
       <c r="E21" s="7"/>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>88</v>
       </c>
@@ -2268,7 +2276,7 @@
       </c>
       <c r="E22" s="7"/>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>90</v>
       </c>
@@ -2283,7 +2291,7 @@
       </c>
       <c r="E23" s="7"/>
     </row>
-    <row r="24" spans="1:5" ht="30">
+    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>94</v>
       </c>
@@ -2298,7 +2306,7 @@
       </c>
       <c r="E24" s="7"/>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>96</v>
       </c>
@@ -2313,7 +2321,7 @@
       </c>
       <c r="E25" s="7"/>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
         <v>98</v>
       </c>
@@ -2328,7 +2336,7 @@
       </c>
       <c r="E26" s="7"/>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
         <v>102</v>
       </c>
@@ -2343,7 +2351,7 @@
       </c>
       <c r="E27" s="7"/>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
         <v>105</v>
       </c>
@@ -2358,7 +2366,7 @@
       </c>
       <c r="E28" s="7"/>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
         <v>108</v>
       </c>
@@ -2373,7 +2381,7 @@
       </c>
       <c r="E29" s="7"/>
     </row>
-    <row r="30" spans="1:5" ht="30">
+    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
         <v>110</v>
       </c>
@@ -2388,7 +2396,7 @@
       </c>
       <c r="E30" s="7"/>
     </row>
-    <row r="31" spans="1:5" ht="30">
+    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
         <v>114</v>
       </c>
@@ -2403,7 +2411,7 @@
       </c>
       <c r="E31" s="7"/>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
         <v>119</v>
       </c>
@@ -2418,7 +2426,7 @@
       </c>
       <c r="E32" s="7"/>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
         <v>120</v>
       </c>
@@ -2433,7 +2441,7 @@
       </c>
       <c r="E33" s="7"/>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
         <v>125</v>
       </c>
@@ -2448,7 +2456,7 @@
       </c>
       <c r="E34" s="7"/>
     </row>
-    <row r="35" spans="1:5" ht="30">
+    <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
         <v>128</v>
       </c>
@@ -2463,7 +2471,7 @@
       </c>
       <c r="E35" s="7"/>
     </row>
-    <row r="36" spans="1:5" ht="30">
+    <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
         <v>131</v>
       </c>
@@ -2478,7 +2486,7 @@
       </c>
       <c r="E36" s="7"/>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
         <v>134</v>
       </c>
@@ -2493,7 +2501,7 @@
       </c>
       <c r="E37" s="7"/>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="9" t="s">
         <v>137</v>
       </c>
@@ -2508,7 +2516,7 @@
       </c>
       <c r="E38" s="7"/>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="s">
         <v>140</v>
       </c>
@@ -2523,7 +2531,7 @@
       </c>
       <c r="E39" s="7"/>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="9" t="s">
         <v>143</v>
       </c>
@@ -2538,7 +2546,7 @@
       </c>
       <c r="E40" s="7"/>
     </row>
-    <row r="41" spans="1:5" ht="30">
+    <row r="41" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
         <v>145</v>
       </c>
@@ -2553,7 +2561,7 @@
       </c>
       <c r="E41" s="7"/>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="9" t="s">
         <v>147</v>
       </c>
@@ -2568,7 +2576,7 @@
       </c>
       <c r="E42" s="7"/>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="9" t="s">
         <v>150</v>
       </c>
@@ -2583,7 +2591,7 @@
       </c>
       <c r="E43" s="7"/>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="9" t="s">
         <v>153</v>
       </c>
@@ -2598,7 +2606,7 @@
       </c>
       <c r="E44" s="7"/>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="9" t="s">
         <v>155</v>
       </c>
@@ -2613,7 +2621,7 @@
       </c>
       <c r="E45" s="7"/>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="12" t="s">
         <v>158</v>
       </c>
@@ -2628,7 +2636,7 @@
       </c>
       <c r="E46" s="7"/>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="12" t="s">
         <v>159</v>
       </c>
@@ -2643,7 +2651,7 @@
       </c>
       <c r="E47" s="7"/>
     </row>
-    <row r="48" spans="1:5" ht="30">
+    <row r="48" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="12" t="s">
         <v>160</v>
       </c>
@@ -2658,7 +2666,7 @@
       </c>
       <c r="E48" s="7"/>
     </row>
-    <row r="49" spans="1:5" ht="30">
+    <row r="49" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="12" t="s">
         <v>161</v>
       </c>
@@ -2673,7 +2681,7 @@
       </c>
       <c r="E49" s="7"/>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="12" t="s">
         <v>164</v>
       </c>
@@ -2688,7 +2696,7 @@
       </c>
       <c r="E50" s="7"/>
     </row>
-    <row r="51" spans="1:5" ht="30">
+    <row r="51" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="9" t="s">
         <v>173</v>
       </c>
@@ -2703,7 +2711,7 @@
       </c>
       <c r="E51" s="7"/>
     </row>
-    <row r="52" spans="1:5">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="9" t="s">
         <v>174</v>
       </c>
@@ -2718,7 +2726,7 @@
       </c>
       <c r="E52" s="7"/>
     </row>
-    <row r="53" spans="1:5">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="9" t="s">
         <v>179</v>
       </c>
@@ -2733,7 +2741,7 @@
       </c>
       <c r="E53" s="7"/>
     </row>
-    <row r="54" spans="1:5">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="9" t="s">
         <v>180</v>
       </c>
@@ -2748,7 +2756,7 @@
       </c>
       <c r="E54" s="7"/>
     </row>
-    <row r="55" spans="1:5">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="9" t="s">
         <v>185</v>
       </c>
@@ -2763,7 +2771,7 @@
       </c>
       <c r="E55" s="7"/>
     </row>
-    <row r="56" spans="1:5">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="s">
         <v>188</v>
       </c>
@@ -2778,7 +2786,7 @@
       </c>
       <c r="E56" s="7"/>
     </row>
-    <row r="57" spans="1:5" ht="30">
+    <row r="57" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="9" t="s">
         <v>191</v>
       </c>
@@ -2793,7 +2801,7 @@
       </c>
       <c r="E57" s="7"/>
     </row>
-    <row r="58" spans="1:5">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="9" t="s">
         <v>194</v>
       </c>
@@ -2808,7 +2816,7 @@
       </c>
       <c r="E58" s="7"/>
     </row>
-    <row r="59" spans="1:5">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
         <v>196</v>
       </c>
@@ -2823,7 +2831,7 @@
       </c>
       <c r="E59" s="7"/>
     </row>
-    <row r="60" spans="1:5" ht="45">
+    <row r="60" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
         <v>199</v>
       </c>
@@ -2838,7 +2846,7 @@
       </c>
       <c r="E60" s="7"/>
     </row>
-    <row r="61" spans="1:5">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="9" t="s">
         <v>202</v>
       </c>
@@ -2853,7 +2861,7 @@
       </c>
       <c r="E61" s="7"/>
     </row>
-    <row r="62" spans="1:5">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="9" t="s">
         <v>204</v>
       </c>
@@ -2868,7 +2876,7 @@
       </c>
       <c r="E62" s="7"/>
     </row>
-    <row r="63" spans="1:5">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="9" t="s">
         <v>206</v>
       </c>
@@ -2883,7 +2891,7 @@
       </c>
       <c r="E63" s="7"/>
     </row>
-    <row r="64" spans="1:5">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="9" t="s">
         <v>208</v>
       </c>
@@ -2898,7 +2906,7 @@
       </c>
       <c r="E64" s="7"/>
     </row>
-    <row r="65" spans="1:5">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="9" t="s">
         <v>217</v>
       </c>
@@ -2913,7 +2921,7 @@
       </c>
       <c r="E65" s="7"/>
     </row>
-    <row r="66" spans="1:5">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="9" t="s">
         <v>218</v>
       </c>
@@ -2928,7 +2936,7 @@
       </c>
       <c r="E66" s="7"/>
     </row>
-    <row r="67" spans="1:5">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="9" t="s">
         <v>223</v>
       </c>
@@ -2943,7 +2951,7 @@
       </c>
       <c r="E67" s="7"/>
     </row>
-    <row r="68" spans="1:5">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="9" t="s">
         <v>224</v>
       </c>
@@ -2958,7 +2966,7 @@
       </c>
       <c r="E68" s="7"/>
     </row>
-    <row r="69" spans="1:5">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="9" t="s">
         <v>225</v>
       </c>
@@ -2973,7 +2981,7 @@
       </c>
       <c r="E69" s="7"/>
     </row>
-    <row r="70" spans="1:5">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="9" t="s">
         <v>226</v>
       </c>
@@ -2988,7 +2996,7 @@
       </c>
       <c r="E70" s="7"/>
     </row>
-    <row r="71" spans="1:5">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="9" t="s">
         <v>233</v>
       </c>
@@ -3003,7 +3011,7 @@
       </c>
       <c r="E71" s="7"/>
     </row>
-    <row r="72" spans="1:5">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="9" t="s">
         <v>237</v>
       </c>
@@ -3018,7 +3026,7 @@
       </c>
       <c r="E72" s="7"/>
     </row>
-    <row r="73" spans="1:5">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="9" t="s">
         <v>239</v>
       </c>
@@ -3033,7 +3041,7 @@
       </c>
       <c r="E73" s="7"/>
     </row>
-    <row r="74" spans="1:5">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="9" t="s">
         <v>243</v>
       </c>
@@ -3048,7 +3056,7 @@
       </c>
       <c r="E74" s="7"/>
     </row>
-    <row r="75" spans="1:5" ht="30">
+    <row r="75" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" s="9" t="s">
         <v>245</v>
       </c>
@@ -3063,7 +3071,7 @@
       </c>
       <c r="E75" s="7"/>
     </row>
-    <row r="76" spans="1:5">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="9" t="s">
         <v>248</v>
       </c>
@@ -3078,7 +3086,7 @@
       </c>
       <c r="E76" s="7"/>
     </row>
-    <row r="77" spans="1:5">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="9" t="s">
         <v>256</v>
       </c>
@@ -3093,7 +3101,7 @@
       </c>
       <c r="E77" s="7"/>
     </row>
-    <row r="78" spans="1:5">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="9" t="s">
         <v>257</v>
       </c>
@@ -3108,7 +3116,7 @@
       </c>
       <c r="E78" s="7"/>
     </row>
-    <row r="79" spans="1:5">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="9" t="s">
         <v>261</v>
       </c>
@@ -3123,7 +3131,7 @@
       </c>
       <c r="E79" s="7"/>
     </row>
-    <row r="80" spans="1:5">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="9" t="s">
         <v>264</v>
       </c>
@@ -3138,7 +3146,7 @@
       </c>
       <c r="E80" s="7"/>
     </row>
-    <row r="81" spans="1:5">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="9" t="s">
         <v>267</v>
       </c>
@@ -3153,7 +3161,7 @@
       </c>
       <c r="E81" s="7"/>
     </row>
-    <row r="82" spans="1:5" ht="30">
+    <row r="82" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A82" s="9" t="s">
         <v>269</v>
       </c>
@@ -3168,7 +3176,7 @@
       </c>
       <c r="E82" s="7"/>
     </row>
-    <row r="83" spans="1:5">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="9" t="s">
         <v>274</v>
       </c>
@@ -3183,7 +3191,7 @@
       </c>
       <c r="E83" s="7"/>
     </row>
-    <row r="84" spans="1:5" ht="30">
+    <row r="84" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A84" s="9" t="s">
         <v>277</v>
       </c>
@@ -3198,7 +3206,7 @@
       </c>
       <c r="E84" s="7"/>
     </row>
-    <row r="85" spans="1:5">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="9" t="s">
         <v>279</v>
       </c>
@@ -3213,7 +3221,7 @@
       </c>
       <c r="E85" s="7"/>
     </row>
-    <row r="86" spans="1:5">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="9" t="s">
         <v>282</v>
       </c>
@@ -3228,7 +3236,7 @@
       </c>
       <c r="E86" s="7"/>
     </row>
-    <row r="87" spans="1:5">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="9" t="s">
         <v>285</v>
       </c>
@@ -3243,7 +3251,7 @@
       </c>
       <c r="E87" s="7"/>
     </row>
-    <row r="88" spans="1:5">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="9" t="s">
         <v>288</v>
       </c>
@@ -3258,7 +3266,7 @@
       </c>
       <c r="E88" s="7"/>
     </row>
-    <row r="89" spans="1:5">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="9" t="s">
         <v>291</v>
       </c>
@@ -3273,7 +3281,7 @@
       </c>
       <c r="E89" s="7"/>
     </row>
-    <row r="90" spans="1:5">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="9" t="s">
         <v>294</v>
       </c>
@@ -3288,7 +3296,7 @@
       </c>
       <c r="E90" s="7"/>
     </row>
-    <row r="91" spans="1:5">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="9" t="s">
         <v>297</v>
       </c>
@@ -3303,7 +3311,7 @@
       </c>
       <c r="E91" s="7"/>
     </row>
-    <row r="92" spans="1:5">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="9" t="s">
         <v>300</v>
       </c>
@@ -3318,7 +3326,7 @@
       </c>
       <c r="E92" s="7"/>
     </row>
-    <row r="93" spans="1:5">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="9" t="s">
         <v>303</v>
       </c>
@@ -3333,7 +3341,7 @@
       </c>
       <c r="E93" s="7"/>
     </row>
-    <row r="94" spans="1:5">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="9" t="s">
         <v>306</v>
       </c>
@@ -3348,7 +3356,7 @@
       </c>
       <c r="E94" s="7"/>
     </row>
-    <row r="95" spans="1:5">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="9" t="s">
         <v>309</v>
       </c>
@@ -3363,7 +3371,7 @@
       </c>
       <c r="E95" s="7"/>
     </row>
-    <row r="96" spans="1:5">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="9" t="s">
         <v>314</v>
       </c>
@@ -3378,7 +3386,7 @@
       </c>
       <c r="E96" s="7"/>
     </row>
-    <row r="97" spans="1:5">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="9" t="s">
         <v>315</v>
       </c>
@@ -3393,7 +3401,7 @@
       </c>
       <c r="E97" s="7"/>
     </row>
-    <row r="98" spans="1:5">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="9" t="s">
         <v>319</v>
       </c>
@@ -3408,7 +3416,7 @@
       </c>
       <c r="E98" s="7"/>
     </row>
-    <row r="99" spans="1:5">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="9" t="s">
         <v>321</v>
       </c>
@@ -3423,7 +3431,7 @@
       </c>
       <c r="E99" s="7"/>
     </row>
-    <row r="100" spans="1:5">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="9" t="s">
         <v>322</v>
       </c>
@@ -3438,7 +3446,7 @@
       </c>
       <c r="E100" s="7"/>
     </row>
-    <row r="101" spans="1:5" ht="30">
+    <row r="101" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A101" s="9" t="s">
         <v>323</v>
       </c>
@@ -3453,7 +3461,7 @@
       </c>
       <c r="E101" s="7"/>
     </row>
-    <row r="102" spans="1:5">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="9" t="s">
         <v>328</v>
       </c>
@@ -3468,7 +3476,7 @@
       </c>
       <c r="E102" s="7"/>
     </row>
-    <row r="103" spans="1:5">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="9" t="s">
         <v>333</v>
       </c>
@@ -3483,7 +3491,7 @@
       </c>
       <c r="E103" s="7"/>
     </row>
-    <row r="104" spans="1:5">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="9" t="s">
         <v>336</v>
       </c>
@@ -3498,7 +3506,7 @@
       </c>
       <c r="E104" s="7"/>
     </row>
-    <row r="105" spans="1:5">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="9" t="s">
         <v>337</v>
       </c>
@@ -3513,7 +3521,7 @@
       </c>
       <c r="E105" s="7"/>
     </row>
-    <row r="106" spans="1:5">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="9" t="s">
         <v>342</v>
       </c>
@@ -3528,7 +3536,7 @@
       </c>
       <c r="E106" s="7"/>
     </row>
-    <row r="107" spans="1:5">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="9" t="s">
         <v>345</v>
       </c>
@@ -3543,7 +3551,7 @@
       </c>
       <c r="E107" s="7"/>
     </row>
-    <row r="108" spans="1:5">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="9" t="s">
         <v>350</v>
       </c>
@@ -3558,7 +3566,7 @@
       </c>
       <c r="E108" s="7"/>
     </row>
-    <row r="109" spans="1:5" ht="30">
+    <row r="109" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A109" s="9" t="s">
         <v>351</v>
       </c>
@@ -3573,7 +3581,7 @@
       </c>
       <c r="E109" s="7"/>
     </row>
-    <row r="110" spans="1:5">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="9" t="s">
         <v>354</v>
       </c>
@@ -3588,7 +3596,7 @@
       </c>
       <c r="E110" s="7"/>
     </row>
-    <row r="111" spans="1:5">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="9" t="s">
         <v>357</v>
       </c>
@@ -3603,7 +3611,7 @@
       </c>
       <c r="E111" s="7"/>
     </row>
-    <row r="112" spans="1:5">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="9" t="s">
         <v>361</v>
       </c>
@@ -3618,7 +3626,7 @@
       </c>
       <c r="E112" s="7"/>
     </row>
-    <row r="113" spans="1:5">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="9" t="s">
         <v>363</v>
       </c>
@@ -3633,7 +3641,7 @@
       </c>
       <c r="E113" s="7"/>
     </row>
-    <row r="114" spans="1:5" ht="30">
+    <row r="114" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A114" s="9" t="s">
         <v>366</v>
       </c>
@@ -3648,7 +3656,7 @@
       </c>
       <c r="E114" s="7"/>
     </row>
-    <row r="115" spans="1:5">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="9" t="s">
         <v>369</v>
       </c>
@@ -3663,7 +3671,7 @@
       </c>
       <c r="E115" s="7"/>
     </row>
-    <row r="116" spans="1:5">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="9" t="s">
         <v>370</v>
       </c>
@@ -3678,7 +3686,7 @@
       </c>
       <c r="E116" s="7"/>
     </row>
-    <row r="117" spans="1:5">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" s="9" t="s">
         <v>371</v>
       </c>
@@ -3693,7 +3701,7 @@
       </c>
       <c r="E117" s="7"/>
     </row>
-    <row r="118" spans="1:5">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" s="9" t="s">
         <v>378</v>
       </c>
@@ -3708,7 +3716,7 @@
       </c>
       <c r="E118" s="7"/>
     </row>
-    <row r="119" spans="1:5">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" s="9" t="s">
         <v>381</v>
       </c>
@@ -3723,7 +3731,7 @@
       </c>
       <c r="E119" s="7"/>
     </row>
-    <row r="120" spans="1:5">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" s="9" t="s">
         <v>384</v>
       </c>
@@ -3738,7 +3746,7 @@
       </c>
       <c r="E120" s="7"/>
     </row>
-    <row r="121" spans="1:5">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="9" t="s">
         <v>387</v>
       </c>
@@ -3753,7 +3761,7 @@
       </c>
       <c r="E121" s="7"/>
     </row>
-    <row r="122" spans="1:5">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" s="7" t="s">
         <v>390</v>
       </c>
@@ -3768,7 +3776,7 @@
       </c>
       <c r="E122" s="7"/>
     </row>
-    <row r="123" spans="1:5">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" s="7" t="s">
         <v>393</v>
       </c>
@@ -3783,7 +3791,7 @@
       </c>
       <c r="E123" s="7"/>
     </row>
-    <row r="124" spans="1:5">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" s="7" t="s">
         <v>396</v>
       </c>
@@ -3798,7 +3806,7 @@
       </c>
       <c r="E124" s="7"/>
     </row>
-    <row r="125" spans="1:5">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" s="9" t="s">
         <v>399</v>
       </c>
@@ -3813,7 +3821,7 @@
       </c>
       <c r="E125" s="7"/>
     </row>
-    <row r="126" spans="1:5">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" s="7" t="s">
         <v>402</v>
       </c>
@@ -3828,7 +3836,7 @@
       </c>
       <c r="E126" s="7"/>
     </row>
-    <row r="127" spans="1:5">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" s="7" t="s">
         <v>405</v>
       </c>
@@ -3843,7 +3851,7 @@
       </c>
       <c r="E127" s="7"/>
     </row>
-    <row r="128" spans="1:5">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" s="7" t="s">
         <v>408</v>
       </c>
@@ -3858,7 +3866,7 @@
       </c>
       <c r="E128" s="7"/>
     </row>
-    <row r="129" spans="1:5">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" s="9" t="s">
         <v>411</v>
       </c>
@@ -3873,7 +3881,7 @@
       </c>
       <c r="E129" s="7"/>
     </row>
-    <row r="130" spans="1:5">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" s="9" t="s">
         <v>414</v>
       </c>
@@ -3888,7 +3896,7 @@
       </c>
       <c r="E130" s="7"/>
     </row>
-    <row r="131" spans="1:5">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" s="9" t="s">
         <v>416</v>
       </c>
@@ -3903,7 +3911,7 @@
       </c>
       <c r="E131" s="7"/>
     </row>
-    <row r="132" spans="1:5">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" s="7" t="s">
         <v>419</v>
       </c>
@@ -3918,7 +3926,7 @@
       </c>
       <c r="E132" s="7"/>
     </row>
-    <row r="133" spans="1:5">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" s="9" t="s">
         <v>422</v>
       </c>
@@ -3933,7 +3941,7 @@
       </c>
       <c r="E133" s="7"/>
     </row>
-    <row r="134" spans="1:5" ht="30">
+    <row r="134" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A134" s="7" t="s">
         <v>425</v>
       </c>
@@ -3948,7 +3956,7 @@
       </c>
       <c r="E134" s="7"/>
     </row>
-    <row r="135" spans="1:5" ht="30">
+    <row r="135" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A135" s="7" t="s">
         <v>426</v>
       </c>
@@ -3963,7 +3971,7 @@
       </c>
       <c r="E135" s="7"/>
     </row>
-    <row r="136" spans="1:5">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" s="9" t="s">
         <v>431</v>
       </c>
@@ -3978,7 +3986,7 @@
       </c>
       <c r="E136" s="7"/>
     </row>
-    <row r="137" spans="1:5">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" s="7" t="s">
         <v>434</v>
       </c>
@@ -3993,7 +4001,7 @@
       </c>
       <c r="E137" s="7"/>
     </row>
-    <row r="138" spans="1:5" ht="45">
+    <row r="138" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A138" s="7" t="s">
         <v>435</v>
       </c>
@@ -4008,7 +4016,7 @@
       </c>
       <c r="E138" s="7"/>
     </row>
-    <row r="139" spans="1:5" ht="30">
+    <row r="139" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A139" s="7" t="s">
         <v>436</v>
       </c>
@@ -4023,7 +4031,7 @@
       </c>
       <c r="E139" s="7"/>
     </row>
-    <row r="140" spans="1:5">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" s="17" t="s">
         <v>443</v>
       </c>
@@ -4038,7 +4046,7 @@
       </c>
       <c r="E140" s="7"/>
     </row>
-    <row r="141" spans="1:5">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" s="17" t="s">
         <v>446</v>
       </c>
@@ -4053,7 +4061,7 @@
       </c>
       <c r="E141" s="7"/>
     </row>
-    <row r="142" spans="1:5">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" s="17" t="s">
         <v>449</v>
       </c>
@@ -4068,7 +4076,7 @@
       </c>
       <c r="E142" s="7"/>
     </row>
-    <row r="143" spans="1:5">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" s="17" t="s">
         <v>452</v>
       </c>
@@ -4083,7 +4091,7 @@
       </c>
       <c r="E143" s="7"/>
     </row>
-    <row r="144" spans="1:5">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" s="17" t="s">
         <v>453</v>
       </c>
@@ -4098,7 +4106,7 @@
       </c>
       <c r="E144" s="7"/>
     </row>
-    <row r="145" spans="1:5">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" s="17" t="s">
         <v>458</v>
       </c>
@@ -4113,7 +4121,7 @@
       </c>
       <c r="E145" s="7"/>
     </row>
-    <row r="146" spans="1:5">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" s="17" t="s">
         <v>461</v>
       </c>
@@ -4128,7 +4136,7 @@
       </c>
       <c r="E146" s="7"/>
     </row>
-    <row r="147" spans="1:5">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" s="17" t="s">
         <v>464</v>
       </c>
@@ -4143,7 +4151,7 @@
       </c>
       <c r="E147" s="7"/>
     </row>
-    <row r="148" spans="1:5">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" s="17" t="s">
         <v>467</v>
       </c>
@@ -4158,7 +4166,7 @@
       </c>
       <c r="E148" s="7"/>
     </row>
-    <row r="149" spans="1:5">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" s="7" t="s">
         <v>470</v>
       </c>
@@ -4173,7 +4181,7 @@
       </c>
       <c r="E149" s="7"/>
     </row>
-    <row r="150" spans="1:5">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" s="7" t="s">
         <v>471</v>
       </c>
@@ -4188,7 +4196,7 @@
       </c>
       <c r="E150" s="7"/>
     </row>
-    <row r="151" spans="1:5">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" s="7" t="s">
         <v>472</v>
       </c>
@@ -4203,7 +4211,7 @@
       </c>
       <c r="E151" s="7"/>
     </row>
-    <row r="152" spans="1:5" ht="30">
+    <row r="152" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A152" s="7" t="s">
         <v>479</v>
       </c>
@@ -4217,6 +4225,21 @@
         <v>5</v>
       </c>
       <c r="E152" s="7"/>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A153" s="17" t="s">
+        <v>482</v>
+      </c>
+      <c r="B153" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="C153" s="8" t="s">
+        <v>483</v>
+      </c>
+      <c r="D153" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E153" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -4229,14 +4252,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView topLeftCell="A10" zoomScale="80" workbookViewId="0">
       <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
@@ -4244,7 +4267,7 @@
     <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>35</v>
       </c>
@@ -4258,7 +4281,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>37</v>
       </c>
@@ -4270,7 +4293,7 @@
       </c>
       <c r="D2" s="7"/>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>38</v>
       </c>
@@ -4282,7 +4305,7 @@
       </c>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>39</v>
       </c>
@@ -4294,7 +4317,7 @@
       </c>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>40</v>
       </c>
@@ -4306,7 +4329,7 @@
       </c>
       <c r="D5" s="7"/>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>41</v>
       </c>
@@ -4318,7 +4341,7 @@
       </c>
       <c r="D6" s="7"/>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>42</v>
       </c>
@@ -4330,7 +4353,7 @@
       </c>
       <c r="D7" s="7"/>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>43</v>
       </c>
@@ -4342,7 +4365,7 @@
       </c>
       <c r="D8" s="7"/>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>44</v>
       </c>
@@ -4354,7 +4377,7 @@
       </c>
       <c r="D9" s="7"/>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>45</v>
       </c>
@@ -4366,7 +4389,7 @@
       </c>
       <c r="D10" s="7"/>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>46</v>
       </c>
@@ -4378,7 +4401,7 @@
       </c>
       <c r="D11" s="7"/>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>48</v>
       </c>
@@ -4390,7 +4413,7 @@
       </c>
       <c r="D12" s="7"/>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>49</v>
       </c>
@@ -4402,7 +4425,7 @@
       </c>
       <c r="D13" s="7"/>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>50</v>
       </c>
@@ -4414,7 +4437,7 @@
       </c>
       <c r="D14" s="7"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>51</v>
       </c>
@@ -4426,7 +4449,7 @@
       </c>
       <c r="D15" s="7"/>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>52</v>
       </c>
@@ -4438,7 +4461,7 @@
       </c>
       <c r="D16" s="7"/>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>53</v>
       </c>
@@ -4450,7 +4473,7 @@
       </c>
       <c r="D17" s="7"/>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>54</v>
       </c>
@@ -4462,7 +4485,7 @@
       </c>
       <c r="D18" s="7"/>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>55</v>
       </c>
@@ -4474,7 +4497,7 @@
       </c>
       <c r="D19" s="7"/>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>56</v>
       </c>
@@ -4486,7 +4509,7 @@
       </c>
       <c r="D20" s="7"/>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>57</v>
       </c>
@@ -4498,7 +4521,7 @@
       </c>
       <c r="D21" s="7"/>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>58</v>
       </c>
@@ -4510,7 +4533,7 @@
       </c>
       <c r="D22" s="7"/>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>59</v>
       </c>
@@ -4522,7 +4545,7 @@
       </c>
       <c r="D23" s="7"/>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>60</v>
       </c>
@@ -4534,7 +4557,7 @@
       </c>
       <c r="D24" s="7"/>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>61</v>
       </c>
@@ -4546,7 +4569,7 @@
       </c>
       <c r="D25" s="7"/>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>47</v>
       </c>
@@ -4565,14 +4588,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A19" sqref="A19:XFD19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
@@ -4580,7 +4603,7 @@
     <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>35</v>
       </c>
@@ -4594,7 +4617,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>37</v>
       </c>
@@ -4606,7 +4629,7 @@
       </c>
       <c r="D2" s="7"/>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>38</v>
       </c>
@@ -4618,7 +4641,7 @@
       </c>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>39</v>
       </c>
@@ -4630,7 +4653,7 @@
       </c>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>40</v>
       </c>
@@ -4642,7 +4665,7 @@
       </c>
       <c r="D5" s="7"/>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>41</v>
       </c>
@@ -4654,7 +4677,7 @@
       </c>
       <c r="D6" s="7"/>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>42</v>
       </c>
@@ -4666,7 +4689,7 @@
       </c>
       <c r="D7" s="7"/>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>43</v>
       </c>
@@ -4678,7 +4701,7 @@
       </c>
       <c r="D8" s="7"/>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>44</v>
       </c>
@@ -4690,7 +4713,7 @@
       </c>
       <c r="D9" s="7"/>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>45</v>
       </c>
@@ -4702,7 +4725,7 @@
       </c>
       <c r="D10" s="7"/>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>46</v>
       </c>
@@ -4714,7 +4737,7 @@
       </c>
       <c r="D11" s="7"/>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>47</v>
       </c>
@@ -4726,7 +4749,7 @@
       </c>
       <c r="D12" s="7"/>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>48</v>
       </c>
@@ -4738,7 +4761,7 @@
       </c>
       <c r="D13" s="7"/>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>49</v>
       </c>
@@ -4750,7 +4773,7 @@
       </c>
       <c r="D14" s="7"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>50</v>
       </c>
@@ -4762,7 +4785,7 @@
       </c>
       <c r="D15" s="7"/>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>51</v>
       </c>
@@ -4774,7 +4797,7 @@
       </c>
       <c r="D16" s="7"/>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>52</v>
       </c>
@@ -4786,7 +4809,7 @@
       </c>
       <c r="D17" s="7"/>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>53</v>
       </c>
@@ -4798,7 +4821,7 @@
       </c>
       <c r="D18" s="7"/>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>54</v>
       </c>
@@ -4810,7 +4833,7 @@
       </c>
       <c r="D19" s="7"/>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>55</v>
       </c>
@@ -4822,7 +4845,7 @@
       </c>
       <c r="D20" s="7"/>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>56</v>
       </c>
@@ -4834,7 +4857,7 @@
       </c>
       <c r="D21" s="7"/>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>57</v>
       </c>
@@ -4846,7 +4869,7 @@
       </c>
       <c r="D22" s="7"/>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>58</v>
       </c>
@@ -4858,7 +4881,7 @@
       </c>
       <c r="D23" s="7"/>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>59</v>
       </c>
@@ -4870,7 +4893,7 @@
       </c>
       <c r="D24" s="7"/>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>60</v>
       </c>
@@ -4882,7 +4905,7 @@
       </c>
       <c r="D25" s="7"/>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>61</v>
       </c>

</xml_diff>

<commit_message>
Adds WAT-134 test script and related changes
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/WAT.xlsx
+++ b/src/test/resources/xls/WAT.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="771" uniqueCount="484">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="775" uniqueCount="487">
   <si>
     <t>TCID</t>
   </si>
@@ -1470,6 +1470,15 @@
   </si>
   <si>
     <t>Verify that system must display a "Suggest updates" button, which when clicked will enter into curation mode.</t>
+  </si>
+  <si>
+    <t>Verify that when User clicks the Suggest updates button -System must display the “Submit updates” button (gray version)</t>
+  </si>
+  <si>
+    <t>WAT134</t>
+  </si>
+  <si>
+    <t>WAT-874</t>
   </si>
 </sst>
 </file>
@@ -1929,10 +1938,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E153"/>
+  <dimension ref="A1:E154"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A133" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C153" sqref="C153"/>
+      <selection activeCell="B154" sqref="B154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4240,6 +4249,21 @@
         <v>5</v>
       </c>
       <c r="E153" s="7"/>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A154" s="17" t="s">
+        <v>485</v>
+      </c>
+      <c r="B154" s="7" t="s">
+        <v>486</v>
+      </c>
+      <c r="C154" s="8" t="s">
+        <v>484</v>
+      </c>
+      <c r="D154" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E154" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
WAT 171 and 172 scripts implementation
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/WAT.xlsx
+++ b/src/test/resources/xls/WAT.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="779" uniqueCount="490">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="787" uniqueCount="496">
   <si>
     <t>TCID</t>
   </si>
@@ -1488,6 +1488,24 @@
   </si>
   <si>
     <t>Verify that the system should only recommend papers to an author record where a last name on the paper matches a last name on the author record.</t>
+  </si>
+  <si>
+    <t>WAT171</t>
+  </si>
+  <si>
+    <t>WAT-1377</t>
+  </si>
+  <si>
+    <t>Verify that No other name components than last name should be considered, i.e., not first name or initials.</t>
+  </si>
+  <si>
+    <t>WAT172</t>
+  </si>
+  <si>
+    <t>WAT-1376</t>
+  </si>
+  <si>
+    <t>Verify that A paper should only be recommended if at least one of its last names exactly matches one of the last name variants on the author record.</t>
   </si>
 </sst>
 </file>
@@ -1945,10 +1963,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E155"/>
+  <dimension ref="A1:E157"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A133" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A155" sqref="A155:E155"/>
+      <selection activeCell="E157" sqref="E157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4286,6 +4304,36 @@
         <v>5</v>
       </c>
       <c r="E155" s="7"/>
+    </row>
+    <row r="156" spans="1:5">
+      <c r="A156" s="7" t="s">
+        <v>490</v>
+      </c>
+      <c r="B156" s="7" t="s">
+        <v>491</v>
+      </c>
+      <c r="C156" s="8" t="s">
+        <v>492</v>
+      </c>
+      <c r="D156" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E156" s="7"/>
+    </row>
+    <row r="157" spans="1:5">
+      <c r="A157" s="7" t="s">
+        <v>493</v>
+      </c>
+      <c r="B157" s="7" t="s">
+        <v>494</v>
+      </c>
+      <c r="C157" s="8" t="s">
+        <v>495</v>
+      </c>
+      <c r="D157" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E157" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Adds WAT-135 & WAT-136 test script and related changes
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/WAT.xlsx
+++ b/src/test/resources/xls/WAT.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13305" windowHeight="2415"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="787" uniqueCount="496">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="795" uniqueCount="502">
   <si>
     <t>TCID</t>
   </si>
@@ -1506,13 +1506,31 @@
   </si>
   <si>
     <t>Verify that A paper should only be recommended if at least one of its last names exactly matches one of the last name variants on the author record.</t>
+  </si>
+  <si>
+    <t>WAT135</t>
+  </si>
+  <si>
+    <t>WAT136</t>
+  </si>
+  <si>
+    <t>Verify that CURATION MODE IS TRIGGERED when the user provides feedback on a recommended publication(Accept Publication), "Review updates" and "Submit updates [blue]" are displayed.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CLONE - Verify that CURATION MODE IS TRIGGERED when the user provides feedback on a recommended publication(Reject Publication), "Review updates" and "Submit updates [blue]" are displayed. </t>
+  </si>
+  <si>
+    <t>WAT-893</t>
+  </si>
+  <si>
+    <t>WAT-1403</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1721,7 +1739,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1753,9 +1771,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1787,6 +1806,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1962,14 +1982,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E157"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E159"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A133" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E157" sqref="E157"/>
+    <sheetView tabSelected="1" topLeftCell="A136" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C162" sqref="C162"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="30.5703125" customWidth="1" collapsed="1"/>
@@ -1978,7 +1998,7 @@
     <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1995,7 +2015,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -2010,7 +2030,7 @@
       </c>
       <c r="E2" s="4"/>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -2025,7 +2045,7 @@
       </c>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>11</v>
       </c>
@@ -2040,7 +2060,7 @@
       </c>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>12</v>
       </c>
@@ -2055,7 +2075,7 @@
       </c>
       <c r="E5" s="7"/>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>14</v>
       </c>
@@ -2070,7 +2090,7 @@
       </c>
       <c r="E6" s="7"/>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>17</v>
       </c>
@@ -2085,7 +2105,7 @@
       </c>
       <c r="E7" s="7"/>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>20</v>
       </c>
@@ -2100,7 +2120,7 @@
       </c>
       <c r="E8" s="7"/>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>22</v>
       </c>
@@ -2115,7 +2135,7 @@
       </c>
       <c r="E9" s="7"/>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>23</v>
       </c>
@@ -2130,7 +2150,7 @@
       </c>
       <c r="E10" s="7"/>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>24</v>
       </c>
@@ -2145,7 +2165,7 @@
       </c>
       <c r="E11" s="7"/>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>25</v>
       </c>
@@ -2160,7 +2180,7 @@
       </c>
       <c r="E12" s="7"/>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>62</v>
       </c>
@@ -2175,7 +2195,7 @@
       </c>
       <c r="E13" s="7"/>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>63</v>
       </c>
@@ -2190,7 +2210,7 @@
       </c>
       <c r="E14" s="7"/>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>64</v>
       </c>
@@ -2205,7 +2225,7 @@
       </c>
       <c r="E15" s="7"/>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>65</v>
       </c>
@@ -2220,7 +2240,7 @@
       </c>
       <c r="E16" s="7"/>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>74</v>
       </c>
@@ -2235,7 +2255,7 @@
       </c>
       <c r="E17" s="7"/>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>75</v>
       </c>
@@ -2250,7 +2270,7 @@
       </c>
       <c r="E18" s="7"/>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>79</v>
       </c>
@@ -2265,7 +2285,7 @@
       </c>
       <c r="E19" s="7"/>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>81</v>
       </c>
@@ -2280,7 +2300,7 @@
       </c>
       <c r="E20" s="7"/>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>82</v>
       </c>
@@ -2295,7 +2315,7 @@
       </c>
       <c r="E21" s="7"/>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>88</v>
       </c>
@@ -2310,7 +2330,7 @@
       </c>
       <c r="E22" s="7"/>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>90</v>
       </c>
@@ -2325,7 +2345,7 @@
       </c>
       <c r="E23" s="7"/>
     </row>
-    <row r="24" spans="1:5" ht="30">
+    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>94</v>
       </c>
@@ -2340,7 +2360,7 @@
       </c>
       <c r="E24" s="7"/>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>96</v>
       </c>
@@ -2355,7 +2375,7 @@
       </c>
       <c r="E25" s="7"/>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
         <v>98</v>
       </c>
@@ -2370,7 +2390,7 @@
       </c>
       <c r="E26" s="7"/>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
         <v>102</v>
       </c>
@@ -2385,7 +2405,7 @@
       </c>
       <c r="E27" s="7"/>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
         <v>105</v>
       </c>
@@ -2400,7 +2420,7 @@
       </c>
       <c r="E28" s="7"/>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
         <v>108</v>
       </c>
@@ -2415,7 +2435,7 @@
       </c>
       <c r="E29" s="7"/>
     </row>
-    <row r="30" spans="1:5" ht="30">
+    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
         <v>110</v>
       </c>
@@ -2430,7 +2450,7 @@
       </c>
       <c r="E30" s="7"/>
     </row>
-    <row r="31" spans="1:5" ht="30">
+    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
         <v>114</v>
       </c>
@@ -2445,7 +2465,7 @@
       </c>
       <c r="E31" s="7"/>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
         <v>119</v>
       </c>
@@ -2460,7 +2480,7 @@
       </c>
       <c r="E32" s="7"/>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
         <v>120</v>
       </c>
@@ -2475,7 +2495,7 @@
       </c>
       <c r="E33" s="7"/>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
         <v>125</v>
       </c>
@@ -2490,7 +2510,7 @@
       </c>
       <c r="E34" s="7"/>
     </row>
-    <row r="35" spans="1:5" ht="30">
+    <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
         <v>128</v>
       </c>
@@ -2505,7 +2525,7 @@
       </c>
       <c r="E35" s="7"/>
     </row>
-    <row r="36" spans="1:5" ht="30">
+    <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
         <v>131</v>
       </c>
@@ -2520,7 +2540,7 @@
       </c>
       <c r="E36" s="7"/>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
         <v>134</v>
       </c>
@@ -2535,7 +2555,7 @@
       </c>
       <c r="E37" s="7"/>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="9" t="s">
         <v>137</v>
       </c>
@@ -2550,7 +2570,7 @@
       </c>
       <c r="E38" s="7"/>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="s">
         <v>140</v>
       </c>
@@ -2565,7 +2585,7 @@
       </c>
       <c r="E39" s="7"/>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="9" t="s">
         <v>143</v>
       </c>
@@ -2580,7 +2600,7 @@
       </c>
       <c r="E40" s="7"/>
     </row>
-    <row r="41" spans="1:5" ht="30">
+    <row r="41" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
         <v>145</v>
       </c>
@@ -2595,7 +2615,7 @@
       </c>
       <c r="E41" s="7"/>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="9" t="s">
         <v>147</v>
       </c>
@@ -2610,7 +2630,7 @@
       </c>
       <c r="E42" s="7"/>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="9" t="s">
         <v>150</v>
       </c>
@@ -2625,7 +2645,7 @@
       </c>
       <c r="E43" s="7"/>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="9" t="s">
         <v>153</v>
       </c>
@@ -2640,7 +2660,7 @@
       </c>
       <c r="E44" s="7"/>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="9" t="s">
         <v>155</v>
       </c>
@@ -2655,7 +2675,7 @@
       </c>
       <c r="E45" s="7"/>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="12" t="s">
         <v>158</v>
       </c>
@@ -2670,7 +2690,7 @@
       </c>
       <c r="E46" s="7"/>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="12" t="s">
         <v>159</v>
       </c>
@@ -2685,7 +2705,7 @@
       </c>
       <c r="E47" s="7"/>
     </row>
-    <row r="48" spans="1:5" ht="30">
+    <row r="48" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="12" t="s">
         <v>160</v>
       </c>
@@ -2700,7 +2720,7 @@
       </c>
       <c r="E48" s="7"/>
     </row>
-    <row r="49" spans="1:5" ht="30">
+    <row r="49" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="12" t="s">
         <v>161</v>
       </c>
@@ -2715,7 +2735,7 @@
       </c>
       <c r="E49" s="7"/>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="12" t="s">
         <v>164</v>
       </c>
@@ -2730,7 +2750,7 @@
       </c>
       <c r="E50" s="7"/>
     </row>
-    <row r="51" spans="1:5" ht="30">
+    <row r="51" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="9" t="s">
         <v>173</v>
       </c>
@@ -2745,7 +2765,7 @@
       </c>
       <c r="E51" s="7"/>
     </row>
-    <row r="52" spans="1:5">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="9" t="s">
         <v>174</v>
       </c>
@@ -2760,7 +2780,7 @@
       </c>
       <c r="E52" s="7"/>
     </row>
-    <row r="53" spans="1:5">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="9" t="s">
         <v>179</v>
       </c>
@@ -2775,7 +2795,7 @@
       </c>
       <c r="E53" s="7"/>
     </row>
-    <row r="54" spans="1:5">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="9" t="s">
         <v>180</v>
       </c>
@@ -2790,7 +2810,7 @@
       </c>
       <c r="E54" s="7"/>
     </row>
-    <row r="55" spans="1:5">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="9" t="s">
         <v>185</v>
       </c>
@@ -2805,7 +2825,7 @@
       </c>
       <c r="E55" s="7"/>
     </row>
-    <row r="56" spans="1:5">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="s">
         <v>188</v>
       </c>
@@ -2820,7 +2840,7 @@
       </c>
       <c r="E56" s="7"/>
     </row>
-    <row r="57" spans="1:5" ht="30">
+    <row r="57" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="9" t="s">
         <v>191</v>
       </c>
@@ -2835,7 +2855,7 @@
       </c>
       <c r="E57" s="7"/>
     </row>
-    <row r="58" spans="1:5">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="9" t="s">
         <v>194</v>
       </c>
@@ -2850,7 +2870,7 @@
       </c>
       <c r="E58" s="7"/>
     </row>
-    <row r="59" spans="1:5">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
         <v>196</v>
       </c>
@@ -2865,7 +2885,7 @@
       </c>
       <c r="E59" s="7"/>
     </row>
-    <row r="60" spans="1:5" ht="45">
+    <row r="60" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
         <v>199</v>
       </c>
@@ -2880,7 +2900,7 @@
       </c>
       <c r="E60" s="7"/>
     </row>
-    <row r="61" spans="1:5">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="9" t="s">
         <v>202</v>
       </c>
@@ -2895,7 +2915,7 @@
       </c>
       <c r="E61" s="7"/>
     </row>
-    <row r="62" spans="1:5">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="9" t="s">
         <v>204</v>
       </c>
@@ -2910,7 +2930,7 @@
       </c>
       <c r="E62" s="7"/>
     </row>
-    <row r="63" spans="1:5">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="9" t="s">
         <v>206</v>
       </c>
@@ -2925,7 +2945,7 @@
       </c>
       <c r="E63" s="7"/>
     </row>
-    <row r="64" spans="1:5">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="9" t="s">
         <v>208</v>
       </c>
@@ -2940,7 +2960,7 @@
       </c>
       <c r="E64" s="7"/>
     </row>
-    <row r="65" spans="1:5">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="9" t="s">
         <v>217</v>
       </c>
@@ -2955,7 +2975,7 @@
       </c>
       <c r="E65" s="7"/>
     </row>
-    <row r="66" spans="1:5">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="9" t="s">
         <v>218</v>
       </c>
@@ -2970,7 +2990,7 @@
       </c>
       <c r="E66" s="7"/>
     </row>
-    <row r="67" spans="1:5">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="9" t="s">
         <v>223</v>
       </c>
@@ -2985,7 +3005,7 @@
       </c>
       <c r="E67" s="7"/>
     </row>
-    <row r="68" spans="1:5">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="9" t="s">
         <v>224</v>
       </c>
@@ -3000,7 +3020,7 @@
       </c>
       <c r="E68" s="7"/>
     </row>
-    <row r="69" spans="1:5">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="9" t="s">
         <v>225</v>
       </c>
@@ -3015,7 +3035,7 @@
       </c>
       <c r="E69" s="7"/>
     </row>
-    <row r="70" spans="1:5">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="9" t="s">
         <v>226</v>
       </c>
@@ -3030,7 +3050,7 @@
       </c>
       <c r="E70" s="7"/>
     </row>
-    <row r="71" spans="1:5">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="9" t="s">
         <v>233</v>
       </c>
@@ -3045,7 +3065,7 @@
       </c>
       <c r="E71" s="7"/>
     </row>
-    <row r="72" spans="1:5">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="9" t="s">
         <v>237</v>
       </c>
@@ -3060,7 +3080,7 @@
       </c>
       <c r="E72" s="7"/>
     </row>
-    <row r="73" spans="1:5">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="9" t="s">
         <v>239</v>
       </c>
@@ -3075,7 +3095,7 @@
       </c>
       <c r="E73" s="7"/>
     </row>
-    <row r="74" spans="1:5">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="9" t="s">
         <v>243</v>
       </c>
@@ -3090,7 +3110,7 @@
       </c>
       <c r="E74" s="7"/>
     </row>
-    <row r="75" spans="1:5" ht="30">
+    <row r="75" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" s="9" t="s">
         <v>245</v>
       </c>
@@ -3105,7 +3125,7 @@
       </c>
       <c r="E75" s="7"/>
     </row>
-    <row r="76" spans="1:5">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="9" t="s">
         <v>248</v>
       </c>
@@ -3120,7 +3140,7 @@
       </c>
       <c r="E76" s="7"/>
     </row>
-    <row r="77" spans="1:5">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="9" t="s">
         <v>256</v>
       </c>
@@ -3135,7 +3155,7 @@
       </c>
       <c r="E77" s="7"/>
     </row>
-    <row r="78" spans="1:5">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="9" t="s">
         <v>257</v>
       </c>
@@ -3150,7 +3170,7 @@
       </c>
       <c r="E78" s="7"/>
     </row>
-    <row r="79" spans="1:5">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="9" t="s">
         <v>261</v>
       </c>
@@ -3165,7 +3185,7 @@
       </c>
       <c r="E79" s="7"/>
     </row>
-    <row r="80" spans="1:5">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="9" t="s">
         <v>264</v>
       </c>
@@ -3180,7 +3200,7 @@
       </c>
       <c r="E80" s="7"/>
     </row>
-    <row r="81" spans="1:5">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="9" t="s">
         <v>267</v>
       </c>
@@ -3195,7 +3215,7 @@
       </c>
       <c r="E81" s="7"/>
     </row>
-    <row r="82" spans="1:5" ht="30">
+    <row r="82" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A82" s="9" t="s">
         <v>269</v>
       </c>
@@ -3210,7 +3230,7 @@
       </c>
       <c r="E82" s="7"/>
     </row>
-    <row r="83" spans="1:5">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="9" t="s">
         <v>274</v>
       </c>
@@ -3225,7 +3245,7 @@
       </c>
       <c r="E83" s="7"/>
     </row>
-    <row r="84" spans="1:5" ht="30">
+    <row r="84" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A84" s="9" t="s">
         <v>277</v>
       </c>
@@ -3240,7 +3260,7 @@
       </c>
       <c r="E84" s="7"/>
     </row>
-    <row r="85" spans="1:5">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="9" t="s">
         <v>279</v>
       </c>
@@ -3255,7 +3275,7 @@
       </c>
       <c r="E85" s="7"/>
     </row>
-    <row r="86" spans="1:5">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="9" t="s">
         <v>282</v>
       </c>
@@ -3270,7 +3290,7 @@
       </c>
       <c r="E86" s="7"/>
     </row>
-    <row r="87" spans="1:5">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="9" t="s">
         <v>285</v>
       </c>
@@ -3285,7 +3305,7 @@
       </c>
       <c r="E87" s="7"/>
     </row>
-    <row r="88" spans="1:5">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="9" t="s">
         <v>288</v>
       </c>
@@ -3300,7 +3320,7 @@
       </c>
       <c r="E88" s="7"/>
     </row>
-    <row r="89" spans="1:5">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="9" t="s">
         <v>291</v>
       </c>
@@ -3315,7 +3335,7 @@
       </c>
       <c r="E89" s="7"/>
     </row>
-    <row r="90" spans="1:5">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="9" t="s">
         <v>294</v>
       </c>
@@ -3330,7 +3350,7 @@
       </c>
       <c r="E90" s="7"/>
     </row>
-    <row r="91" spans="1:5">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="9" t="s">
         <v>297</v>
       </c>
@@ -3345,7 +3365,7 @@
       </c>
       <c r="E91" s="7"/>
     </row>
-    <row r="92" spans="1:5">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="9" t="s">
         <v>300</v>
       </c>
@@ -3360,7 +3380,7 @@
       </c>
       <c r="E92" s="7"/>
     </row>
-    <row r="93" spans="1:5">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="9" t="s">
         <v>303</v>
       </c>
@@ -3375,7 +3395,7 @@
       </c>
       <c r="E93" s="7"/>
     </row>
-    <row r="94" spans="1:5">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="9" t="s">
         <v>306</v>
       </c>
@@ -3390,7 +3410,7 @@
       </c>
       <c r="E94" s="7"/>
     </row>
-    <row r="95" spans="1:5">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="9" t="s">
         <v>309</v>
       </c>
@@ -3405,7 +3425,7 @@
       </c>
       <c r="E95" s="7"/>
     </row>
-    <row r="96" spans="1:5">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="9" t="s">
         <v>314</v>
       </c>
@@ -3420,7 +3440,7 @@
       </c>
       <c r="E96" s="7"/>
     </row>
-    <row r="97" spans="1:5">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="9" t="s">
         <v>315</v>
       </c>
@@ -3435,7 +3455,7 @@
       </c>
       <c r="E97" s="7"/>
     </row>
-    <row r="98" spans="1:5">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="9" t="s">
         <v>319</v>
       </c>
@@ -3450,7 +3470,7 @@
       </c>
       <c r="E98" s="7"/>
     </row>
-    <row r="99" spans="1:5">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="9" t="s">
         <v>321</v>
       </c>
@@ -3465,7 +3485,7 @@
       </c>
       <c r="E99" s="7"/>
     </row>
-    <row r="100" spans="1:5">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="9" t="s">
         <v>322</v>
       </c>
@@ -3480,7 +3500,7 @@
       </c>
       <c r="E100" s="7"/>
     </row>
-    <row r="101" spans="1:5" ht="30">
+    <row r="101" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A101" s="9" t="s">
         <v>323</v>
       </c>
@@ -3495,7 +3515,7 @@
       </c>
       <c r="E101" s="7"/>
     </row>
-    <row r="102" spans="1:5">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="9" t="s">
         <v>328</v>
       </c>
@@ -3510,7 +3530,7 @@
       </c>
       <c r="E102" s="7"/>
     </row>
-    <row r="103" spans="1:5">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="9" t="s">
         <v>333</v>
       </c>
@@ -3525,7 +3545,7 @@
       </c>
       <c r="E103" s="7"/>
     </row>
-    <row r="104" spans="1:5">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="9" t="s">
         <v>336</v>
       </c>
@@ -3540,7 +3560,7 @@
       </c>
       <c r="E104" s="7"/>
     </row>
-    <row r="105" spans="1:5">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="9" t="s">
         <v>337</v>
       </c>
@@ -3555,7 +3575,7 @@
       </c>
       <c r="E105" s="7"/>
     </row>
-    <row r="106" spans="1:5">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="9" t="s">
         <v>342</v>
       </c>
@@ -3570,7 +3590,7 @@
       </c>
       <c r="E106" s="7"/>
     </row>
-    <row r="107" spans="1:5">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="9" t="s">
         <v>345</v>
       </c>
@@ -3585,7 +3605,7 @@
       </c>
       <c r="E107" s="7"/>
     </row>
-    <row r="108" spans="1:5">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="9" t="s">
         <v>350</v>
       </c>
@@ -3600,7 +3620,7 @@
       </c>
       <c r="E108" s="7"/>
     </row>
-    <row r="109" spans="1:5" ht="30">
+    <row r="109" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A109" s="9" t="s">
         <v>351</v>
       </c>
@@ -3615,7 +3635,7 @@
       </c>
       <c r="E109" s="7"/>
     </row>
-    <row r="110" spans="1:5">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="9" t="s">
         <v>354</v>
       </c>
@@ -3630,7 +3650,7 @@
       </c>
       <c r="E110" s="7"/>
     </row>
-    <row r="111" spans="1:5">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="9" t="s">
         <v>357</v>
       </c>
@@ -3645,7 +3665,7 @@
       </c>
       <c r="E111" s="7"/>
     </row>
-    <row r="112" spans="1:5">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="9" t="s">
         <v>361</v>
       </c>
@@ -3660,7 +3680,7 @@
       </c>
       <c r="E112" s="7"/>
     </row>
-    <row r="113" spans="1:5">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="9" t="s">
         <v>363</v>
       </c>
@@ -3675,7 +3695,7 @@
       </c>
       <c r="E113" s="7"/>
     </row>
-    <row r="114" spans="1:5" ht="30">
+    <row r="114" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A114" s="9" t="s">
         <v>366</v>
       </c>
@@ -3690,7 +3710,7 @@
       </c>
       <c r="E114" s="7"/>
     </row>
-    <row r="115" spans="1:5">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="9" t="s">
         <v>369</v>
       </c>
@@ -3705,7 +3725,7 @@
       </c>
       <c r="E115" s="7"/>
     </row>
-    <row r="116" spans="1:5">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="9" t="s">
         <v>370</v>
       </c>
@@ -3720,7 +3740,7 @@
       </c>
       <c r="E116" s="7"/>
     </row>
-    <row r="117" spans="1:5">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" s="9" t="s">
         <v>371</v>
       </c>
@@ -3735,7 +3755,7 @@
       </c>
       <c r="E117" s="7"/>
     </row>
-    <row r="118" spans="1:5">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" s="9" t="s">
         <v>378</v>
       </c>
@@ -3750,7 +3770,7 @@
       </c>
       <c r="E118" s="7"/>
     </row>
-    <row r="119" spans="1:5">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" s="9" t="s">
         <v>381</v>
       </c>
@@ -3765,7 +3785,7 @@
       </c>
       <c r="E119" s="7"/>
     </row>
-    <row r="120" spans="1:5">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" s="9" t="s">
         <v>384</v>
       </c>
@@ -3780,7 +3800,7 @@
       </c>
       <c r="E120" s="7"/>
     </row>
-    <row r="121" spans="1:5">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="9" t="s">
         <v>387</v>
       </c>
@@ -3795,7 +3815,7 @@
       </c>
       <c r="E121" s="7"/>
     </row>
-    <row r="122" spans="1:5">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" s="7" t="s">
         <v>390</v>
       </c>
@@ -3810,7 +3830,7 @@
       </c>
       <c r="E122" s="7"/>
     </row>
-    <row r="123" spans="1:5">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" s="7" t="s">
         <v>393</v>
       </c>
@@ -3825,7 +3845,7 @@
       </c>
       <c r="E123" s="7"/>
     </row>
-    <row r="124" spans="1:5">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" s="7" t="s">
         <v>396</v>
       </c>
@@ -3840,7 +3860,7 @@
       </c>
       <c r="E124" s="7"/>
     </row>
-    <row r="125" spans="1:5">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" s="9" t="s">
         <v>399</v>
       </c>
@@ -3855,7 +3875,7 @@
       </c>
       <c r="E125" s="7"/>
     </row>
-    <row r="126" spans="1:5">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" s="7" t="s">
         <v>402</v>
       </c>
@@ -3870,7 +3890,7 @@
       </c>
       <c r="E126" s="7"/>
     </row>
-    <row r="127" spans="1:5">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" s="7" t="s">
         <v>405</v>
       </c>
@@ -3885,7 +3905,7 @@
       </c>
       <c r="E127" s="7"/>
     </row>
-    <row r="128" spans="1:5">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" s="7" t="s">
         <v>408</v>
       </c>
@@ -3900,7 +3920,7 @@
       </c>
       <c r="E128" s="7"/>
     </row>
-    <row r="129" spans="1:5">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" s="9" t="s">
         <v>411</v>
       </c>
@@ -3915,7 +3935,7 @@
       </c>
       <c r="E129" s="7"/>
     </row>
-    <row r="130" spans="1:5">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" s="9" t="s">
         <v>414</v>
       </c>
@@ -3930,7 +3950,7 @@
       </c>
       <c r="E130" s="7"/>
     </row>
-    <row r="131" spans="1:5">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" s="9" t="s">
         <v>416</v>
       </c>
@@ -3945,7 +3965,7 @@
       </c>
       <c r="E131" s="7"/>
     </row>
-    <row r="132" spans="1:5">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" s="7" t="s">
         <v>419</v>
       </c>
@@ -3960,7 +3980,7 @@
       </c>
       <c r="E132" s="7"/>
     </row>
-    <row r="133" spans="1:5">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" s="9" t="s">
         <v>422</v>
       </c>
@@ -3975,7 +3995,7 @@
       </c>
       <c r="E133" s="7"/>
     </row>
-    <row r="134" spans="1:5" ht="30">
+    <row r="134" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A134" s="7" t="s">
         <v>425</v>
       </c>
@@ -3990,7 +4010,7 @@
       </c>
       <c r="E134" s="7"/>
     </row>
-    <row r="135" spans="1:5" ht="30">
+    <row r="135" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A135" s="7" t="s">
         <v>426</v>
       </c>
@@ -4005,7 +4025,7 @@
       </c>
       <c r="E135" s="7"/>
     </row>
-    <row r="136" spans="1:5">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" s="9" t="s">
         <v>431</v>
       </c>
@@ -4020,7 +4040,7 @@
       </c>
       <c r="E136" s="7"/>
     </row>
-    <row r="137" spans="1:5">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" s="7" t="s">
         <v>434</v>
       </c>
@@ -4035,7 +4055,7 @@
       </c>
       <c r="E137" s="7"/>
     </row>
-    <row r="138" spans="1:5" ht="45">
+    <row r="138" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A138" s="7" t="s">
         <v>435</v>
       </c>
@@ -4050,7 +4070,7 @@
       </c>
       <c r="E138" s="7"/>
     </row>
-    <row r="139" spans="1:5" ht="30">
+    <row r="139" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A139" s="7" t="s">
         <v>436</v>
       </c>
@@ -4065,7 +4085,7 @@
       </c>
       <c r="E139" s="7"/>
     </row>
-    <row r="140" spans="1:5">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" s="17" t="s">
         <v>443</v>
       </c>
@@ -4080,7 +4100,7 @@
       </c>
       <c r="E140" s="7"/>
     </row>
-    <row r="141" spans="1:5">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" s="17" t="s">
         <v>446</v>
       </c>
@@ -4095,7 +4115,7 @@
       </c>
       <c r="E141" s="7"/>
     </row>
-    <row r="142" spans="1:5">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" s="17" t="s">
         <v>449</v>
       </c>
@@ -4110,7 +4130,7 @@
       </c>
       <c r="E142" s="7"/>
     </row>
-    <row r="143" spans="1:5">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" s="17" t="s">
         <v>452</v>
       </c>
@@ -4125,7 +4145,7 @@
       </c>
       <c r="E143" s="7"/>
     </row>
-    <row r="144" spans="1:5">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" s="17" t="s">
         <v>453</v>
       </c>
@@ -4140,7 +4160,7 @@
       </c>
       <c r="E144" s="7"/>
     </row>
-    <row r="145" spans="1:5">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" s="17" t="s">
         <v>458</v>
       </c>
@@ -4155,7 +4175,7 @@
       </c>
       <c r="E145" s="7"/>
     </row>
-    <row r="146" spans="1:5">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" s="17" t="s">
         <v>461</v>
       </c>
@@ -4170,7 +4190,7 @@
       </c>
       <c r="E146" s="7"/>
     </row>
-    <row r="147" spans="1:5">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" s="17" t="s">
         <v>464</v>
       </c>
@@ -4185,7 +4205,7 @@
       </c>
       <c r="E147" s="7"/>
     </row>
-    <row r="148" spans="1:5">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" s="17" t="s">
         <v>467</v>
       </c>
@@ -4200,7 +4220,7 @@
       </c>
       <c r="E148" s="7"/>
     </row>
-    <row r="149" spans="1:5">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" s="7" t="s">
         <v>470</v>
       </c>
@@ -4215,7 +4235,7 @@
       </c>
       <c r="E149" s="7"/>
     </row>
-    <row r="150" spans="1:5">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" s="7" t="s">
         <v>471</v>
       </c>
@@ -4230,7 +4250,7 @@
       </c>
       <c r="E150" s="7"/>
     </row>
-    <row r="151" spans="1:5">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" s="7" t="s">
         <v>472</v>
       </c>
@@ -4245,7 +4265,7 @@
       </c>
       <c r="E151" s="7"/>
     </row>
-    <row r="152" spans="1:5" ht="30">
+    <row r="152" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A152" s="7" t="s">
         <v>479</v>
       </c>
@@ -4260,7 +4280,7 @@
       </c>
       <c r="E152" s="7"/>
     </row>
-    <row r="153" spans="1:5">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" s="17" t="s">
         <v>482</v>
       </c>
@@ -4275,7 +4295,7 @@
       </c>
       <c r="E153" s="7"/>
     </row>
-    <row r="154" spans="1:5">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" s="17" t="s">
         <v>485</v>
       </c>
@@ -4290,7 +4310,7 @@
       </c>
       <c r="E154" s="7"/>
     </row>
-    <row r="155" spans="1:5">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" s="7" t="s">
         <v>487</v>
       </c>
@@ -4305,7 +4325,7 @@
       </c>
       <c r="E155" s="7"/>
     </row>
-    <row r="156" spans="1:5">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" s="7" t="s">
         <v>490</v>
       </c>
@@ -4320,7 +4340,7 @@
       </c>
       <c r="E156" s="7"/>
     </row>
-    <row r="157" spans="1:5">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" s="7" t="s">
         <v>493</v>
       </c>
@@ -4334,6 +4354,36 @@
         <v>5</v>
       </c>
       <c r="E157" s="7"/>
+    </row>
+    <row r="158" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A158" s="7" t="s">
+        <v>496</v>
+      </c>
+      <c r="B158" s="7" t="s">
+        <v>500</v>
+      </c>
+      <c r="C158" s="8" t="s">
+        <v>498</v>
+      </c>
+      <c r="D158" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E158" s="7"/>
+    </row>
+    <row r="159" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A159" s="7" t="s">
+        <v>497</v>
+      </c>
+      <c r="B159" s="7" t="s">
+        <v>501</v>
+      </c>
+      <c r="C159" s="8" t="s">
+        <v>499</v>
+      </c>
+      <c r="D159" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E159" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -4346,14 +4396,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView topLeftCell="A10" zoomScale="80" workbookViewId="0">
       <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
@@ -4361,7 +4411,7 @@
     <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>35</v>
       </c>
@@ -4375,7 +4425,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>37</v>
       </c>
@@ -4387,7 +4437,7 @@
       </c>
       <c r="D2" s="7"/>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>38</v>
       </c>
@@ -4399,7 +4449,7 @@
       </c>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>39</v>
       </c>
@@ -4411,7 +4461,7 @@
       </c>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>40</v>
       </c>
@@ -4423,7 +4473,7 @@
       </c>
       <c r="D5" s="7"/>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>41</v>
       </c>
@@ -4435,7 +4485,7 @@
       </c>
       <c r="D6" s="7"/>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>42</v>
       </c>
@@ -4447,7 +4497,7 @@
       </c>
       <c r="D7" s="7"/>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>43</v>
       </c>
@@ -4459,7 +4509,7 @@
       </c>
       <c r="D8" s="7"/>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>44</v>
       </c>
@@ -4471,7 +4521,7 @@
       </c>
       <c r="D9" s="7"/>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>45</v>
       </c>
@@ -4483,7 +4533,7 @@
       </c>
       <c r="D10" s="7"/>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>46</v>
       </c>
@@ -4495,7 +4545,7 @@
       </c>
       <c r="D11" s="7"/>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>48</v>
       </c>
@@ -4507,7 +4557,7 @@
       </c>
       <c r="D12" s="7"/>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>49</v>
       </c>
@@ -4519,7 +4569,7 @@
       </c>
       <c r="D13" s="7"/>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>50</v>
       </c>
@@ -4531,7 +4581,7 @@
       </c>
       <c r="D14" s="7"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>51</v>
       </c>
@@ -4543,7 +4593,7 @@
       </c>
       <c r="D15" s="7"/>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>52</v>
       </c>
@@ -4555,7 +4605,7 @@
       </c>
       <c r="D16" s="7"/>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>53</v>
       </c>
@@ -4567,7 +4617,7 @@
       </c>
       <c r="D17" s="7"/>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>54</v>
       </c>
@@ -4579,7 +4629,7 @@
       </c>
       <c r="D18" s="7"/>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>55</v>
       </c>
@@ -4591,7 +4641,7 @@
       </c>
       <c r="D19" s="7"/>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>56</v>
       </c>
@@ -4603,7 +4653,7 @@
       </c>
       <c r="D20" s="7"/>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>57</v>
       </c>
@@ -4615,7 +4665,7 @@
       </c>
       <c r="D21" s="7"/>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>58</v>
       </c>
@@ -4627,7 +4677,7 @@
       </c>
       <c r="D22" s="7"/>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>59</v>
       </c>
@@ -4639,7 +4689,7 @@
       </c>
       <c r="D23" s="7"/>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>60</v>
       </c>
@@ -4651,7 +4701,7 @@
       </c>
       <c r="D24" s="7"/>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>61</v>
       </c>
@@ -4663,7 +4713,7 @@
       </c>
       <c r="D25" s="7"/>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>47</v>
       </c>
@@ -4682,14 +4732,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A19" sqref="A19:XFD19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
@@ -4697,7 +4747,7 @@
     <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>35</v>
       </c>
@@ -4711,7 +4761,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>37</v>
       </c>
@@ -4723,7 +4773,7 @@
       </c>
       <c r="D2" s="7"/>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>38</v>
       </c>
@@ -4735,7 +4785,7 @@
       </c>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>39</v>
       </c>
@@ -4747,7 +4797,7 @@
       </c>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>40</v>
       </c>
@@ -4759,7 +4809,7 @@
       </c>
       <c r="D5" s="7"/>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>41</v>
       </c>
@@ -4771,7 +4821,7 @@
       </c>
       <c r="D6" s="7"/>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>42</v>
       </c>
@@ -4783,7 +4833,7 @@
       </c>
       <c r="D7" s="7"/>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>43</v>
       </c>
@@ -4795,7 +4845,7 @@
       </c>
       <c r="D8" s="7"/>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>44</v>
       </c>
@@ -4807,7 +4857,7 @@
       </c>
       <c r="D9" s="7"/>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>45</v>
       </c>
@@ -4819,7 +4869,7 @@
       </c>
       <c r="D10" s="7"/>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>46</v>
       </c>
@@ -4831,7 +4881,7 @@
       </c>
       <c r="D11" s="7"/>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>47</v>
       </c>
@@ -4843,7 +4893,7 @@
       </c>
       <c r="D12" s="7"/>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>48</v>
       </c>
@@ -4855,7 +4905,7 @@
       </c>
       <c r="D13" s="7"/>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>49</v>
       </c>
@@ -4867,7 +4917,7 @@
       </c>
       <c r="D14" s="7"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>50</v>
       </c>
@@ -4879,7 +4929,7 @@
       </c>
       <c r="D15" s="7"/>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>51</v>
       </c>
@@ -4891,7 +4941,7 @@
       </c>
       <c r="D16" s="7"/>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>52</v>
       </c>
@@ -4903,7 +4953,7 @@
       </c>
       <c r="D17" s="7"/>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>53</v>
       </c>
@@ -4915,7 +4965,7 @@
       </c>
       <c r="D18" s="7"/>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>54</v>
       </c>
@@ -4927,7 +4977,7 @@
       </c>
       <c r="D19" s="7"/>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>55</v>
       </c>
@@ -4939,7 +4989,7 @@
       </c>
       <c r="D20" s="7"/>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>56</v>
       </c>
@@ -4951,7 +5001,7 @@
       </c>
       <c r="D21" s="7"/>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>57</v>
       </c>
@@ -4963,7 +5013,7 @@
       </c>
       <c r="D22" s="7"/>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>58</v>
       </c>
@@ -4975,7 +5025,7 @@
       </c>
       <c r="D23" s="7"/>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>59</v>
       </c>
@@ -4987,7 +5037,7 @@
       </c>
       <c r="D24" s="7"/>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>60</v>
       </c>
@@ -4999,7 +5049,7 @@
       </c>
       <c r="D25" s="7"/>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>61</v>
       </c>

</xml_diff>

<commit_message>
Adds WAT-894 test case in WAT xls
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/WAT.xlsx
+++ b/src/test/resources/xls/WAT.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="795" uniqueCount="502">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="795" uniqueCount="503">
   <si>
     <t>TCID</t>
   </si>
@@ -1469,9 +1469,6 @@
     <t>WAT133</t>
   </si>
   <si>
-    <t>Verify that system must display a "Suggest updates" button, which when clicked will enter into curation mode.</t>
-  </si>
-  <si>
     <t>Verify that when User clicks the Suggest updates button -System must display the “Submit updates” button (gray version)</t>
   </si>
   <si>
@@ -1524,6 +1521,12 @@
   </si>
   <si>
     <t>WAT-1403</t>
+  </si>
+  <si>
+    <t>WAT-741 || WAT-894</t>
+  </si>
+  <si>
+    <t>Verify that system must display a "Suggest updates" button, which when clicked will enter into curation mode. || Verify that CURATION MODE IS TRIGGERED when the user selects "Suggest updates" the "Submit updates [gray]" button is displayed. The remove panel and delete individual pubs options are also displayed. "Suggest updates" is hidden.</t>
   </si>
 </sst>
 </file>
@@ -1986,7 +1989,7 @@
   <dimension ref="A1:E159"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A136" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C162" sqref="C162"/>
+      <selection activeCell="C153" sqref="C153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4280,15 +4283,15 @@
       </c>
       <c r="E152" s="7"/>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A153" s="17" t="s">
         <v>482</v>
       </c>
       <c r="B153" s="7" t="s">
-        <v>249</v>
+        <v>501</v>
       </c>
       <c r="C153" s="8" t="s">
-        <v>483</v>
+        <v>502</v>
       </c>
       <c r="D153" s="7" t="s">
         <v>5</v>
@@ -4297,13 +4300,13 @@
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" s="17" t="s">
+        <v>484</v>
+      </c>
+      <c r="B154" s="7" t="s">
         <v>485</v>
       </c>
-      <c r="B154" s="7" t="s">
-        <v>486</v>
-      </c>
       <c r="C154" s="8" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="D154" s="7" t="s">
         <v>5</v>
@@ -4312,13 +4315,13 @@
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" s="7" t="s">
+        <v>486</v>
+      </c>
+      <c r="B155" s="7" t="s">
         <v>487</v>
       </c>
-      <c r="B155" s="7" t="s">
+      <c r="C155" s="8" t="s">
         <v>488</v>
-      </c>
-      <c r="C155" s="8" t="s">
-        <v>489</v>
       </c>
       <c r="D155" s="9" t="s">
         <v>5</v>
@@ -4327,13 +4330,13 @@
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" s="7" t="s">
+        <v>489</v>
+      </c>
+      <c r="B156" s="7" t="s">
         <v>490</v>
       </c>
-      <c r="B156" s="7" t="s">
+      <c r="C156" s="8" t="s">
         <v>491</v>
-      </c>
-      <c r="C156" s="8" t="s">
-        <v>492</v>
       </c>
       <c r="D156" s="7" t="s">
         <v>5</v>
@@ -4342,13 +4345,13 @@
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" s="7" t="s">
+        <v>492</v>
+      </c>
+      <c r="B157" s="7" t="s">
         <v>493</v>
       </c>
-      <c r="B157" s="7" t="s">
+      <c r="C157" s="8" t="s">
         <v>494</v>
-      </c>
-      <c r="C157" s="8" t="s">
-        <v>495</v>
       </c>
       <c r="D157" s="9" t="s">
         <v>5</v>
@@ -4357,13 +4360,13 @@
     </row>
     <row r="158" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A158" s="7" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B158" s="7" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="C158" s="8" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="D158" s="9" t="s">
         <v>5</v>
@@ -4372,13 +4375,13 @@
     </row>
     <row r="159" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A159" s="7" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B159" s="7" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="C159" s="8" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D159" s="9" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
Adds WAT-137 and related changes
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/WAT.xlsx
+++ b/src/test/resources/xls/WAT.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="795" uniqueCount="503">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="799" uniqueCount="506">
   <si>
     <t>TCID</t>
   </si>
@@ -1527,6 +1527,15 @@
   </si>
   <si>
     <t>Verify that system must display a "Suggest updates" button, which when clicked will enter into curation mode. || Verify that CURATION MODE IS TRIGGERED when the user selects "Suggest updates" the "Submit updates [gray]" button is displayed. The remove panel and delete individual pubs options are also displayed. "Suggest updates" is hidden.</t>
+  </si>
+  <si>
+    <t>WAT137</t>
+  </si>
+  <si>
+    <t>Verify that If user hits cancel, feedback is not submitted and the system must display the author record in curation mode.</t>
+  </si>
+  <si>
+    <t>WAT-900</t>
   </si>
 </sst>
 </file>
@@ -1986,10 +1995,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E159"/>
+  <dimension ref="A1:E160"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A136" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C153" sqref="C153"/>
+      <selection activeCell="B160" sqref="B160"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4387,6 +4396,21 @@
         <v>5</v>
       </c>
       <c r="E159" s="7"/>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A160" s="7" t="s">
+        <v>503</v>
+      </c>
+      <c r="B160" s="7" t="s">
+        <v>505</v>
+      </c>
+      <c r="C160" s="8" t="s">
+        <v>504</v>
+      </c>
+      <c r="D160" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E160" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Adds WAT-138 testscript and related changes
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/WAT.xlsx
+++ b/src/test/resources/xls/WAT.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="799" uniqueCount="506">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="803" uniqueCount="509">
   <si>
     <t>TCID</t>
   </si>
@@ -1536,6 +1536,15 @@
   </si>
   <si>
     <t>WAT-900</t>
+  </si>
+  <si>
+    <t>WAT138</t>
+  </si>
+  <si>
+    <t>WAT-744</t>
+  </si>
+  <si>
+    <t>Verify that user cannot edit any data without getting into Curation mode</t>
   </si>
 </sst>
 </file>
@@ -1995,10 +2004,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E160"/>
+  <dimension ref="A1:E161"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A136" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B160" sqref="B160"/>
+      <selection activeCell="C161" sqref="C161"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4411,6 +4420,21 @@
         <v>5</v>
       </c>
       <c r="E160" s="7"/>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A161" s="7" t="s">
+        <v>506</v>
+      </c>
+      <c r="B161" s="7" t="s">
+        <v>507</v>
+      </c>
+      <c r="C161" s="8" t="s">
+        <v>508</v>
+      </c>
+      <c r="D161" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E161" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Adds WAT-140 test script and related changes
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/WAT.xlsx
+++ b/src/test/resources/xls/WAT.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="807" uniqueCount="512">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="811" uniqueCount="515">
   <si>
     <t>TCID</t>
   </si>
@@ -1532,12 +1532,6 @@
     <t>WAT137</t>
   </si>
   <si>
-    <t>Verify that If user hits cancel, feedback is not submitted and the system must display the author record in curation mode.</t>
-  </si>
-  <si>
-    <t>WAT-900</t>
-  </si>
-  <si>
     <t>WAT138</t>
   </si>
   <si>
@@ -1554,6 +1548,21 @@
   </si>
   <si>
     <t>Verify that the system provides a Submit Updates button to submit the changes done in curate mode</t>
+  </si>
+  <si>
+    <t>Verify that if User click on Cancel button the changes done in Curate mode is cleared off.</t>
+  </si>
+  <si>
+    <t>WAT-746</t>
+  </si>
+  <si>
+    <t>WAT140</t>
+  </si>
+  <si>
+    <t>WAT-747</t>
+  </si>
+  <si>
+    <t>Verify that after getting into curation mode, user should be able to remove individual publication.</t>
   </si>
 </sst>
 </file>
@@ -2013,10 +2022,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E162"/>
+  <dimension ref="A1:E163"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A145" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D166" sqref="D166"/>
+      <selection activeCell="C163" sqref="C163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4420,10 +4429,10 @@
         <v>503</v>
       </c>
       <c r="B160" s="7" t="s">
-        <v>505</v>
+        <v>511</v>
       </c>
       <c r="C160" s="8" t="s">
-        <v>504</v>
+        <v>510</v>
       </c>
       <c r="D160" s="9" t="s">
         <v>5</v>
@@ -4432,13 +4441,13 @@
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161" s="7" t="s">
+        <v>504</v>
+      </c>
+      <c r="B161" s="7" t="s">
+        <v>505</v>
+      </c>
+      <c r="C161" s="8" t="s">
         <v>506</v>
-      </c>
-      <c r="B161" s="7" t="s">
-        <v>507</v>
-      </c>
-      <c r="C161" s="8" t="s">
-        <v>508</v>
       </c>
       <c r="D161" s="9" t="s">
         <v>5</v>
@@ -4447,18 +4456,33 @@
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162" s="7" t="s">
+        <v>507</v>
+      </c>
+      <c r="B162" s="7" t="s">
+        <v>508</v>
+      </c>
+      <c r="C162" s="8" t="s">
         <v>509</v>
       </c>
-      <c r="B162" s="7" t="s">
-        <v>510</v>
-      </c>
-      <c r="C162" s="8" t="s">
-        <v>511</v>
-      </c>
       <c r="D162" s="9" t="s">
         <v>5</v>
       </c>
       <c r="E162" s="7"/>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A163" s="7" t="s">
+        <v>512</v>
+      </c>
+      <c r="B163" s="7" t="s">
+        <v>513</v>
+      </c>
+      <c r="C163" s="8" t="s">
+        <v>514</v>
+      </c>
+      <c r="D163" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E163" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
WAT new test script
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/WAT.xlsx
+++ b/src/test/resources/xls/WAT.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13305" windowHeight="2415"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="811" uniqueCount="515">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="814" uniqueCount="518">
   <si>
     <t>TCID</t>
   </si>
@@ -1563,13 +1563,22 @@
   </si>
   <si>
     <t>Verify that after getting into curation mode, user should be able to remove individual publication.</t>
+  </si>
+  <si>
+    <t>WAT173</t>
+  </si>
+  <si>
+    <t>Verity that recommend paper's last names is the set of author last names on that paper.||Verify that An author record's (single or combined record) last names is the set of last names on the authorships that compose the author record.</t>
+  </si>
+  <si>
+    <t>WAT-1374||WAT-1375</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1778,7 +1787,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1810,10 +1819,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1845,7 +1853,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2021,14 +2028,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E163"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E164"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A145" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C163" sqref="C163"/>
+      <selection activeCell="B164" sqref="B164"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="30.5703125" customWidth="1" collapsed="1"/>
@@ -2037,7 +2044,7 @@
     <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2054,7 +2061,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -2069,7 +2076,7 @@
       </c>
       <c r="E2" s="4"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -2084,7 +2091,7 @@
       </c>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" s="7" t="s">
         <v>11</v>
       </c>
@@ -2099,7 +2106,7 @@
       </c>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" s="7" t="s">
         <v>12</v>
       </c>
@@ -2114,7 +2121,7 @@
       </c>
       <c r="E5" s="7"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" s="7" t="s">
         <v>14</v>
       </c>
@@ -2129,7 +2136,7 @@
       </c>
       <c r="E6" s="7"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" s="7" t="s">
         <v>17</v>
       </c>
@@ -2144,7 +2151,7 @@
       </c>
       <c r="E7" s="7"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" s="7" t="s">
         <v>20</v>
       </c>
@@ -2159,7 +2166,7 @@
       </c>
       <c r="E8" s="7"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" s="7" t="s">
         <v>22</v>
       </c>
@@ -2174,7 +2181,7 @@
       </c>
       <c r="E9" s="7"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10" s="7" t="s">
         <v>23</v>
       </c>
@@ -2189,7 +2196,7 @@
       </c>
       <c r="E10" s="7"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11" s="7" t="s">
         <v>24</v>
       </c>
@@ -2204,7 +2211,7 @@
       </c>
       <c r="E11" s="7"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12" s="7" t="s">
         <v>25</v>
       </c>
@@ -2219,7 +2226,7 @@
       </c>
       <c r="E12" s="7"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13" s="7" t="s">
         <v>62</v>
       </c>
@@ -2234,7 +2241,7 @@
       </c>
       <c r="E13" s="7"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="A14" s="7" t="s">
         <v>63</v>
       </c>
@@ -2249,7 +2256,7 @@
       </c>
       <c r="E14" s="7"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="A15" s="7" t="s">
         <v>64</v>
       </c>
@@ -2264,7 +2271,7 @@
       </c>
       <c r="E15" s="7"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="A16" s="7" t="s">
         <v>65</v>
       </c>
@@ -2279,7 +2286,7 @@
       </c>
       <c r="E16" s="7"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5">
       <c r="A17" s="7" t="s">
         <v>74</v>
       </c>
@@ -2294,7 +2301,7 @@
       </c>
       <c r="E17" s="7"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5">
       <c r="A18" s="7" t="s">
         <v>75</v>
       </c>
@@ -2309,7 +2316,7 @@
       </c>
       <c r="E18" s="7"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5">
       <c r="A19" s="7" t="s">
         <v>79</v>
       </c>
@@ -2324,7 +2331,7 @@
       </c>
       <c r="E19" s="7"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5">
       <c r="A20" s="7" t="s">
         <v>81</v>
       </c>
@@ -2339,7 +2346,7 @@
       </c>
       <c r="E20" s="7"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5">
       <c r="A21" s="7" t="s">
         <v>82</v>
       </c>
@@ -2354,7 +2361,7 @@
       </c>
       <c r="E21" s="7"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5">
       <c r="A22" s="7" t="s">
         <v>88</v>
       </c>
@@ -2369,7 +2376,7 @@
       </c>
       <c r="E22" s="7"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5">
       <c r="A23" s="7" t="s">
         <v>90</v>
       </c>
@@ -2384,7 +2391,7 @@
       </c>
       <c r="E23" s="7"/>
     </row>
-    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="30">
       <c r="A24" s="9" t="s">
         <v>94</v>
       </c>
@@ -2399,7 +2406,7 @@
       </c>
       <c r="E24" s="7"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5">
       <c r="A25" s="9" t="s">
         <v>96</v>
       </c>
@@ -2414,7 +2421,7 @@
       </c>
       <c r="E25" s="7"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5">
       <c r="A26" s="9" t="s">
         <v>98</v>
       </c>
@@ -2429,7 +2436,7 @@
       </c>
       <c r="E26" s="7"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5">
       <c r="A27" s="9" t="s">
         <v>102</v>
       </c>
@@ -2444,7 +2451,7 @@
       </c>
       <c r="E27" s="7"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5">
       <c r="A28" s="9" t="s">
         <v>105</v>
       </c>
@@ -2459,7 +2466,7 @@
       </c>
       <c r="E28" s="7"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5">
       <c r="A29" s="9" t="s">
         <v>108</v>
       </c>
@@ -2474,7 +2481,7 @@
       </c>
       <c r="E29" s="7"/>
     </row>
-    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" ht="30">
       <c r="A30" s="9" t="s">
         <v>110</v>
       </c>
@@ -2489,7 +2496,7 @@
       </c>
       <c r="E30" s="7"/>
     </row>
-    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" ht="30">
       <c r="A31" s="9" t="s">
         <v>114</v>
       </c>
@@ -2504,7 +2511,7 @@
       </c>
       <c r="E31" s="7"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5">
       <c r="A32" s="9" t="s">
         <v>119</v>
       </c>
@@ -2519,7 +2526,7 @@
       </c>
       <c r="E32" s="7"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5">
       <c r="A33" s="9" t="s">
         <v>120</v>
       </c>
@@ -2534,7 +2541,7 @@
       </c>
       <c r="E33" s="7"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5">
       <c r="A34" s="9" t="s">
         <v>125</v>
       </c>
@@ -2549,7 +2556,7 @@
       </c>
       <c r="E34" s="7"/>
     </row>
-    <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" ht="30">
       <c r="A35" s="9" t="s">
         <v>128</v>
       </c>
@@ -2564,7 +2571,7 @@
       </c>
       <c r="E35" s="7"/>
     </row>
-    <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" ht="30">
       <c r="A36" s="9" t="s">
         <v>131</v>
       </c>
@@ -2579,7 +2586,7 @@
       </c>
       <c r="E36" s="7"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5">
       <c r="A37" s="9" t="s">
         <v>134</v>
       </c>
@@ -2594,7 +2601,7 @@
       </c>
       <c r="E37" s="7"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5">
       <c r="A38" s="9" t="s">
         <v>137</v>
       </c>
@@ -2609,7 +2616,7 @@
       </c>
       <c r="E38" s="7"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5">
       <c r="A39" s="9" t="s">
         <v>140</v>
       </c>
@@ -2624,7 +2631,7 @@
       </c>
       <c r="E39" s="7"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5">
       <c r="A40" s="9" t="s">
         <v>143</v>
       </c>
@@ -2639,7 +2646,7 @@
       </c>
       <c r="E40" s="7"/>
     </row>
-    <row r="41" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" ht="30">
       <c r="A41" s="9" t="s">
         <v>145</v>
       </c>
@@ -2654,7 +2661,7 @@
       </c>
       <c r="E41" s="7"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5">
       <c r="A42" s="9" t="s">
         <v>147</v>
       </c>
@@ -2669,7 +2676,7 @@
       </c>
       <c r="E42" s="7"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5">
       <c r="A43" s="9" t="s">
         <v>150</v>
       </c>
@@ -2684,7 +2691,7 @@
       </c>
       <c r="E43" s="7"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5">
       <c r="A44" s="9" t="s">
         <v>153</v>
       </c>
@@ -2699,7 +2706,7 @@
       </c>
       <c r="E44" s="7"/>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5">
       <c r="A45" s="9" t="s">
         <v>155</v>
       </c>
@@ -2714,7 +2721,7 @@
       </c>
       <c r="E45" s="7"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5">
       <c r="A46" s="12" t="s">
         <v>158</v>
       </c>
@@ -2729,7 +2736,7 @@
       </c>
       <c r="E46" s="7"/>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5">
       <c r="A47" s="12" t="s">
         <v>159</v>
       </c>
@@ -2744,7 +2751,7 @@
       </c>
       <c r="E47" s="7"/>
     </row>
-    <row r="48" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" ht="30">
       <c r="A48" s="12" t="s">
         <v>160</v>
       </c>
@@ -2759,7 +2766,7 @@
       </c>
       <c r="E48" s="7"/>
     </row>
-    <row r="49" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" ht="30">
       <c r="A49" s="12" t="s">
         <v>161</v>
       </c>
@@ -2774,7 +2781,7 @@
       </c>
       <c r="E49" s="7"/>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5">
       <c r="A50" s="12" t="s">
         <v>164</v>
       </c>
@@ -2789,7 +2796,7 @@
       </c>
       <c r="E50" s="7"/>
     </row>
-    <row r="51" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" ht="30">
       <c r="A51" s="9" t="s">
         <v>173</v>
       </c>
@@ -2804,7 +2811,7 @@
       </c>
       <c r="E51" s="7"/>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5">
       <c r="A52" s="9" t="s">
         <v>174</v>
       </c>
@@ -2819,7 +2826,7 @@
       </c>
       <c r="E52" s="7"/>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5">
       <c r="A53" s="9" t="s">
         <v>179</v>
       </c>
@@ -2834,7 +2841,7 @@
       </c>
       <c r="E53" s="7"/>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5">
       <c r="A54" s="9" t="s">
         <v>180</v>
       </c>
@@ -2849,7 +2856,7 @@
       </c>
       <c r="E54" s="7"/>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5">
       <c r="A55" s="9" t="s">
         <v>185</v>
       </c>
@@ -2864,7 +2871,7 @@
       </c>
       <c r="E55" s="7"/>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5">
       <c r="A56" s="9" t="s">
         <v>188</v>
       </c>
@@ -2879,7 +2886,7 @@
       </c>
       <c r="E56" s="7"/>
     </row>
-    <row r="57" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" ht="30">
       <c r="A57" s="9" t="s">
         <v>191</v>
       </c>
@@ -2894,7 +2901,7 @@
       </c>
       <c r="E57" s="7"/>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5">
       <c r="A58" s="9" t="s">
         <v>194</v>
       </c>
@@ -2909,7 +2916,7 @@
       </c>
       <c r="E58" s="7"/>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5">
       <c r="A59" s="7" t="s">
         <v>196</v>
       </c>
@@ -2924,7 +2931,7 @@
       </c>
       <c r="E59" s="7"/>
     </row>
-    <row r="60" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" ht="45">
       <c r="A60" s="7" t="s">
         <v>199</v>
       </c>
@@ -2939,7 +2946,7 @@
       </c>
       <c r="E60" s="7"/>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5">
       <c r="A61" s="9" t="s">
         <v>202</v>
       </c>
@@ -2954,7 +2961,7 @@
       </c>
       <c r="E61" s="7"/>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5">
       <c r="A62" s="9" t="s">
         <v>204</v>
       </c>
@@ -2969,7 +2976,7 @@
       </c>
       <c r="E62" s="7"/>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5">
       <c r="A63" s="9" t="s">
         <v>206</v>
       </c>
@@ -2984,7 +2991,7 @@
       </c>
       <c r="E63" s="7"/>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5">
       <c r="A64" s="9" t="s">
         <v>208</v>
       </c>
@@ -2999,7 +3006,7 @@
       </c>
       <c r="E64" s="7"/>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5">
       <c r="A65" s="9" t="s">
         <v>217</v>
       </c>
@@ -3014,7 +3021,7 @@
       </c>
       <c r="E65" s="7"/>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5">
       <c r="A66" s="9" t="s">
         <v>218</v>
       </c>
@@ -3029,7 +3036,7 @@
       </c>
       <c r="E66" s="7"/>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5">
       <c r="A67" s="9" t="s">
         <v>223</v>
       </c>
@@ -3044,7 +3051,7 @@
       </c>
       <c r="E67" s="7"/>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5">
       <c r="A68" s="9" t="s">
         <v>224</v>
       </c>
@@ -3059,7 +3066,7 @@
       </c>
       <c r="E68" s="7"/>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5">
       <c r="A69" s="9" t="s">
         <v>225</v>
       </c>
@@ -3074,7 +3081,7 @@
       </c>
       <c r="E69" s="7"/>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5">
       <c r="A70" s="9" t="s">
         <v>226</v>
       </c>
@@ -3089,7 +3096,7 @@
       </c>
       <c r="E70" s="7"/>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5">
       <c r="A71" s="9" t="s">
         <v>233</v>
       </c>
@@ -3104,7 +3111,7 @@
       </c>
       <c r="E71" s="7"/>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5">
       <c r="A72" s="9" t="s">
         <v>237</v>
       </c>
@@ -3119,7 +3126,7 @@
       </c>
       <c r="E72" s="7"/>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5">
       <c r="A73" s="9" t="s">
         <v>239</v>
       </c>
@@ -3134,7 +3141,7 @@
       </c>
       <c r="E73" s="7"/>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5">
       <c r="A74" s="9" t="s">
         <v>243</v>
       </c>
@@ -3149,7 +3156,7 @@
       </c>
       <c r="E74" s="7"/>
     </row>
-    <row r="75" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" ht="30">
       <c r="A75" s="9" t="s">
         <v>245</v>
       </c>
@@ -3164,7 +3171,7 @@
       </c>
       <c r="E75" s="7"/>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5">
       <c r="A76" s="9" t="s">
         <v>248</v>
       </c>
@@ -3179,7 +3186,7 @@
       </c>
       <c r="E76" s="7"/>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5">
       <c r="A77" s="9" t="s">
         <v>256</v>
       </c>
@@ -3194,7 +3201,7 @@
       </c>
       <c r="E77" s="7"/>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5">
       <c r="A78" s="9" t="s">
         <v>257</v>
       </c>
@@ -3209,7 +3216,7 @@
       </c>
       <c r="E78" s="7"/>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5">
       <c r="A79" s="9" t="s">
         <v>261</v>
       </c>
@@ -3224,7 +3231,7 @@
       </c>
       <c r="E79" s="7"/>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5">
       <c r="A80" s="9" t="s">
         <v>264</v>
       </c>
@@ -3239,7 +3246,7 @@
       </c>
       <c r="E80" s="7"/>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5">
       <c r="A81" s="9" t="s">
         <v>267</v>
       </c>
@@ -3254,7 +3261,7 @@
       </c>
       <c r="E81" s="7"/>
     </row>
-    <row r="82" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" ht="30">
       <c r="A82" s="9" t="s">
         <v>269</v>
       </c>
@@ -3269,7 +3276,7 @@
       </c>
       <c r="E82" s="7"/>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5">
       <c r="A83" s="9" t="s">
         <v>274</v>
       </c>
@@ -3284,7 +3291,7 @@
       </c>
       <c r="E83" s="7"/>
     </row>
-    <row r="84" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" ht="30">
       <c r="A84" s="9" t="s">
         <v>277</v>
       </c>
@@ -3299,7 +3306,7 @@
       </c>
       <c r="E84" s="7"/>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5">
       <c r="A85" s="9" t="s">
         <v>279</v>
       </c>
@@ -3314,7 +3321,7 @@
       </c>
       <c r="E85" s="7"/>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5">
       <c r="A86" s="9" t="s">
         <v>282</v>
       </c>
@@ -3329,7 +3336,7 @@
       </c>
       <c r="E86" s="7"/>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5">
       <c r="A87" s="9" t="s">
         <v>285</v>
       </c>
@@ -3344,7 +3351,7 @@
       </c>
       <c r="E87" s="7"/>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5">
       <c r="A88" s="9" t="s">
         <v>288</v>
       </c>
@@ -3359,7 +3366,7 @@
       </c>
       <c r="E88" s="7"/>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5">
       <c r="A89" s="9" t="s">
         <v>291</v>
       </c>
@@ -3374,7 +3381,7 @@
       </c>
       <c r="E89" s="7"/>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5">
       <c r="A90" s="9" t="s">
         <v>294</v>
       </c>
@@ -3389,7 +3396,7 @@
       </c>
       <c r="E90" s="7"/>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5">
       <c r="A91" s="9" t="s">
         <v>297</v>
       </c>
@@ -3404,7 +3411,7 @@
       </c>
       <c r="E91" s="7"/>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5">
       <c r="A92" s="9" t="s">
         <v>300</v>
       </c>
@@ -3419,7 +3426,7 @@
       </c>
       <c r="E92" s="7"/>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5">
       <c r="A93" s="9" t="s">
         <v>303</v>
       </c>
@@ -3434,7 +3441,7 @@
       </c>
       <c r="E93" s="7"/>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5">
       <c r="A94" s="9" t="s">
         <v>306</v>
       </c>
@@ -3449,7 +3456,7 @@
       </c>
       <c r="E94" s="7"/>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5">
       <c r="A95" s="9" t="s">
         <v>309</v>
       </c>
@@ -3464,7 +3471,7 @@
       </c>
       <c r="E95" s="7"/>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5">
       <c r="A96" s="9" t="s">
         <v>314</v>
       </c>
@@ -3479,7 +3486,7 @@
       </c>
       <c r="E96" s="7"/>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5">
       <c r="A97" s="9" t="s">
         <v>315</v>
       </c>
@@ -3494,7 +3501,7 @@
       </c>
       <c r="E97" s="7"/>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5">
       <c r="A98" s="9" t="s">
         <v>319</v>
       </c>
@@ -3509,7 +3516,7 @@
       </c>
       <c r="E98" s="7"/>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5">
       <c r="A99" s="9" t="s">
         <v>321</v>
       </c>
@@ -3524,7 +3531,7 @@
       </c>
       <c r="E99" s="7"/>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5">
       <c r="A100" s="9" t="s">
         <v>322</v>
       </c>
@@ -3539,7 +3546,7 @@
       </c>
       <c r="E100" s="7"/>
     </row>
-    <row r="101" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" ht="30">
       <c r="A101" s="9" t="s">
         <v>323</v>
       </c>
@@ -3554,7 +3561,7 @@
       </c>
       <c r="E101" s="7"/>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5">
       <c r="A102" s="9" t="s">
         <v>328</v>
       </c>
@@ -3569,7 +3576,7 @@
       </c>
       <c r="E102" s="7"/>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5">
       <c r="A103" s="9" t="s">
         <v>333</v>
       </c>
@@ -3584,7 +3591,7 @@
       </c>
       <c r="E103" s="7"/>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5">
       <c r="A104" s="9" t="s">
         <v>336</v>
       </c>
@@ -3599,7 +3606,7 @@
       </c>
       <c r="E104" s="7"/>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5">
       <c r="A105" s="9" t="s">
         <v>337</v>
       </c>
@@ -3614,7 +3621,7 @@
       </c>
       <c r="E105" s="7"/>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5">
       <c r="A106" s="9" t="s">
         <v>342</v>
       </c>
@@ -3629,7 +3636,7 @@
       </c>
       <c r="E106" s="7"/>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5">
       <c r="A107" s="9" t="s">
         <v>345</v>
       </c>
@@ -3644,7 +3651,7 @@
       </c>
       <c r="E107" s="7"/>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5">
       <c r="A108" s="9" t="s">
         <v>350</v>
       </c>
@@ -3659,7 +3666,7 @@
       </c>
       <c r="E108" s="7"/>
     </row>
-    <row r="109" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" ht="30">
       <c r="A109" s="9" t="s">
         <v>351</v>
       </c>
@@ -3674,7 +3681,7 @@
       </c>
       <c r="E109" s="7"/>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5">
       <c r="A110" s="9" t="s">
         <v>354</v>
       </c>
@@ -3689,7 +3696,7 @@
       </c>
       <c r="E110" s="7"/>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5">
       <c r="A111" s="9" t="s">
         <v>357</v>
       </c>
@@ -3704,7 +3711,7 @@
       </c>
       <c r="E111" s="7"/>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5">
       <c r="A112" s="9" t="s">
         <v>361</v>
       </c>
@@ -3719,7 +3726,7 @@
       </c>
       <c r="E112" s="7"/>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5">
       <c r="A113" s="9" t="s">
         <v>363</v>
       </c>
@@ -3734,7 +3741,7 @@
       </c>
       <c r="E113" s="7"/>
     </row>
-    <row r="114" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" ht="30">
       <c r="A114" s="9" t="s">
         <v>366</v>
       </c>
@@ -3749,7 +3756,7 @@
       </c>
       <c r="E114" s="7"/>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5">
       <c r="A115" s="9" t="s">
         <v>369</v>
       </c>
@@ -3764,7 +3771,7 @@
       </c>
       <c r="E115" s="7"/>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5">
       <c r="A116" s="9" t="s">
         <v>370</v>
       </c>
@@ -3779,7 +3786,7 @@
       </c>
       <c r="E116" s="7"/>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5">
       <c r="A117" s="9" t="s">
         <v>371</v>
       </c>
@@ -3794,7 +3801,7 @@
       </c>
       <c r="E117" s="7"/>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5">
       <c r="A118" s="9" t="s">
         <v>378</v>
       </c>
@@ -3809,7 +3816,7 @@
       </c>
       <c r="E118" s="7"/>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5">
       <c r="A119" s="9" t="s">
         <v>381</v>
       </c>
@@ -3824,7 +3831,7 @@
       </c>
       <c r="E119" s="7"/>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5">
       <c r="A120" s="9" t="s">
         <v>384</v>
       </c>
@@ -3839,7 +3846,7 @@
       </c>
       <c r="E120" s="7"/>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5">
       <c r="A121" s="9" t="s">
         <v>387</v>
       </c>
@@ -3854,7 +3861,7 @@
       </c>
       <c r="E121" s="7"/>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5">
       <c r="A122" s="7" t="s">
         <v>390</v>
       </c>
@@ -3869,7 +3876,7 @@
       </c>
       <c r="E122" s="7"/>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5">
       <c r="A123" s="7" t="s">
         <v>393</v>
       </c>
@@ -3884,7 +3891,7 @@
       </c>
       <c r="E123" s="7"/>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5">
       <c r="A124" s="7" t="s">
         <v>396</v>
       </c>
@@ -3899,7 +3906,7 @@
       </c>
       <c r="E124" s="7"/>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5">
       <c r="A125" s="9" t="s">
         <v>399</v>
       </c>
@@ -3914,7 +3921,7 @@
       </c>
       <c r="E125" s="7"/>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5">
       <c r="A126" s="7" t="s">
         <v>402</v>
       </c>
@@ -3929,7 +3936,7 @@
       </c>
       <c r="E126" s="7"/>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5">
       <c r="A127" s="7" t="s">
         <v>405</v>
       </c>
@@ -3944,7 +3951,7 @@
       </c>
       <c r="E127" s="7"/>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5">
       <c r="A128" s="7" t="s">
         <v>408</v>
       </c>
@@ -3959,7 +3966,7 @@
       </c>
       <c r="E128" s="7"/>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5">
       <c r="A129" s="9" t="s">
         <v>411</v>
       </c>
@@ -3974,7 +3981,7 @@
       </c>
       <c r="E129" s="7"/>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5">
       <c r="A130" s="9" t="s">
         <v>414</v>
       </c>
@@ -3989,7 +3996,7 @@
       </c>
       <c r="E130" s="7"/>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5">
       <c r="A131" s="9" t="s">
         <v>416</v>
       </c>
@@ -4004,7 +4011,7 @@
       </c>
       <c r="E131" s="7"/>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5">
       <c r="A132" s="7" t="s">
         <v>419</v>
       </c>
@@ -4019,7 +4026,7 @@
       </c>
       <c r="E132" s="7"/>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5">
       <c r="A133" s="9" t="s">
         <v>422</v>
       </c>
@@ -4034,7 +4041,7 @@
       </c>
       <c r="E133" s="7"/>
     </row>
-    <row r="134" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5" ht="30">
       <c r="A134" s="7" t="s">
         <v>425</v>
       </c>
@@ -4049,7 +4056,7 @@
       </c>
       <c r="E134" s="7"/>
     </row>
-    <row r="135" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5" ht="30">
       <c r="A135" s="7" t="s">
         <v>426</v>
       </c>
@@ -4064,7 +4071,7 @@
       </c>
       <c r="E135" s="7"/>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5">
       <c r="A136" s="9" t="s">
         <v>431</v>
       </c>
@@ -4079,7 +4086,7 @@
       </c>
       <c r="E136" s="7"/>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5">
       <c r="A137" s="7" t="s">
         <v>434</v>
       </c>
@@ -4094,7 +4101,7 @@
       </c>
       <c r="E137" s="7"/>
     </row>
-    <row r="138" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" ht="45">
       <c r="A138" s="7" t="s">
         <v>435</v>
       </c>
@@ -4109,7 +4116,7 @@
       </c>
       <c r="E138" s="7"/>
     </row>
-    <row r="139" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5" ht="30">
       <c r="A139" s="7" t="s">
         <v>436</v>
       </c>
@@ -4124,7 +4131,7 @@
       </c>
       <c r="E139" s="7"/>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5">
       <c r="A140" s="17" t="s">
         <v>443</v>
       </c>
@@ -4139,7 +4146,7 @@
       </c>
       <c r="E140" s="7"/>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5">
       <c r="A141" s="17" t="s">
         <v>446</v>
       </c>
@@ -4154,7 +4161,7 @@
       </c>
       <c r="E141" s="7"/>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:5">
       <c r="A142" s="17" t="s">
         <v>449</v>
       </c>
@@ -4169,7 +4176,7 @@
       </c>
       <c r="E142" s="7"/>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:5">
       <c r="A143" s="17" t="s">
         <v>452</v>
       </c>
@@ -4184,7 +4191,7 @@
       </c>
       <c r="E143" s="7"/>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:5">
       <c r="A144" s="17" t="s">
         <v>453</v>
       </c>
@@ -4199,7 +4206,7 @@
       </c>
       <c r="E144" s="7"/>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:5">
       <c r="A145" s="17" t="s">
         <v>458</v>
       </c>
@@ -4214,7 +4221,7 @@
       </c>
       <c r="E145" s="7"/>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:5">
       <c r="A146" s="17" t="s">
         <v>461</v>
       </c>
@@ -4229,7 +4236,7 @@
       </c>
       <c r="E146" s="7"/>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:5">
       <c r="A147" s="17" t="s">
         <v>464</v>
       </c>
@@ -4244,7 +4251,7 @@
       </c>
       <c r="E147" s="7"/>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:5">
       <c r="A148" s="17" t="s">
         <v>467</v>
       </c>
@@ -4259,7 +4266,7 @@
       </c>
       <c r="E148" s="7"/>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:5">
       <c r="A149" s="7" t="s">
         <v>470</v>
       </c>
@@ -4274,7 +4281,7 @@
       </c>
       <c r="E149" s="7"/>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:5">
       <c r="A150" s="7" t="s">
         <v>471</v>
       </c>
@@ -4289,7 +4296,7 @@
       </c>
       <c r="E150" s="7"/>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:5">
       <c r="A151" s="7" t="s">
         <v>472</v>
       </c>
@@ -4304,7 +4311,7 @@
       </c>
       <c r="E151" s="7"/>
     </row>
-    <row r="152" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:5" ht="30">
       <c r="A152" s="7" t="s">
         <v>479</v>
       </c>
@@ -4319,7 +4326,7 @@
       </c>
       <c r="E152" s="7"/>
     </row>
-    <row r="153" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:5" ht="45">
       <c r="A153" s="17" t="s">
         <v>482</v>
       </c>
@@ -4334,7 +4341,7 @@
       </c>
       <c r="E153" s="7"/>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:5">
       <c r="A154" s="17" t="s">
         <v>484</v>
       </c>
@@ -4349,7 +4356,7 @@
       </c>
       <c r="E154" s="7"/>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:5">
       <c r="A155" s="7" t="s">
         <v>486</v>
       </c>
@@ -4364,7 +4371,7 @@
       </c>
       <c r="E155" s="7"/>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:5">
       <c r="A156" s="7" t="s">
         <v>489</v>
       </c>
@@ -4379,7 +4386,7 @@
       </c>
       <c r="E156" s="7"/>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:5">
       <c r="A157" s="7" t="s">
         <v>492</v>
       </c>
@@ -4394,7 +4401,7 @@
       </c>
       <c r="E157" s="7"/>
     </row>
-    <row r="158" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:5" ht="30">
       <c r="A158" s="7" t="s">
         <v>495</v>
       </c>
@@ -4409,7 +4416,7 @@
       </c>
       <c r="E158" s="7"/>
     </row>
-    <row r="159" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:5" ht="30">
       <c r="A159" s="7" t="s">
         <v>496</v>
       </c>
@@ -4424,7 +4431,7 @@
       </c>
       <c r="E159" s="7"/>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:5">
       <c r="A160" s="7" t="s">
         <v>503</v>
       </c>
@@ -4439,7 +4446,7 @@
       </c>
       <c r="E160" s="7"/>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:5">
       <c r="A161" s="7" t="s">
         <v>504</v>
       </c>
@@ -4454,7 +4461,7 @@
       </c>
       <c r="E161" s="7"/>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:5">
       <c r="A162" s="7" t="s">
         <v>507</v>
       </c>
@@ -4469,7 +4476,7 @@
       </c>
       <c r="E162" s="7"/>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:5">
       <c r="A163" s="7" t="s">
         <v>512</v>
       </c>
@@ -4483,6 +4490,19 @@
         <v>5</v>
       </c>
       <c r="E163" s="7"/>
+    </row>
+    <row r="164" spans="1:5" ht="30">
+      <c r="A164" s="7" t="s">
+        <v>515</v>
+      </c>
+      <c r="B164" s="7" t="s">
+        <v>517</v>
+      </c>
+      <c r="C164" s="8" t="s">
+        <v>516</v>
+      </c>
+      <c r="D164" s="7"/>
+      <c r="E164" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -4495,14 +4515,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView topLeftCell="A10" zoomScale="80" workbookViewId="0">
       <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
@@ -4510,7 +4530,7 @@
     <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="10" t="s">
         <v>35</v>
       </c>
@@ -4524,7 +4544,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="7" t="s">
         <v>37</v>
       </c>
@@ -4536,7 +4556,7 @@
       </c>
       <c r="D2" s="7"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="7" t="s">
         <v>38</v>
       </c>
@@ -4548,7 +4568,7 @@
       </c>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="7" t="s">
         <v>39</v>
       </c>
@@ -4560,7 +4580,7 @@
       </c>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" s="7" t="s">
         <v>40</v>
       </c>
@@ -4572,7 +4592,7 @@
       </c>
       <c r="D5" s="7"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" s="7" t="s">
         <v>41</v>
       </c>
@@ -4584,7 +4604,7 @@
       </c>
       <c r="D6" s="7"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="7" t="s">
         <v>42</v>
       </c>
@@ -4596,7 +4616,7 @@
       </c>
       <c r="D7" s="7"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="7" t="s">
         <v>43</v>
       </c>
@@ -4608,7 +4628,7 @@
       </c>
       <c r="D8" s="7"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="7" t="s">
         <v>44</v>
       </c>
@@ -4620,7 +4640,7 @@
       </c>
       <c r="D9" s="7"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="7" t="s">
         <v>45</v>
       </c>
@@ -4632,7 +4652,7 @@
       </c>
       <c r="D10" s="7"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11" s="7" t="s">
         <v>46</v>
       </c>
@@ -4644,7 +4664,7 @@
       </c>
       <c r="D11" s="7"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="A12" s="7" t="s">
         <v>48</v>
       </c>
@@ -4656,7 +4676,7 @@
       </c>
       <c r="D12" s="7"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="A13" s="7" t="s">
         <v>49</v>
       </c>
@@ -4668,7 +4688,7 @@
       </c>
       <c r="D13" s="7"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="A14" s="7" t="s">
         <v>50</v>
       </c>
@@ -4680,7 +4700,7 @@
       </c>
       <c r="D14" s="7"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="A15" s="7" t="s">
         <v>51</v>
       </c>
@@ -4692,7 +4712,7 @@
       </c>
       <c r="D15" s="7"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="A16" s="7" t="s">
         <v>52</v>
       </c>
@@ -4704,7 +4724,7 @@
       </c>
       <c r="D16" s="7"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4">
       <c r="A17" s="7" t="s">
         <v>53</v>
       </c>
@@ -4716,7 +4736,7 @@
       </c>
       <c r="D17" s="7"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4">
       <c r="A18" s="7" t="s">
         <v>54</v>
       </c>
@@ -4728,7 +4748,7 @@
       </c>
       <c r="D18" s="7"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4">
       <c r="A19" s="7" t="s">
         <v>55</v>
       </c>
@@ -4740,7 +4760,7 @@
       </c>
       <c r="D19" s="7"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4">
       <c r="A20" s="7" t="s">
         <v>56</v>
       </c>
@@ -4752,7 +4772,7 @@
       </c>
       <c r="D20" s="7"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4">
       <c r="A21" s="7" t="s">
         <v>57</v>
       </c>
@@ -4764,7 +4784,7 @@
       </c>
       <c r="D21" s="7"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4">
       <c r="A22" s="7" t="s">
         <v>58</v>
       </c>
@@ -4776,7 +4796,7 @@
       </c>
       <c r="D22" s="7"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4">
       <c r="A23" s="7" t="s">
         <v>59</v>
       </c>
@@ -4788,7 +4808,7 @@
       </c>
       <c r="D23" s="7"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4">
       <c r="A24" s="7" t="s">
         <v>60</v>
       </c>
@@ -4800,7 +4820,7 @@
       </c>
       <c r="D24" s="7"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4">
       <c r="A25" s="7" t="s">
         <v>61</v>
       </c>
@@ -4812,7 +4832,7 @@
       </c>
       <c r="D25" s="7"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4">
       <c r="A26" s="7" t="s">
         <v>47</v>
       </c>
@@ -4831,14 +4851,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A19" sqref="A19:XFD19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
@@ -4846,7 +4866,7 @@
     <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="10" t="s">
         <v>35</v>
       </c>
@@ -4860,7 +4880,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="7" t="s">
         <v>37</v>
       </c>
@@ -4872,7 +4892,7 @@
       </c>
       <c r="D2" s="7"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="7" t="s">
         <v>38</v>
       </c>
@@ -4884,7 +4904,7 @@
       </c>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="7" t="s">
         <v>39</v>
       </c>
@@ -4896,7 +4916,7 @@
       </c>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" s="7" t="s">
         <v>40</v>
       </c>
@@ -4908,7 +4928,7 @@
       </c>
       <c r="D5" s="7"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" s="7" t="s">
         <v>41</v>
       </c>
@@ -4920,7 +4940,7 @@
       </c>
       <c r="D6" s="7"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="7" t="s">
         <v>42</v>
       </c>
@@ -4932,7 +4952,7 @@
       </c>
       <c r="D7" s="7"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="7" t="s">
         <v>43</v>
       </c>
@@ -4944,7 +4964,7 @@
       </c>
       <c r="D8" s="7"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="7" t="s">
         <v>44</v>
       </c>
@@ -4956,7 +4976,7 @@
       </c>
       <c r="D9" s="7"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="7" t="s">
         <v>45</v>
       </c>
@@ -4968,7 +4988,7 @@
       </c>
       <c r="D10" s="7"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11" s="7" t="s">
         <v>46</v>
       </c>
@@ -4980,7 +5000,7 @@
       </c>
       <c r="D11" s="7"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="A12" s="7" t="s">
         <v>47</v>
       </c>
@@ -4992,7 +5012,7 @@
       </c>
       <c r="D12" s="7"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="A13" s="7" t="s">
         <v>48</v>
       </c>
@@ -5004,7 +5024,7 @@
       </c>
       <c r="D13" s="7"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="A14" s="7" t="s">
         <v>49</v>
       </c>
@@ -5016,7 +5036,7 @@
       </c>
       <c r="D14" s="7"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="A15" s="7" t="s">
         <v>50</v>
       </c>
@@ -5028,7 +5048,7 @@
       </c>
       <c r="D15" s="7"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="A16" s="7" t="s">
         <v>51</v>
       </c>
@@ -5040,7 +5060,7 @@
       </c>
       <c r="D16" s="7"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4">
       <c r="A17" s="7" t="s">
         <v>52</v>
       </c>
@@ -5052,7 +5072,7 @@
       </c>
       <c r="D17" s="7"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4">
       <c r="A18" s="7" t="s">
         <v>53</v>
       </c>
@@ -5064,7 +5084,7 @@
       </c>
       <c r="D18" s="7"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4">
       <c r="A19" s="7" t="s">
         <v>54</v>
       </c>
@@ -5076,7 +5096,7 @@
       </c>
       <c r="D19" s="7"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4">
       <c r="A20" s="7" t="s">
         <v>55</v>
       </c>
@@ -5088,7 +5108,7 @@
       </c>
       <c r="D20" s="7"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4">
       <c r="A21" s="7" t="s">
         <v>56</v>
       </c>
@@ -5100,7 +5120,7 @@
       </c>
       <c r="D21" s="7"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4">
       <c r="A22" s="7" t="s">
         <v>57</v>
       </c>
@@ -5112,7 +5132,7 @@
       </c>
       <c r="D22" s="7"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4">
       <c r="A23" s="7" t="s">
         <v>58</v>
       </c>
@@ -5124,7 +5144,7 @@
       </c>
       <c r="D23" s="7"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4">
       <c r="A24" s="7" t="s">
         <v>59</v>
       </c>
@@ -5136,7 +5156,7 @@
       </c>
       <c r="D24" s="7"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4">
       <c r="A25" s="7" t="s">
         <v>60</v>
       </c>
@@ -5148,7 +5168,7 @@
       </c>
       <c r="D25" s="7"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4">
       <c r="A26" s="7" t="s">
         <v>61</v>
       </c>

</xml_diff>

<commit_message>
Adds WAT-141 testscript and related changes
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/WAT.xlsx
+++ b/src/test/resources/xls/WAT.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13305" windowHeight="2415"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="814" uniqueCount="518">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="818" uniqueCount="521">
   <si>
     <t>TCID</t>
   </si>
@@ -1572,13 +1572,22 @@
   </si>
   <si>
     <t>WAT-1374||WAT-1375</t>
+  </si>
+  <si>
+    <t>WAT141</t>
+  </si>
+  <si>
+    <t>WAT-749</t>
+  </si>
+  <si>
+    <t>Verify that after removing a publication, the total publication count should get updated accordingly.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1787,7 +1796,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1819,9 +1828,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1853,6 +1863,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2028,14 +2039,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E164"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E165"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A145" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B164" sqref="B164"/>
+      <selection activeCell="C165" sqref="C165"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="30.5703125" customWidth="1" collapsed="1"/>
@@ -2044,7 +2055,7 @@
     <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2061,7 +2072,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -2076,7 +2087,7 @@
       </c>
       <c r="E2" s="4"/>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -2091,7 +2102,7 @@
       </c>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>11</v>
       </c>
@@ -2106,7 +2117,7 @@
       </c>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>12</v>
       </c>
@@ -2121,7 +2132,7 @@
       </c>
       <c r="E5" s="7"/>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>14</v>
       </c>
@@ -2136,7 +2147,7 @@
       </c>
       <c r="E6" s="7"/>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>17</v>
       </c>
@@ -2151,7 +2162,7 @@
       </c>
       <c r="E7" s="7"/>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>20</v>
       </c>
@@ -2166,7 +2177,7 @@
       </c>
       <c r="E8" s="7"/>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>22</v>
       </c>
@@ -2181,7 +2192,7 @@
       </c>
       <c r="E9" s="7"/>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>23</v>
       </c>
@@ -2196,7 +2207,7 @@
       </c>
       <c r="E10" s="7"/>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>24</v>
       </c>
@@ -2211,7 +2222,7 @@
       </c>
       <c r="E11" s="7"/>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>25</v>
       </c>
@@ -2226,7 +2237,7 @@
       </c>
       <c r="E12" s="7"/>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>62</v>
       </c>
@@ -2241,7 +2252,7 @@
       </c>
       <c r="E13" s="7"/>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>63</v>
       </c>
@@ -2256,7 +2267,7 @@
       </c>
       <c r="E14" s="7"/>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>64</v>
       </c>
@@ -2271,7 +2282,7 @@
       </c>
       <c r="E15" s="7"/>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>65</v>
       </c>
@@ -2286,7 +2297,7 @@
       </c>
       <c r="E16" s="7"/>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>74</v>
       </c>
@@ -2301,7 +2312,7 @@
       </c>
       <c r="E17" s="7"/>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>75</v>
       </c>
@@ -2316,7 +2327,7 @@
       </c>
       <c r="E18" s="7"/>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>79</v>
       </c>
@@ -2331,7 +2342,7 @@
       </c>
       <c r="E19" s="7"/>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>81</v>
       </c>
@@ -2346,7 +2357,7 @@
       </c>
       <c r="E20" s="7"/>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>82</v>
       </c>
@@ -2361,7 +2372,7 @@
       </c>
       <c r="E21" s="7"/>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>88</v>
       </c>
@@ -2376,7 +2387,7 @@
       </c>
       <c r="E22" s="7"/>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>90</v>
       </c>
@@ -2391,7 +2402,7 @@
       </c>
       <c r="E23" s="7"/>
     </row>
-    <row r="24" spans="1:5" ht="30">
+    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>94</v>
       </c>
@@ -2406,7 +2417,7 @@
       </c>
       <c r="E24" s="7"/>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>96</v>
       </c>
@@ -2421,7 +2432,7 @@
       </c>
       <c r="E25" s="7"/>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
         <v>98</v>
       </c>
@@ -2436,7 +2447,7 @@
       </c>
       <c r="E26" s="7"/>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
         <v>102</v>
       </c>
@@ -2451,7 +2462,7 @@
       </c>
       <c r="E27" s="7"/>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
         <v>105</v>
       </c>
@@ -2466,7 +2477,7 @@
       </c>
       <c r="E28" s="7"/>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
         <v>108</v>
       </c>
@@ -2481,7 +2492,7 @@
       </c>
       <c r="E29" s="7"/>
     </row>
-    <row r="30" spans="1:5" ht="30">
+    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
         <v>110</v>
       </c>
@@ -2496,7 +2507,7 @@
       </c>
       <c r="E30" s="7"/>
     </row>
-    <row r="31" spans="1:5" ht="30">
+    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
         <v>114</v>
       </c>
@@ -2511,7 +2522,7 @@
       </c>
       <c r="E31" s="7"/>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
         <v>119</v>
       </c>
@@ -2526,7 +2537,7 @@
       </c>
       <c r="E32" s="7"/>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
         <v>120</v>
       </c>
@@ -2541,7 +2552,7 @@
       </c>
       <c r="E33" s="7"/>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
         <v>125</v>
       </c>
@@ -2556,7 +2567,7 @@
       </c>
       <c r="E34" s="7"/>
     </row>
-    <row r="35" spans="1:5" ht="30">
+    <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
         <v>128</v>
       </c>
@@ -2571,7 +2582,7 @@
       </c>
       <c r="E35" s="7"/>
     </row>
-    <row r="36" spans="1:5" ht="30">
+    <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
         <v>131</v>
       </c>
@@ -2586,7 +2597,7 @@
       </c>
       <c r="E36" s="7"/>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
         <v>134</v>
       </c>
@@ -2601,7 +2612,7 @@
       </c>
       <c r="E37" s="7"/>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="9" t="s">
         <v>137</v>
       </c>
@@ -2616,7 +2627,7 @@
       </c>
       <c r="E38" s="7"/>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="s">
         <v>140</v>
       </c>
@@ -2631,7 +2642,7 @@
       </c>
       <c r="E39" s="7"/>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="9" t="s">
         <v>143</v>
       </c>
@@ -2646,7 +2657,7 @@
       </c>
       <c r="E40" s="7"/>
     </row>
-    <row r="41" spans="1:5" ht="30">
+    <row r="41" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
         <v>145</v>
       </c>
@@ -2661,7 +2672,7 @@
       </c>
       <c r="E41" s="7"/>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="9" t="s">
         <v>147</v>
       </c>
@@ -2676,7 +2687,7 @@
       </c>
       <c r="E42" s="7"/>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="9" t="s">
         <v>150</v>
       </c>
@@ -2691,7 +2702,7 @@
       </c>
       <c r="E43" s="7"/>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="9" t="s">
         <v>153</v>
       </c>
@@ -2706,7 +2717,7 @@
       </c>
       <c r="E44" s="7"/>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="9" t="s">
         <v>155</v>
       </c>
@@ -2721,7 +2732,7 @@
       </c>
       <c r="E45" s="7"/>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="12" t="s">
         <v>158</v>
       </c>
@@ -2736,7 +2747,7 @@
       </c>
       <c r="E46" s="7"/>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="12" t="s">
         <v>159</v>
       </c>
@@ -2751,7 +2762,7 @@
       </c>
       <c r="E47" s="7"/>
     </row>
-    <row r="48" spans="1:5" ht="30">
+    <row r="48" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="12" t="s">
         <v>160</v>
       </c>
@@ -2766,7 +2777,7 @@
       </c>
       <c r="E48" s="7"/>
     </row>
-    <row r="49" spans="1:5" ht="30">
+    <row r="49" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="12" t="s">
         <v>161</v>
       </c>
@@ -2781,7 +2792,7 @@
       </c>
       <c r="E49" s="7"/>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="12" t="s">
         <v>164</v>
       </c>
@@ -2796,7 +2807,7 @@
       </c>
       <c r="E50" s="7"/>
     </row>
-    <row r="51" spans="1:5" ht="30">
+    <row r="51" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="9" t="s">
         <v>173</v>
       </c>
@@ -2811,7 +2822,7 @@
       </c>
       <c r="E51" s="7"/>
     </row>
-    <row r="52" spans="1:5">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="9" t="s">
         <v>174</v>
       </c>
@@ -2826,7 +2837,7 @@
       </c>
       <c r="E52" s="7"/>
     </row>
-    <row r="53" spans="1:5">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="9" t="s">
         <v>179</v>
       </c>
@@ -2841,7 +2852,7 @@
       </c>
       <c r="E53" s="7"/>
     </row>
-    <row r="54" spans="1:5">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="9" t="s">
         <v>180</v>
       </c>
@@ -2856,7 +2867,7 @@
       </c>
       <c r="E54" s="7"/>
     </row>
-    <row r="55" spans="1:5">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="9" t="s">
         <v>185</v>
       </c>
@@ -2871,7 +2882,7 @@
       </c>
       <c r="E55" s="7"/>
     </row>
-    <row r="56" spans="1:5">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="s">
         <v>188</v>
       </c>
@@ -2886,7 +2897,7 @@
       </c>
       <c r="E56" s="7"/>
     </row>
-    <row r="57" spans="1:5" ht="30">
+    <row r="57" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="9" t="s">
         <v>191</v>
       </c>
@@ -2901,7 +2912,7 @@
       </c>
       <c r="E57" s="7"/>
     </row>
-    <row r="58" spans="1:5">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="9" t="s">
         <v>194</v>
       </c>
@@ -2916,7 +2927,7 @@
       </c>
       <c r="E58" s="7"/>
     </row>
-    <row r="59" spans="1:5">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
         <v>196</v>
       </c>
@@ -2931,7 +2942,7 @@
       </c>
       <c r="E59" s="7"/>
     </row>
-    <row r="60" spans="1:5" ht="45">
+    <row r="60" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
         <v>199</v>
       </c>
@@ -2946,7 +2957,7 @@
       </c>
       <c r="E60" s="7"/>
     </row>
-    <row r="61" spans="1:5">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="9" t="s">
         <v>202</v>
       </c>
@@ -2961,7 +2972,7 @@
       </c>
       <c r="E61" s="7"/>
     </row>
-    <row r="62" spans="1:5">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="9" t="s">
         <v>204</v>
       </c>
@@ -2976,7 +2987,7 @@
       </c>
       <c r="E62" s="7"/>
     </row>
-    <row r="63" spans="1:5">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="9" t="s">
         <v>206</v>
       </c>
@@ -2991,7 +3002,7 @@
       </c>
       <c r="E63" s="7"/>
     </row>
-    <row r="64" spans="1:5">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="9" t="s">
         <v>208</v>
       </c>
@@ -3006,7 +3017,7 @@
       </c>
       <c r="E64" s="7"/>
     </row>
-    <row r="65" spans="1:5">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="9" t="s">
         <v>217</v>
       </c>
@@ -3021,7 +3032,7 @@
       </c>
       <c r="E65" s="7"/>
     </row>
-    <row r="66" spans="1:5">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="9" t="s">
         <v>218</v>
       </c>
@@ -3036,7 +3047,7 @@
       </c>
       <c r="E66" s="7"/>
     </row>
-    <row r="67" spans="1:5">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="9" t="s">
         <v>223</v>
       </c>
@@ -3051,7 +3062,7 @@
       </c>
       <c r="E67" s="7"/>
     </row>
-    <row r="68" spans="1:5">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="9" t="s">
         <v>224</v>
       </c>
@@ -3066,7 +3077,7 @@
       </c>
       <c r="E68" s="7"/>
     </row>
-    <row r="69" spans="1:5">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="9" t="s">
         <v>225</v>
       </c>
@@ -3081,7 +3092,7 @@
       </c>
       <c r="E69" s="7"/>
     </row>
-    <row r="70" spans="1:5">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="9" t="s">
         <v>226</v>
       </c>
@@ -3096,7 +3107,7 @@
       </c>
       <c r="E70" s="7"/>
     </row>
-    <row r="71" spans="1:5">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="9" t="s">
         <v>233</v>
       </c>
@@ -3111,7 +3122,7 @@
       </c>
       <c r="E71" s="7"/>
     </row>
-    <row r="72" spans="1:5">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="9" t="s">
         <v>237</v>
       </c>
@@ -3126,7 +3137,7 @@
       </c>
       <c r="E72" s="7"/>
     </row>
-    <row r="73" spans="1:5">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="9" t="s">
         <v>239</v>
       </c>
@@ -3141,7 +3152,7 @@
       </c>
       <c r="E73" s="7"/>
     </row>
-    <row r="74" spans="1:5">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="9" t="s">
         <v>243</v>
       </c>
@@ -3156,7 +3167,7 @@
       </c>
       <c r="E74" s="7"/>
     </row>
-    <row r="75" spans="1:5" ht="30">
+    <row r="75" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" s="9" t="s">
         <v>245</v>
       </c>
@@ -3171,7 +3182,7 @@
       </c>
       <c r="E75" s="7"/>
     </row>
-    <row r="76" spans="1:5">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="9" t="s">
         <v>248</v>
       </c>
@@ -3186,7 +3197,7 @@
       </c>
       <c r="E76" s="7"/>
     </row>
-    <row r="77" spans="1:5">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="9" t="s">
         <v>256</v>
       </c>
@@ -3201,7 +3212,7 @@
       </c>
       <c r="E77" s="7"/>
     </row>
-    <row r="78" spans="1:5">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="9" t="s">
         <v>257</v>
       </c>
@@ -3216,7 +3227,7 @@
       </c>
       <c r="E78" s="7"/>
     </row>
-    <row r="79" spans="1:5">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="9" t="s">
         <v>261</v>
       </c>
@@ -3231,7 +3242,7 @@
       </c>
       <c r="E79" s="7"/>
     </row>
-    <row r="80" spans="1:5">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="9" t="s">
         <v>264</v>
       </c>
@@ -3246,7 +3257,7 @@
       </c>
       <c r="E80" s="7"/>
     </row>
-    <row r="81" spans="1:5">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="9" t="s">
         <v>267</v>
       </c>
@@ -3261,7 +3272,7 @@
       </c>
       <c r="E81" s="7"/>
     </row>
-    <row r="82" spans="1:5" ht="30">
+    <row r="82" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A82" s="9" t="s">
         <v>269</v>
       </c>
@@ -3276,7 +3287,7 @@
       </c>
       <c r="E82" s="7"/>
     </row>
-    <row r="83" spans="1:5">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="9" t="s">
         <v>274</v>
       </c>
@@ -3291,7 +3302,7 @@
       </c>
       <c r="E83" s="7"/>
     </row>
-    <row r="84" spans="1:5" ht="30">
+    <row r="84" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A84" s="9" t="s">
         <v>277</v>
       </c>
@@ -3306,7 +3317,7 @@
       </c>
       <c r="E84" s="7"/>
     </row>
-    <row r="85" spans="1:5">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="9" t="s">
         <v>279</v>
       </c>
@@ -3321,7 +3332,7 @@
       </c>
       <c r="E85" s="7"/>
     </row>
-    <row r="86" spans="1:5">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="9" t="s">
         <v>282</v>
       </c>
@@ -3336,7 +3347,7 @@
       </c>
       <c r="E86" s="7"/>
     </row>
-    <row r="87" spans="1:5">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="9" t="s">
         <v>285</v>
       </c>
@@ -3351,7 +3362,7 @@
       </c>
       <c r="E87" s="7"/>
     </row>
-    <row r="88" spans="1:5">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="9" t="s">
         <v>288</v>
       </c>
@@ -3366,7 +3377,7 @@
       </c>
       <c r="E88" s="7"/>
     </row>
-    <row r="89" spans="1:5">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="9" t="s">
         <v>291</v>
       </c>
@@ -3381,7 +3392,7 @@
       </c>
       <c r="E89" s="7"/>
     </row>
-    <row r="90" spans="1:5">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="9" t="s">
         <v>294</v>
       </c>
@@ -3396,7 +3407,7 @@
       </c>
       <c r="E90" s="7"/>
     </row>
-    <row r="91" spans="1:5">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="9" t="s">
         <v>297</v>
       </c>
@@ -3411,7 +3422,7 @@
       </c>
       <c r="E91" s="7"/>
     </row>
-    <row r="92" spans="1:5">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="9" t="s">
         <v>300</v>
       </c>
@@ -3426,7 +3437,7 @@
       </c>
       <c r="E92" s="7"/>
     </row>
-    <row r="93" spans="1:5">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="9" t="s">
         <v>303</v>
       </c>
@@ -3441,7 +3452,7 @@
       </c>
       <c r="E93" s="7"/>
     </row>
-    <row r="94" spans="1:5">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="9" t="s">
         <v>306</v>
       </c>
@@ -3456,7 +3467,7 @@
       </c>
       <c r="E94" s="7"/>
     </row>
-    <row r="95" spans="1:5">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="9" t="s">
         <v>309</v>
       </c>
@@ -3471,7 +3482,7 @@
       </c>
       <c r="E95" s="7"/>
     </row>
-    <row r="96" spans="1:5">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="9" t="s">
         <v>314</v>
       </c>
@@ -3486,7 +3497,7 @@
       </c>
       <c r="E96" s="7"/>
     </row>
-    <row r="97" spans="1:5">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="9" t="s">
         <v>315</v>
       </c>
@@ -3501,7 +3512,7 @@
       </c>
       <c r="E97" s="7"/>
     </row>
-    <row r="98" spans="1:5">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="9" t="s">
         <v>319</v>
       </c>
@@ -3516,7 +3527,7 @@
       </c>
       <c r="E98" s="7"/>
     </row>
-    <row r="99" spans="1:5">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="9" t="s">
         <v>321</v>
       </c>
@@ -3531,7 +3542,7 @@
       </c>
       <c r="E99" s="7"/>
     </row>
-    <row r="100" spans="1:5">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="9" t="s">
         <v>322</v>
       </c>
@@ -3546,7 +3557,7 @@
       </c>
       <c r="E100" s="7"/>
     </row>
-    <row r="101" spans="1:5" ht="30">
+    <row r="101" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A101" s="9" t="s">
         <v>323</v>
       </c>
@@ -3561,7 +3572,7 @@
       </c>
       <c r="E101" s="7"/>
     </row>
-    <row r="102" spans="1:5">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="9" t="s">
         <v>328</v>
       </c>
@@ -3576,7 +3587,7 @@
       </c>
       <c r="E102" s="7"/>
     </row>
-    <row r="103" spans="1:5">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="9" t="s">
         <v>333</v>
       </c>
@@ -3591,7 +3602,7 @@
       </c>
       <c r="E103" s="7"/>
     </row>
-    <row r="104" spans="1:5">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="9" t="s">
         <v>336</v>
       </c>
@@ -3606,7 +3617,7 @@
       </c>
       <c r="E104" s="7"/>
     </row>
-    <row r="105" spans="1:5">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="9" t="s">
         <v>337</v>
       </c>
@@ -3621,7 +3632,7 @@
       </c>
       <c r="E105" s="7"/>
     </row>
-    <row r="106" spans="1:5">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="9" t="s">
         <v>342</v>
       </c>
@@ -3636,7 +3647,7 @@
       </c>
       <c r="E106" s="7"/>
     </row>
-    <row r="107" spans="1:5">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="9" t="s">
         <v>345</v>
       </c>
@@ -3651,7 +3662,7 @@
       </c>
       <c r="E107" s="7"/>
     </row>
-    <row r="108" spans="1:5">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="9" t="s">
         <v>350</v>
       </c>
@@ -3666,7 +3677,7 @@
       </c>
       <c r="E108" s="7"/>
     </row>
-    <row r="109" spans="1:5" ht="30">
+    <row r="109" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A109" s="9" t="s">
         <v>351</v>
       </c>
@@ -3681,7 +3692,7 @@
       </c>
       <c r="E109" s="7"/>
     </row>
-    <row r="110" spans="1:5">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="9" t="s">
         <v>354</v>
       </c>
@@ -3696,7 +3707,7 @@
       </c>
       <c r="E110" s="7"/>
     </row>
-    <row r="111" spans="1:5">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="9" t="s">
         <v>357</v>
       </c>
@@ -3711,7 +3722,7 @@
       </c>
       <c r="E111" s="7"/>
     </row>
-    <row r="112" spans="1:5">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="9" t="s">
         <v>361</v>
       </c>
@@ -3726,7 +3737,7 @@
       </c>
       <c r="E112" s="7"/>
     </row>
-    <row r="113" spans="1:5">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="9" t="s">
         <v>363</v>
       </c>
@@ -3741,7 +3752,7 @@
       </c>
       <c r="E113" s="7"/>
     </row>
-    <row r="114" spans="1:5" ht="30">
+    <row r="114" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A114" s="9" t="s">
         <v>366</v>
       </c>
@@ -3756,7 +3767,7 @@
       </c>
       <c r="E114" s="7"/>
     </row>
-    <row r="115" spans="1:5">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="9" t="s">
         <v>369</v>
       </c>
@@ -3771,7 +3782,7 @@
       </c>
       <c r="E115" s="7"/>
     </row>
-    <row r="116" spans="1:5">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="9" t="s">
         <v>370</v>
       </c>
@@ -3786,7 +3797,7 @@
       </c>
       <c r="E116" s="7"/>
     </row>
-    <row r="117" spans="1:5">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" s="9" t="s">
         <v>371</v>
       </c>
@@ -3801,7 +3812,7 @@
       </c>
       <c r="E117" s="7"/>
     </row>
-    <row r="118" spans="1:5">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" s="9" t="s">
         <v>378</v>
       </c>
@@ -3816,7 +3827,7 @@
       </c>
       <c r="E118" s="7"/>
     </row>
-    <row r="119" spans="1:5">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" s="9" t="s">
         <v>381</v>
       </c>
@@ -3831,7 +3842,7 @@
       </c>
       <c r="E119" s="7"/>
     </row>
-    <row r="120" spans="1:5">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" s="9" t="s">
         <v>384</v>
       </c>
@@ -3846,7 +3857,7 @@
       </c>
       <c r="E120" s="7"/>
     </row>
-    <row r="121" spans="1:5">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="9" t="s">
         <v>387</v>
       </c>
@@ -3861,7 +3872,7 @@
       </c>
       <c r="E121" s="7"/>
     </row>
-    <row r="122" spans="1:5">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" s="7" t="s">
         <v>390</v>
       </c>
@@ -3876,7 +3887,7 @@
       </c>
       <c r="E122" s="7"/>
     </row>
-    <row r="123" spans="1:5">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" s="7" t="s">
         <v>393</v>
       </c>
@@ -3891,7 +3902,7 @@
       </c>
       <c r="E123" s="7"/>
     </row>
-    <row r="124" spans="1:5">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" s="7" t="s">
         <v>396</v>
       </c>
@@ -3906,7 +3917,7 @@
       </c>
       <c r="E124" s="7"/>
     </row>
-    <row r="125" spans="1:5">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" s="9" t="s">
         <v>399</v>
       </c>
@@ -3921,7 +3932,7 @@
       </c>
       <c r="E125" s="7"/>
     </row>
-    <row r="126" spans="1:5">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" s="7" t="s">
         <v>402</v>
       </c>
@@ -3936,7 +3947,7 @@
       </c>
       <c r="E126" s="7"/>
     </row>
-    <row r="127" spans="1:5">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" s="7" t="s">
         <v>405</v>
       </c>
@@ -3951,7 +3962,7 @@
       </c>
       <c r="E127" s="7"/>
     </row>
-    <row r="128" spans="1:5">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" s="7" t="s">
         <v>408</v>
       </c>
@@ -3966,7 +3977,7 @@
       </c>
       <c r="E128" s="7"/>
     </row>
-    <row r="129" spans="1:5">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" s="9" t="s">
         <v>411</v>
       </c>
@@ -3981,7 +3992,7 @@
       </c>
       <c r="E129" s="7"/>
     </row>
-    <row r="130" spans="1:5">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" s="9" t="s">
         <v>414</v>
       </c>
@@ -3996,7 +4007,7 @@
       </c>
       <c r="E130" s="7"/>
     </row>
-    <row r="131" spans="1:5">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" s="9" t="s">
         <v>416</v>
       </c>
@@ -4011,7 +4022,7 @@
       </c>
       <c r="E131" s="7"/>
     </row>
-    <row r="132" spans="1:5">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" s="7" t="s">
         <v>419</v>
       </c>
@@ -4026,7 +4037,7 @@
       </c>
       <c r="E132" s="7"/>
     </row>
-    <row r="133" spans="1:5">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" s="9" t="s">
         <v>422</v>
       </c>
@@ -4041,7 +4052,7 @@
       </c>
       <c r="E133" s="7"/>
     </row>
-    <row r="134" spans="1:5" ht="30">
+    <row r="134" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A134" s="7" t="s">
         <v>425</v>
       </c>
@@ -4056,7 +4067,7 @@
       </c>
       <c r="E134" s="7"/>
     </row>
-    <row r="135" spans="1:5" ht="30">
+    <row r="135" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A135" s="7" t="s">
         <v>426</v>
       </c>
@@ -4071,7 +4082,7 @@
       </c>
       <c r="E135" s="7"/>
     </row>
-    <row r="136" spans="1:5">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" s="9" t="s">
         <v>431</v>
       </c>
@@ -4086,7 +4097,7 @@
       </c>
       <c r="E136" s="7"/>
     </row>
-    <row r="137" spans="1:5">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" s="7" t="s">
         <v>434</v>
       </c>
@@ -4101,7 +4112,7 @@
       </c>
       <c r="E137" s="7"/>
     </row>
-    <row r="138" spans="1:5" ht="45">
+    <row r="138" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A138" s="7" t="s">
         <v>435</v>
       </c>
@@ -4116,7 +4127,7 @@
       </c>
       <c r="E138" s="7"/>
     </row>
-    <row r="139" spans="1:5" ht="30">
+    <row r="139" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A139" s="7" t="s">
         <v>436</v>
       </c>
@@ -4131,7 +4142,7 @@
       </c>
       <c r="E139" s="7"/>
     </row>
-    <row r="140" spans="1:5">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" s="17" t="s">
         <v>443</v>
       </c>
@@ -4146,7 +4157,7 @@
       </c>
       <c r="E140" s="7"/>
     </row>
-    <row r="141" spans="1:5">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" s="17" t="s">
         <v>446</v>
       </c>
@@ -4161,7 +4172,7 @@
       </c>
       <c r="E141" s="7"/>
     </row>
-    <row r="142" spans="1:5">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" s="17" t="s">
         <v>449</v>
       </c>
@@ -4176,7 +4187,7 @@
       </c>
       <c r="E142" s="7"/>
     </row>
-    <row r="143" spans="1:5">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" s="17" t="s">
         <v>452</v>
       </c>
@@ -4191,7 +4202,7 @@
       </c>
       <c r="E143" s="7"/>
     </row>
-    <row r="144" spans="1:5">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" s="17" t="s">
         <v>453</v>
       </c>
@@ -4206,7 +4217,7 @@
       </c>
       <c r="E144" s="7"/>
     </row>
-    <row r="145" spans="1:5">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" s="17" t="s">
         <v>458</v>
       </c>
@@ -4221,7 +4232,7 @@
       </c>
       <c r="E145" s="7"/>
     </row>
-    <row r="146" spans="1:5">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" s="17" t="s">
         <v>461</v>
       </c>
@@ -4236,7 +4247,7 @@
       </c>
       <c r="E146" s="7"/>
     </row>
-    <row r="147" spans="1:5">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" s="17" t="s">
         <v>464</v>
       </c>
@@ -4251,7 +4262,7 @@
       </c>
       <c r="E147" s="7"/>
     </row>
-    <row r="148" spans="1:5">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" s="17" t="s">
         <v>467</v>
       </c>
@@ -4266,7 +4277,7 @@
       </c>
       <c r="E148" s="7"/>
     </row>
-    <row r="149" spans="1:5">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" s="7" t="s">
         <v>470</v>
       </c>
@@ -4281,7 +4292,7 @@
       </c>
       <c r="E149" s="7"/>
     </row>
-    <row r="150" spans="1:5">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" s="7" t="s">
         <v>471</v>
       </c>
@@ -4296,7 +4307,7 @@
       </c>
       <c r="E150" s="7"/>
     </row>
-    <row r="151" spans="1:5">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" s="7" t="s">
         <v>472</v>
       </c>
@@ -4311,7 +4322,7 @@
       </c>
       <c r="E151" s="7"/>
     </row>
-    <row r="152" spans="1:5" ht="30">
+    <row r="152" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A152" s="7" t="s">
         <v>479</v>
       </c>
@@ -4326,7 +4337,7 @@
       </c>
       <c r="E152" s="7"/>
     </row>
-    <row r="153" spans="1:5" ht="45">
+    <row r="153" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A153" s="17" t="s">
         <v>482</v>
       </c>
@@ -4341,7 +4352,7 @@
       </c>
       <c r="E153" s="7"/>
     </row>
-    <row r="154" spans="1:5">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" s="17" t="s">
         <v>484</v>
       </c>
@@ -4356,7 +4367,7 @@
       </c>
       <c r="E154" s="7"/>
     </row>
-    <row r="155" spans="1:5">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" s="7" t="s">
         <v>486</v>
       </c>
@@ -4371,7 +4382,7 @@
       </c>
       <c r="E155" s="7"/>
     </row>
-    <row r="156" spans="1:5">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" s="7" t="s">
         <v>489</v>
       </c>
@@ -4386,7 +4397,7 @@
       </c>
       <c r="E156" s="7"/>
     </row>
-    <row r="157" spans="1:5">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" s="7" t="s">
         <v>492</v>
       </c>
@@ -4401,7 +4412,7 @@
       </c>
       <c r="E157" s="7"/>
     </row>
-    <row r="158" spans="1:5" ht="30">
+    <row r="158" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A158" s="7" t="s">
         <v>495</v>
       </c>
@@ -4416,7 +4427,7 @@
       </c>
       <c r="E158" s="7"/>
     </row>
-    <row r="159" spans="1:5" ht="30">
+    <row r="159" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A159" s="7" t="s">
         <v>496</v>
       </c>
@@ -4431,7 +4442,7 @@
       </c>
       <c r="E159" s="7"/>
     </row>
-    <row r="160" spans="1:5">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" s="7" t="s">
         <v>503</v>
       </c>
@@ -4446,7 +4457,7 @@
       </c>
       <c r="E160" s="7"/>
     </row>
-    <row r="161" spans="1:5">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161" s="7" t="s">
         <v>504</v>
       </c>
@@ -4461,7 +4472,7 @@
       </c>
       <c r="E161" s="7"/>
     </row>
-    <row r="162" spans="1:5">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162" s="7" t="s">
         <v>507</v>
       </c>
@@ -4476,7 +4487,7 @@
       </c>
       <c r="E162" s="7"/>
     </row>
-    <row r="163" spans="1:5">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" s="7" t="s">
         <v>512</v>
       </c>
@@ -4491,7 +4502,7 @@
       </c>
       <c r="E163" s="7"/>
     </row>
-    <row r="164" spans="1:5" ht="30">
+    <row r="164" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A164" s="7" t="s">
         <v>515</v>
       </c>
@@ -4503,6 +4514,21 @@
       </c>
       <c r="D164" s="7"/>
       <c r="E164" s="7"/>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A165" s="7" t="s">
+        <v>518</v>
+      </c>
+      <c r="B165" s="7" t="s">
+        <v>519</v>
+      </c>
+      <c r="C165" s="8" t="s">
+        <v>520</v>
+      </c>
+      <c r="D165" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E165" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -4515,14 +4541,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView topLeftCell="A10" zoomScale="80" workbookViewId="0">
       <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
@@ -4530,7 +4556,7 @@
     <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>35</v>
       </c>
@@ -4544,7 +4570,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>37</v>
       </c>
@@ -4556,7 +4582,7 @@
       </c>
       <c r="D2" s="7"/>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>38</v>
       </c>
@@ -4568,7 +4594,7 @@
       </c>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>39</v>
       </c>
@@ -4580,7 +4606,7 @@
       </c>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>40</v>
       </c>
@@ -4592,7 +4618,7 @@
       </c>
       <c r="D5" s="7"/>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>41</v>
       </c>
@@ -4604,7 +4630,7 @@
       </c>
       <c r="D6" s="7"/>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>42</v>
       </c>
@@ -4616,7 +4642,7 @@
       </c>
       <c r="D7" s="7"/>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>43</v>
       </c>
@@ -4628,7 +4654,7 @@
       </c>
       <c r="D8" s="7"/>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>44</v>
       </c>
@@ -4640,7 +4666,7 @@
       </c>
       <c r="D9" s="7"/>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>45</v>
       </c>
@@ -4652,7 +4678,7 @@
       </c>
       <c r="D10" s="7"/>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>46</v>
       </c>
@@ -4664,7 +4690,7 @@
       </c>
       <c r="D11" s="7"/>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>48</v>
       </c>
@@ -4676,7 +4702,7 @@
       </c>
       <c r="D12" s="7"/>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>49</v>
       </c>
@@ -4688,7 +4714,7 @@
       </c>
       <c r="D13" s="7"/>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>50</v>
       </c>
@@ -4700,7 +4726,7 @@
       </c>
       <c r="D14" s="7"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>51</v>
       </c>
@@ -4712,7 +4738,7 @@
       </c>
       <c r="D15" s="7"/>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>52</v>
       </c>
@@ -4724,7 +4750,7 @@
       </c>
       <c r="D16" s="7"/>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>53</v>
       </c>
@@ -4736,7 +4762,7 @@
       </c>
       <c r="D17" s="7"/>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>54</v>
       </c>
@@ -4748,7 +4774,7 @@
       </c>
       <c r="D18" s="7"/>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>55</v>
       </c>
@@ -4760,7 +4786,7 @@
       </c>
       <c r="D19" s="7"/>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>56</v>
       </c>
@@ -4772,7 +4798,7 @@
       </c>
       <c r="D20" s="7"/>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>57</v>
       </c>
@@ -4784,7 +4810,7 @@
       </c>
       <c r="D21" s="7"/>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>58</v>
       </c>
@@ -4796,7 +4822,7 @@
       </c>
       <c r="D22" s="7"/>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>59</v>
       </c>
@@ -4808,7 +4834,7 @@
       </c>
       <c r="D23" s="7"/>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>60</v>
       </c>
@@ -4820,7 +4846,7 @@
       </c>
       <c r="D24" s="7"/>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>61</v>
       </c>
@@ -4832,7 +4858,7 @@
       </c>
       <c r="D25" s="7"/>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>47</v>
       </c>
@@ -4851,14 +4877,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A19" sqref="A19:XFD19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
@@ -4866,7 +4892,7 @@
     <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>35</v>
       </c>
@@ -4880,7 +4906,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>37</v>
       </c>
@@ -4892,7 +4918,7 @@
       </c>
       <c r="D2" s="7"/>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>38</v>
       </c>
@@ -4904,7 +4930,7 @@
       </c>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>39</v>
       </c>
@@ -4916,7 +4942,7 @@
       </c>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>40</v>
       </c>
@@ -4928,7 +4954,7 @@
       </c>
       <c r="D5" s="7"/>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>41</v>
       </c>
@@ -4940,7 +4966,7 @@
       </c>
       <c r="D6" s="7"/>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>42</v>
       </c>
@@ -4952,7 +4978,7 @@
       </c>
       <c r="D7" s="7"/>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>43</v>
       </c>
@@ -4964,7 +4990,7 @@
       </c>
       <c r="D8" s="7"/>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>44</v>
       </c>
@@ -4976,7 +5002,7 @@
       </c>
       <c r="D9" s="7"/>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>45</v>
       </c>
@@ -4988,7 +5014,7 @@
       </c>
       <c r="D10" s="7"/>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>46</v>
       </c>
@@ -5000,7 +5026,7 @@
       </c>
       <c r="D11" s="7"/>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>47</v>
       </c>
@@ -5012,7 +5038,7 @@
       </c>
       <c r="D12" s="7"/>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>48</v>
       </c>
@@ -5024,7 +5050,7 @@
       </c>
       <c r="D13" s="7"/>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>49</v>
       </c>
@@ -5036,7 +5062,7 @@
       </c>
       <c r="D14" s="7"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>50</v>
       </c>
@@ -5048,7 +5074,7 @@
       </c>
       <c r="D15" s="7"/>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>51</v>
       </c>
@@ -5060,7 +5086,7 @@
       </c>
       <c r="D16" s="7"/>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>52</v>
       </c>
@@ -5072,7 +5098,7 @@
       </c>
       <c r="D17" s="7"/>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>53</v>
       </c>
@@ -5084,7 +5110,7 @@
       </c>
       <c r="D18" s="7"/>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>54</v>
       </c>
@@ -5096,7 +5122,7 @@
       </c>
       <c r="D19" s="7"/>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>55</v>
       </c>
@@ -5108,7 +5134,7 @@
       </c>
       <c r="D20" s="7"/>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>56</v>
       </c>
@@ -5120,7 +5146,7 @@
       </c>
       <c r="D21" s="7"/>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>57</v>
       </c>
@@ -5132,7 +5158,7 @@
       </c>
       <c r="D22" s="7"/>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>58</v>
       </c>
@@ -5144,7 +5170,7 @@
       </c>
       <c r="D23" s="7"/>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>59</v>
       </c>
@@ -5156,7 +5182,7 @@
       </c>
       <c r="D24" s="7"/>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>60</v>
       </c>
@@ -5168,7 +5194,7 @@
       </c>
       <c r="D25" s="7"/>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>61</v>
       </c>

</xml_diff>

<commit_message>
WAT 174 script implementation
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/WAT.xlsx
+++ b/src/test/resources/xls/WAT.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13305" windowHeight="2415"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="818" uniqueCount="521">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="823" uniqueCount="524">
   <si>
     <t>TCID</t>
   </si>
@@ -1581,13 +1581,22 @@
   </si>
   <si>
     <t>Verify that after removing a publication, the total publication count should get updated accordingly.</t>
+  </si>
+  <si>
+    <t>WAT174</t>
+  </si>
+  <si>
+    <t>WAT-1164||WAT-1165</t>
+  </si>
+  <si>
+    <t>Verify that each publication list should display first few authors followed by ‘More’ link ||Verify that each publication list should expands full authors list by clicking on ‘More’ link</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1796,7 +1805,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1828,10 +1837,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1863,7 +1871,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2039,14 +2046,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E165"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E166"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A145" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C165" sqref="C165"/>
+      <selection activeCell="C166" sqref="C166"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="30.5703125" customWidth="1" collapsed="1"/>
@@ -2055,7 +2062,7 @@
     <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2072,7 +2079,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -2087,7 +2094,7 @@
       </c>
       <c r="E2" s="4"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -2102,7 +2109,7 @@
       </c>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" s="7" t="s">
         <v>11</v>
       </c>
@@ -2117,7 +2124,7 @@
       </c>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" s="7" t="s">
         <v>12</v>
       </c>
@@ -2132,7 +2139,7 @@
       </c>
       <c r="E5" s="7"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" s="7" t="s">
         <v>14</v>
       </c>
@@ -2147,7 +2154,7 @@
       </c>
       <c r="E6" s="7"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" s="7" t="s">
         <v>17</v>
       </c>
@@ -2162,7 +2169,7 @@
       </c>
       <c r="E7" s="7"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" s="7" t="s">
         <v>20</v>
       </c>
@@ -2177,7 +2184,7 @@
       </c>
       <c r="E8" s="7"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" s="7" t="s">
         <v>22</v>
       </c>
@@ -2192,7 +2199,7 @@
       </c>
       <c r="E9" s="7"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10" s="7" t="s">
         <v>23</v>
       </c>
@@ -2207,7 +2214,7 @@
       </c>
       <c r="E10" s="7"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11" s="7" t="s">
         <v>24</v>
       </c>
@@ -2222,7 +2229,7 @@
       </c>
       <c r="E11" s="7"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12" s="7" t="s">
         <v>25</v>
       </c>
@@ -2237,7 +2244,7 @@
       </c>
       <c r="E12" s="7"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13" s="7" t="s">
         <v>62</v>
       </c>
@@ -2252,7 +2259,7 @@
       </c>
       <c r="E13" s="7"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="A14" s="7" t="s">
         <v>63</v>
       </c>
@@ -2267,7 +2274,7 @@
       </c>
       <c r="E14" s="7"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="A15" s="7" t="s">
         <v>64</v>
       </c>
@@ -2282,7 +2289,7 @@
       </c>
       <c r="E15" s="7"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="A16" s="7" t="s">
         <v>65</v>
       </c>
@@ -2297,7 +2304,7 @@
       </c>
       <c r="E16" s="7"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5">
       <c r="A17" s="7" t="s">
         <v>74</v>
       </c>
@@ -2312,7 +2319,7 @@
       </c>
       <c r="E17" s="7"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5">
       <c r="A18" s="7" t="s">
         <v>75</v>
       </c>
@@ -2327,7 +2334,7 @@
       </c>
       <c r="E18" s="7"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5">
       <c r="A19" s="7" t="s">
         <v>79</v>
       </c>
@@ -2342,7 +2349,7 @@
       </c>
       <c r="E19" s="7"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5">
       <c r="A20" s="7" t="s">
         <v>81</v>
       </c>
@@ -2357,7 +2364,7 @@
       </c>
       <c r="E20" s="7"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5">
       <c r="A21" s="7" t="s">
         <v>82</v>
       </c>
@@ -2372,7 +2379,7 @@
       </c>
       <c r="E21" s="7"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5">
       <c r="A22" s="7" t="s">
         <v>88</v>
       </c>
@@ -2387,7 +2394,7 @@
       </c>
       <c r="E22" s="7"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5">
       <c r="A23" s="7" t="s">
         <v>90</v>
       </c>
@@ -2402,7 +2409,7 @@
       </c>
       <c r="E23" s="7"/>
     </row>
-    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="30">
       <c r="A24" s="9" t="s">
         <v>94</v>
       </c>
@@ -2417,7 +2424,7 @@
       </c>
       <c r="E24" s="7"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5">
       <c r="A25" s="9" t="s">
         <v>96</v>
       </c>
@@ -2432,7 +2439,7 @@
       </c>
       <c r="E25" s="7"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5">
       <c r="A26" s="9" t="s">
         <v>98</v>
       </c>
@@ -2447,7 +2454,7 @@
       </c>
       <c r="E26" s="7"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5">
       <c r="A27" s="9" t="s">
         <v>102</v>
       </c>
@@ -2462,7 +2469,7 @@
       </c>
       <c r="E27" s="7"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5">
       <c r="A28" s="9" t="s">
         <v>105</v>
       </c>
@@ -2477,7 +2484,7 @@
       </c>
       <c r="E28" s="7"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5">
       <c r="A29" s="9" t="s">
         <v>108</v>
       </c>
@@ -2492,7 +2499,7 @@
       </c>
       <c r="E29" s="7"/>
     </row>
-    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" ht="30">
       <c r="A30" s="9" t="s">
         <v>110</v>
       </c>
@@ -2507,7 +2514,7 @@
       </c>
       <c r="E30" s="7"/>
     </row>
-    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" ht="30">
       <c r="A31" s="9" t="s">
         <v>114</v>
       </c>
@@ -2522,7 +2529,7 @@
       </c>
       <c r="E31" s="7"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5">
       <c r="A32" s="9" t="s">
         <v>119</v>
       </c>
@@ -2537,7 +2544,7 @@
       </c>
       <c r="E32" s="7"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5">
       <c r="A33" s="9" t="s">
         <v>120</v>
       </c>
@@ -2552,7 +2559,7 @@
       </c>
       <c r="E33" s="7"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5">
       <c r="A34" s="9" t="s">
         <v>125</v>
       </c>
@@ -2567,7 +2574,7 @@
       </c>
       <c r="E34" s="7"/>
     </row>
-    <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" ht="30">
       <c r="A35" s="9" t="s">
         <v>128</v>
       </c>
@@ -2582,7 +2589,7 @@
       </c>
       <c r="E35" s="7"/>
     </row>
-    <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" ht="30">
       <c r="A36" s="9" t="s">
         <v>131</v>
       </c>
@@ -2597,7 +2604,7 @@
       </c>
       <c r="E36" s="7"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5">
       <c r="A37" s="9" t="s">
         <v>134</v>
       </c>
@@ -2612,7 +2619,7 @@
       </c>
       <c r="E37" s="7"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5">
       <c r="A38" s="9" t="s">
         <v>137</v>
       </c>
@@ -2627,7 +2634,7 @@
       </c>
       <c r="E38" s="7"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5">
       <c r="A39" s="9" t="s">
         <v>140</v>
       </c>
@@ -2642,7 +2649,7 @@
       </c>
       <c r="E39" s="7"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5">
       <c r="A40" s="9" t="s">
         <v>143</v>
       </c>
@@ -2657,7 +2664,7 @@
       </c>
       <c r="E40" s="7"/>
     </row>
-    <row r="41" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" ht="30">
       <c r="A41" s="9" t="s">
         <v>145</v>
       </c>
@@ -2672,7 +2679,7 @@
       </c>
       <c r="E41" s="7"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5">
       <c r="A42" s="9" t="s">
         <v>147</v>
       </c>
@@ -2687,7 +2694,7 @@
       </c>
       <c r="E42" s="7"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5">
       <c r="A43" s="9" t="s">
         <v>150</v>
       </c>
@@ -2702,7 +2709,7 @@
       </c>
       <c r="E43" s="7"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5">
       <c r="A44" s="9" t="s">
         <v>153</v>
       </c>
@@ -2717,7 +2724,7 @@
       </c>
       <c r="E44" s="7"/>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5">
       <c r="A45" s="9" t="s">
         <v>155</v>
       </c>
@@ -2732,7 +2739,7 @@
       </c>
       <c r="E45" s="7"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5">
       <c r="A46" s="12" t="s">
         <v>158</v>
       </c>
@@ -2747,7 +2754,7 @@
       </c>
       <c r="E46" s="7"/>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5">
       <c r="A47" s="12" t="s">
         <v>159</v>
       </c>
@@ -2762,7 +2769,7 @@
       </c>
       <c r="E47" s="7"/>
     </row>
-    <row r="48" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" ht="30">
       <c r="A48" s="12" t="s">
         <v>160</v>
       </c>
@@ -2777,7 +2784,7 @@
       </c>
       <c r="E48" s="7"/>
     </row>
-    <row r="49" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" ht="30">
       <c r="A49" s="12" t="s">
         <v>161</v>
       </c>
@@ -2792,7 +2799,7 @@
       </c>
       <c r="E49" s="7"/>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5">
       <c r="A50" s="12" t="s">
         <v>164</v>
       </c>
@@ -2807,7 +2814,7 @@
       </c>
       <c r="E50" s="7"/>
     </row>
-    <row r="51" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" ht="30">
       <c r="A51" s="9" t="s">
         <v>173</v>
       </c>
@@ -2822,7 +2829,7 @@
       </c>
       <c r="E51" s="7"/>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5">
       <c r="A52" s="9" t="s">
         <v>174</v>
       </c>
@@ -2837,7 +2844,7 @@
       </c>
       <c r="E52" s="7"/>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5">
       <c r="A53" s="9" t="s">
         <v>179</v>
       </c>
@@ -2852,7 +2859,7 @@
       </c>
       <c r="E53" s="7"/>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5">
       <c r="A54" s="9" t="s">
         <v>180</v>
       </c>
@@ -2867,7 +2874,7 @@
       </c>
       <c r="E54" s="7"/>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5">
       <c r="A55" s="9" t="s">
         <v>185</v>
       </c>
@@ -2882,7 +2889,7 @@
       </c>
       <c r="E55" s="7"/>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5">
       <c r="A56" s="9" t="s">
         <v>188</v>
       </c>
@@ -2897,7 +2904,7 @@
       </c>
       <c r="E56" s="7"/>
     </row>
-    <row r="57" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" ht="30">
       <c r="A57" s="9" t="s">
         <v>191</v>
       </c>
@@ -2912,7 +2919,7 @@
       </c>
       <c r="E57" s="7"/>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5">
       <c r="A58" s="9" t="s">
         <v>194</v>
       </c>
@@ -2927,7 +2934,7 @@
       </c>
       <c r="E58" s="7"/>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5">
       <c r="A59" s="7" t="s">
         <v>196</v>
       </c>
@@ -2942,7 +2949,7 @@
       </c>
       <c r="E59" s="7"/>
     </row>
-    <row r="60" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" ht="45">
       <c r="A60" s="7" t="s">
         <v>199</v>
       </c>
@@ -2957,7 +2964,7 @@
       </c>
       <c r="E60" s="7"/>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5">
       <c r="A61" s="9" t="s">
         <v>202</v>
       </c>
@@ -2972,7 +2979,7 @@
       </c>
       <c r="E61" s="7"/>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5">
       <c r="A62" s="9" t="s">
         <v>204</v>
       </c>
@@ -2987,7 +2994,7 @@
       </c>
       <c r="E62" s="7"/>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5">
       <c r="A63" s="9" t="s">
         <v>206</v>
       </c>
@@ -3002,7 +3009,7 @@
       </c>
       <c r="E63" s="7"/>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5">
       <c r="A64" s="9" t="s">
         <v>208</v>
       </c>
@@ -3017,7 +3024,7 @@
       </c>
       <c r="E64" s="7"/>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5">
       <c r="A65" s="9" t="s">
         <v>217</v>
       </c>
@@ -3032,7 +3039,7 @@
       </c>
       <c r="E65" s="7"/>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5">
       <c r="A66" s="9" t="s">
         <v>218</v>
       </c>
@@ -3047,7 +3054,7 @@
       </c>
       <c r="E66" s="7"/>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5">
       <c r="A67" s="9" t="s">
         <v>223</v>
       </c>
@@ -3062,7 +3069,7 @@
       </c>
       <c r="E67" s="7"/>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5">
       <c r="A68" s="9" t="s">
         <v>224</v>
       </c>
@@ -3077,7 +3084,7 @@
       </c>
       <c r="E68" s="7"/>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5">
       <c r="A69" s="9" t="s">
         <v>225</v>
       </c>
@@ -3092,7 +3099,7 @@
       </c>
       <c r="E69" s="7"/>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5">
       <c r="A70" s="9" t="s">
         <v>226</v>
       </c>
@@ -3107,7 +3114,7 @@
       </c>
       <c r="E70" s="7"/>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5">
       <c r="A71" s="9" t="s">
         <v>233</v>
       </c>
@@ -3122,7 +3129,7 @@
       </c>
       <c r="E71" s="7"/>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5">
       <c r="A72" s="9" t="s">
         <v>237</v>
       </c>
@@ -3137,7 +3144,7 @@
       </c>
       <c r="E72" s="7"/>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5">
       <c r="A73" s="9" t="s">
         <v>239</v>
       </c>
@@ -3152,7 +3159,7 @@
       </c>
       <c r="E73" s="7"/>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5">
       <c r="A74" s="9" t="s">
         <v>243</v>
       </c>
@@ -3167,7 +3174,7 @@
       </c>
       <c r="E74" s="7"/>
     </row>
-    <row r="75" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" ht="30">
       <c r="A75" s="9" t="s">
         <v>245</v>
       </c>
@@ -3182,7 +3189,7 @@
       </c>
       <c r="E75" s="7"/>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5">
       <c r="A76" s="9" t="s">
         <v>248</v>
       </c>
@@ -3197,7 +3204,7 @@
       </c>
       <c r="E76" s="7"/>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5">
       <c r="A77" s="9" t="s">
         <v>256</v>
       </c>
@@ -3212,7 +3219,7 @@
       </c>
       <c r="E77" s="7"/>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5">
       <c r="A78" s="9" t="s">
         <v>257</v>
       </c>
@@ -3227,7 +3234,7 @@
       </c>
       <c r="E78" s="7"/>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5">
       <c r="A79" s="9" t="s">
         <v>261</v>
       </c>
@@ -3242,7 +3249,7 @@
       </c>
       <c r="E79" s="7"/>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5">
       <c r="A80" s="9" t="s">
         <v>264</v>
       </c>
@@ -3257,7 +3264,7 @@
       </c>
       <c r="E80" s="7"/>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5">
       <c r="A81" s="9" t="s">
         <v>267</v>
       </c>
@@ -3272,7 +3279,7 @@
       </c>
       <c r="E81" s="7"/>
     </row>
-    <row r="82" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" ht="30">
       <c r="A82" s="9" t="s">
         <v>269</v>
       </c>
@@ -3287,7 +3294,7 @@
       </c>
       <c r="E82" s="7"/>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5">
       <c r="A83" s="9" t="s">
         <v>274</v>
       </c>
@@ -3302,7 +3309,7 @@
       </c>
       <c r="E83" s="7"/>
     </row>
-    <row r="84" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" ht="30">
       <c r="A84" s="9" t="s">
         <v>277</v>
       </c>
@@ -3317,7 +3324,7 @@
       </c>
       <c r="E84" s="7"/>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5">
       <c r="A85" s="9" t="s">
         <v>279</v>
       </c>
@@ -3332,7 +3339,7 @@
       </c>
       <c r="E85" s="7"/>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5">
       <c r="A86" s="9" t="s">
         <v>282</v>
       </c>
@@ -3347,7 +3354,7 @@
       </c>
       <c r="E86" s="7"/>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5">
       <c r="A87" s="9" t="s">
         <v>285</v>
       </c>
@@ -3362,7 +3369,7 @@
       </c>
       <c r="E87" s="7"/>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5">
       <c r="A88" s="9" t="s">
         <v>288</v>
       </c>
@@ -3377,7 +3384,7 @@
       </c>
       <c r="E88" s="7"/>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5">
       <c r="A89" s="9" t="s">
         <v>291</v>
       </c>
@@ -3392,7 +3399,7 @@
       </c>
       <c r="E89" s="7"/>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5">
       <c r="A90" s="9" t="s">
         <v>294</v>
       </c>
@@ -3407,7 +3414,7 @@
       </c>
       <c r="E90" s="7"/>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5">
       <c r="A91" s="9" t="s">
         <v>297</v>
       </c>
@@ -3422,7 +3429,7 @@
       </c>
       <c r="E91" s="7"/>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5">
       <c r="A92" s="9" t="s">
         <v>300</v>
       </c>
@@ -3437,7 +3444,7 @@
       </c>
       <c r="E92" s="7"/>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5">
       <c r="A93" s="9" t="s">
         <v>303</v>
       </c>
@@ -3452,7 +3459,7 @@
       </c>
       <c r="E93" s="7"/>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5">
       <c r="A94" s="9" t="s">
         <v>306</v>
       </c>
@@ -3467,7 +3474,7 @@
       </c>
       <c r="E94" s="7"/>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5">
       <c r="A95" s="9" t="s">
         <v>309</v>
       </c>
@@ -3482,7 +3489,7 @@
       </c>
       <c r="E95" s="7"/>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5">
       <c r="A96" s="9" t="s">
         <v>314</v>
       </c>
@@ -3497,7 +3504,7 @@
       </c>
       <c r="E96" s="7"/>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5">
       <c r="A97" s="9" t="s">
         <v>315</v>
       </c>
@@ -3512,7 +3519,7 @@
       </c>
       <c r="E97" s="7"/>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5">
       <c r="A98" s="9" t="s">
         <v>319</v>
       </c>
@@ -3527,7 +3534,7 @@
       </c>
       <c r="E98" s="7"/>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5">
       <c r="A99" s="9" t="s">
         <v>321</v>
       </c>
@@ -3542,7 +3549,7 @@
       </c>
       <c r="E99" s="7"/>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5">
       <c r="A100" s="9" t="s">
         <v>322</v>
       </c>
@@ -3557,7 +3564,7 @@
       </c>
       <c r="E100" s="7"/>
     </row>
-    <row r="101" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" ht="30">
       <c r="A101" s="9" t="s">
         <v>323</v>
       </c>
@@ -3572,7 +3579,7 @@
       </c>
       <c r="E101" s="7"/>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5">
       <c r="A102" s="9" t="s">
         <v>328</v>
       </c>
@@ -3587,7 +3594,7 @@
       </c>
       <c r="E102" s="7"/>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5">
       <c r="A103" s="9" t="s">
         <v>333</v>
       </c>
@@ -3602,7 +3609,7 @@
       </c>
       <c r="E103" s="7"/>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5">
       <c r="A104" s="9" t="s">
         <v>336</v>
       </c>
@@ -3617,7 +3624,7 @@
       </c>
       <c r="E104" s="7"/>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5">
       <c r="A105" s="9" t="s">
         <v>337</v>
       </c>
@@ -3632,7 +3639,7 @@
       </c>
       <c r="E105" s="7"/>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5">
       <c r="A106" s="9" t="s">
         <v>342</v>
       </c>
@@ -3647,7 +3654,7 @@
       </c>
       <c r="E106" s="7"/>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5">
       <c r="A107" s="9" t="s">
         <v>345</v>
       </c>
@@ -3662,7 +3669,7 @@
       </c>
       <c r="E107" s="7"/>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5">
       <c r="A108" s="9" t="s">
         <v>350</v>
       </c>
@@ -3677,7 +3684,7 @@
       </c>
       <c r="E108" s="7"/>
     </row>
-    <row r="109" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" ht="30">
       <c r="A109" s="9" t="s">
         <v>351</v>
       </c>
@@ -3692,7 +3699,7 @@
       </c>
       <c r="E109" s="7"/>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5">
       <c r="A110" s="9" t="s">
         <v>354</v>
       </c>
@@ -3707,7 +3714,7 @@
       </c>
       <c r="E110" s="7"/>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5">
       <c r="A111" s="9" t="s">
         <v>357</v>
       </c>
@@ -3722,7 +3729,7 @@
       </c>
       <c r="E111" s="7"/>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5">
       <c r="A112" s="9" t="s">
         <v>361</v>
       </c>
@@ -3737,7 +3744,7 @@
       </c>
       <c r="E112" s="7"/>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5">
       <c r="A113" s="9" t="s">
         <v>363</v>
       </c>
@@ -3752,7 +3759,7 @@
       </c>
       <c r="E113" s="7"/>
     </row>
-    <row r="114" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" ht="30">
       <c r="A114" s="9" t="s">
         <v>366</v>
       </c>
@@ -3767,7 +3774,7 @@
       </c>
       <c r="E114" s="7"/>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5">
       <c r="A115" s="9" t="s">
         <v>369</v>
       </c>
@@ -3782,7 +3789,7 @@
       </c>
       <c r="E115" s="7"/>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5">
       <c r="A116" s="9" t="s">
         <v>370</v>
       </c>
@@ -3797,7 +3804,7 @@
       </c>
       <c r="E116" s="7"/>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5">
       <c r="A117" s="9" t="s">
         <v>371</v>
       </c>
@@ -3812,7 +3819,7 @@
       </c>
       <c r="E117" s="7"/>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5">
       <c r="A118" s="9" t="s">
         <v>378</v>
       </c>
@@ -3827,7 +3834,7 @@
       </c>
       <c r="E118" s="7"/>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5">
       <c r="A119" s="9" t="s">
         <v>381</v>
       </c>
@@ -3842,7 +3849,7 @@
       </c>
       <c r="E119" s="7"/>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5">
       <c r="A120" s="9" t="s">
         <v>384</v>
       </c>
@@ -3857,7 +3864,7 @@
       </c>
       <c r="E120" s="7"/>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5">
       <c r="A121" s="9" t="s">
         <v>387</v>
       </c>
@@ -3872,7 +3879,7 @@
       </c>
       <c r="E121" s="7"/>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5">
       <c r="A122" s="7" t="s">
         <v>390</v>
       </c>
@@ -3887,7 +3894,7 @@
       </c>
       <c r="E122" s="7"/>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5">
       <c r="A123" s="7" t="s">
         <v>393</v>
       </c>
@@ -3902,7 +3909,7 @@
       </c>
       <c r="E123" s="7"/>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5">
       <c r="A124" s="7" t="s">
         <v>396</v>
       </c>
@@ -3917,7 +3924,7 @@
       </c>
       <c r="E124" s="7"/>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5">
       <c r="A125" s="9" t="s">
         <v>399</v>
       </c>
@@ -3932,7 +3939,7 @@
       </c>
       <c r="E125" s="7"/>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5">
       <c r="A126" s="7" t="s">
         <v>402</v>
       </c>
@@ -3947,7 +3954,7 @@
       </c>
       <c r="E126" s="7"/>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5">
       <c r="A127" s="7" t="s">
         <v>405</v>
       </c>
@@ -3962,7 +3969,7 @@
       </c>
       <c r="E127" s="7"/>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5">
       <c r="A128" s="7" t="s">
         <v>408</v>
       </c>
@@ -3977,7 +3984,7 @@
       </c>
       <c r="E128" s="7"/>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5">
       <c r="A129" s="9" t="s">
         <v>411</v>
       </c>
@@ -3992,7 +3999,7 @@
       </c>
       <c r="E129" s="7"/>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5">
       <c r="A130" s="9" t="s">
         <v>414</v>
       </c>
@@ -4007,7 +4014,7 @@
       </c>
       <c r="E130" s="7"/>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5">
       <c r="A131" s="9" t="s">
         <v>416</v>
       </c>
@@ -4022,7 +4029,7 @@
       </c>
       <c r="E131" s="7"/>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5">
       <c r="A132" s="7" t="s">
         <v>419</v>
       </c>
@@ -4037,7 +4044,7 @@
       </c>
       <c r="E132" s="7"/>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5">
       <c r="A133" s="9" t="s">
         <v>422</v>
       </c>
@@ -4052,7 +4059,7 @@
       </c>
       <c r="E133" s="7"/>
     </row>
-    <row r="134" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5" ht="30">
       <c r="A134" s="7" t="s">
         <v>425</v>
       </c>
@@ -4067,7 +4074,7 @@
       </c>
       <c r="E134" s="7"/>
     </row>
-    <row r="135" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5" ht="30">
       <c r="A135" s="7" t="s">
         <v>426</v>
       </c>
@@ -4082,7 +4089,7 @@
       </c>
       <c r="E135" s="7"/>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5">
       <c r="A136" s="9" t="s">
         <v>431</v>
       </c>
@@ -4097,7 +4104,7 @@
       </c>
       <c r="E136" s="7"/>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5">
       <c r="A137" s="7" t="s">
         <v>434</v>
       </c>
@@ -4112,7 +4119,7 @@
       </c>
       <c r="E137" s="7"/>
     </row>
-    <row r="138" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" ht="45">
       <c r="A138" s="7" t="s">
         <v>435</v>
       </c>
@@ -4127,7 +4134,7 @@
       </c>
       <c r="E138" s="7"/>
     </row>
-    <row r="139" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5" ht="30">
       <c r="A139" s="7" t="s">
         <v>436</v>
       </c>
@@ -4142,7 +4149,7 @@
       </c>
       <c r="E139" s="7"/>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5">
       <c r="A140" s="17" t="s">
         <v>443</v>
       </c>
@@ -4157,7 +4164,7 @@
       </c>
       <c r="E140" s="7"/>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5">
       <c r="A141" s="17" t="s">
         <v>446</v>
       </c>
@@ -4172,7 +4179,7 @@
       </c>
       <c r="E141" s="7"/>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:5">
       <c r="A142" s="17" t="s">
         <v>449</v>
       </c>
@@ -4187,7 +4194,7 @@
       </c>
       <c r="E142" s="7"/>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:5">
       <c r="A143" s="17" t="s">
         <v>452</v>
       </c>
@@ -4202,7 +4209,7 @@
       </c>
       <c r="E143" s="7"/>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:5">
       <c r="A144" s="17" t="s">
         <v>453</v>
       </c>
@@ -4217,7 +4224,7 @@
       </c>
       <c r="E144" s="7"/>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:5">
       <c r="A145" s="17" t="s">
         <v>458</v>
       </c>
@@ -4232,7 +4239,7 @@
       </c>
       <c r="E145" s="7"/>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:5">
       <c r="A146" s="17" t="s">
         <v>461</v>
       </c>
@@ -4247,7 +4254,7 @@
       </c>
       <c r="E146" s="7"/>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:5">
       <c r="A147" s="17" t="s">
         <v>464</v>
       </c>
@@ -4262,7 +4269,7 @@
       </c>
       <c r="E147" s="7"/>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:5">
       <c r="A148" s="17" t="s">
         <v>467</v>
       </c>
@@ -4277,7 +4284,7 @@
       </c>
       <c r="E148" s="7"/>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:5">
       <c r="A149" s="7" t="s">
         <v>470</v>
       </c>
@@ -4292,7 +4299,7 @@
       </c>
       <c r="E149" s="7"/>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:5">
       <c r="A150" s="7" t="s">
         <v>471</v>
       </c>
@@ -4307,7 +4314,7 @@
       </c>
       <c r="E150" s="7"/>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:5">
       <c r="A151" s="7" t="s">
         <v>472</v>
       </c>
@@ -4322,7 +4329,7 @@
       </c>
       <c r="E151" s="7"/>
     </row>
-    <row r="152" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:5" ht="30">
       <c r="A152" s="7" t="s">
         <v>479</v>
       </c>
@@ -4337,7 +4344,7 @@
       </c>
       <c r="E152" s="7"/>
     </row>
-    <row r="153" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:5" ht="45">
       <c r="A153" s="17" t="s">
         <v>482</v>
       </c>
@@ -4352,7 +4359,7 @@
       </c>
       <c r="E153" s="7"/>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:5">
       <c r="A154" s="17" t="s">
         <v>484</v>
       </c>
@@ -4367,7 +4374,7 @@
       </c>
       <c r="E154" s="7"/>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:5">
       <c r="A155" s="7" t="s">
         <v>486</v>
       </c>
@@ -4382,7 +4389,7 @@
       </c>
       <c r="E155" s="7"/>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:5">
       <c r="A156" s="7" t="s">
         <v>489</v>
       </c>
@@ -4397,7 +4404,7 @@
       </c>
       <c r="E156" s="7"/>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:5">
       <c r="A157" s="7" t="s">
         <v>492</v>
       </c>
@@ -4412,7 +4419,7 @@
       </c>
       <c r="E157" s="7"/>
     </row>
-    <row r="158" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:5" ht="30">
       <c r="A158" s="7" t="s">
         <v>495</v>
       </c>
@@ -4427,7 +4434,7 @@
       </c>
       <c r="E158" s="7"/>
     </row>
-    <row r="159" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:5" ht="30">
       <c r="A159" s="7" t="s">
         <v>496</v>
       </c>
@@ -4442,7 +4449,7 @@
       </c>
       <c r="E159" s="7"/>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:5">
       <c r="A160" s="7" t="s">
         <v>503</v>
       </c>
@@ -4457,7 +4464,7 @@
       </c>
       <c r="E160" s="7"/>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:5">
       <c r="A161" s="7" t="s">
         <v>504</v>
       </c>
@@ -4472,7 +4479,7 @@
       </c>
       <c r="E161" s="7"/>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:5">
       <c r="A162" s="7" t="s">
         <v>507</v>
       </c>
@@ -4487,7 +4494,7 @@
       </c>
       <c r="E162" s="7"/>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:5">
       <c r="A163" s="7" t="s">
         <v>512</v>
       </c>
@@ -4502,7 +4509,7 @@
       </c>
       <c r="E163" s="7"/>
     </row>
-    <row r="164" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:5" ht="30">
       <c r="A164" s="7" t="s">
         <v>515</v>
       </c>
@@ -4512,10 +4519,12 @@
       <c r="C164" s="8" t="s">
         <v>516</v>
       </c>
-      <c r="D164" s="7"/>
+      <c r="D164" s="7" t="s">
+        <v>5</v>
+      </c>
       <c r="E164" s="7"/>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:5">
       <c r="A165" s="7" t="s">
         <v>518</v>
       </c>
@@ -4529,6 +4538,21 @@
         <v>5</v>
       </c>
       <c r="E165" s="7"/>
+    </row>
+    <row r="166" spans="1:5" ht="30">
+      <c r="A166" s="7" t="s">
+        <v>521</v>
+      </c>
+      <c r="B166" s="7" t="s">
+        <v>522</v>
+      </c>
+      <c r="C166" s="8" t="s">
+        <v>523</v>
+      </c>
+      <c r="D166" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E166" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -4541,14 +4565,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView topLeftCell="A10" zoomScale="80" workbookViewId="0">
       <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
@@ -4556,7 +4580,7 @@
     <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="10" t="s">
         <v>35</v>
       </c>
@@ -4570,7 +4594,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="7" t="s">
         <v>37</v>
       </c>
@@ -4582,7 +4606,7 @@
       </c>
       <c r="D2" s="7"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="7" t="s">
         <v>38</v>
       </c>
@@ -4594,7 +4618,7 @@
       </c>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="7" t="s">
         <v>39</v>
       </c>
@@ -4606,7 +4630,7 @@
       </c>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" s="7" t="s">
         <v>40</v>
       </c>
@@ -4618,7 +4642,7 @@
       </c>
       <c r="D5" s="7"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" s="7" t="s">
         <v>41</v>
       </c>
@@ -4630,7 +4654,7 @@
       </c>
       <c r="D6" s="7"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="7" t="s">
         <v>42</v>
       </c>
@@ -4642,7 +4666,7 @@
       </c>
       <c r="D7" s="7"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="7" t="s">
         <v>43</v>
       </c>
@@ -4654,7 +4678,7 @@
       </c>
       <c r="D8" s="7"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="7" t="s">
         <v>44</v>
       </c>
@@ -4666,7 +4690,7 @@
       </c>
       <c r="D9" s="7"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="7" t="s">
         <v>45</v>
       </c>
@@ -4678,7 +4702,7 @@
       </c>
       <c r="D10" s="7"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11" s="7" t="s">
         <v>46</v>
       </c>
@@ -4690,7 +4714,7 @@
       </c>
       <c r="D11" s="7"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="A12" s="7" t="s">
         <v>48</v>
       </c>
@@ -4702,7 +4726,7 @@
       </c>
       <c r="D12" s="7"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="A13" s="7" t="s">
         <v>49</v>
       </c>
@@ -4714,7 +4738,7 @@
       </c>
       <c r="D13" s="7"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="A14" s="7" t="s">
         <v>50</v>
       </c>
@@ -4726,7 +4750,7 @@
       </c>
       <c r="D14" s="7"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="A15" s="7" t="s">
         <v>51</v>
       </c>
@@ -4738,7 +4762,7 @@
       </c>
       <c r="D15" s="7"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="A16" s="7" t="s">
         <v>52</v>
       </c>
@@ -4750,7 +4774,7 @@
       </c>
       <c r="D16" s="7"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4">
       <c r="A17" s="7" t="s">
         <v>53</v>
       </c>
@@ -4762,7 +4786,7 @@
       </c>
       <c r="D17" s="7"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4">
       <c r="A18" s="7" t="s">
         <v>54</v>
       </c>
@@ -4774,7 +4798,7 @@
       </c>
       <c r="D18" s="7"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4">
       <c r="A19" s="7" t="s">
         <v>55</v>
       </c>
@@ -4786,7 +4810,7 @@
       </c>
       <c r="D19" s="7"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4">
       <c r="A20" s="7" t="s">
         <v>56</v>
       </c>
@@ -4798,7 +4822,7 @@
       </c>
       <c r="D20" s="7"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4">
       <c r="A21" s="7" t="s">
         <v>57</v>
       </c>
@@ -4810,7 +4834,7 @@
       </c>
       <c r="D21" s="7"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4">
       <c r="A22" s="7" t="s">
         <v>58</v>
       </c>
@@ -4822,7 +4846,7 @@
       </c>
       <c r="D22" s="7"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4">
       <c r="A23" s="7" t="s">
         <v>59</v>
       </c>
@@ -4834,7 +4858,7 @@
       </c>
       <c r="D23" s="7"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4">
       <c r="A24" s="7" t="s">
         <v>60</v>
       </c>
@@ -4846,7 +4870,7 @@
       </c>
       <c r="D24" s="7"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4">
       <c r="A25" s="7" t="s">
         <v>61</v>
       </c>
@@ -4858,7 +4882,7 @@
       </c>
       <c r="D25" s="7"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4">
       <c r="A26" s="7" t="s">
         <v>47</v>
       </c>
@@ -4877,14 +4901,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A19" sqref="A19:XFD19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
@@ -4892,7 +4916,7 @@
     <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="10" t="s">
         <v>35</v>
       </c>
@@ -4906,7 +4930,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="7" t="s">
         <v>37</v>
       </c>
@@ -4918,7 +4942,7 @@
       </c>
       <c r="D2" s="7"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="7" t="s">
         <v>38</v>
       </c>
@@ -4930,7 +4954,7 @@
       </c>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="7" t="s">
         <v>39</v>
       </c>
@@ -4942,7 +4966,7 @@
       </c>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" s="7" t="s">
         <v>40</v>
       </c>
@@ -4954,7 +4978,7 @@
       </c>
       <c r="D5" s="7"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" s="7" t="s">
         <v>41</v>
       </c>
@@ -4966,7 +4990,7 @@
       </c>
       <c r="D6" s="7"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="7" t="s">
         <v>42</v>
       </c>
@@ -4978,7 +5002,7 @@
       </c>
       <c r="D7" s="7"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="7" t="s">
         <v>43</v>
       </c>
@@ -4990,7 +5014,7 @@
       </c>
       <c r="D8" s="7"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="7" t="s">
         <v>44</v>
       </c>
@@ -5002,7 +5026,7 @@
       </c>
       <c r="D9" s="7"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="7" t="s">
         <v>45</v>
       </c>
@@ -5014,7 +5038,7 @@
       </c>
       <c r="D10" s="7"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11" s="7" t="s">
         <v>46</v>
       </c>
@@ -5026,7 +5050,7 @@
       </c>
       <c r="D11" s="7"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="A12" s="7" t="s">
         <v>47</v>
       </c>
@@ -5038,7 +5062,7 @@
       </c>
       <c r="D12" s="7"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="A13" s="7" t="s">
         <v>48</v>
       </c>
@@ -5050,7 +5074,7 @@
       </c>
       <c r="D13" s="7"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="A14" s="7" t="s">
         <v>49</v>
       </c>
@@ -5062,7 +5086,7 @@
       </c>
       <c r="D14" s="7"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="A15" s="7" t="s">
         <v>50</v>
       </c>
@@ -5074,7 +5098,7 @@
       </c>
       <c r="D15" s="7"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="A16" s="7" t="s">
         <v>51</v>
       </c>
@@ -5086,7 +5110,7 @@
       </c>
       <c r="D16" s="7"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4">
       <c r="A17" s="7" t="s">
         <v>52</v>
       </c>
@@ -5098,7 +5122,7 @@
       </c>
       <c r="D17" s="7"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4">
       <c r="A18" s="7" t="s">
         <v>53</v>
       </c>
@@ -5110,7 +5134,7 @@
       </c>
       <c r="D18" s="7"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4">
       <c r="A19" s="7" t="s">
         <v>54</v>
       </c>
@@ -5122,7 +5146,7 @@
       </c>
       <c r="D19" s="7"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4">
       <c r="A20" s="7" t="s">
         <v>55</v>
       </c>
@@ -5134,7 +5158,7 @@
       </c>
       <c r="D20" s="7"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4">
       <c r="A21" s="7" t="s">
         <v>56</v>
       </c>
@@ -5146,7 +5170,7 @@
       </c>
       <c r="D21" s="7"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4">
       <c r="A22" s="7" t="s">
         <v>57</v>
       </c>
@@ -5158,7 +5182,7 @@
       </c>
       <c r="D22" s="7"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4">
       <c r="A23" s="7" t="s">
         <v>58</v>
       </c>
@@ -5170,7 +5194,7 @@
       </c>
       <c r="D23" s="7"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4">
       <c r="A24" s="7" t="s">
         <v>59</v>
       </c>
@@ -5182,7 +5206,7 @@
       </c>
       <c r="D24" s="7"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4">
       <c r="A25" s="7" t="s">
         <v>60</v>
       </c>
@@ -5194,7 +5218,7 @@
       </c>
       <c r="D25" s="7"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4">
       <c r="A26" s="7" t="s">
         <v>61</v>
       </c>

</xml_diff>

<commit_message>
WAT 175,176 scripts implementation
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/WAT.xlsx
+++ b/src/test/resources/xls/WAT.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="823" uniqueCount="524">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="831" uniqueCount="530">
   <si>
     <t>TCID</t>
   </si>
@@ -1590,6 +1590,24 @@
   </si>
   <si>
     <t>Verify that each publication list should display first few authors followed by ‘More’ link ||Verify that each publication list should expands full authors list by clicking on ‘More’ link</t>
+  </si>
+  <si>
+    <t>WAT-1166</t>
+  </si>
+  <si>
+    <t>WAT175</t>
+  </si>
+  <si>
+    <t>Verify that each publication list display full author list by clicking on ‘More’ link and More link turns into ‘Less’</t>
+  </si>
+  <si>
+    <t>WAT176</t>
+  </si>
+  <si>
+    <t>WAT-1167</t>
+  </si>
+  <si>
+    <t>Verify that each publication returns to original state by clicking on ‘Less’ link</t>
   </si>
 </sst>
 </file>
@@ -2047,10 +2065,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E166"/>
+  <dimension ref="A1:E168"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A145" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C166" sqref="C166"/>
+    <sheetView tabSelected="1" topLeftCell="A156" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C175" sqref="C175"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4553,6 +4571,36 @@
         <v>5</v>
       </c>
       <c r="E166" s="7"/>
+    </row>
+    <row r="167" spans="1:5">
+      <c r="A167" s="7" t="s">
+        <v>525</v>
+      </c>
+      <c r="B167" s="7" t="s">
+        <v>524</v>
+      </c>
+      <c r="C167" s="8" t="s">
+        <v>526</v>
+      </c>
+      <c r="D167" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E167" s="7"/>
+    </row>
+    <row r="168" spans="1:5">
+      <c r="A168" s="7" t="s">
+        <v>527</v>
+      </c>
+      <c r="B168" s="7" t="s">
+        <v>528</v>
+      </c>
+      <c r="C168" s="8" t="s">
+        <v>529</v>
+      </c>
+      <c r="D168" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E168" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Adds WAT-142 test script and related changes along with minor changes to the other scripts
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/WAT.xlsx
+++ b/src/test/resources/xls/WAT.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13305" windowHeight="2415"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="843" uniqueCount="539">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="847" uniqueCount="541">
   <si>
     <t>TCID</t>
   </si>
@@ -1635,13 +1635,19 @@
   </si>
   <si>
     <t>Verify that System must display a maximum of 5 organization</t>
+  </si>
+  <si>
+    <t>WAT142</t>
+  </si>
+  <si>
+    <t>Verify that when a user clicks on curate button each Publication should have a "X" symbol, which upon clicking will remove the Publication from the combined author publication list.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1850,7 +1856,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1882,9 +1888,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1916,6 +1923,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2091,14 +2099,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E171"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E172"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A149" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H164" sqref="H164"/>
+      <selection activeCell="C175" sqref="C175"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="30.5703125" customWidth="1" collapsed="1"/>
@@ -2107,7 +2115,7 @@
     <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2124,7 +2132,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -2139,7 +2147,7 @@
       </c>
       <c r="E2" s="4"/>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -2154,7 +2162,7 @@
       </c>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>11</v>
       </c>
@@ -2169,7 +2177,7 @@
       </c>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>12</v>
       </c>
@@ -2184,7 +2192,7 @@
       </c>
       <c r="E5" s="7"/>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>14</v>
       </c>
@@ -2199,7 +2207,7 @@
       </c>
       <c r="E6" s="7"/>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>17</v>
       </c>
@@ -2214,7 +2222,7 @@
       </c>
       <c r="E7" s="7"/>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>20</v>
       </c>
@@ -2229,7 +2237,7 @@
       </c>
       <c r="E8" s="7"/>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>22</v>
       </c>
@@ -2244,7 +2252,7 @@
       </c>
       <c r="E9" s="7"/>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>23</v>
       </c>
@@ -2259,7 +2267,7 @@
       </c>
       <c r="E10" s="7"/>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>24</v>
       </c>
@@ -2274,7 +2282,7 @@
       </c>
       <c r="E11" s="7"/>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>25</v>
       </c>
@@ -2289,7 +2297,7 @@
       </c>
       <c r="E12" s="7"/>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>62</v>
       </c>
@@ -2304,7 +2312,7 @@
       </c>
       <c r="E13" s="7"/>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>63</v>
       </c>
@@ -2319,7 +2327,7 @@
       </c>
       <c r="E14" s="7"/>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>64</v>
       </c>
@@ -2334,7 +2342,7 @@
       </c>
       <c r="E15" s="7"/>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>65</v>
       </c>
@@ -2349,7 +2357,7 @@
       </c>
       <c r="E16" s="7"/>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>74</v>
       </c>
@@ -2364,7 +2372,7 @@
       </c>
       <c r="E17" s="7"/>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>75</v>
       </c>
@@ -2379,7 +2387,7 @@
       </c>
       <c r="E18" s="7"/>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>79</v>
       </c>
@@ -2394,7 +2402,7 @@
       </c>
       <c r="E19" s="7"/>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>81</v>
       </c>
@@ -2409,7 +2417,7 @@
       </c>
       <c r="E20" s="7"/>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>82</v>
       </c>
@@ -2424,7 +2432,7 @@
       </c>
       <c r="E21" s="7"/>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>88</v>
       </c>
@@ -2439,7 +2447,7 @@
       </c>
       <c r="E22" s="7"/>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>90</v>
       </c>
@@ -2454,7 +2462,7 @@
       </c>
       <c r="E23" s="7"/>
     </row>
-    <row r="24" spans="1:5" ht="30">
+    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>94</v>
       </c>
@@ -2469,7 +2477,7 @@
       </c>
       <c r="E24" s="7"/>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>96</v>
       </c>
@@ -2484,7 +2492,7 @@
       </c>
       <c r="E25" s="7"/>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
         <v>98</v>
       </c>
@@ -2499,7 +2507,7 @@
       </c>
       <c r="E26" s="7"/>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
         <v>102</v>
       </c>
@@ -2514,7 +2522,7 @@
       </c>
       <c r="E27" s="7"/>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
         <v>105</v>
       </c>
@@ -2529,7 +2537,7 @@
       </c>
       <c r="E28" s="7"/>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
         <v>108</v>
       </c>
@@ -2544,7 +2552,7 @@
       </c>
       <c r="E29" s="7"/>
     </row>
-    <row r="30" spans="1:5" ht="30">
+    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
         <v>110</v>
       </c>
@@ -2559,7 +2567,7 @@
       </c>
       <c r="E30" s="7"/>
     </row>
-    <row r="31" spans="1:5" ht="30">
+    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
         <v>114</v>
       </c>
@@ -2574,7 +2582,7 @@
       </c>
       <c r="E31" s="7"/>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
         <v>119</v>
       </c>
@@ -2589,7 +2597,7 @@
       </c>
       <c r="E32" s="7"/>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
         <v>120</v>
       </c>
@@ -2604,7 +2612,7 @@
       </c>
       <c r="E33" s="7"/>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
         <v>125</v>
       </c>
@@ -2619,7 +2627,7 @@
       </c>
       <c r="E34" s="7"/>
     </row>
-    <row r="35" spans="1:5" ht="30">
+    <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
         <v>128</v>
       </c>
@@ -2634,7 +2642,7 @@
       </c>
       <c r="E35" s="7"/>
     </row>
-    <row r="36" spans="1:5" ht="30">
+    <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
         <v>131</v>
       </c>
@@ -2649,7 +2657,7 @@
       </c>
       <c r="E36" s="7"/>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
         <v>134</v>
       </c>
@@ -2664,7 +2672,7 @@
       </c>
       <c r="E37" s="7"/>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="9" t="s">
         <v>137</v>
       </c>
@@ -2679,7 +2687,7 @@
       </c>
       <c r="E38" s="7"/>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="s">
         <v>140</v>
       </c>
@@ -2694,7 +2702,7 @@
       </c>
       <c r="E39" s="7"/>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="9" t="s">
         <v>143</v>
       </c>
@@ -2709,7 +2717,7 @@
       </c>
       <c r="E40" s="7"/>
     </row>
-    <row r="41" spans="1:5" ht="30">
+    <row r="41" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
         <v>145</v>
       </c>
@@ -2724,7 +2732,7 @@
       </c>
       <c r="E41" s="7"/>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="9" t="s">
         <v>147</v>
       </c>
@@ -2739,7 +2747,7 @@
       </c>
       <c r="E42" s="7"/>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="9" t="s">
         <v>150</v>
       </c>
@@ -2754,7 +2762,7 @@
       </c>
       <c r="E43" s="7"/>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="9" t="s">
         <v>153</v>
       </c>
@@ -2769,7 +2777,7 @@
       </c>
       <c r="E44" s="7"/>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="9" t="s">
         <v>155</v>
       </c>
@@ -2784,7 +2792,7 @@
       </c>
       <c r="E45" s="7"/>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="12" t="s">
         <v>158</v>
       </c>
@@ -2799,7 +2807,7 @@
       </c>
       <c r="E46" s="7"/>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="12" t="s">
         <v>159</v>
       </c>
@@ -2814,7 +2822,7 @@
       </c>
       <c r="E47" s="7"/>
     </row>
-    <row r="48" spans="1:5" ht="30">
+    <row r="48" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="12" t="s">
         <v>160</v>
       </c>
@@ -2829,7 +2837,7 @@
       </c>
       <c r="E48" s="7"/>
     </row>
-    <row r="49" spans="1:5" ht="30">
+    <row r="49" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="12" t="s">
         <v>161</v>
       </c>
@@ -2844,7 +2852,7 @@
       </c>
       <c r="E49" s="7"/>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="12" t="s">
         <v>164</v>
       </c>
@@ -2859,7 +2867,7 @@
       </c>
       <c r="E50" s="7"/>
     </row>
-    <row r="51" spans="1:5" ht="30">
+    <row r="51" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="9" t="s">
         <v>173</v>
       </c>
@@ -2874,7 +2882,7 @@
       </c>
       <c r="E51" s="7"/>
     </row>
-    <row r="52" spans="1:5">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="9" t="s">
         <v>174</v>
       </c>
@@ -2889,7 +2897,7 @@
       </c>
       <c r="E52" s="7"/>
     </row>
-    <row r="53" spans="1:5">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="9" t="s">
         <v>179</v>
       </c>
@@ -2904,7 +2912,7 @@
       </c>
       <c r="E53" s="7"/>
     </row>
-    <row r="54" spans="1:5">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="9" t="s">
         <v>180</v>
       </c>
@@ -2919,7 +2927,7 @@
       </c>
       <c r="E54" s="7"/>
     </row>
-    <row r="55" spans="1:5">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="9" t="s">
         <v>185</v>
       </c>
@@ -2934,7 +2942,7 @@
       </c>
       <c r="E55" s="7"/>
     </row>
-    <row r="56" spans="1:5">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="s">
         <v>188</v>
       </c>
@@ -2949,7 +2957,7 @@
       </c>
       <c r="E56" s="7"/>
     </row>
-    <row r="57" spans="1:5" ht="30">
+    <row r="57" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="9" t="s">
         <v>191</v>
       </c>
@@ -2964,7 +2972,7 @@
       </c>
       <c r="E57" s="7"/>
     </row>
-    <row r="58" spans="1:5">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="9" t="s">
         <v>194</v>
       </c>
@@ -2979,7 +2987,7 @@
       </c>
       <c r="E58" s="7"/>
     </row>
-    <row r="59" spans="1:5">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
         <v>196</v>
       </c>
@@ -2994,7 +3002,7 @@
       </c>
       <c r="E59" s="7"/>
     </row>
-    <row r="60" spans="1:5" ht="45">
+    <row r="60" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
         <v>199</v>
       </c>
@@ -3009,7 +3017,7 @@
       </c>
       <c r="E60" s="7"/>
     </row>
-    <row r="61" spans="1:5">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="9" t="s">
         <v>202</v>
       </c>
@@ -3024,7 +3032,7 @@
       </c>
       <c r="E61" s="7"/>
     </row>
-    <row r="62" spans="1:5">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="9" t="s">
         <v>204</v>
       </c>
@@ -3039,7 +3047,7 @@
       </c>
       <c r="E62" s="7"/>
     </row>
-    <row r="63" spans="1:5">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="9" t="s">
         <v>206</v>
       </c>
@@ -3054,7 +3062,7 @@
       </c>
       <c r="E63" s="7"/>
     </row>
-    <row r="64" spans="1:5">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="9" t="s">
         <v>208</v>
       </c>
@@ -3069,7 +3077,7 @@
       </c>
       <c r="E64" s="7"/>
     </row>
-    <row r="65" spans="1:5">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="9" t="s">
         <v>217</v>
       </c>
@@ -3084,7 +3092,7 @@
       </c>
       <c r="E65" s="7"/>
     </row>
-    <row r="66" spans="1:5">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="9" t="s">
         <v>218</v>
       </c>
@@ -3099,7 +3107,7 @@
       </c>
       <c r="E66" s="7"/>
     </row>
-    <row r="67" spans="1:5">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="9" t="s">
         <v>223</v>
       </c>
@@ -3114,7 +3122,7 @@
       </c>
       <c r="E67" s="7"/>
     </row>
-    <row r="68" spans="1:5">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="9" t="s">
         <v>224</v>
       </c>
@@ -3129,7 +3137,7 @@
       </c>
       <c r="E68" s="7"/>
     </row>
-    <row r="69" spans="1:5">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="9" t="s">
         <v>225</v>
       </c>
@@ -3144,7 +3152,7 @@
       </c>
       <c r="E69" s="7"/>
     </row>
-    <row r="70" spans="1:5">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="9" t="s">
         <v>226</v>
       </c>
@@ -3159,7 +3167,7 @@
       </c>
       <c r="E70" s="7"/>
     </row>
-    <row r="71" spans="1:5">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="9" t="s">
         <v>233</v>
       </c>
@@ -3174,7 +3182,7 @@
       </c>
       <c r="E71" s="7"/>
     </row>
-    <row r="72" spans="1:5">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="9" t="s">
         <v>237</v>
       </c>
@@ -3189,7 +3197,7 @@
       </c>
       <c r="E72" s="7"/>
     </row>
-    <row r="73" spans="1:5">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="9" t="s">
         <v>239</v>
       </c>
@@ -3204,7 +3212,7 @@
       </c>
       <c r="E73" s="7"/>
     </row>
-    <row r="74" spans="1:5">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="9" t="s">
         <v>243</v>
       </c>
@@ -3219,7 +3227,7 @@
       </c>
       <c r="E74" s="7"/>
     </row>
-    <row r="75" spans="1:5" ht="30">
+    <row r="75" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" s="9" t="s">
         <v>245</v>
       </c>
@@ -3234,7 +3242,7 @@
       </c>
       <c r="E75" s="7"/>
     </row>
-    <row r="76" spans="1:5">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="9" t="s">
         <v>248</v>
       </c>
@@ -3249,7 +3257,7 @@
       </c>
       <c r="E76" s="7"/>
     </row>
-    <row r="77" spans="1:5">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="9" t="s">
         <v>256</v>
       </c>
@@ -3264,7 +3272,7 @@
       </c>
       <c r="E77" s="7"/>
     </row>
-    <row r="78" spans="1:5">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="9" t="s">
         <v>257</v>
       </c>
@@ -3279,7 +3287,7 @@
       </c>
       <c r="E78" s="7"/>
     </row>
-    <row r="79" spans="1:5">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="9" t="s">
         <v>261</v>
       </c>
@@ -3294,7 +3302,7 @@
       </c>
       <c r="E79" s="7"/>
     </row>
-    <row r="80" spans="1:5">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="9" t="s">
         <v>264</v>
       </c>
@@ -3309,7 +3317,7 @@
       </c>
       <c r="E80" s="7"/>
     </row>
-    <row r="81" spans="1:5">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="9" t="s">
         <v>267</v>
       </c>
@@ -3324,7 +3332,7 @@
       </c>
       <c r="E81" s="7"/>
     </row>
-    <row r="82" spans="1:5" ht="30">
+    <row r="82" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A82" s="9" t="s">
         <v>269</v>
       </c>
@@ -3339,7 +3347,7 @@
       </c>
       <c r="E82" s="7"/>
     </row>
-    <row r="83" spans="1:5">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="9" t="s">
         <v>274</v>
       </c>
@@ -3354,7 +3362,7 @@
       </c>
       <c r="E83" s="7"/>
     </row>
-    <row r="84" spans="1:5" ht="30">
+    <row r="84" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A84" s="9" t="s">
         <v>277</v>
       </c>
@@ -3369,7 +3377,7 @@
       </c>
       <c r="E84" s="7"/>
     </row>
-    <row r="85" spans="1:5">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="9" t="s">
         <v>279</v>
       </c>
@@ -3384,7 +3392,7 @@
       </c>
       <c r="E85" s="7"/>
     </row>
-    <row r="86" spans="1:5">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="9" t="s">
         <v>282</v>
       </c>
@@ -3399,7 +3407,7 @@
       </c>
       <c r="E86" s="7"/>
     </row>
-    <row r="87" spans="1:5">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="9" t="s">
         <v>285</v>
       </c>
@@ -3414,7 +3422,7 @@
       </c>
       <c r="E87" s="7"/>
     </row>
-    <row r="88" spans="1:5">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="9" t="s">
         <v>288</v>
       </c>
@@ -3429,7 +3437,7 @@
       </c>
       <c r="E88" s="7"/>
     </row>
-    <row r="89" spans="1:5">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="9" t="s">
         <v>291</v>
       </c>
@@ -3444,7 +3452,7 @@
       </c>
       <c r="E89" s="7"/>
     </row>
-    <row r="90" spans="1:5">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="9" t="s">
         <v>294</v>
       </c>
@@ -3459,7 +3467,7 @@
       </c>
       <c r="E90" s="7"/>
     </row>
-    <row r="91" spans="1:5">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="9" t="s">
         <v>297</v>
       </c>
@@ -3474,7 +3482,7 @@
       </c>
       <c r="E91" s="7"/>
     </row>
-    <row r="92" spans="1:5">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="9" t="s">
         <v>300</v>
       </c>
@@ -3489,7 +3497,7 @@
       </c>
       <c r="E92" s="7"/>
     </row>
-    <row r="93" spans="1:5">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="9" t="s">
         <v>303</v>
       </c>
@@ -3504,7 +3512,7 @@
       </c>
       <c r="E93" s="7"/>
     </row>
-    <row r="94" spans="1:5">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="9" t="s">
         <v>306</v>
       </c>
@@ -3519,7 +3527,7 @@
       </c>
       <c r="E94" s="7"/>
     </row>
-    <row r="95" spans="1:5">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="9" t="s">
         <v>309</v>
       </c>
@@ -3534,7 +3542,7 @@
       </c>
       <c r="E95" s="7"/>
     </row>
-    <row r="96" spans="1:5">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="9" t="s">
         <v>314</v>
       </c>
@@ -3549,7 +3557,7 @@
       </c>
       <c r="E96" s="7"/>
     </row>
-    <row r="97" spans="1:5">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="9" t="s">
         <v>315</v>
       </c>
@@ -3564,7 +3572,7 @@
       </c>
       <c r="E97" s="7"/>
     </row>
-    <row r="98" spans="1:5">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="9" t="s">
         <v>319</v>
       </c>
@@ -3579,7 +3587,7 @@
       </c>
       <c r="E98" s="7"/>
     </row>
-    <row r="99" spans="1:5">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="9" t="s">
         <v>321</v>
       </c>
@@ -3594,7 +3602,7 @@
       </c>
       <c r="E99" s="7"/>
     </row>
-    <row r="100" spans="1:5">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="9" t="s">
         <v>322</v>
       </c>
@@ -3609,7 +3617,7 @@
       </c>
       <c r="E100" s="7"/>
     </row>
-    <row r="101" spans="1:5" ht="30">
+    <row r="101" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A101" s="9" t="s">
         <v>323</v>
       </c>
@@ -3624,7 +3632,7 @@
       </c>
       <c r="E101" s="7"/>
     </row>
-    <row r="102" spans="1:5">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="9" t="s">
         <v>328</v>
       </c>
@@ -3639,7 +3647,7 @@
       </c>
       <c r="E102" s="7"/>
     </row>
-    <row r="103" spans="1:5">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="9" t="s">
         <v>333</v>
       </c>
@@ -3654,7 +3662,7 @@
       </c>
       <c r="E103" s="7"/>
     </row>
-    <row r="104" spans="1:5">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="9" t="s">
         <v>336</v>
       </c>
@@ -3669,7 +3677,7 @@
       </c>
       <c r="E104" s="7"/>
     </row>
-    <row r="105" spans="1:5">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="9" t="s">
         <v>337</v>
       </c>
@@ -3684,7 +3692,7 @@
       </c>
       <c r="E105" s="7"/>
     </row>
-    <row r="106" spans="1:5">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="9" t="s">
         <v>342</v>
       </c>
@@ -3699,7 +3707,7 @@
       </c>
       <c r="E106" s="7"/>
     </row>
-    <row r="107" spans="1:5">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="9" t="s">
         <v>345</v>
       </c>
@@ -3714,7 +3722,7 @@
       </c>
       <c r="E107" s="7"/>
     </row>
-    <row r="108" spans="1:5">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="9" t="s">
         <v>350</v>
       </c>
@@ -3729,7 +3737,7 @@
       </c>
       <c r="E108" s="7"/>
     </row>
-    <row r="109" spans="1:5" ht="30">
+    <row r="109" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A109" s="9" t="s">
         <v>351</v>
       </c>
@@ -3744,7 +3752,7 @@
       </c>
       <c r="E109" s="7"/>
     </row>
-    <row r="110" spans="1:5">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="9" t="s">
         <v>354</v>
       </c>
@@ -3759,7 +3767,7 @@
       </c>
       <c r="E110" s="7"/>
     </row>
-    <row r="111" spans="1:5">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="9" t="s">
         <v>357</v>
       </c>
@@ -3774,7 +3782,7 @@
       </c>
       <c r="E111" s="7"/>
     </row>
-    <row r="112" spans="1:5">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="9" t="s">
         <v>361</v>
       </c>
@@ -3789,7 +3797,7 @@
       </c>
       <c r="E112" s="7"/>
     </row>
-    <row r="113" spans="1:5">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="9" t="s">
         <v>363</v>
       </c>
@@ -3804,7 +3812,7 @@
       </c>
       <c r="E113" s="7"/>
     </row>
-    <row r="114" spans="1:5" ht="30">
+    <row r="114" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A114" s="9" t="s">
         <v>366</v>
       </c>
@@ -3819,7 +3827,7 @@
       </c>
       <c r="E114" s="7"/>
     </row>
-    <row r="115" spans="1:5">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="9" t="s">
         <v>369</v>
       </c>
@@ -3834,7 +3842,7 @@
       </c>
       <c r="E115" s="7"/>
     </row>
-    <row r="116" spans="1:5">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="9" t="s">
         <v>370</v>
       </c>
@@ -3849,7 +3857,7 @@
       </c>
       <c r="E116" s="7"/>
     </row>
-    <row r="117" spans="1:5">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" s="9" t="s">
         <v>371</v>
       </c>
@@ -3864,7 +3872,7 @@
       </c>
       <c r="E117" s="7"/>
     </row>
-    <row r="118" spans="1:5">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" s="9" t="s">
         <v>378</v>
       </c>
@@ -3879,7 +3887,7 @@
       </c>
       <c r="E118" s="7"/>
     </row>
-    <row r="119" spans="1:5">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" s="9" t="s">
         <v>381</v>
       </c>
@@ -3894,7 +3902,7 @@
       </c>
       <c r="E119" s="7"/>
     </row>
-    <row r="120" spans="1:5">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" s="9" t="s">
         <v>384</v>
       </c>
@@ -3909,7 +3917,7 @@
       </c>
       <c r="E120" s="7"/>
     </row>
-    <row r="121" spans="1:5">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="9" t="s">
         <v>387</v>
       </c>
@@ -3924,7 +3932,7 @@
       </c>
       <c r="E121" s="7"/>
     </row>
-    <row r="122" spans="1:5">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" s="7" t="s">
         <v>390</v>
       </c>
@@ -3939,7 +3947,7 @@
       </c>
       <c r="E122" s="7"/>
     </row>
-    <row r="123" spans="1:5">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" s="7" t="s">
         <v>393</v>
       </c>
@@ -3954,7 +3962,7 @@
       </c>
       <c r="E123" s="7"/>
     </row>
-    <row r="124" spans="1:5">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" s="7" t="s">
         <v>396</v>
       </c>
@@ -3969,7 +3977,7 @@
       </c>
       <c r="E124" s="7"/>
     </row>
-    <row r="125" spans="1:5">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" s="9" t="s">
         <v>399</v>
       </c>
@@ -3984,7 +3992,7 @@
       </c>
       <c r="E125" s="7"/>
     </row>
-    <row r="126" spans="1:5">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" s="7" t="s">
         <v>402</v>
       </c>
@@ -3999,7 +4007,7 @@
       </c>
       <c r="E126" s="7"/>
     </row>
-    <row r="127" spans="1:5">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" s="7" t="s">
         <v>405</v>
       </c>
@@ -4014,7 +4022,7 @@
       </c>
       <c r="E127" s="7"/>
     </row>
-    <row r="128" spans="1:5">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" s="7" t="s">
         <v>408</v>
       </c>
@@ -4029,7 +4037,7 @@
       </c>
       <c r="E128" s="7"/>
     </row>
-    <row r="129" spans="1:5">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" s="9" t="s">
         <v>411</v>
       </c>
@@ -4044,7 +4052,7 @@
       </c>
       <c r="E129" s="7"/>
     </row>
-    <row r="130" spans="1:5">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" s="9" t="s">
         <v>414</v>
       </c>
@@ -4059,7 +4067,7 @@
       </c>
       <c r="E130" s="7"/>
     </row>
-    <row r="131" spans="1:5">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" s="9" t="s">
         <v>416</v>
       </c>
@@ -4074,7 +4082,7 @@
       </c>
       <c r="E131" s="7"/>
     </row>
-    <row r="132" spans="1:5">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" s="7" t="s">
         <v>419</v>
       </c>
@@ -4089,7 +4097,7 @@
       </c>
       <c r="E132" s="7"/>
     </row>
-    <row r="133" spans="1:5">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" s="9" t="s">
         <v>422</v>
       </c>
@@ -4104,7 +4112,7 @@
       </c>
       <c r="E133" s="7"/>
     </row>
-    <row r="134" spans="1:5" ht="30">
+    <row r="134" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A134" s="7" t="s">
         <v>425</v>
       </c>
@@ -4119,7 +4127,7 @@
       </c>
       <c r="E134" s="7"/>
     </row>
-    <row r="135" spans="1:5" ht="30">
+    <row r="135" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A135" s="7" t="s">
         <v>426</v>
       </c>
@@ -4134,7 +4142,7 @@
       </c>
       <c r="E135" s="7"/>
     </row>
-    <row r="136" spans="1:5">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" s="9" t="s">
         <v>431</v>
       </c>
@@ -4149,7 +4157,7 @@
       </c>
       <c r="E136" s="7"/>
     </row>
-    <row r="137" spans="1:5">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" s="7" t="s">
         <v>434</v>
       </c>
@@ -4164,7 +4172,7 @@
       </c>
       <c r="E137" s="7"/>
     </row>
-    <row r="138" spans="1:5" ht="45">
+    <row r="138" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A138" s="7" t="s">
         <v>435</v>
       </c>
@@ -4179,7 +4187,7 @@
       </c>
       <c r="E138" s="7"/>
     </row>
-    <row r="139" spans="1:5" ht="30">
+    <row r="139" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A139" s="7" t="s">
         <v>436</v>
       </c>
@@ -4194,7 +4202,7 @@
       </c>
       <c r="E139" s="7"/>
     </row>
-    <row r="140" spans="1:5">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" s="17" t="s">
         <v>443</v>
       </c>
@@ -4209,7 +4217,7 @@
       </c>
       <c r="E140" s="7"/>
     </row>
-    <row r="141" spans="1:5">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" s="17" t="s">
         <v>446</v>
       </c>
@@ -4224,7 +4232,7 @@
       </c>
       <c r="E141" s="7"/>
     </row>
-    <row r="142" spans="1:5">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" s="17" t="s">
         <v>449</v>
       </c>
@@ -4239,7 +4247,7 @@
       </c>
       <c r="E142" s="7"/>
     </row>
-    <row r="143" spans="1:5">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" s="17" t="s">
         <v>452</v>
       </c>
@@ -4254,7 +4262,7 @@
       </c>
       <c r="E143" s="7"/>
     </row>
-    <row r="144" spans="1:5">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" s="17" t="s">
         <v>453</v>
       </c>
@@ -4269,7 +4277,7 @@
       </c>
       <c r="E144" s="7"/>
     </row>
-    <row r="145" spans="1:5">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" s="17" t="s">
         <v>458</v>
       </c>
@@ -4284,7 +4292,7 @@
       </c>
       <c r="E145" s="7"/>
     </row>
-    <row r="146" spans="1:5">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" s="17" t="s">
         <v>461</v>
       </c>
@@ -4299,7 +4307,7 @@
       </c>
       <c r="E146" s="7"/>
     </row>
-    <row r="147" spans="1:5">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" s="17" t="s">
         <v>464</v>
       </c>
@@ -4314,7 +4322,7 @@
       </c>
       <c r="E147" s="7"/>
     </row>
-    <row r="148" spans="1:5">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" s="17" t="s">
         <v>467</v>
       </c>
@@ -4329,7 +4337,7 @@
       </c>
       <c r="E148" s="7"/>
     </row>
-    <row r="149" spans="1:5">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" s="7" t="s">
         <v>470</v>
       </c>
@@ -4344,7 +4352,7 @@
       </c>
       <c r="E149" s="7"/>
     </row>
-    <row r="150" spans="1:5">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" s="7" t="s">
         <v>471</v>
       </c>
@@ -4359,7 +4367,7 @@
       </c>
       <c r="E150" s="7"/>
     </row>
-    <row r="151" spans="1:5">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" s="7" t="s">
         <v>472</v>
       </c>
@@ -4374,7 +4382,7 @@
       </c>
       <c r="E151" s="7"/>
     </row>
-    <row r="152" spans="1:5" ht="30">
+    <row r="152" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A152" s="7" t="s">
         <v>479</v>
       </c>
@@ -4389,7 +4397,7 @@
       </c>
       <c r="E152" s="7"/>
     </row>
-    <row r="153" spans="1:5" ht="45">
+    <row r="153" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A153" s="17" t="s">
         <v>482</v>
       </c>
@@ -4404,7 +4412,7 @@
       </c>
       <c r="E153" s="7"/>
     </row>
-    <row r="154" spans="1:5">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" s="17" t="s">
         <v>484</v>
       </c>
@@ -4419,7 +4427,7 @@
       </c>
       <c r="E154" s="7"/>
     </row>
-    <row r="155" spans="1:5">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" s="7" t="s">
         <v>486</v>
       </c>
@@ -4434,7 +4442,7 @@
       </c>
       <c r="E155" s="7"/>
     </row>
-    <row r="156" spans="1:5">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" s="7" t="s">
         <v>489</v>
       </c>
@@ -4449,7 +4457,7 @@
       </c>
       <c r="E156" s="7"/>
     </row>
-    <row r="157" spans="1:5">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" s="7" t="s">
         <v>492</v>
       </c>
@@ -4464,7 +4472,7 @@
       </c>
       <c r="E157" s="7"/>
     </row>
-    <row r="158" spans="1:5" ht="30">
+    <row r="158" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A158" s="7" t="s">
         <v>495</v>
       </c>
@@ -4479,7 +4487,7 @@
       </c>
       <c r="E158" s="7"/>
     </row>
-    <row r="159" spans="1:5" ht="30">
+    <row r="159" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A159" s="7" t="s">
         <v>496</v>
       </c>
@@ -4494,7 +4502,7 @@
       </c>
       <c r="E159" s="7"/>
     </row>
-    <row r="160" spans="1:5">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" s="7" t="s">
         <v>503</v>
       </c>
@@ -4509,7 +4517,7 @@
       </c>
       <c r="E160" s="7"/>
     </row>
-    <row r="161" spans="1:5">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161" s="7" t="s">
         <v>504</v>
       </c>
@@ -4524,7 +4532,7 @@
       </c>
       <c r="E161" s="7"/>
     </row>
-    <row r="162" spans="1:5">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162" s="7" t="s">
         <v>507</v>
       </c>
@@ -4539,7 +4547,7 @@
       </c>
       <c r="E162" s="7"/>
     </row>
-    <row r="163" spans="1:5">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" s="7" t="s">
         <v>512</v>
       </c>
@@ -4554,7 +4562,7 @@
       </c>
       <c r="E163" s="7"/>
     </row>
-    <row r="164" spans="1:5" ht="30">
+    <row r="164" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A164" s="7" t="s">
         <v>515</v>
       </c>
@@ -4569,7 +4577,7 @@
       </c>
       <c r="E164" s="7"/>
     </row>
-    <row r="165" spans="1:5">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165" s="7" t="s">
         <v>518</v>
       </c>
@@ -4584,7 +4592,7 @@
       </c>
       <c r="E165" s="7"/>
     </row>
-    <row r="166" spans="1:5" ht="30">
+    <row r="166" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A166" s="7" t="s">
         <v>521</v>
       </c>
@@ -4599,7 +4607,7 @@
       </c>
       <c r="E166" s="7"/>
     </row>
-    <row r="167" spans="1:5">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167" s="7" t="s">
         <v>525</v>
       </c>
@@ -4614,7 +4622,7 @@
       </c>
       <c r="E167" s="7"/>
     </row>
-    <row r="168" spans="1:5">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" s="7" t="s">
         <v>527</v>
       </c>
@@ -4629,7 +4637,7 @@
       </c>
       <c r="E168" s="7"/>
     </row>
-    <row r="169" spans="1:5">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" s="7" t="s">
         <v>530</v>
       </c>
@@ -4644,7 +4652,7 @@
       </c>
       <c r="E169" s="7"/>
     </row>
-    <row r="170" spans="1:5">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170" s="7" t="s">
         <v>531</v>
       </c>
@@ -4659,7 +4667,7 @@
       </c>
       <c r="E170" s="7"/>
     </row>
-    <row r="171" spans="1:5">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171" s="7" t="s">
         <v>532</v>
       </c>
@@ -4673,6 +4681,21 @@
         <v>5</v>
       </c>
       <c r="E171" s="7"/>
+    </row>
+    <row r="172" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A172" s="7" t="s">
+        <v>539</v>
+      </c>
+      <c r="B172" s="7" t="s">
+        <v>519</v>
+      </c>
+      <c r="C172" s="8" t="s">
+        <v>540</v>
+      </c>
+      <c r="D172" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E172" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -4685,14 +4708,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView topLeftCell="A10" zoomScale="80" workbookViewId="0">
       <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
@@ -4700,7 +4723,7 @@
     <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>35</v>
       </c>
@@ -4714,7 +4737,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>37</v>
       </c>
@@ -4726,7 +4749,7 @@
       </c>
       <c r="D2" s="7"/>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>38</v>
       </c>
@@ -4738,7 +4761,7 @@
       </c>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>39</v>
       </c>
@@ -4750,7 +4773,7 @@
       </c>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>40</v>
       </c>
@@ -4762,7 +4785,7 @@
       </c>
       <c r="D5" s="7"/>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>41</v>
       </c>
@@ -4774,7 +4797,7 @@
       </c>
       <c r="D6" s="7"/>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>42</v>
       </c>
@@ -4786,7 +4809,7 @@
       </c>
       <c r="D7" s="7"/>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>43</v>
       </c>
@@ -4798,7 +4821,7 @@
       </c>
       <c r="D8" s="7"/>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>44</v>
       </c>
@@ -4810,7 +4833,7 @@
       </c>
       <c r="D9" s="7"/>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>45</v>
       </c>
@@ -4822,7 +4845,7 @@
       </c>
       <c r="D10" s="7"/>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>46</v>
       </c>
@@ -4834,7 +4857,7 @@
       </c>
       <c r="D11" s="7"/>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>48</v>
       </c>
@@ -4846,7 +4869,7 @@
       </c>
       <c r="D12" s="7"/>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>49</v>
       </c>
@@ -4858,7 +4881,7 @@
       </c>
       <c r="D13" s="7"/>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>50</v>
       </c>
@@ -4870,7 +4893,7 @@
       </c>
       <c r="D14" s="7"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>51</v>
       </c>
@@ -4882,7 +4905,7 @@
       </c>
       <c r="D15" s="7"/>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>52</v>
       </c>
@@ -4894,7 +4917,7 @@
       </c>
       <c r="D16" s="7"/>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>53</v>
       </c>
@@ -4906,7 +4929,7 @@
       </c>
       <c r="D17" s="7"/>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>54</v>
       </c>
@@ -4918,7 +4941,7 @@
       </c>
       <c r="D18" s="7"/>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>55</v>
       </c>
@@ -4930,7 +4953,7 @@
       </c>
       <c r="D19" s="7"/>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>56</v>
       </c>
@@ -4942,7 +4965,7 @@
       </c>
       <c r="D20" s="7"/>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>57</v>
       </c>
@@ -4954,7 +4977,7 @@
       </c>
       <c r="D21" s="7"/>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>58</v>
       </c>
@@ -4966,7 +4989,7 @@
       </c>
       <c r="D22" s="7"/>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>59</v>
       </c>
@@ -4978,7 +5001,7 @@
       </c>
       <c r="D23" s="7"/>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>60</v>
       </c>
@@ -4990,7 +5013,7 @@
       </c>
       <c r="D24" s="7"/>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>61</v>
       </c>
@@ -5002,7 +5025,7 @@
       </c>
       <c r="D25" s="7"/>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>47</v>
       </c>
@@ -5021,14 +5044,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A19" sqref="A19:XFD19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
@@ -5036,7 +5059,7 @@
     <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>35</v>
       </c>
@@ -5050,7 +5073,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>37</v>
       </c>
@@ -5062,7 +5085,7 @@
       </c>
       <c r="D2" s="7"/>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>38</v>
       </c>
@@ -5074,7 +5097,7 @@
       </c>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>39</v>
       </c>
@@ -5086,7 +5109,7 @@
       </c>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>40</v>
       </c>
@@ -5098,7 +5121,7 @@
       </c>
       <c r="D5" s="7"/>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>41</v>
       </c>
@@ -5110,7 +5133,7 @@
       </c>
       <c r="D6" s="7"/>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>42</v>
       </c>
@@ -5122,7 +5145,7 @@
       </c>
       <c r="D7" s="7"/>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>43</v>
       </c>
@@ -5134,7 +5157,7 @@
       </c>
       <c r="D8" s="7"/>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>44</v>
       </c>
@@ -5146,7 +5169,7 @@
       </c>
       <c r="D9" s="7"/>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>45</v>
       </c>
@@ -5158,7 +5181,7 @@
       </c>
       <c r="D10" s="7"/>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>46</v>
       </c>
@@ -5170,7 +5193,7 @@
       </c>
       <c r="D11" s="7"/>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>47</v>
       </c>
@@ -5182,7 +5205,7 @@
       </c>
       <c r="D12" s="7"/>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>48</v>
       </c>
@@ -5194,7 +5217,7 @@
       </c>
       <c r="D13" s="7"/>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>49</v>
       </c>
@@ -5206,7 +5229,7 @@
       </c>
       <c r="D14" s="7"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>50</v>
       </c>
@@ -5218,7 +5241,7 @@
       </c>
       <c r="D15" s="7"/>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>51</v>
       </c>
@@ -5230,7 +5253,7 @@
       </c>
       <c r="D16" s="7"/>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>52</v>
       </c>
@@ -5242,7 +5265,7 @@
       </c>
       <c r="D17" s="7"/>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>53</v>
       </c>
@@ -5254,7 +5277,7 @@
       </c>
       <c r="D18" s="7"/>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>54</v>
       </c>
@@ -5266,7 +5289,7 @@
       </c>
       <c r="D19" s="7"/>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>55</v>
       </c>
@@ -5278,7 +5301,7 @@
       </c>
       <c r="D20" s="7"/>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>56</v>
       </c>
@@ -5290,7 +5313,7 @@
       </c>
       <c r="D21" s="7"/>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>57</v>
       </c>
@@ -5302,7 +5325,7 @@
       </c>
       <c r="D22" s="7"/>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>58</v>
       </c>
@@ -5314,7 +5337,7 @@
       </c>
       <c r="D23" s="7"/>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>59</v>
       </c>
@@ -5326,7 +5349,7 @@
       </c>
       <c r="D24" s="7"/>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>60</v>
       </c>
@@ -5338,7 +5361,7 @@
       </c>
       <c r="D25" s="7"/>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>61</v>
       </c>

</xml_diff>

<commit_message>
WAT new scripts 180,181,182, 184
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/WAT.xlsx
+++ b/src/test/resources/xls/WAT.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13305" windowHeight="2415"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="847" uniqueCount="541">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="863" uniqueCount="552">
   <si>
     <t>TCID</t>
   </si>
@@ -1641,13 +1641,46 @@
   </si>
   <si>
     <t>Verify that when a user clicks on curate button each Publication should have a "X" symbol, which upon clicking will remove the Publication from the combined author publication list.</t>
+  </si>
+  <si>
+    <t>WAT180</t>
+  </si>
+  <si>
+    <t>WAT181</t>
+  </si>
+  <si>
+    <t>WAT182</t>
+  </si>
+  <si>
+    <t>WAT183</t>
+  </si>
+  <si>
+    <t>WAT-644</t>
+  </si>
+  <si>
+    <t>Verify that System must display an alternatives name tab after combine 2 or more records</t>
+  </si>
+  <si>
+    <t>WAT-1431</t>
+  </si>
+  <si>
+    <t>Verify that Alternatives name tab getting highlighted when user click on it for combine 2 or more author records</t>
+  </si>
+  <si>
+    <t>WAT-646</t>
+  </si>
+  <si>
+    <t>WAT-645</t>
+  </si>
+  <si>
+    <t>Verify that System must display name variations associated with the author record in the alternative names tab.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1856,7 +1889,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1888,10 +1921,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1923,7 +1955,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2099,14 +2130,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E172"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E176"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A149" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C175" sqref="C175"/>
+    <sheetView tabSelected="1" topLeftCell="A155" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C176" sqref="C176"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="30.5703125" customWidth="1" collapsed="1"/>
@@ -2115,7 +2146,7 @@
     <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2132,7 +2163,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -2147,7 +2178,7 @@
       </c>
       <c r="E2" s="4"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -2162,7 +2193,7 @@
       </c>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" s="7" t="s">
         <v>11</v>
       </c>
@@ -2177,7 +2208,7 @@
       </c>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" s="7" t="s">
         <v>12</v>
       </c>
@@ -2192,7 +2223,7 @@
       </c>
       <c r="E5" s="7"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" s="7" t="s">
         <v>14</v>
       </c>
@@ -2207,7 +2238,7 @@
       </c>
       <c r="E6" s="7"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" s="7" t="s">
         <v>17</v>
       </c>
@@ -2222,7 +2253,7 @@
       </c>
       <c r="E7" s="7"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" s="7" t="s">
         <v>20</v>
       </c>
@@ -2237,7 +2268,7 @@
       </c>
       <c r="E8" s="7"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" s="7" t="s">
         <v>22</v>
       </c>
@@ -2252,7 +2283,7 @@
       </c>
       <c r="E9" s="7"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10" s="7" t="s">
         <v>23</v>
       </c>
@@ -2267,7 +2298,7 @@
       </c>
       <c r="E10" s="7"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11" s="7" t="s">
         <v>24</v>
       </c>
@@ -2282,7 +2313,7 @@
       </c>
       <c r="E11" s="7"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12" s="7" t="s">
         <v>25</v>
       </c>
@@ -2297,7 +2328,7 @@
       </c>
       <c r="E12" s="7"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13" s="7" t="s">
         <v>62</v>
       </c>
@@ -2312,7 +2343,7 @@
       </c>
       <c r="E13" s="7"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="A14" s="7" t="s">
         <v>63</v>
       </c>
@@ -2327,7 +2358,7 @@
       </c>
       <c r="E14" s="7"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="A15" s="7" t="s">
         <v>64</v>
       </c>
@@ -2342,7 +2373,7 @@
       </c>
       <c r="E15" s="7"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="A16" s="7" t="s">
         <v>65</v>
       </c>
@@ -2357,7 +2388,7 @@
       </c>
       <c r="E16" s="7"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5">
       <c r="A17" s="7" t="s">
         <v>74</v>
       </c>
@@ -2372,7 +2403,7 @@
       </c>
       <c r="E17" s="7"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5">
       <c r="A18" s="7" t="s">
         <v>75</v>
       </c>
@@ -2387,7 +2418,7 @@
       </c>
       <c r="E18" s="7"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5">
       <c r="A19" s="7" t="s">
         <v>79</v>
       </c>
@@ -2402,7 +2433,7 @@
       </c>
       <c r="E19" s="7"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5">
       <c r="A20" s="7" t="s">
         <v>81</v>
       </c>
@@ -2417,7 +2448,7 @@
       </c>
       <c r="E20" s="7"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5">
       <c r="A21" s="7" t="s">
         <v>82</v>
       </c>
@@ -2432,7 +2463,7 @@
       </c>
       <c r="E21" s="7"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5">
       <c r="A22" s="7" t="s">
         <v>88</v>
       </c>
@@ -2447,7 +2478,7 @@
       </c>
       <c r="E22" s="7"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5">
       <c r="A23" s="7" t="s">
         <v>90</v>
       </c>
@@ -2462,7 +2493,7 @@
       </c>
       <c r="E23" s="7"/>
     </row>
-    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="30">
       <c r="A24" s="9" t="s">
         <v>94</v>
       </c>
@@ -2477,7 +2508,7 @@
       </c>
       <c r="E24" s="7"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5">
       <c r="A25" s="9" t="s">
         <v>96</v>
       </c>
@@ -2492,7 +2523,7 @@
       </c>
       <c r="E25" s="7"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5">
       <c r="A26" s="9" t="s">
         <v>98</v>
       </c>
@@ -2507,7 +2538,7 @@
       </c>
       <c r="E26" s="7"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5">
       <c r="A27" s="9" t="s">
         <v>102</v>
       </c>
@@ -2522,7 +2553,7 @@
       </c>
       <c r="E27" s="7"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5">
       <c r="A28" s="9" t="s">
         <v>105</v>
       </c>
@@ -2537,7 +2568,7 @@
       </c>
       <c r="E28" s="7"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5">
       <c r="A29" s="9" t="s">
         <v>108</v>
       </c>
@@ -2552,7 +2583,7 @@
       </c>
       <c r="E29" s="7"/>
     </row>
-    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" ht="30">
       <c r="A30" s="9" t="s">
         <v>110</v>
       </c>
@@ -2567,7 +2598,7 @@
       </c>
       <c r="E30" s="7"/>
     </row>
-    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" ht="30">
       <c r="A31" s="9" t="s">
         <v>114</v>
       </c>
@@ -2582,7 +2613,7 @@
       </c>
       <c r="E31" s="7"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5">
       <c r="A32" s="9" t="s">
         <v>119</v>
       </c>
@@ -2597,7 +2628,7 @@
       </c>
       <c r="E32" s="7"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5">
       <c r="A33" s="9" t="s">
         <v>120</v>
       </c>
@@ -2612,7 +2643,7 @@
       </c>
       <c r="E33" s="7"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5">
       <c r="A34" s="9" t="s">
         <v>125</v>
       </c>
@@ -2627,7 +2658,7 @@
       </c>
       <c r="E34" s="7"/>
     </row>
-    <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" ht="30">
       <c r="A35" s="9" t="s">
         <v>128</v>
       </c>
@@ -2642,7 +2673,7 @@
       </c>
       <c r="E35" s="7"/>
     </row>
-    <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" ht="30">
       <c r="A36" s="9" t="s">
         <v>131</v>
       </c>
@@ -2657,7 +2688,7 @@
       </c>
       <c r="E36" s="7"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5">
       <c r="A37" s="9" t="s">
         <v>134</v>
       </c>
@@ -2672,7 +2703,7 @@
       </c>
       <c r="E37" s="7"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5">
       <c r="A38" s="9" t="s">
         <v>137</v>
       </c>
@@ -2687,7 +2718,7 @@
       </c>
       <c r="E38" s="7"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5">
       <c r="A39" s="9" t="s">
         <v>140</v>
       </c>
@@ -2702,7 +2733,7 @@
       </c>
       <c r="E39" s="7"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5">
       <c r="A40" s="9" t="s">
         <v>143</v>
       </c>
@@ -2717,7 +2748,7 @@
       </c>
       <c r="E40" s="7"/>
     </row>
-    <row r="41" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" ht="30">
       <c r="A41" s="9" t="s">
         <v>145</v>
       </c>
@@ -2732,7 +2763,7 @@
       </c>
       <c r="E41" s="7"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5">
       <c r="A42" s="9" t="s">
         <v>147</v>
       </c>
@@ -2747,7 +2778,7 @@
       </c>
       <c r="E42" s="7"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5">
       <c r="A43" s="9" t="s">
         <v>150</v>
       </c>
@@ -2762,7 +2793,7 @@
       </c>
       <c r="E43" s="7"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5">
       <c r="A44" s="9" t="s">
         <v>153</v>
       </c>
@@ -2777,7 +2808,7 @@
       </c>
       <c r="E44" s="7"/>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5">
       <c r="A45" s="9" t="s">
         <v>155</v>
       </c>
@@ -2792,7 +2823,7 @@
       </c>
       <c r="E45" s="7"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5">
       <c r="A46" s="12" t="s">
         <v>158</v>
       </c>
@@ -2807,7 +2838,7 @@
       </c>
       <c r="E46" s="7"/>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5">
       <c r="A47" s="12" t="s">
         <v>159</v>
       </c>
@@ -2822,7 +2853,7 @@
       </c>
       <c r="E47" s="7"/>
     </row>
-    <row r="48" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" ht="30">
       <c r="A48" s="12" t="s">
         <v>160</v>
       </c>
@@ -2837,7 +2868,7 @@
       </c>
       <c r="E48" s="7"/>
     </row>
-    <row r="49" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" ht="30">
       <c r="A49" s="12" t="s">
         <v>161</v>
       </c>
@@ -2852,7 +2883,7 @@
       </c>
       <c r="E49" s="7"/>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5">
       <c r="A50" s="12" t="s">
         <v>164</v>
       </c>
@@ -2867,7 +2898,7 @@
       </c>
       <c r="E50" s="7"/>
     </row>
-    <row r="51" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" ht="30">
       <c r="A51" s="9" t="s">
         <v>173</v>
       </c>
@@ -2882,7 +2913,7 @@
       </c>
       <c r="E51" s="7"/>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5">
       <c r="A52" s="9" t="s">
         <v>174</v>
       </c>
@@ -2897,7 +2928,7 @@
       </c>
       <c r="E52" s="7"/>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5">
       <c r="A53" s="9" t="s">
         <v>179</v>
       </c>
@@ -2912,7 +2943,7 @@
       </c>
       <c r="E53" s="7"/>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5">
       <c r="A54" s="9" t="s">
         <v>180</v>
       </c>
@@ -2927,7 +2958,7 @@
       </c>
       <c r="E54" s="7"/>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5">
       <c r="A55" s="9" t="s">
         <v>185</v>
       </c>
@@ -2942,7 +2973,7 @@
       </c>
       <c r="E55" s="7"/>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5">
       <c r="A56" s="9" t="s">
         <v>188</v>
       </c>
@@ -2957,7 +2988,7 @@
       </c>
       <c r="E56" s="7"/>
     </row>
-    <row r="57" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" ht="30">
       <c r="A57" s="9" t="s">
         <v>191</v>
       </c>
@@ -2972,7 +3003,7 @@
       </c>
       <c r="E57" s="7"/>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5">
       <c r="A58" s="9" t="s">
         <v>194</v>
       </c>
@@ -2987,7 +3018,7 @@
       </c>
       <c r="E58" s="7"/>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5">
       <c r="A59" s="7" t="s">
         <v>196</v>
       </c>
@@ -3002,7 +3033,7 @@
       </c>
       <c r="E59" s="7"/>
     </row>
-    <row r="60" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" ht="45">
       <c r="A60" s="7" t="s">
         <v>199</v>
       </c>
@@ -3017,7 +3048,7 @@
       </c>
       <c r="E60" s="7"/>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5">
       <c r="A61" s="9" t="s">
         <v>202</v>
       </c>
@@ -3032,7 +3063,7 @@
       </c>
       <c r="E61" s="7"/>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5">
       <c r="A62" s="9" t="s">
         <v>204</v>
       </c>
@@ -3047,7 +3078,7 @@
       </c>
       <c r="E62" s="7"/>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5">
       <c r="A63" s="9" t="s">
         <v>206</v>
       </c>
@@ -3062,7 +3093,7 @@
       </c>
       <c r="E63" s="7"/>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5">
       <c r="A64" s="9" t="s">
         <v>208</v>
       </c>
@@ -3077,7 +3108,7 @@
       </c>
       <c r="E64" s="7"/>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5">
       <c r="A65" s="9" t="s">
         <v>217</v>
       </c>
@@ -3092,7 +3123,7 @@
       </c>
       <c r="E65" s="7"/>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5">
       <c r="A66" s="9" t="s">
         <v>218</v>
       </c>
@@ -3107,7 +3138,7 @@
       </c>
       <c r="E66" s="7"/>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5">
       <c r="A67" s="9" t="s">
         <v>223</v>
       </c>
@@ -3122,7 +3153,7 @@
       </c>
       <c r="E67" s="7"/>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5">
       <c r="A68" s="9" t="s">
         <v>224</v>
       </c>
@@ -3137,7 +3168,7 @@
       </c>
       <c r="E68" s="7"/>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5">
       <c r="A69" s="9" t="s">
         <v>225</v>
       </c>
@@ -3152,7 +3183,7 @@
       </c>
       <c r="E69" s="7"/>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5">
       <c r="A70" s="9" t="s">
         <v>226</v>
       </c>
@@ -3167,7 +3198,7 @@
       </c>
       <c r="E70" s="7"/>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5">
       <c r="A71" s="9" t="s">
         <v>233</v>
       </c>
@@ -3182,7 +3213,7 @@
       </c>
       <c r="E71" s="7"/>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5">
       <c r="A72" s="9" t="s">
         <v>237</v>
       </c>
@@ -3197,7 +3228,7 @@
       </c>
       <c r="E72" s="7"/>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5">
       <c r="A73" s="9" t="s">
         <v>239</v>
       </c>
@@ -3212,7 +3243,7 @@
       </c>
       <c r="E73" s="7"/>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5">
       <c r="A74" s="9" t="s">
         <v>243</v>
       </c>
@@ -3227,7 +3258,7 @@
       </c>
       <c r="E74" s="7"/>
     </row>
-    <row r="75" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" ht="30">
       <c r="A75" s="9" t="s">
         <v>245</v>
       </c>
@@ -3242,7 +3273,7 @@
       </c>
       <c r="E75" s="7"/>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5">
       <c r="A76" s="9" t="s">
         <v>248</v>
       </c>
@@ -3257,7 +3288,7 @@
       </c>
       <c r="E76" s="7"/>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5">
       <c r="A77" s="9" t="s">
         <v>256</v>
       </c>
@@ -3272,7 +3303,7 @@
       </c>
       <c r="E77" s="7"/>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5">
       <c r="A78" s="9" t="s">
         <v>257</v>
       </c>
@@ -3287,7 +3318,7 @@
       </c>
       <c r="E78" s="7"/>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5">
       <c r="A79" s="9" t="s">
         <v>261</v>
       </c>
@@ -3302,7 +3333,7 @@
       </c>
       <c r="E79" s="7"/>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5">
       <c r="A80" s="9" t="s">
         <v>264</v>
       </c>
@@ -3317,7 +3348,7 @@
       </c>
       <c r="E80" s="7"/>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5">
       <c r="A81" s="9" t="s">
         <v>267</v>
       </c>
@@ -3332,7 +3363,7 @@
       </c>
       <c r="E81" s="7"/>
     </row>
-    <row r="82" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" ht="30">
       <c r="A82" s="9" t="s">
         <v>269</v>
       </c>
@@ -3347,7 +3378,7 @@
       </c>
       <c r="E82" s="7"/>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5">
       <c r="A83" s="9" t="s">
         <v>274</v>
       </c>
@@ -3362,7 +3393,7 @@
       </c>
       <c r="E83" s="7"/>
     </row>
-    <row r="84" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" ht="30">
       <c r="A84" s="9" t="s">
         <v>277</v>
       </c>
@@ -3377,7 +3408,7 @@
       </c>
       <c r="E84" s="7"/>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5">
       <c r="A85" s="9" t="s">
         <v>279</v>
       </c>
@@ -3392,7 +3423,7 @@
       </c>
       <c r="E85" s="7"/>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5">
       <c r="A86" s="9" t="s">
         <v>282</v>
       </c>
@@ -3407,7 +3438,7 @@
       </c>
       <c r="E86" s="7"/>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5">
       <c r="A87" s="9" t="s">
         <v>285</v>
       </c>
@@ -3422,7 +3453,7 @@
       </c>
       <c r="E87" s="7"/>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5">
       <c r="A88" s="9" t="s">
         <v>288</v>
       </c>
@@ -3437,7 +3468,7 @@
       </c>
       <c r="E88" s="7"/>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5">
       <c r="A89" s="9" t="s">
         <v>291</v>
       </c>
@@ -3452,7 +3483,7 @@
       </c>
       <c r="E89" s="7"/>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5">
       <c r="A90" s="9" t="s">
         <v>294</v>
       </c>
@@ -3467,7 +3498,7 @@
       </c>
       <c r="E90" s="7"/>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5">
       <c r="A91" s="9" t="s">
         <v>297</v>
       </c>
@@ -3482,7 +3513,7 @@
       </c>
       <c r="E91" s="7"/>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5">
       <c r="A92" s="9" t="s">
         <v>300</v>
       </c>
@@ -3497,7 +3528,7 @@
       </c>
       <c r="E92" s="7"/>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5">
       <c r="A93" s="9" t="s">
         <v>303</v>
       </c>
@@ -3512,7 +3543,7 @@
       </c>
       <c r="E93" s="7"/>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5">
       <c r="A94" s="9" t="s">
         <v>306</v>
       </c>
@@ -3527,7 +3558,7 @@
       </c>
       <c r="E94" s="7"/>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5">
       <c r="A95" s="9" t="s">
         <v>309</v>
       </c>
@@ -3542,7 +3573,7 @@
       </c>
       <c r="E95" s="7"/>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5">
       <c r="A96" s="9" t="s">
         <v>314</v>
       </c>
@@ -3557,7 +3588,7 @@
       </c>
       <c r="E96" s="7"/>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5">
       <c r="A97" s="9" t="s">
         <v>315</v>
       </c>
@@ -3572,7 +3603,7 @@
       </c>
       <c r="E97" s="7"/>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5">
       <c r="A98" s="9" t="s">
         <v>319</v>
       </c>
@@ -3587,7 +3618,7 @@
       </c>
       <c r="E98" s="7"/>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5">
       <c r="A99" s="9" t="s">
         <v>321</v>
       </c>
@@ -3602,7 +3633,7 @@
       </c>
       <c r="E99" s="7"/>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5">
       <c r="A100" s="9" t="s">
         <v>322</v>
       </c>
@@ -3617,7 +3648,7 @@
       </c>
       <c r="E100" s="7"/>
     </row>
-    <row r="101" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" ht="30">
       <c r="A101" s="9" t="s">
         <v>323</v>
       </c>
@@ -3632,7 +3663,7 @@
       </c>
       <c r="E101" s="7"/>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5">
       <c r="A102" s="9" t="s">
         <v>328</v>
       </c>
@@ -3647,7 +3678,7 @@
       </c>
       <c r="E102" s="7"/>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5">
       <c r="A103" s="9" t="s">
         <v>333</v>
       </c>
@@ -3662,7 +3693,7 @@
       </c>
       <c r="E103" s="7"/>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5">
       <c r="A104" s="9" t="s">
         <v>336</v>
       </c>
@@ -3677,7 +3708,7 @@
       </c>
       <c r="E104" s="7"/>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5">
       <c r="A105" s="9" t="s">
         <v>337</v>
       </c>
@@ -3692,7 +3723,7 @@
       </c>
       <c r="E105" s="7"/>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5">
       <c r="A106" s="9" t="s">
         <v>342</v>
       </c>
@@ -3707,7 +3738,7 @@
       </c>
       <c r="E106" s="7"/>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5">
       <c r="A107" s="9" t="s">
         <v>345</v>
       </c>
@@ -3722,7 +3753,7 @@
       </c>
       <c r="E107" s="7"/>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5">
       <c r="A108" s="9" t="s">
         <v>350</v>
       </c>
@@ -3737,7 +3768,7 @@
       </c>
       <c r="E108" s="7"/>
     </row>
-    <row r="109" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" ht="30">
       <c r="A109" s="9" t="s">
         <v>351</v>
       </c>
@@ -3752,7 +3783,7 @@
       </c>
       <c r="E109" s="7"/>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5">
       <c r="A110" s="9" t="s">
         <v>354</v>
       </c>
@@ -3767,7 +3798,7 @@
       </c>
       <c r="E110" s="7"/>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5">
       <c r="A111" s="9" t="s">
         <v>357</v>
       </c>
@@ -3782,7 +3813,7 @@
       </c>
       <c r="E111" s="7"/>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5">
       <c r="A112" s="9" t="s">
         <v>361</v>
       </c>
@@ -3797,7 +3828,7 @@
       </c>
       <c r="E112" s="7"/>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5">
       <c r="A113" s="9" t="s">
         <v>363</v>
       </c>
@@ -3812,7 +3843,7 @@
       </c>
       <c r="E113" s="7"/>
     </row>
-    <row r="114" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" ht="30">
       <c r="A114" s="9" t="s">
         <v>366</v>
       </c>
@@ -3827,7 +3858,7 @@
       </c>
       <c r="E114" s="7"/>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5">
       <c r="A115" s="9" t="s">
         <v>369</v>
       </c>
@@ -3842,7 +3873,7 @@
       </c>
       <c r="E115" s="7"/>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5">
       <c r="A116" s="9" t="s">
         <v>370</v>
       </c>
@@ -3857,7 +3888,7 @@
       </c>
       <c r="E116" s="7"/>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5">
       <c r="A117" s="9" t="s">
         <v>371</v>
       </c>
@@ -3872,7 +3903,7 @@
       </c>
       <c r="E117" s="7"/>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5">
       <c r="A118" s="9" t="s">
         <v>378</v>
       </c>
@@ -3887,7 +3918,7 @@
       </c>
       <c r="E118" s="7"/>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5">
       <c r="A119" s="9" t="s">
         <v>381</v>
       </c>
@@ -3902,7 +3933,7 @@
       </c>
       <c r="E119" s="7"/>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5">
       <c r="A120" s="9" t="s">
         <v>384</v>
       </c>
@@ -3917,7 +3948,7 @@
       </c>
       <c r="E120" s="7"/>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5">
       <c r="A121" s="9" t="s">
         <v>387</v>
       </c>
@@ -3932,7 +3963,7 @@
       </c>
       <c r="E121" s="7"/>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5">
       <c r="A122" s="7" t="s">
         <v>390</v>
       </c>
@@ -3947,7 +3978,7 @@
       </c>
       <c r="E122" s="7"/>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5">
       <c r="A123" s="7" t="s">
         <v>393</v>
       </c>
@@ -3962,7 +3993,7 @@
       </c>
       <c r="E123" s="7"/>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5">
       <c r="A124" s="7" t="s">
         <v>396</v>
       </c>
@@ -3977,7 +4008,7 @@
       </c>
       <c r="E124" s="7"/>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5">
       <c r="A125" s="9" t="s">
         <v>399</v>
       </c>
@@ -3992,7 +4023,7 @@
       </c>
       <c r="E125" s="7"/>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5">
       <c r="A126" s="7" t="s">
         <v>402</v>
       </c>
@@ -4007,7 +4038,7 @@
       </c>
       <c r="E126" s="7"/>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5">
       <c r="A127" s="7" t="s">
         <v>405</v>
       </c>
@@ -4022,7 +4053,7 @@
       </c>
       <c r="E127" s="7"/>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5">
       <c r="A128" s="7" t="s">
         <v>408</v>
       </c>
@@ -4037,7 +4068,7 @@
       </c>
       <c r="E128" s="7"/>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5">
       <c r="A129" s="9" t="s">
         <v>411</v>
       </c>
@@ -4052,7 +4083,7 @@
       </c>
       <c r="E129" s="7"/>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5">
       <c r="A130" s="9" t="s">
         <v>414</v>
       </c>
@@ -4067,7 +4098,7 @@
       </c>
       <c r="E130" s="7"/>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5">
       <c r="A131" s="9" t="s">
         <v>416</v>
       </c>
@@ -4082,7 +4113,7 @@
       </c>
       <c r="E131" s="7"/>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5">
       <c r="A132" s="7" t="s">
         <v>419</v>
       </c>
@@ -4097,7 +4128,7 @@
       </c>
       <c r="E132" s="7"/>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5">
       <c r="A133" s="9" t="s">
         <v>422</v>
       </c>
@@ -4112,7 +4143,7 @@
       </c>
       <c r="E133" s="7"/>
     </row>
-    <row r="134" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5" ht="30">
       <c r="A134" s="7" t="s">
         <v>425</v>
       </c>
@@ -4127,7 +4158,7 @@
       </c>
       <c r="E134" s="7"/>
     </row>
-    <row r="135" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5" ht="30">
       <c r="A135" s="7" t="s">
         <v>426</v>
       </c>
@@ -4142,7 +4173,7 @@
       </c>
       <c r="E135" s="7"/>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5">
       <c r="A136" s="9" t="s">
         <v>431</v>
       </c>
@@ -4157,7 +4188,7 @@
       </c>
       <c r="E136" s="7"/>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5">
       <c r="A137" s="7" t="s">
         <v>434</v>
       </c>
@@ -4172,7 +4203,7 @@
       </c>
       <c r="E137" s="7"/>
     </row>
-    <row r="138" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" ht="45">
       <c r="A138" s="7" t="s">
         <v>435</v>
       </c>
@@ -4187,7 +4218,7 @@
       </c>
       <c r="E138" s="7"/>
     </row>
-    <row r="139" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5" ht="30">
       <c r="A139" s="7" t="s">
         <v>436</v>
       </c>
@@ -4202,7 +4233,7 @@
       </c>
       <c r="E139" s="7"/>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5">
       <c r="A140" s="17" t="s">
         <v>443</v>
       </c>
@@ -4217,7 +4248,7 @@
       </c>
       <c r="E140" s="7"/>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5">
       <c r="A141" s="17" t="s">
         <v>446</v>
       </c>
@@ -4232,7 +4263,7 @@
       </c>
       <c r="E141" s="7"/>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:5">
       <c r="A142" s="17" t="s">
         <v>449</v>
       </c>
@@ -4247,7 +4278,7 @@
       </c>
       <c r="E142" s="7"/>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:5">
       <c r="A143" s="17" t="s">
         <v>452</v>
       </c>
@@ -4262,7 +4293,7 @@
       </c>
       <c r="E143" s="7"/>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:5">
       <c r="A144" s="17" t="s">
         <v>453</v>
       </c>
@@ -4277,7 +4308,7 @@
       </c>
       <c r="E144" s="7"/>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:5">
       <c r="A145" s="17" t="s">
         <v>458</v>
       </c>
@@ -4292,7 +4323,7 @@
       </c>
       <c r="E145" s="7"/>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:5">
       <c r="A146" s="17" t="s">
         <v>461</v>
       </c>
@@ -4307,7 +4338,7 @@
       </c>
       <c r="E146" s="7"/>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:5">
       <c r="A147" s="17" t="s">
         <v>464</v>
       </c>
@@ -4322,7 +4353,7 @@
       </c>
       <c r="E147" s="7"/>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:5">
       <c r="A148" s="17" t="s">
         <v>467</v>
       </c>
@@ -4337,7 +4368,7 @@
       </c>
       <c r="E148" s="7"/>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:5">
       <c r="A149" s="7" t="s">
         <v>470</v>
       </c>
@@ -4352,7 +4383,7 @@
       </c>
       <c r="E149" s="7"/>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:5">
       <c r="A150" s="7" t="s">
         <v>471</v>
       </c>
@@ -4367,7 +4398,7 @@
       </c>
       <c r="E150" s="7"/>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:5">
       <c r="A151" s="7" t="s">
         <v>472</v>
       </c>
@@ -4382,7 +4413,7 @@
       </c>
       <c r="E151" s="7"/>
     </row>
-    <row r="152" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:5" ht="30">
       <c r="A152" s="7" t="s">
         <v>479</v>
       </c>
@@ -4397,7 +4428,7 @@
       </c>
       <c r="E152" s="7"/>
     </row>
-    <row r="153" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:5" ht="45">
       <c r="A153" s="17" t="s">
         <v>482</v>
       </c>
@@ -4412,7 +4443,7 @@
       </c>
       <c r="E153" s="7"/>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:5">
       <c r="A154" s="17" t="s">
         <v>484</v>
       </c>
@@ -4427,7 +4458,7 @@
       </c>
       <c r="E154" s="7"/>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:5">
       <c r="A155" s="7" t="s">
         <v>486</v>
       </c>
@@ -4442,7 +4473,7 @@
       </c>
       <c r="E155" s="7"/>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:5">
       <c r="A156" s="7" t="s">
         <v>489</v>
       </c>
@@ -4457,7 +4488,7 @@
       </c>
       <c r="E156" s="7"/>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:5">
       <c r="A157" s="7" t="s">
         <v>492</v>
       </c>
@@ -4472,7 +4503,7 @@
       </c>
       <c r="E157" s="7"/>
     </row>
-    <row r="158" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:5" ht="30">
       <c r="A158" s="7" t="s">
         <v>495</v>
       </c>
@@ -4487,7 +4518,7 @@
       </c>
       <c r="E158" s="7"/>
     </row>
-    <row r="159" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:5" ht="30">
       <c r="A159" s="7" t="s">
         <v>496</v>
       </c>
@@ -4502,7 +4533,7 @@
       </c>
       <c r="E159" s="7"/>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:5">
       <c r="A160" s="7" t="s">
         <v>503</v>
       </c>
@@ -4517,7 +4548,7 @@
       </c>
       <c r="E160" s="7"/>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:5">
       <c r="A161" s="7" t="s">
         <v>504</v>
       </c>
@@ -4532,7 +4563,7 @@
       </c>
       <c r="E161" s="7"/>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:5">
       <c r="A162" s="7" t="s">
         <v>507</v>
       </c>
@@ -4547,7 +4578,7 @@
       </c>
       <c r="E162" s="7"/>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:5">
       <c r="A163" s="7" t="s">
         <v>512</v>
       </c>
@@ -4562,7 +4593,7 @@
       </c>
       <c r="E163" s="7"/>
     </row>
-    <row r="164" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:5" ht="30">
       <c r="A164" s="7" t="s">
         <v>515</v>
       </c>
@@ -4577,7 +4608,7 @@
       </c>
       <c r="E164" s="7"/>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:5">
       <c r="A165" s="7" t="s">
         <v>518</v>
       </c>
@@ -4592,7 +4623,7 @@
       </c>
       <c r="E165" s="7"/>
     </row>
-    <row r="166" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:5" ht="30">
       <c r="A166" s="7" t="s">
         <v>521</v>
       </c>
@@ -4607,7 +4638,7 @@
       </c>
       <c r="E166" s="7"/>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:5">
       <c r="A167" s="7" t="s">
         <v>525</v>
       </c>
@@ -4622,7 +4653,7 @@
       </c>
       <c r="E167" s="7"/>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:5">
       <c r="A168" s="7" t="s">
         <v>527</v>
       </c>
@@ -4637,7 +4668,7 @@
       </c>
       <c r="E168" s="7"/>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:5">
       <c r="A169" s="7" t="s">
         <v>530</v>
       </c>
@@ -4652,7 +4683,7 @@
       </c>
       <c r="E169" s="7"/>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:5">
       <c r="A170" s="7" t="s">
         <v>531</v>
       </c>
@@ -4667,7 +4698,7 @@
       </c>
       <c r="E170" s="7"/>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:5">
       <c r="A171" s="7" t="s">
         <v>532</v>
       </c>
@@ -4682,7 +4713,7 @@
       </c>
       <c r="E171" s="7"/>
     </row>
-    <row r="172" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:5" ht="30">
       <c r="A172" s="7" t="s">
         <v>539</v>
       </c>
@@ -4696,6 +4727,66 @@
         <v>5</v>
       </c>
       <c r="E172" s="7"/>
+    </row>
+    <row r="173" spans="1:5">
+      <c r="A173" s="9" t="s">
+        <v>541</v>
+      </c>
+      <c r="B173" s="7" t="s">
+        <v>545</v>
+      </c>
+      <c r="C173" s="8" t="s">
+        <v>546</v>
+      </c>
+      <c r="D173" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E173" s="7"/>
+    </row>
+    <row r="174" spans="1:5">
+      <c r="A174" s="9" t="s">
+        <v>542</v>
+      </c>
+      <c r="B174" s="7" t="s">
+        <v>547</v>
+      </c>
+      <c r="C174" s="8" t="s">
+        <v>548</v>
+      </c>
+      <c r="D174" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E174" s="7"/>
+    </row>
+    <row r="175" spans="1:5">
+      <c r="A175" s="9" t="s">
+        <v>543</v>
+      </c>
+      <c r="B175" s="7" t="s">
+        <v>549</v>
+      </c>
+      <c r="C175" s="8" t="s">
+        <v>231</v>
+      </c>
+      <c r="D175" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E175" s="7"/>
+    </row>
+    <row r="176" spans="1:5">
+      <c r="A176" s="9" t="s">
+        <v>544</v>
+      </c>
+      <c r="B176" s="7" t="s">
+        <v>550</v>
+      </c>
+      <c r="C176" s="8" t="s">
+        <v>551</v>
+      </c>
+      <c r="D176" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E176" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -4708,14 +4799,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView topLeftCell="A10" zoomScale="80" workbookViewId="0">
       <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
@@ -4723,7 +4814,7 @@
     <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="10" t="s">
         <v>35</v>
       </c>
@@ -4737,7 +4828,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="7" t="s">
         <v>37</v>
       </c>
@@ -4749,7 +4840,7 @@
       </c>
       <c r="D2" s="7"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="7" t="s">
         <v>38</v>
       </c>
@@ -4761,7 +4852,7 @@
       </c>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="7" t="s">
         <v>39</v>
       </c>
@@ -4773,7 +4864,7 @@
       </c>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" s="7" t="s">
         <v>40</v>
       </c>
@@ -4785,7 +4876,7 @@
       </c>
       <c r="D5" s="7"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" s="7" t="s">
         <v>41</v>
       </c>
@@ -4797,7 +4888,7 @@
       </c>
       <c r="D6" s="7"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="7" t="s">
         <v>42</v>
       </c>
@@ -4809,7 +4900,7 @@
       </c>
       <c r="D7" s="7"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="7" t="s">
         <v>43</v>
       </c>
@@ -4821,7 +4912,7 @@
       </c>
       <c r="D8" s="7"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="7" t="s">
         <v>44</v>
       </c>
@@ -4833,7 +4924,7 @@
       </c>
       <c r="D9" s="7"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="7" t="s">
         <v>45</v>
       </c>
@@ -4845,7 +4936,7 @@
       </c>
       <c r="D10" s="7"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11" s="7" t="s">
         <v>46</v>
       </c>
@@ -4857,7 +4948,7 @@
       </c>
       <c r="D11" s="7"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="A12" s="7" t="s">
         <v>48</v>
       </c>
@@ -4869,7 +4960,7 @@
       </c>
       <c r="D12" s="7"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="A13" s="7" t="s">
         <v>49</v>
       </c>
@@ -4881,7 +4972,7 @@
       </c>
       <c r="D13" s="7"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="A14" s="7" t="s">
         <v>50</v>
       </c>
@@ -4893,7 +4984,7 @@
       </c>
       <c r="D14" s="7"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="A15" s="7" t="s">
         <v>51</v>
       </c>
@@ -4905,7 +4996,7 @@
       </c>
       <c r="D15" s="7"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="A16" s="7" t="s">
         <v>52</v>
       </c>
@@ -4917,7 +5008,7 @@
       </c>
       <c r="D16" s="7"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4">
       <c r="A17" s="7" t="s">
         <v>53</v>
       </c>
@@ -4929,7 +5020,7 @@
       </c>
       <c r="D17" s="7"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4">
       <c r="A18" s="7" t="s">
         <v>54</v>
       </c>
@@ -4941,7 +5032,7 @@
       </c>
       <c r="D18" s="7"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4">
       <c r="A19" s="7" t="s">
         <v>55</v>
       </c>
@@ -4953,7 +5044,7 @@
       </c>
       <c r="D19" s="7"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4">
       <c r="A20" s="7" t="s">
         <v>56</v>
       </c>
@@ -4965,7 +5056,7 @@
       </c>
       <c r="D20" s="7"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4">
       <c r="A21" s="7" t="s">
         <v>57</v>
       </c>
@@ -4977,7 +5068,7 @@
       </c>
       <c r="D21" s="7"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4">
       <c r="A22" s="7" t="s">
         <v>58</v>
       </c>
@@ -4989,7 +5080,7 @@
       </c>
       <c r="D22" s="7"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4">
       <c r="A23" s="7" t="s">
         <v>59</v>
       </c>
@@ -5001,7 +5092,7 @@
       </c>
       <c r="D23" s="7"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4">
       <c r="A24" s="7" t="s">
         <v>60</v>
       </c>
@@ -5013,7 +5104,7 @@
       </c>
       <c r="D24" s="7"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4">
       <c r="A25" s="7" t="s">
         <v>61</v>
       </c>
@@ -5025,7 +5116,7 @@
       </c>
       <c r="D25" s="7"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4">
       <c r="A26" s="7" t="s">
         <v>47</v>
       </c>
@@ -5044,14 +5135,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A19" sqref="A19:XFD19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
@@ -5059,7 +5150,7 @@
     <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="10" t="s">
         <v>35</v>
       </c>
@@ -5073,7 +5164,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="7" t="s">
         <v>37</v>
       </c>
@@ -5085,7 +5176,7 @@
       </c>
       <c r="D2" s="7"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="7" t="s">
         <v>38</v>
       </c>
@@ -5097,7 +5188,7 @@
       </c>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="7" t="s">
         <v>39</v>
       </c>
@@ -5109,7 +5200,7 @@
       </c>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" s="7" t="s">
         <v>40</v>
       </c>
@@ -5121,7 +5212,7 @@
       </c>
       <c r="D5" s="7"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" s="7" t="s">
         <v>41</v>
       </c>
@@ -5133,7 +5224,7 @@
       </c>
       <c r="D6" s="7"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="7" t="s">
         <v>42</v>
       </c>
@@ -5145,7 +5236,7 @@
       </c>
       <c r="D7" s="7"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="7" t="s">
         <v>43</v>
       </c>
@@ -5157,7 +5248,7 @@
       </c>
       <c r="D8" s="7"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="7" t="s">
         <v>44</v>
       </c>
@@ -5169,7 +5260,7 @@
       </c>
       <c r="D9" s="7"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="7" t="s">
         <v>45</v>
       </c>
@@ -5181,7 +5272,7 @@
       </c>
       <c r="D10" s="7"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11" s="7" t="s">
         <v>46</v>
       </c>
@@ -5193,7 +5284,7 @@
       </c>
       <c r="D11" s="7"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="A12" s="7" t="s">
         <v>47</v>
       </c>
@@ -5205,7 +5296,7 @@
       </c>
       <c r="D12" s="7"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="A13" s="7" t="s">
         <v>48</v>
       </c>
@@ -5217,7 +5308,7 @@
       </c>
       <c r="D13" s="7"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="A14" s="7" t="s">
         <v>49</v>
       </c>
@@ -5229,7 +5320,7 @@
       </c>
       <c r="D14" s="7"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="A15" s="7" t="s">
         <v>50</v>
       </c>
@@ -5241,7 +5332,7 @@
       </c>
       <c r="D15" s="7"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="A16" s="7" t="s">
         <v>51</v>
       </c>
@@ -5253,7 +5344,7 @@
       </c>
       <c r="D16" s="7"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4">
       <c r="A17" s="7" t="s">
         <v>52</v>
       </c>
@@ -5265,7 +5356,7 @@
       </c>
       <c r="D17" s="7"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4">
       <c r="A18" s="7" t="s">
         <v>53</v>
       </c>
@@ -5277,7 +5368,7 @@
       </c>
       <c r="D18" s="7"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4">
       <c r="A19" s="7" t="s">
         <v>54</v>
       </c>
@@ -5289,7 +5380,7 @@
       </c>
       <c r="D19" s="7"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4">
       <c r="A20" s="7" t="s">
         <v>55</v>
       </c>
@@ -5301,7 +5392,7 @@
       </c>
       <c r="D20" s="7"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4">
       <c r="A21" s="7" t="s">
         <v>56</v>
       </c>
@@ -5313,7 +5404,7 @@
       </c>
       <c r="D21" s="7"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4">
       <c r="A22" s="7" t="s">
         <v>57</v>
       </c>
@@ -5325,7 +5416,7 @@
       </c>
       <c r="D22" s="7"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4">
       <c r="A23" s="7" t="s">
         <v>58</v>
       </c>
@@ -5337,7 +5428,7 @@
       </c>
       <c r="D23" s="7"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4">
       <c r="A24" s="7" t="s">
         <v>59</v>
       </c>
@@ -5349,7 +5440,7 @@
       </c>
       <c r="D24" s="7"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4">
       <c r="A25" s="7" t="s">
         <v>60</v>
       </c>
@@ -5361,7 +5452,7 @@
       </c>
       <c r="D25" s="7"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4">
       <c r="A26" s="7" t="s">
         <v>61</v>
       </c>

</xml_diff>

<commit_message>
Adds WAT-143 testscript and related changes
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/WAT.xlsx
+++ b/src/test/resources/xls/WAT.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13305" windowHeight="2415"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="863" uniqueCount="552">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="867" uniqueCount="555">
   <si>
     <t>TCID</t>
   </si>
@@ -1674,13 +1674,22 @@
   </si>
   <si>
     <t>Verify that System must display name variations associated with the author record in the alternative names tab.</t>
+  </si>
+  <si>
+    <t>WAT143</t>
+  </si>
+  <si>
+    <t>WAT-1304</t>
+  </si>
+  <si>
+    <t>Verify that for a Combined author The left-to-right order of the metrics in the Author Metadata area of the Author Record should be: h-index Sum of Times Cited Citing Articles</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1889,7 +1898,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1921,9 +1930,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1955,6 +1965,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2130,14 +2141,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E176"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E177"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A155" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C176" sqref="C176"/>
+      <selection activeCell="C181" sqref="C181"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="30.5703125" customWidth="1" collapsed="1"/>
@@ -2146,7 +2157,7 @@
     <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2163,7 +2174,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -2178,7 +2189,7 @@
       </c>
       <c r="E2" s="4"/>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -2193,7 +2204,7 @@
       </c>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>11</v>
       </c>
@@ -2208,7 +2219,7 @@
       </c>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>12</v>
       </c>
@@ -2223,7 +2234,7 @@
       </c>
       <c r="E5" s="7"/>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>14</v>
       </c>
@@ -2238,7 +2249,7 @@
       </c>
       <c r="E6" s="7"/>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>17</v>
       </c>
@@ -2253,7 +2264,7 @@
       </c>
       <c r="E7" s="7"/>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>20</v>
       </c>
@@ -2268,7 +2279,7 @@
       </c>
       <c r="E8" s="7"/>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>22</v>
       </c>
@@ -2283,7 +2294,7 @@
       </c>
       <c r="E9" s="7"/>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>23</v>
       </c>
@@ -2298,7 +2309,7 @@
       </c>
       <c r="E10" s="7"/>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>24</v>
       </c>
@@ -2313,7 +2324,7 @@
       </c>
       <c r="E11" s="7"/>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>25</v>
       </c>
@@ -2328,7 +2339,7 @@
       </c>
       <c r="E12" s="7"/>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>62</v>
       </c>
@@ -2343,7 +2354,7 @@
       </c>
       <c r="E13" s="7"/>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>63</v>
       </c>
@@ -2358,7 +2369,7 @@
       </c>
       <c r="E14" s="7"/>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>64</v>
       </c>
@@ -2373,7 +2384,7 @@
       </c>
       <c r="E15" s="7"/>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>65</v>
       </c>
@@ -2388,7 +2399,7 @@
       </c>
       <c r="E16" s="7"/>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>74</v>
       </c>
@@ -2403,7 +2414,7 @@
       </c>
       <c r="E17" s="7"/>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>75</v>
       </c>
@@ -2418,7 +2429,7 @@
       </c>
       <c r="E18" s="7"/>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>79</v>
       </c>
@@ -2433,7 +2444,7 @@
       </c>
       <c r="E19" s="7"/>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>81</v>
       </c>
@@ -2448,7 +2459,7 @@
       </c>
       <c r="E20" s="7"/>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>82</v>
       </c>
@@ -2463,7 +2474,7 @@
       </c>
       <c r="E21" s="7"/>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>88</v>
       </c>
@@ -2478,7 +2489,7 @@
       </c>
       <c r="E22" s="7"/>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>90</v>
       </c>
@@ -2493,7 +2504,7 @@
       </c>
       <c r="E23" s="7"/>
     </row>
-    <row r="24" spans="1:5" ht="30">
+    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>94</v>
       </c>
@@ -2508,7 +2519,7 @@
       </c>
       <c r="E24" s="7"/>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>96</v>
       </c>
@@ -2523,7 +2534,7 @@
       </c>
       <c r="E25" s="7"/>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
         <v>98</v>
       </c>
@@ -2538,7 +2549,7 @@
       </c>
       <c r="E26" s="7"/>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
         <v>102</v>
       </c>
@@ -2553,7 +2564,7 @@
       </c>
       <c r="E27" s="7"/>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
         <v>105</v>
       </c>
@@ -2568,7 +2579,7 @@
       </c>
       <c r="E28" s="7"/>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
         <v>108</v>
       </c>
@@ -2583,7 +2594,7 @@
       </c>
       <c r="E29" s="7"/>
     </row>
-    <row r="30" spans="1:5" ht="30">
+    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
         <v>110</v>
       </c>
@@ -2598,7 +2609,7 @@
       </c>
       <c r="E30" s="7"/>
     </row>
-    <row r="31" spans="1:5" ht="30">
+    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
         <v>114</v>
       </c>
@@ -2613,7 +2624,7 @@
       </c>
       <c r="E31" s="7"/>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
         <v>119</v>
       </c>
@@ -2628,7 +2639,7 @@
       </c>
       <c r="E32" s="7"/>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
         <v>120</v>
       </c>
@@ -2643,7 +2654,7 @@
       </c>
       <c r="E33" s="7"/>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
         <v>125</v>
       </c>
@@ -2658,7 +2669,7 @@
       </c>
       <c r="E34" s="7"/>
     </row>
-    <row r="35" spans="1:5" ht="30">
+    <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
         <v>128</v>
       </c>
@@ -2673,7 +2684,7 @@
       </c>
       <c r="E35" s="7"/>
     </row>
-    <row r="36" spans="1:5" ht="30">
+    <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
         <v>131</v>
       </c>
@@ -2688,7 +2699,7 @@
       </c>
       <c r="E36" s="7"/>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
         <v>134</v>
       </c>
@@ -2703,7 +2714,7 @@
       </c>
       <c r="E37" s="7"/>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="9" t="s">
         <v>137</v>
       </c>
@@ -2718,7 +2729,7 @@
       </c>
       <c r="E38" s="7"/>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="s">
         <v>140</v>
       </c>
@@ -2733,7 +2744,7 @@
       </c>
       <c r="E39" s="7"/>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="9" t="s">
         <v>143</v>
       </c>
@@ -2748,7 +2759,7 @@
       </c>
       <c r="E40" s="7"/>
     </row>
-    <row r="41" spans="1:5" ht="30">
+    <row r="41" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
         <v>145</v>
       </c>
@@ -2763,7 +2774,7 @@
       </c>
       <c r="E41" s="7"/>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="9" t="s">
         <v>147</v>
       </c>
@@ -2778,7 +2789,7 @@
       </c>
       <c r="E42" s="7"/>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="9" t="s">
         <v>150</v>
       </c>
@@ -2793,7 +2804,7 @@
       </c>
       <c r="E43" s="7"/>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="9" t="s">
         <v>153</v>
       </c>
@@ -2808,7 +2819,7 @@
       </c>
       <c r="E44" s="7"/>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="9" t="s">
         <v>155</v>
       </c>
@@ -2823,7 +2834,7 @@
       </c>
       <c r="E45" s="7"/>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="12" t="s">
         <v>158</v>
       </c>
@@ -2838,7 +2849,7 @@
       </c>
       <c r="E46" s="7"/>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="12" t="s">
         <v>159</v>
       </c>
@@ -2853,7 +2864,7 @@
       </c>
       <c r="E47" s="7"/>
     </row>
-    <row r="48" spans="1:5" ht="30">
+    <row r="48" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="12" t="s">
         <v>160</v>
       </c>
@@ -2868,7 +2879,7 @@
       </c>
       <c r="E48" s="7"/>
     </row>
-    <row r="49" spans="1:5" ht="30">
+    <row r="49" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="12" t="s">
         <v>161</v>
       </c>
@@ -2883,7 +2894,7 @@
       </c>
       <c r="E49" s="7"/>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="12" t="s">
         <v>164</v>
       </c>
@@ -2898,7 +2909,7 @@
       </c>
       <c r="E50" s="7"/>
     </row>
-    <row r="51" spans="1:5" ht="30">
+    <row r="51" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="9" t="s">
         <v>173</v>
       </c>
@@ -2913,7 +2924,7 @@
       </c>
       <c r="E51" s="7"/>
     </row>
-    <row r="52" spans="1:5">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="9" t="s">
         <v>174</v>
       </c>
@@ -2928,7 +2939,7 @@
       </c>
       <c r="E52" s="7"/>
     </row>
-    <row r="53" spans="1:5">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="9" t="s">
         <v>179</v>
       </c>
@@ -2943,7 +2954,7 @@
       </c>
       <c r="E53" s="7"/>
     </row>
-    <row r="54" spans="1:5">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="9" t="s">
         <v>180</v>
       </c>
@@ -2958,7 +2969,7 @@
       </c>
       <c r="E54" s="7"/>
     </row>
-    <row r="55" spans="1:5">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="9" t="s">
         <v>185</v>
       </c>
@@ -2973,7 +2984,7 @@
       </c>
       <c r="E55" s="7"/>
     </row>
-    <row r="56" spans="1:5">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="s">
         <v>188</v>
       </c>
@@ -2988,7 +2999,7 @@
       </c>
       <c r="E56" s="7"/>
     </row>
-    <row r="57" spans="1:5" ht="30">
+    <row r="57" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="9" t="s">
         <v>191</v>
       </c>
@@ -3003,7 +3014,7 @@
       </c>
       <c r="E57" s="7"/>
     </row>
-    <row r="58" spans="1:5">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="9" t="s">
         <v>194</v>
       </c>
@@ -3018,7 +3029,7 @@
       </c>
       <c r="E58" s="7"/>
     </row>
-    <row r="59" spans="1:5">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
         <v>196</v>
       </c>
@@ -3033,7 +3044,7 @@
       </c>
       <c r="E59" s="7"/>
     </row>
-    <row r="60" spans="1:5" ht="45">
+    <row r="60" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
         <v>199</v>
       </c>
@@ -3048,7 +3059,7 @@
       </c>
       <c r="E60" s="7"/>
     </row>
-    <row r="61" spans="1:5">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="9" t="s">
         <v>202</v>
       </c>
@@ -3063,7 +3074,7 @@
       </c>
       <c r="E61" s="7"/>
     </row>
-    <row r="62" spans="1:5">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="9" t="s">
         <v>204</v>
       </c>
@@ -3078,7 +3089,7 @@
       </c>
       <c r="E62" s="7"/>
     </row>
-    <row r="63" spans="1:5">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="9" t="s">
         <v>206</v>
       </c>
@@ -3093,7 +3104,7 @@
       </c>
       <c r="E63" s="7"/>
     </row>
-    <row r="64" spans="1:5">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="9" t="s">
         <v>208</v>
       </c>
@@ -3108,7 +3119,7 @@
       </c>
       <c r="E64" s="7"/>
     </row>
-    <row r="65" spans="1:5">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="9" t="s">
         <v>217</v>
       </c>
@@ -3123,7 +3134,7 @@
       </c>
       <c r="E65" s="7"/>
     </row>
-    <row r="66" spans="1:5">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="9" t="s">
         <v>218</v>
       </c>
@@ -3138,7 +3149,7 @@
       </c>
       <c r="E66" s="7"/>
     </row>
-    <row r="67" spans="1:5">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="9" t="s">
         <v>223</v>
       </c>
@@ -3153,7 +3164,7 @@
       </c>
       <c r="E67" s="7"/>
     </row>
-    <row r="68" spans="1:5">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="9" t="s">
         <v>224</v>
       </c>
@@ -3168,7 +3179,7 @@
       </c>
       <c r="E68" s="7"/>
     </row>
-    <row r="69" spans="1:5">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="9" t="s">
         <v>225</v>
       </c>
@@ -3183,7 +3194,7 @@
       </c>
       <c r="E69" s="7"/>
     </row>
-    <row r="70" spans="1:5">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="9" t="s">
         <v>226</v>
       </c>
@@ -3198,7 +3209,7 @@
       </c>
       <c r="E70" s="7"/>
     </row>
-    <row r="71" spans="1:5">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="9" t="s">
         <v>233</v>
       </c>
@@ -3213,7 +3224,7 @@
       </c>
       <c r="E71" s="7"/>
     </row>
-    <row r="72" spans="1:5">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="9" t="s">
         <v>237</v>
       </c>
@@ -3228,7 +3239,7 @@
       </c>
       <c r="E72" s="7"/>
     </row>
-    <row r="73" spans="1:5">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="9" t="s">
         <v>239</v>
       </c>
@@ -3243,7 +3254,7 @@
       </c>
       <c r="E73" s="7"/>
     </row>
-    <row r="74" spans="1:5">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="9" t="s">
         <v>243</v>
       </c>
@@ -3258,7 +3269,7 @@
       </c>
       <c r="E74" s="7"/>
     </row>
-    <row r="75" spans="1:5" ht="30">
+    <row r="75" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" s="9" t="s">
         <v>245</v>
       </c>
@@ -3273,7 +3284,7 @@
       </c>
       <c r="E75" s="7"/>
     </row>
-    <row r="76" spans="1:5">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="9" t="s">
         <v>248</v>
       </c>
@@ -3288,7 +3299,7 @@
       </c>
       <c r="E76" s="7"/>
     </row>
-    <row r="77" spans="1:5">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="9" t="s">
         <v>256</v>
       </c>
@@ -3303,7 +3314,7 @@
       </c>
       <c r="E77" s="7"/>
     </row>
-    <row r="78" spans="1:5">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="9" t="s">
         <v>257</v>
       </c>
@@ -3318,7 +3329,7 @@
       </c>
       <c r="E78" s="7"/>
     </row>
-    <row r="79" spans="1:5">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="9" t="s">
         <v>261</v>
       </c>
@@ -3333,7 +3344,7 @@
       </c>
       <c r="E79" s="7"/>
     </row>
-    <row r="80" spans="1:5">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="9" t="s">
         <v>264</v>
       </c>
@@ -3348,7 +3359,7 @@
       </c>
       <c r="E80" s="7"/>
     </row>
-    <row r="81" spans="1:5">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="9" t="s">
         <v>267</v>
       </c>
@@ -3363,7 +3374,7 @@
       </c>
       <c r="E81" s="7"/>
     </row>
-    <row r="82" spans="1:5" ht="30">
+    <row r="82" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A82" s="9" t="s">
         <v>269</v>
       </c>
@@ -3378,7 +3389,7 @@
       </c>
       <c r="E82" s="7"/>
     </row>
-    <row r="83" spans="1:5">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="9" t="s">
         <v>274</v>
       </c>
@@ -3393,7 +3404,7 @@
       </c>
       <c r="E83" s="7"/>
     </row>
-    <row r="84" spans="1:5" ht="30">
+    <row r="84" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A84" s="9" t="s">
         <v>277</v>
       </c>
@@ -3408,7 +3419,7 @@
       </c>
       <c r="E84" s="7"/>
     </row>
-    <row r="85" spans="1:5">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="9" t="s">
         <v>279</v>
       </c>
@@ -3423,7 +3434,7 @@
       </c>
       <c r="E85" s="7"/>
     </row>
-    <row r="86" spans="1:5">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="9" t="s">
         <v>282</v>
       </c>
@@ -3438,7 +3449,7 @@
       </c>
       <c r="E86" s="7"/>
     </row>
-    <row r="87" spans="1:5">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="9" t="s">
         <v>285</v>
       </c>
@@ -3453,7 +3464,7 @@
       </c>
       <c r="E87" s="7"/>
     </row>
-    <row r="88" spans="1:5">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="9" t="s">
         <v>288</v>
       </c>
@@ -3468,7 +3479,7 @@
       </c>
       <c r="E88" s="7"/>
     </row>
-    <row r="89" spans="1:5">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="9" t="s">
         <v>291</v>
       </c>
@@ -3483,7 +3494,7 @@
       </c>
       <c r="E89" s="7"/>
     </row>
-    <row r="90" spans="1:5">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="9" t="s">
         <v>294</v>
       </c>
@@ -3498,7 +3509,7 @@
       </c>
       <c r="E90" s="7"/>
     </row>
-    <row r="91" spans="1:5">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="9" t="s">
         <v>297</v>
       </c>
@@ -3513,7 +3524,7 @@
       </c>
       <c r="E91" s="7"/>
     </row>
-    <row r="92" spans="1:5">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="9" t="s">
         <v>300</v>
       </c>
@@ -3528,7 +3539,7 @@
       </c>
       <c r="E92" s="7"/>
     </row>
-    <row r="93" spans="1:5">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="9" t="s">
         <v>303</v>
       </c>
@@ -3543,7 +3554,7 @@
       </c>
       <c r="E93" s="7"/>
     </row>
-    <row r="94" spans="1:5">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="9" t="s">
         <v>306</v>
       </c>
@@ -3558,7 +3569,7 @@
       </c>
       <c r="E94" s="7"/>
     </row>
-    <row r="95" spans="1:5">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="9" t="s">
         <v>309</v>
       </c>
@@ -3573,7 +3584,7 @@
       </c>
       <c r="E95" s="7"/>
     </row>
-    <row r="96" spans="1:5">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="9" t="s">
         <v>314</v>
       </c>
@@ -3588,7 +3599,7 @@
       </c>
       <c r="E96" s="7"/>
     </row>
-    <row r="97" spans="1:5">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="9" t="s">
         <v>315</v>
       </c>
@@ -3603,7 +3614,7 @@
       </c>
       <c r="E97" s="7"/>
     </row>
-    <row r="98" spans="1:5">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="9" t="s">
         <v>319</v>
       </c>
@@ -3618,7 +3629,7 @@
       </c>
       <c r="E98" s="7"/>
     </row>
-    <row r="99" spans="1:5">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="9" t="s">
         <v>321</v>
       </c>
@@ -3633,7 +3644,7 @@
       </c>
       <c r="E99" s="7"/>
     </row>
-    <row r="100" spans="1:5">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="9" t="s">
         <v>322</v>
       </c>
@@ -3648,7 +3659,7 @@
       </c>
       <c r="E100" s="7"/>
     </row>
-    <row r="101" spans="1:5" ht="30">
+    <row r="101" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A101" s="9" t="s">
         <v>323</v>
       </c>
@@ -3663,7 +3674,7 @@
       </c>
       <c r="E101" s="7"/>
     </row>
-    <row r="102" spans="1:5">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="9" t="s">
         <v>328</v>
       </c>
@@ -3678,7 +3689,7 @@
       </c>
       <c r="E102" s="7"/>
     </row>
-    <row r="103" spans="1:5">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="9" t="s">
         <v>333</v>
       </c>
@@ -3693,7 +3704,7 @@
       </c>
       <c r="E103" s="7"/>
     </row>
-    <row r="104" spans="1:5">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="9" t="s">
         <v>336</v>
       </c>
@@ -3708,7 +3719,7 @@
       </c>
       <c r="E104" s="7"/>
     </row>
-    <row r="105" spans="1:5">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="9" t="s">
         <v>337</v>
       </c>
@@ -3723,7 +3734,7 @@
       </c>
       <c r="E105" s="7"/>
     </row>
-    <row r="106" spans="1:5">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="9" t="s">
         <v>342</v>
       </c>
@@ -3738,7 +3749,7 @@
       </c>
       <c r="E106" s="7"/>
     </row>
-    <row r="107" spans="1:5">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="9" t="s">
         <v>345</v>
       </c>
@@ -3753,7 +3764,7 @@
       </c>
       <c r="E107" s="7"/>
     </row>
-    <row r="108" spans="1:5">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="9" t="s">
         <v>350</v>
       </c>
@@ -3768,7 +3779,7 @@
       </c>
       <c r="E108" s="7"/>
     </row>
-    <row r="109" spans="1:5" ht="30">
+    <row r="109" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A109" s="9" t="s">
         <v>351</v>
       </c>
@@ -3783,7 +3794,7 @@
       </c>
       <c r="E109" s="7"/>
     </row>
-    <row r="110" spans="1:5">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="9" t="s">
         <v>354</v>
       </c>
@@ -3798,7 +3809,7 @@
       </c>
       <c r="E110" s="7"/>
     </row>
-    <row r="111" spans="1:5">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="9" t="s">
         <v>357</v>
       </c>
@@ -3813,7 +3824,7 @@
       </c>
       <c r="E111" s="7"/>
     </row>
-    <row r="112" spans="1:5">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="9" t="s">
         <v>361</v>
       </c>
@@ -3828,7 +3839,7 @@
       </c>
       <c r="E112" s="7"/>
     </row>
-    <row r="113" spans="1:5">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="9" t="s">
         <v>363</v>
       </c>
@@ -3843,7 +3854,7 @@
       </c>
       <c r="E113" s="7"/>
     </row>
-    <row r="114" spans="1:5" ht="30">
+    <row r="114" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A114" s="9" t="s">
         <v>366</v>
       </c>
@@ -3858,7 +3869,7 @@
       </c>
       <c r="E114" s="7"/>
     </row>
-    <row r="115" spans="1:5">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="9" t="s">
         <v>369</v>
       </c>
@@ -3873,7 +3884,7 @@
       </c>
       <c r="E115" s="7"/>
     </row>
-    <row r="116" spans="1:5">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="9" t="s">
         <v>370</v>
       </c>
@@ -3888,7 +3899,7 @@
       </c>
       <c r="E116" s="7"/>
     </row>
-    <row r="117" spans="1:5">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" s="9" t="s">
         <v>371</v>
       </c>
@@ -3903,7 +3914,7 @@
       </c>
       <c r="E117" s="7"/>
     </row>
-    <row r="118" spans="1:5">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" s="9" t="s">
         <v>378</v>
       </c>
@@ -3918,7 +3929,7 @@
       </c>
       <c r="E118" s="7"/>
     </row>
-    <row r="119" spans="1:5">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" s="9" t="s">
         <v>381</v>
       </c>
@@ -3933,7 +3944,7 @@
       </c>
       <c r="E119" s="7"/>
     </row>
-    <row r="120" spans="1:5">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" s="9" t="s">
         <v>384</v>
       </c>
@@ -3948,7 +3959,7 @@
       </c>
       <c r="E120" s="7"/>
     </row>
-    <row r="121" spans="1:5">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="9" t="s">
         <v>387</v>
       </c>
@@ -3963,7 +3974,7 @@
       </c>
       <c r="E121" s="7"/>
     </row>
-    <row r="122" spans="1:5">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" s="7" t="s">
         <v>390</v>
       </c>
@@ -3978,7 +3989,7 @@
       </c>
       <c r="E122" s="7"/>
     </row>
-    <row r="123" spans="1:5">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" s="7" t="s">
         <v>393</v>
       </c>
@@ -3993,7 +4004,7 @@
       </c>
       <c r="E123" s="7"/>
     </row>
-    <row r="124" spans="1:5">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" s="7" t="s">
         <v>396</v>
       </c>
@@ -4008,7 +4019,7 @@
       </c>
       <c r="E124" s="7"/>
     </row>
-    <row r="125" spans="1:5">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" s="9" t="s">
         <v>399</v>
       </c>
@@ -4023,7 +4034,7 @@
       </c>
       <c r="E125" s="7"/>
     </row>
-    <row r="126" spans="1:5">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" s="7" t="s">
         <v>402</v>
       </c>
@@ -4038,7 +4049,7 @@
       </c>
       <c r="E126" s="7"/>
     </row>
-    <row r="127" spans="1:5">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" s="7" t="s">
         <v>405</v>
       </c>
@@ -4053,7 +4064,7 @@
       </c>
       <c r="E127" s="7"/>
     </row>
-    <row r="128" spans="1:5">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" s="7" t="s">
         <v>408</v>
       </c>
@@ -4068,7 +4079,7 @@
       </c>
       <c r="E128" s="7"/>
     </row>
-    <row r="129" spans="1:5">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" s="9" t="s">
         <v>411</v>
       </c>
@@ -4083,7 +4094,7 @@
       </c>
       <c r="E129" s="7"/>
     </row>
-    <row r="130" spans="1:5">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" s="9" t="s">
         <v>414</v>
       </c>
@@ -4098,7 +4109,7 @@
       </c>
       <c r="E130" s="7"/>
     </row>
-    <row r="131" spans="1:5">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" s="9" t="s">
         <v>416</v>
       </c>
@@ -4113,7 +4124,7 @@
       </c>
       <c r="E131" s="7"/>
     </row>
-    <row r="132" spans="1:5">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" s="7" t="s">
         <v>419</v>
       </c>
@@ -4128,7 +4139,7 @@
       </c>
       <c r="E132" s="7"/>
     </row>
-    <row r="133" spans="1:5">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" s="9" t="s">
         <v>422</v>
       </c>
@@ -4143,7 +4154,7 @@
       </c>
       <c r="E133" s="7"/>
     </row>
-    <row r="134" spans="1:5" ht="30">
+    <row r="134" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A134" s="7" t="s">
         <v>425</v>
       </c>
@@ -4158,7 +4169,7 @@
       </c>
       <c r="E134" s="7"/>
     </row>
-    <row r="135" spans="1:5" ht="30">
+    <row r="135" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A135" s="7" t="s">
         <v>426</v>
       </c>
@@ -4173,7 +4184,7 @@
       </c>
       <c r="E135" s="7"/>
     </row>
-    <row r="136" spans="1:5">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" s="9" t="s">
         <v>431</v>
       </c>
@@ -4188,7 +4199,7 @@
       </c>
       <c r="E136" s="7"/>
     </row>
-    <row r="137" spans="1:5">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" s="7" t="s">
         <v>434</v>
       </c>
@@ -4203,7 +4214,7 @@
       </c>
       <c r="E137" s="7"/>
     </row>
-    <row r="138" spans="1:5" ht="45">
+    <row r="138" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A138" s="7" t="s">
         <v>435</v>
       </c>
@@ -4218,7 +4229,7 @@
       </c>
       <c r="E138" s="7"/>
     </row>
-    <row r="139" spans="1:5" ht="30">
+    <row r="139" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A139" s="7" t="s">
         <v>436</v>
       </c>
@@ -4233,7 +4244,7 @@
       </c>
       <c r="E139" s="7"/>
     </row>
-    <row r="140" spans="1:5">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" s="17" t="s">
         <v>443</v>
       </c>
@@ -4248,7 +4259,7 @@
       </c>
       <c r="E140" s="7"/>
     </row>
-    <row r="141" spans="1:5">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" s="17" t="s">
         <v>446</v>
       </c>
@@ -4263,7 +4274,7 @@
       </c>
       <c r="E141" s="7"/>
     </row>
-    <row r="142" spans="1:5">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" s="17" t="s">
         <v>449</v>
       </c>
@@ -4278,7 +4289,7 @@
       </c>
       <c r="E142" s="7"/>
     </row>
-    <row r="143" spans="1:5">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" s="17" t="s">
         <v>452</v>
       </c>
@@ -4293,7 +4304,7 @@
       </c>
       <c r="E143" s="7"/>
     </row>
-    <row r="144" spans="1:5">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" s="17" t="s">
         <v>453</v>
       </c>
@@ -4308,7 +4319,7 @@
       </c>
       <c r="E144" s="7"/>
     </row>
-    <row r="145" spans="1:5">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" s="17" t="s">
         <v>458</v>
       </c>
@@ -4323,7 +4334,7 @@
       </c>
       <c r="E145" s="7"/>
     </row>
-    <row r="146" spans="1:5">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" s="17" t="s">
         <v>461</v>
       </c>
@@ -4338,7 +4349,7 @@
       </c>
       <c r="E146" s="7"/>
     </row>
-    <row r="147" spans="1:5">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" s="17" t="s">
         <v>464</v>
       </c>
@@ -4353,7 +4364,7 @@
       </c>
       <c r="E147" s="7"/>
     </row>
-    <row r="148" spans="1:5">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" s="17" t="s">
         <v>467</v>
       </c>
@@ -4368,7 +4379,7 @@
       </c>
       <c r="E148" s="7"/>
     </row>
-    <row r="149" spans="1:5">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" s="7" t="s">
         <v>470</v>
       </c>
@@ -4383,7 +4394,7 @@
       </c>
       <c r="E149" s="7"/>
     </row>
-    <row r="150" spans="1:5">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" s="7" t="s">
         <v>471</v>
       </c>
@@ -4398,7 +4409,7 @@
       </c>
       <c r="E150" s="7"/>
     </row>
-    <row r="151" spans="1:5">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" s="7" t="s">
         <v>472</v>
       </c>
@@ -4413,7 +4424,7 @@
       </c>
       <c r="E151" s="7"/>
     </row>
-    <row r="152" spans="1:5" ht="30">
+    <row r="152" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A152" s="7" t="s">
         <v>479</v>
       </c>
@@ -4428,7 +4439,7 @@
       </c>
       <c r="E152" s="7"/>
     </row>
-    <row r="153" spans="1:5" ht="45">
+    <row r="153" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A153" s="17" t="s">
         <v>482</v>
       </c>
@@ -4443,7 +4454,7 @@
       </c>
       <c r="E153" s="7"/>
     </row>
-    <row r="154" spans="1:5">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" s="17" t="s">
         <v>484</v>
       </c>
@@ -4458,7 +4469,7 @@
       </c>
       <c r="E154" s="7"/>
     </row>
-    <row r="155" spans="1:5">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" s="7" t="s">
         <v>486</v>
       </c>
@@ -4473,7 +4484,7 @@
       </c>
       <c r="E155" s="7"/>
     </row>
-    <row r="156" spans="1:5">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" s="7" t="s">
         <v>489</v>
       </c>
@@ -4488,7 +4499,7 @@
       </c>
       <c r="E156" s="7"/>
     </row>
-    <row r="157" spans="1:5">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" s="7" t="s">
         <v>492</v>
       </c>
@@ -4503,7 +4514,7 @@
       </c>
       <c r="E157" s="7"/>
     </row>
-    <row r="158" spans="1:5" ht="30">
+    <row r="158" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A158" s="7" t="s">
         <v>495</v>
       </c>
@@ -4518,7 +4529,7 @@
       </c>
       <c r="E158" s="7"/>
     </row>
-    <row r="159" spans="1:5" ht="30">
+    <row r="159" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A159" s="7" t="s">
         <v>496</v>
       </c>
@@ -4533,7 +4544,7 @@
       </c>
       <c r="E159" s="7"/>
     </row>
-    <row r="160" spans="1:5">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" s="7" t="s">
         <v>503</v>
       </c>
@@ -4548,7 +4559,7 @@
       </c>
       <c r="E160" s="7"/>
     </row>
-    <row r="161" spans="1:5">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161" s="7" t="s">
         <v>504</v>
       </c>
@@ -4563,7 +4574,7 @@
       </c>
       <c r="E161" s="7"/>
     </row>
-    <row r="162" spans="1:5">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162" s="7" t="s">
         <v>507</v>
       </c>
@@ -4578,7 +4589,7 @@
       </c>
       <c r="E162" s="7"/>
     </row>
-    <row r="163" spans="1:5">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" s="7" t="s">
         <v>512</v>
       </c>
@@ -4593,7 +4604,7 @@
       </c>
       <c r="E163" s="7"/>
     </row>
-    <row r="164" spans="1:5" ht="30">
+    <row r="164" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A164" s="7" t="s">
         <v>515</v>
       </c>
@@ -4608,7 +4619,7 @@
       </c>
       <c r="E164" s="7"/>
     </row>
-    <row r="165" spans="1:5">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165" s="7" t="s">
         <v>518</v>
       </c>
@@ -4623,7 +4634,7 @@
       </c>
       <c r="E165" s="7"/>
     </row>
-    <row r="166" spans="1:5" ht="30">
+    <row r="166" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A166" s="7" t="s">
         <v>521</v>
       </c>
@@ -4638,7 +4649,7 @@
       </c>
       <c r="E166" s="7"/>
     </row>
-    <row r="167" spans="1:5">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167" s="7" t="s">
         <v>525</v>
       </c>
@@ -4653,7 +4664,7 @@
       </c>
       <c r="E167" s="7"/>
     </row>
-    <row r="168" spans="1:5">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" s="7" t="s">
         <v>527</v>
       </c>
@@ -4668,7 +4679,7 @@
       </c>
       <c r="E168" s="7"/>
     </row>
-    <row r="169" spans="1:5">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" s="7" t="s">
         <v>530</v>
       </c>
@@ -4683,7 +4694,7 @@
       </c>
       <c r="E169" s="7"/>
     </row>
-    <row r="170" spans="1:5">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170" s="7" t="s">
         <v>531</v>
       </c>
@@ -4698,7 +4709,7 @@
       </c>
       <c r="E170" s="7"/>
     </row>
-    <row r="171" spans="1:5">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171" s="7" t="s">
         <v>532</v>
       </c>
@@ -4713,7 +4724,7 @@
       </c>
       <c r="E171" s="7"/>
     </row>
-    <row r="172" spans="1:5" ht="30">
+    <row r="172" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A172" s="7" t="s">
         <v>539</v>
       </c>
@@ -4728,7 +4739,7 @@
       </c>
       <c r="E172" s="7"/>
     </row>
-    <row r="173" spans="1:5">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173" s="9" t="s">
         <v>541</v>
       </c>
@@ -4743,7 +4754,7 @@
       </c>
       <c r="E173" s="7"/>
     </row>
-    <row r="174" spans="1:5">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A174" s="9" t="s">
         <v>542</v>
       </c>
@@ -4758,7 +4769,7 @@
       </c>
       <c r="E174" s="7"/>
     </row>
-    <row r="175" spans="1:5">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A175" s="9" t="s">
         <v>543</v>
       </c>
@@ -4773,7 +4784,7 @@
       </c>
       <c r="E175" s="7"/>
     </row>
-    <row r="176" spans="1:5">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A176" s="9" t="s">
         <v>544</v>
       </c>
@@ -4787,6 +4798,21 @@
         <v>5</v>
       </c>
       <c r="E176" s="7"/>
+    </row>
+    <row r="177" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A177" s="7" t="s">
+        <v>552</v>
+      </c>
+      <c r="B177" s="7" t="s">
+        <v>553</v>
+      </c>
+      <c r="C177" s="8" t="s">
+        <v>554</v>
+      </c>
+      <c r="D177" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E177" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -4799,14 +4825,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView topLeftCell="A10" zoomScale="80" workbookViewId="0">
       <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
@@ -4814,7 +4840,7 @@
     <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>35</v>
       </c>
@@ -4828,7 +4854,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>37</v>
       </c>
@@ -4840,7 +4866,7 @@
       </c>
       <c r="D2" s="7"/>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>38</v>
       </c>
@@ -4852,7 +4878,7 @@
       </c>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>39</v>
       </c>
@@ -4864,7 +4890,7 @@
       </c>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>40</v>
       </c>
@@ -4876,7 +4902,7 @@
       </c>
       <c r="D5" s="7"/>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>41</v>
       </c>
@@ -4888,7 +4914,7 @@
       </c>
       <c r="D6" s="7"/>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>42</v>
       </c>
@@ -4900,7 +4926,7 @@
       </c>
       <c r="D7" s="7"/>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>43</v>
       </c>
@@ -4912,7 +4938,7 @@
       </c>
       <c r="D8" s="7"/>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>44</v>
       </c>
@@ -4924,7 +4950,7 @@
       </c>
       <c r="D9" s="7"/>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>45</v>
       </c>
@@ -4936,7 +4962,7 @@
       </c>
       <c r="D10" s="7"/>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>46</v>
       </c>
@@ -4948,7 +4974,7 @@
       </c>
       <c r="D11" s="7"/>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>48</v>
       </c>
@@ -4960,7 +4986,7 @@
       </c>
       <c r="D12" s="7"/>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>49</v>
       </c>
@@ -4972,7 +4998,7 @@
       </c>
       <c r="D13" s="7"/>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>50</v>
       </c>
@@ -4984,7 +5010,7 @@
       </c>
       <c r="D14" s="7"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>51</v>
       </c>
@@ -4996,7 +5022,7 @@
       </c>
       <c r="D15" s="7"/>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>52</v>
       </c>
@@ -5008,7 +5034,7 @@
       </c>
       <c r="D16" s="7"/>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>53</v>
       </c>
@@ -5020,7 +5046,7 @@
       </c>
       <c r="D17" s="7"/>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>54</v>
       </c>
@@ -5032,7 +5058,7 @@
       </c>
       <c r="D18" s="7"/>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>55</v>
       </c>
@@ -5044,7 +5070,7 @@
       </c>
       <c r="D19" s="7"/>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>56</v>
       </c>
@@ -5056,7 +5082,7 @@
       </c>
       <c r="D20" s="7"/>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>57</v>
       </c>
@@ -5068,7 +5094,7 @@
       </c>
       <c r="D21" s="7"/>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>58</v>
       </c>
@@ -5080,7 +5106,7 @@
       </c>
       <c r="D22" s="7"/>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>59</v>
       </c>
@@ -5092,7 +5118,7 @@
       </c>
       <c r="D23" s="7"/>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>60</v>
       </c>
@@ -5104,7 +5130,7 @@
       </c>
       <c r="D24" s="7"/>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>61</v>
       </c>
@@ -5116,7 +5142,7 @@
       </c>
       <c r="D25" s="7"/>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>47</v>
       </c>
@@ -5135,14 +5161,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A19" sqref="A19:XFD19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
@@ -5150,7 +5176,7 @@
     <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>35</v>
       </c>
@@ -5164,7 +5190,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>37</v>
       </c>
@@ -5176,7 +5202,7 @@
       </c>
       <c r="D2" s="7"/>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>38</v>
       </c>
@@ -5188,7 +5214,7 @@
       </c>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>39</v>
       </c>
@@ -5200,7 +5226,7 @@
       </c>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>40</v>
       </c>
@@ -5212,7 +5238,7 @@
       </c>
       <c r="D5" s="7"/>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>41</v>
       </c>
@@ -5224,7 +5250,7 @@
       </c>
       <c r="D6" s="7"/>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>42</v>
       </c>
@@ -5236,7 +5262,7 @@
       </c>
       <c r="D7" s="7"/>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>43</v>
       </c>
@@ -5248,7 +5274,7 @@
       </c>
       <c r="D8" s="7"/>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>44</v>
       </c>
@@ -5260,7 +5286,7 @@
       </c>
       <c r="D9" s="7"/>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>45</v>
       </c>
@@ -5272,7 +5298,7 @@
       </c>
       <c r="D10" s="7"/>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>46</v>
       </c>
@@ -5284,7 +5310,7 @@
       </c>
       <c r="D11" s="7"/>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>47</v>
       </c>
@@ -5296,7 +5322,7 @@
       </c>
       <c r="D12" s="7"/>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>48</v>
       </c>
@@ -5308,7 +5334,7 @@
       </c>
       <c r="D13" s="7"/>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>49</v>
       </c>
@@ -5320,7 +5346,7 @@
       </c>
       <c r="D14" s="7"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>50</v>
       </c>
@@ -5332,7 +5358,7 @@
       </c>
       <c r="D15" s="7"/>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>51</v>
       </c>
@@ -5344,7 +5370,7 @@
       </c>
       <c r="D16" s="7"/>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>52</v>
       </c>
@@ -5356,7 +5382,7 @@
       </c>
       <c r="D17" s="7"/>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>53</v>
       </c>
@@ -5368,7 +5394,7 @@
       </c>
       <c r="D18" s="7"/>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>54</v>
       </c>
@@ -5380,7 +5406,7 @@
       </c>
       <c r="D19" s="7"/>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>55</v>
       </c>
@@ -5392,7 +5418,7 @@
       </c>
       <c r="D20" s="7"/>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>56</v>
       </c>
@@ -5404,7 +5430,7 @@
       </c>
       <c r="D21" s="7"/>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>57</v>
       </c>
@@ -5416,7 +5442,7 @@
       </c>
       <c r="D22" s="7"/>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>58</v>
       </c>
@@ -5428,7 +5454,7 @@
       </c>
       <c r="D23" s="7"/>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>59</v>
       </c>
@@ -5440,7 +5466,7 @@
       </c>
       <c r="D24" s="7"/>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>60</v>
       </c>
@@ -5452,7 +5478,7 @@
       </c>
       <c r="D25" s="7"/>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>61</v>
       </c>

</xml_diff>

<commit_message>
Adds WAT-144 testscript and related changes
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/WAT.xlsx
+++ b/src/test/resources/xls/WAT.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="867" uniqueCount="555">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="871" uniqueCount="558">
   <si>
     <t>TCID</t>
   </si>
@@ -1683,6 +1683,15 @@
   </si>
   <si>
     <t>Verify that for a Combined author The left-to-right order of the metrics in the Author Metadata area of the Author Record should be: h-index Sum of Times Cited Citing Articles</t>
+  </si>
+  <si>
+    <t>WAT144</t>
+  </si>
+  <si>
+    <t>WAT-1300</t>
+  </si>
+  <si>
+    <t>Verify that for a Combined author the "Total Citing Publications" value will be less than or equal to the "Total Citations" value.</t>
   </si>
 </sst>
 </file>
@@ -1744,7 +1753,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -1767,11 +1776,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1809,6 +1833,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2142,10 +2169,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E177"/>
+  <dimension ref="A1:E178"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A155" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C181" sqref="C181"/>
+      <selection activeCell="C178" sqref="C178"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4813,6 +4840,20 @@
         <v>5</v>
       </c>
       <c r="E177" s="7"/>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A178" s="7" t="s">
+        <v>555</v>
+      </c>
+      <c r="B178" s="7" t="s">
+        <v>556</v>
+      </c>
+      <c r="C178" s="18" t="s">
+        <v>557</v>
+      </c>
+      <c r="D178" s="9" t="s">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Adds WAT-145 testscript and related changes
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/WAT.xlsx
+++ b/src/test/resources/xls/WAT.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="871" uniqueCount="558">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="875" uniqueCount="561">
   <si>
     <t>TCID</t>
   </si>
@@ -1692,6 +1692,15 @@
   </si>
   <si>
     <t>Verify that for a Combined author the "Total Citing Publications" value will be less than or equal to the "Total Citations" value.</t>
+  </si>
+  <si>
+    <t>Verify that on the Combined Author Record page, in the Combined Author Metadata panel, the system should display a "Total Citing Publications" metric.</t>
+  </si>
+  <si>
+    <t>WAT145</t>
+  </si>
+  <si>
+    <t>WAT-1298</t>
   </si>
 </sst>
 </file>
@@ -2169,10 +2178,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E178"/>
+  <dimension ref="A1:E179"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A155" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C178" sqref="C178"/>
+      <selection activeCell="B179" sqref="B179"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4852,6 +4861,20 @@
         <v>557</v>
       </c>
       <c r="D178" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A179" s="7" t="s">
+        <v>559</v>
+      </c>
+      <c r="B179" s="7" t="s">
+        <v>560</v>
+      </c>
+      <c r="C179" s="18" t="s">
+        <v>558</v>
+      </c>
+      <c r="D179" s="9" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adds WAT-146 test script and related changes
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/WAT.xlsx
+++ b/src/test/resources/xls/WAT.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="875" uniqueCount="561">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="879" uniqueCount="564">
   <si>
     <t>TCID</t>
   </si>
@@ -1701,6 +1701,15 @@
   </si>
   <si>
     <t>WAT-1298</t>
+  </si>
+  <si>
+    <t>WAT146</t>
+  </si>
+  <si>
+    <t>WAT-1305</t>
+  </si>
+  <si>
+    <t>Verify that the metrics should carry labels (spelled/worded exactly as listed above)</t>
   </si>
 </sst>
 </file>
@@ -1762,7 +1771,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -1785,26 +1794,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1842,9 +1836,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2178,10 +2169,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E179"/>
+  <dimension ref="A1:E180"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A155" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B179" sqref="B179"/>
+    <sheetView tabSelected="1" topLeftCell="A167" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E180" sqref="A1:E180"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4857,12 +4848,13 @@
       <c r="B178" s="7" t="s">
         <v>556</v>
       </c>
-      <c r="C178" s="18" t="s">
+      <c r="C178" s="16" t="s">
         <v>557</v>
       </c>
       <c r="D178" s="9" t="s">
         <v>5</v>
       </c>
+      <c r="E178" s="7"/>
     </row>
     <row r="179" spans="1:5" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A179" s="7" t="s">
@@ -4871,12 +4863,28 @@
       <c r="B179" s="7" t="s">
         <v>560</v>
       </c>
-      <c r="C179" s="18" t="s">
+      <c r="C179" s="16" t="s">
         <v>558</v>
       </c>
       <c r="D179" s="9" t="s">
         <v>5</v>
       </c>
+      <c r="E179" s="7"/>
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A180" s="7" t="s">
+        <v>561</v>
+      </c>
+      <c r="B180" s="7" t="s">
+        <v>562</v>
+      </c>
+      <c r="C180" s="16" t="s">
+        <v>563</v>
+      </c>
+      <c r="D180" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E180" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Adds WAT-147 testscript and related changes
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/WAT.xlsx
+++ b/src/test/resources/xls/WAT.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="879" uniqueCount="564">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="883" uniqueCount="567">
   <si>
     <t>TCID</t>
   </si>
@@ -1710,6 +1710,15 @@
   </si>
   <si>
     <t>Verify that the metrics should carry labels (spelled/worded exactly as listed above)</t>
+  </si>
+  <si>
+    <t>WAT147</t>
+  </si>
+  <si>
+    <t>WAT-1296</t>
+  </si>
+  <si>
+    <t>"Verify that for a single author The left-to-right order of the metrics in the Author Metadata area of the Author Record should be: h-index Sum of Times Cited Citing Articles"</t>
   </si>
 </sst>
 </file>
@@ -1771,7 +1780,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -1794,11 +1803,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1836,6 +1860,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2169,10 +2196,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E180"/>
+  <dimension ref="A1:E181"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A167" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E180" sqref="A1:E180"/>
+      <selection activeCell="C184" sqref="C184"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4885,6 +4912,21 @@
         <v>5</v>
       </c>
       <c r="E180" s="7"/>
+    </row>
+    <row r="181" spans="1:5" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A181" s="7" t="s">
+        <v>564</v>
+      </c>
+      <c r="B181" s="7" t="s">
+        <v>565</v>
+      </c>
+      <c r="C181" s="18" t="s">
+        <v>566</v>
+      </c>
+      <c r="D181" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E181" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Adds WAT-148 testscript and related changes
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/WAT.xlsx
+++ b/src/test/resources/xls/WAT.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="883" uniqueCount="567">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="887" uniqueCount="570">
   <si>
     <t>TCID</t>
   </si>
@@ -1719,6 +1719,15 @@
   </si>
   <si>
     <t>"Verify that for a single author The left-to-right order of the metrics in the Author Metadata area of the Author Record should be: h-index Sum of Times Cited Citing Articles"</t>
+  </si>
+  <si>
+    <t>WAT148</t>
+  </si>
+  <si>
+    <t>WAT-1292</t>
+  </si>
+  <si>
+    <t>Verify that for a single author the "Total Citing Publications" value will be less than or equal to the "Total Citations" value.</t>
   </si>
 </sst>
 </file>
@@ -2196,10 +2205,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E181"/>
+  <dimension ref="A1:E182"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A167" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C184" sqref="C184"/>
+      <selection activeCell="C186" sqref="C186"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4927,6 +4936,21 @@
         <v>5</v>
       </c>
       <c r="E181" s="7"/>
+    </row>
+    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A182" s="7" t="s">
+        <v>567</v>
+      </c>
+      <c r="B182" s="7" t="s">
+        <v>568</v>
+      </c>
+      <c r="C182" s="18" t="s">
+        <v>569</v>
+      </c>
+      <c r="D182" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E182" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Adds WAT-149 testscript and related changes
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/WAT.xlsx
+++ b/src/test/resources/xls/WAT.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="887" uniqueCount="570">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="891" uniqueCount="573">
   <si>
     <t>TCID</t>
   </si>
@@ -1728,6 +1728,15 @@
   </si>
   <si>
     <t>Verify that for a single author the "Total Citing Publications" value will be less than or equal to the "Total Citations" value.</t>
+  </si>
+  <si>
+    <t>WAT149</t>
+  </si>
+  <si>
+    <t>Verify that on the Single Author Record page, in the Combined Author Metadata panel, the system should display a "Total Citing Publications" metric.</t>
+  </si>
+  <si>
+    <t>WAT-1290</t>
   </si>
 </sst>
 </file>
@@ -2205,10 +2214,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E182"/>
+  <dimension ref="A1:E183"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A167" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C186" sqref="C186"/>
+      <selection activeCell="C192" sqref="C192"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4951,6 +4960,21 @@
         <v>5</v>
       </c>
       <c r="E182" s="7"/>
+    </row>
+    <row r="183" spans="1:5" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A183" s="7" t="s">
+        <v>570</v>
+      </c>
+      <c r="B183" s="7" t="s">
+        <v>572</v>
+      </c>
+      <c r="C183" s="16" t="s">
+        <v>571</v>
+      </c>
+      <c r="D183" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E183" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
WAT new scritps implementation
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/WAT.xlsx
+++ b/src/test/resources/xls/WAT.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13305" windowHeight="2415"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="891" uniqueCount="573">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="899" uniqueCount="579">
   <si>
     <t>TCID</t>
   </si>
@@ -1737,13 +1737,31 @@
   </si>
   <si>
     <t>WAT-1290</t>
+  </si>
+  <si>
+    <t>WAT184</t>
+  </si>
+  <si>
+    <t>WAT185</t>
+  </si>
+  <si>
+    <t>WAT-343</t>
+  </si>
+  <si>
+    <t>Verify that System must display the author's ORCiD (when available) as a URI</t>
+  </si>
+  <si>
+    <t>Verify that System must display the author's ResearcherID (when available)</t>
+  </si>
+  <si>
+    <t>WAT-345</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1798,7 +1816,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -1821,26 +1839,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1878,9 +1881,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1970,7 +1970,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2002,10 +2002,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2037,7 +2036,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2213,14 +2211,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E183"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E185"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A167" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="C192" sqref="C192"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="30.5703125" customWidth="1" collapsed="1"/>
@@ -2229,7 +2227,7 @@
     <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2246,7 +2244,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -2261,7 +2259,7 @@
       </c>
       <c r="E2" s="4"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -2276,7 +2274,7 @@
       </c>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" s="7" t="s">
         <v>11</v>
       </c>
@@ -2291,7 +2289,7 @@
       </c>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" s="7" t="s">
         <v>12</v>
       </c>
@@ -2306,7 +2304,7 @@
       </c>
       <c r="E5" s="7"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" s="7" t="s">
         <v>14</v>
       </c>
@@ -2321,7 +2319,7 @@
       </c>
       <c r="E6" s="7"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" s="7" t="s">
         <v>17</v>
       </c>
@@ -2336,7 +2334,7 @@
       </c>
       <c r="E7" s="7"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" s="7" t="s">
         <v>20</v>
       </c>
@@ -2351,7 +2349,7 @@
       </c>
       <c r="E8" s="7"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" s="7" t="s">
         <v>22</v>
       </c>
@@ -2366,7 +2364,7 @@
       </c>
       <c r="E9" s="7"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10" s="7" t="s">
         <v>23</v>
       </c>
@@ -2381,7 +2379,7 @@
       </c>
       <c r="E10" s="7"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11" s="7" t="s">
         <v>24</v>
       </c>
@@ -2396,7 +2394,7 @@
       </c>
       <c r="E11" s="7"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12" s="7" t="s">
         <v>25</v>
       </c>
@@ -2411,7 +2409,7 @@
       </c>
       <c r="E12" s="7"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13" s="7" t="s">
         <v>62</v>
       </c>
@@ -2426,7 +2424,7 @@
       </c>
       <c r="E13" s="7"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="A14" s="7" t="s">
         <v>63</v>
       </c>
@@ -2441,7 +2439,7 @@
       </c>
       <c r="E14" s="7"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="A15" s="7" t="s">
         <v>64</v>
       </c>
@@ -2456,7 +2454,7 @@
       </c>
       <c r="E15" s="7"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="A16" s="7" t="s">
         <v>65</v>
       </c>
@@ -2471,7 +2469,7 @@
       </c>
       <c r="E16" s="7"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5">
       <c r="A17" s="7" t="s">
         <v>74</v>
       </c>
@@ -2486,7 +2484,7 @@
       </c>
       <c r="E17" s="7"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5">
       <c r="A18" s="7" t="s">
         <v>75</v>
       </c>
@@ -2501,7 +2499,7 @@
       </c>
       <c r="E18" s="7"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5">
       <c r="A19" s="7" t="s">
         <v>79</v>
       </c>
@@ -2516,7 +2514,7 @@
       </c>
       <c r="E19" s="7"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5">
       <c r="A20" s="7" t="s">
         <v>81</v>
       </c>
@@ -2531,7 +2529,7 @@
       </c>
       <c r="E20" s="7"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5">
       <c r="A21" s="7" t="s">
         <v>82</v>
       </c>
@@ -2546,7 +2544,7 @@
       </c>
       <c r="E21" s="7"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5">
       <c r="A22" s="7" t="s">
         <v>88</v>
       </c>
@@ -2561,7 +2559,7 @@
       </c>
       <c r="E22" s="7"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5">
       <c r="A23" s="7" t="s">
         <v>90</v>
       </c>
@@ -2576,7 +2574,7 @@
       </c>
       <c r="E23" s="7"/>
     </row>
-    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="30">
       <c r="A24" s="9" t="s">
         <v>94</v>
       </c>
@@ -2591,7 +2589,7 @@
       </c>
       <c r="E24" s="7"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5">
       <c r="A25" s="9" t="s">
         <v>96</v>
       </c>
@@ -2606,7 +2604,7 @@
       </c>
       <c r="E25" s="7"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5">
       <c r="A26" s="9" t="s">
         <v>98</v>
       </c>
@@ -2621,7 +2619,7 @@
       </c>
       <c r="E26" s="7"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5">
       <c r="A27" s="9" t="s">
         <v>102</v>
       </c>
@@ -2636,7 +2634,7 @@
       </c>
       <c r="E27" s="7"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5">
       <c r="A28" s="9" t="s">
         <v>105</v>
       </c>
@@ -2651,7 +2649,7 @@
       </c>
       <c r="E28" s="7"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5">
       <c r="A29" s="9" t="s">
         <v>108</v>
       </c>
@@ -2666,7 +2664,7 @@
       </c>
       <c r="E29" s="7"/>
     </row>
-    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" ht="30">
       <c r="A30" s="9" t="s">
         <v>110</v>
       </c>
@@ -2681,7 +2679,7 @@
       </c>
       <c r="E30" s="7"/>
     </row>
-    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" ht="30">
       <c r="A31" s="9" t="s">
         <v>114</v>
       </c>
@@ -2696,7 +2694,7 @@
       </c>
       <c r="E31" s="7"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5">
       <c r="A32" s="9" t="s">
         <v>119</v>
       </c>
@@ -2711,7 +2709,7 @@
       </c>
       <c r="E32" s="7"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5">
       <c r="A33" s="9" t="s">
         <v>120</v>
       </c>
@@ -2726,7 +2724,7 @@
       </c>
       <c r="E33" s="7"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5">
       <c r="A34" s="9" t="s">
         <v>125</v>
       </c>
@@ -2741,7 +2739,7 @@
       </c>
       <c r="E34" s="7"/>
     </row>
-    <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" ht="30">
       <c r="A35" s="9" t="s">
         <v>128</v>
       </c>
@@ -2756,7 +2754,7 @@
       </c>
       <c r="E35" s="7"/>
     </row>
-    <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" ht="30">
       <c r="A36" s="9" t="s">
         <v>131</v>
       </c>
@@ -2771,7 +2769,7 @@
       </c>
       <c r="E36" s="7"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5">
       <c r="A37" s="9" t="s">
         <v>134</v>
       </c>
@@ -2786,7 +2784,7 @@
       </c>
       <c r="E37" s="7"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5">
       <c r="A38" s="9" t="s">
         <v>137</v>
       </c>
@@ -2801,7 +2799,7 @@
       </c>
       <c r="E38" s="7"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5">
       <c r="A39" s="9" t="s">
         <v>140</v>
       </c>
@@ -2816,7 +2814,7 @@
       </c>
       <c r="E39" s="7"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5">
       <c r="A40" s="9" t="s">
         <v>143</v>
       </c>
@@ -2831,7 +2829,7 @@
       </c>
       <c r="E40" s="7"/>
     </row>
-    <row r="41" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" ht="30">
       <c r="A41" s="9" t="s">
         <v>145</v>
       </c>
@@ -2846,7 +2844,7 @@
       </c>
       <c r="E41" s="7"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5">
       <c r="A42" s="9" t="s">
         <v>147</v>
       </c>
@@ -2861,7 +2859,7 @@
       </c>
       <c r="E42" s="7"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5">
       <c r="A43" s="9" t="s">
         <v>150</v>
       </c>
@@ -2876,7 +2874,7 @@
       </c>
       <c r="E43" s="7"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5">
       <c r="A44" s="9" t="s">
         <v>153</v>
       </c>
@@ -2891,7 +2889,7 @@
       </c>
       <c r="E44" s="7"/>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5">
       <c r="A45" s="9" t="s">
         <v>155</v>
       </c>
@@ -2906,7 +2904,7 @@
       </c>
       <c r="E45" s="7"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5">
       <c r="A46" s="12" t="s">
         <v>158</v>
       </c>
@@ -2921,7 +2919,7 @@
       </c>
       <c r="E46" s="7"/>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5">
       <c r="A47" s="12" t="s">
         <v>159</v>
       </c>
@@ -2936,7 +2934,7 @@
       </c>
       <c r="E47" s="7"/>
     </row>
-    <row r="48" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" ht="30">
       <c r="A48" s="12" t="s">
         <v>160</v>
       </c>
@@ -2951,7 +2949,7 @@
       </c>
       <c r="E48" s="7"/>
     </row>
-    <row r="49" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" ht="30">
       <c r="A49" s="12" t="s">
         <v>161</v>
       </c>
@@ -2966,7 +2964,7 @@
       </c>
       <c r="E49" s="7"/>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5">
       <c r="A50" s="12" t="s">
         <v>164</v>
       </c>
@@ -2981,7 +2979,7 @@
       </c>
       <c r="E50" s="7"/>
     </row>
-    <row r="51" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" ht="30">
       <c r="A51" s="9" t="s">
         <v>173</v>
       </c>
@@ -2996,7 +2994,7 @@
       </c>
       <c r="E51" s="7"/>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5">
       <c r="A52" s="9" t="s">
         <v>174</v>
       </c>
@@ -3011,7 +3009,7 @@
       </c>
       <c r="E52" s="7"/>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5">
       <c r="A53" s="9" t="s">
         <v>179</v>
       </c>
@@ -3026,7 +3024,7 @@
       </c>
       <c r="E53" s="7"/>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5">
       <c r="A54" s="9" t="s">
         <v>180</v>
       </c>
@@ -3041,7 +3039,7 @@
       </c>
       <c r="E54" s="7"/>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5">
       <c r="A55" s="9" t="s">
         <v>185</v>
       </c>
@@ -3056,7 +3054,7 @@
       </c>
       <c r="E55" s="7"/>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5">
       <c r="A56" s="9" t="s">
         <v>188</v>
       </c>
@@ -3071,7 +3069,7 @@
       </c>
       <c r="E56" s="7"/>
     </row>
-    <row r="57" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" ht="30">
       <c r="A57" s="9" t="s">
         <v>191</v>
       </c>
@@ -3086,7 +3084,7 @@
       </c>
       <c r="E57" s="7"/>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5">
       <c r="A58" s="9" t="s">
         <v>194</v>
       </c>
@@ -3101,7 +3099,7 @@
       </c>
       <c r="E58" s="7"/>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5">
       <c r="A59" s="7" t="s">
         <v>196</v>
       </c>
@@ -3116,7 +3114,7 @@
       </c>
       <c r="E59" s="7"/>
     </row>
-    <row r="60" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" ht="45">
       <c r="A60" s="7" t="s">
         <v>199</v>
       </c>
@@ -3131,7 +3129,7 @@
       </c>
       <c r="E60" s="7"/>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5">
       <c r="A61" s="9" t="s">
         <v>202</v>
       </c>
@@ -3146,7 +3144,7 @@
       </c>
       <c r="E61" s="7"/>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5">
       <c r="A62" s="9" t="s">
         <v>204</v>
       </c>
@@ -3161,7 +3159,7 @@
       </c>
       <c r="E62" s="7"/>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5">
       <c r="A63" s="9" t="s">
         <v>206</v>
       </c>
@@ -3176,7 +3174,7 @@
       </c>
       <c r="E63" s="7"/>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5">
       <c r="A64" s="9" t="s">
         <v>208</v>
       </c>
@@ -3191,7 +3189,7 @@
       </c>
       <c r="E64" s="7"/>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5">
       <c r="A65" s="9" t="s">
         <v>217</v>
       </c>
@@ -3206,7 +3204,7 @@
       </c>
       <c r="E65" s="7"/>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5">
       <c r="A66" s="9" t="s">
         <v>218</v>
       </c>
@@ -3221,7 +3219,7 @@
       </c>
       <c r="E66" s="7"/>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5">
       <c r="A67" s="9" t="s">
         <v>223</v>
       </c>
@@ -3236,7 +3234,7 @@
       </c>
       <c r="E67" s="7"/>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5">
       <c r="A68" s="9" t="s">
         <v>224</v>
       </c>
@@ -3251,7 +3249,7 @@
       </c>
       <c r="E68" s="7"/>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5">
       <c r="A69" s="9" t="s">
         <v>225</v>
       </c>
@@ -3266,7 +3264,7 @@
       </c>
       <c r="E69" s="7"/>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5">
       <c r="A70" s="9" t="s">
         <v>226</v>
       </c>
@@ -3281,7 +3279,7 @@
       </c>
       <c r="E70" s="7"/>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5">
       <c r="A71" s="9" t="s">
         <v>233</v>
       </c>
@@ -3296,7 +3294,7 @@
       </c>
       <c r="E71" s="7"/>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5">
       <c r="A72" s="9" t="s">
         <v>237</v>
       </c>
@@ -3311,7 +3309,7 @@
       </c>
       <c r="E72" s="7"/>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5">
       <c r="A73" s="9" t="s">
         <v>239</v>
       </c>
@@ -3326,7 +3324,7 @@
       </c>
       <c r="E73" s="7"/>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5">
       <c r="A74" s="9" t="s">
         <v>243</v>
       </c>
@@ -3341,7 +3339,7 @@
       </c>
       <c r="E74" s="7"/>
     </row>
-    <row r="75" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" ht="30">
       <c r="A75" s="9" t="s">
         <v>245</v>
       </c>
@@ -3356,7 +3354,7 @@
       </c>
       <c r="E75" s="7"/>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5">
       <c r="A76" s="9" t="s">
         <v>248</v>
       </c>
@@ -3371,7 +3369,7 @@
       </c>
       <c r="E76" s="7"/>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5">
       <c r="A77" s="9" t="s">
         <v>256</v>
       </c>
@@ -3386,7 +3384,7 @@
       </c>
       <c r="E77" s="7"/>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5">
       <c r="A78" s="9" t="s">
         <v>257</v>
       </c>
@@ -3401,7 +3399,7 @@
       </c>
       <c r="E78" s="7"/>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5">
       <c r="A79" s="9" t="s">
         <v>261</v>
       </c>
@@ -3416,7 +3414,7 @@
       </c>
       <c r="E79" s="7"/>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5">
       <c r="A80" s="9" t="s">
         <v>264</v>
       </c>
@@ -3431,7 +3429,7 @@
       </c>
       <c r="E80" s="7"/>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5">
       <c r="A81" s="9" t="s">
         <v>267</v>
       </c>
@@ -3446,7 +3444,7 @@
       </c>
       <c r="E81" s="7"/>
     </row>
-    <row r="82" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" ht="30">
       <c r="A82" s="9" t="s">
         <v>269</v>
       </c>
@@ -3461,7 +3459,7 @@
       </c>
       <c r="E82" s="7"/>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5">
       <c r="A83" s="9" t="s">
         <v>274</v>
       </c>
@@ -3476,7 +3474,7 @@
       </c>
       <c r="E83" s="7"/>
     </row>
-    <row r="84" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" ht="30">
       <c r="A84" s="9" t="s">
         <v>277</v>
       </c>
@@ -3491,7 +3489,7 @@
       </c>
       <c r="E84" s="7"/>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5">
       <c r="A85" s="9" t="s">
         <v>279</v>
       </c>
@@ -3506,7 +3504,7 @@
       </c>
       <c r="E85" s="7"/>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5">
       <c r="A86" s="9" t="s">
         <v>282</v>
       </c>
@@ -3521,7 +3519,7 @@
       </c>
       <c r="E86" s="7"/>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5">
       <c r="A87" s="9" t="s">
         <v>285</v>
       </c>
@@ -3536,7 +3534,7 @@
       </c>
       <c r="E87" s="7"/>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5">
       <c r="A88" s="9" t="s">
         <v>288</v>
       </c>
@@ -3551,7 +3549,7 @@
       </c>
       <c r="E88" s="7"/>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5">
       <c r="A89" s="9" t="s">
         <v>291</v>
       </c>
@@ -3566,7 +3564,7 @@
       </c>
       <c r="E89" s="7"/>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5">
       <c r="A90" s="9" t="s">
         <v>294</v>
       </c>
@@ -3581,7 +3579,7 @@
       </c>
       <c r="E90" s="7"/>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5">
       <c r="A91" s="9" t="s">
         <v>297</v>
       </c>
@@ -3596,7 +3594,7 @@
       </c>
       <c r="E91" s="7"/>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5">
       <c r="A92" s="9" t="s">
         <v>300</v>
       </c>
@@ -3611,7 +3609,7 @@
       </c>
       <c r="E92" s="7"/>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5">
       <c r="A93" s="9" t="s">
         <v>303</v>
       </c>
@@ -3626,7 +3624,7 @@
       </c>
       <c r="E93" s="7"/>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5">
       <c r="A94" s="9" t="s">
         <v>306</v>
       </c>
@@ -3641,7 +3639,7 @@
       </c>
       <c r="E94" s="7"/>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5">
       <c r="A95" s="9" t="s">
         <v>309</v>
       </c>
@@ -3656,7 +3654,7 @@
       </c>
       <c r="E95" s="7"/>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5">
       <c r="A96" s="9" t="s">
         <v>314</v>
       </c>
@@ -3671,7 +3669,7 @@
       </c>
       <c r="E96" s="7"/>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5">
       <c r="A97" s="9" t="s">
         <v>315</v>
       </c>
@@ -3686,7 +3684,7 @@
       </c>
       <c r="E97" s="7"/>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5">
       <c r="A98" s="9" t="s">
         <v>319</v>
       </c>
@@ -3701,7 +3699,7 @@
       </c>
       <c r="E98" s="7"/>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5">
       <c r="A99" s="9" t="s">
         <v>321</v>
       </c>
@@ -3716,7 +3714,7 @@
       </c>
       <c r="E99" s="7"/>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5">
       <c r="A100" s="9" t="s">
         <v>322</v>
       </c>
@@ -3731,7 +3729,7 @@
       </c>
       <c r="E100" s="7"/>
     </row>
-    <row r="101" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" ht="30">
       <c r="A101" s="9" t="s">
         <v>323</v>
       </c>
@@ -3746,7 +3744,7 @@
       </c>
       <c r="E101" s="7"/>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5">
       <c r="A102" s="9" t="s">
         <v>328</v>
       </c>
@@ -3761,7 +3759,7 @@
       </c>
       <c r="E102" s="7"/>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5">
       <c r="A103" s="9" t="s">
         <v>333</v>
       </c>
@@ -3776,7 +3774,7 @@
       </c>
       <c r="E103" s="7"/>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5">
       <c r="A104" s="9" t="s">
         <v>336</v>
       </c>
@@ -3791,7 +3789,7 @@
       </c>
       <c r="E104" s="7"/>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5">
       <c r="A105" s="9" t="s">
         <v>337</v>
       </c>
@@ -3806,7 +3804,7 @@
       </c>
       <c r="E105" s="7"/>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5">
       <c r="A106" s="9" t="s">
         <v>342</v>
       </c>
@@ -3821,7 +3819,7 @@
       </c>
       <c r="E106" s="7"/>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5">
       <c r="A107" s="9" t="s">
         <v>345</v>
       </c>
@@ -3836,7 +3834,7 @@
       </c>
       <c r="E107" s="7"/>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5">
       <c r="A108" s="9" t="s">
         <v>350</v>
       </c>
@@ -3851,7 +3849,7 @@
       </c>
       <c r="E108" s="7"/>
     </row>
-    <row r="109" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" ht="30">
       <c r="A109" s="9" t="s">
         <v>351</v>
       </c>
@@ -3866,7 +3864,7 @@
       </c>
       <c r="E109" s="7"/>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5">
       <c r="A110" s="9" t="s">
         <v>354</v>
       </c>
@@ -3881,7 +3879,7 @@
       </c>
       <c r="E110" s="7"/>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5">
       <c r="A111" s="9" t="s">
         <v>357</v>
       </c>
@@ -3896,7 +3894,7 @@
       </c>
       <c r="E111" s="7"/>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5">
       <c r="A112" s="9" t="s">
         <v>361</v>
       </c>
@@ -3911,7 +3909,7 @@
       </c>
       <c r="E112" s="7"/>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5">
       <c r="A113" s="9" t="s">
         <v>363</v>
       </c>
@@ -3926,7 +3924,7 @@
       </c>
       <c r="E113" s="7"/>
     </row>
-    <row r="114" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" ht="30">
       <c r="A114" s="9" t="s">
         <v>366</v>
       </c>
@@ -3941,7 +3939,7 @@
       </c>
       <c r="E114" s="7"/>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5">
       <c r="A115" s="9" t="s">
         <v>369</v>
       </c>
@@ -3956,7 +3954,7 @@
       </c>
       <c r="E115" s="7"/>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5">
       <c r="A116" s="9" t="s">
         <v>370</v>
       </c>
@@ -3971,7 +3969,7 @@
       </c>
       <c r="E116" s="7"/>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5">
       <c r="A117" s="9" t="s">
         <v>371</v>
       </c>
@@ -3986,7 +3984,7 @@
       </c>
       <c r="E117" s="7"/>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5">
       <c r="A118" s="9" t="s">
         <v>378</v>
       </c>
@@ -4001,7 +3999,7 @@
       </c>
       <c r="E118" s="7"/>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5">
       <c r="A119" s="9" t="s">
         <v>381</v>
       </c>
@@ -4016,7 +4014,7 @@
       </c>
       <c r="E119" s="7"/>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5">
       <c r="A120" s="9" t="s">
         <v>384</v>
       </c>
@@ -4031,7 +4029,7 @@
       </c>
       <c r="E120" s="7"/>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5">
       <c r="A121" s="9" t="s">
         <v>387</v>
       </c>
@@ -4046,7 +4044,7 @@
       </c>
       <c r="E121" s="7"/>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5">
       <c r="A122" s="7" t="s">
         <v>390</v>
       </c>
@@ -4061,7 +4059,7 @@
       </c>
       <c r="E122" s="7"/>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5">
       <c r="A123" s="7" t="s">
         <v>393</v>
       </c>
@@ -4076,7 +4074,7 @@
       </c>
       <c r="E123" s="7"/>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5">
       <c r="A124" s="7" t="s">
         <v>396</v>
       </c>
@@ -4091,7 +4089,7 @@
       </c>
       <c r="E124" s="7"/>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5">
       <c r="A125" s="9" t="s">
         <v>399</v>
       </c>
@@ -4106,7 +4104,7 @@
       </c>
       <c r="E125" s="7"/>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5">
       <c r="A126" s="7" t="s">
         <v>402</v>
       </c>
@@ -4121,7 +4119,7 @@
       </c>
       <c r="E126" s="7"/>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5">
       <c r="A127" s="7" t="s">
         <v>405</v>
       </c>
@@ -4136,7 +4134,7 @@
       </c>
       <c r="E127" s="7"/>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5">
       <c r="A128" s="7" t="s">
         <v>408</v>
       </c>
@@ -4151,7 +4149,7 @@
       </c>
       <c r="E128" s="7"/>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5">
       <c r="A129" s="9" t="s">
         <v>411</v>
       </c>
@@ -4166,7 +4164,7 @@
       </c>
       <c r="E129" s="7"/>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5">
       <c r="A130" s="9" t="s">
         <v>414</v>
       </c>
@@ -4181,7 +4179,7 @@
       </c>
       <c r="E130" s="7"/>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5">
       <c r="A131" s="9" t="s">
         <v>416</v>
       </c>
@@ -4196,7 +4194,7 @@
       </c>
       <c r="E131" s="7"/>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5">
       <c r="A132" s="7" t="s">
         <v>419</v>
       </c>
@@ -4211,7 +4209,7 @@
       </c>
       <c r="E132" s="7"/>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5">
       <c r="A133" s="9" t="s">
         <v>422</v>
       </c>
@@ -4226,7 +4224,7 @@
       </c>
       <c r="E133" s="7"/>
     </row>
-    <row r="134" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5" ht="30">
       <c r="A134" s="7" t="s">
         <v>425</v>
       </c>
@@ -4241,7 +4239,7 @@
       </c>
       <c r="E134" s="7"/>
     </row>
-    <row r="135" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5" ht="30">
       <c r="A135" s="7" t="s">
         <v>426</v>
       </c>
@@ -4256,7 +4254,7 @@
       </c>
       <c r="E135" s="7"/>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5">
       <c r="A136" s="9" t="s">
         <v>431</v>
       </c>
@@ -4271,7 +4269,7 @@
       </c>
       <c r="E136" s="7"/>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5">
       <c r="A137" s="7" t="s">
         <v>434</v>
       </c>
@@ -4286,7 +4284,7 @@
       </c>
       <c r="E137" s="7"/>
     </row>
-    <row r="138" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" ht="45">
       <c r="A138" s="7" t="s">
         <v>435</v>
       </c>
@@ -4301,7 +4299,7 @@
       </c>
       <c r="E138" s="7"/>
     </row>
-    <row r="139" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5" ht="30">
       <c r="A139" s="7" t="s">
         <v>436</v>
       </c>
@@ -4316,7 +4314,7 @@
       </c>
       <c r="E139" s="7"/>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5">
       <c r="A140" s="17" t="s">
         <v>443</v>
       </c>
@@ -4331,7 +4329,7 @@
       </c>
       <c r="E140" s="7"/>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5">
       <c r="A141" s="17" t="s">
         <v>446</v>
       </c>
@@ -4346,7 +4344,7 @@
       </c>
       <c r="E141" s="7"/>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:5">
       <c r="A142" s="17" t="s">
         <v>449</v>
       </c>
@@ -4361,7 +4359,7 @@
       </c>
       <c r="E142" s="7"/>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:5">
       <c r="A143" s="17" t="s">
         <v>452</v>
       </c>
@@ -4376,7 +4374,7 @@
       </c>
       <c r="E143" s="7"/>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:5">
       <c r="A144" s="17" t="s">
         <v>453</v>
       </c>
@@ -4391,7 +4389,7 @@
       </c>
       <c r="E144" s="7"/>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:5">
       <c r="A145" s="17" t="s">
         <v>458</v>
       </c>
@@ -4406,7 +4404,7 @@
       </c>
       <c r="E145" s="7"/>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:5">
       <c r="A146" s="17" t="s">
         <v>461</v>
       </c>
@@ -4421,7 +4419,7 @@
       </c>
       <c r="E146" s="7"/>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:5">
       <c r="A147" s="17" t="s">
         <v>464</v>
       </c>
@@ -4436,7 +4434,7 @@
       </c>
       <c r="E147" s="7"/>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:5">
       <c r="A148" s="17" t="s">
         <v>467</v>
       </c>
@@ -4451,7 +4449,7 @@
       </c>
       <c r="E148" s="7"/>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:5">
       <c r="A149" s="7" t="s">
         <v>470</v>
       </c>
@@ -4466,7 +4464,7 @@
       </c>
       <c r="E149" s="7"/>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:5">
       <c r="A150" s="7" t="s">
         <v>471</v>
       </c>
@@ -4481,7 +4479,7 @@
       </c>
       <c r="E150" s="7"/>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:5">
       <c r="A151" s="7" t="s">
         <v>472</v>
       </c>
@@ -4496,7 +4494,7 @@
       </c>
       <c r="E151" s="7"/>
     </row>
-    <row r="152" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:5" ht="30">
       <c r="A152" s="7" t="s">
         <v>479</v>
       </c>
@@ -4511,7 +4509,7 @@
       </c>
       <c r="E152" s="7"/>
     </row>
-    <row r="153" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:5" ht="45">
       <c r="A153" s="17" t="s">
         <v>482</v>
       </c>
@@ -4526,7 +4524,7 @@
       </c>
       <c r="E153" s="7"/>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:5">
       <c r="A154" s="17" t="s">
         <v>484</v>
       </c>
@@ -4541,7 +4539,7 @@
       </c>
       <c r="E154" s="7"/>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:5">
       <c r="A155" s="7" t="s">
         <v>486</v>
       </c>
@@ -4556,7 +4554,7 @@
       </c>
       <c r="E155" s="7"/>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:5">
       <c r="A156" s="7" t="s">
         <v>489</v>
       </c>
@@ -4571,7 +4569,7 @@
       </c>
       <c r="E156" s="7"/>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:5">
       <c r="A157" s="7" t="s">
         <v>492</v>
       </c>
@@ -4586,7 +4584,7 @@
       </c>
       <c r="E157" s="7"/>
     </row>
-    <row r="158" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:5" ht="30">
       <c r="A158" s="7" t="s">
         <v>495</v>
       </c>
@@ -4601,7 +4599,7 @@
       </c>
       <c r="E158" s="7"/>
     </row>
-    <row r="159" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:5" ht="30">
       <c r="A159" s="7" t="s">
         <v>496</v>
       </c>
@@ -4616,7 +4614,7 @@
       </c>
       <c r="E159" s="7"/>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:5">
       <c r="A160" s="7" t="s">
         <v>503</v>
       </c>
@@ -4631,7 +4629,7 @@
       </c>
       <c r="E160" s="7"/>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:5">
       <c r="A161" s="7" t="s">
         <v>504</v>
       </c>
@@ -4646,7 +4644,7 @@
       </c>
       <c r="E161" s="7"/>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:5">
       <c r="A162" s="7" t="s">
         <v>507</v>
       </c>
@@ -4661,7 +4659,7 @@
       </c>
       <c r="E162" s="7"/>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:5">
       <c r="A163" s="7" t="s">
         <v>512</v>
       </c>
@@ -4676,7 +4674,7 @@
       </c>
       <c r="E163" s="7"/>
     </row>
-    <row r="164" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:5" ht="30">
       <c r="A164" s="7" t="s">
         <v>515</v>
       </c>
@@ -4691,7 +4689,7 @@
       </c>
       <c r="E164" s="7"/>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:5">
       <c r="A165" s="7" t="s">
         <v>518</v>
       </c>
@@ -4706,7 +4704,7 @@
       </c>
       <c r="E165" s="7"/>
     </row>
-    <row r="166" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:5" ht="30">
       <c r="A166" s="7" t="s">
         <v>521</v>
       </c>
@@ -4721,7 +4719,7 @@
       </c>
       <c r="E166" s="7"/>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:5">
       <c r="A167" s="7" t="s">
         <v>525</v>
       </c>
@@ -4736,7 +4734,7 @@
       </c>
       <c r="E167" s="7"/>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:5">
       <c r="A168" s="7" t="s">
         <v>527</v>
       </c>
@@ -4751,7 +4749,7 @@
       </c>
       <c r="E168" s="7"/>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:5">
       <c r="A169" s="7" t="s">
         <v>530</v>
       </c>
@@ -4766,7 +4764,7 @@
       </c>
       <c r="E169" s="7"/>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:5">
       <c r="A170" s="7" t="s">
         <v>531</v>
       </c>
@@ -4781,7 +4779,7 @@
       </c>
       <c r="E170" s="7"/>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:5">
       <c r="A171" s="7" t="s">
         <v>532</v>
       </c>
@@ -4796,7 +4794,7 @@
       </c>
       <c r="E171" s="7"/>
     </row>
-    <row r="172" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:5" ht="30">
       <c r="A172" s="7" t="s">
         <v>539</v>
       </c>
@@ -4811,7 +4809,7 @@
       </c>
       <c r="E172" s="7"/>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:5">
       <c r="A173" s="9" t="s">
         <v>541</v>
       </c>
@@ -4826,7 +4824,7 @@
       </c>
       <c r="E173" s="7"/>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:5">
       <c r="A174" s="9" t="s">
         <v>542</v>
       </c>
@@ -4841,7 +4839,7 @@
       </c>
       <c r="E174" s="7"/>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:5">
       <c r="A175" s="9" t="s">
         <v>543</v>
       </c>
@@ -4856,7 +4854,7 @@
       </c>
       <c r="E175" s="7"/>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:5">
       <c r="A176" s="9" t="s">
         <v>544</v>
       </c>
@@ -4871,7 +4869,7 @@
       </c>
       <c r="E176" s="7"/>
     </row>
-    <row r="177" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:5" ht="30">
       <c r="A177" s="7" t="s">
         <v>552</v>
       </c>
@@ -4886,14 +4884,14 @@
       </c>
       <c r="E177" s="7"/>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:5">
       <c r="A178" s="7" t="s">
         <v>555</v>
       </c>
       <c r="B178" s="7" t="s">
         <v>556</v>
       </c>
-      <c r="C178" s="16" t="s">
+      <c r="C178" s="8" t="s">
         <v>557</v>
       </c>
       <c r="D178" s="9" t="s">
@@ -4901,14 +4899,14 @@
       </c>
       <c r="E178" s="7"/>
     </row>
-    <row r="179" spans="1:5" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:5" ht="30">
       <c r="A179" s="7" t="s">
         <v>559</v>
       </c>
       <c r="B179" s="7" t="s">
         <v>560</v>
       </c>
-      <c r="C179" s="16" t="s">
+      <c r="C179" s="8" t="s">
         <v>558</v>
       </c>
       <c r="D179" s="9" t="s">
@@ -4916,14 +4914,14 @@
       </c>
       <c r="E179" s="7"/>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:5">
       <c r="A180" s="7" t="s">
         <v>561</v>
       </c>
       <c r="B180" s="7" t="s">
         <v>562</v>
       </c>
-      <c r="C180" s="16" t="s">
+      <c r="C180" s="8" t="s">
         <v>563</v>
       </c>
       <c r="D180" s="9" t="s">
@@ -4931,14 +4929,14 @@
       </c>
       <c r="E180" s="7"/>
     </row>
-    <row r="181" spans="1:5" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:5" ht="30">
       <c r="A181" s="7" t="s">
         <v>564</v>
       </c>
       <c r="B181" s="7" t="s">
         <v>565</v>
       </c>
-      <c r="C181" s="18" t="s">
+      <c r="C181" s="8" t="s">
         <v>566</v>
       </c>
       <c r="D181" s="9" t="s">
@@ -4946,14 +4944,14 @@
       </c>
       <c r="E181" s="7"/>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:5">
       <c r="A182" s="7" t="s">
         <v>567</v>
       </c>
       <c r="B182" s="7" t="s">
         <v>568</v>
       </c>
-      <c r="C182" s="18" t="s">
+      <c r="C182" s="8" t="s">
         <v>569</v>
       </c>
       <c r="D182" s="9" t="s">
@@ -4961,20 +4959,50 @@
       </c>
       <c r="E182" s="7"/>
     </row>
-    <row r="183" spans="1:5" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:5">
       <c r="A183" s="7" t="s">
         <v>570</v>
       </c>
       <c r="B183" s="7" t="s">
         <v>572</v>
       </c>
-      <c r="C183" s="16" t="s">
+      <c r="C183" s="8" t="s">
         <v>571</v>
       </c>
       <c r="D183" s="9" t="s">
         <v>5</v>
       </c>
       <c r="E183" s="7"/>
+    </row>
+    <row r="184" spans="1:5">
+      <c r="A184" s="9" t="s">
+        <v>573</v>
+      </c>
+      <c r="B184" s="7" t="s">
+        <v>575</v>
+      </c>
+      <c r="C184" s="8" t="s">
+        <v>576</v>
+      </c>
+      <c r="D184" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E184" s="7"/>
+    </row>
+    <row r="185" spans="1:5">
+      <c r="A185" s="9" t="s">
+        <v>574</v>
+      </c>
+      <c r="B185" s="7" t="s">
+        <v>578</v>
+      </c>
+      <c r="C185" s="8" t="s">
+        <v>577</v>
+      </c>
+      <c r="D185" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E185" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -4987,14 +5015,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView topLeftCell="A10" zoomScale="80" workbookViewId="0">
       <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
@@ -5002,7 +5030,7 @@
     <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="10" t="s">
         <v>35</v>
       </c>
@@ -5016,7 +5044,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="7" t="s">
         <v>37</v>
       </c>
@@ -5028,7 +5056,7 @@
       </c>
       <c r="D2" s="7"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="7" t="s">
         <v>38</v>
       </c>
@@ -5040,7 +5068,7 @@
       </c>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="7" t="s">
         <v>39</v>
       </c>
@@ -5052,7 +5080,7 @@
       </c>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" s="7" t="s">
         <v>40</v>
       </c>
@@ -5064,7 +5092,7 @@
       </c>
       <c r="D5" s="7"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" s="7" t="s">
         <v>41</v>
       </c>
@@ -5076,7 +5104,7 @@
       </c>
       <c r="D6" s="7"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="7" t="s">
         <v>42</v>
       </c>
@@ -5088,7 +5116,7 @@
       </c>
       <c r="D7" s="7"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="7" t="s">
         <v>43</v>
       </c>
@@ -5100,7 +5128,7 @@
       </c>
       <c r="D8" s="7"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="7" t="s">
         <v>44</v>
       </c>
@@ -5112,7 +5140,7 @@
       </c>
       <c r="D9" s="7"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="7" t="s">
         <v>45</v>
       </c>
@@ -5124,7 +5152,7 @@
       </c>
       <c r="D10" s="7"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11" s="7" t="s">
         <v>46</v>
       </c>
@@ -5136,7 +5164,7 @@
       </c>
       <c r="D11" s="7"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="A12" s="7" t="s">
         <v>48</v>
       </c>
@@ -5148,7 +5176,7 @@
       </c>
       <c r="D12" s="7"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="A13" s="7" t="s">
         <v>49</v>
       </c>
@@ -5160,7 +5188,7 @@
       </c>
       <c r="D13" s="7"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="A14" s="7" t="s">
         <v>50</v>
       </c>
@@ -5172,7 +5200,7 @@
       </c>
       <c r="D14" s="7"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="A15" s="7" t="s">
         <v>51</v>
       </c>
@@ -5184,7 +5212,7 @@
       </c>
       <c r="D15" s="7"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="A16" s="7" t="s">
         <v>52</v>
       </c>
@@ -5196,7 +5224,7 @@
       </c>
       <c r="D16" s="7"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4">
       <c r="A17" s="7" t="s">
         <v>53</v>
       </c>
@@ -5208,7 +5236,7 @@
       </c>
       <c r="D17" s="7"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4">
       <c r="A18" s="7" t="s">
         <v>54</v>
       </c>
@@ -5220,7 +5248,7 @@
       </c>
       <c r="D18" s="7"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4">
       <c r="A19" s="7" t="s">
         <v>55</v>
       </c>
@@ -5232,7 +5260,7 @@
       </c>
       <c r="D19" s="7"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4">
       <c r="A20" s="7" t="s">
         <v>56</v>
       </c>
@@ -5244,7 +5272,7 @@
       </c>
       <c r="D20" s="7"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4">
       <c r="A21" s="7" t="s">
         <v>57</v>
       </c>
@@ -5256,7 +5284,7 @@
       </c>
       <c r="D21" s="7"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4">
       <c r="A22" s="7" t="s">
         <v>58</v>
       </c>
@@ -5268,7 +5296,7 @@
       </c>
       <c r="D22" s="7"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4">
       <c r="A23" s="7" t="s">
         <v>59</v>
       </c>
@@ -5280,7 +5308,7 @@
       </c>
       <c r="D23" s="7"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4">
       <c r="A24" s="7" t="s">
         <v>60</v>
       </c>
@@ -5292,7 +5320,7 @@
       </c>
       <c r="D24" s="7"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4">
       <c r="A25" s="7" t="s">
         <v>61</v>
       </c>
@@ -5304,7 +5332,7 @@
       </c>
       <c r="D25" s="7"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4">
       <c r="A26" s="7" t="s">
         <v>47</v>
       </c>
@@ -5323,14 +5351,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A19" sqref="A19:XFD19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
@@ -5338,7 +5366,7 @@
     <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="10" t="s">
         <v>35</v>
       </c>
@@ -5352,7 +5380,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="7" t="s">
         <v>37</v>
       </c>
@@ -5364,7 +5392,7 @@
       </c>
       <c r="D2" s="7"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="7" t="s">
         <v>38</v>
       </c>
@@ -5376,7 +5404,7 @@
       </c>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="7" t="s">
         <v>39</v>
       </c>
@@ -5388,7 +5416,7 @@
       </c>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" s="7" t="s">
         <v>40</v>
       </c>
@@ -5400,7 +5428,7 @@
       </c>
       <c r="D5" s="7"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" s="7" t="s">
         <v>41</v>
       </c>
@@ -5412,7 +5440,7 @@
       </c>
       <c r="D6" s="7"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="7" t="s">
         <v>42</v>
       </c>
@@ -5424,7 +5452,7 @@
       </c>
       <c r="D7" s="7"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="7" t="s">
         <v>43</v>
       </c>
@@ -5436,7 +5464,7 @@
       </c>
       <c r="D8" s="7"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="7" t="s">
         <v>44</v>
       </c>
@@ -5448,7 +5476,7 @@
       </c>
       <c r="D9" s="7"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="7" t="s">
         <v>45</v>
       </c>
@@ -5460,7 +5488,7 @@
       </c>
       <c r="D10" s="7"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11" s="7" t="s">
         <v>46</v>
       </c>
@@ -5472,7 +5500,7 @@
       </c>
       <c r="D11" s="7"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="A12" s="7" t="s">
         <v>47</v>
       </c>
@@ -5484,7 +5512,7 @@
       </c>
       <c r="D12" s="7"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="A13" s="7" t="s">
         <v>48</v>
       </c>
@@ -5496,7 +5524,7 @@
       </c>
       <c r="D13" s="7"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="A14" s="7" t="s">
         <v>49</v>
       </c>
@@ -5508,7 +5536,7 @@
       </c>
       <c r="D14" s="7"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="A15" s="7" t="s">
         <v>50</v>
       </c>
@@ -5520,7 +5548,7 @@
       </c>
       <c r="D15" s="7"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="A16" s="7" t="s">
         <v>51</v>
       </c>
@@ -5532,7 +5560,7 @@
       </c>
       <c r="D16" s="7"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4">
       <c r="A17" s="7" t="s">
         <v>52</v>
       </c>
@@ -5544,7 +5572,7 @@
       </c>
       <c r="D17" s="7"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4">
       <c r="A18" s="7" t="s">
         <v>53</v>
       </c>
@@ -5556,7 +5584,7 @@
       </c>
       <c r="D18" s="7"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4">
       <c r="A19" s="7" t="s">
         <v>54</v>
       </c>
@@ -5568,7 +5596,7 @@
       </c>
       <c r="D19" s="7"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4">
       <c r="A20" s="7" t="s">
         <v>55</v>
       </c>
@@ -5580,7 +5608,7 @@
       </c>
       <c r="D20" s="7"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4">
       <c r="A21" s="7" t="s">
         <v>56</v>
       </c>
@@ -5592,7 +5620,7 @@
       </c>
       <c r="D21" s="7"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4">
       <c r="A22" s="7" t="s">
         <v>57</v>
       </c>
@@ -5604,7 +5632,7 @@
       </c>
       <c r="D22" s="7"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4">
       <c r="A23" s="7" t="s">
         <v>58</v>
       </c>
@@ -5616,7 +5644,7 @@
       </c>
       <c r="D23" s="7"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4">
       <c r="A24" s="7" t="s">
         <v>59</v>
       </c>
@@ -5628,7 +5656,7 @@
       </c>
       <c r="D24" s="7"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4">
       <c r="A25" s="7" t="s">
         <v>60</v>
       </c>
@@ -5640,7 +5668,7 @@
       </c>
       <c r="D25" s="7"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4">
       <c r="A26" s="7" t="s">
         <v>61</v>
       </c>

</xml_diff>

<commit_message>
Minor change in WAT.xls
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/WAT.xlsx
+++ b/src/test/resources/xls/WAT.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13305" windowHeight="2415"/>
@@ -1075,12 +1075,6 @@
     <t>WAT63</t>
   </si>
   <si>
-    <t>Verify that System must display the 'Total Times Cited' label with count in the metrics tab || Verify that System must display the 'H-index' label with count in the metrics tab.</t>
-  </si>
-  <si>
-    <t>WAT-375||WAT-377</t>
-  </si>
-  <si>
     <t>WAT110</t>
   </si>
   <si>
@@ -1385,15 +1379,9 @@
     <t>WAT-1214</t>
   </si>
   <si>
-    <t>WAT-1215</t>
-  </si>
-  <si>
     <t>Verify that user is able to see the selections they made in the Journal filter in Author search results page</t>
   </si>
   <si>
-    <t>Verify that user is able to see the selections they made in the Subject Category filter in Author search results page</t>
-  </si>
-  <si>
     <t>WAT129</t>
   </si>
   <si>
@@ -1755,13 +1743,25 @@
   </si>
   <si>
     <t>WAT-345</t>
+  </si>
+  <si>
+    <t>WAT-1215||WAT-306</t>
+  </si>
+  <si>
+    <t>Verify that user is able to see the selections they made in the Subject Category filter in Author search results page||Verify that system provides the filter option "Filter by Subject Categories" in the Author search result page</t>
+  </si>
+  <si>
+    <t>WAT-375||WAT-377||WAT-632</t>
+  </si>
+  <si>
+    <t>Verify that System must display the 'Total Times Cited' label with count in the metrics tab || Verify that System must display the 'H-index' label with count in the metrics tab.|| Verify that the System displays the H-index in the metrics tab.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1970,7 +1970,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2002,9 +2002,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2036,6 +2037,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2211,14 +2213,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E185"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A167" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C192" sqref="C192"/>
+    <sheetView tabSelected="1" topLeftCell="A98" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B109" sqref="B109:C109"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="30.5703125" customWidth="1" collapsed="1"/>
@@ -2227,7 +2229,7 @@
     <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2244,7 +2246,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -2259,7 +2261,7 @@
       </c>
       <c r="E2" s="4"/>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -2274,7 +2276,7 @@
       </c>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>11</v>
       </c>
@@ -2289,7 +2291,7 @@
       </c>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>12</v>
       </c>
@@ -2304,7 +2306,7 @@
       </c>
       <c r="E5" s="7"/>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>14</v>
       </c>
@@ -2319,7 +2321,7 @@
       </c>
       <c r="E6" s="7"/>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>17</v>
       </c>
@@ -2334,7 +2336,7 @@
       </c>
       <c r="E7" s="7"/>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>20</v>
       </c>
@@ -2349,7 +2351,7 @@
       </c>
       <c r="E8" s="7"/>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>22</v>
       </c>
@@ -2364,7 +2366,7 @@
       </c>
       <c r="E9" s="7"/>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>23</v>
       </c>
@@ -2379,7 +2381,7 @@
       </c>
       <c r="E10" s="7"/>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>24</v>
       </c>
@@ -2394,7 +2396,7 @@
       </c>
       <c r="E11" s="7"/>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>25</v>
       </c>
@@ -2409,7 +2411,7 @@
       </c>
       <c r="E12" s="7"/>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>62</v>
       </c>
@@ -2424,7 +2426,7 @@
       </c>
       <c r="E13" s="7"/>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>63</v>
       </c>
@@ -2439,7 +2441,7 @@
       </c>
       <c r="E14" s="7"/>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>64</v>
       </c>
@@ -2454,7 +2456,7 @@
       </c>
       <c r="E15" s="7"/>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>65</v>
       </c>
@@ -2469,7 +2471,7 @@
       </c>
       <c r="E16" s="7"/>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>74</v>
       </c>
@@ -2484,7 +2486,7 @@
       </c>
       <c r="E17" s="7"/>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>75</v>
       </c>
@@ -2499,7 +2501,7 @@
       </c>
       <c r="E18" s="7"/>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>79</v>
       </c>
@@ -2514,7 +2516,7 @@
       </c>
       <c r="E19" s="7"/>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>81</v>
       </c>
@@ -2529,7 +2531,7 @@
       </c>
       <c r="E20" s="7"/>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>82</v>
       </c>
@@ -2544,7 +2546,7 @@
       </c>
       <c r="E21" s="7"/>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>88</v>
       </c>
@@ -2559,7 +2561,7 @@
       </c>
       <c r="E22" s="7"/>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>90</v>
       </c>
@@ -2574,7 +2576,7 @@
       </c>
       <c r="E23" s="7"/>
     </row>
-    <row r="24" spans="1:5" ht="30">
+    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>94</v>
       </c>
@@ -2589,7 +2591,7 @@
       </c>
       <c r="E24" s="7"/>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>96</v>
       </c>
@@ -2604,7 +2606,7 @@
       </c>
       <c r="E25" s="7"/>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
         <v>98</v>
       </c>
@@ -2619,7 +2621,7 @@
       </c>
       <c r="E26" s="7"/>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
         <v>102</v>
       </c>
@@ -2634,7 +2636,7 @@
       </c>
       <c r="E27" s="7"/>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
         <v>105</v>
       </c>
@@ -2649,7 +2651,7 @@
       </c>
       <c r="E28" s="7"/>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
         <v>108</v>
       </c>
@@ -2664,7 +2666,7 @@
       </c>
       <c r="E29" s="7"/>
     </row>
-    <row r="30" spans="1:5" ht="30">
+    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
         <v>110</v>
       </c>
@@ -2679,7 +2681,7 @@
       </c>
       <c r="E30" s="7"/>
     </row>
-    <row r="31" spans="1:5" ht="30">
+    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
         <v>114</v>
       </c>
@@ -2694,7 +2696,7 @@
       </c>
       <c r="E31" s="7"/>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
         <v>119</v>
       </c>
@@ -2709,7 +2711,7 @@
       </c>
       <c r="E32" s="7"/>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
         <v>120</v>
       </c>
@@ -2724,7 +2726,7 @@
       </c>
       <c r="E33" s="7"/>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
         <v>125</v>
       </c>
@@ -2739,7 +2741,7 @@
       </c>
       <c r="E34" s="7"/>
     </row>
-    <row r="35" spans="1:5" ht="30">
+    <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
         <v>128</v>
       </c>
@@ -2754,7 +2756,7 @@
       </c>
       <c r="E35" s="7"/>
     </row>
-    <row r="36" spans="1:5" ht="30">
+    <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
         <v>131</v>
       </c>
@@ -2769,7 +2771,7 @@
       </c>
       <c r="E36" s="7"/>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
         <v>134</v>
       </c>
@@ -2784,7 +2786,7 @@
       </c>
       <c r="E37" s="7"/>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="9" t="s">
         <v>137</v>
       </c>
@@ -2799,7 +2801,7 @@
       </c>
       <c r="E38" s="7"/>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="s">
         <v>140</v>
       </c>
@@ -2814,7 +2816,7 @@
       </c>
       <c r="E39" s="7"/>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="9" t="s">
         <v>143</v>
       </c>
@@ -2829,7 +2831,7 @@
       </c>
       <c r="E40" s="7"/>
     </row>
-    <row r="41" spans="1:5" ht="30">
+    <row r="41" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
         <v>145</v>
       </c>
@@ -2844,7 +2846,7 @@
       </c>
       <c r="E41" s="7"/>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="9" t="s">
         <v>147</v>
       </c>
@@ -2859,7 +2861,7 @@
       </c>
       <c r="E42" s="7"/>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="9" t="s">
         <v>150</v>
       </c>
@@ -2874,7 +2876,7 @@
       </c>
       <c r="E43" s="7"/>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="9" t="s">
         <v>153</v>
       </c>
@@ -2889,7 +2891,7 @@
       </c>
       <c r="E44" s="7"/>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="9" t="s">
         <v>155</v>
       </c>
@@ -2904,7 +2906,7 @@
       </c>
       <c r="E45" s="7"/>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="12" t="s">
         <v>158</v>
       </c>
@@ -2919,7 +2921,7 @@
       </c>
       <c r="E46" s="7"/>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="12" t="s">
         <v>159</v>
       </c>
@@ -2934,7 +2936,7 @@
       </c>
       <c r="E47" s="7"/>
     </row>
-    <row r="48" spans="1:5" ht="30">
+    <row r="48" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="12" t="s">
         <v>160</v>
       </c>
@@ -2949,7 +2951,7 @@
       </c>
       <c r="E48" s="7"/>
     </row>
-    <row r="49" spans="1:5" ht="30">
+    <row r="49" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="12" t="s">
         <v>161</v>
       </c>
@@ -2964,7 +2966,7 @@
       </c>
       <c r="E49" s="7"/>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="12" t="s">
         <v>164</v>
       </c>
@@ -2979,7 +2981,7 @@
       </c>
       <c r="E50" s="7"/>
     </row>
-    <row r="51" spans="1:5" ht="30">
+    <row r="51" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="9" t="s">
         <v>173</v>
       </c>
@@ -2994,7 +2996,7 @@
       </c>
       <c r="E51" s="7"/>
     </row>
-    <row r="52" spans="1:5">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="9" t="s">
         <v>174</v>
       </c>
@@ -3009,7 +3011,7 @@
       </c>
       <c r="E52" s="7"/>
     </row>
-    <row r="53" spans="1:5">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="9" t="s">
         <v>179</v>
       </c>
@@ -3024,7 +3026,7 @@
       </c>
       <c r="E53" s="7"/>
     </row>
-    <row r="54" spans="1:5">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="9" t="s">
         <v>180</v>
       </c>
@@ -3039,7 +3041,7 @@
       </c>
       <c r="E54" s="7"/>
     </row>
-    <row r="55" spans="1:5">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="9" t="s">
         <v>185</v>
       </c>
@@ -3054,7 +3056,7 @@
       </c>
       <c r="E55" s="7"/>
     </row>
-    <row r="56" spans="1:5">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="s">
         <v>188</v>
       </c>
@@ -3069,7 +3071,7 @@
       </c>
       <c r="E56" s="7"/>
     </row>
-    <row r="57" spans="1:5" ht="30">
+    <row r="57" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="9" t="s">
         <v>191</v>
       </c>
@@ -3084,7 +3086,7 @@
       </c>
       <c r="E57" s="7"/>
     </row>
-    <row r="58" spans="1:5">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="9" t="s">
         <v>194</v>
       </c>
@@ -3099,7 +3101,7 @@
       </c>
       <c r="E58" s="7"/>
     </row>
-    <row r="59" spans="1:5">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
         <v>196</v>
       </c>
@@ -3114,7 +3116,7 @@
       </c>
       <c r="E59" s="7"/>
     </row>
-    <row r="60" spans="1:5" ht="45">
+    <row r="60" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
         <v>199</v>
       </c>
@@ -3129,7 +3131,7 @@
       </c>
       <c r="E60" s="7"/>
     </row>
-    <row r="61" spans="1:5">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="9" t="s">
         <v>202</v>
       </c>
@@ -3144,7 +3146,7 @@
       </c>
       <c r="E61" s="7"/>
     </row>
-    <row r="62" spans="1:5">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="9" t="s">
         <v>204</v>
       </c>
@@ -3159,7 +3161,7 @@
       </c>
       <c r="E62" s="7"/>
     </row>
-    <row r="63" spans="1:5">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="9" t="s">
         <v>206</v>
       </c>
@@ -3174,7 +3176,7 @@
       </c>
       <c r="E63" s="7"/>
     </row>
-    <row r="64" spans="1:5">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="9" t="s">
         <v>208</v>
       </c>
@@ -3189,7 +3191,7 @@
       </c>
       <c r="E64" s="7"/>
     </row>
-    <row r="65" spans="1:5">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="9" t="s">
         <v>217</v>
       </c>
@@ -3204,7 +3206,7 @@
       </c>
       <c r="E65" s="7"/>
     </row>
-    <row r="66" spans="1:5">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="9" t="s">
         <v>218</v>
       </c>
@@ -3219,7 +3221,7 @@
       </c>
       <c r="E66" s="7"/>
     </row>
-    <row r="67" spans="1:5">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="9" t="s">
         <v>223</v>
       </c>
@@ -3234,7 +3236,7 @@
       </c>
       <c r="E67" s="7"/>
     </row>
-    <row r="68" spans="1:5">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="9" t="s">
         <v>224</v>
       </c>
@@ -3249,7 +3251,7 @@
       </c>
       <c r="E68" s="7"/>
     </row>
-    <row r="69" spans="1:5">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="9" t="s">
         <v>225</v>
       </c>
@@ -3264,7 +3266,7 @@
       </c>
       <c r="E69" s="7"/>
     </row>
-    <row r="70" spans="1:5">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="9" t="s">
         <v>226</v>
       </c>
@@ -3279,7 +3281,7 @@
       </c>
       <c r="E70" s="7"/>
     </row>
-    <row r="71" spans="1:5">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="9" t="s">
         <v>233</v>
       </c>
@@ -3294,7 +3296,7 @@
       </c>
       <c r="E71" s="7"/>
     </row>
-    <row r="72" spans="1:5">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="9" t="s">
         <v>237</v>
       </c>
@@ -3309,7 +3311,7 @@
       </c>
       <c r="E72" s="7"/>
     </row>
-    <row r="73" spans="1:5">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="9" t="s">
         <v>239</v>
       </c>
@@ -3324,7 +3326,7 @@
       </c>
       <c r="E73" s="7"/>
     </row>
-    <row r="74" spans="1:5">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="9" t="s">
         <v>243</v>
       </c>
@@ -3339,7 +3341,7 @@
       </c>
       <c r="E74" s="7"/>
     </row>
-    <row r="75" spans="1:5" ht="30">
+    <row r="75" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" s="9" t="s">
         <v>245</v>
       </c>
@@ -3354,7 +3356,7 @@
       </c>
       <c r="E75" s="7"/>
     </row>
-    <row r="76" spans="1:5">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="9" t="s">
         <v>248</v>
       </c>
@@ -3369,7 +3371,7 @@
       </c>
       <c r="E76" s="7"/>
     </row>
-    <row r="77" spans="1:5">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="9" t="s">
         <v>256</v>
       </c>
@@ -3384,7 +3386,7 @@
       </c>
       <c r="E77" s="7"/>
     </row>
-    <row r="78" spans="1:5">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="9" t="s">
         <v>257</v>
       </c>
@@ -3399,7 +3401,7 @@
       </c>
       <c r="E78" s="7"/>
     </row>
-    <row r="79" spans="1:5">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="9" t="s">
         <v>261</v>
       </c>
@@ -3414,7 +3416,7 @@
       </c>
       <c r="E79" s="7"/>
     </row>
-    <row r="80" spans="1:5">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="9" t="s">
         <v>264</v>
       </c>
@@ -3429,7 +3431,7 @@
       </c>
       <c r="E80" s="7"/>
     </row>
-    <row r="81" spans="1:5">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="9" t="s">
         <v>267</v>
       </c>
@@ -3444,7 +3446,7 @@
       </c>
       <c r="E81" s="7"/>
     </row>
-    <row r="82" spans="1:5" ht="30">
+    <row r="82" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A82" s="9" t="s">
         <v>269</v>
       </c>
@@ -3459,7 +3461,7 @@
       </c>
       <c r="E82" s="7"/>
     </row>
-    <row r="83" spans="1:5">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="9" t="s">
         <v>274</v>
       </c>
@@ -3474,7 +3476,7 @@
       </c>
       <c r="E83" s="7"/>
     </row>
-    <row r="84" spans="1:5" ht="30">
+    <row r="84" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A84" s="9" t="s">
         <v>277</v>
       </c>
@@ -3489,7 +3491,7 @@
       </c>
       <c r="E84" s="7"/>
     </row>
-    <row r="85" spans="1:5">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="9" t="s">
         <v>279</v>
       </c>
@@ -3504,7 +3506,7 @@
       </c>
       <c r="E85" s="7"/>
     </row>
-    <row r="86" spans="1:5">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="9" t="s">
         <v>282</v>
       </c>
@@ -3519,7 +3521,7 @@
       </c>
       <c r="E86" s="7"/>
     </row>
-    <row r="87" spans="1:5">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="9" t="s">
         <v>285</v>
       </c>
@@ -3534,7 +3536,7 @@
       </c>
       <c r="E87" s="7"/>
     </row>
-    <row r="88" spans="1:5">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="9" t="s">
         <v>288</v>
       </c>
@@ -3549,7 +3551,7 @@
       </c>
       <c r="E88" s="7"/>
     </row>
-    <row r="89" spans="1:5">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="9" t="s">
         <v>291</v>
       </c>
@@ -3564,7 +3566,7 @@
       </c>
       <c r="E89" s="7"/>
     </row>
-    <row r="90" spans="1:5">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="9" t="s">
         <v>294</v>
       </c>
@@ -3579,7 +3581,7 @@
       </c>
       <c r="E90" s="7"/>
     </row>
-    <row r="91" spans="1:5">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="9" t="s">
         <v>297</v>
       </c>
@@ -3594,7 +3596,7 @@
       </c>
       <c r="E91" s="7"/>
     </row>
-    <row r="92" spans="1:5">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="9" t="s">
         <v>300</v>
       </c>
@@ -3609,7 +3611,7 @@
       </c>
       <c r="E92" s="7"/>
     </row>
-    <row r="93" spans="1:5">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="9" t="s">
         <v>303</v>
       </c>
@@ -3624,7 +3626,7 @@
       </c>
       <c r="E93" s="7"/>
     </row>
-    <row r="94" spans="1:5">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="9" t="s">
         <v>306</v>
       </c>
@@ -3639,7 +3641,7 @@
       </c>
       <c r="E94" s="7"/>
     </row>
-    <row r="95" spans="1:5">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="9" t="s">
         <v>309</v>
       </c>
@@ -3654,7 +3656,7 @@
       </c>
       <c r="E95" s="7"/>
     </row>
-    <row r="96" spans="1:5">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="9" t="s">
         <v>314</v>
       </c>
@@ -3669,7 +3671,7 @@
       </c>
       <c r="E96" s="7"/>
     </row>
-    <row r="97" spans="1:5">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="9" t="s">
         <v>315</v>
       </c>
@@ -3684,7 +3686,7 @@
       </c>
       <c r="E97" s="7"/>
     </row>
-    <row r="98" spans="1:5">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="9" t="s">
         <v>319</v>
       </c>
@@ -3699,7 +3701,7 @@
       </c>
       <c r="E98" s="7"/>
     </row>
-    <row r="99" spans="1:5">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="9" t="s">
         <v>321</v>
       </c>
@@ -3714,7 +3716,7 @@
       </c>
       <c r="E99" s="7"/>
     </row>
-    <row r="100" spans="1:5">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="9" t="s">
         <v>322</v>
       </c>
@@ -3729,7 +3731,7 @@
       </c>
       <c r="E100" s="7"/>
     </row>
-    <row r="101" spans="1:5" ht="30">
+    <row r="101" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A101" s="9" t="s">
         <v>323</v>
       </c>
@@ -3744,7 +3746,7 @@
       </c>
       <c r="E101" s="7"/>
     </row>
-    <row r="102" spans="1:5">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="9" t="s">
         <v>328</v>
       </c>
@@ -3759,7 +3761,7 @@
       </c>
       <c r="E102" s="7"/>
     </row>
-    <row r="103" spans="1:5">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="9" t="s">
         <v>333</v>
       </c>
@@ -3774,7 +3776,7 @@
       </c>
       <c r="E103" s="7"/>
     </row>
-    <row r="104" spans="1:5">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="9" t="s">
         <v>336</v>
       </c>
@@ -3789,7 +3791,7 @@
       </c>
       <c r="E104" s="7"/>
     </row>
-    <row r="105" spans="1:5">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="9" t="s">
         <v>337</v>
       </c>
@@ -3804,7 +3806,7 @@
       </c>
       <c r="E105" s="7"/>
     </row>
-    <row r="106" spans="1:5">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="9" t="s">
         <v>342</v>
       </c>
@@ -3819,7 +3821,7 @@
       </c>
       <c r="E106" s="7"/>
     </row>
-    <row r="107" spans="1:5">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="9" t="s">
         <v>345</v>
       </c>
@@ -3834,7 +3836,7 @@
       </c>
       <c r="E107" s="7"/>
     </row>
-    <row r="108" spans="1:5">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="9" t="s">
         <v>350</v>
       </c>
@@ -3849,1002 +3851,1002 @@
       </c>
       <c r="E108" s="7"/>
     </row>
-    <row r="109" spans="1:5" ht="30">
+    <row r="109" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A109" s="9" t="s">
         <v>351</v>
       </c>
       <c r="B109" s="9" t="s">
+        <v>577</v>
+      </c>
+      <c r="C109" s="8" t="s">
+        <v>578</v>
+      </c>
+      <c r="D109" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E109" s="7"/>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A110" s="9" t="s">
+        <v>352</v>
+      </c>
+      <c r="B110" s="9" t="s">
         <v>353</v>
       </c>
-      <c r="C109" s="8" t="s">
-        <v>352</v>
-      </c>
-      <c r="D109" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="E109" s="7"/>
-    </row>
-    <row r="110" spans="1:5">
-      <c r="A110" s="9" t="s">
+      <c r="C110" s="8" t="s">
         <v>354</v>
       </c>
-      <c r="B110" s="9" t="s">
+      <c r="D110" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E110" s="7"/>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A111" s="9" t="s">
         <v>355</v>
       </c>
-      <c r="C110" s="8" t="s">
+      <c r="B111" s="9" t="s">
         <v>356</v>
       </c>
-      <c r="D110" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="E110" s="7"/>
-    </row>
-    <row r="111" spans="1:5">
-      <c r="A111" s="9" t="s">
+      <c r="C111" s="8" t="s">
         <v>357</v>
       </c>
-      <c r="B111" s="9" t="s">
+      <c r="D111" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E111" s="7"/>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A112" s="9" t="s">
+        <v>359</v>
+      </c>
+      <c r="B112" s="9" t="s">
         <v>358</v>
       </c>
-      <c r="C111" s="8" t="s">
-        <v>359</v>
-      </c>
-      <c r="D111" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="E111" s="7"/>
-    </row>
-    <row r="112" spans="1:5">
-      <c r="A112" s="9" t="s">
+      <c r="C112" s="16" t="s">
+        <v>360</v>
+      </c>
+      <c r="D112" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E112" s="7"/>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A113" s="9" t="s">
         <v>361</v>
       </c>
-      <c r="B112" s="9" t="s">
-        <v>360</v>
-      </c>
-      <c r="C112" s="16" t="s">
+      <c r="B113" s="9" t="s">
         <v>362</v>
       </c>
-      <c r="D112" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="E112" s="7"/>
-    </row>
-    <row r="113" spans="1:5">
-      <c r="A113" s="9" t="s">
+      <c r="C113" s="16" t="s">
         <v>363</v>
       </c>
-      <c r="B113" s="9" t="s">
+      <c r="D113" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E113" s="7"/>
+    </row>
+    <row r="114" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A114" s="9" t="s">
         <v>364</v>
       </c>
-      <c r="C113" s="16" t="s">
+      <c r="B114" s="7" t="s">
         <v>365</v>
       </c>
-      <c r="D113" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="E113" s="7"/>
-    </row>
-    <row r="114" spans="1:5" ht="30">
-      <c r="A114" s="9" t="s">
+      <c r="C114" s="8" t="s">
         <v>366</v>
       </c>
-      <c r="B114" s="7" t="s">
+      <c r="D114" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E114" s="7"/>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A115" s="9" t="s">
         <v>367</v>
       </c>
-      <c r="C114" s="8" t="s">
+      <c r="B115" s="7" t="s">
+        <v>370</v>
+      </c>
+      <c r="C115" s="8" t="s">
+        <v>372</v>
+      </c>
+      <c r="D115" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E115" s="7"/>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A116" s="9" t="s">
         <v>368</v>
       </c>
-      <c r="D114" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E114" s="7"/>
-    </row>
-    <row r="115" spans="1:5">
-      <c r="A115" s="9" t="s">
+      <c r="B116" s="7" t="s">
+        <v>371</v>
+      </c>
+      <c r="C116" s="8" t="s">
+        <v>373</v>
+      </c>
+      <c r="D116" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E116" s="7"/>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A117" s="9" t="s">
         <v>369</v>
       </c>
-      <c r="B115" s="7" t="s">
-        <v>372</v>
-      </c>
-      <c r="C115" s="8" t="s">
+      <c r="B117" s="7" t="s">
         <v>374</v>
       </c>
-      <c r="D115" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E115" s="7"/>
-    </row>
-    <row r="116" spans="1:5">
-      <c r="A116" s="9" t="s">
-        <v>370</v>
-      </c>
-      <c r="B116" s="7" t="s">
-        <v>373</v>
-      </c>
-      <c r="C116" s="8" t="s">
+      <c r="C117" s="7" t="s">
         <v>375</v>
       </c>
-      <c r="D116" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E116" s="7"/>
-    </row>
-    <row r="117" spans="1:5">
-      <c r="A117" s="9" t="s">
-        <v>371</v>
-      </c>
-      <c r="B117" s="7" t="s">
+      <c r="D117" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E117" s="7"/>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A118" s="9" t="s">
         <v>376</v>
       </c>
-      <c r="C117" s="7" t="s">
+      <c r="B118" s="7" t="s">
         <v>377</v>
       </c>
-      <c r="D117" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E117" s="7"/>
-    </row>
-    <row r="118" spans="1:5">
-      <c r="A118" s="9" t="s">
+      <c r="C118" s="7" t="s">
         <v>378</v>
       </c>
-      <c r="B118" s="7" t="s">
+      <c r="D118" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E118" s="7"/>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A119" s="9" t="s">
         <v>379</v>
       </c>
-      <c r="C118" s="7" t="s">
+      <c r="B119" s="7" t="s">
         <v>380</v>
       </c>
-      <c r="D118" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E118" s="7"/>
-    </row>
-    <row r="119" spans="1:5">
-      <c r="A119" s="9" t="s">
+      <c r="C119" s="7" t="s">
         <v>381</v>
       </c>
-      <c r="B119" s="7" t="s">
+      <c r="D119" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E119" s="7"/>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A120" s="9" t="s">
         <v>382</v>
       </c>
-      <c r="C119" s="7" t="s">
+      <c r="B120" s="7" t="s">
         <v>383</v>
       </c>
-      <c r="D119" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E119" s="7"/>
-    </row>
-    <row r="120" spans="1:5">
-      <c r="A120" s="9" t="s">
+      <c r="C120" s="7" t="s">
         <v>384</v>
       </c>
-      <c r="B120" s="7" t="s">
+      <c r="D120" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E120" s="7"/>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A121" s="9" t="s">
         <v>385</v>
       </c>
-      <c r="C120" s="7" t="s">
+      <c r="B121" s="7" t="s">
         <v>386</v>
       </c>
-      <c r="D120" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E120" s="7"/>
-    </row>
-    <row r="121" spans="1:5">
-      <c r="A121" s="9" t="s">
+      <c r="C121" s="7" t="s">
         <v>387</v>
       </c>
-      <c r="B121" s="7" t="s">
+      <c r="D121" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E121" s="7"/>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A122" s="7" t="s">
         <v>388</v>
       </c>
-      <c r="C121" s="7" t="s">
+      <c r="B122" s="7" t="s">
         <v>389</v>
       </c>
-      <c r="D121" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E121" s="7"/>
-    </row>
-    <row r="122" spans="1:5">
-      <c r="A122" s="7" t="s">
+      <c r="C122" s="7" t="s">
         <v>390</v>
       </c>
-      <c r="B122" s="7" t="s">
+      <c r="D122" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E122" s="7"/>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A123" s="7" t="s">
         <v>391</v>
       </c>
-      <c r="C122" s="7" t="s">
+      <c r="B123" s="7" t="s">
         <v>392</v>
       </c>
-      <c r="D122" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E122" s="7"/>
-    </row>
-    <row r="123" spans="1:5">
-      <c r="A123" s="7" t="s">
+      <c r="C123" s="7" t="s">
         <v>393</v>
       </c>
-      <c r="B123" s="7" t="s">
+      <c r="D123" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E123" s="7"/>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A124" s="7" t="s">
         <v>394</v>
       </c>
-      <c r="C123" s="7" t="s">
+      <c r="B124" s="7" t="s">
         <v>395</v>
       </c>
-      <c r="D123" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E123" s="7"/>
-    </row>
-    <row r="124" spans="1:5">
-      <c r="A124" s="7" t="s">
+      <c r="C124" s="7" t="s">
         <v>396</v>
       </c>
-      <c r="B124" s="7" t="s">
+      <c r="D124" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E124" s="7"/>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A125" s="9" t="s">
         <v>397</v>
       </c>
-      <c r="C124" s="7" t="s">
+      <c r="B125" s="7" t="s">
         <v>398</v>
       </c>
-      <c r="D124" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="E124" s="7"/>
-    </row>
-    <row r="125" spans="1:5">
-      <c r="A125" s="9" t="s">
+      <c r="C125" s="7" t="s">
         <v>399</v>
       </c>
-      <c r="B125" s="7" t="s">
+      <c r="D125" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E125" s="7"/>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A126" s="7" t="s">
         <v>400</v>
       </c>
-      <c r="C125" s="7" t="s">
+      <c r="B126" s="7" t="s">
         <v>401</v>
       </c>
-      <c r="D125" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E125" s="7"/>
-    </row>
-    <row r="126" spans="1:5">
-      <c r="A126" s="7" t="s">
+      <c r="C126" s="7" t="s">
         <v>402</v>
       </c>
-      <c r="B126" s="7" t="s">
+      <c r="D126" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E126" s="7"/>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A127" s="7" t="s">
         <v>403</v>
       </c>
-      <c r="C126" s="7" t="s">
+      <c r="B127" s="7" t="s">
         <v>404</v>
       </c>
-      <c r="D126" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="E126" s="7"/>
-    </row>
-    <row r="127" spans="1:5">
-      <c r="A127" s="7" t="s">
+      <c r="C127" s="7" t="s">
         <v>405</v>
       </c>
-      <c r="B127" s="7" t="s">
+      <c r="D127" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E127" s="7"/>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A128" s="7" t="s">
         <v>406</v>
       </c>
-      <c r="C127" s="7" t="s">
+      <c r="B128" s="7" t="s">
         <v>407</v>
       </c>
-      <c r="D127" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="E127" s="7"/>
-    </row>
-    <row r="128" spans="1:5">
-      <c r="A128" s="7" t="s">
+      <c r="C128" s="7" t="s">
         <v>408</v>
       </c>
-      <c r="B128" s="7" t="s">
+      <c r="D128" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E128" s="7"/>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A129" s="9" t="s">
         <v>409</v>
       </c>
-      <c r="C128" s="7" t="s">
+      <c r="B129" s="7" t="s">
         <v>410</v>
       </c>
-      <c r="D128" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="E128" s="7"/>
-    </row>
-    <row r="129" spans="1:5">
-      <c r="A129" s="9" t="s">
+      <c r="C129" s="7" t="s">
         <v>411</v>
       </c>
-      <c r="B129" s="7" t="s">
+      <c r="D129" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E129" s="7"/>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A130" s="9" t="s">
         <v>412</v>
       </c>
-      <c r="C129" s="7" t="s">
+      <c r="B130" s="7" t="s">
+        <v>410</v>
+      </c>
+      <c r="C130" s="7" t="s">
         <v>413</v>
       </c>
-      <c r="D129" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E129" s="7"/>
-    </row>
-    <row r="130" spans="1:5">
-      <c r="A130" s="9" t="s">
+      <c r="D130" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E130" s="7"/>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A131" s="9" t="s">
         <v>414</v>
       </c>
-      <c r="B130" s="7" t="s">
-        <v>412</v>
-      </c>
-      <c r="C130" s="7" t="s">
+      <c r="B131" s="7" t="s">
+        <v>416</v>
+      </c>
+      <c r="C131" s="7" t="s">
         <v>415</v>
       </c>
-      <c r="D130" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E130" s="7"/>
-    </row>
-    <row r="131" spans="1:5">
-      <c r="A131" s="9" t="s">
-        <v>416</v>
-      </c>
-      <c r="B131" s="7" t="s">
+      <c r="D131" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E131" s="7"/>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A132" s="7" t="s">
+        <v>417</v>
+      </c>
+      <c r="B132" s="7" t="s">
         <v>418</v>
       </c>
-      <c r="C131" s="7" t="s">
-        <v>417</v>
-      </c>
-      <c r="D131" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E131" s="7"/>
-    </row>
-    <row r="132" spans="1:5">
-      <c r="A132" s="7" t="s">
+      <c r="C132" s="8" t="s">
         <v>419</v>
       </c>
-      <c r="B132" s="7" t="s">
+      <c r="D132" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E132" s="7"/>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A133" s="9" t="s">
         <v>420</v>
       </c>
-      <c r="C132" s="8" t="s">
+      <c r="B133" s="7" t="s">
         <v>421</v>
       </c>
-      <c r="D132" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="E132" s="7"/>
-    </row>
-    <row r="133" spans="1:5">
-      <c r="A133" s="9" t="s">
+      <c r="C133" s="7" t="s">
         <v>422</v>
       </c>
-      <c r="B133" s="7" t="s">
+      <c r="D133" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E133" s="7"/>
+    </row>
+    <row r="134" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A134" s="7" t="s">
         <v>423</v>
       </c>
-      <c r="C133" s="7" t="s">
+      <c r="B134" s="7" t="s">
+        <v>425</v>
+      </c>
+      <c r="C134" s="8" t="s">
+        <v>426</v>
+      </c>
+      <c r="D134" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E134" s="7"/>
+    </row>
+    <row r="135" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A135" s="7" t="s">
         <v>424</v>
       </c>
-      <c r="D133" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E133" s="7"/>
-    </row>
-    <row r="134" spans="1:5" ht="30">
-      <c r="A134" s="7" t="s">
-        <v>425</v>
-      </c>
-      <c r="B134" s="7" t="s">
+      <c r="B135" s="7" t="s">
         <v>427</v>
       </c>
-      <c r="C134" s="8" t="s">
+      <c r="C135" s="8" t="s">
         <v>428</v>
       </c>
-      <c r="D134" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E134" s="7"/>
-    </row>
-    <row r="135" spans="1:5" ht="30">
-      <c r="A135" s="7" t="s">
-        <v>426</v>
-      </c>
-      <c r="B135" s="7" t="s">
+      <c r="D135" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E135" s="7"/>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A136" s="9" t="s">
         <v>429</v>
       </c>
-      <c r="C135" s="8" t="s">
+      <c r="B136" s="7" t="s">
         <v>430</v>
       </c>
-      <c r="D135" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E135" s="7"/>
-    </row>
-    <row r="136" spans="1:5">
-      <c r="A136" s="9" t="s">
+      <c r="C136" s="7" t="s">
         <v>431</v>
       </c>
-      <c r="B136" s="7" t="s">
+      <c r="D136" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E136" s="7"/>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A137" s="7" t="s">
         <v>432</v>
       </c>
-      <c r="C136" s="7" t="s">
+      <c r="B137" s="7" t="s">
+        <v>436</v>
+      </c>
+      <c r="C137" s="7" t="s">
+        <v>435</v>
+      </c>
+      <c r="D137" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E137" s="7"/>
+    </row>
+    <row r="138" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A138" s="7" t="s">
         <v>433</v>
       </c>
-      <c r="D136" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E136" s="7"/>
-    </row>
-    <row r="137" spans="1:5">
-      <c r="A137" s="7" t="s">
+      <c r="B138" s="7" t="s">
+        <v>437</v>
+      </c>
+      <c r="C138" s="8" t="s">
+        <v>438</v>
+      </c>
+      <c r="D138" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E138" s="7"/>
+    </row>
+    <row r="139" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A139" s="7" t="s">
         <v>434</v>
       </c>
-      <c r="B137" s="7" t="s">
-        <v>438</v>
-      </c>
-      <c r="C137" s="7" t="s">
-        <v>437</v>
-      </c>
-      <c r="D137" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E137" s="7"/>
-    </row>
-    <row r="138" spans="1:5" ht="45">
-      <c r="A138" s="7" t="s">
-        <v>435</v>
-      </c>
-      <c r="B138" s="7" t="s">
+      <c r="B139" s="7" t="s">
+        <v>440</v>
+      </c>
+      <c r="C139" s="8" t="s">
         <v>439</v>
       </c>
-      <c r="C138" s="8" t="s">
-        <v>440</v>
-      </c>
-      <c r="D138" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E138" s="7"/>
-    </row>
-    <row r="139" spans="1:5" ht="30">
-      <c r="A139" s="7" t="s">
-        <v>436</v>
-      </c>
-      <c r="B139" s="7" t="s">
+      <c r="D139" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E139" s="7"/>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A140" s="17" t="s">
+        <v>441</v>
+      </c>
+      <c r="B140" s="7" t="s">
         <v>442</v>
       </c>
-      <c r="C139" s="8" t="s">
-        <v>441</v>
-      </c>
-      <c r="D139" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E139" s="7"/>
-    </row>
-    <row r="140" spans="1:5">
-      <c r="A140" s="17" t="s">
+      <c r="C140" s="8" t="s">
         <v>443</v>
       </c>
-      <c r="B140" s="7" t="s">
+      <c r="D140" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E140" s="7"/>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A141" s="17" t="s">
         <v>444</v>
       </c>
-      <c r="C140" s="8" t="s">
+      <c r="B141" s="7" t="s">
         <v>445</v>
       </c>
-      <c r="D140" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E140" s="7"/>
-    </row>
-    <row r="141" spans="1:5">
-      <c r="A141" s="17" t="s">
+      <c r="C141" s="8" t="s">
         <v>446</v>
       </c>
-      <c r="B141" s="7" t="s">
+      <c r="D141" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E141" s="7"/>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A142" s="17" t="s">
         <v>447</v>
       </c>
-      <c r="C141" s="8" t="s">
+      <c r="B142" s="7" t="s">
         <v>448</v>
       </c>
-      <c r="D141" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E141" s="7"/>
-    </row>
-    <row r="142" spans="1:5">
-      <c r="A142" s="17" t="s">
+      <c r="C142" s="8" t="s">
         <v>449</v>
       </c>
-      <c r="B142" s="7" t="s">
+      <c r="D142" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E142" s="7"/>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A143" s="17" t="s">
         <v>450</v>
       </c>
-      <c r="C142" s="8" t="s">
+      <c r="B143" s="7" t="s">
+        <v>452</v>
+      </c>
+      <c r="C143" s="8" t="s">
+        <v>453</v>
+      </c>
+      <c r="D143" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E143" s="7"/>
+    </row>
+    <row r="144" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A144" s="17" t="s">
         <v>451</v>
       </c>
-      <c r="D142" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E142" s="7"/>
-    </row>
-    <row r="143" spans="1:5">
-      <c r="A143" s="17" t="s">
-        <v>452</v>
-      </c>
-      <c r="B143" s="7" t="s">
+      <c r="B144" s="7" t="s">
+        <v>575</v>
+      </c>
+      <c r="C144" s="8" t="s">
+        <v>576</v>
+      </c>
+      <c r="D144" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E144" s="7"/>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A145" s="17" t="s">
         <v>454</v>
       </c>
-      <c r="C143" s="8" t="s">
+      <c r="B145" s="7" t="s">
+        <v>455</v>
+      </c>
+      <c r="C145" s="8" t="s">
         <v>456</v>
       </c>
-      <c r="D143" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E143" s="7"/>
-    </row>
-    <row r="144" spans="1:5">
-      <c r="A144" s="17" t="s">
-        <v>453</v>
-      </c>
-      <c r="B144" s="7" t="s">
-        <v>455</v>
-      </c>
-      <c r="C144" s="8" t="s">
+      <c r="D145" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E145" s="7"/>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A146" s="17" t="s">
         <v>457</v>
       </c>
-      <c r="D144" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E144" s="7"/>
-    </row>
-    <row r="145" spans="1:5">
-      <c r="A145" s="17" t="s">
+      <c r="B146" s="7" t="s">
+        <v>459</v>
+      </c>
+      <c r="C146" s="8" t="s">
         <v>458</v>
       </c>
-      <c r="B145" s="7" t="s">
-        <v>459</v>
-      </c>
-      <c r="C145" s="8" t="s">
+      <c r="D146" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E146" s="7"/>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A147" s="17" t="s">
         <v>460</v>
       </c>
-      <c r="D145" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E145" s="7"/>
-    </row>
-    <row r="146" spans="1:5">
-      <c r="A146" s="17" t="s">
+      <c r="B147" s="7" t="s">
+        <v>462</v>
+      </c>
+      <c r="C147" s="8" t="s">
         <v>461</v>
       </c>
-      <c r="B146" s="7" t="s">
+      <c r="D147" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E147" s="7"/>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A148" s="17" t="s">
         <v>463</v>
       </c>
-      <c r="C146" s="8" t="s">
-        <v>462</v>
-      </c>
-      <c r="D146" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E146" s="7"/>
-    </row>
-    <row r="147" spans="1:5">
-      <c r="A147" s="17" t="s">
+      <c r="B148" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="B147" s="7" t="s">
+      <c r="C148" s="8" t="s">
+        <v>465</v>
+      </c>
+      <c r="D148" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E148" s="7"/>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A149" s="7" t="s">
         <v>466</v>
       </c>
-      <c r="C147" s="8" t="s">
-        <v>465</v>
-      </c>
-      <c r="D147" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E147" s="7"/>
-    </row>
-    <row r="148" spans="1:5">
-      <c r="A148" s="17" t="s">
+      <c r="B149" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="C149" s="8" t="s">
+        <v>472</v>
+      </c>
+      <c r="D149" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E149" s="7"/>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A150" s="7" t="s">
         <v>467</v>
       </c>
-      <c r="B148" s="7" t="s">
+      <c r="B150" s="7" t="s">
+        <v>470</v>
+      </c>
+      <c r="C150" s="8" t="s">
+        <v>473</v>
+      </c>
+      <c r="D150" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E150" s="7"/>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A151" s="7" t="s">
         <v>468</v>
       </c>
-      <c r="C148" s="8" t="s">
-        <v>469</v>
-      </c>
-      <c r="D148" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E148" s="7"/>
-    </row>
-    <row r="149" spans="1:5">
-      <c r="A149" s="7" t="s">
-        <v>470</v>
-      </c>
-      <c r="B149" s="7" t="s">
-        <v>473</v>
-      </c>
-      <c r="C149" s="8" t="s">
+      <c r="B151" s="7" t="s">
+        <v>471</v>
+      </c>
+      <c r="C151" s="8" t="s">
+        <v>474</v>
+      </c>
+      <c r="D151" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E151" s="7"/>
+    </row>
+    <row r="152" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A152" s="7" t="s">
+        <v>475</v>
+      </c>
+      <c r="B152" s="7" t="s">
         <v>476</v>
       </c>
-      <c r="D149" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E149" s="7"/>
-    </row>
-    <row r="150" spans="1:5">
-      <c r="A150" s="7" t="s">
-        <v>471</v>
-      </c>
-      <c r="B150" s="7" t="s">
-        <v>474</v>
-      </c>
-      <c r="C150" s="8" t="s">
+      <c r="C152" s="8" t="s">
         <v>477</v>
       </c>
-      <c r="D150" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E150" s="7"/>
-    </row>
-    <row r="151" spans="1:5">
-      <c r="A151" s="7" t="s">
-        <v>472</v>
-      </c>
-      <c r="B151" s="7" t="s">
-        <v>475</v>
-      </c>
-      <c r="C151" s="8" t="s">
+      <c r="D152" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E152" s="7"/>
+    </row>
+    <row r="153" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A153" s="17" t="s">
         <v>478</v>
       </c>
-      <c r="D151" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E151" s="7"/>
-    </row>
-    <row r="152" spans="1:5" ht="30">
-      <c r="A152" s="7" t="s">
+      <c r="B153" s="7" t="s">
+        <v>497</v>
+      </c>
+      <c r="C153" s="8" t="s">
+        <v>498</v>
+      </c>
+      <c r="D153" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E153" s="7"/>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A154" s="17" t="s">
+        <v>480</v>
+      </c>
+      <c r="B154" s="7" t="s">
+        <v>481</v>
+      </c>
+      <c r="C154" s="8" t="s">
         <v>479</v>
       </c>
-      <c r="B152" s="7" t="s">
-        <v>480</v>
-      </c>
-      <c r="C152" s="8" t="s">
-        <v>481</v>
-      </c>
-      <c r="D152" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="E152" s="7"/>
-    </row>
-    <row r="153" spans="1:5" ht="45">
-      <c r="A153" s="17" t="s">
+      <c r="D154" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E154" s="7"/>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A155" s="7" t="s">
         <v>482</v>
       </c>
-      <c r="B153" s="7" t="s">
+      <c r="B155" s="7" t="s">
+        <v>483</v>
+      </c>
+      <c r="C155" s="8" t="s">
+        <v>484</v>
+      </c>
+      <c r="D155" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E155" s="7"/>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A156" s="7" t="s">
+        <v>485</v>
+      </c>
+      <c r="B156" s="7" t="s">
+        <v>486</v>
+      </c>
+      <c r="C156" s="8" t="s">
+        <v>487</v>
+      </c>
+      <c r="D156" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E156" s="7"/>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A157" s="7" t="s">
+        <v>488</v>
+      </c>
+      <c r="B157" s="7" t="s">
+        <v>489</v>
+      </c>
+      <c r="C157" s="8" t="s">
+        <v>490</v>
+      </c>
+      <c r="D157" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E157" s="7"/>
+    </row>
+    <row r="158" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A158" s="7" t="s">
+        <v>491</v>
+      </c>
+      <c r="B158" s="7" t="s">
+        <v>495</v>
+      </c>
+      <c r="C158" s="8" t="s">
+        <v>493</v>
+      </c>
+      <c r="D158" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E158" s="7"/>
+    </row>
+    <row r="159" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A159" s="7" t="s">
+        <v>492</v>
+      </c>
+      <c r="B159" s="7" t="s">
+        <v>496</v>
+      </c>
+      <c r="C159" s="8" t="s">
+        <v>494</v>
+      </c>
+      <c r="D159" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E159" s="7"/>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A160" s="7" t="s">
+        <v>499</v>
+      </c>
+      <c r="B160" s="7" t="s">
+        <v>507</v>
+      </c>
+      <c r="C160" s="8" t="s">
+        <v>506</v>
+      </c>
+      <c r="D160" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E160" s="7"/>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A161" s="7" t="s">
+        <v>500</v>
+      </c>
+      <c r="B161" s="7" t="s">
         <v>501</v>
       </c>
-      <c r="C153" s="8" t="s">
+      <c r="C161" s="8" t="s">
         <v>502</v>
       </c>
-      <c r="D153" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E153" s="7"/>
-    </row>
-    <row r="154" spans="1:5">
-      <c r="A154" s="17" t="s">
-        <v>484</v>
-      </c>
-      <c r="B154" s="7" t="s">
-        <v>485</v>
-      </c>
-      <c r="C154" s="8" t="s">
-        <v>483</v>
-      </c>
-      <c r="D154" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E154" s="7"/>
-    </row>
-    <row r="155" spans="1:5">
-      <c r="A155" s="7" t="s">
-        <v>486</v>
-      </c>
-      <c r="B155" s="7" t="s">
-        <v>487</v>
-      </c>
-      <c r="C155" s="8" t="s">
-        <v>488</v>
-      </c>
-      <c r="D155" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="E155" s="7"/>
-    </row>
-    <row r="156" spans="1:5">
-      <c r="A156" s="7" t="s">
-        <v>489</v>
-      </c>
-      <c r="B156" s="7" t="s">
-        <v>490</v>
-      </c>
-      <c r="C156" s="8" t="s">
-        <v>491</v>
-      </c>
-      <c r="D156" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E156" s="7"/>
-    </row>
-    <row r="157" spans="1:5">
-      <c r="A157" s="7" t="s">
-        <v>492</v>
-      </c>
-      <c r="B157" s="7" t="s">
-        <v>493</v>
-      </c>
-      <c r="C157" s="8" t="s">
-        <v>494</v>
-      </c>
-      <c r="D157" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="E157" s="7"/>
-    </row>
-    <row r="158" spans="1:5" ht="30">
-      <c r="A158" s="7" t="s">
-        <v>495</v>
-      </c>
-      <c r="B158" s="7" t="s">
-        <v>499</v>
-      </c>
-      <c r="C158" s="8" t="s">
-        <v>497</v>
-      </c>
-      <c r="D158" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="E158" s="7"/>
-    </row>
-    <row r="159" spans="1:5" ht="30">
-      <c r="A159" s="7" t="s">
-        <v>496</v>
-      </c>
-      <c r="B159" s="7" t="s">
-        <v>500</v>
-      </c>
-      <c r="C159" s="8" t="s">
-        <v>498</v>
-      </c>
-      <c r="D159" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="E159" s="7"/>
-    </row>
-    <row r="160" spans="1:5">
-      <c r="A160" s="7" t="s">
+      <c r="D161" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E161" s="7"/>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A162" s="7" t="s">
         <v>503</v>
       </c>
-      <c r="B160" s="7" t="s">
+      <c r="B162" s="7" t="s">
+        <v>504</v>
+      </c>
+      <c r="C162" s="8" t="s">
+        <v>505</v>
+      </c>
+      <c r="D162" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E162" s="7"/>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A163" s="7" t="s">
+        <v>508</v>
+      </c>
+      <c r="B163" s="7" t="s">
+        <v>509</v>
+      </c>
+      <c r="C163" s="8" t="s">
+        <v>510</v>
+      </c>
+      <c r="D163" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E163" s="7"/>
+    </row>
+    <row r="164" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A164" s="7" t="s">
         <v>511</v>
       </c>
-      <c r="C160" s="8" t="s">
-        <v>510</v>
-      </c>
-      <c r="D160" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="E160" s="7"/>
-    </row>
-    <row r="161" spans="1:5">
-      <c r="A161" s="7" t="s">
-        <v>504</v>
-      </c>
-      <c r="B161" s="7" t="s">
-        <v>505</v>
-      </c>
-      <c r="C161" s="8" t="s">
-        <v>506</v>
-      </c>
-      <c r="D161" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="E161" s="7"/>
-    </row>
-    <row r="162" spans="1:5">
-      <c r="A162" s="7" t="s">
-        <v>507</v>
-      </c>
-      <c r="B162" s="7" t="s">
-        <v>508</v>
-      </c>
-      <c r="C162" s="8" t="s">
-        <v>509</v>
-      </c>
-      <c r="D162" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="E162" s="7"/>
-    </row>
-    <row r="163" spans="1:5">
-      <c r="A163" s="7" t="s">
+      <c r="B164" s="7" t="s">
+        <v>513</v>
+      </c>
+      <c r="C164" s="8" t="s">
         <v>512</v>
       </c>
-      <c r="B163" s="7" t="s">
-        <v>513</v>
-      </c>
-      <c r="C163" s="8" t="s">
+      <c r="D164" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E164" s="7"/>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A165" s="7" t="s">
         <v>514</v>
       </c>
-      <c r="D163" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="E163" s="7"/>
-    </row>
-    <row r="164" spans="1:5" ht="30">
-      <c r="A164" s="7" t="s">
+      <c r="B165" s="7" t="s">
         <v>515</v>
       </c>
-      <c r="B164" s="7" t="s">
+      <c r="C165" s="8" t="s">
+        <v>516</v>
+      </c>
+      <c r="D165" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E165" s="7"/>
+    </row>
+    <row r="166" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A166" s="7" t="s">
         <v>517</v>
       </c>
-      <c r="C164" s="8" t="s">
-        <v>516</v>
-      </c>
-      <c r="D164" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E164" s="7"/>
-    </row>
-    <row r="165" spans="1:5">
-      <c r="A165" s="7" t="s">
+      <c r="B166" s="7" t="s">
         <v>518</v>
       </c>
-      <c r="B165" s="7" t="s">
+      <c r="C166" s="8" t="s">
         <v>519</v>
       </c>
-      <c r="C165" s="8" t="s">
+      <c r="D166" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E166" s="7"/>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A167" s="7" t="s">
+        <v>521</v>
+      </c>
+      <c r="B167" s="7" t="s">
         <v>520</v>
       </c>
-      <c r="D165" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="E165" s="7"/>
-    </row>
-    <row r="166" spans="1:5" ht="30">
-      <c r="A166" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="B166" s="7" t="s">
+      <c r="C167" s="8" t="s">
         <v>522</v>
       </c>
-      <c r="C166" s="8" t="s">
+      <c r="D167" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E167" s="7"/>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A168" s="7" t="s">
         <v>523</v>
       </c>
-      <c r="D166" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E166" s="7"/>
-    </row>
-    <row r="167" spans="1:5">
-      <c r="A167" s="7" t="s">
+      <c r="B168" s="7" t="s">
+        <v>524</v>
+      </c>
+      <c r="C168" s="8" t="s">
         <v>525</v>
       </c>
-      <c r="B167" s="7" t="s">
-        <v>524</v>
-      </c>
-      <c r="C167" s="8" t="s">
+      <c r="D168" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E168" s="7"/>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A169" s="7" t="s">
         <v>526</v>
       </c>
-      <c r="D167" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E167" s="7"/>
-    </row>
-    <row r="168" spans="1:5">
-      <c r="A168" s="7" t="s">
+      <c r="B169" s="7" t="s">
+        <v>529</v>
+      </c>
+      <c r="C169" s="8" t="s">
+        <v>532</v>
+      </c>
+      <c r="D169" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E169" s="7"/>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A170" s="7" t="s">
         <v>527</v>
       </c>
-      <c r="B168" s="7" t="s">
+      <c r="B170" s="7" t="s">
+        <v>530</v>
+      </c>
+      <c r="C170" s="8" t="s">
+        <v>533</v>
+      </c>
+      <c r="D170" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E170" s="7"/>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A171" s="7" t="s">
         <v>528</v>
       </c>
-      <c r="C168" s="8" t="s">
-        <v>529</v>
-      </c>
-      <c r="D168" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="E168" s="7"/>
-    </row>
-    <row r="169" spans="1:5">
-      <c r="A169" s="7" t="s">
-        <v>530</v>
-      </c>
-      <c r="B169" s="7" t="s">
-        <v>533</v>
-      </c>
-      <c r="C169" s="8" t="s">
+      <c r="B171" s="7" t="s">
+        <v>531</v>
+      </c>
+      <c r="C171" s="8" t="s">
+        <v>534</v>
+      </c>
+      <c r="D171" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E171" s="7"/>
+    </row>
+    <row r="172" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A172" s="7" t="s">
+        <v>535</v>
+      </c>
+      <c r="B172" s="7" t="s">
+        <v>515</v>
+      </c>
+      <c r="C172" s="8" t="s">
         <v>536</v>
       </c>
-      <c r="D169" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E169" s="7"/>
-    </row>
-    <row r="170" spans="1:5">
-      <c r="A170" s="7" t="s">
-        <v>531</v>
-      </c>
-      <c r="B170" s="7" t="s">
-        <v>534</v>
-      </c>
-      <c r="C170" s="8" t="s">
+      <c r="D172" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E172" s="7"/>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A173" s="9" t="s">
         <v>537</v>
       </c>
-      <c r="D170" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E170" s="7"/>
-    </row>
-    <row r="171" spans="1:5">
-      <c r="A171" s="7" t="s">
-        <v>532</v>
-      </c>
-      <c r="B171" s="7" t="s">
-        <v>535</v>
-      </c>
-      <c r="C171" s="8" t="s">
+      <c r="B173" s="7" t="s">
+        <v>541</v>
+      </c>
+      <c r="C173" s="8" t="s">
+        <v>542</v>
+      </c>
+      <c r="D173" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E173" s="7"/>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A174" s="9" t="s">
         <v>538</v>
       </c>
-      <c r="D171" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E171" s="7"/>
-    </row>
-    <row r="172" spans="1:5" ht="30">
-      <c r="A172" s="7" t="s">
+      <c r="B174" s="7" t="s">
+        <v>543</v>
+      </c>
+      <c r="C174" s="8" t="s">
+        <v>544</v>
+      </c>
+      <c r="D174" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E174" s="7"/>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A175" s="9" t="s">
         <v>539</v>
       </c>
-      <c r="B172" s="7" t="s">
-        <v>519</v>
-      </c>
-      <c r="C172" s="8" t="s">
-        <v>540</v>
-      </c>
-      <c r="D172" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="E172" s="7"/>
-    </row>
-    <row r="173" spans="1:5">
-      <c r="A173" s="9" t="s">
-        <v>541</v>
-      </c>
-      <c r="B173" s="7" t="s">
+      <c r="B175" s="7" t="s">
         <v>545</v>
-      </c>
-      <c r="C173" s="8" t="s">
-        <v>546</v>
-      </c>
-      <c r="D173" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E173" s="7"/>
-    </row>
-    <row r="174" spans="1:5">
-      <c r="A174" s="9" t="s">
-        <v>542</v>
-      </c>
-      <c r="B174" s="7" t="s">
-        <v>547</v>
-      </c>
-      <c r="C174" s="8" t="s">
-        <v>548</v>
-      </c>
-      <c r="D174" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E174" s="7"/>
-    </row>
-    <row r="175" spans="1:5">
-      <c r="A175" s="9" t="s">
-        <v>543</v>
-      </c>
-      <c r="B175" s="7" t="s">
-        <v>549</v>
       </c>
       <c r="C175" s="8" t="s">
         <v>231</v>
@@ -4854,150 +4856,150 @@
       </c>
       <c r="E175" s="7"/>
     </row>
-    <row r="176" spans="1:5">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A176" s="9" t="s">
-        <v>544</v>
+        <v>540</v>
       </c>
       <c r="B176" s="7" t="s">
+        <v>546</v>
+      </c>
+      <c r="C176" s="8" t="s">
+        <v>547</v>
+      </c>
+      <c r="D176" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E176" s="7"/>
+    </row>
+    <row r="177" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A177" s="7" t="s">
+        <v>548</v>
+      </c>
+      <c r="B177" s="7" t="s">
+        <v>549</v>
+      </c>
+      <c r="C177" s="8" t="s">
         <v>550</v>
       </c>
-      <c r="C176" s="8" t="s">
+      <c r="D177" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E177" s="7"/>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A178" s="7" t="s">
         <v>551</v>
       </c>
-      <c r="D176" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E176" s="7"/>
-    </row>
-    <row r="177" spans="1:5" ht="30">
-      <c r="A177" s="7" t="s">
+      <c r="B178" s="7" t="s">
         <v>552</v>
       </c>
-      <c r="B177" s="7" t="s">
+      <c r="C178" s="8" t="s">
         <v>553</v>
       </c>
-      <c r="C177" s="8" t="s">
+      <c r="D178" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E178" s="7"/>
+    </row>
+    <row r="179" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A179" s="7" t="s">
+        <v>555</v>
+      </c>
+      <c r="B179" s="7" t="s">
+        <v>556</v>
+      </c>
+      <c r="C179" s="8" t="s">
         <v>554</v>
       </c>
-      <c r="D177" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="E177" s="7"/>
-    </row>
-    <row r="178" spans="1:5">
-      <c r="A178" s="7" t="s">
-        <v>555</v>
-      </c>
-      <c r="B178" s="7" t="s">
-        <v>556</v>
-      </c>
-      <c r="C178" s="8" t="s">
+      <c r="D179" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E179" s="7"/>
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A180" s="7" t="s">
         <v>557</v>
       </c>
-      <c r="D178" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="E178" s="7"/>
-    </row>
-    <row r="179" spans="1:5" ht="30">
-      <c r="A179" s="7" t="s">
+      <c r="B180" s="7" t="s">
+        <v>558</v>
+      </c>
+      <c r="C180" s="8" t="s">
         <v>559</v>
       </c>
-      <c r="B179" s="7" t="s">
+      <c r="D180" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E180" s="7"/>
+    </row>
+    <row r="181" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A181" s="7" t="s">
         <v>560</v>
       </c>
-      <c r="C179" s="8" t="s">
-        <v>558</v>
-      </c>
-      <c r="D179" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="E179" s="7"/>
-    </row>
-    <row r="180" spans="1:5">
-      <c r="A180" s="7" t="s">
+      <c r="B181" s="7" t="s">
         <v>561</v>
       </c>
-      <c r="B180" s="7" t="s">
+      <c r="C181" s="8" t="s">
         <v>562</v>
       </c>
-      <c r="C180" s="8" t="s">
+      <c r="D181" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E181" s="7"/>
+    </row>
+    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A182" s="7" t="s">
         <v>563</v>
       </c>
-      <c r="D180" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="E180" s="7"/>
-    </row>
-    <row r="181" spans="1:5" ht="30">
-      <c r="A181" s="7" t="s">
+      <c r="B182" s="7" t="s">
         <v>564</v>
       </c>
-      <c r="B181" s="7" t="s">
+      <c r="C182" s="8" t="s">
         <v>565</v>
       </c>
-      <c r="C181" s="8" t="s">
+      <c r="D182" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E182" s="7"/>
+    </row>
+    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A183" s="7" t="s">
         <v>566</v>
       </c>
-      <c r="D181" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="E181" s="7"/>
-    </row>
-    <row r="182" spans="1:5">
-      <c r="A182" s="7" t="s">
+      <c r="B183" s="7" t="s">
+        <v>568</v>
+      </c>
+      <c r="C183" s="8" t="s">
         <v>567</v>
       </c>
-      <c r="B182" s="7" t="s">
-        <v>568</v>
-      </c>
-      <c r="C182" s="8" t="s">
+      <c r="D183" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E183" s="7"/>
+    </row>
+    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A184" s="9" t="s">
         <v>569</v>
       </c>
-      <c r="D182" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="E182" s="7"/>
-    </row>
-    <row r="183" spans="1:5">
-      <c r="A183" s="7" t="s">
+      <c r="B184" s="7" t="s">
+        <v>571</v>
+      </c>
+      <c r="C184" s="8" t="s">
+        <v>572</v>
+      </c>
+      <c r="D184" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E184" s="7"/>
+    </row>
+    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A185" s="9" t="s">
         <v>570</v>
       </c>
-      <c r="B183" s="7" t="s">
-        <v>572</v>
-      </c>
-      <c r="C183" s="8" t="s">
-        <v>571</v>
-      </c>
-      <c r="D183" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="E183" s="7"/>
-    </row>
-    <row r="184" spans="1:5">
-      <c r="A184" s="9" t="s">
+      <c r="B185" s="7" t="s">
+        <v>574</v>
+      </c>
+      <c r="C185" s="8" t="s">
         <v>573</v>
-      </c>
-      <c r="B184" s="7" t="s">
-        <v>575</v>
-      </c>
-      <c r="C184" s="8" t="s">
-        <v>576</v>
-      </c>
-      <c r="D184" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="E184" s="7"/>
-    </row>
-    <row r="185" spans="1:5">
-      <c r="A185" s="9" t="s">
-        <v>574</v>
-      </c>
-      <c r="B185" s="7" t="s">
-        <v>578</v>
-      </c>
-      <c r="C185" s="8" t="s">
-        <v>577</v>
       </c>
       <c r="D185" s="9" t="s">
         <v>5</v>
@@ -5015,14 +5017,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView topLeftCell="A10" zoomScale="80" workbookViewId="0">
       <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
@@ -5030,7 +5032,7 @@
     <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>35</v>
       </c>
@@ -5044,7 +5046,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>37</v>
       </c>
@@ -5056,7 +5058,7 @@
       </c>
       <c r="D2" s="7"/>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>38</v>
       </c>
@@ -5068,7 +5070,7 @@
       </c>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>39</v>
       </c>
@@ -5080,7 +5082,7 @@
       </c>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>40</v>
       </c>
@@ -5092,7 +5094,7 @@
       </c>
       <c r="D5" s="7"/>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>41</v>
       </c>
@@ -5104,7 +5106,7 @@
       </c>
       <c r="D6" s="7"/>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>42</v>
       </c>
@@ -5116,7 +5118,7 @@
       </c>
       <c r="D7" s="7"/>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>43</v>
       </c>
@@ -5128,7 +5130,7 @@
       </c>
       <c r="D8" s="7"/>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>44</v>
       </c>
@@ -5140,7 +5142,7 @@
       </c>
       <c r="D9" s="7"/>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>45</v>
       </c>
@@ -5152,7 +5154,7 @@
       </c>
       <c r="D10" s="7"/>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>46</v>
       </c>
@@ -5164,7 +5166,7 @@
       </c>
       <c r="D11" s="7"/>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>48</v>
       </c>
@@ -5176,7 +5178,7 @@
       </c>
       <c r="D12" s="7"/>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>49</v>
       </c>
@@ -5188,7 +5190,7 @@
       </c>
       <c r="D13" s="7"/>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>50</v>
       </c>
@@ -5200,7 +5202,7 @@
       </c>
       <c r="D14" s="7"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>51</v>
       </c>
@@ -5212,7 +5214,7 @@
       </c>
       <c r="D15" s="7"/>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>52</v>
       </c>
@@ -5224,7 +5226,7 @@
       </c>
       <c r="D16" s="7"/>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>53</v>
       </c>
@@ -5236,7 +5238,7 @@
       </c>
       <c r="D17" s="7"/>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>54</v>
       </c>
@@ -5248,7 +5250,7 @@
       </c>
       <c r="D18" s="7"/>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>55</v>
       </c>
@@ -5260,7 +5262,7 @@
       </c>
       <c r="D19" s="7"/>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>56</v>
       </c>
@@ -5272,7 +5274,7 @@
       </c>
       <c r="D20" s="7"/>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>57</v>
       </c>
@@ -5284,7 +5286,7 @@
       </c>
       <c r="D21" s="7"/>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>58</v>
       </c>
@@ -5296,7 +5298,7 @@
       </c>
       <c r="D22" s="7"/>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>59</v>
       </c>
@@ -5308,7 +5310,7 @@
       </c>
       <c r="D23" s="7"/>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>60</v>
       </c>
@@ -5320,7 +5322,7 @@
       </c>
       <c r="D24" s="7"/>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>61</v>
       </c>
@@ -5332,7 +5334,7 @@
       </c>
       <c r="D25" s="7"/>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>47</v>
       </c>
@@ -5351,14 +5353,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A19" sqref="A19:XFD19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
@@ -5366,7 +5368,7 @@
     <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>35</v>
       </c>
@@ -5380,7 +5382,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>37</v>
       </c>
@@ -5392,7 +5394,7 @@
       </c>
       <c r="D2" s="7"/>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>38</v>
       </c>
@@ -5404,7 +5406,7 @@
       </c>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>39</v>
       </c>
@@ -5416,7 +5418,7 @@
       </c>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>40</v>
       </c>
@@ -5428,7 +5430,7 @@
       </c>
       <c r="D5" s="7"/>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>41</v>
       </c>
@@ -5440,7 +5442,7 @@
       </c>
       <c r="D6" s="7"/>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>42</v>
       </c>
@@ -5452,7 +5454,7 @@
       </c>
       <c r="D7" s="7"/>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>43</v>
       </c>
@@ -5464,7 +5466,7 @@
       </c>
       <c r="D8" s="7"/>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>44</v>
       </c>
@@ -5476,7 +5478,7 @@
       </c>
       <c r="D9" s="7"/>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>45</v>
       </c>
@@ -5488,7 +5490,7 @@
       </c>
       <c r="D10" s="7"/>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>46</v>
       </c>
@@ -5500,7 +5502,7 @@
       </c>
       <c r="D11" s="7"/>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>47</v>
       </c>
@@ -5512,7 +5514,7 @@
       </c>
       <c r="D12" s="7"/>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>48</v>
       </c>
@@ -5524,7 +5526,7 @@
       </c>
       <c r="D13" s="7"/>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>49</v>
       </c>
@@ -5536,7 +5538,7 @@
       </c>
       <c r="D14" s="7"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>50</v>
       </c>
@@ -5548,7 +5550,7 @@
       </c>
       <c r="D15" s="7"/>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>51</v>
       </c>
@@ -5560,7 +5562,7 @@
       </c>
       <c r="D16" s="7"/>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>52</v>
       </c>
@@ -5572,7 +5574,7 @@
       </c>
       <c r="D17" s="7"/>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>53</v>
       </c>
@@ -5584,7 +5586,7 @@
       </c>
       <c r="D18" s="7"/>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>54</v>
       </c>
@@ -5596,7 +5598,7 @@
       </c>
       <c r="D19" s="7"/>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>55</v>
       </c>
@@ -5608,7 +5610,7 @@
       </c>
       <c r="D20" s="7"/>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>56</v>
       </c>
@@ -5620,7 +5622,7 @@
       </c>
       <c r="D21" s="7"/>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>57</v>
       </c>
@@ -5632,7 +5634,7 @@
       </c>
       <c r="D22" s="7"/>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>58</v>
       </c>
@@ -5644,7 +5646,7 @@
       </c>
       <c r="D23" s="7"/>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>59</v>
       </c>
@@ -5656,7 +5658,7 @@
       </c>
       <c r="D24" s="7"/>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>60</v>
       </c>
@@ -5668,7 +5670,7 @@
       </c>
       <c r="D25" s="7"/>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>61</v>
       </c>

</xml_diff>

<commit_message>
Adds WAT-190 & WAT-191 test script and related changes
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/WAT.xlsx
+++ b/src/test/resources/xls/WAT.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13305" windowHeight="2415"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="907" uniqueCount="585">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="915" uniqueCount="591">
   <si>
     <t>TCID</t>
   </si>
@@ -1773,13 +1773,31 @@
   </si>
   <si>
     <t>Verify that updated(accepted/rejected) recommended paper last names exactly matches one of the last name variants on the author record.</t>
+  </si>
+  <si>
+    <t>WAT190</t>
+  </si>
+  <si>
+    <t>WAT191</t>
+  </si>
+  <si>
+    <t>WAT-919</t>
+  </si>
+  <si>
+    <t>WAT-912</t>
+  </si>
+  <si>
+    <t>Verify that System must display a maximum of 3 recommendations on the author record at a time(For Single Author)</t>
+  </si>
+  <si>
+    <t>Verify that System must display a maximum of 3 recommendations on the author record at a time(For Cmbined Author)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1988,7 +2006,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2020,9 +2038,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2054,6 +2073,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2229,14 +2249,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E187"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E189"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A164" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I177" sqref="I177"/>
+      <selection activeCell="C189" sqref="C189"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="30.5703125" customWidth="1" collapsed="1"/>
@@ -2245,7 +2265,7 @@
     <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2262,7 +2282,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -2277,7 +2297,7 @@
       </c>
       <c r="E2" s="4"/>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -2292,7 +2312,7 @@
       </c>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>11</v>
       </c>
@@ -2307,7 +2327,7 @@
       </c>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>12</v>
       </c>
@@ -2322,7 +2342,7 @@
       </c>
       <c r="E5" s="7"/>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>14</v>
       </c>
@@ -2337,7 +2357,7 @@
       </c>
       <c r="E6" s="7"/>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>17</v>
       </c>
@@ -2352,7 +2372,7 @@
       </c>
       <c r="E7" s="7"/>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>20</v>
       </c>
@@ -2367,7 +2387,7 @@
       </c>
       <c r="E8" s="7"/>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>22</v>
       </c>
@@ -2382,7 +2402,7 @@
       </c>
       <c r="E9" s="7"/>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>23</v>
       </c>
@@ -2397,7 +2417,7 @@
       </c>
       <c r="E10" s="7"/>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>24</v>
       </c>
@@ -2412,7 +2432,7 @@
       </c>
       <c r="E11" s="7"/>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>25</v>
       </c>
@@ -2427,7 +2447,7 @@
       </c>
       <c r="E12" s="7"/>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>62</v>
       </c>
@@ -2442,7 +2462,7 @@
       </c>
       <c r="E13" s="7"/>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>63</v>
       </c>
@@ -2457,7 +2477,7 @@
       </c>
       <c r="E14" s="7"/>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>64</v>
       </c>
@@ -2472,7 +2492,7 @@
       </c>
       <c r="E15" s="7"/>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>65</v>
       </c>
@@ -2487,7 +2507,7 @@
       </c>
       <c r="E16" s="7"/>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>74</v>
       </c>
@@ -2502,7 +2522,7 @@
       </c>
       <c r="E17" s="7"/>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>75</v>
       </c>
@@ -2517,7 +2537,7 @@
       </c>
       <c r="E18" s="7"/>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>79</v>
       </c>
@@ -2532,7 +2552,7 @@
       </c>
       <c r="E19" s="7"/>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>81</v>
       </c>
@@ -2547,7 +2567,7 @@
       </c>
       <c r="E20" s="7"/>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>82</v>
       </c>
@@ -2562,7 +2582,7 @@
       </c>
       <c r="E21" s="7"/>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>88</v>
       </c>
@@ -2577,7 +2597,7 @@
       </c>
       <c r="E22" s="7"/>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>90</v>
       </c>
@@ -2592,7 +2612,7 @@
       </c>
       <c r="E23" s="7"/>
     </row>
-    <row r="24" spans="1:5" ht="30">
+    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>94</v>
       </c>
@@ -2607,7 +2627,7 @@
       </c>
       <c r="E24" s="7"/>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>96</v>
       </c>
@@ -2622,7 +2642,7 @@
       </c>
       <c r="E25" s="7"/>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
         <v>98</v>
       </c>
@@ -2637,7 +2657,7 @@
       </c>
       <c r="E26" s="7"/>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
         <v>102</v>
       </c>
@@ -2652,7 +2672,7 @@
       </c>
       <c r="E27" s="7"/>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
         <v>105</v>
       </c>
@@ -2667,7 +2687,7 @@
       </c>
       <c r="E28" s="7"/>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
         <v>108</v>
       </c>
@@ -2682,7 +2702,7 @@
       </c>
       <c r="E29" s="7"/>
     </row>
-    <row r="30" spans="1:5" ht="30">
+    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
         <v>110</v>
       </c>
@@ -2697,7 +2717,7 @@
       </c>
       <c r="E30" s="7"/>
     </row>
-    <row r="31" spans="1:5" ht="30">
+    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
         <v>114</v>
       </c>
@@ -2712,7 +2732,7 @@
       </c>
       <c r="E31" s="7"/>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
         <v>119</v>
       </c>
@@ -2727,7 +2747,7 @@
       </c>
       <c r="E32" s="7"/>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
         <v>120</v>
       </c>
@@ -2742,7 +2762,7 @@
       </c>
       <c r="E33" s="7"/>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
         <v>125</v>
       </c>
@@ -2757,7 +2777,7 @@
       </c>
       <c r="E34" s="7"/>
     </row>
-    <row r="35" spans="1:5" ht="30">
+    <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
         <v>128</v>
       </c>
@@ -2772,7 +2792,7 @@
       </c>
       <c r="E35" s="7"/>
     </row>
-    <row r="36" spans="1:5" ht="30">
+    <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
         <v>131</v>
       </c>
@@ -2787,7 +2807,7 @@
       </c>
       <c r="E36" s="7"/>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
         <v>134</v>
       </c>
@@ -2802,7 +2822,7 @@
       </c>
       <c r="E37" s="7"/>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="9" t="s">
         <v>137</v>
       </c>
@@ -2817,7 +2837,7 @@
       </c>
       <c r="E38" s="7"/>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="s">
         <v>140</v>
       </c>
@@ -2832,7 +2852,7 @@
       </c>
       <c r="E39" s="7"/>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="9" t="s">
         <v>143</v>
       </c>
@@ -2847,7 +2867,7 @@
       </c>
       <c r="E40" s="7"/>
     </row>
-    <row r="41" spans="1:5" ht="30">
+    <row r="41" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
         <v>145</v>
       </c>
@@ -2862,7 +2882,7 @@
       </c>
       <c r="E41" s="7"/>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="9" t="s">
         <v>147</v>
       </c>
@@ -2877,7 +2897,7 @@
       </c>
       <c r="E42" s="7"/>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="9" t="s">
         <v>150</v>
       </c>
@@ -2892,7 +2912,7 @@
       </c>
       <c r="E43" s="7"/>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="9" t="s">
         <v>153</v>
       </c>
@@ -2907,7 +2927,7 @@
       </c>
       <c r="E44" s="7"/>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="9" t="s">
         <v>155</v>
       </c>
@@ -2922,7 +2942,7 @@
       </c>
       <c r="E45" s="7"/>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="12" t="s">
         <v>158</v>
       </c>
@@ -2937,7 +2957,7 @@
       </c>
       <c r="E46" s="7"/>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="12" t="s">
         <v>159</v>
       </c>
@@ -2952,7 +2972,7 @@
       </c>
       <c r="E47" s="7"/>
     </row>
-    <row r="48" spans="1:5" ht="30">
+    <row r="48" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="12" t="s">
         <v>160</v>
       </c>
@@ -2967,7 +2987,7 @@
       </c>
       <c r="E48" s="7"/>
     </row>
-    <row r="49" spans="1:5" ht="30">
+    <row r="49" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="12" t="s">
         <v>161</v>
       </c>
@@ -2982,7 +3002,7 @@
       </c>
       <c r="E49" s="7"/>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="12" t="s">
         <v>164</v>
       </c>
@@ -2997,7 +3017,7 @@
       </c>
       <c r="E50" s="7"/>
     </row>
-    <row r="51" spans="1:5" ht="30">
+    <row r="51" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="9" t="s">
         <v>173</v>
       </c>
@@ -3012,7 +3032,7 @@
       </c>
       <c r="E51" s="7"/>
     </row>
-    <row r="52" spans="1:5">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="9" t="s">
         <v>174</v>
       </c>
@@ -3027,7 +3047,7 @@
       </c>
       <c r="E52" s="7"/>
     </row>
-    <row r="53" spans="1:5">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="9" t="s">
         <v>179</v>
       </c>
@@ -3042,7 +3062,7 @@
       </c>
       <c r="E53" s="7"/>
     </row>
-    <row r="54" spans="1:5">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="9" t="s">
         <v>180</v>
       </c>
@@ -3057,7 +3077,7 @@
       </c>
       <c r="E54" s="7"/>
     </row>
-    <row r="55" spans="1:5">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="9" t="s">
         <v>185</v>
       </c>
@@ -3072,7 +3092,7 @@
       </c>
       <c r="E55" s="7"/>
     </row>
-    <row r="56" spans="1:5">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="s">
         <v>188</v>
       </c>
@@ -3087,7 +3107,7 @@
       </c>
       <c r="E56" s="7"/>
     </row>
-    <row r="57" spans="1:5" ht="30">
+    <row r="57" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="9" t="s">
         <v>191</v>
       </c>
@@ -3102,7 +3122,7 @@
       </c>
       <c r="E57" s="7"/>
     </row>
-    <row r="58" spans="1:5">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="9" t="s">
         <v>194</v>
       </c>
@@ -3117,7 +3137,7 @@
       </c>
       <c r="E58" s="7"/>
     </row>
-    <row r="59" spans="1:5">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
         <v>196</v>
       </c>
@@ -3132,7 +3152,7 @@
       </c>
       <c r="E59" s="7"/>
     </row>
-    <row r="60" spans="1:5" ht="45">
+    <row r="60" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
         <v>199</v>
       </c>
@@ -3147,7 +3167,7 @@
       </c>
       <c r="E60" s="7"/>
     </row>
-    <row r="61" spans="1:5">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="9" t="s">
         <v>202</v>
       </c>
@@ -3162,7 +3182,7 @@
       </c>
       <c r="E61" s="7"/>
     </row>
-    <row r="62" spans="1:5">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="9" t="s">
         <v>204</v>
       </c>
@@ -3177,7 +3197,7 @@
       </c>
       <c r="E62" s="7"/>
     </row>
-    <row r="63" spans="1:5">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="9" t="s">
         <v>206</v>
       </c>
@@ -3192,7 +3212,7 @@
       </c>
       <c r="E63" s="7"/>
     </row>
-    <row r="64" spans="1:5">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="9" t="s">
         <v>208</v>
       </c>
@@ -3207,7 +3227,7 @@
       </c>
       <c r="E64" s="7"/>
     </row>
-    <row r="65" spans="1:5">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="9" t="s">
         <v>217</v>
       </c>
@@ -3222,7 +3242,7 @@
       </c>
       <c r="E65" s="7"/>
     </row>
-    <row r="66" spans="1:5">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="9" t="s">
         <v>218</v>
       </c>
@@ -3237,7 +3257,7 @@
       </c>
       <c r="E66" s="7"/>
     </row>
-    <row r="67" spans="1:5">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="9" t="s">
         <v>223</v>
       </c>
@@ -3252,7 +3272,7 @@
       </c>
       <c r="E67" s="7"/>
     </row>
-    <row r="68" spans="1:5">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="9" t="s">
         <v>224</v>
       </c>
@@ -3267,7 +3287,7 @@
       </c>
       <c r="E68" s="7"/>
     </row>
-    <row r="69" spans="1:5">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="9" t="s">
         <v>225</v>
       </c>
@@ -3282,7 +3302,7 @@
       </c>
       <c r="E69" s="7"/>
     </row>
-    <row r="70" spans="1:5">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="9" t="s">
         <v>226</v>
       </c>
@@ -3297,7 +3317,7 @@
       </c>
       <c r="E70" s="7"/>
     </row>
-    <row r="71" spans="1:5">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="9" t="s">
         <v>233</v>
       </c>
@@ -3312,7 +3332,7 @@
       </c>
       <c r="E71" s="7"/>
     </row>
-    <row r="72" spans="1:5">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="9" t="s">
         <v>237</v>
       </c>
@@ -3327,7 +3347,7 @@
       </c>
       <c r="E72" s="7"/>
     </row>
-    <row r="73" spans="1:5">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="9" t="s">
         <v>239</v>
       </c>
@@ -3342,7 +3362,7 @@
       </c>
       <c r="E73" s="7"/>
     </row>
-    <row r="74" spans="1:5">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="9" t="s">
         <v>243</v>
       </c>
@@ -3357,7 +3377,7 @@
       </c>
       <c r="E74" s="7"/>
     </row>
-    <row r="75" spans="1:5" ht="30">
+    <row r="75" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" s="9" t="s">
         <v>245</v>
       </c>
@@ -3372,7 +3392,7 @@
       </c>
       <c r="E75" s="7"/>
     </row>
-    <row r="76" spans="1:5">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="9" t="s">
         <v>248</v>
       </c>
@@ -3387,7 +3407,7 @@
       </c>
       <c r="E76" s="7"/>
     </row>
-    <row r="77" spans="1:5">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="9" t="s">
         <v>256</v>
       </c>
@@ -3402,7 +3422,7 @@
       </c>
       <c r="E77" s="7"/>
     </row>
-    <row r="78" spans="1:5">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="9" t="s">
         <v>257</v>
       </c>
@@ -3417,7 +3437,7 @@
       </c>
       <c r="E78" s="7"/>
     </row>
-    <row r="79" spans="1:5">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="9" t="s">
         <v>261</v>
       </c>
@@ -3432,7 +3452,7 @@
       </c>
       <c r="E79" s="7"/>
     </row>
-    <row r="80" spans="1:5">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="9" t="s">
         <v>264</v>
       </c>
@@ -3447,7 +3467,7 @@
       </c>
       <c r="E80" s="7"/>
     </row>
-    <row r="81" spans="1:5">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="9" t="s">
         <v>267</v>
       </c>
@@ -3462,7 +3482,7 @@
       </c>
       <c r="E81" s="7"/>
     </row>
-    <row r="82" spans="1:5" ht="30">
+    <row r="82" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A82" s="9" t="s">
         <v>269</v>
       </c>
@@ -3477,7 +3497,7 @@
       </c>
       <c r="E82" s="7"/>
     </row>
-    <row r="83" spans="1:5">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="9" t="s">
         <v>274</v>
       </c>
@@ -3492,7 +3512,7 @@
       </c>
       <c r="E83" s="7"/>
     </row>
-    <row r="84" spans="1:5" ht="30">
+    <row r="84" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A84" s="9" t="s">
         <v>277</v>
       </c>
@@ -3507,7 +3527,7 @@
       </c>
       <c r="E84" s="7"/>
     </row>
-    <row r="85" spans="1:5">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="9" t="s">
         <v>279</v>
       </c>
@@ -3522,7 +3542,7 @@
       </c>
       <c r="E85" s="7"/>
     </row>
-    <row r="86" spans="1:5">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="9" t="s">
         <v>282</v>
       </c>
@@ -3537,7 +3557,7 @@
       </c>
       <c r="E86" s="7"/>
     </row>
-    <row r="87" spans="1:5">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="9" t="s">
         <v>285</v>
       </c>
@@ -3552,7 +3572,7 @@
       </c>
       <c r="E87" s="7"/>
     </row>
-    <row r="88" spans="1:5">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="9" t="s">
         <v>288</v>
       </c>
@@ -3567,7 +3587,7 @@
       </c>
       <c r="E88" s="7"/>
     </row>
-    <row r="89" spans="1:5">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="9" t="s">
         <v>291</v>
       </c>
@@ -3582,7 +3602,7 @@
       </c>
       <c r="E89" s="7"/>
     </row>
-    <row r="90" spans="1:5">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="9" t="s">
         <v>294</v>
       </c>
@@ -3597,7 +3617,7 @@
       </c>
       <c r="E90" s="7"/>
     </row>
-    <row r="91" spans="1:5">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="9" t="s">
         <v>297</v>
       </c>
@@ -3612,7 +3632,7 @@
       </c>
       <c r="E91" s="7"/>
     </row>
-    <row r="92" spans="1:5">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="9" t="s">
         <v>300</v>
       </c>
@@ -3627,7 +3647,7 @@
       </c>
       <c r="E92" s="7"/>
     </row>
-    <row r="93" spans="1:5">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="9" t="s">
         <v>303</v>
       </c>
@@ -3642,7 +3662,7 @@
       </c>
       <c r="E93" s="7"/>
     </row>
-    <row r="94" spans="1:5">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="9" t="s">
         <v>306</v>
       </c>
@@ -3657,7 +3677,7 @@
       </c>
       <c r="E94" s="7"/>
     </row>
-    <row r="95" spans="1:5">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="9" t="s">
         <v>309</v>
       </c>
@@ -3672,7 +3692,7 @@
       </c>
       <c r="E95" s="7"/>
     </row>
-    <row r="96" spans="1:5">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="9" t="s">
         <v>314</v>
       </c>
@@ -3687,7 +3707,7 @@
       </c>
       <c r="E96" s="7"/>
     </row>
-    <row r="97" spans="1:5">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="9" t="s">
         <v>315</v>
       </c>
@@ -3702,7 +3722,7 @@
       </c>
       <c r="E97" s="7"/>
     </row>
-    <row r="98" spans="1:5">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="9" t="s">
         <v>319</v>
       </c>
@@ -3717,7 +3737,7 @@
       </c>
       <c r="E98" s="7"/>
     </row>
-    <row r="99" spans="1:5">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="9" t="s">
         <v>321</v>
       </c>
@@ -3732,7 +3752,7 @@
       </c>
       <c r="E99" s="7"/>
     </row>
-    <row r="100" spans="1:5">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="9" t="s">
         <v>322</v>
       </c>
@@ -3747,7 +3767,7 @@
       </c>
       <c r="E100" s="7"/>
     </row>
-    <row r="101" spans="1:5" ht="30">
+    <row r="101" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A101" s="9" t="s">
         <v>323</v>
       </c>
@@ -3762,7 +3782,7 @@
       </c>
       <c r="E101" s="7"/>
     </row>
-    <row r="102" spans="1:5">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="9" t="s">
         <v>328</v>
       </c>
@@ -3777,7 +3797,7 @@
       </c>
       <c r="E102" s="7"/>
     </row>
-    <row r="103" spans="1:5">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="9" t="s">
         <v>333</v>
       </c>
@@ -3792,7 +3812,7 @@
       </c>
       <c r="E103" s="7"/>
     </row>
-    <row r="104" spans="1:5">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="9" t="s">
         <v>336</v>
       </c>
@@ -3807,7 +3827,7 @@
       </c>
       <c r="E104" s="7"/>
     </row>
-    <row r="105" spans="1:5">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="9" t="s">
         <v>337</v>
       </c>
@@ -3822,7 +3842,7 @@
       </c>
       <c r="E105" s="7"/>
     </row>
-    <row r="106" spans="1:5">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="9" t="s">
         <v>342</v>
       </c>
@@ -3837,7 +3857,7 @@
       </c>
       <c r="E106" s="7"/>
     </row>
-    <row r="107" spans="1:5">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="9" t="s">
         <v>345</v>
       </c>
@@ -3852,7 +3872,7 @@
       </c>
       <c r="E107" s="7"/>
     </row>
-    <row r="108" spans="1:5">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="9" t="s">
         <v>350</v>
       </c>
@@ -3867,7 +3887,7 @@
       </c>
       <c r="E108" s="7"/>
     </row>
-    <row r="109" spans="1:5" ht="30">
+    <row r="109" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A109" s="9" t="s">
         <v>351</v>
       </c>
@@ -3882,7 +3902,7 @@
       </c>
       <c r="E109" s="7"/>
     </row>
-    <row r="110" spans="1:5">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="9" t="s">
         <v>352</v>
       </c>
@@ -3897,7 +3917,7 @@
       </c>
       <c r="E110" s="7"/>
     </row>
-    <row r="111" spans="1:5">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="9" t="s">
         <v>355</v>
       </c>
@@ -3912,7 +3932,7 @@
       </c>
       <c r="E111" s="7"/>
     </row>
-    <row r="112" spans="1:5">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="9" t="s">
         <v>359</v>
       </c>
@@ -3927,7 +3947,7 @@
       </c>
       <c r="E112" s="7"/>
     </row>
-    <row r="113" spans="1:5">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="9" t="s">
         <v>361</v>
       </c>
@@ -3942,7 +3962,7 @@
       </c>
       <c r="E113" s="7"/>
     </row>
-    <row r="114" spans="1:5" ht="30">
+    <row r="114" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A114" s="9" t="s">
         <v>364</v>
       </c>
@@ -3957,7 +3977,7 @@
       </c>
       <c r="E114" s="7"/>
     </row>
-    <row r="115" spans="1:5">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="9" t="s">
         <v>367</v>
       </c>
@@ -3972,7 +3992,7 @@
       </c>
       <c r="E115" s="7"/>
     </row>
-    <row r="116" spans="1:5">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="9" t="s">
         <v>368</v>
       </c>
@@ -3987,7 +4007,7 @@
       </c>
       <c r="E116" s="7"/>
     </row>
-    <row r="117" spans="1:5">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" s="9" t="s">
         <v>369</v>
       </c>
@@ -4002,7 +4022,7 @@
       </c>
       <c r="E117" s="7"/>
     </row>
-    <row r="118" spans="1:5">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" s="9" t="s">
         <v>376</v>
       </c>
@@ -4017,7 +4037,7 @@
       </c>
       <c r="E118" s="7"/>
     </row>
-    <row r="119" spans="1:5">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" s="9" t="s">
         <v>379</v>
       </c>
@@ -4032,7 +4052,7 @@
       </c>
       <c r="E119" s="7"/>
     </row>
-    <row r="120" spans="1:5">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" s="9" t="s">
         <v>382</v>
       </c>
@@ -4047,7 +4067,7 @@
       </c>
       <c r="E120" s="7"/>
     </row>
-    <row r="121" spans="1:5">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="9" t="s">
         <v>385</v>
       </c>
@@ -4062,7 +4082,7 @@
       </c>
       <c r="E121" s="7"/>
     </row>
-    <row r="122" spans="1:5">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" s="7" t="s">
         <v>388</v>
       </c>
@@ -4077,7 +4097,7 @@
       </c>
       <c r="E122" s="7"/>
     </row>
-    <row r="123" spans="1:5">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" s="7" t="s">
         <v>391</v>
       </c>
@@ -4092,7 +4112,7 @@
       </c>
       <c r="E123" s="7"/>
     </row>
-    <row r="124" spans="1:5">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" s="7" t="s">
         <v>394</v>
       </c>
@@ -4107,7 +4127,7 @@
       </c>
       <c r="E124" s="7"/>
     </row>
-    <row r="125" spans="1:5">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" s="9" t="s">
         <v>397</v>
       </c>
@@ -4122,7 +4142,7 @@
       </c>
       <c r="E125" s="7"/>
     </row>
-    <row r="126" spans="1:5">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" s="7" t="s">
         <v>400</v>
       </c>
@@ -4137,7 +4157,7 @@
       </c>
       <c r="E126" s="7"/>
     </row>
-    <row r="127" spans="1:5">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" s="7" t="s">
         <v>403</v>
       </c>
@@ -4152,7 +4172,7 @@
       </c>
       <c r="E127" s="7"/>
     </row>
-    <row r="128" spans="1:5">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" s="7" t="s">
         <v>406</v>
       </c>
@@ -4167,7 +4187,7 @@
       </c>
       <c r="E128" s="7"/>
     </row>
-    <row r="129" spans="1:5">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" s="9" t="s">
         <v>409</v>
       </c>
@@ -4182,7 +4202,7 @@
       </c>
       <c r="E129" s="7"/>
     </row>
-    <row r="130" spans="1:5">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" s="9" t="s">
         <v>412</v>
       </c>
@@ -4197,7 +4217,7 @@
       </c>
       <c r="E130" s="7"/>
     </row>
-    <row r="131" spans="1:5">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" s="9" t="s">
         <v>414</v>
       </c>
@@ -4212,7 +4232,7 @@
       </c>
       <c r="E131" s="7"/>
     </row>
-    <row r="132" spans="1:5">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" s="7" t="s">
         <v>417</v>
       </c>
@@ -4227,7 +4247,7 @@
       </c>
       <c r="E132" s="7"/>
     </row>
-    <row r="133" spans="1:5">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" s="9" t="s">
         <v>420</v>
       </c>
@@ -4242,7 +4262,7 @@
       </c>
       <c r="E133" s="7"/>
     </row>
-    <row r="134" spans="1:5" ht="30">
+    <row r="134" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A134" s="7" t="s">
         <v>423</v>
       </c>
@@ -4257,7 +4277,7 @@
       </c>
       <c r="E134" s="7"/>
     </row>
-    <row r="135" spans="1:5" ht="30">
+    <row r="135" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A135" s="7" t="s">
         <v>424</v>
       </c>
@@ -4272,7 +4292,7 @@
       </c>
       <c r="E135" s="7"/>
     </row>
-    <row r="136" spans="1:5">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" s="9" t="s">
         <v>429</v>
       </c>
@@ -4287,7 +4307,7 @@
       </c>
       <c r="E136" s="7"/>
     </row>
-    <row r="137" spans="1:5">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" s="7" t="s">
         <v>432</v>
       </c>
@@ -4302,7 +4322,7 @@
       </c>
       <c r="E137" s="7"/>
     </row>
-    <row r="138" spans="1:5" ht="45">
+    <row r="138" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A138" s="7" t="s">
         <v>433</v>
       </c>
@@ -4317,7 +4337,7 @@
       </c>
       <c r="E138" s="7"/>
     </row>
-    <row r="139" spans="1:5" ht="30">
+    <row r="139" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A139" s="7" t="s">
         <v>434</v>
       </c>
@@ -4332,7 +4352,7 @@
       </c>
       <c r="E139" s="7"/>
     </row>
-    <row r="140" spans="1:5">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" s="17" t="s">
         <v>441</v>
       </c>
@@ -4347,7 +4367,7 @@
       </c>
       <c r="E140" s="7"/>
     </row>
-    <row r="141" spans="1:5">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" s="17" t="s">
         <v>444</v>
       </c>
@@ -4362,7 +4382,7 @@
       </c>
       <c r="E141" s="7"/>
     </row>
-    <row r="142" spans="1:5">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" s="17" t="s">
         <v>447</v>
       </c>
@@ -4377,7 +4397,7 @@
       </c>
       <c r="E142" s="7"/>
     </row>
-    <row r="143" spans="1:5">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" s="17" t="s">
         <v>450</v>
       </c>
@@ -4392,7 +4412,7 @@
       </c>
       <c r="E143" s="7"/>
     </row>
-    <row r="144" spans="1:5" ht="30">
+    <row r="144" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A144" s="17" t="s">
         <v>451</v>
       </c>
@@ -4407,7 +4427,7 @@
       </c>
       <c r="E144" s="7"/>
     </row>
-    <row r="145" spans="1:5">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" s="17" t="s">
         <v>454</v>
       </c>
@@ -4422,7 +4442,7 @@
       </c>
       <c r="E145" s="7"/>
     </row>
-    <row r="146" spans="1:5">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" s="17" t="s">
         <v>457</v>
       </c>
@@ -4437,7 +4457,7 @@
       </c>
       <c r="E146" s="7"/>
     </row>
-    <row r="147" spans="1:5">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" s="17" t="s">
         <v>460</v>
       </c>
@@ -4452,7 +4472,7 @@
       </c>
       <c r="E147" s="7"/>
     </row>
-    <row r="148" spans="1:5">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" s="17" t="s">
         <v>463</v>
       </c>
@@ -4467,7 +4487,7 @@
       </c>
       <c r="E148" s="7"/>
     </row>
-    <row r="149" spans="1:5">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" s="7" t="s">
         <v>466</v>
       </c>
@@ -4482,7 +4502,7 @@
       </c>
       <c r="E149" s="7"/>
     </row>
-    <row r="150" spans="1:5">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" s="7" t="s">
         <v>467</v>
       </c>
@@ -4497,7 +4517,7 @@
       </c>
       <c r="E150" s="7"/>
     </row>
-    <row r="151" spans="1:5">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" s="7" t="s">
         <v>468</v>
       </c>
@@ -4512,7 +4532,7 @@
       </c>
       <c r="E151" s="7"/>
     </row>
-    <row r="152" spans="1:5" ht="30">
+    <row r="152" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A152" s="7" t="s">
         <v>475</v>
       </c>
@@ -4527,7 +4547,7 @@
       </c>
       <c r="E152" s="7"/>
     </row>
-    <row r="153" spans="1:5" ht="45">
+    <row r="153" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A153" s="17" t="s">
         <v>478</v>
       </c>
@@ -4542,7 +4562,7 @@
       </c>
       <c r="E153" s="7"/>
     </row>
-    <row r="154" spans="1:5">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" s="17" t="s">
         <v>480</v>
       </c>
@@ -4557,7 +4577,7 @@
       </c>
       <c r="E154" s="7"/>
     </row>
-    <row r="155" spans="1:5">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" s="7" t="s">
         <v>482</v>
       </c>
@@ -4572,7 +4592,7 @@
       </c>
       <c r="E155" s="7"/>
     </row>
-    <row r="156" spans="1:5">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" s="7" t="s">
         <v>485</v>
       </c>
@@ -4587,7 +4607,7 @@
       </c>
       <c r="E156" s="7"/>
     </row>
-    <row r="157" spans="1:5">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" s="7" t="s">
         <v>488</v>
       </c>
@@ -4602,7 +4622,7 @@
       </c>
       <c r="E157" s="7"/>
     </row>
-    <row r="158" spans="1:5" ht="30">
+    <row r="158" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A158" s="7" t="s">
         <v>491</v>
       </c>
@@ -4617,7 +4637,7 @@
       </c>
       <c r="E158" s="7"/>
     </row>
-    <row r="159" spans="1:5" ht="30">
+    <row r="159" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A159" s="7" t="s">
         <v>492</v>
       </c>
@@ -4632,7 +4652,7 @@
       </c>
       <c r="E159" s="7"/>
     </row>
-    <row r="160" spans="1:5">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" s="7" t="s">
         <v>499</v>
       </c>
@@ -4647,7 +4667,7 @@
       </c>
       <c r="E160" s="7"/>
     </row>
-    <row r="161" spans="1:5">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161" s="7" t="s">
         <v>500</v>
       </c>
@@ -4662,7 +4682,7 @@
       </c>
       <c r="E161" s="7"/>
     </row>
-    <row r="162" spans="1:5">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162" s="7" t="s">
         <v>503</v>
       </c>
@@ -4677,7 +4697,7 @@
       </c>
       <c r="E162" s="7"/>
     </row>
-    <row r="163" spans="1:5">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" s="7" t="s">
         <v>508</v>
       </c>
@@ -4692,7 +4712,7 @@
       </c>
       <c r="E163" s="7"/>
     </row>
-    <row r="164" spans="1:5" ht="30">
+    <row r="164" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A164" s="7" t="s">
         <v>511</v>
       </c>
@@ -4707,7 +4727,7 @@
       </c>
       <c r="E164" s="7"/>
     </row>
-    <row r="165" spans="1:5">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165" s="7" t="s">
         <v>514</v>
       </c>
@@ -4722,7 +4742,7 @@
       </c>
       <c r="E165" s="7"/>
     </row>
-    <row r="166" spans="1:5" ht="30">
+    <row r="166" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A166" s="7" t="s">
         <v>517</v>
       </c>
@@ -4737,7 +4757,7 @@
       </c>
       <c r="E166" s="7"/>
     </row>
-    <row r="167" spans="1:5">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167" s="7" t="s">
         <v>521</v>
       </c>
@@ -4752,7 +4772,7 @@
       </c>
       <c r="E167" s="7"/>
     </row>
-    <row r="168" spans="1:5">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" s="7" t="s">
         <v>523</v>
       </c>
@@ -4767,7 +4787,7 @@
       </c>
       <c r="E168" s="7"/>
     </row>
-    <row r="169" spans="1:5">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" s="7" t="s">
         <v>526</v>
       </c>
@@ -4782,7 +4802,7 @@
       </c>
       <c r="E169" s="7"/>
     </row>
-    <row r="170" spans="1:5">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170" s="7" t="s">
         <v>527</v>
       </c>
@@ -4797,7 +4817,7 @@
       </c>
       <c r="E170" s="7"/>
     </row>
-    <row r="171" spans="1:5">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171" s="7" t="s">
         <v>528</v>
       </c>
@@ -4812,7 +4832,7 @@
       </c>
       <c r="E171" s="7"/>
     </row>
-    <row r="172" spans="1:5" ht="30">
+    <row r="172" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A172" s="7" t="s">
         <v>535</v>
       </c>
@@ -4827,7 +4847,7 @@
       </c>
       <c r="E172" s="7"/>
     </row>
-    <row r="173" spans="1:5">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173" s="9" t="s">
         <v>537</v>
       </c>
@@ -4842,7 +4862,7 @@
       </c>
       <c r="E173" s="7"/>
     </row>
-    <row r="174" spans="1:5">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A174" s="9" t="s">
         <v>538</v>
       </c>
@@ -4857,7 +4877,7 @@
       </c>
       <c r="E174" s="7"/>
     </row>
-    <row r="175" spans="1:5">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A175" s="9" t="s">
         <v>539</v>
       </c>
@@ -4872,7 +4892,7 @@
       </c>
       <c r="E175" s="7"/>
     </row>
-    <row r="176" spans="1:5">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A176" s="9" t="s">
         <v>540</v>
       </c>
@@ -4887,7 +4907,7 @@
       </c>
       <c r="E176" s="7"/>
     </row>
-    <row r="177" spans="1:5" ht="30">
+    <row r="177" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A177" s="7" t="s">
         <v>548</v>
       </c>
@@ -4902,7 +4922,7 @@
       </c>
       <c r="E177" s="7"/>
     </row>
-    <row r="178" spans="1:5">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A178" s="7" t="s">
         <v>551</v>
       </c>
@@ -4917,7 +4937,7 @@
       </c>
       <c r="E178" s="7"/>
     </row>
-    <row r="179" spans="1:5" ht="30">
+    <row r="179" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A179" s="7" t="s">
         <v>555</v>
       </c>
@@ -4932,7 +4952,7 @@
       </c>
       <c r="E179" s="7"/>
     </row>
-    <row r="180" spans="1:5">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A180" s="7" t="s">
         <v>557</v>
       </c>
@@ -4947,7 +4967,7 @@
       </c>
       <c r="E180" s="7"/>
     </row>
-    <row r="181" spans="1:5" ht="30">
+    <row r="181" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A181" s="7" t="s">
         <v>560</v>
       </c>
@@ -4962,7 +4982,7 @@
       </c>
       <c r="E181" s="7"/>
     </row>
-    <row r="182" spans="1:5">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A182" s="7" t="s">
         <v>563</v>
       </c>
@@ -4977,7 +4997,7 @@
       </c>
       <c r="E182" s="7"/>
     </row>
-    <row r="183" spans="1:5">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A183" s="7" t="s">
         <v>566</v>
       </c>
@@ -4992,7 +5012,7 @@
       </c>
       <c r="E183" s="7"/>
     </row>
-    <row r="184" spans="1:5">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A184" s="9" t="s">
         <v>569</v>
       </c>
@@ -5007,7 +5027,7 @@
       </c>
       <c r="E184" s="7"/>
     </row>
-    <row r="185" spans="1:5">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A185" s="9" t="s">
         <v>570</v>
       </c>
@@ -5022,7 +5042,7 @@
       </c>
       <c r="E185" s="7"/>
     </row>
-    <row r="186" spans="1:5">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A186" s="9" t="s">
         <v>579</v>
       </c>
@@ -5037,7 +5057,7 @@
       </c>
       <c r="E186" s="7"/>
     </row>
-    <row r="187" spans="1:5">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A187" s="9" t="s">
         <v>582</v>
       </c>
@@ -5051,6 +5071,36 @@
         <v>5</v>
       </c>
       <c r="E187" s="7"/>
+    </row>
+    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A188" s="9" t="s">
+        <v>585</v>
+      </c>
+      <c r="B188" s="7" t="s">
+        <v>587</v>
+      </c>
+      <c r="C188" s="8" t="s">
+        <v>589</v>
+      </c>
+      <c r="D188" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E188" s="7"/>
+    </row>
+    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A189" s="9" t="s">
+        <v>586</v>
+      </c>
+      <c r="B189" s="7" t="s">
+        <v>588</v>
+      </c>
+      <c r="C189" s="8" t="s">
+        <v>590</v>
+      </c>
+      <c r="D189" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E189" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -5063,14 +5113,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView topLeftCell="A10" zoomScale="80" workbookViewId="0">
       <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
@@ -5078,7 +5128,7 @@
     <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>35</v>
       </c>
@@ -5092,7 +5142,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>37</v>
       </c>
@@ -5104,7 +5154,7 @@
       </c>
       <c r="D2" s="7"/>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>38</v>
       </c>
@@ -5116,7 +5166,7 @@
       </c>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>39</v>
       </c>
@@ -5128,7 +5178,7 @@
       </c>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>40</v>
       </c>
@@ -5140,7 +5190,7 @@
       </c>
       <c r="D5" s="7"/>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>41</v>
       </c>
@@ -5152,7 +5202,7 @@
       </c>
       <c r="D6" s="7"/>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>42</v>
       </c>
@@ -5164,7 +5214,7 @@
       </c>
       <c r="D7" s="7"/>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>43</v>
       </c>
@@ -5176,7 +5226,7 @@
       </c>
       <c r="D8" s="7"/>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>44</v>
       </c>
@@ -5188,7 +5238,7 @@
       </c>
       <c r="D9" s="7"/>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>45</v>
       </c>
@@ -5200,7 +5250,7 @@
       </c>
       <c r="D10" s="7"/>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>46</v>
       </c>
@@ -5212,7 +5262,7 @@
       </c>
       <c r="D11" s="7"/>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>48</v>
       </c>
@@ -5224,7 +5274,7 @@
       </c>
       <c r="D12" s="7"/>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>49</v>
       </c>
@@ -5236,7 +5286,7 @@
       </c>
       <c r="D13" s="7"/>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>50</v>
       </c>
@@ -5248,7 +5298,7 @@
       </c>
       <c r="D14" s="7"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>51</v>
       </c>
@@ -5260,7 +5310,7 @@
       </c>
       <c r="D15" s="7"/>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>52</v>
       </c>
@@ -5272,7 +5322,7 @@
       </c>
       <c r="D16" s="7"/>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>53</v>
       </c>
@@ -5284,7 +5334,7 @@
       </c>
       <c r="D17" s="7"/>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>54</v>
       </c>
@@ -5296,7 +5346,7 @@
       </c>
       <c r="D18" s="7"/>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>55</v>
       </c>
@@ -5308,7 +5358,7 @@
       </c>
       <c r="D19" s="7"/>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>56</v>
       </c>
@@ -5320,7 +5370,7 @@
       </c>
       <c r="D20" s="7"/>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>57</v>
       </c>
@@ -5332,7 +5382,7 @@
       </c>
       <c r="D21" s="7"/>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>58</v>
       </c>
@@ -5344,7 +5394,7 @@
       </c>
       <c r="D22" s="7"/>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>59</v>
       </c>
@@ -5356,7 +5406,7 @@
       </c>
       <c r="D23" s="7"/>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>60</v>
       </c>
@@ -5368,7 +5418,7 @@
       </c>
       <c r="D24" s="7"/>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>61</v>
       </c>
@@ -5380,7 +5430,7 @@
       </c>
       <c r="D25" s="7"/>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>47</v>
       </c>
@@ -5399,14 +5449,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A19" sqref="A19:XFD19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
@@ -5414,7 +5464,7 @@
     <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>35</v>
       </c>
@@ -5428,7 +5478,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>37</v>
       </c>
@@ -5440,7 +5490,7 @@
       </c>
       <c r="D2" s="7"/>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>38</v>
       </c>
@@ -5452,7 +5502,7 @@
       </c>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>39</v>
       </c>
@@ -5464,7 +5514,7 @@
       </c>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>40</v>
       </c>
@@ -5476,7 +5526,7 @@
       </c>
       <c r="D5" s="7"/>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>41</v>
       </c>
@@ -5488,7 +5538,7 @@
       </c>
       <c r="D6" s="7"/>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>42</v>
       </c>
@@ -5500,7 +5550,7 @@
       </c>
       <c r="D7" s="7"/>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>43</v>
       </c>
@@ -5512,7 +5562,7 @@
       </c>
       <c r="D8" s="7"/>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>44</v>
       </c>
@@ -5524,7 +5574,7 @@
       </c>
       <c r="D9" s="7"/>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>45</v>
       </c>
@@ -5536,7 +5586,7 @@
       </c>
       <c r="D10" s="7"/>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>46</v>
       </c>
@@ -5548,7 +5598,7 @@
       </c>
       <c r="D11" s="7"/>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>47</v>
       </c>
@@ -5560,7 +5610,7 @@
       </c>
       <c r="D12" s="7"/>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>48</v>
       </c>
@@ -5572,7 +5622,7 @@
       </c>
       <c r="D13" s="7"/>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>49</v>
       </c>
@@ -5584,7 +5634,7 @@
       </c>
       <c r="D14" s="7"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>50</v>
       </c>
@@ -5596,7 +5646,7 @@
       </c>
       <c r="D15" s="7"/>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>51</v>
       </c>
@@ -5608,7 +5658,7 @@
       </c>
       <c r="D16" s="7"/>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>52</v>
       </c>
@@ -5620,7 +5670,7 @@
       </c>
       <c r="D17" s="7"/>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>53</v>
       </c>
@@ -5632,7 +5682,7 @@
       </c>
       <c r="D18" s="7"/>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>54</v>
       </c>
@@ -5644,7 +5694,7 @@
       </c>
       <c r="D19" s="7"/>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>55</v>
       </c>
@@ -5656,7 +5706,7 @@
       </c>
       <c r="D20" s="7"/>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>56</v>
       </c>
@@ -5668,7 +5718,7 @@
       </c>
       <c r="D21" s="7"/>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>57</v>
       </c>
@@ -5680,7 +5730,7 @@
       </c>
       <c r="D22" s="7"/>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>58</v>
       </c>
@@ -5692,7 +5742,7 @@
       </c>
       <c r="D23" s="7"/>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>59</v>
       </c>
@@ -5704,7 +5754,7 @@
       </c>
       <c r="D24" s="7"/>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>60</v>
       </c>
@@ -5716,7 +5766,7 @@
       </c>
       <c r="D25" s="7"/>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>61</v>
       </c>

</xml_diff>

<commit_message>
Adds WAT-192 test script and related changes
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/WAT.xlsx
+++ b/src/test/resources/xls/WAT.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="915" uniqueCount="591">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="919" uniqueCount="594">
   <si>
     <t>TCID</t>
   </si>
@@ -1791,6 +1791,15 @@
   </si>
   <si>
     <t>Verify that System must display a maximum of 3 recommendations on the author record at a time(For Cmbined Author)</t>
+  </si>
+  <si>
+    <t>WAT192</t>
+  </si>
+  <si>
+    <t>WAT-634</t>
+  </si>
+  <si>
+    <t>Verify that If the user enters a name, then toggles to ORCiD search tab, then toggles back to name search tab, the name entered should still be visible. Same for the ORCiD.</t>
   </si>
 </sst>
 </file>
@@ -2250,10 +2259,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E189"/>
+  <dimension ref="A1:E190"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A164" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C189" sqref="C189"/>
+    <sheetView tabSelected="1" topLeftCell="A173" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C190" sqref="C190"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5101,6 +5110,21 @@
         <v>5</v>
       </c>
       <c r="E189" s="7"/>
+    </row>
+    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A190" s="9" t="s">
+        <v>591</v>
+      </c>
+      <c r="B190" s="7" t="s">
+        <v>592</v>
+      </c>
+      <c r="C190" s="8" t="s">
+        <v>593</v>
+      </c>
+      <c r="D190" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E190" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Adds WAT-193 testscript and related changes
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/WAT.xlsx
+++ b/src/test/resources/xls/WAT.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13305" windowHeight="2415"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="923" uniqueCount="597">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="927" uniqueCount="600">
   <si>
     <t>TCID</t>
   </si>
@@ -1809,13 +1809,22 @@
   </si>
   <si>
     <t>Verify that System must display a 'Submit updates' button on the combined author record page.</t>
+  </si>
+  <si>
+    <t>WAT193</t>
+  </si>
+  <si>
+    <t>WAT-1261</t>
+  </si>
+  <si>
+    <t>Verify that user should not be able to submit feedback without entering curation mode</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2024,7 +2033,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2056,9 +2065,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2090,6 +2100,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2265,14 +2276,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E191"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E192"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A173" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C196" sqref="C196"/>
+      <selection activeCell="C192" sqref="C192"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="30.5703125" customWidth="1" collapsed="1"/>
@@ -2281,7 +2292,7 @@
     <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2298,7 +2309,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -2313,7 +2324,7 @@
       </c>
       <c r="E2" s="4"/>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -2328,7 +2339,7 @@
       </c>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>11</v>
       </c>
@@ -2343,7 +2354,7 @@
       </c>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>12</v>
       </c>
@@ -2358,7 +2369,7 @@
       </c>
       <c r="E5" s="7"/>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>14</v>
       </c>
@@ -2373,7 +2384,7 @@
       </c>
       <c r="E6" s="7"/>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>17</v>
       </c>
@@ -2388,7 +2399,7 @@
       </c>
       <c r="E7" s="7"/>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>20</v>
       </c>
@@ -2403,7 +2414,7 @@
       </c>
       <c r="E8" s="7"/>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>22</v>
       </c>
@@ -2418,7 +2429,7 @@
       </c>
       <c r="E9" s="7"/>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>23</v>
       </c>
@@ -2433,7 +2444,7 @@
       </c>
       <c r="E10" s="7"/>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>24</v>
       </c>
@@ -2448,7 +2459,7 @@
       </c>
       <c r="E11" s="7"/>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>25</v>
       </c>
@@ -2463,7 +2474,7 @@
       </c>
       <c r="E12" s="7"/>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>62</v>
       </c>
@@ -2478,7 +2489,7 @@
       </c>
       <c r="E13" s="7"/>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>63</v>
       </c>
@@ -2493,7 +2504,7 @@
       </c>
       <c r="E14" s="7"/>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>64</v>
       </c>
@@ -2508,7 +2519,7 @@
       </c>
       <c r="E15" s="7"/>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>65</v>
       </c>
@@ -2523,7 +2534,7 @@
       </c>
       <c r="E16" s="7"/>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>74</v>
       </c>
@@ -2538,7 +2549,7 @@
       </c>
       <c r="E17" s="7"/>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>75</v>
       </c>
@@ -2553,7 +2564,7 @@
       </c>
       <c r="E18" s="7"/>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>79</v>
       </c>
@@ -2568,7 +2579,7 @@
       </c>
       <c r="E19" s="7"/>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>81</v>
       </c>
@@ -2583,7 +2594,7 @@
       </c>
       <c r="E20" s="7"/>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>82</v>
       </c>
@@ -2598,7 +2609,7 @@
       </c>
       <c r="E21" s="7"/>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>88</v>
       </c>
@@ -2613,7 +2624,7 @@
       </c>
       <c r="E22" s="7"/>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>90</v>
       </c>
@@ -2628,7 +2639,7 @@
       </c>
       <c r="E23" s="7"/>
     </row>
-    <row r="24" spans="1:5" ht="30">
+    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>94</v>
       </c>
@@ -2643,7 +2654,7 @@
       </c>
       <c r="E24" s="7"/>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>96</v>
       </c>
@@ -2658,7 +2669,7 @@
       </c>
       <c r="E25" s="7"/>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
         <v>98</v>
       </c>
@@ -2673,7 +2684,7 @@
       </c>
       <c r="E26" s="7"/>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
         <v>102</v>
       </c>
@@ -2688,7 +2699,7 @@
       </c>
       <c r="E27" s="7"/>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
         <v>105</v>
       </c>
@@ -2703,7 +2714,7 @@
       </c>
       <c r="E28" s="7"/>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
         <v>108</v>
       </c>
@@ -2718,7 +2729,7 @@
       </c>
       <c r="E29" s="7"/>
     </row>
-    <row r="30" spans="1:5" ht="30">
+    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
         <v>110</v>
       </c>
@@ -2733,7 +2744,7 @@
       </c>
       <c r="E30" s="7"/>
     </row>
-    <row r="31" spans="1:5" ht="30">
+    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
         <v>114</v>
       </c>
@@ -2748,7 +2759,7 @@
       </c>
       <c r="E31" s="7"/>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
         <v>119</v>
       </c>
@@ -2763,7 +2774,7 @@
       </c>
       <c r="E32" s="7"/>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
         <v>120</v>
       </c>
@@ -2778,7 +2789,7 @@
       </c>
       <c r="E33" s="7"/>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
         <v>125</v>
       </c>
@@ -2793,7 +2804,7 @@
       </c>
       <c r="E34" s="7"/>
     </row>
-    <row r="35" spans="1:5" ht="30">
+    <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
         <v>128</v>
       </c>
@@ -2808,7 +2819,7 @@
       </c>
       <c r="E35" s="7"/>
     </row>
-    <row r="36" spans="1:5" ht="30">
+    <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
         <v>131</v>
       </c>
@@ -2823,7 +2834,7 @@
       </c>
       <c r="E36" s="7"/>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
         <v>134</v>
       </c>
@@ -2838,7 +2849,7 @@
       </c>
       <c r="E37" s="7"/>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="9" t="s">
         <v>137</v>
       </c>
@@ -2853,7 +2864,7 @@
       </c>
       <c r="E38" s="7"/>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="s">
         <v>140</v>
       </c>
@@ -2868,7 +2879,7 @@
       </c>
       <c r="E39" s="7"/>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="9" t="s">
         <v>143</v>
       </c>
@@ -2883,7 +2894,7 @@
       </c>
       <c r="E40" s="7"/>
     </row>
-    <row r="41" spans="1:5" ht="30">
+    <row r="41" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
         <v>145</v>
       </c>
@@ -2898,7 +2909,7 @@
       </c>
       <c r="E41" s="7"/>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="9" t="s">
         <v>147</v>
       </c>
@@ -2913,7 +2924,7 @@
       </c>
       <c r="E42" s="7"/>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="9" t="s">
         <v>150</v>
       </c>
@@ -2928,7 +2939,7 @@
       </c>
       <c r="E43" s="7"/>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="9" t="s">
         <v>153</v>
       </c>
@@ -2943,7 +2954,7 @@
       </c>
       <c r="E44" s="7"/>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="9" t="s">
         <v>155</v>
       </c>
@@ -2958,7 +2969,7 @@
       </c>
       <c r="E45" s="7"/>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="12" t="s">
         <v>158</v>
       </c>
@@ -2973,7 +2984,7 @@
       </c>
       <c r="E46" s="7"/>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="12" t="s">
         <v>159</v>
       </c>
@@ -2988,7 +2999,7 @@
       </c>
       <c r="E47" s="7"/>
     </row>
-    <row r="48" spans="1:5" ht="30">
+    <row r="48" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="12" t="s">
         <v>160</v>
       </c>
@@ -3003,7 +3014,7 @@
       </c>
       <c r="E48" s="7"/>
     </row>
-    <row r="49" spans="1:5" ht="30">
+    <row r="49" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="12" t="s">
         <v>161</v>
       </c>
@@ -3018,7 +3029,7 @@
       </c>
       <c r="E49" s="7"/>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="12" t="s">
         <v>164</v>
       </c>
@@ -3033,7 +3044,7 @@
       </c>
       <c r="E50" s="7"/>
     </row>
-    <row r="51" spans="1:5" ht="30">
+    <row r="51" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="9" t="s">
         <v>173</v>
       </c>
@@ -3048,7 +3059,7 @@
       </c>
       <c r="E51" s="7"/>
     </row>
-    <row r="52" spans="1:5">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="9" t="s">
         <v>174</v>
       </c>
@@ -3063,7 +3074,7 @@
       </c>
       <c r="E52" s="7"/>
     </row>
-    <row r="53" spans="1:5">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="9" t="s">
         <v>179</v>
       </c>
@@ -3078,7 +3089,7 @@
       </c>
       <c r="E53" s="7"/>
     </row>
-    <row r="54" spans="1:5">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="9" t="s">
         <v>180</v>
       </c>
@@ -3093,7 +3104,7 @@
       </c>
       <c r="E54" s="7"/>
     </row>
-    <row r="55" spans="1:5">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="9" t="s">
         <v>185</v>
       </c>
@@ -3108,7 +3119,7 @@
       </c>
       <c r="E55" s="7"/>
     </row>
-    <row r="56" spans="1:5">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="s">
         <v>188</v>
       </c>
@@ -3123,7 +3134,7 @@
       </c>
       <c r="E56" s="7"/>
     </row>
-    <row r="57" spans="1:5" ht="30">
+    <row r="57" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="9" t="s">
         <v>191</v>
       </c>
@@ -3138,7 +3149,7 @@
       </c>
       <c r="E57" s="7"/>
     </row>
-    <row r="58" spans="1:5">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="9" t="s">
         <v>194</v>
       </c>
@@ -3153,7 +3164,7 @@
       </c>
       <c r="E58" s="7"/>
     </row>
-    <row r="59" spans="1:5">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
         <v>196</v>
       </c>
@@ -3168,7 +3179,7 @@
       </c>
       <c r="E59" s="7"/>
     </row>
-    <row r="60" spans="1:5" ht="45">
+    <row r="60" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
         <v>199</v>
       </c>
@@ -3183,7 +3194,7 @@
       </c>
       <c r="E60" s="7"/>
     </row>
-    <row r="61" spans="1:5">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="9" t="s">
         <v>202</v>
       </c>
@@ -3198,7 +3209,7 @@
       </c>
       <c r="E61" s="7"/>
     </row>
-    <row r="62" spans="1:5">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="9" t="s">
         <v>204</v>
       </c>
@@ -3213,7 +3224,7 @@
       </c>
       <c r="E62" s="7"/>
     </row>
-    <row r="63" spans="1:5">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="9" t="s">
         <v>206</v>
       </c>
@@ -3228,7 +3239,7 @@
       </c>
       <c r="E63" s="7"/>
     </row>
-    <row r="64" spans="1:5">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="9" t="s">
         <v>208</v>
       </c>
@@ -3243,7 +3254,7 @@
       </c>
       <c r="E64" s="7"/>
     </row>
-    <row r="65" spans="1:5">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="9" t="s">
         <v>217</v>
       </c>
@@ -3258,7 +3269,7 @@
       </c>
       <c r="E65" s="7"/>
     </row>
-    <row r="66" spans="1:5">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="9" t="s">
         <v>218</v>
       </c>
@@ -3273,7 +3284,7 @@
       </c>
       <c r="E66" s="7"/>
     </row>
-    <row r="67" spans="1:5">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="9" t="s">
         <v>223</v>
       </c>
@@ -3288,7 +3299,7 @@
       </c>
       <c r="E67" s="7"/>
     </row>
-    <row r="68" spans="1:5">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="9" t="s">
         <v>224</v>
       </c>
@@ -3303,7 +3314,7 @@
       </c>
       <c r="E68" s="7"/>
     </row>
-    <row r="69" spans="1:5">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="9" t="s">
         <v>225</v>
       </c>
@@ -3318,7 +3329,7 @@
       </c>
       <c r="E69" s="7"/>
     </row>
-    <row r="70" spans="1:5">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="9" t="s">
         <v>226</v>
       </c>
@@ -3333,7 +3344,7 @@
       </c>
       <c r="E70" s="7"/>
     </row>
-    <row r="71" spans="1:5">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="9" t="s">
         <v>233</v>
       </c>
@@ -3348,7 +3359,7 @@
       </c>
       <c r="E71" s="7"/>
     </row>
-    <row r="72" spans="1:5">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="9" t="s">
         <v>237</v>
       </c>
@@ -3363,7 +3374,7 @@
       </c>
       <c r="E72" s="7"/>
     </row>
-    <row r="73" spans="1:5">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="9" t="s">
         <v>239</v>
       </c>
@@ -3378,7 +3389,7 @@
       </c>
       <c r="E73" s="7"/>
     </row>
-    <row r="74" spans="1:5">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="9" t="s">
         <v>243</v>
       </c>
@@ -3393,7 +3404,7 @@
       </c>
       <c r="E74" s="7"/>
     </row>
-    <row r="75" spans="1:5" ht="30">
+    <row r="75" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" s="9" t="s">
         <v>245</v>
       </c>
@@ -3408,7 +3419,7 @@
       </c>
       <c r="E75" s="7"/>
     </row>
-    <row r="76" spans="1:5">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="9" t="s">
         <v>248</v>
       </c>
@@ -3423,7 +3434,7 @@
       </c>
       <c r="E76" s="7"/>
     </row>
-    <row r="77" spans="1:5">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="9" t="s">
         <v>256</v>
       </c>
@@ -3438,7 +3449,7 @@
       </c>
       <c r="E77" s="7"/>
     </row>
-    <row r="78" spans="1:5">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="9" t="s">
         <v>257</v>
       </c>
@@ -3453,7 +3464,7 @@
       </c>
       <c r="E78" s="7"/>
     </row>
-    <row r="79" spans="1:5">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="9" t="s">
         <v>261</v>
       </c>
@@ -3468,7 +3479,7 @@
       </c>
       <c r="E79" s="7"/>
     </row>
-    <row r="80" spans="1:5">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="9" t="s">
         <v>264</v>
       </c>
@@ -3483,7 +3494,7 @@
       </c>
       <c r="E80" s="7"/>
     </row>
-    <row r="81" spans="1:5">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="9" t="s">
         <v>267</v>
       </c>
@@ -3498,7 +3509,7 @@
       </c>
       <c r="E81" s="7"/>
     </row>
-    <row r="82" spans="1:5" ht="30">
+    <row r="82" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A82" s="9" t="s">
         <v>269</v>
       </c>
@@ -3513,7 +3524,7 @@
       </c>
       <c r="E82" s="7"/>
     </row>
-    <row r="83" spans="1:5">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="9" t="s">
         <v>274</v>
       </c>
@@ -3528,7 +3539,7 @@
       </c>
       <c r="E83" s="7"/>
     </row>
-    <row r="84" spans="1:5" ht="30">
+    <row r="84" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A84" s="9" t="s">
         <v>277</v>
       </c>
@@ -3543,7 +3554,7 @@
       </c>
       <c r="E84" s="7"/>
     </row>
-    <row r="85" spans="1:5">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="9" t="s">
         <v>279</v>
       </c>
@@ -3558,7 +3569,7 @@
       </c>
       <c r="E85" s="7"/>
     </row>
-    <row r="86" spans="1:5">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="9" t="s">
         <v>282</v>
       </c>
@@ -3573,7 +3584,7 @@
       </c>
       <c r="E86" s="7"/>
     </row>
-    <row r="87" spans="1:5">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="9" t="s">
         <v>285</v>
       </c>
@@ -3588,7 +3599,7 @@
       </c>
       <c r="E87" s="7"/>
     </row>
-    <row r="88" spans="1:5">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="9" t="s">
         <v>288</v>
       </c>
@@ -3603,7 +3614,7 @@
       </c>
       <c r="E88" s="7"/>
     </row>
-    <row r="89" spans="1:5">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="9" t="s">
         <v>291</v>
       </c>
@@ -3618,7 +3629,7 @@
       </c>
       <c r="E89" s="7"/>
     </row>
-    <row r="90" spans="1:5">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="9" t="s">
         <v>294</v>
       </c>
@@ -3633,7 +3644,7 @@
       </c>
       <c r="E90" s="7"/>
     </row>
-    <row r="91" spans="1:5">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="9" t="s">
         <v>297</v>
       </c>
@@ -3648,7 +3659,7 @@
       </c>
       <c r="E91" s="7"/>
     </row>
-    <row r="92" spans="1:5">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="9" t="s">
         <v>300</v>
       </c>
@@ -3663,7 +3674,7 @@
       </c>
       <c r="E92" s="7"/>
     </row>
-    <row r="93" spans="1:5">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="9" t="s">
         <v>303</v>
       </c>
@@ -3678,7 +3689,7 @@
       </c>
       <c r="E93" s="7"/>
     </row>
-    <row r="94" spans="1:5">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="9" t="s">
         <v>306</v>
       </c>
@@ -3693,7 +3704,7 @@
       </c>
       <c r="E94" s="7"/>
     </row>
-    <row r="95" spans="1:5">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="9" t="s">
         <v>309</v>
       </c>
@@ -3708,7 +3719,7 @@
       </c>
       <c r="E95" s="7"/>
     </row>
-    <row r="96" spans="1:5">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="9" t="s">
         <v>314</v>
       </c>
@@ -3723,7 +3734,7 @@
       </c>
       <c r="E96" s="7"/>
     </row>
-    <row r="97" spans="1:5">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="9" t="s">
         <v>315</v>
       </c>
@@ -3738,7 +3749,7 @@
       </c>
       <c r="E97" s="7"/>
     </row>
-    <row r="98" spans="1:5">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="9" t="s">
         <v>319</v>
       </c>
@@ -3753,7 +3764,7 @@
       </c>
       <c r="E98" s="7"/>
     </row>
-    <row r="99" spans="1:5">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="9" t="s">
         <v>321</v>
       </c>
@@ -3768,7 +3779,7 @@
       </c>
       <c r="E99" s="7"/>
     </row>
-    <row r="100" spans="1:5">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="9" t="s">
         <v>322</v>
       </c>
@@ -3783,7 +3794,7 @@
       </c>
       <c r="E100" s="7"/>
     </row>
-    <row r="101" spans="1:5" ht="30">
+    <row r="101" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A101" s="9" t="s">
         <v>323</v>
       </c>
@@ -3798,7 +3809,7 @@
       </c>
       <c r="E101" s="7"/>
     </row>
-    <row r="102" spans="1:5">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="9" t="s">
         <v>328</v>
       </c>
@@ -3813,7 +3824,7 @@
       </c>
       <c r="E102" s="7"/>
     </row>
-    <row r="103" spans="1:5">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="9" t="s">
         <v>333</v>
       </c>
@@ -3828,7 +3839,7 @@
       </c>
       <c r="E103" s="7"/>
     </row>
-    <row r="104" spans="1:5">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="9" t="s">
         <v>336</v>
       </c>
@@ -3843,7 +3854,7 @@
       </c>
       <c r="E104" s="7"/>
     </row>
-    <row r="105" spans="1:5">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="9" t="s">
         <v>337</v>
       </c>
@@ -3858,7 +3869,7 @@
       </c>
       <c r="E105" s="7"/>
     </row>
-    <row r="106" spans="1:5">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="9" t="s">
         <v>342</v>
       </c>
@@ -3873,7 +3884,7 @@
       </c>
       <c r="E106" s="7"/>
     </row>
-    <row r="107" spans="1:5">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="9" t="s">
         <v>345</v>
       </c>
@@ -3888,7 +3899,7 @@
       </c>
       <c r="E107" s="7"/>
     </row>
-    <row r="108" spans="1:5">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="9" t="s">
         <v>350</v>
       </c>
@@ -3903,7 +3914,7 @@
       </c>
       <c r="E108" s="7"/>
     </row>
-    <row r="109" spans="1:5" ht="30">
+    <row r="109" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A109" s="9" t="s">
         <v>351</v>
       </c>
@@ -3918,7 +3929,7 @@
       </c>
       <c r="E109" s="7"/>
     </row>
-    <row r="110" spans="1:5">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="9" t="s">
         <v>352</v>
       </c>
@@ -3933,7 +3944,7 @@
       </c>
       <c r="E110" s="7"/>
     </row>
-    <row r="111" spans="1:5">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="9" t="s">
         <v>355</v>
       </c>
@@ -3948,7 +3959,7 @@
       </c>
       <c r="E111" s="7"/>
     </row>
-    <row r="112" spans="1:5">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="9" t="s">
         <v>359</v>
       </c>
@@ -3963,7 +3974,7 @@
       </c>
       <c r="E112" s="7"/>
     </row>
-    <row r="113" spans="1:5">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="9" t="s">
         <v>361</v>
       </c>
@@ -3978,7 +3989,7 @@
       </c>
       <c r="E113" s="7"/>
     </row>
-    <row r="114" spans="1:5" ht="30">
+    <row r="114" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A114" s="9" t="s">
         <v>364</v>
       </c>
@@ -3993,7 +4004,7 @@
       </c>
       <c r="E114" s="7"/>
     </row>
-    <row r="115" spans="1:5">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="9" t="s">
         <v>367</v>
       </c>
@@ -4008,7 +4019,7 @@
       </c>
       <c r="E115" s="7"/>
     </row>
-    <row r="116" spans="1:5">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="9" t="s">
         <v>368</v>
       </c>
@@ -4023,7 +4034,7 @@
       </c>
       <c r="E116" s="7"/>
     </row>
-    <row r="117" spans="1:5">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" s="9" t="s">
         <v>369</v>
       </c>
@@ -4038,7 +4049,7 @@
       </c>
       <c r="E117" s="7"/>
     </row>
-    <row r="118" spans="1:5">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" s="9" t="s">
         <v>376</v>
       </c>
@@ -4053,7 +4064,7 @@
       </c>
       <c r="E118" s="7"/>
     </row>
-    <row r="119" spans="1:5">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" s="9" t="s">
         <v>379</v>
       </c>
@@ -4068,7 +4079,7 @@
       </c>
       <c r="E119" s="7"/>
     </row>
-    <row r="120" spans="1:5">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" s="9" t="s">
         <v>382</v>
       </c>
@@ -4083,7 +4094,7 @@
       </c>
       <c r="E120" s="7"/>
     </row>
-    <row r="121" spans="1:5">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="9" t="s">
         <v>385</v>
       </c>
@@ -4098,7 +4109,7 @@
       </c>
       <c r="E121" s="7"/>
     </row>
-    <row r="122" spans="1:5">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" s="7" t="s">
         <v>388</v>
       </c>
@@ -4113,7 +4124,7 @@
       </c>
       <c r="E122" s="7"/>
     </row>
-    <row r="123" spans="1:5">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" s="7" t="s">
         <v>391</v>
       </c>
@@ -4128,7 +4139,7 @@
       </c>
       <c r="E123" s="7"/>
     </row>
-    <row r="124" spans="1:5">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" s="7" t="s">
         <v>394</v>
       </c>
@@ -4143,7 +4154,7 @@
       </c>
       <c r="E124" s="7"/>
     </row>
-    <row r="125" spans="1:5">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" s="9" t="s">
         <v>397</v>
       </c>
@@ -4158,7 +4169,7 @@
       </c>
       <c r="E125" s="7"/>
     </row>
-    <row r="126" spans="1:5">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" s="7" t="s">
         <v>400</v>
       </c>
@@ -4173,7 +4184,7 @@
       </c>
       <c r="E126" s="7"/>
     </row>
-    <row r="127" spans="1:5">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" s="7" t="s">
         <v>403</v>
       </c>
@@ -4188,7 +4199,7 @@
       </c>
       <c r="E127" s="7"/>
     </row>
-    <row r="128" spans="1:5">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" s="7" t="s">
         <v>406</v>
       </c>
@@ -4203,7 +4214,7 @@
       </c>
       <c r="E128" s="7"/>
     </row>
-    <row r="129" spans="1:5">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" s="9" t="s">
         <v>409</v>
       </c>
@@ -4218,7 +4229,7 @@
       </c>
       <c r="E129" s="7"/>
     </row>
-    <row r="130" spans="1:5">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" s="9" t="s">
         <v>412</v>
       </c>
@@ -4233,7 +4244,7 @@
       </c>
       <c r="E130" s="7"/>
     </row>
-    <row r="131" spans="1:5">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" s="9" t="s">
         <v>414</v>
       </c>
@@ -4248,7 +4259,7 @@
       </c>
       <c r="E131" s="7"/>
     </row>
-    <row r="132" spans="1:5">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" s="7" t="s">
         <v>417</v>
       </c>
@@ -4263,7 +4274,7 @@
       </c>
       <c r="E132" s="7"/>
     </row>
-    <row r="133" spans="1:5">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" s="9" t="s">
         <v>420</v>
       </c>
@@ -4278,7 +4289,7 @@
       </c>
       <c r="E133" s="7"/>
     </row>
-    <row r="134" spans="1:5" ht="30">
+    <row r="134" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A134" s="7" t="s">
         <v>423</v>
       </c>
@@ -4293,7 +4304,7 @@
       </c>
       <c r="E134" s="7"/>
     </row>
-    <row r="135" spans="1:5" ht="30">
+    <row r="135" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A135" s="7" t="s">
         <v>424</v>
       </c>
@@ -4308,7 +4319,7 @@
       </c>
       <c r="E135" s="7"/>
     </row>
-    <row r="136" spans="1:5">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" s="9" t="s">
         <v>429</v>
       </c>
@@ -4323,7 +4334,7 @@
       </c>
       <c r="E136" s="7"/>
     </row>
-    <row r="137" spans="1:5">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" s="7" t="s">
         <v>432</v>
       </c>
@@ -4338,7 +4349,7 @@
       </c>
       <c r="E137" s="7"/>
     </row>
-    <row r="138" spans="1:5" ht="45">
+    <row r="138" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A138" s="7" t="s">
         <v>433</v>
       </c>
@@ -4353,7 +4364,7 @@
       </c>
       <c r="E138" s="7"/>
     </row>
-    <row r="139" spans="1:5" ht="30">
+    <row r="139" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A139" s="7" t="s">
         <v>434</v>
       </c>
@@ -4368,7 +4379,7 @@
       </c>
       <c r="E139" s="7"/>
     </row>
-    <row r="140" spans="1:5">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" s="17" t="s">
         <v>441</v>
       </c>
@@ -4383,7 +4394,7 @@
       </c>
       <c r="E140" s="7"/>
     </row>
-    <row r="141" spans="1:5">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" s="17" t="s">
         <v>444</v>
       </c>
@@ -4398,7 +4409,7 @@
       </c>
       <c r="E141" s="7"/>
     </row>
-    <row r="142" spans="1:5">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" s="17" t="s">
         <v>447</v>
       </c>
@@ -4413,7 +4424,7 @@
       </c>
       <c r="E142" s="7"/>
     </row>
-    <row r="143" spans="1:5">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" s="17" t="s">
         <v>450</v>
       </c>
@@ -4428,7 +4439,7 @@
       </c>
       <c r="E143" s="7"/>
     </row>
-    <row r="144" spans="1:5" ht="30">
+    <row r="144" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A144" s="17" t="s">
         <v>451</v>
       </c>
@@ -4443,7 +4454,7 @@
       </c>
       <c r="E144" s="7"/>
     </row>
-    <row r="145" spans="1:5">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" s="17" t="s">
         <v>454</v>
       </c>
@@ -4458,7 +4469,7 @@
       </c>
       <c r="E145" s="7"/>
     </row>
-    <row r="146" spans="1:5">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" s="17" t="s">
         <v>457</v>
       </c>
@@ -4473,7 +4484,7 @@
       </c>
       <c r="E146" s="7"/>
     </row>
-    <row r="147" spans="1:5">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" s="17" t="s">
         <v>460</v>
       </c>
@@ -4488,7 +4499,7 @@
       </c>
       <c r="E147" s="7"/>
     </row>
-    <row r="148" spans="1:5">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" s="17" t="s">
         <v>463</v>
       </c>
@@ -4503,7 +4514,7 @@
       </c>
       <c r="E148" s="7"/>
     </row>
-    <row r="149" spans="1:5">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" s="7" t="s">
         <v>466</v>
       </c>
@@ -4518,7 +4529,7 @@
       </c>
       <c r="E149" s="7"/>
     </row>
-    <row r="150" spans="1:5">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" s="7" t="s">
         <v>467</v>
       </c>
@@ -4533,7 +4544,7 @@
       </c>
       <c r="E150" s="7"/>
     </row>
-    <row r="151" spans="1:5">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" s="7" t="s">
         <v>468</v>
       </c>
@@ -4548,7 +4559,7 @@
       </c>
       <c r="E151" s="7"/>
     </row>
-    <row r="152" spans="1:5" ht="30">
+    <row r="152" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A152" s="7" t="s">
         <v>475</v>
       </c>
@@ -4563,7 +4574,7 @@
       </c>
       <c r="E152" s="7"/>
     </row>
-    <row r="153" spans="1:5" ht="45">
+    <row r="153" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A153" s="17" t="s">
         <v>478</v>
       </c>
@@ -4578,7 +4589,7 @@
       </c>
       <c r="E153" s="7"/>
     </row>
-    <row r="154" spans="1:5">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" s="17" t="s">
         <v>480</v>
       </c>
@@ -4593,7 +4604,7 @@
       </c>
       <c r="E154" s="7"/>
     </row>
-    <row r="155" spans="1:5">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" s="7" t="s">
         <v>482</v>
       </c>
@@ -4608,7 +4619,7 @@
       </c>
       <c r="E155" s="7"/>
     </row>
-    <row r="156" spans="1:5">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" s="7" t="s">
         <v>485</v>
       </c>
@@ -4623,7 +4634,7 @@
       </c>
       <c r="E156" s="7"/>
     </row>
-    <row r="157" spans="1:5">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" s="7" t="s">
         <v>488</v>
       </c>
@@ -4638,7 +4649,7 @@
       </c>
       <c r="E157" s="7"/>
     </row>
-    <row r="158" spans="1:5" ht="30">
+    <row r="158" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A158" s="7" t="s">
         <v>491</v>
       </c>
@@ -4653,7 +4664,7 @@
       </c>
       <c r="E158" s="7"/>
     </row>
-    <row r="159" spans="1:5" ht="30">
+    <row r="159" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A159" s="7" t="s">
         <v>492</v>
       </c>
@@ -4668,7 +4679,7 @@
       </c>
       <c r="E159" s="7"/>
     </row>
-    <row r="160" spans="1:5">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" s="7" t="s">
         <v>499</v>
       </c>
@@ -4683,7 +4694,7 @@
       </c>
       <c r="E160" s="7"/>
     </row>
-    <row r="161" spans="1:5">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161" s="7" t="s">
         <v>500</v>
       </c>
@@ -4698,7 +4709,7 @@
       </c>
       <c r="E161" s="7"/>
     </row>
-    <row r="162" spans="1:5">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162" s="7" t="s">
         <v>503</v>
       </c>
@@ -4713,7 +4724,7 @@
       </c>
       <c r="E162" s="7"/>
     </row>
-    <row r="163" spans="1:5">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" s="7" t="s">
         <v>508</v>
       </c>
@@ -4728,7 +4739,7 @@
       </c>
       <c r="E163" s="7"/>
     </row>
-    <row r="164" spans="1:5" ht="30">
+    <row r="164" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A164" s="7" t="s">
         <v>511</v>
       </c>
@@ -4743,7 +4754,7 @@
       </c>
       <c r="E164" s="7"/>
     </row>
-    <row r="165" spans="1:5">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165" s="7" t="s">
         <v>514</v>
       </c>
@@ -4758,7 +4769,7 @@
       </c>
       <c r="E165" s="7"/>
     </row>
-    <row r="166" spans="1:5" ht="30">
+    <row r="166" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A166" s="7" t="s">
         <v>517</v>
       </c>
@@ -4773,7 +4784,7 @@
       </c>
       <c r="E166" s="7"/>
     </row>
-    <row r="167" spans="1:5">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167" s="7" t="s">
         <v>521</v>
       </c>
@@ -4788,7 +4799,7 @@
       </c>
       <c r="E167" s="7"/>
     </row>
-    <row r="168" spans="1:5">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" s="7" t="s">
         <v>523</v>
       </c>
@@ -4803,7 +4814,7 @@
       </c>
       <c r="E168" s="7"/>
     </row>
-    <row r="169" spans="1:5">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" s="7" t="s">
         <v>526</v>
       </c>
@@ -4818,7 +4829,7 @@
       </c>
       <c r="E169" s="7"/>
     </row>
-    <row r="170" spans="1:5">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170" s="7" t="s">
         <v>527</v>
       </c>
@@ -4833,7 +4844,7 @@
       </c>
       <c r="E170" s="7"/>
     </row>
-    <row r="171" spans="1:5">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171" s="7" t="s">
         <v>528</v>
       </c>
@@ -4848,7 +4859,7 @@
       </c>
       <c r="E171" s="7"/>
     </row>
-    <row r="172" spans="1:5" ht="30">
+    <row r="172" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A172" s="7" t="s">
         <v>535</v>
       </c>
@@ -4863,7 +4874,7 @@
       </c>
       <c r="E172" s="7"/>
     </row>
-    <row r="173" spans="1:5">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173" s="9" t="s">
         <v>537</v>
       </c>
@@ -4878,7 +4889,7 @@
       </c>
       <c r="E173" s="7"/>
     </row>
-    <row r="174" spans="1:5">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A174" s="9" t="s">
         <v>538</v>
       </c>
@@ -4893,7 +4904,7 @@
       </c>
       <c r="E174" s="7"/>
     </row>
-    <row r="175" spans="1:5">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A175" s="9" t="s">
         <v>539</v>
       </c>
@@ -4908,7 +4919,7 @@
       </c>
       <c r="E175" s="7"/>
     </row>
-    <row r="176" spans="1:5">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A176" s="9" t="s">
         <v>540</v>
       </c>
@@ -4923,7 +4934,7 @@
       </c>
       <c r="E176" s="7"/>
     </row>
-    <row r="177" spans="1:5" ht="30">
+    <row r="177" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A177" s="7" t="s">
         <v>548</v>
       </c>
@@ -4938,7 +4949,7 @@
       </c>
       <c r="E177" s="7"/>
     </row>
-    <row r="178" spans="1:5">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A178" s="7" t="s">
         <v>551</v>
       </c>
@@ -4953,7 +4964,7 @@
       </c>
       <c r="E178" s="7"/>
     </row>
-    <row r="179" spans="1:5" ht="30">
+    <row r="179" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A179" s="7" t="s">
         <v>555</v>
       </c>
@@ -4968,7 +4979,7 @@
       </c>
       <c r="E179" s="7"/>
     </row>
-    <row r="180" spans="1:5">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A180" s="7" t="s">
         <v>557</v>
       </c>
@@ -4983,7 +4994,7 @@
       </c>
       <c r="E180" s="7"/>
     </row>
-    <row r="181" spans="1:5" ht="30">
+    <row r="181" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A181" s="7" t="s">
         <v>560</v>
       </c>
@@ -4998,7 +5009,7 @@
       </c>
       <c r="E181" s="7"/>
     </row>
-    <row r="182" spans="1:5">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A182" s="7" t="s">
         <v>563</v>
       </c>
@@ -5013,7 +5024,7 @@
       </c>
       <c r="E182" s="7"/>
     </row>
-    <row r="183" spans="1:5">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A183" s="7" t="s">
         <v>566</v>
       </c>
@@ -5028,7 +5039,7 @@
       </c>
       <c r="E183" s="7"/>
     </row>
-    <row r="184" spans="1:5">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A184" s="9" t="s">
         <v>569</v>
       </c>
@@ -5043,7 +5054,7 @@
       </c>
       <c r="E184" s="7"/>
     </row>
-    <row r="185" spans="1:5">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A185" s="9" t="s">
         <v>570</v>
       </c>
@@ -5058,7 +5069,7 @@
       </c>
       <c r="E185" s="7"/>
     </row>
-    <row r="186" spans="1:5">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A186" s="9" t="s">
         <v>579</v>
       </c>
@@ -5073,7 +5084,7 @@
       </c>
       <c r="E186" s="7"/>
     </row>
-    <row r="187" spans="1:5">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A187" s="9" t="s">
         <v>582</v>
       </c>
@@ -5088,7 +5099,7 @@
       </c>
       <c r="E187" s="7"/>
     </row>
-    <row r="188" spans="1:5">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A188" s="9" t="s">
         <v>585</v>
       </c>
@@ -5103,7 +5114,7 @@
       </c>
       <c r="E188" s="7"/>
     </row>
-    <row r="189" spans="1:5">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A189" s="9" t="s">
         <v>586</v>
       </c>
@@ -5118,7 +5129,7 @@
       </c>
       <c r="E189" s="7"/>
     </row>
-    <row r="190" spans="1:5" ht="30">
+    <row r="190" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A190" s="9" t="s">
         <v>591</v>
       </c>
@@ -5133,7 +5144,7 @@
       </c>
       <c r="E190" s="7"/>
     </row>
-    <row r="191" spans="1:5">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A191" s="9" t="s">
         <v>594</v>
       </c>
@@ -5147,6 +5158,21 @@
         <v>5</v>
       </c>
       <c r="E191" s="7"/>
+    </row>
+    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A192" s="9" t="s">
+        <v>597</v>
+      </c>
+      <c r="B192" s="7" t="s">
+        <v>598</v>
+      </c>
+      <c r="C192" s="8" t="s">
+        <v>599</v>
+      </c>
+      <c r="D192" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E192" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -5159,14 +5185,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView topLeftCell="A10" zoomScale="80" workbookViewId="0">
       <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
@@ -5174,7 +5200,7 @@
     <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>35</v>
       </c>
@@ -5188,7 +5214,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>37</v>
       </c>
@@ -5200,7 +5226,7 @@
       </c>
       <c r="D2" s="7"/>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>38</v>
       </c>
@@ -5212,7 +5238,7 @@
       </c>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>39</v>
       </c>
@@ -5224,7 +5250,7 @@
       </c>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>40</v>
       </c>
@@ -5236,7 +5262,7 @@
       </c>
       <c r="D5" s="7"/>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>41</v>
       </c>
@@ -5248,7 +5274,7 @@
       </c>
       <c r="D6" s="7"/>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>42</v>
       </c>
@@ -5260,7 +5286,7 @@
       </c>
       <c r="D7" s="7"/>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>43</v>
       </c>
@@ -5272,7 +5298,7 @@
       </c>
       <c r="D8" s="7"/>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>44</v>
       </c>
@@ -5284,7 +5310,7 @@
       </c>
       <c r="D9" s="7"/>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>45</v>
       </c>
@@ -5296,7 +5322,7 @@
       </c>
       <c r="D10" s="7"/>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>46</v>
       </c>
@@ -5308,7 +5334,7 @@
       </c>
       <c r="D11" s="7"/>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>48</v>
       </c>
@@ -5320,7 +5346,7 @@
       </c>
       <c r="D12" s="7"/>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>49</v>
       </c>
@@ -5332,7 +5358,7 @@
       </c>
       <c r="D13" s="7"/>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>50</v>
       </c>
@@ -5344,7 +5370,7 @@
       </c>
       <c r="D14" s="7"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>51</v>
       </c>
@@ -5356,7 +5382,7 @@
       </c>
       <c r="D15" s="7"/>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>52</v>
       </c>
@@ -5368,7 +5394,7 @@
       </c>
       <c r="D16" s="7"/>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>53</v>
       </c>
@@ -5380,7 +5406,7 @@
       </c>
       <c r="D17" s="7"/>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>54</v>
       </c>
@@ -5392,7 +5418,7 @@
       </c>
       <c r="D18" s="7"/>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>55</v>
       </c>
@@ -5404,7 +5430,7 @@
       </c>
       <c r="D19" s="7"/>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>56</v>
       </c>
@@ -5416,7 +5442,7 @@
       </c>
       <c r="D20" s="7"/>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>57</v>
       </c>
@@ -5428,7 +5454,7 @@
       </c>
       <c r="D21" s="7"/>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>58</v>
       </c>
@@ -5440,7 +5466,7 @@
       </c>
       <c r="D22" s="7"/>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>59</v>
       </c>
@@ -5452,7 +5478,7 @@
       </c>
       <c r="D23" s="7"/>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>60</v>
       </c>
@@ -5464,7 +5490,7 @@
       </c>
       <c r="D24" s="7"/>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>61</v>
       </c>
@@ -5476,7 +5502,7 @@
       </c>
       <c r="D25" s="7"/>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>47</v>
       </c>
@@ -5495,14 +5521,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A19" sqref="A19:XFD19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
@@ -5510,7 +5536,7 @@
     <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>35</v>
       </c>
@@ -5524,7 +5550,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>37</v>
       </c>
@@ -5536,7 +5562,7 @@
       </c>
       <c r="D2" s="7"/>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>38</v>
       </c>
@@ -5548,7 +5574,7 @@
       </c>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>39</v>
       </c>
@@ -5560,7 +5586,7 @@
       </c>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>40</v>
       </c>
@@ -5572,7 +5598,7 @@
       </c>
       <c r="D5" s="7"/>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>41</v>
       </c>
@@ -5584,7 +5610,7 @@
       </c>
       <c r="D6" s="7"/>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>42</v>
       </c>
@@ -5596,7 +5622,7 @@
       </c>
       <c r="D7" s="7"/>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>43</v>
       </c>
@@ -5608,7 +5634,7 @@
       </c>
       <c r="D8" s="7"/>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>44</v>
       </c>
@@ -5620,7 +5646,7 @@
       </c>
       <c r="D9" s="7"/>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>45</v>
       </c>
@@ -5632,7 +5658,7 @@
       </c>
       <c r="D10" s="7"/>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>46</v>
       </c>
@@ -5644,7 +5670,7 @@
       </c>
       <c r="D11" s="7"/>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>47</v>
       </c>
@@ -5656,7 +5682,7 @@
       </c>
       <c r="D12" s="7"/>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>48</v>
       </c>
@@ -5668,7 +5694,7 @@
       </c>
       <c r="D13" s="7"/>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>49</v>
       </c>
@@ -5680,7 +5706,7 @@
       </c>
       <c r="D14" s="7"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>50</v>
       </c>
@@ -5692,7 +5718,7 @@
       </c>
       <c r="D15" s="7"/>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>51</v>
       </c>
@@ -5704,7 +5730,7 @@
       </c>
       <c r="D16" s="7"/>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>52</v>
       </c>
@@ -5716,7 +5742,7 @@
       </c>
       <c r="D17" s="7"/>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>53</v>
       </c>
@@ -5728,7 +5754,7 @@
       </c>
       <c r="D18" s="7"/>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>54</v>
       </c>
@@ -5740,7 +5766,7 @@
       </c>
       <c r="D19" s="7"/>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>55</v>
       </c>
@@ -5752,7 +5778,7 @@
       </c>
       <c r="D20" s="7"/>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>56</v>
       </c>
@@ -5764,7 +5790,7 @@
       </c>
       <c r="D21" s="7"/>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>57</v>
       </c>
@@ -5776,7 +5802,7 @@
       </c>
       <c r="D22" s="7"/>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>58</v>
       </c>
@@ -5788,7 +5814,7 @@
       </c>
       <c r="D23" s="7"/>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>59</v>
       </c>
@@ -5800,7 +5826,7 @@
       </c>
       <c r="D24" s="7"/>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>60</v>
       </c>
@@ -5812,7 +5838,7 @@
       </c>
       <c r="D25" s="7"/>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>61</v>
       </c>

</xml_diff>

<commit_message>
Adds WAT-194 test script and related changes
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/WAT.xlsx
+++ b/src/test/resources/xls/WAT.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="927" uniqueCount="600">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="931" uniqueCount="603">
   <si>
     <t>TCID</t>
   </si>
@@ -1818,6 +1818,15 @@
   </si>
   <si>
     <t>Verify that user should not be able to submit feedback without entering curation mode</t>
+  </si>
+  <si>
+    <t>WAT194</t>
+  </si>
+  <si>
+    <t>WAT-1259</t>
+  </si>
+  <si>
+    <t>Verify that user should not land into mid curation mode after returning from a cancelled curation</t>
   </si>
 </sst>
 </file>
@@ -2277,10 +2286,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E192"/>
+  <dimension ref="A1:E193"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A173" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C192" sqref="C192"/>
+    <sheetView tabSelected="1" topLeftCell="A178" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C193" sqref="C193"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5173,6 +5182,21 @@
         <v>5</v>
       </c>
       <c r="E192" s="7"/>
+    </row>
+    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A193" s="9" t="s">
+        <v>600</v>
+      </c>
+      <c r="B193" s="7" t="s">
+        <v>601</v>
+      </c>
+      <c r="C193" s="8" t="s">
+        <v>602</v>
+      </c>
+      <c r="D193" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E193" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Adds WAT-195 testscript and related changes
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/WAT.xlsx
+++ b/src/test/resources/xls/WAT.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="931" uniqueCount="603">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="935" uniqueCount="606">
   <si>
     <t>TCID</t>
   </si>
@@ -1502,9 +1502,6 @@
     <t>Verify that CURATION MODE IS TRIGGERED when the user provides feedback on a recommended publication(Accept Publication), "Review updates" and "Submit updates [blue]" are displayed.</t>
   </si>
   <si>
-    <t xml:space="preserve">CLONE - Verify that CURATION MODE IS TRIGGERED when the user provides feedback on a recommended publication(Reject Publication), "Review updates" and "Submit updates [blue]" are displayed. </t>
-  </si>
-  <si>
     <t>WAT-893</t>
   </si>
   <si>
@@ -1827,6 +1824,18 @@
   </si>
   <si>
     <t>Verify that user should not land into mid curation mode after returning from a cancelled curation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that CURATION MODE IS TRIGGERED when the user provides feedback on a recommended publication(Reject Publication), "Review updates" and "Submit updates [blue]" are displayed. </t>
+  </si>
+  <si>
+    <t>WAT195</t>
+  </si>
+  <si>
+    <t>WAT-1257</t>
+  </si>
+  <si>
+    <t>Verify that rejoining an In-Progress curation has delete option for Publication</t>
   </si>
 </sst>
 </file>
@@ -2286,10 +2295,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E193"/>
+  <dimension ref="A1:E194"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A178" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C193" sqref="C193"/>
+    <sheetView tabSelected="1" topLeftCell="A187" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C201" sqref="C201"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3928,10 +3937,10 @@
         <v>351</v>
       </c>
       <c r="B109" s="9" t="s">
+        <v>576</v>
+      </c>
+      <c r="C109" s="8" t="s">
         <v>577</v>
-      </c>
-      <c r="C109" s="8" t="s">
-        <v>578</v>
       </c>
       <c r="D109" s="9" t="s">
         <v>5</v>
@@ -4453,10 +4462,10 @@
         <v>451</v>
       </c>
       <c r="B144" s="7" t="s">
+        <v>574</v>
+      </c>
+      <c r="C144" s="8" t="s">
         <v>575</v>
-      </c>
-      <c r="C144" s="8" t="s">
-        <v>576</v>
       </c>
       <c r="D144" s="7" t="s">
         <v>5</v>
@@ -4588,10 +4597,10 @@
         <v>478</v>
       </c>
       <c r="B153" s="7" t="s">
+        <v>496</v>
+      </c>
+      <c r="C153" s="8" t="s">
         <v>497</v>
-      </c>
-      <c r="C153" s="8" t="s">
-        <v>498</v>
       </c>
       <c r="D153" s="7" t="s">
         <v>5</v>
@@ -4663,7 +4672,7 @@
         <v>491</v>
       </c>
       <c r="B158" s="7" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="C158" s="8" t="s">
         <v>493</v>
@@ -4678,10 +4687,10 @@
         <v>492</v>
       </c>
       <c r="B159" s="7" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="C159" s="8" t="s">
-        <v>494</v>
+        <v>602</v>
       </c>
       <c r="D159" s="9" t="s">
         <v>5</v>
@@ -4690,13 +4699,13 @@
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" s="7" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="B160" s="7" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C160" s="8" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="D160" s="9" t="s">
         <v>5</v>
@@ -4705,13 +4714,13 @@
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161" s="7" t="s">
+        <v>499</v>
+      </c>
+      <c r="B161" s="7" t="s">
         <v>500</v>
       </c>
-      <c r="B161" s="7" t="s">
+      <c r="C161" s="8" t="s">
         <v>501</v>
-      </c>
-      <c r="C161" s="8" t="s">
-        <v>502</v>
       </c>
       <c r="D161" s="9" t="s">
         <v>5</v>
@@ -4720,13 +4729,13 @@
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162" s="7" t="s">
+        <v>502</v>
+      </c>
+      <c r="B162" s="7" t="s">
         <v>503</v>
       </c>
-      <c r="B162" s="7" t="s">
+      <c r="C162" s="8" t="s">
         <v>504</v>
-      </c>
-      <c r="C162" s="8" t="s">
-        <v>505</v>
       </c>
       <c r="D162" s="9" t="s">
         <v>5</v>
@@ -4735,13 +4744,13 @@
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" s="7" t="s">
+        <v>507</v>
+      </c>
+      <c r="B163" s="7" t="s">
         <v>508</v>
       </c>
-      <c r="B163" s="7" t="s">
+      <c r="C163" s="8" t="s">
         <v>509</v>
-      </c>
-      <c r="C163" s="8" t="s">
-        <v>510</v>
       </c>
       <c r="D163" s="9" t="s">
         <v>5</v>
@@ -4750,13 +4759,13 @@
     </row>
     <row r="164" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A164" s="7" t="s">
+        <v>510</v>
+      </c>
+      <c r="B164" s="7" t="s">
+        <v>512</v>
+      </c>
+      <c r="C164" s="8" t="s">
         <v>511</v>
-      </c>
-      <c r="B164" s="7" t="s">
-        <v>513</v>
-      </c>
-      <c r="C164" s="8" t="s">
-        <v>512</v>
       </c>
       <c r="D164" s="7" t="s">
         <v>5</v>
@@ -4765,13 +4774,13 @@
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165" s="7" t="s">
+        <v>513</v>
+      </c>
+      <c r="B165" s="7" t="s">
         <v>514</v>
       </c>
-      <c r="B165" s="7" t="s">
+      <c r="C165" s="8" t="s">
         <v>515</v>
-      </c>
-      <c r="C165" s="8" t="s">
-        <v>516</v>
       </c>
       <c r="D165" s="9" t="s">
         <v>5</v>
@@ -4780,13 +4789,13 @@
     </row>
     <row r="166" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A166" s="7" t="s">
+        <v>516</v>
+      </c>
+      <c r="B166" s="7" t="s">
         <v>517</v>
       </c>
-      <c r="B166" s="7" t="s">
+      <c r="C166" s="8" t="s">
         <v>518</v>
-      </c>
-      <c r="C166" s="8" t="s">
-        <v>519</v>
       </c>
       <c r="D166" s="7" t="s">
         <v>5</v>
@@ -4795,13 +4804,13 @@
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167" s="7" t="s">
+        <v>520</v>
+      </c>
+      <c r="B167" s="7" t="s">
+        <v>519</v>
+      </c>
+      <c r="C167" s="8" t="s">
         <v>521</v>
-      </c>
-      <c r="B167" s="7" t="s">
-        <v>520</v>
-      </c>
-      <c r="C167" s="8" t="s">
-        <v>522</v>
       </c>
       <c r="D167" s="7" t="s">
         <v>5</v>
@@ -4810,13 +4819,13 @@
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" s="7" t="s">
+        <v>522</v>
+      </c>
+      <c r="B168" s="7" t="s">
         <v>523</v>
       </c>
-      <c r="B168" s="7" t="s">
+      <c r="C168" s="8" t="s">
         <v>524</v>
-      </c>
-      <c r="C168" s="8" t="s">
-        <v>525</v>
       </c>
       <c r="D168" s="9" t="s">
         <v>5</v>
@@ -4825,13 +4834,13 @@
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" s="7" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="B169" s="7" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="C169" s="8" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="D169" s="7" t="s">
         <v>5</v>
@@ -4840,13 +4849,13 @@
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170" s="7" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="B170" s="7" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="C170" s="8" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="D170" s="7" t="s">
         <v>5</v>
@@ -4855,13 +4864,13 @@
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171" s="7" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="B171" s="7" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="C171" s="8" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="D171" s="7" t="s">
         <v>5</v>
@@ -4870,13 +4879,13 @@
     </row>
     <row r="172" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A172" s="7" t="s">
+        <v>534</v>
+      </c>
+      <c r="B172" s="7" t="s">
+        <v>514</v>
+      </c>
+      <c r="C172" s="8" t="s">
         <v>535</v>
-      </c>
-      <c r="B172" s="7" t="s">
-        <v>515</v>
-      </c>
-      <c r="C172" s="8" t="s">
-        <v>536</v>
       </c>
       <c r="D172" s="9" t="s">
         <v>5</v>
@@ -4885,13 +4894,13 @@
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173" s="9" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="B173" s="7" t="s">
+        <v>540</v>
+      </c>
+      <c r="C173" s="8" t="s">
         <v>541</v>
-      </c>
-      <c r="C173" s="8" t="s">
-        <v>542</v>
       </c>
       <c r="D173" s="7" t="s">
         <v>5</v>
@@ -4900,13 +4909,13 @@
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A174" s="9" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="B174" s="7" t="s">
+        <v>542</v>
+      </c>
+      <c r="C174" s="8" t="s">
         <v>543</v>
-      </c>
-      <c r="C174" s="8" t="s">
-        <v>544</v>
       </c>
       <c r="D174" s="7" t="s">
         <v>5</v>
@@ -4915,10 +4924,10 @@
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A175" s="9" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="B175" s="7" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C175" s="8" t="s">
         <v>231</v>
@@ -4930,13 +4939,13 @@
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A176" s="9" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="B176" s="7" t="s">
+        <v>545</v>
+      </c>
+      <c r="C176" s="8" t="s">
         <v>546</v>
-      </c>
-      <c r="C176" s="8" t="s">
-        <v>547</v>
       </c>
       <c r="D176" s="7" t="s">
         <v>5</v>
@@ -4945,13 +4954,13 @@
     </row>
     <row r="177" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A177" s="7" t="s">
+        <v>547</v>
+      </c>
+      <c r="B177" s="7" t="s">
         <v>548</v>
       </c>
-      <c r="B177" s="7" t="s">
+      <c r="C177" s="8" t="s">
         <v>549</v>
-      </c>
-      <c r="C177" s="8" t="s">
-        <v>550</v>
       </c>
       <c r="D177" s="9" t="s">
         <v>5</v>
@@ -4960,13 +4969,13 @@
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A178" s="7" t="s">
+        <v>550</v>
+      </c>
+      <c r="B178" s="7" t="s">
         <v>551</v>
       </c>
-      <c r="B178" s="7" t="s">
+      <c r="C178" s="8" t="s">
         <v>552</v>
-      </c>
-      <c r="C178" s="8" t="s">
-        <v>553</v>
       </c>
       <c r="D178" s="9" t="s">
         <v>5</v>
@@ -4975,13 +4984,13 @@
     </row>
     <row r="179" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A179" s="7" t="s">
+        <v>554</v>
+      </c>
+      <c r="B179" s="7" t="s">
         <v>555</v>
       </c>
-      <c r="B179" s="7" t="s">
-        <v>556</v>
-      </c>
       <c r="C179" s="8" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="D179" s="9" t="s">
         <v>5</v>
@@ -4990,13 +4999,13 @@
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A180" s="7" t="s">
+        <v>556</v>
+      </c>
+      <c r="B180" s="7" t="s">
         <v>557</v>
       </c>
-      <c r="B180" s="7" t="s">
+      <c r="C180" s="8" t="s">
         <v>558</v>
-      </c>
-      <c r="C180" s="8" t="s">
-        <v>559</v>
       </c>
       <c r="D180" s="9" t="s">
         <v>5</v>
@@ -5005,13 +5014,13 @@
     </row>
     <row r="181" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A181" s="7" t="s">
+        <v>559</v>
+      </c>
+      <c r="B181" s="7" t="s">
         <v>560</v>
       </c>
-      <c r="B181" s="7" t="s">
+      <c r="C181" s="8" t="s">
         <v>561</v>
-      </c>
-      <c r="C181" s="8" t="s">
-        <v>562</v>
       </c>
       <c r="D181" s="9" t="s">
         <v>5</v>
@@ -5020,13 +5029,13 @@
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A182" s="7" t="s">
+        <v>562</v>
+      </c>
+      <c r="B182" s="7" t="s">
         <v>563</v>
       </c>
-      <c r="B182" s="7" t="s">
+      <c r="C182" s="8" t="s">
         <v>564</v>
-      </c>
-      <c r="C182" s="8" t="s">
-        <v>565</v>
       </c>
       <c r="D182" s="9" t="s">
         <v>5</v>
@@ -5035,13 +5044,13 @@
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A183" s="7" t="s">
+        <v>565</v>
+      </c>
+      <c r="B183" s="7" t="s">
+        <v>567</v>
+      </c>
+      <c r="C183" s="8" t="s">
         <v>566</v>
-      </c>
-      <c r="B183" s="7" t="s">
-        <v>568</v>
-      </c>
-      <c r="C183" s="8" t="s">
-        <v>567</v>
       </c>
       <c r="D183" s="9" t="s">
         <v>5</v>
@@ -5050,13 +5059,13 @@
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A184" s="9" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="B184" s="7" t="s">
+        <v>570</v>
+      </c>
+      <c r="C184" s="8" t="s">
         <v>571</v>
-      </c>
-      <c r="C184" s="8" t="s">
-        <v>572</v>
       </c>
       <c r="D184" s="9" t="s">
         <v>5</v>
@@ -5065,13 +5074,13 @@
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A185" s="9" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="B185" s="7" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="C185" s="8" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="D185" s="9" t="s">
         <v>5</v>
@@ -5080,13 +5089,13 @@
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A186" s="9" t="s">
+        <v>578</v>
+      </c>
+      <c r="B186" s="7" t="s">
         <v>579</v>
       </c>
-      <c r="B186" s="7" t="s">
+      <c r="C186" s="8" t="s">
         <v>580</v>
-      </c>
-      <c r="C186" s="8" t="s">
-        <v>581</v>
       </c>
       <c r="D186" s="7" t="s">
         <v>5</v>
@@ -5095,13 +5104,13 @@
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A187" s="9" t="s">
+        <v>581</v>
+      </c>
+      <c r="B187" s="7" t="s">
         <v>582</v>
       </c>
-      <c r="B187" s="7" t="s">
+      <c r="C187" s="8" t="s">
         <v>583</v>
-      </c>
-      <c r="C187" s="8" t="s">
-        <v>584</v>
       </c>
       <c r="D187" s="7" t="s">
         <v>5</v>
@@ -5110,13 +5119,13 @@
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A188" s="9" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="B188" s="7" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="C188" s="8" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D188" s="7" t="s">
         <v>5</v>
@@ -5125,13 +5134,13 @@
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A189" s="9" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="B189" s="7" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="C189" s="8" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D189" s="7" t="s">
         <v>5</v>
@@ -5140,13 +5149,13 @@
     </row>
     <row r="190" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A190" s="9" t="s">
+        <v>590</v>
+      </c>
+      <c r="B190" s="7" t="s">
         <v>591</v>
       </c>
-      <c r="B190" s="7" t="s">
+      <c r="C190" s="8" t="s">
         <v>592</v>
-      </c>
-      <c r="C190" s="8" t="s">
-        <v>593</v>
       </c>
       <c r="D190" s="7" t="s">
         <v>5</v>
@@ -5155,13 +5164,13 @@
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A191" s="9" t="s">
+        <v>593</v>
+      </c>
+      <c r="B191" s="7" t="s">
         <v>594</v>
       </c>
-      <c r="B191" s="7" t="s">
+      <c r="C191" s="8" t="s">
         <v>595</v>
-      </c>
-      <c r="C191" s="8" t="s">
-        <v>596</v>
       </c>
       <c r="D191" s="7" t="s">
         <v>5</v>
@@ -5170,13 +5179,13 @@
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A192" s="9" t="s">
+        <v>596</v>
+      </c>
+      <c r="B192" s="7" t="s">
         <v>597</v>
       </c>
-      <c r="B192" s="7" t="s">
+      <c r="C192" s="8" t="s">
         <v>598</v>
-      </c>
-      <c r="C192" s="8" t="s">
-        <v>599</v>
       </c>
       <c r="D192" s="7" t="s">
         <v>5</v>
@@ -5185,18 +5194,33 @@
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A193" s="9" t="s">
+        <v>599</v>
+      </c>
+      <c r="B193" s="7" t="s">
         <v>600</v>
       </c>
-      <c r="B193" s="7" t="s">
+      <c r="C193" s="8" t="s">
         <v>601</v>
       </c>
-      <c r="C193" s="8" t="s">
-        <v>602</v>
-      </c>
       <c r="D193" s="7" t="s">
         <v>5</v>
       </c>
       <c r="E193" s="7"/>
+    </row>
+    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A194" s="9" t="s">
+        <v>603</v>
+      </c>
+      <c r="B194" s="7" t="s">
+        <v>604</v>
+      </c>
+      <c r="C194" s="8" t="s">
+        <v>605</v>
+      </c>
+      <c r="D194" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E194" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Adds WAT-196 testscript and related changes
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/WAT.xlsx
+++ b/src/test/resources/xls/WAT.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="935" uniqueCount="606">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="939" uniqueCount="609">
   <si>
     <t>TCID</t>
   </si>
@@ -1836,6 +1836,15 @@
   </si>
   <si>
     <t>Verify that rejoining an In-Progress curation has delete option for Publication</t>
+  </si>
+  <si>
+    <t>WAT196</t>
+  </si>
+  <si>
+    <t>WAT-1256</t>
+  </si>
+  <si>
+    <t>Verify that remove Publication Bulk panel options are not shown in non-curation mode.</t>
   </si>
 </sst>
 </file>
@@ -1897,7 +1906,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -1920,11 +1929,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1962,6 +1986,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2295,10 +2322,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E194"/>
+  <dimension ref="A1:E195"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A187" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C201" sqref="C201"/>
+      <selection activeCell="C195" sqref="C195"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5221,6 +5248,21 @@
         <v>5</v>
       </c>
       <c r="E194" s="7"/>
+    </row>
+    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A195" s="9" t="s">
+        <v>606</v>
+      </c>
+      <c r="B195" s="7" t="s">
+        <v>607</v>
+      </c>
+      <c r="C195" s="18" t="s">
+        <v>608</v>
+      </c>
+      <c r="D195" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E195" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Adds WAT-197 test script and related changes
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/WAT.xlsx
+++ b/src/test/resources/xls/WAT.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="939" uniqueCount="609">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="943" uniqueCount="612">
   <si>
     <t>TCID</t>
   </si>
@@ -1845,6 +1845,15 @@
   </si>
   <si>
     <t>Verify that remove Publication Bulk panel options are not shown in non-curation mode.</t>
+  </si>
+  <si>
+    <t>WAT197</t>
+  </si>
+  <si>
+    <t>WAT-1254</t>
+  </si>
+  <si>
+    <t>Verify that publication list has no "X" mark in non curation mode</t>
   </si>
 </sst>
 </file>
@@ -2322,10 +2331,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E195"/>
+  <dimension ref="A1:E196"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A187" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C195" sqref="C195"/>
+      <selection activeCell="A196" sqref="A196:E196"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5263,6 +5272,21 @@
         <v>5</v>
       </c>
       <c r="E195" s="7"/>
+    </row>
+    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A196" s="9" t="s">
+        <v>609</v>
+      </c>
+      <c r="B196" s="7" t="s">
+        <v>610</v>
+      </c>
+      <c r="C196" s="18" t="s">
+        <v>611</v>
+      </c>
+      <c r="D196" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E196" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Adds WAT-198 test script and related changes
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/WAT.xlsx
+++ b/src/test/resources/xls/WAT.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="943" uniqueCount="612">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="947" uniqueCount="615">
   <si>
     <t>TCID</t>
   </si>
@@ -1854,6 +1854,15 @@
   </si>
   <si>
     <t>Verify that publication list has no "X" mark in non curation mode</t>
+  </si>
+  <si>
+    <t>WAT198</t>
+  </si>
+  <si>
+    <t>WAT-1253</t>
+  </si>
+  <si>
+    <t>Verify that undo option for publication in Author record page should not be available in non curation mode</t>
   </si>
 </sst>
 </file>
@@ -2331,10 +2340,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E196"/>
+  <dimension ref="A1:E197"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A187" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A196" sqref="A196:E196"/>
+      <selection activeCell="C197" sqref="C197"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5287,6 +5296,21 @@
         <v>5</v>
       </c>
       <c r="E196" s="7"/>
+    </row>
+    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A197" s="9" t="s">
+        <v>612</v>
+      </c>
+      <c r="B197" s="7" t="s">
+        <v>613</v>
+      </c>
+      <c r="C197" s="18" t="s">
+        <v>614</v>
+      </c>
+      <c r="D197" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E197" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
WAT new scripts implementation
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/WAT.xlsx
+++ b/src/test/resources/xls/WAT.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13305" windowHeight="2415"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="947" uniqueCount="615">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="955" uniqueCount="621">
   <si>
     <t>TCID</t>
   </si>
@@ -1863,13 +1863,31 @@
   </si>
   <si>
     <t>Verify that undo option for publication in Author record page should not be available in non curation mode</t>
+  </si>
+  <si>
+    <t>WAT188</t>
+  </si>
+  <si>
+    <t>WAT-774</t>
+  </si>
+  <si>
+    <t>Verify that system must display Submit updates modal before submit feedback when user clicks on 'Submit updates' button</t>
+  </si>
+  <si>
+    <t>WAT189</t>
+  </si>
+  <si>
+    <t>WAT-770||WAT-772||WAT-773</t>
+  </si>
+  <si>
+    <t>Verify that User must have the ability to submit an author record after combining 2 or more author records.||Verify that system must submit the feedback when user clicks on 'Submit updates' button ||Verify that success confirmation message relates to submit feedback should display when user clicks on 'Submit updates' button</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1949,24 +1967,22 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </left>
       <right style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </right>
       <top style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -2005,9 +2021,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2096,7 +2111,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2128,10 +2143,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2163,7 +2177,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2339,14 +2352,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E197"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E199"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A187" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C197" sqref="C197"/>
+      <selection activeCell="D199" sqref="D199"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="30.5703125" customWidth="1" collapsed="1"/>
@@ -2355,7 +2368,7 @@
     <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2372,7 +2385,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -2387,7 +2400,7 @@
       </c>
       <c r="E2" s="4"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -2402,7 +2415,7 @@
       </c>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" s="7" t="s">
         <v>11</v>
       </c>
@@ -2417,7 +2430,7 @@
       </c>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" s="7" t="s">
         <v>12</v>
       </c>
@@ -2432,7 +2445,7 @@
       </c>
       <c r="E5" s="7"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" s="7" t="s">
         <v>14</v>
       </c>
@@ -2447,7 +2460,7 @@
       </c>
       <c r="E6" s="7"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" s="7" t="s">
         <v>17</v>
       </c>
@@ -2462,7 +2475,7 @@
       </c>
       <c r="E7" s="7"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" s="7" t="s">
         <v>20</v>
       </c>
@@ -2477,7 +2490,7 @@
       </c>
       <c r="E8" s="7"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" s="7" t="s">
         <v>22</v>
       </c>
@@ -2492,7 +2505,7 @@
       </c>
       <c r="E9" s="7"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10" s="7" t="s">
         <v>23</v>
       </c>
@@ -2507,7 +2520,7 @@
       </c>
       <c r="E10" s="7"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11" s="7" t="s">
         <v>24</v>
       </c>
@@ -2522,7 +2535,7 @@
       </c>
       <c r="E11" s="7"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12" s="7" t="s">
         <v>25</v>
       </c>
@@ -2537,7 +2550,7 @@
       </c>
       <c r="E12" s="7"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13" s="7" t="s">
         <v>62</v>
       </c>
@@ -2552,7 +2565,7 @@
       </c>
       <c r="E13" s="7"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="A14" s="7" t="s">
         <v>63</v>
       </c>
@@ -2567,7 +2580,7 @@
       </c>
       <c r="E14" s="7"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="A15" s="7" t="s">
         <v>64</v>
       </c>
@@ -2582,7 +2595,7 @@
       </c>
       <c r="E15" s="7"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="A16" s="7" t="s">
         <v>65</v>
       </c>
@@ -2597,7 +2610,7 @@
       </c>
       <c r="E16" s="7"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5">
       <c r="A17" s="7" t="s">
         <v>74</v>
       </c>
@@ -2612,7 +2625,7 @@
       </c>
       <c r="E17" s="7"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5">
       <c r="A18" s="7" t="s">
         <v>75</v>
       </c>
@@ -2627,7 +2640,7 @@
       </c>
       <c r="E18" s="7"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5">
       <c r="A19" s="7" t="s">
         <v>79</v>
       </c>
@@ -2642,7 +2655,7 @@
       </c>
       <c r="E19" s="7"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5">
       <c r="A20" s="7" t="s">
         <v>81</v>
       </c>
@@ -2657,7 +2670,7 @@
       </c>
       <c r="E20" s="7"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5">
       <c r="A21" s="7" t="s">
         <v>82</v>
       </c>
@@ -2672,7 +2685,7 @@
       </c>
       <c r="E21" s="7"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5">
       <c r="A22" s="7" t="s">
         <v>88</v>
       </c>
@@ -2687,7 +2700,7 @@
       </c>
       <c r="E22" s="7"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5">
       <c r="A23" s="7" t="s">
         <v>90</v>
       </c>
@@ -2702,7 +2715,7 @@
       </c>
       <c r="E23" s="7"/>
     </row>
-    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="30">
       <c r="A24" s="9" t="s">
         <v>94</v>
       </c>
@@ -2717,7 +2730,7 @@
       </c>
       <c r="E24" s="7"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5">
       <c r="A25" s="9" t="s">
         <v>96</v>
       </c>
@@ -2732,7 +2745,7 @@
       </c>
       <c r="E25" s="7"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5">
       <c r="A26" s="9" t="s">
         <v>98</v>
       </c>
@@ -2747,7 +2760,7 @@
       </c>
       <c r="E26" s="7"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5">
       <c r="A27" s="9" t="s">
         <v>102</v>
       </c>
@@ -2762,7 +2775,7 @@
       </c>
       <c r="E27" s="7"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5">
       <c r="A28" s="9" t="s">
         <v>105</v>
       </c>
@@ -2777,7 +2790,7 @@
       </c>
       <c r="E28" s="7"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5">
       <c r="A29" s="9" t="s">
         <v>108</v>
       </c>
@@ -2792,7 +2805,7 @@
       </c>
       <c r="E29" s="7"/>
     </row>
-    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" ht="30">
       <c r="A30" s="9" t="s">
         <v>110</v>
       </c>
@@ -2807,7 +2820,7 @@
       </c>
       <c r="E30" s="7"/>
     </row>
-    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" ht="30">
       <c r="A31" s="9" t="s">
         <v>114</v>
       </c>
@@ -2822,7 +2835,7 @@
       </c>
       <c r="E31" s="7"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5">
       <c r="A32" s="9" t="s">
         <v>119</v>
       </c>
@@ -2837,7 +2850,7 @@
       </c>
       <c r="E32" s="7"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5">
       <c r="A33" s="9" t="s">
         <v>120</v>
       </c>
@@ -2852,7 +2865,7 @@
       </c>
       <c r="E33" s="7"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5">
       <c r="A34" s="9" t="s">
         <v>125</v>
       </c>
@@ -2867,7 +2880,7 @@
       </c>
       <c r="E34" s="7"/>
     </row>
-    <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" ht="30">
       <c r="A35" s="9" t="s">
         <v>128</v>
       </c>
@@ -2882,7 +2895,7 @@
       </c>
       <c r="E35" s="7"/>
     </row>
-    <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" ht="30">
       <c r="A36" s="9" t="s">
         <v>131</v>
       </c>
@@ -2897,7 +2910,7 @@
       </c>
       <c r="E36" s="7"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5">
       <c r="A37" s="9" t="s">
         <v>134</v>
       </c>
@@ -2912,7 +2925,7 @@
       </c>
       <c r="E37" s="7"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5">
       <c r="A38" s="9" t="s">
         <v>137</v>
       </c>
@@ -2927,7 +2940,7 @@
       </c>
       <c r="E38" s="7"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5">
       <c r="A39" s="9" t="s">
         <v>140</v>
       </c>
@@ -2942,7 +2955,7 @@
       </c>
       <c r="E39" s="7"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5">
       <c r="A40" s="9" t="s">
         <v>143</v>
       </c>
@@ -2957,7 +2970,7 @@
       </c>
       <c r="E40" s="7"/>
     </row>
-    <row r="41" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" ht="30">
       <c r="A41" s="9" t="s">
         <v>145</v>
       </c>
@@ -2972,7 +2985,7 @@
       </c>
       <c r="E41" s="7"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5">
       <c r="A42" s="9" t="s">
         <v>147</v>
       </c>
@@ -2987,7 +3000,7 @@
       </c>
       <c r="E42" s="7"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5">
       <c r="A43" s="9" t="s">
         <v>150</v>
       </c>
@@ -3002,7 +3015,7 @@
       </c>
       <c r="E43" s="7"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5">
       <c r="A44" s="9" t="s">
         <v>153</v>
       </c>
@@ -3017,7 +3030,7 @@
       </c>
       <c r="E44" s="7"/>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5">
       <c r="A45" s="9" t="s">
         <v>155</v>
       </c>
@@ -3032,7 +3045,7 @@
       </c>
       <c r="E45" s="7"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5">
       <c r="A46" s="12" t="s">
         <v>158</v>
       </c>
@@ -3047,7 +3060,7 @@
       </c>
       <c r="E46" s="7"/>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5">
       <c r="A47" s="12" t="s">
         <v>159</v>
       </c>
@@ -3062,7 +3075,7 @@
       </c>
       <c r="E47" s="7"/>
     </row>
-    <row r="48" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" ht="30">
       <c r="A48" s="12" t="s">
         <v>160</v>
       </c>
@@ -3077,7 +3090,7 @@
       </c>
       <c r="E48" s="7"/>
     </row>
-    <row r="49" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" ht="30">
       <c r="A49" s="12" t="s">
         <v>161</v>
       </c>
@@ -3092,7 +3105,7 @@
       </c>
       <c r="E49" s="7"/>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5">
       <c r="A50" s="12" t="s">
         <v>164</v>
       </c>
@@ -3107,7 +3120,7 @@
       </c>
       <c r="E50" s="7"/>
     </row>
-    <row r="51" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" ht="30">
       <c r="A51" s="9" t="s">
         <v>173</v>
       </c>
@@ -3122,7 +3135,7 @@
       </c>
       <c r="E51" s="7"/>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5">
       <c r="A52" s="9" t="s">
         <v>174</v>
       </c>
@@ -3137,7 +3150,7 @@
       </c>
       <c r="E52" s="7"/>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5">
       <c r="A53" s="9" t="s">
         <v>179</v>
       </c>
@@ -3152,7 +3165,7 @@
       </c>
       <c r="E53" s="7"/>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5">
       <c r="A54" s="9" t="s">
         <v>180</v>
       </c>
@@ -3167,7 +3180,7 @@
       </c>
       <c r="E54" s="7"/>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5">
       <c r="A55" s="9" t="s">
         <v>185</v>
       </c>
@@ -3182,7 +3195,7 @@
       </c>
       <c r="E55" s="7"/>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5">
       <c r="A56" s="9" t="s">
         <v>188</v>
       </c>
@@ -3197,7 +3210,7 @@
       </c>
       <c r="E56" s="7"/>
     </row>
-    <row r="57" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" ht="30">
       <c r="A57" s="9" t="s">
         <v>191</v>
       </c>
@@ -3212,7 +3225,7 @@
       </c>
       <c r="E57" s="7"/>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5">
       <c r="A58" s="9" t="s">
         <v>194</v>
       </c>
@@ -3227,7 +3240,7 @@
       </c>
       <c r="E58" s="7"/>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5">
       <c r="A59" s="7" t="s">
         <v>196</v>
       </c>
@@ -3242,7 +3255,7 @@
       </c>
       <c r="E59" s="7"/>
     </row>
-    <row r="60" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" ht="45">
       <c r="A60" s="7" t="s">
         <v>199</v>
       </c>
@@ -3257,7 +3270,7 @@
       </c>
       <c r="E60" s="7"/>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5">
       <c r="A61" s="9" t="s">
         <v>202</v>
       </c>
@@ -3272,7 +3285,7 @@
       </c>
       <c r="E61" s="7"/>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5">
       <c r="A62" s="9" t="s">
         <v>204</v>
       </c>
@@ -3287,7 +3300,7 @@
       </c>
       <c r="E62" s="7"/>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5">
       <c r="A63" s="9" t="s">
         <v>206</v>
       </c>
@@ -3302,7 +3315,7 @@
       </c>
       <c r="E63" s="7"/>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5">
       <c r="A64" s="9" t="s">
         <v>208</v>
       </c>
@@ -3317,7 +3330,7 @@
       </c>
       <c r="E64" s="7"/>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5">
       <c r="A65" s="9" t="s">
         <v>217</v>
       </c>
@@ -3332,7 +3345,7 @@
       </c>
       <c r="E65" s="7"/>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5">
       <c r="A66" s="9" t="s">
         <v>218</v>
       </c>
@@ -3347,7 +3360,7 @@
       </c>
       <c r="E66" s="7"/>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5">
       <c r="A67" s="9" t="s">
         <v>223</v>
       </c>
@@ -3362,7 +3375,7 @@
       </c>
       <c r="E67" s="7"/>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5">
       <c r="A68" s="9" t="s">
         <v>224</v>
       </c>
@@ -3377,7 +3390,7 @@
       </c>
       <c r="E68" s="7"/>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5">
       <c r="A69" s="9" t="s">
         <v>225</v>
       </c>
@@ -3392,7 +3405,7 @@
       </c>
       <c r="E69" s="7"/>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5">
       <c r="A70" s="9" t="s">
         <v>226</v>
       </c>
@@ -3407,7 +3420,7 @@
       </c>
       <c r="E70" s="7"/>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5">
       <c r="A71" s="9" t="s">
         <v>233</v>
       </c>
@@ -3422,7 +3435,7 @@
       </c>
       <c r="E71" s="7"/>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5">
       <c r="A72" s="9" t="s">
         <v>237</v>
       </c>
@@ -3437,7 +3450,7 @@
       </c>
       <c r="E72" s="7"/>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5">
       <c r="A73" s="9" t="s">
         <v>239</v>
       </c>
@@ -3452,7 +3465,7 @@
       </c>
       <c r="E73" s="7"/>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5">
       <c r="A74" s="9" t="s">
         <v>243</v>
       </c>
@@ -3467,7 +3480,7 @@
       </c>
       <c r="E74" s="7"/>
     </row>
-    <row r="75" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" ht="30">
       <c r="A75" s="9" t="s">
         <v>245</v>
       </c>
@@ -3482,7 +3495,7 @@
       </c>
       <c r="E75" s="7"/>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5">
       <c r="A76" s="9" t="s">
         <v>248</v>
       </c>
@@ -3497,7 +3510,7 @@
       </c>
       <c r="E76" s="7"/>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5">
       <c r="A77" s="9" t="s">
         <v>256</v>
       </c>
@@ -3512,7 +3525,7 @@
       </c>
       <c r="E77" s="7"/>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5">
       <c r="A78" s="9" t="s">
         <v>257</v>
       </c>
@@ -3527,7 +3540,7 @@
       </c>
       <c r="E78" s="7"/>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5">
       <c r="A79" s="9" t="s">
         <v>261</v>
       </c>
@@ -3542,7 +3555,7 @@
       </c>
       <c r="E79" s="7"/>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5">
       <c r="A80" s="9" t="s">
         <v>264</v>
       </c>
@@ -3557,7 +3570,7 @@
       </c>
       <c r="E80" s="7"/>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5">
       <c r="A81" s="9" t="s">
         <v>267</v>
       </c>
@@ -3572,7 +3585,7 @@
       </c>
       <c r="E81" s="7"/>
     </row>
-    <row r="82" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" ht="30">
       <c r="A82" s="9" t="s">
         <v>269</v>
       </c>
@@ -3587,7 +3600,7 @@
       </c>
       <c r="E82" s="7"/>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5">
       <c r="A83" s="9" t="s">
         <v>274</v>
       </c>
@@ -3602,7 +3615,7 @@
       </c>
       <c r="E83" s="7"/>
     </row>
-    <row r="84" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" ht="30">
       <c r="A84" s="9" t="s">
         <v>277</v>
       </c>
@@ -3617,7 +3630,7 @@
       </c>
       <c r="E84" s="7"/>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5">
       <c r="A85" s="9" t="s">
         <v>279</v>
       </c>
@@ -3632,7 +3645,7 @@
       </c>
       <c r="E85" s="7"/>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5">
       <c r="A86" s="9" t="s">
         <v>282</v>
       </c>
@@ -3647,7 +3660,7 @@
       </c>
       <c r="E86" s="7"/>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5">
       <c r="A87" s="9" t="s">
         <v>285</v>
       </c>
@@ -3662,7 +3675,7 @@
       </c>
       <c r="E87" s="7"/>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5">
       <c r="A88" s="9" t="s">
         <v>288</v>
       </c>
@@ -3677,7 +3690,7 @@
       </c>
       <c r="E88" s="7"/>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5">
       <c r="A89" s="9" t="s">
         <v>291</v>
       </c>
@@ -3692,7 +3705,7 @@
       </c>
       <c r="E89" s="7"/>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5">
       <c r="A90" s="9" t="s">
         <v>294</v>
       </c>
@@ -3707,7 +3720,7 @@
       </c>
       <c r="E90" s="7"/>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5">
       <c r="A91" s="9" t="s">
         <v>297</v>
       </c>
@@ -3722,7 +3735,7 @@
       </c>
       <c r="E91" s="7"/>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5">
       <c r="A92" s="9" t="s">
         <v>300</v>
       </c>
@@ -3737,7 +3750,7 @@
       </c>
       <c r="E92" s="7"/>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5">
       <c r="A93" s="9" t="s">
         <v>303</v>
       </c>
@@ -3752,7 +3765,7 @@
       </c>
       <c r="E93" s="7"/>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5">
       <c r="A94" s="9" t="s">
         <v>306</v>
       </c>
@@ -3767,7 +3780,7 @@
       </c>
       <c r="E94" s="7"/>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5">
       <c r="A95" s="9" t="s">
         <v>309</v>
       </c>
@@ -3782,7 +3795,7 @@
       </c>
       <c r="E95" s="7"/>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5">
       <c r="A96" s="9" t="s">
         <v>314</v>
       </c>
@@ -3797,7 +3810,7 @@
       </c>
       <c r="E96" s="7"/>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5">
       <c r="A97" s="9" t="s">
         <v>315</v>
       </c>
@@ -3812,7 +3825,7 @@
       </c>
       <c r="E97" s="7"/>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5">
       <c r="A98" s="9" t="s">
         <v>319</v>
       </c>
@@ -3827,7 +3840,7 @@
       </c>
       <c r="E98" s="7"/>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5">
       <c r="A99" s="9" t="s">
         <v>321</v>
       </c>
@@ -3842,7 +3855,7 @@
       </c>
       <c r="E99" s="7"/>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5">
       <c r="A100" s="9" t="s">
         <v>322</v>
       </c>
@@ -3857,7 +3870,7 @@
       </c>
       <c r="E100" s="7"/>
     </row>
-    <row r="101" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" ht="30">
       <c r="A101" s="9" t="s">
         <v>323</v>
       </c>
@@ -3872,7 +3885,7 @@
       </c>
       <c r="E101" s="7"/>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5">
       <c r="A102" s="9" t="s">
         <v>328</v>
       </c>
@@ -3887,7 +3900,7 @@
       </c>
       <c r="E102" s="7"/>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5">
       <c r="A103" s="9" t="s">
         <v>333</v>
       </c>
@@ -3902,7 +3915,7 @@
       </c>
       <c r="E103" s="7"/>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5">
       <c r="A104" s="9" t="s">
         <v>336</v>
       </c>
@@ -3917,7 +3930,7 @@
       </c>
       <c r="E104" s="7"/>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5">
       <c r="A105" s="9" t="s">
         <v>337</v>
       </c>
@@ -3932,7 +3945,7 @@
       </c>
       <c r="E105" s="7"/>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5">
       <c r="A106" s="9" t="s">
         <v>342</v>
       </c>
@@ -3947,7 +3960,7 @@
       </c>
       <c r="E106" s="7"/>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5">
       <c r="A107" s="9" t="s">
         <v>345</v>
       </c>
@@ -3962,7 +3975,7 @@
       </c>
       <c r="E107" s="7"/>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5">
       <c r="A108" s="9" t="s">
         <v>350</v>
       </c>
@@ -3977,7 +3990,7 @@
       </c>
       <c r="E108" s="7"/>
     </row>
-    <row r="109" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" ht="30">
       <c r="A109" s="9" t="s">
         <v>351</v>
       </c>
@@ -3992,7 +4005,7 @@
       </c>
       <c r="E109" s="7"/>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5">
       <c r="A110" s="9" t="s">
         <v>352</v>
       </c>
@@ -4007,7 +4020,7 @@
       </c>
       <c r="E110" s="7"/>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5">
       <c r="A111" s="9" t="s">
         <v>355</v>
       </c>
@@ -4022,7 +4035,7 @@
       </c>
       <c r="E111" s="7"/>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5">
       <c r="A112" s="9" t="s">
         <v>359</v>
       </c>
@@ -4037,7 +4050,7 @@
       </c>
       <c r="E112" s="7"/>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5">
       <c r="A113" s="9" t="s">
         <v>361</v>
       </c>
@@ -4052,7 +4065,7 @@
       </c>
       <c r="E113" s="7"/>
     </row>
-    <row r="114" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" ht="30">
       <c r="A114" s="9" t="s">
         <v>364</v>
       </c>
@@ -4067,7 +4080,7 @@
       </c>
       <c r="E114" s="7"/>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5">
       <c r="A115" s="9" t="s">
         <v>367</v>
       </c>
@@ -4082,7 +4095,7 @@
       </c>
       <c r="E115" s="7"/>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5">
       <c r="A116" s="9" t="s">
         <v>368</v>
       </c>
@@ -4097,7 +4110,7 @@
       </c>
       <c r="E116" s="7"/>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5">
       <c r="A117" s="9" t="s">
         <v>369</v>
       </c>
@@ -4112,7 +4125,7 @@
       </c>
       <c r="E117" s="7"/>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5">
       <c r="A118" s="9" t="s">
         <v>376</v>
       </c>
@@ -4127,7 +4140,7 @@
       </c>
       <c r="E118" s="7"/>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5">
       <c r="A119" s="9" t="s">
         <v>379</v>
       </c>
@@ -4142,7 +4155,7 @@
       </c>
       <c r="E119" s="7"/>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5">
       <c r="A120" s="9" t="s">
         <v>382</v>
       </c>
@@ -4157,7 +4170,7 @@
       </c>
       <c r="E120" s="7"/>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5">
       <c r="A121" s="9" t="s">
         <v>385</v>
       </c>
@@ -4172,7 +4185,7 @@
       </c>
       <c r="E121" s="7"/>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5">
       <c r="A122" s="7" t="s">
         <v>388</v>
       </c>
@@ -4187,7 +4200,7 @@
       </c>
       <c r="E122" s="7"/>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5">
       <c r="A123" s="7" t="s">
         <v>391</v>
       </c>
@@ -4202,7 +4215,7 @@
       </c>
       <c r="E123" s="7"/>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5">
       <c r="A124" s="7" t="s">
         <v>394</v>
       </c>
@@ -4217,7 +4230,7 @@
       </c>
       <c r="E124" s="7"/>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5">
       <c r="A125" s="9" t="s">
         <v>397</v>
       </c>
@@ -4232,7 +4245,7 @@
       </c>
       <c r="E125" s="7"/>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5">
       <c r="A126" s="7" t="s">
         <v>400</v>
       </c>
@@ -4247,7 +4260,7 @@
       </c>
       <c r="E126" s="7"/>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5">
       <c r="A127" s="7" t="s">
         <v>403</v>
       </c>
@@ -4262,7 +4275,7 @@
       </c>
       <c r="E127" s="7"/>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5">
       <c r="A128" s="7" t="s">
         <v>406</v>
       </c>
@@ -4277,7 +4290,7 @@
       </c>
       <c r="E128" s="7"/>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5">
       <c r="A129" s="9" t="s">
         <v>409</v>
       </c>
@@ -4292,7 +4305,7 @@
       </c>
       <c r="E129" s="7"/>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5">
       <c r="A130" s="9" t="s">
         <v>412</v>
       </c>
@@ -4307,7 +4320,7 @@
       </c>
       <c r="E130" s="7"/>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5">
       <c r="A131" s="9" t="s">
         <v>414</v>
       </c>
@@ -4322,7 +4335,7 @@
       </c>
       <c r="E131" s="7"/>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5">
       <c r="A132" s="7" t="s">
         <v>417</v>
       </c>
@@ -4337,7 +4350,7 @@
       </c>
       <c r="E132" s="7"/>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5">
       <c r="A133" s="9" t="s">
         <v>420</v>
       </c>
@@ -4352,7 +4365,7 @@
       </c>
       <c r="E133" s="7"/>
     </row>
-    <row r="134" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5" ht="30">
       <c r="A134" s="7" t="s">
         <v>423</v>
       </c>
@@ -4367,7 +4380,7 @@
       </c>
       <c r="E134" s="7"/>
     </row>
-    <row r="135" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5" ht="30">
       <c r="A135" s="7" t="s">
         <v>424</v>
       </c>
@@ -4382,7 +4395,7 @@
       </c>
       <c r="E135" s="7"/>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5">
       <c r="A136" s="9" t="s">
         <v>429</v>
       </c>
@@ -4397,7 +4410,7 @@
       </c>
       <c r="E136" s="7"/>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5">
       <c r="A137" s="7" t="s">
         <v>432</v>
       </c>
@@ -4412,7 +4425,7 @@
       </c>
       <c r="E137" s="7"/>
     </row>
-    <row r="138" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" ht="45">
       <c r="A138" s="7" t="s">
         <v>433</v>
       </c>
@@ -4427,7 +4440,7 @@
       </c>
       <c r="E138" s="7"/>
     </row>
-    <row r="139" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5" ht="30">
       <c r="A139" s="7" t="s">
         <v>434</v>
       </c>
@@ -4442,7 +4455,7 @@
       </c>
       <c r="E139" s="7"/>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5">
       <c r="A140" s="17" t="s">
         <v>441</v>
       </c>
@@ -4457,7 +4470,7 @@
       </c>
       <c r="E140" s="7"/>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5">
       <c r="A141" s="17" t="s">
         <v>444</v>
       </c>
@@ -4472,7 +4485,7 @@
       </c>
       <c r="E141" s="7"/>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:5">
       <c r="A142" s="17" t="s">
         <v>447</v>
       </c>
@@ -4487,7 +4500,7 @@
       </c>
       <c r="E142" s="7"/>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:5">
       <c r="A143" s="17" t="s">
         <v>450</v>
       </c>
@@ -4502,7 +4515,7 @@
       </c>
       <c r="E143" s="7"/>
     </row>
-    <row r="144" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:5" ht="30">
       <c r="A144" s="17" t="s">
         <v>451</v>
       </c>
@@ -4517,7 +4530,7 @@
       </c>
       <c r="E144" s="7"/>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:5">
       <c r="A145" s="17" t="s">
         <v>454</v>
       </c>
@@ -4532,7 +4545,7 @@
       </c>
       <c r="E145" s="7"/>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:5">
       <c r="A146" s="17" t="s">
         <v>457</v>
       </c>
@@ -4547,7 +4560,7 @@
       </c>
       <c r="E146" s="7"/>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:5">
       <c r="A147" s="17" t="s">
         <v>460</v>
       </c>
@@ -4562,7 +4575,7 @@
       </c>
       <c r="E147" s="7"/>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:5">
       <c r="A148" s="17" t="s">
         <v>463</v>
       </c>
@@ -4577,7 +4590,7 @@
       </c>
       <c r="E148" s="7"/>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:5">
       <c r="A149" s="7" t="s">
         <v>466</v>
       </c>
@@ -4592,7 +4605,7 @@
       </c>
       <c r="E149" s="7"/>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:5">
       <c r="A150" s="7" t="s">
         <v>467</v>
       </c>
@@ -4607,7 +4620,7 @@
       </c>
       <c r="E150" s="7"/>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:5">
       <c r="A151" s="7" t="s">
         <v>468</v>
       </c>
@@ -4622,7 +4635,7 @@
       </c>
       <c r="E151" s="7"/>
     </row>
-    <row r="152" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:5" ht="30">
       <c r="A152" s="7" t="s">
         <v>475</v>
       </c>
@@ -4637,7 +4650,7 @@
       </c>
       <c r="E152" s="7"/>
     </row>
-    <row r="153" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:5" ht="45">
       <c r="A153" s="17" t="s">
         <v>478</v>
       </c>
@@ -4652,7 +4665,7 @@
       </c>
       <c r="E153" s="7"/>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:5">
       <c r="A154" s="17" t="s">
         <v>480</v>
       </c>
@@ -4667,7 +4680,7 @@
       </c>
       <c r="E154" s="7"/>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:5">
       <c r="A155" s="7" t="s">
         <v>482</v>
       </c>
@@ -4682,7 +4695,7 @@
       </c>
       <c r="E155" s="7"/>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:5">
       <c r="A156" s="7" t="s">
         <v>485</v>
       </c>
@@ -4697,7 +4710,7 @@
       </c>
       <c r="E156" s="7"/>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:5">
       <c r="A157" s="7" t="s">
         <v>488</v>
       </c>
@@ -4712,7 +4725,7 @@
       </c>
       <c r="E157" s="7"/>
     </row>
-    <row r="158" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:5" ht="30">
       <c r="A158" s="7" t="s">
         <v>491</v>
       </c>
@@ -4727,7 +4740,7 @@
       </c>
       <c r="E158" s="7"/>
     </row>
-    <row r="159" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:5" ht="30">
       <c r="A159" s="7" t="s">
         <v>492</v>
       </c>
@@ -4742,7 +4755,7 @@
       </c>
       <c r="E159" s="7"/>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:5">
       <c r="A160" s="7" t="s">
         <v>498</v>
       </c>
@@ -4757,7 +4770,7 @@
       </c>
       <c r="E160" s="7"/>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:5">
       <c r="A161" s="7" t="s">
         <v>499</v>
       </c>
@@ -4772,7 +4785,7 @@
       </c>
       <c r="E161" s="7"/>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:5">
       <c r="A162" s="7" t="s">
         <v>502</v>
       </c>
@@ -4787,7 +4800,7 @@
       </c>
       <c r="E162" s="7"/>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:5">
       <c r="A163" s="7" t="s">
         <v>507</v>
       </c>
@@ -4802,7 +4815,7 @@
       </c>
       <c r="E163" s="7"/>
     </row>
-    <row r="164" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:5" ht="30">
       <c r="A164" s="7" t="s">
         <v>510</v>
       </c>
@@ -4817,7 +4830,7 @@
       </c>
       <c r="E164" s="7"/>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:5">
       <c r="A165" s="7" t="s">
         <v>513</v>
       </c>
@@ -4832,7 +4845,7 @@
       </c>
       <c r="E165" s="7"/>
     </row>
-    <row r="166" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:5" ht="30">
       <c r="A166" s="7" t="s">
         <v>516</v>
       </c>
@@ -4847,7 +4860,7 @@
       </c>
       <c r="E166" s="7"/>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:5">
       <c r="A167" s="7" t="s">
         <v>520</v>
       </c>
@@ -4862,7 +4875,7 @@
       </c>
       <c r="E167" s="7"/>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:5">
       <c r="A168" s="7" t="s">
         <v>522</v>
       </c>
@@ -4877,7 +4890,7 @@
       </c>
       <c r="E168" s="7"/>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:5">
       <c r="A169" s="7" t="s">
         <v>525</v>
       </c>
@@ -4892,7 +4905,7 @@
       </c>
       <c r="E169" s="7"/>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:5">
       <c r="A170" s="7" t="s">
         <v>526</v>
       </c>
@@ -4907,7 +4920,7 @@
       </c>
       <c r="E170" s="7"/>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:5">
       <c r="A171" s="7" t="s">
         <v>527</v>
       </c>
@@ -4922,7 +4935,7 @@
       </c>
       <c r="E171" s="7"/>
     </row>
-    <row r="172" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:5" ht="30">
       <c r="A172" s="7" t="s">
         <v>534</v>
       </c>
@@ -4937,7 +4950,7 @@
       </c>
       <c r="E172" s="7"/>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:5">
       <c r="A173" s="9" t="s">
         <v>536</v>
       </c>
@@ -4952,7 +4965,7 @@
       </c>
       <c r="E173" s="7"/>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:5">
       <c r="A174" s="9" t="s">
         <v>537</v>
       </c>
@@ -4967,7 +4980,7 @@
       </c>
       <c r="E174" s="7"/>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:5">
       <c r="A175" s="9" t="s">
         <v>538</v>
       </c>
@@ -4982,7 +4995,7 @@
       </c>
       <c r="E175" s="7"/>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:5">
       <c r="A176" s="9" t="s">
         <v>539</v>
       </c>
@@ -4997,7 +5010,7 @@
       </c>
       <c r="E176" s="7"/>
     </row>
-    <row r="177" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:5" ht="30">
       <c r="A177" s="7" t="s">
         <v>547</v>
       </c>
@@ -5012,7 +5025,7 @@
       </c>
       <c r="E177" s="7"/>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:5">
       <c r="A178" s="7" t="s">
         <v>550</v>
       </c>
@@ -5027,7 +5040,7 @@
       </c>
       <c r="E178" s="7"/>
     </row>
-    <row r="179" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:5" ht="30">
       <c r="A179" s="7" t="s">
         <v>554</v>
       </c>
@@ -5042,7 +5055,7 @@
       </c>
       <c r="E179" s="7"/>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:5">
       <c r="A180" s="7" t="s">
         <v>556</v>
       </c>
@@ -5057,7 +5070,7 @@
       </c>
       <c r="E180" s="7"/>
     </row>
-    <row r="181" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:5" ht="30">
       <c r="A181" s="7" t="s">
         <v>559</v>
       </c>
@@ -5072,7 +5085,7 @@
       </c>
       <c r="E181" s="7"/>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:5">
       <c r="A182" s="7" t="s">
         <v>562</v>
       </c>
@@ -5087,7 +5100,7 @@
       </c>
       <c r="E182" s="7"/>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:5">
       <c r="A183" s="7" t="s">
         <v>565</v>
       </c>
@@ -5102,7 +5115,7 @@
       </c>
       <c r="E183" s="7"/>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:5">
       <c r="A184" s="9" t="s">
         <v>568</v>
       </c>
@@ -5117,7 +5130,7 @@
       </c>
       <c r="E184" s="7"/>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:5">
       <c r="A185" s="9" t="s">
         <v>569</v>
       </c>
@@ -5132,7 +5145,7 @@
       </c>
       <c r="E185" s="7"/>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:5">
       <c r="A186" s="9" t="s">
         <v>578</v>
       </c>
@@ -5147,7 +5160,7 @@
       </c>
       <c r="E186" s="7"/>
     </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:5">
       <c r="A187" s="9" t="s">
         <v>581</v>
       </c>
@@ -5162,7 +5175,7 @@
       </c>
       <c r="E187" s="7"/>
     </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:5">
       <c r="A188" s="9" t="s">
         <v>584</v>
       </c>
@@ -5177,7 +5190,7 @@
       </c>
       <c r="E188" s="7"/>
     </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:5">
       <c r="A189" s="9" t="s">
         <v>585</v>
       </c>
@@ -5192,7 +5205,7 @@
       </c>
       <c r="E189" s="7"/>
     </row>
-    <row r="190" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:5" ht="30">
       <c r="A190" s="9" t="s">
         <v>590</v>
       </c>
@@ -5207,7 +5220,7 @@
       </c>
       <c r="E190" s="7"/>
     </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:5">
       <c r="A191" s="9" t="s">
         <v>593</v>
       </c>
@@ -5222,7 +5235,7 @@
       </c>
       <c r="E191" s="7"/>
     </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:5">
       <c r="A192" s="9" t="s">
         <v>596</v>
       </c>
@@ -5237,7 +5250,7 @@
       </c>
       <c r="E192" s="7"/>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:5">
       <c r="A193" s="9" t="s">
         <v>599</v>
       </c>
@@ -5252,7 +5265,7 @@
       </c>
       <c r="E193" s="7"/>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:5">
       <c r="A194" s="9" t="s">
         <v>603</v>
       </c>
@@ -5267,14 +5280,14 @@
       </c>
       <c r="E194" s="7"/>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:5">
       <c r="A195" s="9" t="s">
         <v>606</v>
       </c>
       <c r="B195" s="7" t="s">
         <v>607</v>
       </c>
-      <c r="C195" s="18" t="s">
+      <c r="C195" s="8" t="s">
         <v>608</v>
       </c>
       <c r="D195" s="7" t="s">
@@ -5282,14 +5295,14 @@
       </c>
       <c r="E195" s="7"/>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:5">
       <c r="A196" s="9" t="s">
         <v>609</v>
       </c>
       <c r="B196" s="7" t="s">
         <v>610</v>
       </c>
-      <c r="C196" s="18" t="s">
+      <c r="C196" s="8" t="s">
         <v>611</v>
       </c>
       <c r="D196" s="7" t="s">
@@ -5297,20 +5310,50 @@
       </c>
       <c r="E196" s="7"/>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A197" s="9" t="s">
+    <row r="197" spans="1:5">
+      <c r="A197" s="18" t="s">
         <v>612</v>
       </c>
-      <c r="B197" s="7" t="s">
+      <c r="B197" s="19" t="s">
         <v>613</v>
       </c>
-      <c r="C197" s="18" t="s">
+      <c r="C197" s="8" t="s">
         <v>614</v>
       </c>
-      <c r="D197" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E197" s="7"/>
+      <c r="D197" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="E197" s="19"/>
+    </row>
+    <row r="198" spans="1:5">
+      <c r="A198" s="7" t="s">
+        <v>615</v>
+      </c>
+      <c r="B198" s="7" t="s">
+        <v>616</v>
+      </c>
+      <c r="C198" s="8" t="s">
+        <v>617</v>
+      </c>
+      <c r="D198" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E198" s="7"/>
+    </row>
+    <row r="199" spans="1:5" ht="45">
+      <c r="A199" s="7" t="s">
+        <v>618</v>
+      </c>
+      <c r="B199" s="7" t="s">
+        <v>619</v>
+      </c>
+      <c r="C199" s="8" t="s">
+        <v>620</v>
+      </c>
+      <c r="D199" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E199" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -5323,14 +5366,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView topLeftCell="A10" zoomScale="80" workbookViewId="0">
       <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
@@ -5338,7 +5381,7 @@
     <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="10" t="s">
         <v>35</v>
       </c>
@@ -5352,7 +5395,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="7" t="s">
         <v>37</v>
       </c>
@@ -5364,7 +5407,7 @@
       </c>
       <c r="D2" s="7"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="7" t="s">
         <v>38</v>
       </c>
@@ -5376,7 +5419,7 @@
       </c>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="7" t="s">
         <v>39</v>
       </c>
@@ -5388,7 +5431,7 @@
       </c>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" s="7" t="s">
         <v>40</v>
       </c>
@@ -5400,7 +5443,7 @@
       </c>
       <c r="D5" s="7"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" s="7" t="s">
         <v>41</v>
       </c>
@@ -5412,7 +5455,7 @@
       </c>
       <c r="D6" s="7"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="7" t="s">
         <v>42</v>
       </c>
@@ -5424,7 +5467,7 @@
       </c>
       <c r="D7" s="7"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="7" t="s">
         <v>43</v>
       </c>
@@ -5436,7 +5479,7 @@
       </c>
       <c r="D8" s="7"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="7" t="s">
         <v>44</v>
       </c>
@@ -5448,7 +5491,7 @@
       </c>
       <c r="D9" s="7"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="7" t="s">
         <v>45</v>
       </c>
@@ -5460,7 +5503,7 @@
       </c>
       <c r="D10" s="7"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11" s="7" t="s">
         <v>46</v>
       </c>
@@ -5472,7 +5515,7 @@
       </c>
       <c r="D11" s="7"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="A12" s="7" t="s">
         <v>48</v>
       </c>
@@ -5484,7 +5527,7 @@
       </c>
       <c r="D12" s="7"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="A13" s="7" t="s">
         <v>49</v>
       </c>
@@ -5496,7 +5539,7 @@
       </c>
       <c r="D13" s="7"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="A14" s="7" t="s">
         <v>50</v>
       </c>
@@ -5508,7 +5551,7 @@
       </c>
       <c r="D14" s="7"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="A15" s="7" t="s">
         <v>51</v>
       </c>
@@ -5520,7 +5563,7 @@
       </c>
       <c r="D15" s="7"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="A16" s="7" t="s">
         <v>52</v>
       </c>
@@ -5532,7 +5575,7 @@
       </c>
       <c r="D16" s="7"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4">
       <c r="A17" s="7" t="s">
         <v>53</v>
       </c>
@@ -5544,7 +5587,7 @@
       </c>
       <c r="D17" s="7"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4">
       <c r="A18" s="7" t="s">
         <v>54</v>
       </c>
@@ -5556,7 +5599,7 @@
       </c>
       <c r="D18" s="7"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4">
       <c r="A19" s="7" t="s">
         <v>55</v>
       </c>
@@ -5568,7 +5611,7 @@
       </c>
       <c r="D19" s="7"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4">
       <c r="A20" s="7" t="s">
         <v>56</v>
       </c>
@@ -5580,7 +5623,7 @@
       </c>
       <c r="D20" s="7"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4">
       <c r="A21" s="7" t="s">
         <v>57</v>
       </c>
@@ -5592,7 +5635,7 @@
       </c>
       <c r="D21" s="7"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4">
       <c r="A22" s="7" t="s">
         <v>58</v>
       </c>
@@ -5604,7 +5647,7 @@
       </c>
       <c r="D22" s="7"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4">
       <c r="A23" s="7" t="s">
         <v>59</v>
       </c>
@@ -5616,7 +5659,7 @@
       </c>
       <c r="D23" s="7"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4">
       <c r="A24" s="7" t="s">
         <v>60</v>
       </c>
@@ -5628,7 +5671,7 @@
       </c>
       <c r="D24" s="7"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4">
       <c r="A25" s="7" t="s">
         <v>61</v>
       </c>
@@ -5640,7 +5683,7 @@
       </c>
       <c r="D25" s="7"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4">
       <c r="A26" s="7" t="s">
         <v>47</v>
       </c>
@@ -5659,14 +5702,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A19" sqref="A19:XFD19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
@@ -5674,7 +5717,7 @@
     <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="10" t="s">
         <v>35</v>
       </c>
@@ -5688,7 +5731,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="7" t="s">
         <v>37</v>
       </c>
@@ -5700,7 +5743,7 @@
       </c>
       <c r="D2" s="7"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="7" t="s">
         <v>38</v>
       </c>
@@ -5712,7 +5755,7 @@
       </c>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="7" t="s">
         <v>39</v>
       </c>
@@ -5724,7 +5767,7 @@
       </c>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" s="7" t="s">
         <v>40</v>
       </c>
@@ -5736,7 +5779,7 @@
       </c>
       <c r="D5" s="7"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" s="7" t="s">
         <v>41</v>
       </c>
@@ -5748,7 +5791,7 @@
       </c>
       <c r="D6" s="7"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="7" t="s">
         <v>42</v>
       </c>
@@ -5760,7 +5803,7 @@
       </c>
       <c r="D7" s="7"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="7" t="s">
         <v>43</v>
       </c>
@@ -5772,7 +5815,7 @@
       </c>
       <c r="D8" s="7"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="7" t="s">
         <v>44</v>
       </c>
@@ -5784,7 +5827,7 @@
       </c>
       <c r="D9" s="7"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="7" t="s">
         <v>45</v>
       </c>
@@ -5796,7 +5839,7 @@
       </c>
       <c r="D10" s="7"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11" s="7" t="s">
         <v>46</v>
       </c>
@@ -5808,7 +5851,7 @@
       </c>
       <c r="D11" s="7"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="A12" s="7" t="s">
         <v>47</v>
       </c>
@@ -5820,7 +5863,7 @@
       </c>
       <c r="D12" s="7"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="A13" s="7" t="s">
         <v>48</v>
       </c>
@@ -5832,7 +5875,7 @@
       </c>
       <c r="D13" s="7"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="A14" s="7" t="s">
         <v>49</v>
       </c>
@@ -5844,7 +5887,7 @@
       </c>
       <c r="D14" s="7"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="A15" s="7" t="s">
         <v>50</v>
       </c>
@@ -5856,7 +5899,7 @@
       </c>
       <c r="D15" s="7"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="A16" s="7" t="s">
         <v>51</v>
       </c>
@@ -5868,7 +5911,7 @@
       </c>
       <c r="D16" s="7"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4">
       <c r="A17" s="7" t="s">
         <v>52</v>
       </c>
@@ -5880,7 +5923,7 @@
       </c>
       <c r="D17" s="7"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4">
       <c r="A18" s="7" t="s">
         <v>53</v>
       </c>
@@ -5892,7 +5935,7 @@
       </c>
       <c r="D18" s="7"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4">
       <c r="A19" s="7" t="s">
         <v>54</v>
       </c>
@@ -5904,7 +5947,7 @@
       </c>
       <c r="D19" s="7"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4">
       <c r="A20" s="7" t="s">
         <v>55</v>
       </c>
@@ -5916,7 +5959,7 @@
       </c>
       <c r="D20" s="7"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4">
       <c r="A21" s="7" t="s">
         <v>56</v>
       </c>
@@ -5928,7 +5971,7 @@
       </c>
       <c r="D21" s="7"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4">
       <c r="A22" s="7" t="s">
         <v>57</v>
       </c>
@@ -5940,7 +5983,7 @@
       </c>
       <c r="D22" s="7"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4">
       <c r="A23" s="7" t="s">
         <v>58</v>
       </c>
@@ -5952,7 +5995,7 @@
       </c>
       <c r="D23" s="7"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4">
       <c r="A24" s="7" t="s">
         <v>59</v>
       </c>
@@ -5964,7 +6007,7 @@
       </c>
       <c r="D24" s="7"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4">
       <c r="A25" s="7" t="s">
         <v>60</v>
       </c>
@@ -5976,7 +6019,7 @@
       </c>
       <c r="D25" s="7"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4">
       <c r="A26" s="7" t="s">
         <v>61</v>
       </c>

</xml_diff>

<commit_message>
Adds WAT-199 test script and related changes
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/WAT.xlsx
+++ b/src/test/resources/xls/WAT.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13305" windowHeight="2415"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="955" uniqueCount="621">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="959" uniqueCount="624">
   <si>
     <t>TCID</t>
   </si>
@@ -1881,13 +1881,22 @@
   </si>
   <si>
     <t>Verify that User must have the ability to submit an author record after combining 2 or more author records.||Verify that system must submit the feedback when user clicks on 'Submit updates' button ||Verify that success confirmation message relates to submit feedback should display when user clicks on 'Submit updates' button</t>
+  </si>
+  <si>
+    <t>WAT199</t>
+  </si>
+  <si>
+    <t>WAT-1387</t>
+  </si>
+  <si>
+    <t>Verify that If after canceling, the user then begins curation again,the Publications List should contain all publications, and the Bulk Remove panels should have all values un-checked.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2111,7 +2120,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2143,9 +2152,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2177,6 +2187,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2352,14 +2363,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E199"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E200"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A187" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D199" sqref="D199"/>
+      <selection activeCell="C204" sqref="C204"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="30.5703125" customWidth="1" collapsed="1"/>
@@ -2368,7 +2379,7 @@
     <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2385,7 +2396,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -2400,7 +2411,7 @@
       </c>
       <c r="E2" s="4"/>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -2415,7 +2426,7 @@
       </c>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>11</v>
       </c>
@@ -2430,7 +2441,7 @@
       </c>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>12</v>
       </c>
@@ -2445,7 +2456,7 @@
       </c>
       <c r="E5" s="7"/>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>14</v>
       </c>
@@ -2460,7 +2471,7 @@
       </c>
       <c r="E6" s="7"/>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>17</v>
       </c>
@@ -2475,7 +2486,7 @@
       </c>
       <c r="E7" s="7"/>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>20</v>
       </c>
@@ -2490,7 +2501,7 @@
       </c>
       <c r="E8" s="7"/>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>22</v>
       </c>
@@ -2505,7 +2516,7 @@
       </c>
       <c r="E9" s="7"/>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>23</v>
       </c>
@@ -2520,7 +2531,7 @@
       </c>
       <c r="E10" s="7"/>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>24</v>
       </c>
@@ -2535,7 +2546,7 @@
       </c>
       <c r="E11" s="7"/>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>25</v>
       </c>
@@ -2550,7 +2561,7 @@
       </c>
       <c r="E12" s="7"/>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>62</v>
       </c>
@@ -2565,7 +2576,7 @@
       </c>
       <c r="E13" s="7"/>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>63</v>
       </c>
@@ -2580,7 +2591,7 @@
       </c>
       <c r="E14" s="7"/>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>64</v>
       </c>
@@ -2595,7 +2606,7 @@
       </c>
       <c r="E15" s="7"/>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>65</v>
       </c>
@@ -2610,7 +2621,7 @@
       </c>
       <c r="E16" s="7"/>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>74</v>
       </c>
@@ -2625,7 +2636,7 @@
       </c>
       <c r="E17" s="7"/>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>75</v>
       </c>
@@ -2640,7 +2651,7 @@
       </c>
       <c r="E18" s="7"/>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>79</v>
       </c>
@@ -2655,7 +2666,7 @@
       </c>
       <c r="E19" s="7"/>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>81</v>
       </c>
@@ -2670,7 +2681,7 @@
       </c>
       <c r="E20" s="7"/>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>82</v>
       </c>
@@ -2685,7 +2696,7 @@
       </c>
       <c r="E21" s="7"/>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>88</v>
       </c>
@@ -2700,7 +2711,7 @@
       </c>
       <c r="E22" s="7"/>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>90</v>
       </c>
@@ -2715,7 +2726,7 @@
       </c>
       <c r="E23" s="7"/>
     </row>
-    <row r="24" spans="1:5" ht="30">
+    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>94</v>
       </c>
@@ -2730,7 +2741,7 @@
       </c>
       <c r="E24" s="7"/>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>96</v>
       </c>
@@ -2745,7 +2756,7 @@
       </c>
       <c r="E25" s="7"/>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
         <v>98</v>
       </c>
@@ -2760,7 +2771,7 @@
       </c>
       <c r="E26" s="7"/>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
         <v>102</v>
       </c>
@@ -2775,7 +2786,7 @@
       </c>
       <c r="E27" s="7"/>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
         <v>105</v>
       </c>
@@ -2790,7 +2801,7 @@
       </c>
       <c r="E28" s="7"/>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
         <v>108</v>
       </c>
@@ -2805,7 +2816,7 @@
       </c>
       <c r="E29" s="7"/>
     </row>
-    <row r="30" spans="1:5" ht="30">
+    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
         <v>110</v>
       </c>
@@ -2820,7 +2831,7 @@
       </c>
       <c r="E30" s="7"/>
     </row>
-    <row r="31" spans="1:5" ht="30">
+    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
         <v>114</v>
       </c>
@@ -2835,7 +2846,7 @@
       </c>
       <c r="E31" s="7"/>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
         <v>119</v>
       </c>
@@ -2850,7 +2861,7 @@
       </c>
       <c r="E32" s="7"/>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
         <v>120</v>
       </c>
@@ -2865,7 +2876,7 @@
       </c>
       <c r="E33" s="7"/>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
         <v>125</v>
       </c>
@@ -2880,7 +2891,7 @@
       </c>
       <c r="E34" s="7"/>
     </row>
-    <row r="35" spans="1:5" ht="30">
+    <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
         <v>128</v>
       </c>
@@ -2895,7 +2906,7 @@
       </c>
       <c r="E35" s="7"/>
     </row>
-    <row r="36" spans="1:5" ht="30">
+    <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
         <v>131</v>
       </c>
@@ -2910,7 +2921,7 @@
       </c>
       <c r="E36" s="7"/>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
         <v>134</v>
       </c>
@@ -2925,7 +2936,7 @@
       </c>
       <c r="E37" s="7"/>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="9" t="s">
         <v>137</v>
       </c>
@@ -2940,7 +2951,7 @@
       </c>
       <c r="E38" s="7"/>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="s">
         <v>140</v>
       </c>
@@ -2955,7 +2966,7 @@
       </c>
       <c r="E39" s="7"/>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="9" t="s">
         <v>143</v>
       </c>
@@ -2970,7 +2981,7 @@
       </c>
       <c r="E40" s="7"/>
     </row>
-    <row r="41" spans="1:5" ht="30">
+    <row r="41" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
         <v>145</v>
       </c>
@@ -2985,7 +2996,7 @@
       </c>
       <c r="E41" s="7"/>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="9" t="s">
         <v>147</v>
       </c>
@@ -3000,7 +3011,7 @@
       </c>
       <c r="E42" s="7"/>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="9" t="s">
         <v>150</v>
       </c>
@@ -3015,7 +3026,7 @@
       </c>
       <c r="E43" s="7"/>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="9" t="s">
         <v>153</v>
       </c>
@@ -3030,7 +3041,7 @@
       </c>
       <c r="E44" s="7"/>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="9" t="s">
         <v>155</v>
       </c>
@@ -3045,7 +3056,7 @@
       </c>
       <c r="E45" s="7"/>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="12" t="s">
         <v>158</v>
       </c>
@@ -3060,7 +3071,7 @@
       </c>
       <c r="E46" s="7"/>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="12" t="s">
         <v>159</v>
       </c>
@@ -3075,7 +3086,7 @@
       </c>
       <c r="E47" s="7"/>
     </row>
-    <row r="48" spans="1:5" ht="30">
+    <row r="48" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="12" t="s">
         <v>160</v>
       </c>
@@ -3090,7 +3101,7 @@
       </c>
       <c r="E48" s="7"/>
     </row>
-    <row r="49" spans="1:5" ht="30">
+    <row r="49" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="12" t="s">
         <v>161</v>
       </c>
@@ -3105,7 +3116,7 @@
       </c>
       <c r="E49" s="7"/>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="12" t="s">
         <v>164</v>
       </c>
@@ -3120,7 +3131,7 @@
       </c>
       <c r="E50" s="7"/>
     </row>
-    <row r="51" spans="1:5" ht="30">
+    <row r="51" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="9" t="s">
         <v>173</v>
       </c>
@@ -3135,7 +3146,7 @@
       </c>
       <c r="E51" s="7"/>
     </row>
-    <row r="52" spans="1:5">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="9" t="s">
         <v>174</v>
       </c>
@@ -3150,7 +3161,7 @@
       </c>
       <c r="E52" s="7"/>
     </row>
-    <row r="53" spans="1:5">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="9" t="s">
         <v>179</v>
       </c>
@@ -3165,7 +3176,7 @@
       </c>
       <c r="E53" s="7"/>
     </row>
-    <row r="54" spans="1:5">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="9" t="s">
         <v>180</v>
       </c>
@@ -3180,7 +3191,7 @@
       </c>
       <c r="E54" s="7"/>
     </row>
-    <row r="55" spans="1:5">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="9" t="s">
         <v>185</v>
       </c>
@@ -3195,7 +3206,7 @@
       </c>
       <c r="E55" s="7"/>
     </row>
-    <row r="56" spans="1:5">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="s">
         <v>188</v>
       </c>
@@ -3210,7 +3221,7 @@
       </c>
       <c r="E56" s="7"/>
     </row>
-    <row r="57" spans="1:5" ht="30">
+    <row r="57" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="9" t="s">
         <v>191</v>
       </c>
@@ -3225,7 +3236,7 @@
       </c>
       <c r="E57" s="7"/>
     </row>
-    <row r="58" spans="1:5">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="9" t="s">
         <v>194</v>
       </c>
@@ -3240,7 +3251,7 @@
       </c>
       <c r="E58" s="7"/>
     </row>
-    <row r="59" spans="1:5">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
         <v>196</v>
       </c>
@@ -3255,7 +3266,7 @@
       </c>
       <c r="E59" s="7"/>
     </row>
-    <row r="60" spans="1:5" ht="45">
+    <row r="60" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
         <v>199</v>
       </c>
@@ -3270,7 +3281,7 @@
       </c>
       <c r="E60" s="7"/>
     </row>
-    <row r="61" spans="1:5">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="9" t="s">
         <v>202</v>
       </c>
@@ -3285,7 +3296,7 @@
       </c>
       <c r="E61" s="7"/>
     </row>
-    <row r="62" spans="1:5">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="9" t="s">
         <v>204</v>
       </c>
@@ -3300,7 +3311,7 @@
       </c>
       <c r="E62" s="7"/>
     </row>
-    <row r="63" spans="1:5">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="9" t="s">
         <v>206</v>
       </c>
@@ -3315,7 +3326,7 @@
       </c>
       <c r="E63" s="7"/>
     </row>
-    <row r="64" spans="1:5">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="9" t="s">
         <v>208</v>
       </c>
@@ -3330,7 +3341,7 @@
       </c>
       <c r="E64" s="7"/>
     </row>
-    <row r="65" spans="1:5">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="9" t="s">
         <v>217</v>
       </c>
@@ -3345,7 +3356,7 @@
       </c>
       <c r="E65" s="7"/>
     </row>
-    <row r="66" spans="1:5">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="9" t="s">
         <v>218</v>
       </c>
@@ -3360,7 +3371,7 @@
       </c>
       <c r="E66" s="7"/>
     </row>
-    <row r="67" spans="1:5">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="9" t="s">
         <v>223</v>
       </c>
@@ -3375,7 +3386,7 @@
       </c>
       <c r="E67" s="7"/>
     </row>
-    <row r="68" spans="1:5">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="9" t="s">
         <v>224</v>
       </c>
@@ -3390,7 +3401,7 @@
       </c>
       <c r="E68" s="7"/>
     </row>
-    <row r="69" spans="1:5">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="9" t="s">
         <v>225</v>
       </c>
@@ -3405,7 +3416,7 @@
       </c>
       <c r="E69" s="7"/>
     </row>
-    <row r="70" spans="1:5">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="9" t="s">
         <v>226</v>
       </c>
@@ -3420,7 +3431,7 @@
       </c>
       <c r="E70" s="7"/>
     </row>
-    <row r="71" spans="1:5">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="9" t="s">
         <v>233</v>
       </c>
@@ -3435,7 +3446,7 @@
       </c>
       <c r="E71" s="7"/>
     </row>
-    <row r="72" spans="1:5">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="9" t="s">
         <v>237</v>
       </c>
@@ -3450,7 +3461,7 @@
       </c>
       <c r="E72" s="7"/>
     </row>
-    <row r="73" spans="1:5">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="9" t="s">
         <v>239</v>
       </c>
@@ -3465,7 +3476,7 @@
       </c>
       <c r="E73" s="7"/>
     </row>
-    <row r="74" spans="1:5">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="9" t="s">
         <v>243</v>
       </c>
@@ -3480,7 +3491,7 @@
       </c>
       <c r="E74" s="7"/>
     </row>
-    <row r="75" spans="1:5" ht="30">
+    <row r="75" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" s="9" t="s">
         <v>245</v>
       </c>
@@ -3495,7 +3506,7 @@
       </c>
       <c r="E75" s="7"/>
     </row>
-    <row r="76" spans="1:5">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="9" t="s">
         <v>248</v>
       </c>
@@ -3510,7 +3521,7 @@
       </c>
       <c r="E76" s="7"/>
     </row>
-    <row r="77" spans="1:5">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="9" t="s">
         <v>256</v>
       </c>
@@ -3525,7 +3536,7 @@
       </c>
       <c r="E77" s="7"/>
     </row>
-    <row r="78" spans="1:5">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="9" t="s">
         <v>257</v>
       </c>
@@ -3540,7 +3551,7 @@
       </c>
       <c r="E78" s="7"/>
     </row>
-    <row r="79" spans="1:5">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="9" t="s">
         <v>261</v>
       </c>
@@ -3555,7 +3566,7 @@
       </c>
       <c r="E79" s="7"/>
     </row>
-    <row r="80" spans="1:5">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="9" t="s">
         <v>264</v>
       </c>
@@ -3570,7 +3581,7 @@
       </c>
       <c r="E80" s="7"/>
     </row>
-    <row r="81" spans="1:5">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="9" t="s">
         <v>267</v>
       </c>
@@ -3585,7 +3596,7 @@
       </c>
       <c r="E81" s="7"/>
     </row>
-    <row r="82" spans="1:5" ht="30">
+    <row r="82" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A82" s="9" t="s">
         <v>269</v>
       </c>
@@ -3600,7 +3611,7 @@
       </c>
       <c r="E82" s="7"/>
     </row>
-    <row r="83" spans="1:5">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" 